<commit_message>
HardSkill ahora maneja los mismos atributos que son servidos por la API del backend, sin embargo el servicio sigue levantandose de la json.db, sigue pendiente manejar estilos y validaciones y TESTEAR
</commit_message>
<xml_diff>
--- a/Cuadro-de-estado.xlsx
+++ b/Cuadro-de-estado.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="69">
   <si>
     <t>BACKEND</t>
   </si>
@@ -136,9 +136,6 @@
   </si>
   <si>
     <t>(0)</t>
-  </si>
-  <si>
-    <t>Interfase RESPONSIVA</t>
   </si>
   <si>
     <t>Valida-cion Inputs</t>
@@ -198,9 +195,6 @@
     <t>Patrón DTO</t>
   </si>
   <si>
-    <t>Sin interfase</t>
-  </si>
-  <si>
     <r>
       <t>Funcio- nalidad</t>
     </r>
@@ -317,6 +311,15 @@
   </si>
   <si>
     <t>ESTADO DEL PROYECTO Y ORDEN PARA AVANZAR</t>
+  </si>
+  <si>
+    <t>Sin interface</t>
+  </si>
+  <si>
+    <t>Interface RESPONSIVA</t>
+  </si>
+  <si>
+    <t>Reutilizar componentes (p.e atributos de person, skills, etc.) Modules, componentes para pruebas</t>
   </si>
 </sst>
 </file>
@@ -966,7 +969,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1000,7 +1003,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1010,15 +1012,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1051,106 +1044,130 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1451,8 +1468,8 @@
   </sheetPr>
   <dimension ref="A1:M55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1469,107 +1486,107 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="23.25">
-      <c r="A1" s="78" t="s">
-        <v>67</v>
-      </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
-      <c r="J1" s="78"/>
-      <c r="K1" s="78"/>
-      <c r="L1" s="78"/>
+      <c r="A1" s="77" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
+      <c r="L1" s="77"/>
     </row>
     <row r="2" spans="1:12" ht="15.75" thickBot="1"/>
     <row r="3" spans="1:12" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="61" t="s">
-        <v>42</v>
-      </c>
-      <c r="B3" s="44"/>
-      <c r="C3" s="22" t="s">
+      <c r="A3" s="71" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="72"/>
+      <c r="C3" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="22" t="s">
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="75"/>
+      <c r="H3" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="23"/>
-      <c r="J3" s="70"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="25" t="s">
+      <c r="I3" s="74"/>
+      <c r="J3" s="76"/>
+      <c r="K3" s="75"/>
+      <c r="L3" s="21" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:12" s="3" customFormat="1" ht="40.5" customHeight="1" thickBot="1">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="17" t="s">
         <v>21</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>3</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F4" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G4" s="11" t="s">
         <v>47</v>
-      </c>
-      <c r="G4" s="11" t="s">
-        <v>49</v>
       </c>
       <c r="H4" s="9" t="s">
         <v>1</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J4" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K4" s="11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="L4" s="12" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="4.5" customHeight="1">
-      <c r="A5" s="40"/>
-      <c r="B5" s="41"/>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="42"/>
-      <c r="I5" s="42"/>
-      <c r="J5" s="42"/>
-      <c r="K5" s="42"/>
-      <c r="L5" s="42"/>
+      <c r="A5" s="36"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="38"/>
+      <c r="J5" s="38"/>
+      <c r="K5" s="38"/>
+      <c r="L5" s="38"/>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="25" t="s">
         <v>14</v>
       </c>
       <c r="C6" s="16"/>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
-      <c r="F6" s="6"/>
+      <c r="F6" s="13"/>
       <c r="G6" s="7"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
@@ -1578,30 +1595,30 @@
       <c r="L6" s="4"/>
     </row>
     <row r="7" spans="1:12" ht="4.5" customHeight="1">
-      <c r="A7" s="40"/>
-      <c r="B7" s="41"/>
-      <c r="C7" s="42"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="42"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="42"/>
-      <c r="H7" s="42"/>
-      <c r="I7" s="42"/>
-      <c r="J7" s="42"/>
-      <c r="K7" s="42"/>
-      <c r="L7" s="42"/>
+      <c r="A7" s="36"/>
+      <c r="B7" s="37"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="38"/>
+      <c r="J7" s="38"/>
+      <c r="K7" s="38"/>
+      <c r="L7" s="38"/>
     </row>
     <row r="8" spans="1:12">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="17"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="6"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
       <c r="G8" s="7"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
@@ -1610,28 +1627,28 @@
       <c r="L8" s="4"/>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" s="36" t="s">
+      <c r="A9" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="37"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="34"/>
       <c r="F9" s="6"/>
       <c r="G9" s="7"/>
       <c r="H9" s="13"/>
       <c r="I9" s="13"/>
       <c r="J9" s="4"/>
-      <c r="K9" s="39"/>
+      <c r="K9" s="35"/>
       <c r="L9" s="4"/>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="29" t="s">
+      <c r="B10" s="25" t="s">
         <v>13</v>
       </c>
       <c r="C10" s="7"/>
@@ -1646,10 +1663,10 @@
       <c r="L10" s="4"/>
     </row>
     <row r="11" spans="1:12">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="25" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="16"/>
@@ -1664,24 +1681,24 @@
       <c r="L11" s="4"/>
     </row>
     <row r="12" spans="1:12" ht="4.5" customHeight="1">
-      <c r="A12" s="40"/>
-      <c r="B12" s="41"/>
-      <c r="C12" s="42"/>
-      <c r="D12" s="42"/>
-      <c r="E12" s="42"/>
-      <c r="F12" s="42"/>
-      <c r="G12" s="42"/>
-      <c r="H12" s="42"/>
-      <c r="I12" s="42"/>
-      <c r="J12" s="42"/>
-      <c r="K12" s="42"/>
-      <c r="L12" s="42"/>
+      <c r="A12" s="36"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="38"/>
+      <c r="L12" s="38"/>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="29" t="s">
+      <c r="B13" s="25" t="s">
         <v>13</v>
       </c>
       <c r="C13" s="16"/>
@@ -1693,13 +1710,13 @@
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
       <c r="K13" s="7"/>
-      <c r="L13" s="43"/>
+      <c r="L13" s="39"/>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="29" t="s">
+      <c r="B14" s="25" t="s">
         <v>13</v>
       </c>
       <c r="C14" s="16"/>
@@ -1711,27 +1728,27 @@
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
       <c r="K14" s="7"/>
-      <c r="L14" s="43"/>
+      <c r="L14" s="39"/>
     </row>
     <row r="15" spans="1:12" ht="4.5" customHeight="1">
-      <c r="A15" s="40"/>
-      <c r="B15" s="41"/>
-      <c r="C15" s="42"/>
-      <c r="D15" s="42"/>
-      <c r="E15" s="42"/>
-      <c r="F15" s="42"/>
-      <c r="G15" s="42"/>
-      <c r="H15" s="42"/>
-      <c r="I15" s="42"/>
-      <c r="J15" s="42"/>
-      <c r="K15" s="42"/>
-      <c r="L15" s="42"/>
+      <c r="A15" s="36"/>
+      <c r="B15" s="37"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="38"/>
+      <c r="J15" s="38"/>
+      <c r="K15" s="38"/>
+      <c r="L15" s="38"/>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="19" t="s">
+      <c r="A16" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="21"/>
+      <c r="B16" s="20"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
@@ -1744,10 +1761,10 @@
       <c r="L16" s="4"/>
     </row>
     <row r="17" spans="1:13">
-      <c r="A17" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="B17" s="29" t="s">
+      <c r="A17" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C17" s="16"/>
@@ -1762,10 +1779,10 @@
       <c r="L17" s="4"/>
     </row>
     <row r="18" spans="1:13">
-      <c r="A18" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="B18" s="29" t="s">
+      <c r="A18" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C18" s="16"/>
@@ -1780,10 +1797,10 @@
       <c r="L18" s="4"/>
     </row>
     <row r="19" spans="1:13">
-      <c r="A19" s="19" t="s">
+      <c r="A19" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="21"/>
+      <c r="B19" s="20"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
@@ -1796,40 +1813,40 @@
       <c r="L19" s="4"/>
     </row>
     <row r="20" spans="1:13">
-      <c r="A20" s="31" t="s">
+      <c r="A20" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="32"/>
+      <c r="B20" s="28"/>
       <c r="C20" s="8"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="33"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29"/>
       <c r="F20" s="6"/>
       <c r="G20" s="8"/>
-      <c r="H20" s="34"/>
-      <c r="I20" s="34"/>
+      <c r="H20" s="30"/>
+      <c r="I20" s="30"/>
       <c r="J20" s="4"/>
-      <c r="K20" s="35"/>
+      <c r="K20" s="31"/>
       <c r="L20" s="4"/>
     </row>
     <row r="21" spans="1:13" ht="4.5" customHeight="1">
-      <c r="A21" s="40"/>
-      <c r="B21" s="41"/>
-      <c r="C21" s="42"/>
-      <c r="D21" s="42"/>
-      <c r="E21" s="42"/>
-      <c r="F21" s="42"/>
-      <c r="G21" s="42"/>
-      <c r="H21" s="42"/>
-      <c r="I21" s="42"/>
-      <c r="J21" s="42"/>
-      <c r="K21" s="42"/>
-      <c r="L21" s="42"/>
+      <c r="A21" s="36"/>
+      <c r="B21" s="37"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="38"/>
+      <c r="H21" s="38"/>
+      <c r="I21" s="38"/>
+      <c r="J21" s="38"/>
+      <c r="K21" s="38"/>
+      <c r="L21" s="38"/>
     </row>
     <row r="22" spans="1:13">
-      <c r="A22" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="B22" s="21"/>
+      <c r="A22" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" s="20"/>
       <c r="C22" s="16"/>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
@@ -1842,24 +1859,24 @@
       <c r="L22" s="4"/>
     </row>
     <row r="23" spans="1:13" ht="4.5" customHeight="1">
-      <c r="A23" s="40"/>
-      <c r="B23" s="41"/>
-      <c r="C23" s="42"/>
-      <c r="D23" s="42"/>
-      <c r="E23" s="42"/>
-      <c r="F23" s="42"/>
-      <c r="G23" s="42"/>
-      <c r="H23" s="42"/>
-      <c r="I23" s="42"/>
-      <c r="J23" s="42"/>
-      <c r="K23" s="42"/>
-      <c r="L23" s="42"/>
+      <c r="A23" s="36"/>
+      <c r="B23" s="37"/>
+      <c r="C23" s="38"/>
+      <c r="D23" s="38"/>
+      <c r="E23" s="38"/>
+      <c r="F23" s="38"/>
+      <c r="G23" s="38"/>
+      <c r="H23" s="38"/>
+      <c r="I23" s="38"/>
+      <c r="J23" s="38"/>
+      <c r="K23" s="38"/>
+      <c r="L23" s="38"/>
     </row>
     <row r="24" spans="1:13">
-      <c r="A24" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="B24" s="45"/>
+      <c r="A24" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" s="40"/>
       <c r="C24" s="7"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
@@ -1872,13 +1889,13 @@
       <c r="L24" s="4"/>
     </row>
     <row r="25" spans="1:13">
-      <c r="A25" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="B25" s="29" t="s">
+      <c r="A25" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="C25" s="27"/>
+      <c r="C25" s="23"/>
       <c r="D25" s="8"/>
       <c r="E25" s="8"/>
       <c r="F25" s="6"/>
@@ -1890,217 +1907,219 @@
       <c r="L25" s="7"/>
     </row>
     <row r="26" spans="1:13" ht="4.5" customHeight="1" thickBot="1">
-      <c r="A26" s="40"/>
-      <c r="B26" s="41"/>
-      <c r="C26" s="42"/>
-      <c r="D26" s="42"/>
-      <c r="E26" s="42"/>
-      <c r="F26" s="42"/>
-      <c r="G26" s="42"/>
-      <c r="H26" s="42"/>
-      <c r="I26" s="42"/>
-      <c r="J26" s="42"/>
-      <c r="K26" s="42"/>
-      <c r="L26" s="42"/>
+      <c r="A26" s="36"/>
+      <c r="B26" s="37"/>
+      <c r="C26" s="38"/>
+      <c r="D26" s="38"/>
+      <c r="E26" s="38"/>
+      <c r="F26" s="38"/>
+      <c r="G26" s="38"/>
+      <c r="H26" s="38"/>
+      <c r="I26" s="38"/>
+      <c r="J26" s="38"/>
+      <c r="K26" s="38"/>
+      <c r="L26" s="38"/>
     </row>
     <row r="27" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A27" s="28"/>
-      <c r="B27" s="30"/>
-      <c r="C27" s="22" t="s">
+      <c r="A27" s="24"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="23"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="23"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="22" t="s">
+      <c r="D27" s="74"/>
+      <c r="E27" s="74"/>
+      <c r="F27" s="74"/>
+      <c r="G27" s="75"/>
+      <c r="H27" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="I27" s="23"/>
-      <c r="J27" s="70"/>
-      <c r="K27" s="24"/>
-      <c r="L27" s="25" t="s">
+      <c r="I27" s="74"/>
+      <c r="J27" s="76"/>
+      <c r="K27" s="75"/>
+      <c r="L27" s="21" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A28" s="62" t="s">
+      <c r="A28" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="63"/>
-      <c r="C28" s="46"/>
-      <c r="D28" s="47"/>
-      <c r="E28" s="47"/>
-      <c r="F28" s="47"/>
-      <c r="G28" s="48"/>
-      <c r="H28" s="46"/>
-      <c r="I28" s="47"/>
-      <c r="J28" s="47"/>
-      <c r="K28" s="48"/>
-      <c r="L28" s="53"/>
+      <c r="B28" s="49"/>
+      <c r="C28" s="50"/>
+      <c r="D28" s="51"/>
+      <c r="E28" s="51"/>
+      <c r="F28" s="51"/>
+      <c r="G28" s="52"/>
+      <c r="H28" s="50"/>
+      <c r="I28" s="51"/>
+      <c r="J28" s="51"/>
+      <c r="K28" s="52"/>
+      <c r="L28" s="42"/>
     </row>
     <row r="29" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A29" s="62" t="s">
-        <v>65</v>
-      </c>
-      <c r="B29" s="63"/>
-      <c r="C29" s="71"/>
-      <c r="D29" s="72"/>
-      <c r="E29" s="72"/>
-      <c r="F29" s="72"/>
-      <c r="G29" s="73"/>
-      <c r="H29" s="46"/>
-      <c r="I29" s="47"/>
-      <c r="J29" s="47"/>
-      <c r="K29" s="48"/>
+      <c r="A29" s="48" t="s">
+        <v>63</v>
+      </c>
+      <c r="B29" s="49"/>
+      <c r="C29" s="45"/>
+      <c r="D29" s="46"/>
+      <c r="E29" s="46"/>
+      <c r="F29" s="46"/>
+      <c r="G29" s="47"/>
+      <c r="H29" s="50"/>
+      <c r="I29" s="51"/>
+      <c r="J29" s="51"/>
+      <c r="K29" s="52"/>
     </row>
     <row r="30" spans="1:13" ht="4.5" customHeight="1">
-      <c r="A30" s="40"/>
-      <c r="B30" s="41"/>
-      <c r="C30" s="42"/>
-      <c r="D30" s="42"/>
-      <c r="E30" s="42"/>
-      <c r="F30" s="42"/>
-      <c r="G30" s="42"/>
-      <c r="H30" s="42"/>
-      <c r="I30" s="42"/>
-      <c r="J30" s="42"/>
-      <c r="K30" s="42"/>
-      <c r="L30" s="42"/>
+      <c r="A30" s="36"/>
+      <c r="B30" s="37"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="38"/>
+      <c r="K30" s="38"/>
+      <c r="L30" s="38"/>
     </row>
     <row r="31" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A31" s="64" t="s">
-        <v>43</v>
-      </c>
-      <c r="B31" s="65"/>
-      <c r="C31" s="66"/>
-      <c r="D31" s="67"/>
-      <c r="E31" s="67"/>
-      <c r="F31" s="67"/>
-      <c r="G31" s="68"/>
-      <c r="H31" s="69"/>
-      <c r="I31" s="67"/>
-      <c r="J31" s="67"/>
-      <c r="K31" s="68"/>
-      <c r="L31" s="26" t="s">
+      <c r="A31" s="60" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31" s="61"/>
+      <c r="C31" s="67"/>
+      <c r="D31" s="68"/>
+      <c r="E31" s="68"/>
+      <c r="F31" s="68"/>
+      <c r="G31" s="69"/>
+      <c r="H31" s="70"/>
+      <c r="I31" s="68"/>
+      <c r="J31" s="68"/>
+      <c r="K31" s="69"/>
+      <c r="L31" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="M31" s="50"/>
+      <c r="M31" s="41"/>
     </row>
     <row r="32" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A32" s="64" t="s">
-        <v>40</v>
-      </c>
-      <c r="B32" s="65"/>
-      <c r="C32" s="58"/>
-      <c r="D32" s="59"/>
-      <c r="E32" s="59"/>
-      <c r="F32" s="59"/>
-      <c r="G32" s="60"/>
-      <c r="H32" s="71" t="s">
-        <v>45</v>
-      </c>
-      <c r="I32" s="72"/>
-      <c r="J32" s="72"/>
-      <c r="K32" s="72"/>
-      <c r="L32" s="73"/>
-      <c r="M32" s="50"/>
-    </row>
-    <row r="33" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A33" s="64" t="s">
+      <c r="A32" s="60" t="s">
+        <v>67</v>
+      </c>
+      <c r="B32" s="61"/>
+      <c r="C32" s="57"/>
+      <c r="D32" s="58"/>
+      <c r="E32" s="58"/>
+      <c r="F32" s="58"/>
+      <c r="G32" s="59"/>
+      <c r="H32" s="45" t="s">
+        <v>66</v>
+      </c>
+      <c r="I32" s="46"/>
+      <c r="J32" s="46"/>
+      <c r="K32" s="46"/>
+      <c r="L32" s="47"/>
+      <c r="M32" s="41"/>
+    </row>
+    <row r="33" spans="1:13" ht="30.75" customHeight="1" thickBot="1">
+      <c r="A33" s="81" t="s">
         <v>37</v>
       </c>
-      <c r="B33" s="65"/>
-      <c r="C33" s="46"/>
-      <c r="D33" s="47"/>
-      <c r="E33" s="47"/>
-      <c r="F33" s="47"/>
-      <c r="G33" s="48"/>
-      <c r="H33" s="51"/>
-      <c r="I33" s="52"/>
-      <c r="J33" s="52"/>
-      <c r="K33" s="54"/>
-      <c r="M33" s="50"/>
+      <c r="B33" s="82"/>
+      <c r="C33" s="78" t="s">
+        <v>68</v>
+      </c>
+      <c r="D33" s="79"/>
+      <c r="E33" s="79"/>
+      <c r="F33" s="79"/>
+      <c r="G33" s="80"/>
+      <c r="H33" s="64"/>
+      <c r="I33" s="65"/>
+      <c r="J33" s="65"/>
+      <c r="K33" s="66"/>
+      <c r="M33" s="41"/>
     </row>
     <row r="34" spans="1:13" ht="4.5" customHeight="1" thickBot="1">
-      <c r="A34" s="40"/>
-      <c r="B34" s="41"/>
-      <c r="C34" s="42"/>
-      <c r="D34" s="42"/>
-      <c r="E34" s="42"/>
-      <c r="F34" s="42"/>
-      <c r="G34" s="42"/>
-      <c r="H34" s="42"/>
-      <c r="I34" s="42"/>
-      <c r="J34" s="42"/>
-      <c r="K34" s="42"/>
+      <c r="A34" s="36"/>
+      <c r="B34" s="37"/>
+      <c r="C34" s="38"/>
+      <c r="D34" s="38"/>
+      <c r="E34" s="38"/>
+      <c r="F34" s="38"/>
+      <c r="G34" s="38"/>
+      <c r="H34" s="38"/>
+      <c r="I34" s="38"/>
+      <c r="J34" s="38"/>
+      <c r="K34" s="38"/>
     </row>
     <row r="35" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A35" s="64" t="s">
+      <c r="A35" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="65"/>
-      <c r="C35" s="46"/>
-      <c r="D35" s="47"/>
-      <c r="E35" s="47"/>
-      <c r="F35" s="47"/>
-      <c r="G35" s="48"/>
-      <c r="H35" s="46"/>
-      <c r="I35" s="47"/>
-      <c r="J35" s="47"/>
-      <c r="K35" s="48"/>
-      <c r="M35" s="50"/>
+      <c r="B35" s="61"/>
+      <c r="C35" s="50"/>
+      <c r="D35" s="51"/>
+      <c r="E35" s="51"/>
+      <c r="F35" s="51"/>
+      <c r="G35" s="52"/>
+      <c r="H35" s="50"/>
+      <c r="I35" s="51"/>
+      <c r="J35" s="51"/>
+      <c r="K35" s="52"/>
+      <c r="M35" s="41"/>
     </row>
     <row r="36" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A36" s="64" t="s">
+      <c r="A36" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="65"/>
-      <c r="C36" s="46"/>
-      <c r="D36" s="47"/>
-      <c r="E36" s="47"/>
-      <c r="F36" s="47"/>
-      <c r="G36" s="48"/>
-      <c r="H36" s="46"/>
-      <c r="I36" s="47"/>
-      <c r="J36" s="47"/>
-      <c r="K36" s="48"/>
-      <c r="M36" s="50"/>
+      <c r="B36" s="61"/>
+      <c r="C36" s="50"/>
+      <c r="D36" s="51"/>
+      <c r="E36" s="51"/>
+      <c r="F36" s="51"/>
+      <c r="G36" s="52"/>
+      <c r="H36" s="50"/>
+      <c r="I36" s="51"/>
+      <c r="J36" s="51"/>
+      <c r="K36" s="52"/>
+      <c r="M36" s="41"/>
     </row>
     <row r="37" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A37" s="64" t="s">
+      <c r="A37" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="B37" s="65"/>
-      <c r="C37" s="46"/>
-      <c r="D37" s="47"/>
-      <c r="E37" s="47"/>
-      <c r="F37" s="47"/>
-      <c r="G37" s="48"/>
-      <c r="H37" s="46"/>
-      <c r="I37" s="47"/>
-      <c r="J37" s="47"/>
-      <c r="K37" s="48"/>
-      <c r="M37" s="50"/>
+      <c r="B37" s="61"/>
+      <c r="C37" s="50"/>
+      <c r="D37" s="51"/>
+      <c r="E37" s="51"/>
+      <c r="F37" s="51"/>
+      <c r="G37" s="52"/>
+      <c r="H37" s="50"/>
+      <c r="I37" s="51"/>
+      <c r="J37" s="51"/>
+      <c r="K37" s="52"/>
+      <c r="M37" s="41"/>
     </row>
     <row r="39" spans="1:13">
-      <c r="A39" s="75" t="s">
+      <c r="A39" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="B39" s="49"/>
-      <c r="C39" s="49"/>
-      <c r="D39" s="49"/>
-      <c r="E39" s="49"/>
+      <c r="B39" s="54"/>
+      <c r="C39" s="54"/>
+      <c r="D39" s="54"/>
+      <c r="E39" s="54"/>
     </row>
     <row r="40" spans="1:13">
       <c r="A40" s="14" t="s">
         <v>26</v>
       </c>
       <c r="B40" s="13"/>
-      <c r="C40" s="76" t="s">
+      <c r="C40" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="D40" s="77"/>
+      <c r="D40" s="56"/>
       <c r="E40" s="7"/>
     </row>
     <row r="41" spans="1:13">
@@ -2108,10 +2127,10 @@
         <v>22</v>
       </c>
       <c r="B41" s="5"/>
-      <c r="C41" s="76" t="s">
+      <c r="C41" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="D41" s="77"/>
+      <c r="D41" s="56"/>
       <c r="E41" s="8"/>
     </row>
     <row r="42" spans="1:13">
@@ -2122,179 +2141,205 @@
     </row>
     <row r="43" spans="1:13" ht="15.75" thickBot="1"/>
     <row r="44" spans="1:13">
-      <c r="A44" s="55" t="s">
+      <c r="A44" s="62" t="s">
         <v>38</v>
       </c>
-      <c r="B44" s="56"/>
-      <c r="C44" s="56"/>
-      <c r="D44" s="56"/>
-      <c r="E44" s="56"/>
-      <c r="F44" s="56"/>
-      <c r="G44" s="56"/>
-      <c r="H44" s="56"/>
-      <c r="I44" s="56"/>
-      <c r="J44" s="56"/>
-      <c r="K44" s="56"/>
-      <c r="L44" s="56"/>
+      <c r="B44" s="63"/>
+      <c r="C44" s="63"/>
+      <c r="D44" s="63"/>
+      <c r="E44" s="63"/>
+      <c r="F44" s="63"/>
+      <c r="G44" s="63"/>
+      <c r="H44" s="63"/>
+      <c r="I44" s="63"/>
+      <c r="J44" s="63"/>
+      <c r="K44" s="63"/>
+      <c r="L44" s="63"/>
     </row>
     <row r="45" spans="1:13">
-      <c r="A45" s="57" t="s">
+      <c r="A45" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="B45" s="74" t="s">
+      <c r="B45" s="44" t="s">
+        <v>60</v>
+      </c>
+      <c r="C45" s="44"/>
+      <c r="D45" s="44"/>
+      <c r="E45" s="44"/>
+      <c r="F45" s="44"/>
+      <c r="G45" s="44"/>
+      <c r="H45" s="44"/>
+      <c r="I45" s="44"/>
+      <c r="J45" s="44"/>
+      <c r="K45" s="44"/>
+      <c r="L45" s="44"/>
+    </row>
+    <row r="46" spans="1:13" ht="30" customHeight="1">
+      <c r="A46" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="B46" s="44" t="s">
+        <v>64</v>
+      </c>
+      <c r="C46" s="44"/>
+      <c r="D46" s="44"/>
+      <c r="E46" s="44"/>
+      <c r="F46" s="44"/>
+      <c r="G46" s="44"/>
+      <c r="H46" s="44"/>
+      <c r="I46" s="44"/>
+      <c r="J46" s="44"/>
+      <c r="K46" s="44"/>
+      <c r="L46" s="44"/>
+    </row>
+    <row r="47" spans="1:13" ht="15" customHeight="1">
+      <c r="A47" s="43" t="s">
+        <v>33</v>
+      </c>
+      <c r="B47" s="44" t="s">
+        <v>61</v>
+      </c>
+      <c r="C47" s="44"/>
+      <c r="D47" s="44"/>
+      <c r="E47" s="44"/>
+      <c r="F47" s="44"/>
+      <c r="G47" s="44"/>
+      <c r="H47" s="44"/>
+      <c r="I47" s="44"/>
+      <c r="J47" s="44"/>
+      <c r="K47" s="44"/>
+      <c r="L47" s="44"/>
+    </row>
+    <row r="48" spans="1:13">
+      <c r="A48" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="B48" s="44" t="s">
         <v>62</v>
       </c>
-      <c r="C45" s="74"/>
-      <c r="D45" s="74"/>
-      <c r="E45" s="74"/>
-      <c r="F45" s="74"/>
-      <c r="G45" s="74"/>
-      <c r="H45" s="74"/>
-      <c r="I45" s="74"/>
-      <c r="J45" s="74"/>
-      <c r="K45" s="74"/>
-      <c r="L45" s="74"/>
-    </row>
-    <row r="46" spans="1:13" ht="30" customHeight="1">
-      <c r="A46" s="57" t="s">
-        <v>32</v>
-      </c>
-      <c r="B46" s="74" t="s">
-        <v>66</v>
-      </c>
-      <c r="C46" s="74"/>
-      <c r="D46" s="74"/>
-      <c r="E46" s="74"/>
-      <c r="F46" s="74"/>
-      <c r="G46" s="74"/>
-      <c r="H46" s="74"/>
-      <c r="I46" s="74"/>
-      <c r="J46" s="74"/>
-      <c r="K46" s="74"/>
-      <c r="L46" s="74"/>
-    </row>
-    <row r="47" spans="1:13" ht="15" customHeight="1">
-      <c r="A47" s="57" t="s">
-        <v>33</v>
-      </c>
-      <c r="B47" s="74" t="s">
-        <v>63</v>
-      </c>
-      <c r="C47" s="74"/>
-      <c r="D47" s="74"/>
-      <c r="E47" s="74"/>
-      <c r="F47" s="74"/>
-      <c r="G47" s="74"/>
-      <c r="H47" s="74"/>
-      <c r="I47" s="74"/>
-      <c r="J47" s="74"/>
-      <c r="K47" s="74"/>
-      <c r="L47" s="74"/>
-    </row>
-    <row r="48" spans="1:13">
-      <c r="A48" s="57" t="s">
-        <v>34</v>
-      </c>
-      <c r="B48" s="74" t="s">
-        <v>64</v>
-      </c>
-      <c r="C48" s="74"/>
-      <c r="D48" s="74"/>
-      <c r="E48" s="74"/>
-      <c r="F48" s="74"/>
-      <c r="G48" s="74"/>
-      <c r="H48" s="74"/>
-      <c r="I48" s="74"/>
-      <c r="J48" s="74"/>
-      <c r="K48" s="74"/>
-      <c r="L48" s="74"/>
+      <c r="C48" s="44"/>
+      <c r="D48" s="44"/>
+      <c r="E48" s="44"/>
+      <c r="F48" s="44"/>
+      <c r="G48" s="44"/>
+      <c r="H48" s="44"/>
+      <c r="I48" s="44"/>
+      <c r="J48" s="44"/>
+      <c r="K48" s="44"/>
+      <c r="L48" s="44"/>
     </row>
     <row r="49" spans="1:12">
-      <c r="A49" s="57" t="s">
+      <c r="A49" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="B49" s="74" t="s">
-        <v>51</v>
-      </c>
-      <c r="C49" s="74"/>
-      <c r="D49" s="74"/>
-      <c r="E49" s="74"/>
-      <c r="F49" s="74"/>
-      <c r="G49" s="74"/>
-      <c r="H49" s="74"/>
-      <c r="I49" s="74"/>
-      <c r="J49" s="74"/>
-      <c r="K49" s="74"/>
-      <c r="L49" s="74"/>
+      <c r="B49" s="44" t="s">
+        <v>49</v>
+      </c>
+      <c r="C49" s="44"/>
+      <c r="D49" s="44"/>
+      <c r="E49" s="44"/>
+      <c r="F49" s="44"/>
+      <c r="G49" s="44"/>
+      <c r="H49" s="44"/>
+      <c r="I49" s="44"/>
+      <c r="J49" s="44"/>
+      <c r="K49" s="44"/>
+      <c r="L49" s="44"/>
     </row>
     <row r="50" spans="1:12">
-      <c r="A50" s="57" t="s">
+      <c r="A50" s="43" t="s">
+        <v>57</v>
+      </c>
+      <c r="B50" s="44" t="s">
+        <v>36</v>
+      </c>
+      <c r="C50" s="44"/>
+      <c r="D50" s="44"/>
+      <c r="E50" s="44"/>
+      <c r="F50" s="44"/>
+      <c r="G50" s="44"/>
+      <c r="H50" s="44"/>
+      <c r="I50" s="44"/>
+      <c r="J50" s="44"/>
+      <c r="K50" s="44"/>
+      <c r="L50" s="44"/>
+    </row>
+    <row r="51" spans="1:12">
+      <c r="A51" s="43" t="s">
+        <v>55</v>
+      </c>
+      <c r="B51" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="B50" s="74" t="s">
-        <v>36</v>
-      </c>
-      <c r="C50" s="74"/>
-      <c r="D50" s="74"/>
-      <c r="E50" s="74"/>
-      <c r="F50" s="74"/>
-      <c r="G50" s="74"/>
-      <c r="H50" s="74"/>
-      <c r="I50" s="74"/>
-      <c r="J50" s="74"/>
-      <c r="K50" s="74"/>
-      <c r="L50" s="74"/>
-    </row>
-    <row r="51" spans="1:12">
-      <c r="A51" s="57" t="s">
-        <v>57</v>
-      </c>
-      <c r="B51" s="74" t="s">
-        <v>61</v>
-      </c>
-      <c r="C51" s="74"/>
-      <c r="D51" s="74"/>
-      <c r="E51" s="74"/>
-      <c r="F51" s="74"/>
-      <c r="G51" s="74"/>
-      <c r="H51" s="74"/>
-      <c r="I51" s="74"/>
-      <c r="J51" s="74"/>
-      <c r="K51" s="74"/>
-      <c r="L51" s="74"/>
+      <c r="C51" s="44"/>
+      <c r="D51" s="44"/>
+      <c r="E51" s="44"/>
+      <c r="F51" s="44"/>
+      <c r="G51" s="44"/>
+      <c r="H51" s="44"/>
+      <c r="I51" s="44"/>
+      <c r="J51" s="44"/>
+      <c r="K51" s="44"/>
+      <c r="L51" s="44"/>
     </row>
     <row r="52" spans="1:12">
-      <c r="A52" s="57" t="s">
+      <c r="A52" s="43" t="s">
+        <v>56</v>
+      </c>
+      <c r="B52" s="44" t="s">
         <v>58</v>
       </c>
-      <c r="B52" s="74" t="s">
-        <v>60</v>
-      </c>
-      <c r="C52" s="74"/>
-      <c r="D52" s="74"/>
-      <c r="E52" s="74"/>
-      <c r="F52" s="74"/>
-      <c r="G52" s="74"/>
-      <c r="H52" s="74"/>
-      <c r="I52" s="74"/>
-      <c r="J52" s="74"/>
-      <c r="K52" s="74"/>
-      <c r="L52" s="74"/>
+      <c r="C52" s="44"/>
+      <c r="D52" s="44"/>
+      <c r="E52" s="44"/>
+      <c r="F52" s="44"/>
+      <c r="G52" s="44"/>
+      <c r="H52" s="44"/>
+      <c r="I52" s="44"/>
+      <c r="J52" s="44"/>
+      <c r="K52" s="44"/>
+      <c r="L52" s="44"/>
     </row>
     <row r="53" spans="1:12">
-      <c r="C53" s="50"/>
+      <c r="C53" s="41"/>
     </row>
     <row r="54" spans="1:12">
-      <c r="C54" s="50"/>
+      <c r="C54" s="41"/>
     </row>
     <row r="55" spans="1:12">
-      <c r="B55" s="50"/>
+      <c r="B55" s="41"/>
     </row>
   </sheetData>
   <sortState ref="A24:K25">
     <sortCondition ref="A3"/>
   </sortState>
   <mergeCells count="42">
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="H27:K27"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="H28:K28"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="H33:K33"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="H31:K31"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="B49:L49"/>
+    <mergeCell ref="B50:L50"/>
+    <mergeCell ref="H35:K35"/>
+    <mergeCell ref="H36:K36"/>
+    <mergeCell ref="H37:K37"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:B37"/>
     <mergeCell ref="B51:L51"/>
     <mergeCell ref="B52:L52"/>
     <mergeCell ref="C29:G29"/>
@@ -2306,37 +2351,11 @@
     <mergeCell ref="B45:L45"/>
     <mergeCell ref="C32:G32"/>
     <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
     <mergeCell ref="H32:L32"/>
     <mergeCell ref="A44:L44"/>
     <mergeCell ref="B46:L46"/>
     <mergeCell ref="B47:L47"/>
     <mergeCell ref="B48:L48"/>
-    <mergeCell ref="B49:L49"/>
-    <mergeCell ref="B50:L50"/>
-    <mergeCell ref="H35:K35"/>
-    <mergeCell ref="H36:K36"/>
-    <mergeCell ref="H37:K37"/>
-    <mergeCell ref="H33:K33"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="H31:K31"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="H27:K27"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="H28:K28"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="A1:L1"/>
   </mergeCells>
   <pageMargins left="0.51" right="0.35" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="89" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
actualizado cuadro control del proyecto
</commit_message>
<xml_diff>
--- a/Cuadro-de-estado.xlsx
+++ b/Cuadro-de-estado.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="69">
   <si>
     <t>BACKEND</t>
   </si>
@@ -136,9 +136,6 @@
   </si>
   <si>
     <t>(0)</t>
-  </si>
-  <si>
-    <t>Interfase RESPONSIVA</t>
   </si>
   <si>
     <t>Valida-cion Inputs</t>
@@ -198,9 +195,6 @@
     <t>Patrón DTO</t>
   </si>
   <si>
-    <t>Sin interfase</t>
-  </si>
-  <si>
     <r>
       <t>Funcio- nalidad</t>
     </r>
@@ -317,6 +311,15 @@
   </si>
   <si>
     <t>ESTADO DEL PROYECTO Y ORDEN PARA AVANZAR</t>
+  </si>
+  <si>
+    <t>Sin interface</t>
+  </si>
+  <si>
+    <t>Interface RESPONSIVA</t>
+  </si>
+  <si>
+    <t>Reutilizar componentes (p.e atributos de person, skills, etc.) Modules, componentes para pruebas</t>
   </si>
 </sst>
 </file>
@@ -521,7 +524,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="36">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -707,17 +710,6 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -966,7 +958,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -999,26 +991,16 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1026,24 +1008,22 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1051,105 +1031,129 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1451,8 +1455,8 @@
   </sheetPr>
   <dimension ref="A1:M55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32:B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1469,107 +1473,107 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="23.25">
-      <c r="A1" s="78" t="s">
-        <v>67</v>
-      </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
-      <c r="J1" s="78"/>
-      <c r="K1" s="78"/>
-      <c r="L1" s="78"/>
+      <c r="A1" s="42" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="42"/>
+      <c r="L1" s="42"/>
     </row>
     <row r="2" spans="1:12" ht="15.75" thickBot="1"/>
     <row r="3" spans="1:12" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="61" t="s">
-        <v>42</v>
+      <c r="A3" s="43" t="s">
+        <v>41</v>
       </c>
       <c r="B3" s="44"/>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="22" t="s">
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="23"/>
-      <c r="J3" s="70"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="25" t="s">
+      <c r="I3" s="46"/>
+      <c r="J3" s="48"/>
+      <c r="K3" s="47"/>
+      <c r="L3" s="21" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:12" s="3" customFormat="1" ht="40.5" customHeight="1" thickBot="1">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="17" t="s">
         <v>21</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>3</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F4" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G4" s="11" t="s">
         <v>47</v>
-      </c>
-      <c r="G4" s="11" t="s">
-        <v>49</v>
       </c>
       <c r="H4" s="9" t="s">
         <v>1</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J4" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K4" s="11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="L4" s="12" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="4.5" customHeight="1">
-      <c r="A5" s="40"/>
-      <c r="B5" s="41"/>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="42"/>
-      <c r="I5" s="42"/>
-      <c r="J5" s="42"/>
-      <c r="K5" s="42"/>
-      <c r="L5" s="42"/>
+      <c r="A5" s="34"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
+      <c r="H5" s="36"/>
+      <c r="I5" s="36"/>
+      <c r="J5" s="36"/>
+      <c r="K5" s="36"/>
+      <c r="L5" s="36"/>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="25" t="s">
         <v>14</v>
       </c>
       <c r="C6" s="16"/>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
-      <c r="F6" s="6"/>
+      <c r="F6" s="13"/>
       <c r="G6" s="7"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
@@ -1578,30 +1582,30 @@
       <c r="L6" s="4"/>
     </row>
     <row r="7" spans="1:12" ht="4.5" customHeight="1">
-      <c r="A7" s="40"/>
-      <c r="B7" s="41"/>
-      <c r="C7" s="42"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="42"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="42"/>
-      <c r="H7" s="42"/>
-      <c r="I7" s="42"/>
-      <c r="J7" s="42"/>
-      <c r="K7" s="42"/>
-      <c r="L7" s="42"/>
+      <c r="A7" s="34"/>
+      <c r="B7" s="35"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="36"/>
+      <c r="I7" s="36"/>
+      <c r="J7" s="36"/>
+      <c r="K7" s="36"/>
+      <c r="L7" s="36"/>
     </row>
     <row r="8" spans="1:12">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="17"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="6"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
       <c r="G8" s="7"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
@@ -1610,34 +1614,34 @@
       <c r="L8" s="4"/>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" s="36" t="s">
+      <c r="A9" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="37"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="6"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
       <c r="G9" s="7"/>
       <c r="H9" s="13"/>
       <c r="I9" s="13"/>
       <c r="J9" s="4"/>
-      <c r="K9" s="39"/>
+      <c r="K9" s="33"/>
       <c r="L9" s="4"/>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="29" t="s">
+      <c r="B10" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="6"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
       <c r="G10" s="7"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
@@ -1646,10 +1650,10 @@
       <c r="L10" s="4"/>
     </row>
     <row r="11" spans="1:12">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="25" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="16"/>
@@ -1664,24 +1668,24 @@
       <c r="L11" s="4"/>
     </row>
     <row r="12" spans="1:12" ht="4.5" customHeight="1">
-      <c r="A12" s="40"/>
-      <c r="B12" s="41"/>
-      <c r="C12" s="42"/>
-      <c r="D12" s="42"/>
-      <c r="E12" s="42"/>
-      <c r="F12" s="42"/>
-      <c r="G12" s="42"/>
-      <c r="H12" s="42"/>
-      <c r="I12" s="42"/>
-      <c r="J12" s="42"/>
-      <c r="K12" s="42"/>
-      <c r="L12" s="42"/>
+      <c r="A12" s="34"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="36"/>
+      <c r="H12" s="36"/>
+      <c r="I12" s="36"/>
+      <c r="J12" s="36"/>
+      <c r="K12" s="36"/>
+      <c r="L12" s="36"/>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="29" t="s">
+      <c r="B13" s="25" t="s">
         <v>13</v>
       </c>
       <c r="C13" s="16"/>
@@ -1693,13 +1697,13 @@
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
       <c r="K13" s="7"/>
-      <c r="L13" s="43"/>
+      <c r="L13" s="37"/>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="29" t="s">
+      <c r="B14" s="25" t="s">
         <v>13</v>
       </c>
       <c r="C14" s="16"/>
@@ -1711,27 +1715,27 @@
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
       <c r="K14" s="7"/>
-      <c r="L14" s="43"/>
+      <c r="L14" s="37"/>
     </row>
     <row r="15" spans="1:12" ht="4.5" customHeight="1">
-      <c r="A15" s="40"/>
-      <c r="B15" s="41"/>
-      <c r="C15" s="42"/>
-      <c r="D15" s="42"/>
-      <c r="E15" s="42"/>
-      <c r="F15" s="42"/>
-      <c r="G15" s="42"/>
-      <c r="H15" s="42"/>
-      <c r="I15" s="42"/>
-      <c r="J15" s="42"/>
-      <c r="K15" s="42"/>
-      <c r="L15" s="42"/>
+      <c r="A15" s="34"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="36"/>
+      <c r="I15" s="36"/>
+      <c r="J15" s="36"/>
+      <c r="K15" s="36"/>
+      <c r="L15" s="36"/>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="19" t="s">
+      <c r="A16" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="21"/>
+      <c r="B16" s="20"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
@@ -1744,10 +1748,10 @@
       <c r="L16" s="4"/>
     </row>
     <row r="17" spans="1:13">
-      <c r="A17" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="B17" s="29" t="s">
+      <c r="A17" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C17" s="16"/>
@@ -1762,10 +1766,10 @@
       <c r="L17" s="4"/>
     </row>
     <row r="18" spans="1:13">
-      <c r="A18" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="B18" s="29" t="s">
+      <c r="A18" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C18" s="16"/>
@@ -1780,10 +1784,10 @@
       <c r="L18" s="4"/>
     </row>
     <row r="19" spans="1:13">
-      <c r="A19" s="19" t="s">
+      <c r="A19" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="21"/>
+      <c r="B19" s="20"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
@@ -1796,40 +1800,40 @@
       <c r="L19" s="4"/>
     </row>
     <row r="20" spans="1:13">
-      <c r="A20" s="31" t="s">
+      <c r="A20" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="32"/>
+      <c r="B20" s="28"/>
       <c r="C20" s="8"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="33"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29"/>
       <c r="F20" s="6"/>
       <c r="G20" s="8"/>
-      <c r="H20" s="34"/>
-      <c r="I20" s="34"/>
+      <c r="H20" s="30"/>
+      <c r="I20" s="30"/>
       <c r="J20" s="4"/>
-      <c r="K20" s="35"/>
+      <c r="K20" s="31"/>
       <c r="L20" s="4"/>
     </row>
     <row r="21" spans="1:13" ht="4.5" customHeight="1">
-      <c r="A21" s="40"/>
-      <c r="B21" s="41"/>
-      <c r="C21" s="42"/>
-      <c r="D21" s="42"/>
-      <c r="E21" s="42"/>
-      <c r="F21" s="42"/>
-      <c r="G21" s="42"/>
-      <c r="H21" s="42"/>
-      <c r="I21" s="42"/>
-      <c r="J21" s="42"/>
-      <c r="K21" s="42"/>
-      <c r="L21" s="42"/>
+      <c r="A21" s="34"/>
+      <c r="B21" s="35"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="36"/>
+      <c r="G21" s="36"/>
+      <c r="H21" s="36"/>
+      <c r="I21" s="36"/>
+      <c r="J21" s="36"/>
+      <c r="K21" s="36"/>
+      <c r="L21" s="36"/>
     </row>
     <row r="22" spans="1:13">
-      <c r="A22" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="B22" s="21"/>
+      <c r="A22" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" s="20"/>
       <c r="C22" s="16"/>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
@@ -1842,27 +1846,27 @@
       <c r="L22" s="4"/>
     </row>
     <row r="23" spans="1:13" ht="4.5" customHeight="1">
-      <c r="A23" s="40"/>
-      <c r="B23" s="41"/>
-      <c r="C23" s="42"/>
-      <c r="D23" s="42"/>
-      <c r="E23" s="42"/>
-      <c r="F23" s="42"/>
-      <c r="G23" s="42"/>
-      <c r="H23" s="42"/>
-      <c r="I23" s="42"/>
-      <c r="J23" s="42"/>
-      <c r="K23" s="42"/>
-      <c r="L23" s="42"/>
+      <c r="A23" s="34"/>
+      <c r="B23" s="35"/>
+      <c r="C23" s="36"/>
+      <c r="D23" s="36"/>
+      <c r="E23" s="36"/>
+      <c r="F23" s="36"/>
+      <c r="G23" s="36"/>
+      <c r="H23" s="36"/>
+      <c r="I23" s="36"/>
+      <c r="J23" s="36"/>
+      <c r="K23" s="36"/>
+      <c r="L23" s="36"/>
     </row>
     <row r="24" spans="1:13">
-      <c r="A24" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="B24" s="45"/>
-      <c r="C24" s="7"/>
+      <c r="A24" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" s="38"/>
+      <c r="C24" s="8"/>
       <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
+      <c r="E24" s="8"/>
       <c r="F24" s="6"/>
       <c r="G24" s="7"/>
       <c r="H24" s="4"/>
@@ -1872,13 +1876,13 @@
       <c r="L24" s="4"/>
     </row>
     <row r="25" spans="1:13">
-      <c r="A25" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="B25" s="29" t="s">
+      <c r="A25" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="C25" s="27"/>
+      <c r="C25" s="23"/>
       <c r="D25" s="8"/>
       <c r="E25" s="8"/>
       <c r="F25" s="6"/>
@@ -1890,217 +1894,219 @@
       <c r="L25" s="7"/>
     </row>
     <row r="26" spans="1:13" ht="4.5" customHeight="1" thickBot="1">
-      <c r="A26" s="40"/>
-      <c r="B26" s="41"/>
-      <c r="C26" s="42"/>
-      <c r="D26" s="42"/>
-      <c r="E26" s="42"/>
-      <c r="F26" s="42"/>
-      <c r="G26" s="42"/>
-      <c r="H26" s="42"/>
-      <c r="I26" s="42"/>
-      <c r="J26" s="42"/>
-      <c r="K26" s="42"/>
-      <c r="L26" s="42"/>
+      <c r="A26" s="34"/>
+      <c r="B26" s="35"/>
+      <c r="C26" s="36"/>
+      <c r="D26" s="36"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="36"/>
+      <c r="G26" s="36"/>
+      <c r="H26" s="36"/>
+      <c r="I26" s="36"/>
+      <c r="J26" s="36"/>
+      <c r="K26" s="36"/>
+      <c r="L26" s="36"/>
     </row>
     <row r="27" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A27" s="28"/>
-      <c r="B27" s="30"/>
-      <c r="C27" s="22" t="s">
+      <c r="A27" s="24"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="23"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="23"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="22" t="s">
+      <c r="D27" s="46"/>
+      <c r="E27" s="46"/>
+      <c r="F27" s="46"/>
+      <c r="G27" s="47"/>
+      <c r="H27" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="I27" s="23"/>
-      <c r="J27" s="70"/>
-      <c r="K27" s="24"/>
-      <c r="L27" s="25" t="s">
+      <c r="I27" s="46"/>
+      <c r="J27" s="48"/>
+      <c r="K27" s="47"/>
+      <c r="L27" s="21" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A28" s="62" t="s">
+      <c r="A28" s="65" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="63"/>
-      <c r="C28" s="46"/>
-      <c r="D28" s="47"/>
-      <c r="E28" s="47"/>
-      <c r="F28" s="47"/>
-      <c r="G28" s="48"/>
-      <c r="H28" s="46"/>
-      <c r="I28" s="47"/>
-      <c r="J28" s="47"/>
-      <c r="K28" s="48"/>
-      <c r="L28" s="53"/>
+      <c r="B28" s="66"/>
+      <c r="C28" s="49"/>
+      <c r="D28" s="50"/>
+      <c r="E28" s="50"/>
+      <c r="F28" s="50"/>
+      <c r="G28" s="51"/>
+      <c r="H28" s="49"/>
+      <c r="I28" s="50"/>
+      <c r="J28" s="50"/>
+      <c r="K28" s="51"/>
+      <c r="L28" s="40"/>
     </row>
     <row r="29" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A29" s="62" t="s">
-        <v>65</v>
-      </c>
-      <c r="B29" s="63"/>
-      <c r="C29" s="71"/>
-      <c r="D29" s="72"/>
-      <c r="E29" s="72"/>
-      <c r="F29" s="72"/>
-      <c r="G29" s="73"/>
-      <c r="H29" s="46"/>
-      <c r="I29" s="47"/>
-      <c r="J29" s="47"/>
-      <c r="K29" s="48"/>
+      <c r="A29" s="65" t="s">
+        <v>63</v>
+      </c>
+      <c r="B29" s="66"/>
+      <c r="C29" s="69"/>
+      <c r="D29" s="70"/>
+      <c r="E29" s="70"/>
+      <c r="F29" s="70"/>
+      <c r="G29" s="71"/>
+      <c r="H29" s="49"/>
+      <c r="I29" s="50"/>
+      <c r="J29" s="50"/>
+      <c r="K29" s="51"/>
     </row>
     <row r="30" spans="1:13" ht="4.5" customHeight="1">
-      <c r="A30" s="40"/>
-      <c r="B30" s="41"/>
-      <c r="C30" s="42"/>
-      <c r="D30" s="42"/>
-      <c r="E30" s="42"/>
-      <c r="F30" s="42"/>
-      <c r="G30" s="42"/>
-      <c r="H30" s="42"/>
-      <c r="I30" s="42"/>
-      <c r="J30" s="42"/>
-      <c r="K30" s="42"/>
-      <c r="L30" s="42"/>
+      <c r="A30" s="34"/>
+      <c r="B30" s="35"/>
+      <c r="C30" s="36"/>
+      <c r="D30" s="36"/>
+      <c r="E30" s="36"/>
+      <c r="F30" s="36"/>
+      <c r="G30" s="36"/>
+      <c r="H30" s="36"/>
+      <c r="I30" s="36"/>
+      <c r="J30" s="36"/>
+      <c r="K30" s="36"/>
+      <c r="L30" s="36"/>
     </row>
     <row r="31" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A31" s="64" t="s">
-        <v>43</v>
-      </c>
-      <c r="B31" s="65"/>
-      <c r="C31" s="66"/>
-      <c r="D31" s="67"/>
-      <c r="E31" s="67"/>
-      <c r="F31" s="67"/>
-      <c r="G31" s="68"/>
-      <c r="H31" s="69"/>
-      <c r="I31" s="67"/>
-      <c r="J31" s="67"/>
-      <c r="K31" s="68"/>
-      <c r="L31" s="26" t="s">
+      <c r="A31" s="62" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31" s="63"/>
+      <c r="C31" s="58"/>
+      <c r="D31" s="59"/>
+      <c r="E31" s="59"/>
+      <c r="F31" s="59"/>
+      <c r="G31" s="60"/>
+      <c r="H31" s="61"/>
+      <c r="I31" s="59"/>
+      <c r="J31" s="59"/>
+      <c r="K31" s="60"/>
+      <c r="L31" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="M31" s="50"/>
+      <c r="M31" s="39"/>
     </row>
     <row r="32" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A32" s="64" t="s">
-        <v>40</v>
-      </c>
-      <c r="B32" s="65"/>
-      <c r="C32" s="58"/>
-      <c r="D32" s="59"/>
-      <c r="E32" s="59"/>
-      <c r="F32" s="59"/>
-      <c r="G32" s="60"/>
-      <c r="H32" s="71" t="s">
-        <v>45</v>
-      </c>
-      <c r="I32" s="72"/>
-      <c r="J32" s="72"/>
-      <c r="K32" s="72"/>
-      <c r="L32" s="73"/>
-      <c r="M32" s="50"/>
-    </row>
-    <row r="33" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A33" s="64" t="s">
+      <c r="A32" s="62" t="s">
+        <v>67</v>
+      </c>
+      <c r="B32" s="63"/>
+      <c r="C32" s="78"/>
+      <c r="D32" s="79"/>
+      <c r="E32" s="79"/>
+      <c r="F32" s="79"/>
+      <c r="G32" s="80"/>
+      <c r="H32" s="69" t="s">
+        <v>66</v>
+      </c>
+      <c r="I32" s="70"/>
+      <c r="J32" s="70"/>
+      <c r="K32" s="70"/>
+      <c r="L32" s="71"/>
+      <c r="M32" s="39"/>
+    </row>
+    <row r="33" spans="1:13" ht="30.75" customHeight="1" thickBot="1">
+      <c r="A33" s="67" t="s">
         <v>37</v>
       </c>
-      <c r="B33" s="65"/>
-      <c r="C33" s="46"/>
-      <c r="D33" s="47"/>
-      <c r="E33" s="47"/>
-      <c r="F33" s="47"/>
-      <c r="G33" s="48"/>
-      <c r="H33" s="51"/>
-      <c r="I33" s="52"/>
-      <c r="J33" s="52"/>
+      <c r="B33" s="68"/>
+      <c r="C33" s="55" t="s">
+        <v>68</v>
+      </c>
+      <c r="D33" s="56"/>
+      <c r="E33" s="56"/>
+      <c r="F33" s="56"/>
+      <c r="G33" s="57"/>
+      <c r="H33" s="52"/>
+      <c r="I33" s="53"/>
+      <c r="J33" s="53"/>
       <c r="K33" s="54"/>
-      <c r="M33" s="50"/>
+      <c r="M33" s="39"/>
     </row>
     <row r="34" spans="1:13" ht="4.5" customHeight="1" thickBot="1">
-      <c r="A34" s="40"/>
-      <c r="B34" s="41"/>
-      <c r="C34" s="42"/>
-      <c r="D34" s="42"/>
-      <c r="E34" s="42"/>
-      <c r="F34" s="42"/>
-      <c r="G34" s="42"/>
-      <c r="H34" s="42"/>
-      <c r="I34" s="42"/>
-      <c r="J34" s="42"/>
-      <c r="K34" s="42"/>
+      <c r="A34" s="34"/>
+      <c r="B34" s="35"/>
+      <c r="C34" s="36"/>
+      <c r="D34" s="36"/>
+      <c r="E34" s="36"/>
+      <c r="F34" s="36"/>
+      <c r="G34" s="36"/>
+      <c r="H34" s="36"/>
+      <c r="I34" s="36"/>
+      <c r="J34" s="36"/>
+      <c r="K34" s="36"/>
     </row>
     <row r="35" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A35" s="64" t="s">
+      <c r="A35" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="65"/>
-      <c r="C35" s="46"/>
-      <c r="D35" s="47"/>
-      <c r="E35" s="47"/>
-      <c r="F35" s="47"/>
-      <c r="G35" s="48"/>
-      <c r="H35" s="46"/>
-      <c r="I35" s="47"/>
-      <c r="J35" s="47"/>
-      <c r="K35" s="48"/>
-      <c r="M35" s="50"/>
+      <c r="B35" s="63"/>
+      <c r="C35" s="49"/>
+      <c r="D35" s="50"/>
+      <c r="E35" s="50"/>
+      <c r="F35" s="50"/>
+      <c r="G35" s="51"/>
+      <c r="H35" s="49"/>
+      <c r="I35" s="50"/>
+      <c r="J35" s="50"/>
+      <c r="K35" s="51"/>
+      <c r="M35" s="39"/>
     </row>
     <row r="36" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A36" s="64" t="s">
+      <c r="A36" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="65"/>
-      <c r="C36" s="46"/>
-      <c r="D36" s="47"/>
-      <c r="E36" s="47"/>
-      <c r="F36" s="47"/>
-      <c r="G36" s="48"/>
-      <c r="H36" s="46"/>
-      <c r="I36" s="47"/>
-      <c r="J36" s="47"/>
-      <c r="K36" s="48"/>
-      <c r="M36" s="50"/>
+      <c r="B36" s="63"/>
+      <c r="C36" s="49"/>
+      <c r="D36" s="50"/>
+      <c r="E36" s="50"/>
+      <c r="F36" s="50"/>
+      <c r="G36" s="51"/>
+      <c r="H36" s="49"/>
+      <c r="I36" s="50"/>
+      <c r="J36" s="50"/>
+      <c r="K36" s="51"/>
+      <c r="M36" s="39"/>
     </row>
     <row r="37" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A37" s="64" t="s">
+      <c r="A37" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="B37" s="65"/>
-      <c r="C37" s="46"/>
-      <c r="D37" s="47"/>
-      <c r="E37" s="47"/>
-      <c r="F37" s="47"/>
-      <c r="G37" s="48"/>
-      <c r="H37" s="46"/>
-      <c r="I37" s="47"/>
-      <c r="J37" s="47"/>
-      <c r="K37" s="48"/>
-      <c r="M37" s="50"/>
+      <c r="B37" s="63"/>
+      <c r="C37" s="49"/>
+      <c r="D37" s="50"/>
+      <c r="E37" s="50"/>
+      <c r="F37" s="50"/>
+      <c r="G37" s="51"/>
+      <c r="H37" s="49"/>
+      <c r="I37" s="50"/>
+      <c r="J37" s="50"/>
+      <c r="K37" s="51"/>
+      <c r="M37" s="39"/>
     </row>
     <row r="39" spans="1:13">
-      <c r="A39" s="75" t="s">
+      <c r="A39" s="72" t="s">
         <v>27</v>
       </c>
-      <c r="B39" s="49"/>
-      <c r="C39" s="49"/>
-      <c r="D39" s="49"/>
-      <c r="E39" s="49"/>
+      <c r="B39" s="73"/>
+      <c r="C39" s="73"/>
+      <c r="D39" s="73"/>
+      <c r="E39" s="73"/>
     </row>
     <row r="40" spans="1:13">
       <c r="A40" s="14" t="s">
         <v>26</v>
       </c>
       <c r="B40" s="13"/>
-      <c r="C40" s="76" t="s">
+      <c r="C40" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="D40" s="77"/>
+      <c r="D40" s="75"/>
       <c r="E40" s="7"/>
     </row>
     <row r="41" spans="1:13">
@@ -2108,10 +2114,10 @@
         <v>22</v>
       </c>
       <c r="B41" s="5"/>
-      <c r="C41" s="76" t="s">
+      <c r="C41" s="74" t="s">
         <v>24</v>
       </c>
-      <c r="D41" s="77"/>
+      <c r="D41" s="75"/>
       <c r="E41" s="8"/>
     </row>
     <row r="42" spans="1:13">
@@ -2122,173 +2128,173 @@
     </row>
     <row r="43" spans="1:13" ht="15.75" thickBot="1"/>
     <row r="44" spans="1:13">
-      <c r="A44" s="55" t="s">
+      <c r="A44" s="76" t="s">
         <v>38</v>
       </c>
-      <c r="B44" s="56"/>
-      <c r="C44" s="56"/>
-      <c r="D44" s="56"/>
-      <c r="E44" s="56"/>
-      <c r="F44" s="56"/>
-      <c r="G44" s="56"/>
-      <c r="H44" s="56"/>
-      <c r="I44" s="56"/>
-      <c r="J44" s="56"/>
-      <c r="K44" s="56"/>
-      <c r="L44" s="56"/>
+      <c r="B44" s="77"/>
+      <c r="C44" s="77"/>
+      <c r="D44" s="77"/>
+      <c r="E44" s="77"/>
+      <c r="F44" s="77"/>
+      <c r="G44" s="77"/>
+      <c r="H44" s="77"/>
+      <c r="I44" s="77"/>
+      <c r="J44" s="77"/>
+      <c r="K44" s="77"/>
+      <c r="L44" s="77"/>
     </row>
     <row r="45" spans="1:13">
-      <c r="A45" s="57" t="s">
+      <c r="A45" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="B45" s="74" t="s">
+      <c r="B45" s="64" t="s">
+        <v>60</v>
+      </c>
+      <c r="C45" s="64"/>
+      <c r="D45" s="64"/>
+      <c r="E45" s="64"/>
+      <c r="F45" s="64"/>
+      <c r="G45" s="64"/>
+      <c r="H45" s="64"/>
+      <c r="I45" s="64"/>
+      <c r="J45" s="64"/>
+      <c r="K45" s="64"/>
+      <c r="L45" s="64"/>
+    </row>
+    <row r="46" spans="1:13" ht="30" customHeight="1">
+      <c r="A46" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="B46" s="64" t="s">
+        <v>64</v>
+      </c>
+      <c r="C46" s="64"/>
+      <c r="D46" s="64"/>
+      <c r="E46" s="64"/>
+      <c r="F46" s="64"/>
+      <c r="G46" s="64"/>
+      <c r="H46" s="64"/>
+      <c r="I46" s="64"/>
+      <c r="J46" s="64"/>
+      <c r="K46" s="64"/>
+      <c r="L46" s="64"/>
+    </row>
+    <row r="47" spans="1:13" ht="15" customHeight="1">
+      <c r="A47" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="B47" s="64" t="s">
+        <v>61</v>
+      </c>
+      <c r="C47" s="64"/>
+      <c r="D47" s="64"/>
+      <c r="E47" s="64"/>
+      <c r="F47" s="64"/>
+      <c r="G47" s="64"/>
+      <c r="H47" s="64"/>
+      <c r="I47" s="64"/>
+      <c r="J47" s="64"/>
+      <c r="K47" s="64"/>
+      <c r="L47" s="64"/>
+    </row>
+    <row r="48" spans="1:13">
+      <c r="A48" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="B48" s="64" t="s">
         <v>62</v>
       </c>
-      <c r="C45" s="74"/>
-      <c r="D45" s="74"/>
-      <c r="E45" s="74"/>
-      <c r="F45" s="74"/>
-      <c r="G45" s="74"/>
-      <c r="H45" s="74"/>
-      <c r="I45" s="74"/>
-      <c r="J45" s="74"/>
-      <c r="K45" s="74"/>
-      <c r="L45" s="74"/>
-    </row>
-    <row r="46" spans="1:13" ht="30" customHeight="1">
-      <c r="A46" s="57" t="s">
-        <v>32</v>
-      </c>
-      <c r="B46" s="74" t="s">
-        <v>66</v>
-      </c>
-      <c r="C46" s="74"/>
-      <c r="D46" s="74"/>
-      <c r="E46" s="74"/>
-      <c r="F46" s="74"/>
-      <c r="G46" s="74"/>
-      <c r="H46" s="74"/>
-      <c r="I46" s="74"/>
-      <c r="J46" s="74"/>
-      <c r="K46" s="74"/>
-      <c r="L46" s="74"/>
-    </row>
-    <row r="47" spans="1:13" ht="15" customHeight="1">
-      <c r="A47" s="57" t="s">
-        <v>33</v>
-      </c>
-      <c r="B47" s="74" t="s">
-        <v>63</v>
-      </c>
-      <c r="C47" s="74"/>
-      <c r="D47" s="74"/>
-      <c r="E47" s="74"/>
-      <c r="F47" s="74"/>
-      <c r="G47" s="74"/>
-      <c r="H47" s="74"/>
-      <c r="I47" s="74"/>
-      <c r="J47" s="74"/>
-      <c r="K47" s="74"/>
-      <c r="L47" s="74"/>
-    </row>
-    <row r="48" spans="1:13">
-      <c r="A48" s="57" t="s">
-        <v>34</v>
-      </c>
-      <c r="B48" s="74" t="s">
-        <v>64</v>
-      </c>
-      <c r="C48" s="74"/>
-      <c r="D48" s="74"/>
-      <c r="E48" s="74"/>
-      <c r="F48" s="74"/>
-      <c r="G48" s="74"/>
-      <c r="H48" s="74"/>
-      <c r="I48" s="74"/>
-      <c r="J48" s="74"/>
-      <c r="K48" s="74"/>
-      <c r="L48" s="74"/>
+      <c r="C48" s="64"/>
+      <c r="D48" s="64"/>
+      <c r="E48" s="64"/>
+      <c r="F48" s="64"/>
+      <c r="G48" s="64"/>
+      <c r="H48" s="64"/>
+      <c r="I48" s="64"/>
+      <c r="J48" s="64"/>
+      <c r="K48" s="64"/>
+      <c r="L48" s="64"/>
     </row>
     <row r="49" spans="1:12">
-      <c r="A49" s="57" t="s">
+      <c r="A49" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="B49" s="74" t="s">
-        <v>51</v>
-      </c>
-      <c r="C49" s="74"/>
-      <c r="D49" s="74"/>
-      <c r="E49" s="74"/>
-      <c r="F49" s="74"/>
-      <c r="G49" s="74"/>
-      <c r="H49" s="74"/>
-      <c r="I49" s="74"/>
-      <c r="J49" s="74"/>
-      <c r="K49" s="74"/>
-      <c r="L49" s="74"/>
+      <c r="B49" s="64" t="s">
+        <v>49</v>
+      </c>
+      <c r="C49" s="64"/>
+      <c r="D49" s="64"/>
+      <c r="E49" s="64"/>
+      <c r="F49" s="64"/>
+      <c r="G49" s="64"/>
+      <c r="H49" s="64"/>
+      <c r="I49" s="64"/>
+      <c r="J49" s="64"/>
+      <c r="K49" s="64"/>
+      <c r="L49" s="64"/>
     </row>
     <row r="50" spans="1:12">
-      <c r="A50" s="57" t="s">
+      <c r="A50" s="41" t="s">
+        <v>57</v>
+      </c>
+      <c r="B50" s="64" t="s">
+        <v>36</v>
+      </c>
+      <c r="C50" s="64"/>
+      <c r="D50" s="64"/>
+      <c r="E50" s="64"/>
+      <c r="F50" s="64"/>
+      <c r="G50" s="64"/>
+      <c r="H50" s="64"/>
+      <c r="I50" s="64"/>
+      <c r="J50" s="64"/>
+      <c r="K50" s="64"/>
+      <c r="L50" s="64"/>
+    </row>
+    <row r="51" spans="1:12">
+      <c r="A51" s="41" t="s">
+        <v>55</v>
+      </c>
+      <c r="B51" s="64" t="s">
         <v>59</v>
       </c>
-      <c r="B50" s="74" t="s">
-        <v>36</v>
-      </c>
-      <c r="C50" s="74"/>
-      <c r="D50" s="74"/>
-      <c r="E50" s="74"/>
-      <c r="F50" s="74"/>
-      <c r="G50" s="74"/>
-      <c r="H50" s="74"/>
-      <c r="I50" s="74"/>
-      <c r="J50" s="74"/>
-      <c r="K50" s="74"/>
-      <c r="L50" s="74"/>
-    </row>
-    <row r="51" spans="1:12">
-      <c r="A51" s="57" t="s">
-        <v>57</v>
-      </c>
-      <c r="B51" s="74" t="s">
-        <v>61</v>
-      </c>
-      <c r="C51" s="74"/>
-      <c r="D51" s="74"/>
-      <c r="E51" s="74"/>
-      <c r="F51" s="74"/>
-      <c r="G51" s="74"/>
-      <c r="H51" s="74"/>
-      <c r="I51" s="74"/>
-      <c r="J51" s="74"/>
-      <c r="K51" s="74"/>
-      <c r="L51" s="74"/>
+      <c r="C51" s="64"/>
+      <c r="D51" s="64"/>
+      <c r="E51" s="64"/>
+      <c r="F51" s="64"/>
+      <c r="G51" s="64"/>
+      <c r="H51" s="64"/>
+      <c r="I51" s="64"/>
+      <c r="J51" s="64"/>
+      <c r="K51" s="64"/>
+      <c r="L51" s="64"/>
     </row>
     <row r="52" spans="1:12">
-      <c r="A52" s="57" t="s">
+      <c r="A52" s="41" t="s">
+        <v>56</v>
+      </c>
+      <c r="B52" s="64" t="s">
         <v>58</v>
       </c>
-      <c r="B52" s="74" t="s">
-        <v>60</v>
-      </c>
-      <c r="C52" s="74"/>
-      <c r="D52" s="74"/>
-      <c r="E52" s="74"/>
-      <c r="F52" s="74"/>
-      <c r="G52" s="74"/>
-      <c r="H52" s="74"/>
-      <c r="I52" s="74"/>
-      <c r="J52" s="74"/>
-      <c r="K52" s="74"/>
-      <c r="L52" s="74"/>
+      <c r="C52" s="64"/>
+      <c r="D52" s="64"/>
+      <c r="E52" s="64"/>
+      <c r="F52" s="64"/>
+      <c r="G52" s="64"/>
+      <c r="H52" s="64"/>
+      <c r="I52" s="64"/>
+      <c r="J52" s="64"/>
+      <c r="K52" s="64"/>
+      <c r="L52" s="64"/>
     </row>
     <row r="53" spans="1:12">
-      <c r="C53" s="50"/>
+      <c r="C53" s="39"/>
     </row>
     <row r="54" spans="1:12">
-      <c r="C54" s="50"/>
+      <c r="C54" s="39"/>
     </row>
     <row r="55" spans="1:12">
-      <c r="B55" s="50"/>
+      <c r="B55" s="39"/>
     </row>
   </sheetData>
   <sortState ref="A24:K25">
@@ -2306,11 +2312,6 @@
     <mergeCell ref="B45:L45"/>
     <mergeCell ref="C32:G32"/>
     <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
     <mergeCell ref="H32:L32"/>
     <mergeCell ref="A44:L44"/>
     <mergeCell ref="B46:L46"/>
@@ -2321,22 +2322,27 @@
     <mergeCell ref="H35:K35"/>
     <mergeCell ref="H36:K36"/>
     <mergeCell ref="H37:K37"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:B37"/>
     <mergeCell ref="H33:K33"/>
     <mergeCell ref="C33:G33"/>
     <mergeCell ref="C31:G31"/>
     <mergeCell ref="H31:K31"/>
     <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A1:L1"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C27:G27"/>
     <mergeCell ref="H27:K27"/>
     <mergeCell ref="C28:G28"/>
     <mergeCell ref="H28:K28"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
     <mergeCell ref="H3:K3"/>
     <mergeCell ref="C3:G3"/>
-    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A28:B28"/>
   </mergeCells>
   <pageMargins left="0.51" right="0.35" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="89" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
idem HardSkill y Project. Incluido codigo JS para el widget en el componente de HardSkill, uso de regex en el template. Ajuste en modelo Person del backend.
</commit_message>
<xml_diff>
--- a/Cuadro-de-estado.xlsx
+++ b/Cuadro-de-estado.xlsx
@@ -462,7 +462,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -523,6 +523,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="35">
     <border>
@@ -1016,7 +1022,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1069,6 +1074,12 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1105,21 +1116,15 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1141,21 +1146,22 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1456,7 +1462,7 @@
   <dimension ref="A1:M55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32:B32"/>
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1473,40 +1479,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="23.25">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="41" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
-      <c r="K1" s="42"/>
-      <c r="L1" s="42"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
     </row>
     <row r="2" spans="1:12" ht="15.75" thickBot="1"/>
     <row r="3" spans="1:12" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="44"/>
-      <c r="C3" s="45" t="s">
+      <c r="B3" s="43"/>
+      <c r="C3" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="45" t="s">
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="46"/>
-      <c r="J3" s="48"/>
-      <c r="K3" s="47"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="46"/>
       <c r="L3" s="21" t="s">
         <v>4</v>
       </c>
@@ -1550,18 +1556,18 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="4.5" customHeight="1">
-      <c r="A5" s="34"/>
-      <c r="B5" s="35"/>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="36"/>
-      <c r="I5" s="36"/>
-      <c r="J5" s="36"/>
-      <c r="K5" s="36"/>
-      <c r="L5" s="36"/>
+      <c r="A5" s="33"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="35"/>
+      <c r="K5" s="35"/>
+      <c r="L5" s="35"/>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="18" t="s">
@@ -1582,18 +1588,18 @@
       <c r="L6" s="4"/>
     </row>
     <row r="7" spans="1:12" ht="4.5" customHeight="1">
-      <c r="A7" s="34"/>
-      <c r="B7" s="35"/>
-      <c r="C7" s="36"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
-      <c r="G7" s="36"/>
-      <c r="H7" s="36"/>
-      <c r="I7" s="36"/>
-      <c r="J7" s="36"/>
-      <c r="K7" s="36"/>
-      <c r="L7" s="36"/>
+      <c r="A7" s="33"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="35"/>
+      <c r="H7" s="35"/>
+      <c r="I7" s="35"/>
+      <c r="J7" s="35"/>
+      <c r="K7" s="35"/>
+      <c r="L7" s="35"/>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="18" t="s">
@@ -1614,21 +1620,21 @@
       <c r="L8" s="4"/>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" s="32" t="s">
+      <c r="A9" s="31" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="19" t="s">
         <v>13</v>
       </c>
       <c r="C9" s="13"/>
-      <c r="D9" s="5"/>
+      <c r="D9" s="13"/>
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
       <c r="G9" s="7"/>
       <c r="H9" s="13"/>
       <c r="I9" s="13"/>
       <c r="J9" s="4"/>
-      <c r="K9" s="33"/>
+      <c r="K9" s="32"/>
       <c r="L9" s="4"/>
     </row>
     <row r="10" spans="1:12">
@@ -1656,10 +1662,10 @@
       <c r="B11" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="16"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="6"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
       <c r="G11" s="7"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
@@ -1668,21 +1674,21 @@
       <c r="L11" s="4"/>
     </row>
     <row r="12" spans="1:12" ht="4.5" customHeight="1">
-      <c r="A12" s="34"/>
-      <c r="B12" s="35"/>
-      <c r="C12" s="36"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="36"/>
-      <c r="H12" s="36"/>
-      <c r="I12" s="36"/>
-      <c r="J12" s="36"/>
-      <c r="K12" s="36"/>
-      <c r="L12" s="36"/>
+      <c r="A12" s="33"/>
+      <c r="B12" s="34"/>
+      <c r="C12" s="35"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="35"/>
+      <c r="F12" s="35"/>
+      <c r="G12" s="35"/>
+      <c r="H12" s="35"/>
+      <c r="I12" s="35"/>
+      <c r="J12" s="35"/>
+      <c r="K12" s="35"/>
+      <c r="L12" s="35"/>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="80" t="s">
         <v>16</v>
       </c>
       <c r="B13" s="25" t="s">
@@ -1697,10 +1703,10 @@
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
       <c r="K13" s="7"/>
-      <c r="L13" s="37"/>
+      <c r="L13" s="36"/>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="80" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="25" t="s">
@@ -1715,24 +1721,24 @@
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
       <c r="K14" s="7"/>
-      <c r="L14" s="37"/>
+      <c r="L14" s="36"/>
     </row>
     <row r="15" spans="1:12" ht="4.5" customHeight="1">
-      <c r="A15" s="34"/>
-      <c r="B15" s="35"/>
-      <c r="C15" s="36"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="36"/>
-      <c r="I15" s="36"/>
-      <c r="J15" s="36"/>
-      <c r="K15" s="36"/>
-      <c r="L15" s="36"/>
+      <c r="A15" s="33"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="35"/>
+      <c r="I15" s="35"/>
+      <c r="J15" s="35"/>
+      <c r="K15" s="35"/>
+      <c r="L15" s="35"/>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="80" t="s">
         <v>30</v>
       </c>
       <c r="B16" s="20"/>
@@ -1784,7 +1790,7 @@
       <c r="L18" s="4"/>
     </row>
     <row r="19" spans="1:13">
-      <c r="A19" s="18" t="s">
+      <c r="A19" s="80" t="s">
         <v>9</v>
       </c>
       <c r="B19" s="20"/>
@@ -1800,34 +1806,34 @@
       <c r="L19" s="4"/>
     </row>
     <row r="20" spans="1:13">
-      <c r="A20" s="27" t="s">
+      <c r="A20" s="80" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="28"/>
+      <c r="B20" s="27"/>
       <c r="C20" s="8"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="29"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="28"/>
       <c r="F20" s="6"/>
       <c r="G20" s="8"/>
-      <c r="H20" s="30"/>
-      <c r="I20" s="30"/>
+      <c r="H20" s="29"/>
+      <c r="I20" s="29"/>
       <c r="J20" s="4"/>
-      <c r="K20" s="31"/>
+      <c r="K20" s="30"/>
       <c r="L20" s="4"/>
     </row>
     <row r="21" spans="1:13" ht="4.5" customHeight="1">
-      <c r="A21" s="34"/>
-      <c r="B21" s="35"/>
-      <c r="C21" s="36"/>
-      <c r="D21" s="36"/>
-      <c r="E21" s="36"/>
-      <c r="F21" s="36"/>
-      <c r="G21" s="36"/>
-      <c r="H21" s="36"/>
-      <c r="I21" s="36"/>
-      <c r="J21" s="36"/>
-      <c r="K21" s="36"/>
-      <c r="L21" s="36"/>
+      <c r="A21" s="33"/>
+      <c r="B21" s="34"/>
+      <c r="C21" s="35"/>
+      <c r="D21" s="35"/>
+      <c r="E21" s="35"/>
+      <c r="F21" s="35"/>
+      <c r="G21" s="35"/>
+      <c r="H21" s="35"/>
+      <c r="I21" s="35"/>
+      <c r="J21" s="35"/>
+      <c r="K21" s="35"/>
+      <c r="L21" s="35"/>
     </row>
     <row r="22" spans="1:13">
       <c r="A22" s="18" t="s">
@@ -1846,24 +1852,24 @@
       <c r="L22" s="4"/>
     </row>
     <row r="23" spans="1:13" ht="4.5" customHeight="1">
-      <c r="A23" s="34"/>
-      <c r="B23" s="35"/>
-      <c r="C23" s="36"/>
-      <c r="D23" s="36"/>
-      <c r="E23" s="36"/>
-      <c r="F23" s="36"/>
-      <c r="G23" s="36"/>
-      <c r="H23" s="36"/>
-      <c r="I23" s="36"/>
-      <c r="J23" s="36"/>
-      <c r="K23" s="36"/>
-      <c r="L23" s="36"/>
+      <c r="A23" s="33"/>
+      <c r="B23" s="34"/>
+      <c r="C23" s="35"/>
+      <c r="D23" s="35"/>
+      <c r="E23" s="35"/>
+      <c r="F23" s="35"/>
+      <c r="G23" s="35"/>
+      <c r="H23" s="35"/>
+      <c r="I23" s="35"/>
+      <c r="J23" s="35"/>
+      <c r="K23" s="35"/>
+      <c r="L23" s="35"/>
     </row>
     <row r="24" spans="1:13">
       <c r="A24" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="B24" s="38"/>
+      <c r="B24" s="37"/>
       <c r="C24" s="8"/>
       <c r="D24" s="5"/>
       <c r="E24" s="8"/>
@@ -1894,219 +1900,219 @@
       <c r="L25" s="7"/>
     </row>
     <row r="26" spans="1:13" ht="4.5" customHeight="1" thickBot="1">
-      <c r="A26" s="34"/>
-      <c r="B26" s="35"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="36"/>
-      <c r="E26" s="36"/>
-      <c r="F26" s="36"/>
-      <c r="G26" s="36"/>
-      <c r="H26" s="36"/>
-      <c r="I26" s="36"/>
-      <c r="J26" s="36"/>
-      <c r="K26" s="36"/>
-      <c r="L26" s="36"/>
+      <c r="A26" s="33"/>
+      <c r="B26" s="34"/>
+      <c r="C26" s="35"/>
+      <c r="D26" s="35"/>
+      <c r="E26" s="35"/>
+      <c r="F26" s="35"/>
+      <c r="G26" s="35"/>
+      <c r="H26" s="35"/>
+      <c r="I26" s="35"/>
+      <c r="J26" s="35"/>
+      <c r="K26" s="35"/>
+      <c r="L26" s="35"/>
     </row>
     <row r="27" spans="1:13" ht="15.75" thickBot="1">
       <c r="A27" s="24"/>
       <c r="B27" s="26"/>
-      <c r="C27" s="45" t="s">
+      <c r="C27" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="46"/>
-      <c r="E27" s="46"/>
-      <c r="F27" s="46"/>
-      <c r="G27" s="47"/>
-      <c r="H27" s="45" t="s">
+      <c r="D27" s="45"/>
+      <c r="E27" s="45"/>
+      <c r="F27" s="45"/>
+      <c r="G27" s="46"/>
+      <c r="H27" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="I27" s="46"/>
-      <c r="J27" s="48"/>
-      <c r="K27" s="47"/>
+      <c r="I27" s="45"/>
+      <c r="J27" s="47"/>
+      <c r="K27" s="46"/>
       <c r="L27" s="21" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A28" s="65" t="s">
+      <c r="A28" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="66"/>
-      <c r="C28" s="49"/>
-      <c r="D28" s="50"/>
-      <c r="E28" s="50"/>
-      <c r="F28" s="50"/>
-      <c r="G28" s="51"/>
-      <c r="H28" s="49"/>
-      <c r="I28" s="50"/>
-      <c r="J28" s="50"/>
-      <c r="K28" s="51"/>
-      <c r="L28" s="40"/>
+      <c r="B28" s="52"/>
+      <c r="C28" s="48"/>
+      <c r="D28" s="49"/>
+      <c r="E28" s="49"/>
+      <c r="F28" s="49"/>
+      <c r="G28" s="50"/>
+      <c r="H28" s="48"/>
+      <c r="I28" s="49"/>
+      <c r="J28" s="49"/>
+      <c r="K28" s="50"/>
+      <c r="L28" s="39"/>
     </row>
     <row r="29" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A29" s="65" t="s">
+      <c r="A29" s="51" t="s">
         <v>63</v>
       </c>
-      <c r="B29" s="66"/>
-      <c r="C29" s="69"/>
-      <c r="D29" s="70"/>
-      <c r="E29" s="70"/>
-      <c r="F29" s="70"/>
-      <c r="G29" s="71"/>
-      <c r="H29" s="49"/>
-      <c r="I29" s="50"/>
-      <c r="J29" s="50"/>
-      <c r="K29" s="51"/>
+      <c r="B29" s="52"/>
+      <c r="C29" s="68"/>
+      <c r="D29" s="69"/>
+      <c r="E29" s="69"/>
+      <c r="F29" s="69"/>
+      <c r="G29" s="70"/>
+      <c r="H29" s="48"/>
+      <c r="I29" s="49"/>
+      <c r="J29" s="49"/>
+      <c r="K29" s="50"/>
     </row>
     <row r="30" spans="1:13" ht="4.5" customHeight="1">
-      <c r="A30" s="34"/>
-      <c r="B30" s="35"/>
-      <c r="C30" s="36"/>
-      <c r="D30" s="36"/>
-      <c r="E30" s="36"/>
-      <c r="F30" s="36"/>
-      <c r="G30" s="36"/>
-      <c r="H30" s="36"/>
-      <c r="I30" s="36"/>
-      <c r="J30" s="36"/>
-      <c r="K30" s="36"/>
-      <c r="L30" s="36"/>
+      <c r="A30" s="33"/>
+      <c r="B30" s="34"/>
+      <c r="C30" s="35"/>
+      <c r="D30" s="35"/>
+      <c r="E30" s="35"/>
+      <c r="F30" s="35"/>
+      <c r="G30" s="35"/>
+      <c r="H30" s="35"/>
+      <c r="I30" s="35"/>
+      <c r="J30" s="35"/>
+      <c r="K30" s="35"/>
+      <c r="L30" s="35"/>
     </row>
     <row r="31" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A31" s="62" t="s">
+      <c r="A31" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="B31" s="63"/>
-      <c r="C31" s="58"/>
-      <c r="D31" s="59"/>
-      <c r="E31" s="59"/>
-      <c r="F31" s="59"/>
-      <c r="G31" s="60"/>
-      <c r="H31" s="61"/>
-      <c r="I31" s="59"/>
-      <c r="J31" s="59"/>
-      <c r="K31" s="60"/>
+      <c r="B31" s="64"/>
+      <c r="C31" s="59"/>
+      <c r="D31" s="60"/>
+      <c r="E31" s="60"/>
+      <c r="F31" s="60"/>
+      <c r="G31" s="61"/>
+      <c r="H31" s="62"/>
+      <c r="I31" s="60"/>
+      <c r="J31" s="60"/>
+      <c r="K31" s="61"/>
       <c r="L31" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="M31" s="39"/>
+      <c r="M31" s="38"/>
     </row>
     <row r="32" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A32" s="62" t="s">
+      <c r="A32" s="63" t="s">
         <v>67</v>
       </c>
-      <c r="B32" s="63"/>
-      <c r="C32" s="78"/>
-      <c r="D32" s="79"/>
-      <c r="E32" s="79"/>
-      <c r="F32" s="79"/>
-      <c r="G32" s="80"/>
-      <c r="H32" s="69" t="s">
+      <c r="B32" s="64"/>
+      <c r="C32" s="75"/>
+      <c r="D32" s="76"/>
+      <c r="E32" s="76"/>
+      <c r="F32" s="76"/>
+      <c r="G32" s="77"/>
+      <c r="H32" s="68" t="s">
         <v>66</v>
       </c>
-      <c r="I32" s="70"/>
-      <c r="J32" s="70"/>
-      <c r="K32" s="70"/>
-      <c r="L32" s="71"/>
-      <c r="M32" s="39"/>
+      <c r="I32" s="69"/>
+      <c r="J32" s="69"/>
+      <c r="K32" s="69"/>
+      <c r="L32" s="70"/>
+      <c r="M32" s="38"/>
     </row>
     <row r="33" spans="1:13" ht="30.75" customHeight="1" thickBot="1">
-      <c r="A33" s="67" t="s">
+      <c r="A33" s="65" t="s">
         <v>37</v>
       </c>
-      <c r="B33" s="68"/>
-      <c r="C33" s="55" t="s">
+      <c r="B33" s="66"/>
+      <c r="C33" s="56" t="s">
         <v>68</v>
       </c>
-      <c r="D33" s="56"/>
-      <c r="E33" s="56"/>
-      <c r="F33" s="56"/>
-      <c r="G33" s="57"/>
-      <c r="H33" s="52"/>
-      <c r="I33" s="53"/>
-      <c r="J33" s="53"/>
-      <c r="K33" s="54"/>
-      <c r="M33" s="39"/>
+      <c r="D33" s="57"/>
+      <c r="E33" s="57"/>
+      <c r="F33" s="57"/>
+      <c r="G33" s="58"/>
+      <c r="H33" s="53"/>
+      <c r="I33" s="54"/>
+      <c r="J33" s="54"/>
+      <c r="K33" s="55"/>
+      <c r="M33" s="38"/>
     </row>
     <row r="34" spans="1:13" ht="4.5" customHeight="1" thickBot="1">
-      <c r="A34" s="34"/>
-      <c r="B34" s="35"/>
-      <c r="C34" s="36"/>
-      <c r="D34" s="36"/>
-      <c r="E34" s="36"/>
-      <c r="F34" s="36"/>
-      <c r="G34" s="36"/>
-      <c r="H34" s="36"/>
-      <c r="I34" s="36"/>
-      <c r="J34" s="36"/>
-      <c r="K34" s="36"/>
+      <c r="A34" s="33"/>
+      <c r="B34" s="34"/>
+      <c r="C34" s="35"/>
+      <c r="D34" s="35"/>
+      <c r="E34" s="35"/>
+      <c r="F34" s="35"/>
+      <c r="G34" s="35"/>
+      <c r="H34" s="35"/>
+      <c r="I34" s="35"/>
+      <c r="J34" s="35"/>
+      <c r="K34" s="35"/>
     </row>
     <row r="35" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A35" s="62" t="s">
+      <c r="A35" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="63"/>
-      <c r="C35" s="49"/>
-      <c r="D35" s="50"/>
-      <c r="E35" s="50"/>
-      <c r="F35" s="50"/>
-      <c r="G35" s="51"/>
-      <c r="H35" s="49"/>
-      <c r="I35" s="50"/>
-      <c r="J35" s="50"/>
-      <c r="K35" s="51"/>
-      <c r="M35" s="39"/>
+      <c r="B35" s="64"/>
+      <c r="C35" s="48"/>
+      <c r="D35" s="49"/>
+      <c r="E35" s="49"/>
+      <c r="F35" s="49"/>
+      <c r="G35" s="50"/>
+      <c r="H35" s="48"/>
+      <c r="I35" s="49"/>
+      <c r="J35" s="49"/>
+      <c r="K35" s="50"/>
+      <c r="M35" s="38"/>
     </row>
     <row r="36" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A36" s="62" t="s">
+      <c r="A36" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="63"/>
-      <c r="C36" s="49"/>
-      <c r="D36" s="50"/>
-      <c r="E36" s="50"/>
-      <c r="F36" s="50"/>
-      <c r="G36" s="51"/>
-      <c r="H36" s="49"/>
-      <c r="I36" s="50"/>
-      <c r="J36" s="50"/>
-      <c r="K36" s="51"/>
-      <c r="M36" s="39"/>
+      <c r="B36" s="64"/>
+      <c r="C36" s="48"/>
+      <c r="D36" s="49"/>
+      <c r="E36" s="49"/>
+      <c r="F36" s="49"/>
+      <c r="G36" s="50"/>
+      <c r="H36" s="48"/>
+      <c r="I36" s="49"/>
+      <c r="J36" s="49"/>
+      <c r="K36" s="50"/>
+      <c r="M36" s="38"/>
     </row>
     <row r="37" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A37" s="62" t="s">
+      <c r="A37" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="B37" s="63"/>
-      <c r="C37" s="49"/>
-      <c r="D37" s="50"/>
-      <c r="E37" s="50"/>
-      <c r="F37" s="50"/>
-      <c r="G37" s="51"/>
-      <c r="H37" s="49"/>
-      <c r="I37" s="50"/>
-      <c r="J37" s="50"/>
-      <c r="K37" s="51"/>
-      <c r="M37" s="39"/>
+      <c r="B37" s="64"/>
+      <c r="C37" s="48"/>
+      <c r="D37" s="49"/>
+      <c r="E37" s="49"/>
+      <c r="F37" s="49"/>
+      <c r="G37" s="50"/>
+      <c r="H37" s="48"/>
+      <c r="I37" s="49"/>
+      <c r="J37" s="49"/>
+      <c r="K37" s="50"/>
+      <c r="M37" s="38"/>
     </row>
     <row r="39" spans="1:13">
-      <c r="A39" s="72" t="s">
+      <c r="A39" s="71" t="s">
         <v>27</v>
       </c>
-      <c r="B39" s="73"/>
-      <c r="C39" s="73"/>
-      <c r="D39" s="73"/>
-      <c r="E39" s="73"/>
+      <c r="B39" s="72"/>
+      <c r="C39" s="72"/>
+      <c r="D39" s="72"/>
+      <c r="E39" s="72"/>
     </row>
     <row r="40" spans="1:13">
       <c r="A40" s="14" t="s">
         <v>26</v>
       </c>
       <c r="B40" s="13"/>
-      <c r="C40" s="74" t="s">
+      <c r="C40" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="D40" s="75"/>
+      <c r="D40" s="74"/>
       <c r="E40" s="7"/>
     </row>
     <row r="41" spans="1:13">
@@ -2114,10 +2120,10 @@
         <v>22</v>
       </c>
       <c r="B41" s="5"/>
-      <c r="C41" s="74" t="s">
+      <c r="C41" s="73" t="s">
         <v>24</v>
       </c>
-      <c r="D41" s="75"/>
+      <c r="D41" s="74"/>
       <c r="E41" s="8"/>
     </row>
     <row r="42" spans="1:13">
@@ -2128,173 +2134,173 @@
     </row>
     <row r="43" spans="1:13" ht="15.75" thickBot="1"/>
     <row r="44" spans="1:13">
-      <c r="A44" s="76" t="s">
+      <c r="A44" s="78" t="s">
         <v>38</v>
       </c>
-      <c r="B44" s="77"/>
-      <c r="C44" s="77"/>
-      <c r="D44" s="77"/>
-      <c r="E44" s="77"/>
-      <c r="F44" s="77"/>
-      <c r="G44" s="77"/>
-      <c r="H44" s="77"/>
-      <c r="I44" s="77"/>
-      <c r="J44" s="77"/>
-      <c r="K44" s="77"/>
-      <c r="L44" s="77"/>
+      <c r="B44" s="79"/>
+      <c r="C44" s="79"/>
+      <c r="D44" s="79"/>
+      <c r="E44" s="79"/>
+      <c r="F44" s="79"/>
+      <c r="G44" s="79"/>
+      <c r="H44" s="79"/>
+      <c r="I44" s="79"/>
+      <c r="J44" s="79"/>
+      <c r="K44" s="79"/>
+      <c r="L44" s="79"/>
     </row>
     <row r="45" spans="1:13">
-      <c r="A45" s="41" t="s">
+      <c r="A45" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="B45" s="64" t="s">
+      <c r="B45" s="67" t="s">
         <v>60</v>
       </c>
-      <c r="C45" s="64"/>
-      <c r="D45" s="64"/>
-      <c r="E45" s="64"/>
-      <c r="F45" s="64"/>
-      <c r="G45" s="64"/>
-      <c r="H45" s="64"/>
-      <c r="I45" s="64"/>
-      <c r="J45" s="64"/>
-      <c r="K45" s="64"/>
-      <c r="L45" s="64"/>
+      <c r="C45" s="67"/>
+      <c r="D45" s="67"/>
+      <c r="E45" s="67"/>
+      <c r="F45" s="67"/>
+      <c r="G45" s="67"/>
+      <c r="H45" s="67"/>
+      <c r="I45" s="67"/>
+      <c r="J45" s="67"/>
+      <c r="K45" s="67"/>
+      <c r="L45" s="67"/>
     </row>
     <row r="46" spans="1:13" ht="30" customHeight="1">
-      <c r="A46" s="41" t="s">
+      <c r="A46" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="B46" s="64" t="s">
+      <c r="B46" s="67" t="s">
         <v>64</v>
       </c>
-      <c r="C46" s="64"/>
-      <c r="D46" s="64"/>
-      <c r="E46" s="64"/>
-      <c r="F46" s="64"/>
-      <c r="G46" s="64"/>
-      <c r="H46" s="64"/>
-      <c r="I46" s="64"/>
-      <c r="J46" s="64"/>
-      <c r="K46" s="64"/>
-      <c r="L46" s="64"/>
+      <c r="C46" s="67"/>
+      <c r="D46" s="67"/>
+      <c r="E46" s="67"/>
+      <c r="F46" s="67"/>
+      <c r="G46" s="67"/>
+      <c r="H46" s="67"/>
+      <c r="I46" s="67"/>
+      <c r="J46" s="67"/>
+      <c r="K46" s="67"/>
+      <c r="L46" s="67"/>
     </row>
     <row r="47" spans="1:13" ht="15" customHeight="1">
-      <c r="A47" s="41" t="s">
+      <c r="A47" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="B47" s="64" t="s">
+      <c r="B47" s="67" t="s">
         <v>61</v>
       </c>
-      <c r="C47" s="64"/>
-      <c r="D47" s="64"/>
-      <c r="E47" s="64"/>
-      <c r="F47" s="64"/>
-      <c r="G47" s="64"/>
-      <c r="H47" s="64"/>
-      <c r="I47" s="64"/>
-      <c r="J47" s="64"/>
-      <c r="K47" s="64"/>
-      <c r="L47" s="64"/>
+      <c r="C47" s="67"/>
+      <c r="D47" s="67"/>
+      <c r="E47" s="67"/>
+      <c r="F47" s="67"/>
+      <c r="G47" s="67"/>
+      <c r="H47" s="67"/>
+      <c r="I47" s="67"/>
+      <c r="J47" s="67"/>
+      <c r="K47" s="67"/>
+      <c r="L47" s="67"/>
     </row>
     <row r="48" spans="1:13">
-      <c r="A48" s="41" t="s">
+      <c r="A48" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="B48" s="64" t="s">
+      <c r="B48" s="67" t="s">
         <v>62</v>
       </c>
-      <c r="C48" s="64"/>
-      <c r="D48" s="64"/>
-      <c r="E48" s="64"/>
-      <c r="F48" s="64"/>
-      <c r="G48" s="64"/>
-      <c r="H48" s="64"/>
-      <c r="I48" s="64"/>
-      <c r="J48" s="64"/>
-      <c r="K48" s="64"/>
-      <c r="L48" s="64"/>
+      <c r="C48" s="67"/>
+      <c r="D48" s="67"/>
+      <c r="E48" s="67"/>
+      <c r="F48" s="67"/>
+      <c r="G48" s="67"/>
+      <c r="H48" s="67"/>
+      <c r="I48" s="67"/>
+      <c r="J48" s="67"/>
+      <c r="K48" s="67"/>
+      <c r="L48" s="67"/>
     </row>
     <row r="49" spans="1:12">
-      <c r="A49" s="41" t="s">
+      <c r="A49" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="B49" s="64" t="s">
+      <c r="B49" s="67" t="s">
         <v>49</v>
       </c>
-      <c r="C49" s="64"/>
-      <c r="D49" s="64"/>
-      <c r="E49" s="64"/>
-      <c r="F49" s="64"/>
-      <c r="G49" s="64"/>
-      <c r="H49" s="64"/>
-      <c r="I49" s="64"/>
-      <c r="J49" s="64"/>
-      <c r="K49" s="64"/>
-      <c r="L49" s="64"/>
+      <c r="C49" s="67"/>
+      <c r="D49" s="67"/>
+      <c r="E49" s="67"/>
+      <c r="F49" s="67"/>
+      <c r="G49" s="67"/>
+      <c r="H49" s="67"/>
+      <c r="I49" s="67"/>
+      <c r="J49" s="67"/>
+      <c r="K49" s="67"/>
+      <c r="L49" s="67"/>
     </row>
     <row r="50" spans="1:12">
-      <c r="A50" s="41" t="s">
+      <c r="A50" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="B50" s="64" t="s">
+      <c r="B50" s="67" t="s">
         <v>36</v>
       </c>
-      <c r="C50" s="64"/>
-      <c r="D50" s="64"/>
-      <c r="E50" s="64"/>
-      <c r="F50" s="64"/>
-      <c r="G50" s="64"/>
-      <c r="H50" s="64"/>
-      <c r="I50" s="64"/>
-      <c r="J50" s="64"/>
-      <c r="K50" s="64"/>
-      <c r="L50" s="64"/>
+      <c r="C50" s="67"/>
+      <c r="D50" s="67"/>
+      <c r="E50" s="67"/>
+      <c r="F50" s="67"/>
+      <c r="G50" s="67"/>
+      <c r="H50" s="67"/>
+      <c r="I50" s="67"/>
+      <c r="J50" s="67"/>
+      <c r="K50" s="67"/>
+      <c r="L50" s="67"/>
     </row>
     <row r="51" spans="1:12">
-      <c r="A51" s="41" t="s">
+      <c r="A51" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="B51" s="64" t="s">
+      <c r="B51" s="67" t="s">
         <v>59</v>
       </c>
-      <c r="C51" s="64"/>
-      <c r="D51" s="64"/>
-      <c r="E51" s="64"/>
-      <c r="F51" s="64"/>
-      <c r="G51" s="64"/>
-      <c r="H51" s="64"/>
-      <c r="I51" s="64"/>
-      <c r="J51" s="64"/>
-      <c r="K51" s="64"/>
-      <c r="L51" s="64"/>
+      <c r="C51" s="67"/>
+      <c r="D51" s="67"/>
+      <c r="E51" s="67"/>
+      <c r="F51" s="67"/>
+      <c r="G51" s="67"/>
+      <c r="H51" s="67"/>
+      <c r="I51" s="67"/>
+      <c r="J51" s="67"/>
+      <c r="K51" s="67"/>
+      <c r="L51" s="67"/>
     </row>
     <row r="52" spans="1:12">
-      <c r="A52" s="41" t="s">
+      <c r="A52" s="40" t="s">
         <v>56</v>
       </c>
-      <c r="B52" s="64" t="s">
+      <c r="B52" s="67" t="s">
         <v>58</v>
       </c>
-      <c r="C52" s="64"/>
-      <c r="D52" s="64"/>
-      <c r="E52" s="64"/>
-      <c r="F52" s="64"/>
-      <c r="G52" s="64"/>
-      <c r="H52" s="64"/>
-      <c r="I52" s="64"/>
-      <c r="J52" s="64"/>
-      <c r="K52" s="64"/>
-      <c r="L52" s="64"/>
+      <c r="C52" s="67"/>
+      <c r="D52" s="67"/>
+      <c r="E52" s="67"/>
+      <c r="F52" s="67"/>
+      <c r="G52" s="67"/>
+      <c r="H52" s="67"/>
+      <c r="I52" s="67"/>
+      <c r="J52" s="67"/>
+      <c r="K52" s="67"/>
+      <c r="L52" s="67"/>
     </row>
     <row r="53" spans="1:12">
-      <c r="C53" s="39"/>
+      <c r="C53" s="38"/>
     </row>
     <row r="54" spans="1:12">
-      <c r="C54" s="39"/>
+      <c r="C54" s="38"/>
     </row>
     <row r="55" spans="1:12">
-      <c r="B55" s="39"/>
+      <c r="B55" s="38"/>
     </row>
   </sheetData>
   <sortState ref="A24:K25">

</xml_diff>

<commit_message>
Interest, Hardskill, Softskill funcionalidad, estilo, formulario con validacion -completo y comprobada la persistencia en la DB
</commit_message>
<xml_diff>
--- a/Cuadro-de-estado.xlsx
+++ b/Cuadro-de-estado.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="70">
   <si>
     <t>BACKEND</t>
   </si>
@@ -114,9 +114,6 @@
     <t>DESPLIEGUE</t>
   </si>
   <si>
-    <t>(1)</t>
-  </si>
-  <si>
     <t>(2)</t>
   </si>
   <si>
@@ -136,9 +133,6 @@
   </si>
   <si>
     <t>(0)</t>
-  </si>
-  <si>
-    <t>Valida-cion Inputs</t>
   </si>
   <si>
     <r>
@@ -211,22 +205,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>Data Convert Object</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(1)</t>
-    </r>
-  </si>
-  <si>
     <t>Integri- dad(4)</t>
   </si>
   <si>
@@ -304,12 +282,6 @@
     <t>Funcionando en localHost, se obtienen los JSON y se actualiza en la Base de Datos</t>
   </si>
   <si>
-    <t>ANULAR EndPoint usados en Test</t>
-  </si>
-  <si>
-    <t>Por cambios en el DER y nombres de atributos, debo crear clases para compatibilizar Modelos BackEnd con Clases FrontEnd. Creo que es mejor que multiples cambios en el codigo de las vistas.</t>
-  </si>
-  <si>
     <t>ESTADO DEL PROYECTO Y ORDEN PARA AVANZAR</t>
   </si>
   <si>
@@ -320,13 +292,31 @@
   </si>
   <si>
     <t>Reutilizar componentes (p.e atributos de person, skills, etc.) Modules, componentes para pruebas</t>
+  </si>
+  <si>
+    <t>Captura de Excepciones</t>
+  </si>
+  <si>
+    <t>Valida-cion FORM's</t>
+  </si>
+  <si>
+    <t>@Column(unique = true)</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/15372654/uniqueconstraint-and-columnunique-true-in-hibernate-annotation</t>
+  </si>
+  <si>
+    <t>Match Back Object</t>
+  </si>
+  <si>
+    <t>Valor agregado</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="18">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -461,8 +451,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12.65"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -529,8 +548,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="35">
+  <borders count="34">
     <border>
       <left/>
       <right/>
@@ -752,15 +777,6 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -961,10 +977,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -998,14 +1018,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1015,20 +1035,20 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1036,7 +1056,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1044,13 +1064,22 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1062,7 +1091,7 @@
     <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1074,10 +1103,10 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1089,42 +1118,78 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1134,36 +1199,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1459,10 +1503,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M55"/>
+  <dimension ref="A1:P54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1478,46 +1522,46 @@
     <col min="10" max="12" width="7.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="23.25">
-      <c r="A1" s="41" t="s">
-        <v>65</v>
-      </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="41"/>
-    </row>
-    <row r="2" spans="1:12" ht="15.75" thickBot="1"/>
-    <row r="3" spans="1:12" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="42" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3" s="43"/>
-      <c r="C3" s="44" t="s">
+    <row r="1" spans="1:16" ht="23.25">
+      <c r="A1" s="46" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+    </row>
+    <row r="2" spans="1:16" ht="15.75" thickBot="1"/>
+    <row r="3" spans="1:16" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1">
+      <c r="A3" s="47" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="48"/>
+      <c r="C3" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="44" t="s">
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="45"/>
-      <c r="J3" s="47"/>
-      <c r="K3" s="46"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="52"/>
+      <c r="K3" s="51"/>
       <c r="L3" s="21" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="3" customFormat="1" ht="40.5" customHeight="1" thickBot="1">
+    <row r="4" spans="1:16" s="3" customFormat="1" ht="40.5" customHeight="1" thickBot="1">
       <c r="A4" s="17" t="s">
         <v>29</v>
       </c>
@@ -1525,37 +1569,43 @@
         <v>21</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>3</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>40</v>
+        <v>68</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="H4" s="9" t="s">
         <v>1</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="J4" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="K4" s="11" t="s">
         <v>43</v>
-      </c>
-      <c r="K4" s="11" t="s">
-        <v>46</v>
       </c>
       <c r="L4" s="12" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" ht="4.5" customHeight="1">
+      <c r="N4" s="42" t="s">
+        <v>66</v>
+      </c>
+      <c r="P4" s="43" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="4.5" customHeight="1">
       <c r="A5" s="33"/>
       <c r="B5" s="34"/>
       <c r="C5" s="35"/>
@@ -1569,7 +1619,7 @@
       <c r="K5" s="35"/>
       <c r="L5" s="35"/>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:16">
       <c r="A6" s="18" t="s">
         <v>15</v>
       </c>
@@ -1578,8 +1628,8 @@
       </c>
       <c r="C6" s="16"/>
       <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
@@ -1587,7 +1637,7 @@
       <c r="K6" s="7"/>
       <c r="L6" s="4"/>
     </row>
-    <row r="7" spans="1:12" ht="4.5" customHeight="1">
+    <row r="7" spans="1:16" ht="4.5" customHeight="1">
       <c r="A7" s="33"/>
       <c r="B7" s="34"/>
       <c r="C7" s="35"/>
@@ -1601,7 +1651,7 @@
       <c r="K7" s="35"/>
       <c r="L7" s="35"/>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:16">
       <c r="A8" s="18" t="s">
         <v>11</v>
       </c>
@@ -1619,7 +1669,7 @@
       <c r="K8" s="7"/>
       <c r="L8" s="4"/>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:16">
       <c r="A9" s="31" t="s">
         <v>10</v>
       </c>
@@ -1637,7 +1687,7 @@
       <c r="K9" s="32"/>
       <c r="L9" s="4"/>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:16">
       <c r="A10" s="18" t="s">
         <v>20</v>
       </c>
@@ -1645,7 +1695,7 @@
         <v>13</v>
       </c>
       <c r="C10" s="13"/>
-      <c r="D10" s="5"/>
+      <c r="D10" s="13"/>
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
       <c r="G10" s="7"/>
@@ -1655,7 +1705,7 @@
       <c r="K10" s="7"/>
       <c r="L10" s="4"/>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:16">
       <c r="A11" s="18" t="s">
         <v>17</v>
       </c>
@@ -1665,7 +1715,7 @@
       <c r="C11" s="13"/>
       <c r="D11" s="5"/>
       <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
+      <c r="F11" s="7"/>
       <c r="G11" s="7"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
@@ -1673,7 +1723,7 @@
       <c r="K11" s="7"/>
       <c r="L11" s="4"/>
     </row>
-    <row r="12" spans="1:12" ht="4.5" customHeight="1">
+    <row r="12" spans="1:16" ht="4.5" customHeight="1">
       <c r="A12" s="33"/>
       <c r="B12" s="34"/>
       <c r="C12" s="35"/>
@@ -1687,8 +1737,8 @@
       <c r="K12" s="35"/>
       <c r="L12" s="35"/>
     </row>
-    <row r="13" spans="1:12">
-      <c r="A13" s="80" t="s">
+    <row r="13" spans="1:16">
+      <c r="A13" s="41" t="s">
         <v>16</v>
       </c>
       <c r="B13" s="25" t="s">
@@ -1696,17 +1746,17 @@
       </c>
       <c r="C13" s="16"/>
       <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="8"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="7"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
       <c r="K13" s="7"/>
       <c r="L13" s="36"/>
     </row>
-    <row r="14" spans="1:12">
-      <c r="A14" s="80" t="s">
+    <row r="14" spans="1:16">
+      <c r="A14" s="41" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="25" t="s">
@@ -1714,16 +1764,16 @@
       </c>
       <c r="C14" s="16"/>
       <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="8"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="7"/>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
       <c r="K14" s="7"/>
       <c r="L14" s="36"/>
     </row>
-    <row r="15" spans="1:12" ht="4.5" customHeight="1">
+    <row r="15" spans="1:16" ht="4.5" customHeight="1">
       <c r="A15" s="33"/>
       <c r="B15" s="34"/>
       <c r="C15" s="35"/>
@@ -1737,16 +1787,16 @@
       <c r="K15" s="35"/>
       <c r="L15" s="35"/>
     </row>
-    <row r="16" spans="1:12">
-      <c r="A16" s="80" t="s">
+    <row r="16" spans="1:16">
+      <c r="A16" s="41" t="s">
         <v>30</v>
       </c>
       <c r="B16" s="20"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="8"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="7"/>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
@@ -1755,16 +1805,16 @@
     </row>
     <row r="17" spans="1:13">
       <c r="A17" s="18" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B17" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C17" s="16"/>
       <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="8"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="7"/>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
@@ -1773,16 +1823,16 @@
     </row>
     <row r="18" spans="1:13">
       <c r="A18" s="18" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B18" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C18" s="16"/>
       <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="8"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="7"/>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
@@ -1790,15 +1840,15 @@
       <c r="L18" s="4"/>
     </row>
     <row r="19" spans="1:13">
-      <c r="A19" s="80" t="s">
+      <c r="A19" s="41" t="s">
         <v>9</v>
       </c>
       <c r="B19" s="20"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="8"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="7"/>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
@@ -1806,15 +1856,15 @@
       <c r="L19" s="4"/>
     </row>
     <row r="20" spans="1:13">
-      <c r="A20" s="80" t="s">
+      <c r="A20" s="41" t="s">
         <v>18</v>
       </c>
       <c r="B20" s="27"/>
       <c r="C20" s="8"/>
       <c r="D20" s="28"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="8"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="7"/>
       <c r="H20" s="29"/>
       <c r="I20" s="29"/>
       <c r="J20" s="4"/>
@@ -1837,13 +1887,13 @@
     </row>
     <row r="22" spans="1:13">
       <c r="A22" s="18" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B22" s="20"/>
       <c r="C22" s="16"/>
       <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="8"/>
       <c r="G22" s="7"/>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
@@ -1867,13 +1917,13 @@
     </row>
     <row r="24" spans="1:13">
       <c r="A24" s="18" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B24" s="37"/>
       <c r="C24" s="8"/>
       <c r="D24" s="5"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="8"/>
       <c r="G24" s="7"/>
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
@@ -1883,15 +1933,15 @@
     </row>
     <row r="25" spans="1:13">
       <c r="A25" s="18" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B25" s="25" t="s">
         <v>13</v>
       </c>
       <c r="C25" s="23"/>
       <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="8"/>
       <c r="G25" s="8"/>
       <c r="H25" s="7"/>
       <c r="I25" s="7"/>
@@ -1916,214 +1966,216 @@
     <row r="27" spans="1:13" ht="15.75" thickBot="1">
       <c r="A27" s="24"/>
       <c r="B27" s="26"/>
-      <c r="C27" s="44" t="s">
+      <c r="C27" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="45"/>
-      <c r="E27" s="45"/>
-      <c r="F27" s="45"/>
-      <c r="G27" s="46"/>
-      <c r="H27" s="44" t="s">
+      <c r="D27" s="50"/>
+      <c r="E27" s="50"/>
+      <c r="F27" s="50"/>
+      <c r="G27" s="51"/>
+      <c r="H27" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="I27" s="45"/>
-      <c r="J27" s="47"/>
-      <c r="K27" s="46"/>
+      <c r="I27" s="50"/>
+      <c r="J27" s="52"/>
+      <c r="K27" s="51"/>
       <c r="L27" s="21" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A28" s="51" t="s">
+      <c r="A28" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="52"/>
-      <c r="C28" s="48"/>
-      <c r="D28" s="49"/>
-      <c r="E28" s="49"/>
-      <c r="F28" s="49"/>
-      <c r="G28" s="50"/>
-      <c r="H28" s="48"/>
-      <c r="I28" s="49"/>
-      <c r="J28" s="49"/>
-      <c r="K28" s="50"/>
+      <c r="B28" s="57"/>
+      <c r="C28" s="53"/>
+      <c r="D28" s="54"/>
+      <c r="E28" s="54"/>
+      <c r="F28" s="54"/>
+      <c r="G28" s="55"/>
+      <c r="H28" s="53"/>
+      <c r="I28" s="54"/>
+      <c r="J28" s="54"/>
+      <c r="K28" s="55"/>
       <c r="L28" s="39"/>
     </row>
-    <row r="29" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A29" s="51" t="s">
+    <row r="29" spans="1:13" ht="4.5" customHeight="1">
+      <c r="A29" s="33"/>
+      <c r="B29" s="34"/>
+      <c r="C29" s="35"/>
+      <c r="D29" s="35"/>
+      <c r="E29" s="35"/>
+      <c r="F29" s="35"/>
+      <c r="G29" s="35"/>
+      <c r="H29" s="35"/>
+      <c r="I29" s="35"/>
+      <c r="J29" s="35"/>
+      <c r="K29" s="35"/>
+      <c r="L29" s="35"/>
+    </row>
+    <row r="30" spans="1:13" ht="15.75" thickBot="1">
+      <c r="A30" s="68" t="s">
+        <v>40</v>
+      </c>
+      <c r="B30" s="69"/>
+      <c r="C30" s="64"/>
+      <c r="D30" s="65"/>
+      <c r="E30" s="65"/>
+      <c r="F30" s="65"/>
+      <c r="G30" s="66"/>
+      <c r="H30" s="67"/>
+      <c r="I30" s="65"/>
+      <c r="J30" s="65"/>
+      <c r="K30" s="66"/>
+      <c r="L30" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="M30" s="38"/>
+    </row>
+    <row r="31" spans="1:13" ht="15.75" thickBot="1">
+      <c r="A31" s="68" t="s">
+        <v>62</v>
+      </c>
+      <c r="B31" s="69"/>
+      <c r="C31" s="75"/>
+      <c r="D31" s="76"/>
+      <c r="E31" s="76"/>
+      <c r="F31" s="76"/>
+      <c r="G31" s="77"/>
+      <c r="H31" s="85" t="s">
+        <v>61</v>
+      </c>
+      <c r="I31" s="86"/>
+      <c r="J31" s="86"/>
+      <c r="K31" s="86"/>
+      <c r="L31" s="87"/>
+      <c r="M31" s="38"/>
+    </row>
+    <row r="32" spans="1:13" ht="16.5" thickBot="1">
+      <c r="A32" s="72" t="s">
+        <v>64</v>
+      </c>
+      <c r="B32" s="73"/>
+      <c r="C32" s="64"/>
+      <c r="D32" s="65"/>
+      <c r="E32" s="65"/>
+      <c r="F32" s="65"/>
+      <c r="G32" s="66"/>
+      <c r="H32" s="67"/>
+      <c r="I32" s="65"/>
+      <c r="J32" s="65"/>
+      <c r="K32" s="66"/>
+      <c r="M32" s="38"/>
+    </row>
+    <row r="33" spans="1:13" ht="30.75" customHeight="1" thickBot="1">
+      <c r="A33" s="70" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" s="71"/>
+      <c r="C33" s="61" t="s">
         <v>63</v>
       </c>
-      <c r="B29" s="52"/>
-      <c r="C29" s="68"/>
-      <c r="D29" s="69"/>
-      <c r="E29" s="69"/>
-      <c r="F29" s="69"/>
-      <c r="G29" s="70"/>
-      <c r="H29" s="48"/>
-      <c r="I29" s="49"/>
-      <c r="J29" s="49"/>
-      <c r="K29" s="50"/>
-    </row>
-    <row r="30" spans="1:13" ht="4.5" customHeight="1">
-      <c r="A30" s="33"/>
-      <c r="B30" s="34"/>
-      <c r="C30" s="35"/>
-      <c r="D30" s="35"/>
-      <c r="E30" s="35"/>
-      <c r="F30" s="35"/>
-      <c r="G30" s="35"/>
-      <c r="H30" s="35"/>
-      <c r="I30" s="35"/>
-      <c r="J30" s="35"/>
-      <c r="K30" s="35"/>
-      <c r="L30" s="35"/>
-    </row>
-    <row r="31" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A31" s="63" t="s">
-        <v>42</v>
-      </c>
-      <c r="B31" s="64"/>
-      <c r="C31" s="59"/>
-      <c r="D31" s="60"/>
-      <c r="E31" s="60"/>
-      <c r="F31" s="60"/>
-      <c r="G31" s="61"/>
-      <c r="H31" s="62"/>
-      <c r="I31" s="60"/>
-      <c r="J31" s="60"/>
-      <c r="K31" s="61"/>
-      <c r="L31" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="M31" s="38"/>
-    </row>
-    <row r="32" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A32" s="63" t="s">
-        <v>67</v>
-      </c>
-      <c r="B32" s="64"/>
-      <c r="C32" s="75"/>
-      <c r="D32" s="76"/>
-      <c r="E32" s="76"/>
-      <c r="F32" s="76"/>
-      <c r="G32" s="77"/>
-      <c r="H32" s="68" t="s">
-        <v>66</v>
-      </c>
-      <c r="I32" s="69"/>
-      <c r="J32" s="69"/>
-      <c r="K32" s="69"/>
-      <c r="L32" s="70"/>
-      <c r="M32" s="38"/>
-    </row>
-    <row r="33" spans="1:13" ht="30.75" customHeight="1" thickBot="1">
-      <c r="A33" s="65" t="s">
-        <v>37</v>
-      </c>
-      <c r="B33" s="66"/>
-      <c r="C33" s="56" t="s">
-        <v>68</v>
-      </c>
-      <c r="D33" s="57"/>
-      <c r="E33" s="57"/>
-      <c r="F33" s="57"/>
-      <c r="G33" s="58"/>
-      <c r="H33" s="53"/>
-      <c r="I33" s="54"/>
-      <c r="J33" s="54"/>
-      <c r="K33" s="55"/>
+      <c r="D33" s="62"/>
+      <c r="E33" s="62"/>
+      <c r="F33" s="62"/>
+      <c r="G33" s="63"/>
+      <c r="H33" s="58"/>
+      <c r="I33" s="59"/>
+      <c r="J33" s="59"/>
+      <c r="K33" s="60"/>
       <c r="M33" s="38"/>
     </row>
     <row r="34" spans="1:13" ht="4.5" customHeight="1" thickBot="1">
       <c r="A34" s="33"/>
       <c r="B34" s="34"/>
-      <c r="C34" s="35"/>
-      <c r="D34" s="35"/>
-      <c r="E34" s="35"/>
-      <c r="F34" s="35"/>
-      <c r="G34" s="35"/>
+      <c r="C34" s="44"/>
+      <c r="D34" s="44"/>
+      <c r="E34" s="44"/>
+      <c r="F34" s="44"/>
+      <c r="G34" s="44"/>
       <c r="H34" s="35"/>
       <c r="I34" s="35"/>
       <c r="J34" s="35"/>
       <c r="K34" s="35"/>
     </row>
     <row r="35" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A35" s="63" t="s">
+      <c r="A35" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="64"/>
-      <c r="C35" s="48"/>
-      <c r="D35" s="49"/>
-      <c r="E35" s="49"/>
-      <c r="F35" s="49"/>
-      <c r="G35" s="50"/>
-      <c r="H35" s="48"/>
-      <c r="I35" s="49"/>
-      <c r="J35" s="49"/>
-      <c r="K35" s="50"/>
+      <c r="B35" s="69"/>
+      <c r="C35" s="75"/>
+      <c r="D35" s="76"/>
+      <c r="E35" s="76"/>
+      <c r="F35" s="76"/>
+      <c r="G35" s="77"/>
+      <c r="H35" s="75"/>
+      <c r="I35" s="76"/>
+      <c r="J35" s="76"/>
+      <c r="K35" s="77"/>
       <c r="M35" s="38"/>
     </row>
     <row r="36" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A36" s="63" t="s">
+      <c r="A36" s="68" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="64"/>
-      <c r="C36" s="48"/>
-      <c r="D36" s="49"/>
-      <c r="E36" s="49"/>
-      <c r="F36" s="49"/>
-      <c r="G36" s="50"/>
-      <c r="H36" s="48"/>
-      <c r="I36" s="49"/>
-      <c r="J36" s="49"/>
-      <c r="K36" s="50"/>
+      <c r="B36" s="69"/>
+      <c r="C36" s="75"/>
+      <c r="D36" s="76"/>
+      <c r="E36" s="76"/>
+      <c r="F36" s="76"/>
+      <c r="G36" s="77"/>
+      <c r="H36" s="75"/>
+      <c r="I36" s="76"/>
+      <c r="J36" s="76"/>
+      <c r="K36" s="77"/>
       <c r="M36" s="38"/>
     </row>
     <row r="37" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A37" s="63" t="s">
+      <c r="A37" s="68" t="s">
         <v>8</v>
       </c>
-      <c r="B37" s="64"/>
-      <c r="C37" s="48"/>
-      <c r="D37" s="49"/>
-      <c r="E37" s="49"/>
-      <c r="F37" s="49"/>
-      <c r="G37" s="50"/>
-      <c r="H37" s="48"/>
-      <c r="I37" s="49"/>
-      <c r="J37" s="49"/>
-      <c r="K37" s="50"/>
+      <c r="B37" s="69"/>
+      <c r="C37" s="75"/>
+      <c r="D37" s="76"/>
+      <c r="E37" s="76"/>
+      <c r="F37" s="76"/>
+      <c r="G37" s="77"/>
+      <c r="H37" s="75"/>
+      <c r="I37" s="76"/>
+      <c r="J37" s="76"/>
+      <c r="K37" s="77"/>
       <c r="M37" s="38"/>
     </row>
-    <row r="39" spans="1:13">
-      <c r="A39" s="71" t="s">
+    <row r="38" spans="1:13" ht="15.75" thickBot="1"/>
+    <row r="39" spans="1:13" ht="15.75" thickBot="1">
+      <c r="A39" s="80" t="s">
         <v>27</v>
       </c>
-      <c r="B39" s="72"/>
-      <c r="C39" s="72"/>
-      <c r="D39" s="72"/>
-      <c r="E39" s="72"/>
+      <c r="B39" s="81"/>
+      <c r="C39" s="81"/>
+      <c r="D39" s="81"/>
+      <c r="E39" s="82"/>
     </row>
     <row r="40" spans="1:13">
       <c r="A40" s="14" t="s">
         <v>26</v>
       </c>
       <c r="B40" s="13"/>
-      <c r="C40" s="73" t="s">
+      <c r="C40" s="83" t="s">
         <v>23</v>
       </c>
-      <c r="D40" s="74"/>
-      <c r="E40" s="7"/>
+      <c r="D40" s="84"/>
+      <c r="E40" s="32"/>
     </row>
     <row r="41" spans="1:13">
       <c r="A41" s="15" t="s">
         <v>22</v>
       </c>
       <c r="B41" s="5"/>
-      <c r="C41" s="73" t="s">
+      <c r="C41" s="83" t="s">
         <v>24</v>
       </c>
-      <c r="D41" s="74"/>
+      <c r="D41" s="84"/>
       <c r="E41" s="8"/>
     </row>
     <row r="42" spans="1:13">
@@ -2131,200 +2183,180 @@
         <v>25</v>
       </c>
       <c r="B42" s="6"/>
+      <c r="C42" s="78" t="s">
+        <v>69</v>
+      </c>
+      <c r="D42" s="79"/>
+      <c r="E42" s="45"/>
     </row>
     <row r="43" spans="1:13" ht="15.75" thickBot="1"/>
     <row r="44" spans="1:13">
-      <c r="A44" s="78" t="s">
-        <v>38</v>
-      </c>
-      <c r="B44" s="79"/>
-      <c r="C44" s="79"/>
-      <c r="D44" s="79"/>
-      <c r="E44" s="79"/>
-      <c r="F44" s="79"/>
-      <c r="G44" s="79"/>
-      <c r="H44" s="79"/>
-      <c r="I44" s="79"/>
-      <c r="J44" s="79"/>
-      <c r="K44" s="79"/>
-      <c r="L44" s="79"/>
+      <c r="A44" s="88" t="s">
+        <v>37</v>
+      </c>
+      <c r="B44" s="89"/>
+      <c r="C44" s="89"/>
+      <c r="D44" s="89"/>
+      <c r="E44" s="89"/>
+      <c r="F44" s="89"/>
+      <c r="G44" s="89"/>
+      <c r="H44" s="89"/>
+      <c r="I44" s="89"/>
+      <c r="J44" s="89"/>
+      <c r="K44" s="89"/>
+      <c r="L44" s="89"/>
     </row>
     <row r="45" spans="1:13">
       <c r="A45" s="40" t="s">
-        <v>39</v>
-      </c>
-      <c r="B45" s="67" t="s">
-        <v>60</v>
-      </c>
-      <c r="C45" s="67"/>
-      <c r="D45" s="67"/>
-      <c r="E45" s="67"/>
-      <c r="F45" s="67"/>
-      <c r="G45" s="67"/>
-      <c r="H45" s="67"/>
-      <c r="I45" s="67"/>
-      <c r="J45" s="67"/>
-      <c r="K45" s="67"/>
-      <c r="L45" s="67"/>
-    </row>
-    <row r="46" spans="1:13" ht="30" customHeight="1">
+        <v>38</v>
+      </c>
+      <c r="B45" s="74" t="s">
+        <v>57</v>
+      </c>
+      <c r="C45" s="74"/>
+      <c r="D45" s="74"/>
+      <c r="E45" s="74"/>
+      <c r="F45" s="74"/>
+      <c r="G45" s="74"/>
+      <c r="H45" s="74"/>
+      <c r="I45" s="74"/>
+      <c r="J45" s="74"/>
+      <c r="K45" s="74"/>
+      <c r="L45" s="74"/>
+    </row>
+    <row r="46" spans="1:13" ht="15" customHeight="1">
       <c r="A46" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="B46" s="67" t="s">
-        <v>64</v>
-      </c>
-      <c r="C46" s="67"/>
-      <c r="D46" s="67"/>
-      <c r="E46" s="67"/>
-      <c r="F46" s="67"/>
-      <c r="G46" s="67"/>
-      <c r="H46" s="67"/>
-      <c r="I46" s="67"/>
-      <c r="J46" s="67"/>
-      <c r="K46" s="67"/>
-      <c r="L46" s="67"/>
-    </row>
-    <row r="47" spans="1:13" ht="15" customHeight="1">
+      <c r="B46" s="74" t="s">
+        <v>58</v>
+      </c>
+      <c r="C46" s="74"/>
+      <c r="D46" s="74"/>
+      <c r="E46" s="74"/>
+      <c r="F46" s="74"/>
+      <c r="G46" s="74"/>
+      <c r="H46" s="74"/>
+      <c r="I46" s="74"/>
+      <c r="J46" s="74"/>
+      <c r="K46" s="74"/>
+      <c r="L46" s="74"/>
+    </row>
+    <row r="47" spans="1:13">
       <c r="A47" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="B47" s="67" t="s">
-        <v>61</v>
-      </c>
-      <c r="C47" s="67"/>
-      <c r="D47" s="67"/>
-      <c r="E47" s="67"/>
-      <c r="F47" s="67"/>
-      <c r="G47" s="67"/>
-      <c r="H47" s="67"/>
-      <c r="I47" s="67"/>
-      <c r="J47" s="67"/>
-      <c r="K47" s="67"/>
-      <c r="L47" s="67"/>
+      <c r="B47" s="74" t="s">
+        <v>59</v>
+      </c>
+      <c r="C47" s="74"/>
+      <c r="D47" s="74"/>
+      <c r="E47" s="74"/>
+      <c r="F47" s="74"/>
+      <c r="G47" s="74"/>
+      <c r="H47" s="74"/>
+      <c r="I47" s="74"/>
+      <c r="J47" s="74"/>
+      <c r="K47" s="74"/>
+      <c r="L47" s="74"/>
     </row>
     <row r="48" spans="1:13">
       <c r="A48" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="B48" s="67" t="s">
-        <v>62</v>
-      </c>
-      <c r="C48" s="67"/>
-      <c r="D48" s="67"/>
-      <c r="E48" s="67"/>
-      <c r="F48" s="67"/>
-      <c r="G48" s="67"/>
-      <c r="H48" s="67"/>
-      <c r="I48" s="67"/>
-      <c r="J48" s="67"/>
-      <c r="K48" s="67"/>
-      <c r="L48" s="67"/>
+      <c r="B48" s="74" t="s">
+        <v>46</v>
+      </c>
+      <c r="C48" s="74"/>
+      <c r="D48" s="74"/>
+      <c r="E48" s="74"/>
+      <c r="F48" s="74"/>
+      <c r="G48" s="74"/>
+      <c r="H48" s="74"/>
+      <c r="I48" s="74"/>
+      <c r="J48" s="74"/>
+      <c r="K48" s="74"/>
+      <c r="L48" s="74"/>
     </row>
     <row r="49" spans="1:12">
       <c r="A49" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="B49" s="74" t="s">
         <v>35</v>
       </c>
-      <c r="B49" s="67" t="s">
-        <v>49</v>
-      </c>
-      <c r="C49" s="67"/>
-      <c r="D49" s="67"/>
-      <c r="E49" s="67"/>
-      <c r="F49" s="67"/>
-      <c r="G49" s="67"/>
-      <c r="H49" s="67"/>
-      <c r="I49" s="67"/>
-      <c r="J49" s="67"/>
-      <c r="K49" s="67"/>
-      <c r="L49" s="67"/>
+      <c r="C49" s="74"/>
+      <c r="D49" s="74"/>
+      <c r="E49" s="74"/>
+      <c r="F49" s="74"/>
+      <c r="G49" s="74"/>
+      <c r="H49" s="74"/>
+      <c r="I49" s="74"/>
+      <c r="J49" s="74"/>
+      <c r="K49" s="74"/>
+      <c r="L49" s="74"/>
     </row>
     <row r="50" spans="1:12">
       <c r="A50" s="40" t="s">
-        <v>57</v>
-      </c>
-      <c r="B50" s="67" t="s">
-        <v>36</v>
-      </c>
-      <c r="C50" s="67"/>
-      <c r="D50" s="67"/>
-      <c r="E50" s="67"/>
-      <c r="F50" s="67"/>
-      <c r="G50" s="67"/>
-      <c r="H50" s="67"/>
-      <c r="I50" s="67"/>
-      <c r="J50" s="67"/>
-      <c r="K50" s="67"/>
-      <c r="L50" s="67"/>
+        <v>52</v>
+      </c>
+      <c r="B50" s="74" t="s">
+        <v>56</v>
+      </c>
+      <c r="C50" s="74"/>
+      <c r="D50" s="74"/>
+      <c r="E50" s="74"/>
+      <c r="F50" s="74"/>
+      <c r="G50" s="74"/>
+      <c r="H50" s="74"/>
+      <c r="I50" s="74"/>
+      <c r="J50" s="74"/>
+      <c r="K50" s="74"/>
+      <c r="L50" s="74"/>
     </row>
     <row r="51" spans="1:12">
       <c r="A51" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="B51" s="74" t="s">
         <v>55</v>
       </c>
-      <c r="B51" s="67" t="s">
-        <v>59</v>
-      </c>
-      <c r="C51" s="67"/>
-      <c r="D51" s="67"/>
-      <c r="E51" s="67"/>
-      <c r="F51" s="67"/>
-      <c r="G51" s="67"/>
-      <c r="H51" s="67"/>
-      <c r="I51" s="67"/>
-      <c r="J51" s="67"/>
-      <c r="K51" s="67"/>
-      <c r="L51" s="67"/>
+      <c r="C51" s="74"/>
+      <c r="D51" s="74"/>
+      <c r="E51" s="74"/>
+      <c r="F51" s="74"/>
+      <c r="G51" s="74"/>
+      <c r="H51" s="74"/>
+      <c r="I51" s="74"/>
+      <c r="J51" s="74"/>
+      <c r="K51" s="74"/>
+      <c r="L51" s="74"/>
     </row>
     <row r="52" spans="1:12">
-      <c r="A52" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="B52" s="67" t="s">
-        <v>58</v>
-      </c>
-      <c r="C52" s="67"/>
-      <c r="D52" s="67"/>
-      <c r="E52" s="67"/>
-      <c r="F52" s="67"/>
-      <c r="G52" s="67"/>
-      <c r="H52" s="67"/>
-      <c r="I52" s="67"/>
-      <c r="J52" s="67"/>
-      <c r="K52" s="67"/>
-      <c r="L52" s="67"/>
+      <c r="C52" s="38"/>
     </row>
     <row r="53" spans="1:12">
       <c r="C53" s="38"/>
     </row>
     <row r="54" spans="1:12">
-      <c r="C54" s="38"/>
-    </row>
-    <row r="55" spans="1:12">
-      <c r="B55" s="38"/>
+      <c r="B54" s="38"/>
     </row>
   </sheetData>
   <sortState ref="A24:K25">
     <sortCondition ref="A3"/>
   </sortState>
   <mergeCells count="42">
+    <mergeCell ref="B50:L50"/>
     <mergeCell ref="B51:L51"/>
-    <mergeCell ref="B52:L52"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="H29:K29"/>
     <mergeCell ref="A39:E39"/>
     <mergeCell ref="C40:D40"/>
     <mergeCell ref="C41:D41"/>
     <mergeCell ref="B45:L45"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="H32:L32"/>
     <mergeCell ref="A44:L44"/>
     <mergeCell ref="B46:L46"/>
     <mergeCell ref="B47:L47"/>
     <mergeCell ref="B48:L48"/>
     <mergeCell ref="B49:L49"/>
-    <mergeCell ref="B50:L50"/>
     <mergeCell ref="H35:K35"/>
     <mergeCell ref="H36:K36"/>
     <mergeCell ref="H37:K37"/>
@@ -2334,12 +2366,19 @@
     <mergeCell ref="A35:B35"/>
     <mergeCell ref="A36:B36"/>
     <mergeCell ref="A37:B37"/>
+    <mergeCell ref="C42:D42"/>
     <mergeCell ref="H33:K33"/>
     <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="H30:K30"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="H32:K32"/>
     <mergeCell ref="C31:G31"/>
-    <mergeCell ref="H31:K31"/>
     <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="H31:L31"/>
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C27:G27"/>
@@ -2350,8 +2389,11 @@
     <mergeCell ref="C3:G3"/>
     <mergeCell ref="A28:B28"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="P4" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.51" right="0.35" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="89" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="89" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Matcheo back front de atributo date de las entidades Project y Person. Tambien se corrigio en el frontend la definicion de los modelos Hardskill, softskill, interest y project , se cambio el atributo userid por [person] que es el que tiene en el backend
</commit_message>
<xml_diff>
--- a/Cuadro-de-estado.xlsx
+++ b/Cuadro-de-estado.xlsx
@@ -1118,6 +1118,60 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1127,54 +1181,9 @@
     <xf numFmtId="0" fontId="21" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1188,15 +1197,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1506,7 +1506,7 @@
   <dimension ref="A1:P54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+      <selection activeCell="N33" sqref="N33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1634,7 +1634,7 @@
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
-      <c r="K6" s="7"/>
+      <c r="K6" s="5"/>
       <c r="L6" s="4"/>
     </row>
     <row r="7" spans="1:16" ht="4.5" customHeight="1">
@@ -1713,9 +1713,9 @@
         <v>13</v>
       </c>
       <c r="C11" s="13"/>
-      <c r="D11" s="5"/>
+      <c r="D11" s="13"/>
       <c r="E11" s="13"/>
-      <c r="F11" s="7"/>
+      <c r="F11" s="13"/>
       <c r="G11" s="7"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
@@ -2014,71 +2014,71 @@
       <c r="L29" s="35"/>
     </row>
     <row r="30" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A30" s="68" t="s">
+      <c r="A30" s="65" t="s">
         <v>40</v>
       </c>
-      <c r="B30" s="69"/>
-      <c r="C30" s="64"/>
-      <c r="D30" s="65"/>
-      <c r="E30" s="65"/>
-      <c r="F30" s="65"/>
-      <c r="G30" s="66"/>
-      <c r="H30" s="67"/>
-      <c r="I30" s="65"/>
-      <c r="J30" s="65"/>
-      <c r="K30" s="66"/>
+      <c r="B30" s="66"/>
+      <c r="C30" s="61"/>
+      <c r="D30" s="62"/>
+      <c r="E30" s="62"/>
+      <c r="F30" s="62"/>
+      <c r="G30" s="63"/>
+      <c r="H30" s="64"/>
+      <c r="I30" s="62"/>
+      <c r="J30" s="62"/>
+      <c r="K30" s="63"/>
       <c r="L30" s="22" t="s">
         <v>5</v>
       </c>
       <c r="M30" s="38"/>
     </row>
     <row r="31" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A31" s="68" t="s">
+      <c r="A31" s="65" t="s">
         <v>62</v>
       </c>
-      <c r="B31" s="69"/>
-      <c r="C31" s="75"/>
-      <c r="D31" s="76"/>
-      <c r="E31" s="76"/>
-      <c r="F31" s="76"/>
-      <c r="G31" s="77"/>
-      <c r="H31" s="85" t="s">
+      <c r="B31" s="66"/>
+      <c r="C31" s="71"/>
+      <c r="D31" s="72"/>
+      <c r="E31" s="72"/>
+      <c r="F31" s="72"/>
+      <c r="G31" s="73"/>
+      <c r="H31" s="74" t="s">
         <v>61</v>
       </c>
-      <c r="I31" s="86"/>
-      <c r="J31" s="86"/>
-      <c r="K31" s="86"/>
-      <c r="L31" s="87"/>
+      <c r="I31" s="75"/>
+      <c r="J31" s="75"/>
+      <c r="K31" s="75"/>
+      <c r="L31" s="76"/>
       <c r="M31" s="38"/>
     </row>
     <row r="32" spans="1:13" ht="16.5" thickBot="1">
-      <c r="A32" s="72" t="s">
+      <c r="A32" s="69" t="s">
         <v>64</v>
       </c>
-      <c r="B32" s="73"/>
-      <c r="C32" s="64"/>
-      <c r="D32" s="65"/>
-      <c r="E32" s="65"/>
-      <c r="F32" s="65"/>
-      <c r="G32" s="66"/>
-      <c r="H32" s="67"/>
-      <c r="I32" s="65"/>
-      <c r="J32" s="65"/>
-      <c r="K32" s="66"/>
+      <c r="B32" s="70"/>
+      <c r="C32" s="61"/>
+      <c r="D32" s="62"/>
+      <c r="E32" s="62"/>
+      <c r="F32" s="62"/>
+      <c r="G32" s="63"/>
+      <c r="H32" s="64"/>
+      <c r="I32" s="62"/>
+      <c r="J32" s="62"/>
+      <c r="K32" s="63"/>
       <c r="M32" s="38"/>
     </row>
     <row r="33" spans="1:13" ht="30.75" customHeight="1" thickBot="1">
-      <c r="A33" s="70" t="s">
+      <c r="A33" s="67" t="s">
         <v>36</v>
       </c>
-      <c r="B33" s="71"/>
-      <c r="C33" s="61" t="s">
+      <c r="B33" s="68"/>
+      <c r="C33" s="79" t="s">
         <v>63</v>
       </c>
-      <c r="D33" s="62"/>
-      <c r="E33" s="62"/>
-      <c r="F33" s="62"/>
-      <c r="G33" s="63"/>
+      <c r="D33" s="80"/>
+      <c r="E33" s="80"/>
+      <c r="F33" s="80"/>
+      <c r="G33" s="81"/>
       <c r="H33" s="58"/>
       <c r="I33" s="59"/>
       <c r="J33" s="59"/>
@@ -2099,72 +2099,72 @@
       <c r="K34" s="35"/>
     </row>
     <row r="35" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A35" s="68" t="s">
+      <c r="A35" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="69"/>
-      <c r="C35" s="75"/>
-      <c r="D35" s="76"/>
-      <c r="E35" s="76"/>
-      <c r="F35" s="76"/>
-      <c r="G35" s="77"/>
-      <c r="H35" s="75"/>
-      <c r="I35" s="76"/>
-      <c r="J35" s="76"/>
-      <c r="K35" s="77"/>
+      <c r="B35" s="66"/>
+      <c r="C35" s="71"/>
+      <c r="D35" s="72"/>
+      <c r="E35" s="72"/>
+      <c r="F35" s="72"/>
+      <c r="G35" s="73"/>
+      <c r="H35" s="71"/>
+      <c r="I35" s="72"/>
+      <c r="J35" s="72"/>
+      <c r="K35" s="73"/>
       <c r="M35" s="38"/>
     </row>
     <row r="36" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A36" s="68" t="s">
+      <c r="A36" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="69"/>
-      <c r="C36" s="75"/>
-      <c r="D36" s="76"/>
-      <c r="E36" s="76"/>
-      <c r="F36" s="76"/>
-      <c r="G36" s="77"/>
-      <c r="H36" s="75"/>
-      <c r="I36" s="76"/>
-      <c r="J36" s="76"/>
-      <c r="K36" s="77"/>
+      <c r="B36" s="66"/>
+      <c r="C36" s="71"/>
+      <c r="D36" s="72"/>
+      <c r="E36" s="72"/>
+      <c r="F36" s="72"/>
+      <c r="G36" s="73"/>
+      <c r="H36" s="71"/>
+      <c r="I36" s="72"/>
+      <c r="J36" s="72"/>
+      <c r="K36" s="73"/>
       <c r="M36" s="38"/>
     </row>
     <row r="37" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A37" s="68" t="s">
+      <c r="A37" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="B37" s="69"/>
-      <c r="C37" s="75"/>
-      <c r="D37" s="76"/>
-      <c r="E37" s="76"/>
-      <c r="F37" s="76"/>
-      <c r="G37" s="77"/>
-      <c r="H37" s="75"/>
-      <c r="I37" s="76"/>
-      <c r="J37" s="76"/>
-      <c r="K37" s="77"/>
+      <c r="B37" s="66"/>
+      <c r="C37" s="71"/>
+      <c r="D37" s="72"/>
+      <c r="E37" s="72"/>
+      <c r="F37" s="72"/>
+      <c r="G37" s="73"/>
+      <c r="H37" s="71"/>
+      <c r="I37" s="72"/>
+      <c r="J37" s="72"/>
+      <c r="K37" s="73"/>
       <c r="M37" s="38"/>
     </row>
     <row r="38" spans="1:13" ht="15.75" thickBot="1"/>
     <row r="39" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A39" s="80" t="s">
+      <c r="A39" s="83" t="s">
         <v>27</v>
       </c>
-      <c r="B39" s="81"/>
-      <c r="C39" s="81"/>
-      <c r="D39" s="81"/>
-      <c r="E39" s="82"/>
+      <c r="B39" s="84"/>
+      <c r="C39" s="84"/>
+      <c r="D39" s="84"/>
+      <c r="E39" s="85"/>
     </row>
     <row r="40" spans="1:13">
       <c r="A40" s="14" t="s">
         <v>26</v>
       </c>
       <c r="B40" s="13"/>
-      <c r="C40" s="83" t="s">
+      <c r="C40" s="86" t="s">
         <v>23</v>
       </c>
-      <c r="D40" s="84"/>
+      <c r="D40" s="87"/>
       <c r="E40" s="32"/>
     </row>
     <row r="41" spans="1:13">
@@ -2172,10 +2172,10 @@
         <v>22</v>
       </c>
       <c r="B41" s="5"/>
-      <c r="C41" s="83" t="s">
+      <c r="C41" s="86" t="s">
         <v>24</v>
       </c>
-      <c r="D41" s="84"/>
+      <c r="D41" s="87"/>
       <c r="E41" s="8"/>
     </row>
     <row r="42" spans="1:13">
@@ -2183,10 +2183,10 @@
         <v>25</v>
       </c>
       <c r="B42" s="6"/>
-      <c r="C42" s="78" t="s">
+      <c r="C42" s="77" t="s">
         <v>69</v>
       </c>
-      <c r="D42" s="79"/>
+      <c r="D42" s="78"/>
       <c r="E42" s="45"/>
     </row>
     <row r="43" spans="1:13" ht="15.75" thickBot="1"/>
@@ -2210,127 +2210,127 @@
       <c r="A45" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="B45" s="74" t="s">
+      <c r="B45" s="82" t="s">
         <v>57</v>
       </c>
-      <c r="C45" s="74"/>
-      <c r="D45" s="74"/>
-      <c r="E45" s="74"/>
-      <c r="F45" s="74"/>
-      <c r="G45" s="74"/>
-      <c r="H45" s="74"/>
-      <c r="I45" s="74"/>
-      <c r="J45" s="74"/>
-      <c r="K45" s="74"/>
-      <c r="L45" s="74"/>
+      <c r="C45" s="82"/>
+      <c r="D45" s="82"/>
+      <c r="E45" s="82"/>
+      <c r="F45" s="82"/>
+      <c r="G45" s="82"/>
+      <c r="H45" s="82"/>
+      <c r="I45" s="82"/>
+      <c r="J45" s="82"/>
+      <c r="K45" s="82"/>
+      <c r="L45" s="82"/>
     </row>
     <row r="46" spans="1:13" ht="15" customHeight="1">
       <c r="A46" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="B46" s="74" t="s">
+      <c r="B46" s="82" t="s">
         <v>58</v>
       </c>
-      <c r="C46" s="74"/>
-      <c r="D46" s="74"/>
-      <c r="E46" s="74"/>
-      <c r="F46" s="74"/>
-      <c r="G46" s="74"/>
-      <c r="H46" s="74"/>
-      <c r="I46" s="74"/>
-      <c r="J46" s="74"/>
-      <c r="K46" s="74"/>
-      <c r="L46" s="74"/>
+      <c r="C46" s="82"/>
+      <c r="D46" s="82"/>
+      <c r="E46" s="82"/>
+      <c r="F46" s="82"/>
+      <c r="G46" s="82"/>
+      <c r="H46" s="82"/>
+      <c r="I46" s="82"/>
+      <c r="J46" s="82"/>
+      <c r="K46" s="82"/>
+      <c r="L46" s="82"/>
     </row>
     <row r="47" spans="1:13">
       <c r="A47" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="B47" s="74" t="s">
+      <c r="B47" s="82" t="s">
         <v>59</v>
       </c>
-      <c r="C47" s="74"/>
-      <c r="D47" s="74"/>
-      <c r="E47" s="74"/>
-      <c r="F47" s="74"/>
-      <c r="G47" s="74"/>
-      <c r="H47" s="74"/>
-      <c r="I47" s="74"/>
-      <c r="J47" s="74"/>
-      <c r="K47" s="74"/>
-      <c r="L47" s="74"/>
+      <c r="C47" s="82"/>
+      <c r="D47" s="82"/>
+      <c r="E47" s="82"/>
+      <c r="F47" s="82"/>
+      <c r="G47" s="82"/>
+      <c r="H47" s="82"/>
+      <c r="I47" s="82"/>
+      <c r="J47" s="82"/>
+      <c r="K47" s="82"/>
+      <c r="L47" s="82"/>
     </row>
     <row r="48" spans="1:13">
       <c r="A48" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="B48" s="74" t="s">
+      <c r="B48" s="82" t="s">
         <v>46</v>
       </c>
-      <c r="C48" s="74"/>
-      <c r="D48" s="74"/>
-      <c r="E48" s="74"/>
-      <c r="F48" s="74"/>
-      <c r="G48" s="74"/>
-      <c r="H48" s="74"/>
-      <c r="I48" s="74"/>
-      <c r="J48" s="74"/>
-      <c r="K48" s="74"/>
-      <c r="L48" s="74"/>
+      <c r="C48" s="82"/>
+      <c r="D48" s="82"/>
+      <c r="E48" s="82"/>
+      <c r="F48" s="82"/>
+      <c r="G48" s="82"/>
+      <c r="H48" s="82"/>
+      <c r="I48" s="82"/>
+      <c r="J48" s="82"/>
+      <c r="K48" s="82"/>
+      <c r="L48" s="82"/>
     </row>
     <row r="49" spans="1:12">
       <c r="A49" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="B49" s="74" t="s">
+      <c r="B49" s="82" t="s">
         <v>35</v>
       </c>
-      <c r="C49" s="74"/>
-      <c r="D49" s="74"/>
-      <c r="E49" s="74"/>
-      <c r="F49" s="74"/>
-      <c r="G49" s="74"/>
-      <c r="H49" s="74"/>
-      <c r="I49" s="74"/>
-      <c r="J49" s="74"/>
-      <c r="K49" s="74"/>
-      <c r="L49" s="74"/>
+      <c r="C49" s="82"/>
+      <c r="D49" s="82"/>
+      <c r="E49" s="82"/>
+      <c r="F49" s="82"/>
+      <c r="G49" s="82"/>
+      <c r="H49" s="82"/>
+      <c r="I49" s="82"/>
+      <c r="J49" s="82"/>
+      <c r="K49" s="82"/>
+      <c r="L49" s="82"/>
     </row>
     <row r="50" spans="1:12">
       <c r="A50" s="40" t="s">
         <v>52</v>
       </c>
-      <c r="B50" s="74" t="s">
+      <c r="B50" s="82" t="s">
         <v>56</v>
       </c>
-      <c r="C50" s="74"/>
-      <c r="D50" s="74"/>
-      <c r="E50" s="74"/>
-      <c r="F50" s="74"/>
-      <c r="G50" s="74"/>
-      <c r="H50" s="74"/>
-      <c r="I50" s="74"/>
-      <c r="J50" s="74"/>
-      <c r="K50" s="74"/>
-      <c r="L50" s="74"/>
+      <c r="C50" s="82"/>
+      <c r="D50" s="82"/>
+      <c r="E50" s="82"/>
+      <c r="F50" s="82"/>
+      <c r="G50" s="82"/>
+      <c r="H50" s="82"/>
+      <c r="I50" s="82"/>
+      <c r="J50" s="82"/>
+      <c r="K50" s="82"/>
+      <c r="L50" s="82"/>
     </row>
     <row r="51" spans="1:12">
       <c r="A51" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="B51" s="74" t="s">
+      <c r="B51" s="82" t="s">
         <v>55</v>
       </c>
-      <c r="C51" s="74"/>
-      <c r="D51" s="74"/>
-      <c r="E51" s="74"/>
-      <c r="F51" s="74"/>
-      <c r="G51" s="74"/>
-      <c r="H51" s="74"/>
-      <c r="I51" s="74"/>
-      <c r="J51" s="74"/>
-      <c r="K51" s="74"/>
-      <c r="L51" s="74"/>
+      <c r="C51" s="82"/>
+      <c r="D51" s="82"/>
+      <c r="E51" s="82"/>
+      <c r="F51" s="82"/>
+      <c r="G51" s="82"/>
+      <c r="H51" s="82"/>
+      <c r="I51" s="82"/>
+      <c r="J51" s="82"/>
+      <c r="K51" s="82"/>
+      <c r="L51" s="82"/>
     </row>
     <row r="52" spans="1:12">
       <c r="C52" s="38"/>
@@ -2357,18 +2357,18 @@
     <mergeCell ref="B47:L47"/>
     <mergeCell ref="B48:L48"/>
     <mergeCell ref="B49:L49"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="H33:K33"/>
+    <mergeCell ref="C33:G33"/>
     <mergeCell ref="H35:K35"/>
     <mergeCell ref="H36:K36"/>
     <mergeCell ref="H37:K37"/>
     <mergeCell ref="C35:G35"/>
     <mergeCell ref="C36:G36"/>
     <mergeCell ref="C37:G37"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="H33:K33"/>
-    <mergeCell ref="C33:G33"/>
     <mergeCell ref="C30:G30"/>
     <mergeCell ref="H30:K30"/>
     <mergeCell ref="A30:B30"/>

</xml_diff>

<commit_message>
funcionalidad y estilo a personal-form, quedan pendientes
</commit_message>
<xml_diff>
--- a/Cuadro-de-estado.xlsx
+++ b/Cuadro-de-estado.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="80">
   <si>
     <t>BACKEND</t>
   </si>
@@ -311,12 +311,42 @@
   <si>
     <t>Valor agregado</t>
   </si>
+  <si>
+    <t>Postergados/Pendientes importantes</t>
+  </si>
+  <si>
+    <t>Upload files</t>
+  </si>
+  <si>
+    <t>https://blog.angular-university.io/angular-file-upload/</t>
+  </si>
+  <si>
+    <t>DatePicker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bootstrap / material ? </t>
+  </si>
+  <si>
+    <t>Layout</t>
+  </si>
+  <si>
+    <t>switch flip/cards</t>
+  </si>
+  <si>
+    <t>Status Cards, Status data personal</t>
+  </si>
+  <si>
+    <t>Validation form</t>
+  </si>
+  <si>
+    <t>Agregar atributo en Person, con la url de ubicación de google.maps</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -480,6 +510,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="13">
     <fill>
@@ -555,7 +593,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="34">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -974,6 +1012,15 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -984,7 +1031,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1073,6 +1120,102 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1109,101 +1252,11 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1503,10 +1556,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P54"/>
+  <dimension ref="A1:T54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="N33" sqref="N33"/>
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1522,46 +1575,46 @@
     <col min="10" max="12" width="7.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="23.25">
-      <c r="A1" s="46" t="s">
+    <row r="1" spans="1:20" ht="23.25">
+      <c r="A1" s="78" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-    </row>
-    <row r="2" spans="1:16" ht="15.75" thickBot="1"/>
-    <row r="3" spans="1:16" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="47" t="s">
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="78"/>
+      <c r="K1" s="78"/>
+      <c r="L1" s="78"/>
+    </row>
+    <row r="2" spans="1:20" ht="15.75" thickBot="1"/>
+    <row r="3" spans="1:20" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1">
+      <c r="A3" s="79" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="48"/>
-      <c r="C3" s="49" t="s">
+      <c r="B3" s="80"/>
+      <c r="C3" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="49" t="s">
+      <c r="D3" s="82"/>
+      <c r="E3" s="82"/>
+      <c r="F3" s="82"/>
+      <c r="G3" s="83"/>
+      <c r="H3" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="50"/>
-      <c r="J3" s="52"/>
-      <c r="K3" s="51"/>
+      <c r="I3" s="82"/>
+      <c r="J3" s="84"/>
+      <c r="K3" s="83"/>
       <c r="L3" s="21" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:16" s="3" customFormat="1" ht="40.5" customHeight="1" thickBot="1">
+    <row r="4" spans="1:20" s="3" customFormat="1" ht="40.5" customHeight="1" thickBot="1">
       <c r="A4" s="17" t="s">
         <v>29</v>
       </c>
@@ -1605,7 +1658,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="4.5" customHeight="1">
+    <row r="5" spans="1:20" ht="4.5" customHeight="1">
       <c r="A5" s="33"/>
       <c r="B5" s="34"/>
       <c r="C5" s="35"/>
@@ -1619,25 +1672,34 @@
       <c r="K5" s="35"/>
       <c r="L5" s="35"/>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:20">
       <c r="A6" s="18" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="7"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
       <c r="E6" s="13"/>
-      <c r="F6" s="7"/>
+      <c r="F6" s="6"/>
       <c r="G6" s="7"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
       <c r="K6" s="5"/>
       <c r="L6" s="4"/>
-    </row>
-    <row r="7" spans="1:16" ht="4.5" customHeight="1">
+      <c r="N6" s="90" t="s">
+        <v>70</v>
+      </c>
+      <c r="O6" s="91"/>
+      <c r="P6" s="91"/>
+      <c r="Q6" s="91"/>
+      <c r="R6" s="91"/>
+      <c r="S6" s="91"/>
+      <c r="T6" s="91"/>
+    </row>
+    <row r="7" spans="1:20" ht="4.5" customHeight="1">
       <c r="A7" s="33"/>
       <c r="B7" s="34"/>
       <c r="C7" s="35"/>
@@ -1651,7 +1713,7 @@
       <c r="K7" s="35"/>
       <c r="L7" s="35"/>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:20">
       <c r="A8" s="18" t="s">
         <v>11</v>
       </c>
@@ -1668,8 +1730,18 @@
       <c r="J8" s="4"/>
       <c r="K8" s="7"/>
       <c r="L8" s="4"/>
-    </row>
-    <row r="9" spans="1:16">
+      <c r="N8" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="O8" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="6"/>
+    </row>
+    <row r="9" spans="1:20">
       <c r="A9" s="31" t="s">
         <v>10</v>
       </c>
@@ -1686,8 +1758,12 @@
       <c r="J9" s="4"/>
       <c r="K9" s="32"/>
       <c r="L9" s="4"/>
-    </row>
-    <row r="10" spans="1:16">
+      <c r="O9" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="P9" s="6"/>
+    </row>
+    <row r="10" spans="1:20">
       <c r="A10" s="18" t="s">
         <v>20</v>
       </c>
@@ -1705,7 +1781,7 @@
       <c r="K10" s="7"/>
       <c r="L10" s="4"/>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:20">
       <c r="A11" s="18" t="s">
         <v>17</v>
       </c>
@@ -1722,8 +1798,14 @@
       <c r="J11" s="4"/>
       <c r="K11" s="7"/>
       <c r="L11" s="4"/>
-    </row>
-    <row r="12" spans="1:16" ht="4.5" customHeight="1">
+      <c r="N11" t="s">
+        <v>73</v>
+      </c>
+      <c r="O11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" ht="4.5" customHeight="1">
       <c r="A12" s="33"/>
       <c r="B12" s="34"/>
       <c r="C12" s="35"/>
@@ -1737,14 +1819,12 @@
       <c r="K12" s="35"/>
       <c r="L12" s="35"/>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:20">
       <c r="A13" s="41" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="16"/>
+        <v>30</v>
+      </c>
+      <c r="B13" s="20"/>
+      <c r="C13" s="8"/>
       <c r="D13" s="8"/>
       <c r="E13" s="6"/>
       <c r="F13" s="8"/>
@@ -1753,14 +1833,14 @@
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
       <c r="K13" s="7"/>
-      <c r="L13" s="36"/>
-    </row>
-    <row r="14" spans="1:16">
-      <c r="A14" s="41" t="s">
-        <v>19</v>
+      <c r="L13" s="4"/>
+    </row>
+    <row r="14" spans="1:20">
+      <c r="A14" s="18" t="s">
+        <v>47</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C14" s="16"/>
       <c r="D14" s="8"/>
@@ -1771,25 +1851,32 @@
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
       <c r="K14" s="7"/>
-      <c r="L14" s="36"/>
-    </row>
-    <row r="15" spans="1:16" ht="4.5" customHeight="1">
-      <c r="A15" s="33"/>
-      <c r="B15" s="34"/>
-      <c r="C15" s="35"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="35"/>
-      <c r="G15" s="35"/>
-      <c r="H15" s="35"/>
-      <c r="I15" s="35"/>
-      <c r="J15" s="35"/>
-      <c r="K15" s="35"/>
-      <c r="L15" s="35"/>
-    </row>
-    <row r="16" spans="1:16">
+      <c r="L14" s="4"/>
+      <c r="N14" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20">
+      <c r="A15" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="16"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="4"/>
+    </row>
+    <row r="16" spans="1:20">
       <c r="A16" s="41" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="B16" s="20"/>
       <c r="C16" s="8"/>
@@ -1802,13 +1889,19 @@
       <c r="J16" s="4"/>
       <c r="K16" s="7"/>
       <c r="L16" s="4"/>
-    </row>
-    <row r="17" spans="1:13">
-      <c r="A17" s="18" t="s">
-        <v>47</v>
+      <c r="N16" t="s">
+        <v>75</v>
+      </c>
+      <c r="O16" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
+      <c r="A17" s="41" t="s">
+        <v>16</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C17" s="16"/>
       <c r="D17" s="8"/>
@@ -1819,14 +1912,17 @@
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
       <c r="K17" s="7"/>
-      <c r="L17" s="4"/>
-    </row>
-    <row r="18" spans="1:13">
-      <c r="A18" s="18" t="s">
-        <v>48</v>
+      <c r="L17" s="36"/>
+      <c r="O17" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
+      <c r="A18" s="41" t="s">
+        <v>19</v>
       </c>
       <c r="B18" s="25" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C18" s="16"/>
       <c r="D18" s="8"/>
@@ -1837,25 +1933,23 @@
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
       <c r="K18" s="7"/>
-      <c r="L18" s="4"/>
-    </row>
-    <row r="19" spans="1:13">
-      <c r="A19" s="41" t="s">
-        <v>9</v>
-      </c>
-      <c r="B19" s="20"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="7"/>
-      <c r="L19" s="4"/>
-    </row>
-    <row r="20" spans="1:13">
+      <c r="L18" s="36"/>
+    </row>
+    <row r="19" spans="1:15" ht="4.5" customHeight="1">
+      <c r="A19" s="33"/>
+      <c r="B19" s="34"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="35"/>
+      <c r="H19" s="35"/>
+      <c r="I19" s="35"/>
+      <c r="J19" s="35"/>
+      <c r="K19" s="35"/>
+      <c r="L19" s="35"/>
+    </row>
+    <row r="20" spans="1:15">
       <c r="A20" s="41" t="s">
         <v>18</v>
       </c>
@@ -1871,7 +1965,7 @@
       <c r="K20" s="30"/>
       <c r="L20" s="4"/>
     </row>
-    <row r="21" spans="1:13" ht="4.5" customHeight="1">
+    <row r="21" spans="1:15" ht="4.5" customHeight="1">
       <c r="A21" s="33"/>
       <c r="B21" s="34"/>
       <c r="C21" s="35"/>
@@ -1885,7 +1979,7 @@
       <c r="K21" s="35"/>
       <c r="L21" s="35"/>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:15">
       <c r="A22" s="18" t="s">
         <v>49</v>
       </c>
@@ -1901,7 +1995,7 @@
       <c r="K22" s="7"/>
       <c r="L22" s="4"/>
     </row>
-    <row r="23" spans="1:13" ht="4.5" customHeight="1">
+    <row r="23" spans="1:15" ht="4.5" customHeight="1">
       <c r="A23" s="33"/>
       <c r="B23" s="34"/>
       <c r="C23" s="35"/>
@@ -1915,7 +2009,7 @@
       <c r="K23" s="35"/>
       <c r="L23" s="35"/>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:15">
       <c r="A24" s="18" t="s">
         <v>50</v>
       </c>
@@ -1931,7 +2025,7 @@
       <c r="K24" s="7"/>
       <c r="L24" s="4"/>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:15">
       <c r="A25" s="18" t="s">
         <v>51</v>
       </c>
@@ -1949,7 +2043,7 @@
       <c r="K25" s="7"/>
       <c r="L25" s="7"/>
     </row>
-    <row r="26" spans="1:13" ht="4.5" customHeight="1" thickBot="1">
+    <row r="26" spans="1:15" ht="4.5" customHeight="1" thickBot="1">
       <c r="A26" s="33"/>
       <c r="B26" s="34"/>
       <c r="C26" s="35"/>
@@ -1963,43 +2057,43 @@
       <c r="K26" s="35"/>
       <c r="L26" s="35"/>
     </row>
-    <row r="27" spans="1:13" ht="15.75" thickBot="1">
+    <row r="27" spans="1:15" ht="15.75" thickBot="1">
       <c r="A27" s="24"/>
       <c r="B27" s="26"/>
-      <c r="C27" s="49" t="s">
+      <c r="C27" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="50"/>
-      <c r="E27" s="50"/>
-      <c r="F27" s="50"/>
-      <c r="G27" s="51"/>
-      <c r="H27" s="49" t="s">
+      <c r="D27" s="82"/>
+      <c r="E27" s="82"/>
+      <c r="F27" s="82"/>
+      <c r="G27" s="83"/>
+      <c r="H27" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="I27" s="50"/>
-      <c r="J27" s="52"/>
-      <c r="K27" s="51"/>
+      <c r="I27" s="82"/>
+      <c r="J27" s="84"/>
+      <c r="K27" s="83"/>
       <c r="L27" s="21" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A28" s="56" t="s">
+    <row r="28" spans="1:15" ht="15.75" thickBot="1">
+      <c r="A28" s="88" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="57"/>
-      <c r="C28" s="53"/>
-      <c r="D28" s="54"/>
-      <c r="E28" s="54"/>
-      <c r="F28" s="54"/>
-      <c r="G28" s="55"/>
-      <c r="H28" s="53"/>
-      <c r="I28" s="54"/>
-      <c r="J28" s="54"/>
-      <c r="K28" s="55"/>
+      <c r="B28" s="89"/>
+      <c r="C28" s="85"/>
+      <c r="D28" s="86"/>
+      <c r="E28" s="86"/>
+      <c r="F28" s="86"/>
+      <c r="G28" s="87"/>
+      <c r="H28" s="85"/>
+      <c r="I28" s="86"/>
+      <c r="J28" s="86"/>
+      <c r="K28" s="87"/>
       <c r="L28" s="39"/>
     </row>
-    <row r="29" spans="1:13" ht="4.5" customHeight="1">
+    <row r="29" spans="1:15" ht="4.5" customHeight="1">
       <c r="A29" s="33"/>
       <c r="B29" s="34"/>
       <c r="C29" s="35"/>
@@ -2013,72 +2107,72 @@
       <c r="K29" s="35"/>
       <c r="L29" s="35"/>
     </row>
-    <row r="30" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A30" s="65" t="s">
+    <row r="30" spans="1:15" ht="15.75" thickBot="1">
+      <c r="A30" s="54" t="s">
         <v>40</v>
       </c>
-      <c r="B30" s="66"/>
-      <c r="C30" s="61"/>
-      <c r="D30" s="62"/>
-      <c r="E30" s="62"/>
-      <c r="F30" s="62"/>
-      <c r="G30" s="63"/>
-      <c r="H30" s="64"/>
-      <c r="I30" s="62"/>
-      <c r="J30" s="62"/>
-      <c r="K30" s="63"/>
+      <c r="B30" s="55"/>
+      <c r="C30" s="67"/>
+      <c r="D30" s="68"/>
+      <c r="E30" s="68"/>
+      <c r="F30" s="68"/>
+      <c r="G30" s="69"/>
+      <c r="H30" s="70"/>
+      <c r="I30" s="68"/>
+      <c r="J30" s="68"/>
+      <c r="K30" s="69"/>
       <c r="L30" s="22" t="s">
         <v>5</v>
       </c>
       <c r="M30" s="38"/>
     </row>
-    <row r="31" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A31" s="65" t="s">
+    <row r="31" spans="1:15" ht="15.75" thickBot="1">
+      <c r="A31" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="B31" s="66"/>
-      <c r="C31" s="71"/>
-      <c r="D31" s="72"/>
-      <c r="E31" s="72"/>
-      <c r="F31" s="72"/>
-      <c r="G31" s="73"/>
-      <c r="H31" s="74" t="s">
+      <c r="B31" s="55"/>
+      <c r="C31" s="64"/>
+      <c r="D31" s="65"/>
+      <c r="E31" s="65"/>
+      <c r="F31" s="65"/>
+      <c r="G31" s="66"/>
+      <c r="H31" s="75" t="s">
         <v>61</v>
       </c>
-      <c r="I31" s="75"/>
-      <c r="J31" s="75"/>
-      <c r="K31" s="75"/>
-      <c r="L31" s="76"/>
+      <c r="I31" s="76"/>
+      <c r="J31" s="76"/>
+      <c r="K31" s="76"/>
+      <c r="L31" s="77"/>
       <c r="M31" s="38"/>
     </row>
-    <row r="32" spans="1:13" ht="16.5" thickBot="1">
-      <c r="A32" s="69" t="s">
+    <row r="32" spans="1:15" ht="16.5" thickBot="1">
+      <c r="A32" s="73" t="s">
         <v>64</v>
       </c>
-      <c r="B32" s="70"/>
-      <c r="C32" s="61"/>
-      <c r="D32" s="62"/>
-      <c r="E32" s="62"/>
-      <c r="F32" s="62"/>
-      <c r="G32" s="63"/>
-      <c r="H32" s="64"/>
-      <c r="I32" s="62"/>
-      <c r="J32" s="62"/>
-      <c r="K32" s="63"/>
+      <c r="B32" s="74"/>
+      <c r="C32" s="67"/>
+      <c r="D32" s="68"/>
+      <c r="E32" s="68"/>
+      <c r="F32" s="68"/>
+      <c r="G32" s="69"/>
+      <c r="H32" s="70"/>
+      <c r="I32" s="68"/>
+      <c r="J32" s="68"/>
+      <c r="K32" s="69"/>
       <c r="M32" s="38"/>
     </row>
     <row r="33" spans="1:13" ht="30.75" customHeight="1" thickBot="1">
-      <c r="A33" s="67" t="s">
+      <c r="A33" s="71" t="s">
         <v>36</v>
       </c>
-      <c r="B33" s="68"/>
-      <c r="C33" s="79" t="s">
+      <c r="B33" s="72"/>
+      <c r="C33" s="61" t="s">
         <v>63</v>
       </c>
-      <c r="D33" s="80"/>
-      <c r="E33" s="80"/>
-      <c r="F33" s="80"/>
-      <c r="G33" s="81"/>
+      <c r="D33" s="62"/>
+      <c r="E33" s="62"/>
+      <c r="F33" s="62"/>
+      <c r="G33" s="63"/>
       <c r="H33" s="58"/>
       <c r="I33" s="59"/>
       <c r="J33" s="59"/>
@@ -2099,72 +2193,72 @@
       <c r="K34" s="35"/>
     </row>
     <row r="35" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A35" s="65" t="s">
+      <c r="A35" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="66"/>
-      <c r="C35" s="71"/>
-      <c r="D35" s="72"/>
-      <c r="E35" s="72"/>
-      <c r="F35" s="72"/>
-      <c r="G35" s="73"/>
-      <c r="H35" s="71"/>
-      <c r="I35" s="72"/>
-      <c r="J35" s="72"/>
-      <c r="K35" s="73"/>
+      <c r="B35" s="55"/>
+      <c r="C35" s="64"/>
+      <c r="D35" s="65"/>
+      <c r="E35" s="65"/>
+      <c r="F35" s="65"/>
+      <c r="G35" s="66"/>
+      <c r="H35" s="64"/>
+      <c r="I35" s="65"/>
+      <c r="J35" s="65"/>
+      <c r="K35" s="66"/>
       <c r="M35" s="38"/>
     </row>
     <row r="36" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A36" s="65" t="s">
+      <c r="A36" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="66"/>
-      <c r="C36" s="71"/>
-      <c r="D36" s="72"/>
-      <c r="E36" s="72"/>
-      <c r="F36" s="72"/>
-      <c r="G36" s="73"/>
-      <c r="H36" s="71"/>
-      <c r="I36" s="72"/>
-      <c r="J36" s="72"/>
-      <c r="K36" s="73"/>
+      <c r="B36" s="55"/>
+      <c r="C36" s="64"/>
+      <c r="D36" s="65"/>
+      <c r="E36" s="65"/>
+      <c r="F36" s="65"/>
+      <c r="G36" s="66"/>
+      <c r="H36" s="64"/>
+      <c r="I36" s="65"/>
+      <c r="J36" s="65"/>
+      <c r="K36" s="66"/>
       <c r="M36" s="38"/>
     </row>
     <row r="37" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A37" s="65" t="s">
+      <c r="A37" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="B37" s="66"/>
-      <c r="C37" s="71"/>
-      <c r="D37" s="72"/>
-      <c r="E37" s="72"/>
-      <c r="F37" s="72"/>
-      <c r="G37" s="73"/>
-      <c r="H37" s="71"/>
-      <c r="I37" s="72"/>
-      <c r="J37" s="72"/>
-      <c r="K37" s="73"/>
+      <c r="B37" s="55"/>
+      <c r="C37" s="64"/>
+      <c r="D37" s="65"/>
+      <c r="E37" s="65"/>
+      <c r="F37" s="65"/>
+      <c r="G37" s="66"/>
+      <c r="H37" s="64"/>
+      <c r="I37" s="65"/>
+      <c r="J37" s="65"/>
+      <c r="K37" s="66"/>
       <c r="M37" s="38"/>
     </row>
     <row r="38" spans="1:13" ht="15.75" thickBot="1"/>
     <row r="39" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A39" s="83" t="s">
+      <c r="A39" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="B39" s="84"/>
-      <c r="C39" s="84"/>
-      <c r="D39" s="84"/>
-      <c r="E39" s="85"/>
+      <c r="B39" s="48"/>
+      <c r="C39" s="48"/>
+      <c r="D39" s="48"/>
+      <c r="E39" s="49"/>
     </row>
     <row r="40" spans="1:13">
       <c r="A40" s="14" t="s">
         <v>26</v>
       </c>
       <c r="B40" s="13"/>
-      <c r="C40" s="86" t="s">
+      <c r="C40" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="D40" s="87"/>
+      <c r="D40" s="51"/>
       <c r="E40" s="32"/>
     </row>
     <row r="41" spans="1:13">
@@ -2172,10 +2266,10 @@
         <v>22</v>
       </c>
       <c r="B41" s="5"/>
-      <c r="C41" s="86" t="s">
+      <c r="C41" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="D41" s="87"/>
+      <c r="D41" s="51"/>
       <c r="E41" s="8"/>
     </row>
     <row r="42" spans="1:13">
@@ -2183,154 +2277,154 @@
         <v>25</v>
       </c>
       <c r="B42" s="6"/>
-      <c r="C42" s="77" t="s">
+      <c r="C42" s="56" t="s">
         <v>69</v>
       </c>
-      <c r="D42" s="78"/>
+      <c r="D42" s="57"/>
       <c r="E42" s="45"/>
     </row>
     <row r="43" spans="1:13" ht="15.75" thickBot="1"/>
     <row r="44" spans="1:13">
-      <c r="A44" s="88" t="s">
+      <c r="A44" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="B44" s="89"/>
-      <c r="C44" s="89"/>
-      <c r="D44" s="89"/>
-      <c r="E44" s="89"/>
-      <c r="F44" s="89"/>
-      <c r="G44" s="89"/>
-      <c r="H44" s="89"/>
-      <c r="I44" s="89"/>
-      <c r="J44" s="89"/>
-      <c r="K44" s="89"/>
-      <c r="L44" s="89"/>
+      <c r="B44" s="53"/>
+      <c r="C44" s="53"/>
+      <c r="D44" s="53"/>
+      <c r="E44" s="53"/>
+      <c r="F44" s="53"/>
+      <c r="G44" s="53"/>
+      <c r="H44" s="53"/>
+      <c r="I44" s="53"/>
+      <c r="J44" s="53"/>
+      <c r="K44" s="53"/>
+      <c r="L44" s="53"/>
     </row>
     <row r="45" spans="1:13">
       <c r="A45" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="B45" s="82" t="s">
+      <c r="B45" s="46" t="s">
         <v>57</v>
       </c>
-      <c r="C45" s="82"/>
-      <c r="D45" s="82"/>
-      <c r="E45" s="82"/>
-      <c r="F45" s="82"/>
-      <c r="G45" s="82"/>
-      <c r="H45" s="82"/>
-      <c r="I45" s="82"/>
-      <c r="J45" s="82"/>
-      <c r="K45" s="82"/>
-      <c r="L45" s="82"/>
+      <c r="C45" s="46"/>
+      <c r="D45" s="46"/>
+      <c r="E45" s="46"/>
+      <c r="F45" s="46"/>
+      <c r="G45" s="46"/>
+      <c r="H45" s="46"/>
+      <c r="I45" s="46"/>
+      <c r="J45" s="46"/>
+      <c r="K45" s="46"/>
+      <c r="L45" s="46"/>
     </row>
     <row r="46" spans="1:13" ht="15" customHeight="1">
       <c r="A46" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="B46" s="82" t="s">
+      <c r="B46" s="46" t="s">
         <v>58</v>
       </c>
-      <c r="C46" s="82"/>
-      <c r="D46" s="82"/>
-      <c r="E46" s="82"/>
-      <c r="F46" s="82"/>
-      <c r="G46" s="82"/>
-      <c r="H46" s="82"/>
-      <c r="I46" s="82"/>
-      <c r="J46" s="82"/>
-      <c r="K46" s="82"/>
-      <c r="L46" s="82"/>
+      <c r="C46" s="46"/>
+      <c r="D46" s="46"/>
+      <c r="E46" s="46"/>
+      <c r="F46" s="46"/>
+      <c r="G46" s="46"/>
+      <c r="H46" s="46"/>
+      <c r="I46" s="46"/>
+      <c r="J46" s="46"/>
+      <c r="K46" s="46"/>
+      <c r="L46" s="46"/>
     </row>
     <row r="47" spans="1:13">
       <c r="A47" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="B47" s="82" t="s">
+      <c r="B47" s="46" t="s">
         <v>59</v>
       </c>
-      <c r="C47" s="82"/>
-      <c r="D47" s="82"/>
-      <c r="E47" s="82"/>
-      <c r="F47" s="82"/>
-      <c r="G47" s="82"/>
-      <c r="H47" s="82"/>
-      <c r="I47" s="82"/>
-      <c r="J47" s="82"/>
-      <c r="K47" s="82"/>
-      <c r="L47" s="82"/>
+      <c r="C47" s="46"/>
+      <c r="D47" s="46"/>
+      <c r="E47" s="46"/>
+      <c r="F47" s="46"/>
+      <c r="G47" s="46"/>
+      <c r="H47" s="46"/>
+      <c r="I47" s="46"/>
+      <c r="J47" s="46"/>
+      <c r="K47" s="46"/>
+      <c r="L47" s="46"/>
     </row>
     <row r="48" spans="1:13">
       <c r="A48" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="B48" s="82" t="s">
+      <c r="B48" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="C48" s="82"/>
-      <c r="D48" s="82"/>
-      <c r="E48" s="82"/>
-      <c r="F48" s="82"/>
-      <c r="G48" s="82"/>
-      <c r="H48" s="82"/>
-      <c r="I48" s="82"/>
-      <c r="J48" s="82"/>
-      <c r="K48" s="82"/>
-      <c r="L48" s="82"/>
+      <c r="C48" s="46"/>
+      <c r="D48" s="46"/>
+      <c r="E48" s="46"/>
+      <c r="F48" s="46"/>
+      <c r="G48" s="46"/>
+      <c r="H48" s="46"/>
+      <c r="I48" s="46"/>
+      <c r="J48" s="46"/>
+      <c r="K48" s="46"/>
+      <c r="L48" s="46"/>
     </row>
     <row r="49" spans="1:12">
       <c r="A49" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="B49" s="82" t="s">
+      <c r="B49" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="C49" s="82"/>
-      <c r="D49" s="82"/>
-      <c r="E49" s="82"/>
-      <c r="F49" s="82"/>
-      <c r="G49" s="82"/>
-      <c r="H49" s="82"/>
-      <c r="I49" s="82"/>
-      <c r="J49" s="82"/>
-      <c r="K49" s="82"/>
-      <c r="L49" s="82"/>
+      <c r="C49" s="46"/>
+      <c r="D49" s="46"/>
+      <c r="E49" s="46"/>
+      <c r="F49" s="46"/>
+      <c r="G49" s="46"/>
+      <c r="H49" s="46"/>
+      <c r="I49" s="46"/>
+      <c r="J49" s="46"/>
+      <c r="K49" s="46"/>
+      <c r="L49" s="46"/>
     </row>
     <row r="50" spans="1:12">
       <c r="A50" s="40" t="s">
         <v>52</v>
       </c>
-      <c r="B50" s="82" t="s">
+      <c r="B50" s="46" t="s">
         <v>56</v>
       </c>
-      <c r="C50" s="82"/>
-      <c r="D50" s="82"/>
-      <c r="E50" s="82"/>
-      <c r="F50" s="82"/>
-      <c r="G50" s="82"/>
-      <c r="H50" s="82"/>
-      <c r="I50" s="82"/>
-      <c r="J50" s="82"/>
-      <c r="K50" s="82"/>
-      <c r="L50" s="82"/>
+      <c r="C50" s="46"/>
+      <c r="D50" s="46"/>
+      <c r="E50" s="46"/>
+      <c r="F50" s="46"/>
+      <c r="G50" s="46"/>
+      <c r="H50" s="46"/>
+      <c r="I50" s="46"/>
+      <c r="J50" s="46"/>
+      <c r="K50" s="46"/>
+      <c r="L50" s="46"/>
     </row>
     <row r="51" spans="1:12">
       <c r="A51" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="B51" s="82" t="s">
+      <c r="B51" s="46" t="s">
         <v>55</v>
       </c>
-      <c r="C51" s="82"/>
-      <c r="D51" s="82"/>
-      <c r="E51" s="82"/>
-      <c r="F51" s="82"/>
-      <c r="G51" s="82"/>
-      <c r="H51" s="82"/>
-      <c r="I51" s="82"/>
-      <c r="J51" s="82"/>
-      <c r="K51" s="82"/>
-      <c r="L51" s="82"/>
+      <c r="C51" s="46"/>
+      <c r="D51" s="46"/>
+      <c r="E51" s="46"/>
+      <c r="F51" s="46"/>
+      <c r="G51" s="46"/>
+      <c r="H51" s="46"/>
+      <c r="I51" s="46"/>
+      <c r="J51" s="46"/>
+      <c r="K51" s="46"/>
+      <c r="L51" s="46"/>
     </row>
     <row r="52" spans="1:12">
       <c r="C52" s="38"/>
@@ -2345,18 +2439,27 @@
   <sortState ref="A24:K25">
     <sortCondition ref="A3"/>
   </sortState>
-  <mergeCells count="42">
-    <mergeCell ref="B50:L50"/>
-    <mergeCell ref="B51:L51"/>
-    <mergeCell ref="A39:E39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="B45:L45"/>
-    <mergeCell ref="A44:L44"/>
-    <mergeCell ref="B46:L46"/>
-    <mergeCell ref="B47:L47"/>
-    <mergeCell ref="B48:L48"/>
-    <mergeCell ref="B49:L49"/>
+  <mergeCells count="43">
+    <mergeCell ref="N6:T6"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="H27:K27"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="H28:K28"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="H30:K30"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="H32:K32"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="H31:L31"/>
     <mergeCell ref="A35:B35"/>
     <mergeCell ref="A36:B36"/>
     <mergeCell ref="A37:B37"/>
@@ -2369,25 +2472,17 @@
     <mergeCell ref="C35:G35"/>
     <mergeCell ref="C36:G36"/>
     <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="H30:K30"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="H32:K32"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="H31:L31"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="H27:K27"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="H28:K28"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="B50:L50"/>
+    <mergeCell ref="B51:L51"/>
+    <mergeCell ref="A39:E39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="B45:L45"/>
+    <mergeCell ref="A44:L44"/>
+    <mergeCell ref="B46:L46"/>
+    <mergeCell ref="B47:L47"/>
+    <mergeCell ref="B48:L48"/>
+    <mergeCell ref="B49:L49"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="P4" r:id="rId1"/>

</xml_diff>

<commit_message>
Iniciando componente Organization, actializando cuadro de estado
</commit_message>
<xml_diff>
--- a/Cuadro-de-estado.xlsx
+++ b/Cuadro-de-estado.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="85">
   <si>
     <t>BACKEND</t>
   </si>
@@ -340,6 +340,21 @@
   </si>
   <si>
     <t>Agregar atributo en Person, con la url de ubicación de google.maps</t>
+  </si>
+  <si>
+    <t>Entity Organization, Degree no tienen filtro por Person</t>
+  </si>
+  <si>
+    <t>La consulta traeria a todas y cualquier modificacion</t>
+  </si>
+  <si>
+    <t>alteraria a todos los Portfolios.</t>
+  </si>
+  <si>
+    <t>Aún existen componentes/servicios que apuntan a mock-data</t>
+  </si>
+  <si>
+    <t>tel, red</t>
   </si>
 </sst>
 </file>
@@ -519,7 +534,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -592,6 +607,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="35">
     <border>
@@ -1093,7 +1114,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1120,6 +1140,120 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1144,120 +1278,7 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1559,7 +1580,7 @@
   <dimension ref="A1:T54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M28" sqref="M28"/>
+      <selection activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1576,40 +1597,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="23.25">
-      <c r="A1" s="78" t="s">
+      <c r="A1" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
-      <c r="J1" s="78"/>
-      <c r="K1" s="78"/>
-      <c r="L1" s="78"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
     </row>
     <row r="2" spans="1:20" ht="15.75" thickBot="1"/>
     <row r="3" spans="1:20" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="79" t="s">
+      <c r="A3" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="80"/>
-      <c r="C3" s="81" t="s">
+      <c r="B3" s="49"/>
+      <c r="C3" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="82"/>
-      <c r="E3" s="82"/>
-      <c r="F3" s="82"/>
-      <c r="G3" s="83"/>
-      <c r="H3" s="81" t="s">
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="82"/>
-      <c r="J3" s="84"/>
-      <c r="K3" s="83"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="52"/>
       <c r="L3" s="21" t="s">
         <v>4</v>
       </c>
@@ -1651,26 +1672,26 @@
       <c r="L4" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="N4" s="42" t="s">
+      <c r="N4" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="P4" s="43" t="s">
+      <c r="P4" s="42" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="4.5" customHeight="1">
-      <c r="A5" s="33"/>
-      <c r="B5" s="34"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35"/>
-      <c r="I5" s="35"/>
-      <c r="J5" s="35"/>
-      <c r="K5" s="35"/>
-      <c r="L5" s="35"/>
+      <c r="A5" s="32"/>
+      <c r="B5" s="33"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="34"/>
+      <c r="I5" s="34"/>
+      <c r="J5" s="34"/>
+      <c r="K5" s="34"/>
+      <c r="L5" s="34"/>
     </row>
     <row r="6" spans="1:20">
       <c r="A6" s="18" t="s">
@@ -1679,7 +1700,9 @@
       <c r="B6" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="6"/>
+      <c r="C6" s="6" t="s">
+        <v>84</v>
+      </c>
       <c r="D6" s="6"/>
       <c r="E6" s="13"/>
       <c r="F6" s="6"/>
@@ -1689,29 +1712,29 @@
       <c r="J6" s="4"/>
       <c r="K6" s="5"/>
       <c r="L6" s="4"/>
-      <c r="N6" s="90" t="s">
+      <c r="N6" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="O6" s="91"/>
-      <c r="P6" s="91"/>
-      <c r="Q6" s="91"/>
-      <c r="R6" s="91"/>
-      <c r="S6" s="91"/>
-      <c r="T6" s="91"/>
+      <c r="O6" s="46"/>
+      <c r="P6" s="46"/>
+      <c r="Q6" s="46"/>
+      <c r="R6" s="46"/>
+      <c r="S6" s="46"/>
+      <c r="T6" s="46"/>
     </row>
     <row r="7" spans="1:20" ht="4.5" customHeight="1">
-      <c r="A7" s="33"/>
-      <c r="B7" s="34"/>
-      <c r="C7" s="35"/>
-      <c r="D7" s="35"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
-      <c r="H7" s="35"/>
-      <c r="I7" s="35"/>
-      <c r="J7" s="35"/>
-      <c r="K7" s="35"/>
-      <c r="L7" s="35"/>
+      <c r="A7" s="32"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="34"/>
+      <c r="J7" s="34"/>
+      <c r="K7" s="34"/>
+      <c r="L7" s="34"/>
     </row>
     <row r="8" spans="1:20">
       <c r="A8" s="18" t="s">
@@ -1742,7 +1765,7 @@
       <c r="S8" s="6"/>
     </row>
     <row r="9" spans="1:20">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="30" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="19" t="s">
@@ -1756,7 +1779,7 @@
       <c r="H9" s="13"/>
       <c r="I9" s="13"/>
       <c r="J9" s="4"/>
-      <c r="K9" s="32"/>
+      <c r="K9" s="31"/>
       <c r="L9" s="4"/>
       <c r="O9" s="6" t="s">
         <v>78</v>
@@ -1806,34 +1829,34 @@
       </c>
     </row>
     <row r="12" spans="1:20" ht="4.5" customHeight="1">
-      <c r="A12" s="33"/>
-      <c r="B12" s="34"/>
-      <c r="C12" s="35"/>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="35"/>
-      <c r="J12" s="35"/>
-      <c r="K12" s="35"/>
-      <c r="L12" s="35"/>
+      <c r="A12" s="32"/>
+      <c r="B12" s="33"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="34"/>
+      <c r="J12" s="34"/>
+      <c r="K12" s="34"/>
+      <c r="L12" s="34"/>
     </row>
     <row r="13" spans="1:20">
-      <c r="A13" s="41" t="s">
+      <c r="A13" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="20"/>
+      <c r="B13" s="6"/>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
       <c r="E13" s="6"/>
       <c r="F13" s="8"/>
       <c r="G13" s="7"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
       <c r="K13" s="7"/>
-      <c r="L13" s="4"/>
+      <c r="L13" s="6"/>
     </row>
     <row r="14" spans="1:20">
       <c r="A14" s="18" t="s">
@@ -1875,20 +1898,20 @@
       <c r="L15" s="4"/>
     </row>
     <row r="16" spans="1:20">
-      <c r="A16" s="41" t="s">
+      <c r="A16" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="20"/>
+      <c r="B16" s="6"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
       <c r="E16" s="6"/>
       <c r="F16" s="8"/>
       <c r="G16" s="7"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
       <c r="K16" s="7"/>
-      <c r="L16" s="4"/>
+      <c r="L16" s="6"/>
       <c r="N16" t="s">
         <v>75</v>
       </c>
@@ -1896,8 +1919,8 @@
         <v>76</v>
       </c>
     </row>
-    <row r="17" spans="1:15">
-      <c r="A17" s="41" t="s">
+    <row r="17" spans="1:18">
+      <c r="A17" s="40" t="s">
         <v>16</v>
       </c>
       <c r="B17" s="25" t="s">
@@ -1912,13 +1935,13 @@
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
       <c r="K17" s="7"/>
-      <c r="L17" s="36"/>
+      <c r="L17" s="35"/>
       <c r="O17" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="18" spans="1:15">
-      <c r="A18" s="41" t="s">
+    <row r="18" spans="1:18">
+      <c r="A18" s="40" t="s">
         <v>19</v>
       </c>
       <c r="B18" s="25" t="s">
@@ -1933,24 +1956,24 @@
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
       <c r="K18" s="7"/>
-      <c r="L18" s="36"/>
-    </row>
-    <row r="19" spans="1:15" ht="4.5" customHeight="1">
-      <c r="A19" s="33"/>
-      <c r="B19" s="34"/>
-      <c r="C19" s="35"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="35"/>
-      <c r="F19" s="35"/>
-      <c r="G19" s="35"/>
-      <c r="H19" s="35"/>
-      <c r="I19" s="35"/>
-      <c r="J19" s="35"/>
-      <c r="K19" s="35"/>
-      <c r="L19" s="35"/>
-    </row>
-    <row r="20" spans="1:15">
-      <c r="A20" s="41" t="s">
+      <c r="L18" s="35"/>
+    </row>
+    <row r="19" spans="1:18" ht="4.5" customHeight="1">
+      <c r="A19" s="32"/>
+      <c r="B19" s="33"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="34"/>
+      <c r="E19" s="34"/>
+      <c r="F19" s="34"/>
+      <c r="G19" s="34"/>
+      <c r="H19" s="34"/>
+      <c r="I19" s="34"/>
+      <c r="J19" s="34"/>
+      <c r="K19" s="34"/>
+      <c r="L19" s="34"/>
+    </row>
+    <row r="20" spans="1:18">
+      <c r="A20" s="40" t="s">
         <v>18</v>
       </c>
       <c r="B20" s="27"/>
@@ -1959,27 +1982,30 @@
       <c r="E20" s="6"/>
       <c r="F20" s="28"/>
       <c r="G20" s="7"/>
-      <c r="H20" s="29"/>
-      <c r="I20" s="29"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="30"/>
-      <c r="L20" s="4"/>
-    </row>
-    <row r="21" spans="1:15" ht="4.5" customHeight="1">
-      <c r="A21" s="33"/>
-      <c r="B21" s="34"/>
-      <c r="C21" s="35"/>
-      <c r="D21" s="35"/>
-      <c r="E21" s="35"/>
-      <c r="F21" s="35"/>
-      <c r="G21" s="35"/>
-      <c r="H21" s="35"/>
-      <c r="I21" s="35"/>
-      <c r="J21" s="35"/>
-      <c r="K21" s="35"/>
-      <c r="L21" s="35"/>
-    </row>
-    <row r="22" spans="1:15">
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="29"/>
+      <c r="L20" s="6"/>
+      <c r="N20" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" ht="4.5" customHeight="1">
+      <c r="A21" s="32"/>
+      <c r="B21" s="33"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="34"/>
+      <c r="G21" s="34"/>
+      <c r="H21" s="34"/>
+      <c r="I21" s="34"/>
+      <c r="J21" s="34"/>
+      <c r="K21" s="34"/>
+      <c r="L21" s="34"/>
+    </row>
+    <row r="22" spans="1:18">
       <c r="A22" s="18" t="s">
         <v>49</v>
       </c>
@@ -1994,26 +2020,29 @@
       <c r="J22" s="4"/>
       <c r="K22" s="7"/>
       <c r="L22" s="4"/>
-    </row>
-    <row r="23" spans="1:15" ht="4.5" customHeight="1">
-      <c r="A23" s="33"/>
-      <c r="B23" s="34"/>
-      <c r="C23" s="35"/>
-      <c r="D23" s="35"/>
-      <c r="E23" s="35"/>
-      <c r="F23" s="35"/>
-      <c r="G23" s="35"/>
-      <c r="H23" s="35"/>
-      <c r="I23" s="35"/>
-      <c r="J23" s="35"/>
-      <c r="K23" s="35"/>
-      <c r="L23" s="35"/>
-    </row>
-    <row r="24" spans="1:15">
+      <c r="O22" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" ht="4.5" customHeight="1">
+      <c r="A23" s="32"/>
+      <c r="B23" s="33"/>
+      <c r="C23" s="34"/>
+      <c r="D23" s="34"/>
+      <c r="E23" s="34"/>
+      <c r="F23" s="34"/>
+      <c r="G23" s="34"/>
+      <c r="H23" s="34"/>
+      <c r="I23" s="34"/>
+      <c r="J23" s="34"/>
+      <c r="K23" s="34"/>
+      <c r="L23" s="34"/>
+    </row>
+    <row r="24" spans="1:18">
       <c r="A24" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="B24" s="37"/>
+      <c r="B24" s="36"/>
       <c r="C24" s="8"/>
       <c r="D24" s="5"/>
       <c r="E24" s="6"/>
@@ -2024,8 +2053,11 @@
       <c r="J24" s="4"/>
       <c r="K24" s="7"/>
       <c r="L24" s="4"/>
-    </row>
-    <row r="25" spans="1:15">
+      <c r="O24" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18">
       <c r="A25" s="18" t="s">
         <v>51</v>
       </c>
@@ -2043,233 +2075,240 @@
       <c r="K25" s="7"/>
       <c r="L25" s="7"/>
     </row>
-    <row r="26" spans="1:15" ht="4.5" customHeight="1" thickBot="1">
-      <c r="A26" s="33"/>
-      <c r="B26" s="34"/>
-      <c r="C26" s="35"/>
-      <c r="D26" s="35"/>
-      <c r="E26" s="35"/>
-      <c r="F26" s="35"/>
-      <c r="G26" s="35"/>
-      <c r="H26" s="35"/>
-      <c r="I26" s="35"/>
-      <c r="J26" s="35"/>
-      <c r="K26" s="35"/>
-      <c r="L26" s="35"/>
-    </row>
-    <row r="27" spans="1:15" ht="15.75" thickBot="1">
+    <row r="26" spans="1:18" ht="4.5" customHeight="1" thickBot="1">
+      <c r="A26" s="32"/>
+      <c r="B26" s="33"/>
+      <c r="C26" s="34"/>
+      <c r="D26" s="34"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="34"/>
+      <c r="G26" s="34"/>
+      <c r="H26" s="34"/>
+      <c r="I26" s="34"/>
+      <c r="J26" s="34"/>
+      <c r="K26" s="34"/>
+      <c r="L26" s="34"/>
+    </row>
+    <row r="27" spans="1:18" ht="15.75" thickBot="1">
       <c r="A27" s="24"/>
       <c r="B27" s="26"/>
-      <c r="C27" s="81" t="s">
+      <c r="C27" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="82"/>
-      <c r="E27" s="82"/>
-      <c r="F27" s="82"/>
-      <c r="G27" s="83"/>
-      <c r="H27" s="81" t="s">
+      <c r="D27" s="51"/>
+      <c r="E27" s="51"/>
+      <c r="F27" s="51"/>
+      <c r="G27" s="52"/>
+      <c r="H27" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="I27" s="82"/>
-      <c r="J27" s="84"/>
-      <c r="K27" s="83"/>
+      <c r="I27" s="51"/>
+      <c r="J27" s="53"/>
+      <c r="K27" s="52"/>
       <c r="L27" s="21" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A28" s="88" t="s">
+      <c r="N27" s="91" t="s">
+        <v>83</v>
+      </c>
+      <c r="O27" s="91"/>
+      <c r="P27" s="91"/>
+      <c r="Q27" s="91"/>
+      <c r="R27" s="91"/>
+    </row>
+    <row r="28" spans="1:18" ht="15.75" thickBot="1">
+      <c r="A28" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="89"/>
-      <c r="C28" s="85"/>
-      <c r="D28" s="86"/>
-      <c r="E28" s="86"/>
-      <c r="F28" s="86"/>
-      <c r="G28" s="87"/>
-      <c r="H28" s="85"/>
-      <c r="I28" s="86"/>
-      <c r="J28" s="86"/>
-      <c r="K28" s="87"/>
-      <c r="L28" s="39"/>
-    </row>
-    <row r="29" spans="1:15" ht="4.5" customHeight="1">
-      <c r="A29" s="33"/>
-      <c r="B29" s="34"/>
-      <c r="C29" s="35"/>
-      <c r="D29" s="35"/>
-      <c r="E29" s="35"/>
-      <c r="F29" s="35"/>
-      <c r="G29" s="35"/>
-      <c r="H29" s="35"/>
-      <c r="I29" s="35"/>
-      <c r="J29" s="35"/>
-      <c r="K29" s="35"/>
-      <c r="L29" s="35"/>
-    </row>
-    <row r="30" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A30" s="54" t="s">
+      <c r="B28" s="58"/>
+      <c r="C28" s="54"/>
+      <c r="D28" s="55"/>
+      <c r="E28" s="55"/>
+      <c r="F28" s="55"/>
+      <c r="G28" s="56"/>
+      <c r="H28" s="54"/>
+      <c r="I28" s="55"/>
+      <c r="J28" s="55"/>
+      <c r="K28" s="56"/>
+      <c r="L28" s="38"/>
+    </row>
+    <row r="29" spans="1:18" ht="4.5" customHeight="1">
+      <c r="A29" s="32"/>
+      <c r="B29" s="33"/>
+      <c r="C29" s="34"/>
+      <c r="D29" s="34"/>
+      <c r="E29" s="34"/>
+      <c r="F29" s="34"/>
+      <c r="G29" s="34"/>
+      <c r="H29" s="34"/>
+      <c r="I29" s="34"/>
+      <c r="J29" s="34"/>
+      <c r="K29" s="34"/>
+      <c r="L29" s="34"/>
+    </row>
+    <row r="30" spans="1:18" ht="15.75" thickBot="1">
+      <c r="A30" s="63" t="s">
         <v>40</v>
       </c>
-      <c r="B30" s="55"/>
-      <c r="C30" s="67"/>
-      <c r="D30" s="68"/>
-      <c r="E30" s="68"/>
-      <c r="F30" s="68"/>
-      <c r="G30" s="69"/>
-      <c r="H30" s="70"/>
-      <c r="I30" s="68"/>
-      <c r="J30" s="68"/>
-      <c r="K30" s="69"/>
+      <c r="B30" s="64"/>
+      <c r="C30" s="59"/>
+      <c r="D30" s="60"/>
+      <c r="E30" s="60"/>
+      <c r="F30" s="60"/>
+      <c r="G30" s="61"/>
+      <c r="H30" s="62"/>
+      <c r="I30" s="60"/>
+      <c r="J30" s="60"/>
+      <c r="K30" s="61"/>
       <c r="L30" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="M30" s="38"/>
-    </row>
-    <row r="31" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A31" s="54" t="s">
+      <c r="M30" s="37"/>
+    </row>
+    <row r="31" spans="1:18" ht="15.75" thickBot="1">
+      <c r="A31" s="63" t="s">
         <v>62</v>
       </c>
-      <c r="B31" s="55"/>
-      <c r="C31" s="64"/>
-      <c r="D31" s="65"/>
-      <c r="E31" s="65"/>
-      <c r="F31" s="65"/>
-      <c r="G31" s="66"/>
-      <c r="H31" s="75" t="s">
+      <c r="B31" s="64"/>
+      <c r="C31" s="69"/>
+      <c r="D31" s="70"/>
+      <c r="E31" s="70"/>
+      <c r="F31" s="70"/>
+      <c r="G31" s="71"/>
+      <c r="H31" s="72" t="s">
         <v>61</v>
       </c>
-      <c r="I31" s="76"/>
-      <c r="J31" s="76"/>
-      <c r="K31" s="76"/>
-      <c r="L31" s="77"/>
-      <c r="M31" s="38"/>
-    </row>
-    <row r="32" spans="1:15" ht="16.5" thickBot="1">
-      <c r="A32" s="73" t="s">
+      <c r="I31" s="73"/>
+      <c r="J31" s="73"/>
+      <c r="K31" s="73"/>
+      <c r="L31" s="74"/>
+      <c r="M31" s="37"/>
+    </row>
+    <row r="32" spans="1:18" ht="16.5" thickBot="1">
+      <c r="A32" s="67" t="s">
         <v>64</v>
       </c>
-      <c r="B32" s="74"/>
-      <c r="C32" s="67"/>
-      <c r="D32" s="68"/>
-      <c r="E32" s="68"/>
-      <c r="F32" s="68"/>
-      <c r="G32" s="69"/>
-      <c r="H32" s="70"/>
-      <c r="I32" s="68"/>
-      <c r="J32" s="68"/>
-      <c r="K32" s="69"/>
-      <c r="M32" s="38"/>
+      <c r="B32" s="68"/>
+      <c r="C32" s="59"/>
+      <c r="D32" s="60"/>
+      <c r="E32" s="60"/>
+      <c r="F32" s="60"/>
+      <c r="G32" s="61"/>
+      <c r="H32" s="62"/>
+      <c r="I32" s="60"/>
+      <c r="J32" s="60"/>
+      <c r="K32" s="61"/>
+      <c r="M32" s="37"/>
     </row>
     <row r="33" spans="1:13" ht="30.75" customHeight="1" thickBot="1">
-      <c r="A33" s="71" t="s">
+      <c r="A33" s="65" t="s">
         <v>36</v>
       </c>
-      <c r="B33" s="72"/>
-      <c r="C33" s="61" t="s">
+      <c r="B33" s="66"/>
+      <c r="C33" s="80" t="s">
         <v>63</v>
       </c>
-      <c r="D33" s="62"/>
-      <c r="E33" s="62"/>
-      <c r="F33" s="62"/>
-      <c r="G33" s="63"/>
-      <c r="H33" s="58"/>
-      <c r="I33" s="59"/>
-      <c r="J33" s="59"/>
-      <c r="K33" s="60"/>
-      <c r="M33" s="38"/>
+      <c r="D33" s="81"/>
+      <c r="E33" s="81"/>
+      <c r="F33" s="81"/>
+      <c r="G33" s="82"/>
+      <c r="H33" s="77"/>
+      <c r="I33" s="78"/>
+      <c r="J33" s="78"/>
+      <c r="K33" s="79"/>
+      <c r="M33" s="37"/>
     </row>
     <row r="34" spans="1:13" ht="4.5" customHeight="1" thickBot="1">
-      <c r="A34" s="33"/>
-      <c r="B34" s="34"/>
-      <c r="C34" s="44"/>
-      <c r="D34" s="44"/>
-      <c r="E34" s="44"/>
-      <c r="F34" s="44"/>
-      <c r="G34" s="44"/>
-      <c r="H34" s="35"/>
-      <c r="I34" s="35"/>
-      <c r="J34" s="35"/>
-      <c r="K34" s="35"/>
+      <c r="A34" s="32"/>
+      <c r="B34" s="33"/>
+      <c r="C34" s="43"/>
+      <c r="D34" s="43"/>
+      <c r="E34" s="43"/>
+      <c r="F34" s="43"/>
+      <c r="G34" s="43"/>
+      <c r="H34" s="34"/>
+      <c r="I34" s="34"/>
+      <c r="J34" s="34"/>
+      <c r="K34" s="34"/>
     </row>
     <row r="35" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A35" s="54" t="s">
+      <c r="A35" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="55"/>
-      <c r="C35" s="64"/>
-      <c r="D35" s="65"/>
-      <c r="E35" s="65"/>
-      <c r="F35" s="65"/>
-      <c r="G35" s="66"/>
-      <c r="H35" s="64"/>
-      <c r="I35" s="65"/>
-      <c r="J35" s="65"/>
-      <c r="K35" s="66"/>
-      <c r="M35" s="38"/>
+      <c r="B35" s="64"/>
+      <c r="C35" s="69"/>
+      <c r="D35" s="70"/>
+      <c r="E35" s="70"/>
+      <c r="F35" s="70"/>
+      <c r="G35" s="71"/>
+      <c r="H35" s="69"/>
+      <c r="I35" s="70"/>
+      <c r="J35" s="70"/>
+      <c r="K35" s="71"/>
+      <c r="M35" s="37"/>
     </row>
     <row r="36" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A36" s="54" t="s">
+      <c r="A36" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="55"/>
-      <c r="C36" s="64"/>
-      <c r="D36" s="65"/>
-      <c r="E36" s="65"/>
-      <c r="F36" s="65"/>
-      <c r="G36" s="66"/>
-      <c r="H36" s="64"/>
-      <c r="I36" s="65"/>
-      <c r="J36" s="65"/>
-      <c r="K36" s="66"/>
-      <c r="M36" s="38"/>
+      <c r="B36" s="64"/>
+      <c r="C36" s="69"/>
+      <c r="D36" s="70"/>
+      <c r="E36" s="70"/>
+      <c r="F36" s="70"/>
+      <c r="G36" s="71"/>
+      <c r="H36" s="69"/>
+      <c r="I36" s="70"/>
+      <c r="J36" s="70"/>
+      <c r="K36" s="71"/>
+      <c r="M36" s="37"/>
     </row>
     <row r="37" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A37" s="54" t="s">
+      <c r="A37" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="B37" s="55"/>
-      <c r="C37" s="64"/>
-      <c r="D37" s="65"/>
-      <c r="E37" s="65"/>
-      <c r="F37" s="65"/>
-      <c r="G37" s="66"/>
-      <c r="H37" s="64"/>
-      <c r="I37" s="65"/>
-      <c r="J37" s="65"/>
-      <c r="K37" s="66"/>
-      <c r="M37" s="38"/>
+      <c r="B37" s="64"/>
+      <c r="C37" s="69"/>
+      <c r="D37" s="70"/>
+      <c r="E37" s="70"/>
+      <c r="F37" s="70"/>
+      <c r="G37" s="71"/>
+      <c r="H37" s="69"/>
+      <c r="I37" s="70"/>
+      <c r="J37" s="70"/>
+      <c r="K37" s="71"/>
+      <c r="M37" s="37"/>
     </row>
     <row r="38" spans="1:13" ht="15.75" thickBot="1"/>
     <row r="39" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A39" s="47" t="s">
+      <c r="A39" s="84" t="s">
         <v>27</v>
       </c>
-      <c r="B39" s="48"/>
-      <c r="C39" s="48"/>
-      <c r="D39" s="48"/>
-      <c r="E39" s="49"/>
+      <c r="B39" s="85"/>
+      <c r="C39" s="85"/>
+      <c r="D39" s="85"/>
+      <c r="E39" s="86"/>
     </row>
     <row r="40" spans="1:13">
       <c r="A40" s="14" t="s">
         <v>26</v>
       </c>
       <c r="B40" s="13"/>
-      <c r="C40" s="50" t="s">
+      <c r="C40" s="87" t="s">
         <v>23</v>
       </c>
-      <c r="D40" s="51"/>
-      <c r="E40" s="32"/>
+      <c r="D40" s="88"/>
+      <c r="E40" s="31"/>
     </row>
     <row r="41" spans="1:13">
       <c r="A41" s="15" t="s">
         <v>22</v>
       </c>
       <c r="B41" s="5"/>
-      <c r="C41" s="50" t="s">
+      <c r="C41" s="87" t="s">
         <v>24</v>
       </c>
-      <c r="D41" s="51"/>
+      <c r="D41" s="88"/>
       <c r="E41" s="8"/>
     </row>
     <row r="42" spans="1:13">
@@ -2277,189 +2316,180 @@
         <v>25</v>
       </c>
       <c r="B42" s="6"/>
-      <c r="C42" s="56" t="s">
+      <c r="C42" s="75" t="s">
         <v>69</v>
       </c>
-      <c r="D42" s="57"/>
-      <c r="E42" s="45"/>
+      <c r="D42" s="76"/>
+      <c r="E42" s="44"/>
     </row>
     <row r="43" spans="1:13" ht="15.75" thickBot="1"/>
     <row r="44" spans="1:13">
-      <c r="A44" s="52" t="s">
+      <c r="A44" s="89" t="s">
         <v>37</v>
       </c>
-      <c r="B44" s="53"/>
-      <c r="C44" s="53"/>
-      <c r="D44" s="53"/>
-      <c r="E44" s="53"/>
-      <c r="F44" s="53"/>
-      <c r="G44" s="53"/>
-      <c r="H44" s="53"/>
-      <c r="I44" s="53"/>
-      <c r="J44" s="53"/>
-      <c r="K44" s="53"/>
-      <c r="L44" s="53"/>
+      <c r="B44" s="90"/>
+      <c r="C44" s="90"/>
+      <c r="D44" s="90"/>
+      <c r="E44" s="90"/>
+      <c r="F44" s="90"/>
+      <c r="G44" s="90"/>
+      <c r="H44" s="90"/>
+      <c r="I44" s="90"/>
+      <c r="J44" s="90"/>
+      <c r="K44" s="90"/>
+      <c r="L44" s="90"/>
     </row>
     <row r="45" spans="1:13">
-      <c r="A45" s="40" t="s">
+      <c r="A45" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="B45" s="46" t="s">
+      <c r="B45" s="83" t="s">
         <v>57</v>
       </c>
-      <c r="C45" s="46"/>
-      <c r="D45" s="46"/>
-      <c r="E45" s="46"/>
-      <c r="F45" s="46"/>
-      <c r="G45" s="46"/>
-      <c r="H45" s="46"/>
-      <c r="I45" s="46"/>
-      <c r="J45" s="46"/>
-      <c r="K45" s="46"/>
-      <c r="L45" s="46"/>
+      <c r="C45" s="83"/>
+      <c r="D45" s="83"/>
+      <c r="E45" s="83"/>
+      <c r="F45" s="83"/>
+      <c r="G45" s="83"/>
+      <c r="H45" s="83"/>
+      <c r="I45" s="83"/>
+      <c r="J45" s="83"/>
+      <c r="K45" s="83"/>
+      <c r="L45" s="83"/>
     </row>
     <row r="46" spans="1:13" ht="15" customHeight="1">
-      <c r="A46" s="40" t="s">
+      <c r="A46" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="B46" s="46" t="s">
+      <c r="B46" s="83" t="s">
         <v>58</v>
       </c>
-      <c r="C46" s="46"/>
-      <c r="D46" s="46"/>
-      <c r="E46" s="46"/>
-      <c r="F46" s="46"/>
-      <c r="G46" s="46"/>
-      <c r="H46" s="46"/>
-      <c r="I46" s="46"/>
-      <c r="J46" s="46"/>
-      <c r="K46" s="46"/>
-      <c r="L46" s="46"/>
+      <c r="C46" s="83"/>
+      <c r="D46" s="83"/>
+      <c r="E46" s="83"/>
+      <c r="F46" s="83"/>
+      <c r="G46" s="83"/>
+      <c r="H46" s="83"/>
+      <c r="I46" s="83"/>
+      <c r="J46" s="83"/>
+      <c r="K46" s="83"/>
+      <c r="L46" s="83"/>
     </row>
     <row r="47" spans="1:13">
-      <c r="A47" s="40" t="s">
+      <c r="A47" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="B47" s="46" t="s">
+      <c r="B47" s="83" t="s">
         <v>59</v>
       </c>
-      <c r="C47" s="46"/>
-      <c r="D47" s="46"/>
-      <c r="E47" s="46"/>
-      <c r="F47" s="46"/>
-      <c r="G47" s="46"/>
-      <c r="H47" s="46"/>
-      <c r="I47" s="46"/>
-      <c r="J47" s="46"/>
-      <c r="K47" s="46"/>
-      <c r="L47" s="46"/>
+      <c r="C47" s="83"/>
+      <c r="D47" s="83"/>
+      <c r="E47" s="83"/>
+      <c r="F47" s="83"/>
+      <c r="G47" s="83"/>
+      <c r="H47" s="83"/>
+      <c r="I47" s="83"/>
+      <c r="J47" s="83"/>
+      <c r="K47" s="83"/>
+      <c r="L47" s="83"/>
     </row>
     <row r="48" spans="1:13">
-      <c r="A48" s="40" t="s">
+      <c r="A48" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="B48" s="46" t="s">
+      <c r="B48" s="83" t="s">
         <v>46</v>
       </c>
-      <c r="C48" s="46"/>
-      <c r="D48" s="46"/>
-      <c r="E48" s="46"/>
-      <c r="F48" s="46"/>
-      <c r="G48" s="46"/>
-      <c r="H48" s="46"/>
-      <c r="I48" s="46"/>
-      <c r="J48" s="46"/>
-      <c r="K48" s="46"/>
-      <c r="L48" s="46"/>
+      <c r="C48" s="83"/>
+      <c r="D48" s="83"/>
+      <c r="E48" s="83"/>
+      <c r="F48" s="83"/>
+      <c r="G48" s="83"/>
+      <c r="H48" s="83"/>
+      <c r="I48" s="83"/>
+      <c r="J48" s="83"/>
+      <c r="K48" s="83"/>
+      <c r="L48" s="83"/>
     </row>
     <row r="49" spans="1:12">
-      <c r="A49" s="40" t="s">
+      <c r="A49" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="B49" s="46" t="s">
+      <c r="B49" s="83" t="s">
         <v>35</v>
       </c>
-      <c r="C49" s="46"/>
-      <c r="D49" s="46"/>
-      <c r="E49" s="46"/>
-      <c r="F49" s="46"/>
-      <c r="G49" s="46"/>
-      <c r="H49" s="46"/>
-      <c r="I49" s="46"/>
-      <c r="J49" s="46"/>
-      <c r="K49" s="46"/>
-      <c r="L49" s="46"/>
+      <c r="C49" s="83"/>
+      <c r="D49" s="83"/>
+      <c r="E49" s="83"/>
+      <c r="F49" s="83"/>
+      <c r="G49" s="83"/>
+      <c r="H49" s="83"/>
+      <c r="I49" s="83"/>
+      <c r="J49" s="83"/>
+      <c r="K49" s="83"/>
+      <c r="L49" s="83"/>
     </row>
     <row r="50" spans="1:12">
-      <c r="A50" s="40" t="s">
+      <c r="A50" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="B50" s="46" t="s">
+      <c r="B50" s="83" t="s">
         <v>56</v>
       </c>
-      <c r="C50" s="46"/>
-      <c r="D50" s="46"/>
-      <c r="E50" s="46"/>
-      <c r="F50" s="46"/>
-      <c r="G50" s="46"/>
-      <c r="H50" s="46"/>
-      <c r="I50" s="46"/>
-      <c r="J50" s="46"/>
-      <c r="K50" s="46"/>
-      <c r="L50" s="46"/>
+      <c r="C50" s="83"/>
+      <c r="D50" s="83"/>
+      <c r="E50" s="83"/>
+      <c r="F50" s="83"/>
+      <c r="G50" s="83"/>
+      <c r="H50" s="83"/>
+      <c r="I50" s="83"/>
+      <c r="J50" s="83"/>
+      <c r="K50" s="83"/>
+      <c r="L50" s="83"/>
     </row>
     <row r="51" spans="1:12">
-      <c r="A51" s="40" t="s">
+      <c r="A51" s="39" t="s">
         <v>53</v>
       </c>
-      <c r="B51" s="46" t="s">
+      <c r="B51" s="83" t="s">
         <v>55</v>
       </c>
-      <c r="C51" s="46"/>
-      <c r="D51" s="46"/>
-      <c r="E51" s="46"/>
-      <c r="F51" s="46"/>
-      <c r="G51" s="46"/>
-      <c r="H51" s="46"/>
-      <c r="I51" s="46"/>
-      <c r="J51" s="46"/>
-      <c r="K51" s="46"/>
-      <c r="L51" s="46"/>
+      <c r="C51" s="83"/>
+      <c r="D51" s="83"/>
+      <c r="E51" s="83"/>
+      <c r="F51" s="83"/>
+      <c r="G51" s="83"/>
+      <c r="H51" s="83"/>
+      <c r="I51" s="83"/>
+      <c r="J51" s="83"/>
+      <c r="K51" s="83"/>
+      <c r="L51" s="83"/>
     </row>
     <row r="52" spans="1:12">
-      <c r="C52" s="38"/>
+      <c r="C52" s="37"/>
     </row>
     <row r="53" spans="1:12">
-      <c r="C53" s="38"/>
+      <c r="C53" s="37"/>
     </row>
     <row r="54" spans="1:12">
-      <c r="B54" s="38"/>
+      <c r="B54" s="37"/>
     </row>
   </sheetData>
   <sortState ref="A24:K25">
     <sortCondition ref="A3"/>
   </sortState>
   <mergeCells count="43">
-    <mergeCell ref="N6:T6"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="H27:K27"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="H28:K28"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="H30:K30"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="H32:K32"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="H31:L31"/>
+    <mergeCell ref="B50:L50"/>
+    <mergeCell ref="B51:L51"/>
+    <mergeCell ref="A39:E39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="B45:L45"/>
+    <mergeCell ref="A44:L44"/>
+    <mergeCell ref="B46:L46"/>
+    <mergeCell ref="B47:L47"/>
+    <mergeCell ref="B48:L48"/>
+    <mergeCell ref="B49:L49"/>
     <mergeCell ref="A35:B35"/>
     <mergeCell ref="A36:B36"/>
     <mergeCell ref="A37:B37"/>
@@ -2472,17 +2502,26 @@
     <mergeCell ref="C35:G35"/>
     <mergeCell ref="C36:G36"/>
     <mergeCell ref="C37:G37"/>
-    <mergeCell ref="B50:L50"/>
-    <mergeCell ref="B51:L51"/>
-    <mergeCell ref="A39:E39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="B45:L45"/>
-    <mergeCell ref="A44:L44"/>
-    <mergeCell ref="B46:L46"/>
-    <mergeCell ref="B47:L47"/>
-    <mergeCell ref="B48:L48"/>
-    <mergeCell ref="B49:L49"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="H30:K30"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="H32:K32"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="H31:L31"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="H28:K28"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="N6:T6"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="H27:K27"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="P4" r:id="rId1"/>

</xml_diff>

<commit_message>
MAtcheados los modelos del back con el front: Organization, Roleposition. Lograda la funcionalidad de Organization. Falta revizar integridad y persistencia con el back, validacion del form LaboralCareer mejorar algo el estilo y habilitar altas y modificaciones de Organization y Roleposition, en este punto el form toma de select option los Roles y las Organizaciones
</commit_message>
<xml_diff>
--- a/Cuadro-de-estado.xlsx
+++ b/Cuadro-de-estado.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="85">
   <si>
     <t>BACKEND</t>
   </si>
@@ -354,7 +354,7 @@
     <t>Aún existen componentes/servicios que apuntan a mock-data</t>
   </si>
   <si>
-    <t>tel, red</t>
+    <t>Phone, socialNetwork</t>
   </si>
 </sst>
 </file>
@@ -614,7 +614,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="35">
+  <borders count="34">
     <border>
       <left/>
       <right/>
@@ -901,19 +901,6 @@
       </left>
       <right/>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -1052,7 +1039,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1110,11 +1097,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1123,7 +1107,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1140,7 +1124,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1149,10 +1134,10 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1164,7 +1149,7 @@
     <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1176,12 +1161,15 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1189,9 +1177,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1275,10 +1260,9 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1580,7 +1564,7 @@
   <dimension ref="A1:T54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M33" sqref="M33"/>
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1672,26 +1656,26 @@
       <c r="L4" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="N4" s="41" t="s">
+      <c r="N4" s="40" t="s">
         <v>66</v>
       </c>
-      <c r="P4" s="42" t="s">
+      <c r="P4" s="41" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="4.5" customHeight="1">
-      <c r="A5" s="32"/>
-      <c r="B5" s="33"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="34"/>
-      <c r="I5" s="34"/>
-      <c r="J5" s="34"/>
-      <c r="K5" s="34"/>
-      <c r="L5" s="34"/>
+      <c r="A5" s="31"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="33"/>
+      <c r="J5" s="33"/>
+      <c r="K5" s="33"/>
+      <c r="L5" s="33"/>
     </row>
     <row r="6" spans="1:20">
       <c r="A6" s="18" t="s">
@@ -1723,18 +1707,18 @@
       <c r="T6" s="46"/>
     </row>
     <row r="7" spans="1:20" ht="4.5" customHeight="1">
-      <c r="A7" s="32"/>
-      <c r="B7" s="33"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="34"/>
-      <c r="J7" s="34"/>
-      <c r="K7" s="34"/>
-      <c r="L7" s="34"/>
+      <c r="A7" s="31"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="33"/>
+      <c r="I7" s="33"/>
+      <c r="J7" s="33"/>
+      <c r="K7" s="33"/>
+      <c r="L7" s="33"/>
     </row>
     <row r="8" spans="1:20">
       <c r="A8" s="18" t="s">
@@ -1765,7 +1749,7 @@
       <c r="S8" s="6"/>
     </row>
     <row r="9" spans="1:20">
-      <c r="A9" s="30" t="s">
+      <c r="A9" s="29" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="19" t="s">
@@ -1779,7 +1763,7 @@
       <c r="H9" s="13"/>
       <c r="I9" s="13"/>
       <c r="J9" s="4"/>
-      <c r="K9" s="31"/>
+      <c r="K9" s="30"/>
       <c r="L9" s="4"/>
       <c r="O9" s="6" t="s">
         <v>78</v>
@@ -1829,28 +1813,30 @@
       </c>
     </row>
     <row r="12" spans="1:20" ht="4.5" customHeight="1">
-      <c r="A12" s="32"/>
-      <c r="B12" s="33"/>
-      <c r="C12" s="34"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="34"/>
-      <c r="J12" s="34"/>
-      <c r="K12" s="34"/>
-      <c r="L12" s="34"/>
+      <c r="A12" s="31"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="33"/>
+      <c r="I12" s="33"/>
+      <c r="J12" s="33"/>
+      <c r="K12" s="33"/>
+      <c r="L12" s="33"/>
     </row>
     <row r="13" spans="1:20">
-      <c r="A13" s="40" t="s">
+      <c r="A13" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="8"/>
+      <c r="B13" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="7"/>
       <c r="G13" s="7"/>
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
@@ -1859,24 +1845,24 @@
       <c r="L13" s="6"/>
     </row>
     <row r="14" spans="1:20">
-      <c r="A14" s="18" t="s">
-        <v>47</v>
+      <c r="A14" s="39" t="s">
+        <v>18</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="16"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="8"/>
+        <v>13</v>
+      </c>
+      <c r="C14" s="8"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="27"/>
       <c r="G14" s="7"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="4"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="28"/>
+      <c r="L14" s="6"/>
       <c r="N14" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:20">
@@ -1886,19 +1872,19 @@
       <c r="B15" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="16"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="8"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="16"/>
       <c r="G15" s="7"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
       <c r="K15" s="7"/>
-      <c r="L15" s="4"/>
+      <c r="L15" s="6"/>
     </row>
     <row r="16" spans="1:20">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="39" t="s">
         <v>9</v>
       </c>
       <c r="B16" s="6"/>
@@ -1920,11 +1906,11 @@
       </c>
     </row>
     <row r="17" spans="1:18">
-      <c r="A17" s="40" t="s">
-        <v>16</v>
+      <c r="A17" s="18" t="s">
+        <v>47</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C17" s="16"/>
       <c r="D17" s="8"/>
@@ -1935,75 +1921,77 @@
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
       <c r="K17" s="7"/>
-      <c r="L17" s="35"/>
-      <c r="O17" t="s">
+      <c r="L17" s="4"/>
+      <c r="N17" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" ht="4.5" customHeight="1">
+      <c r="A18" s="31"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="33"/>
+      <c r="K18" s="33"/>
+      <c r="L18" s="33"/>
+    </row>
+    <row r="19" spans="1:18">
+      <c r="A19" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="16"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="34"/>
+      <c r="O19" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="18" spans="1:18">
-      <c r="A18" s="40" t="s">
+    <row r="20" spans="1:18">
+      <c r="A20" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="25" t="s">
+      <c r="B20" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="16"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="35"/>
-    </row>
-    <row r="19" spans="1:18" ht="4.5" customHeight="1">
-      <c r="A19" s="32"/>
-      <c r="B19" s="33"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="34"/>
-      <c r="E19" s="34"/>
-      <c r="F19" s="34"/>
-      <c r="G19" s="34"/>
-      <c r="H19" s="34"/>
-      <c r="I19" s="34"/>
-      <c r="J19" s="34"/>
-      <c r="K19" s="34"/>
-      <c r="L19" s="34"/>
-    </row>
-    <row r="20" spans="1:18">
-      <c r="A20" s="40" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="27"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="28"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="8"/>
       <c r="E20" s="6"/>
-      <c r="F20" s="28"/>
+      <c r="F20" s="8"/>
       <c r="G20" s="7"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="29"/>
-      <c r="L20" s="6"/>
-      <c r="N20" t="s">
-        <v>80</v>
-      </c>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="34"/>
     </row>
     <row r="21" spans="1:18" ht="4.5" customHeight="1">
-      <c r="A21" s="32"/>
-      <c r="B21" s="33"/>
-      <c r="C21" s="34"/>
-      <c r="D21" s="34"/>
-      <c r="E21" s="34"/>
-      <c r="F21" s="34"/>
-      <c r="G21" s="34"/>
-      <c r="H21" s="34"/>
-      <c r="I21" s="34"/>
-      <c r="J21" s="34"/>
-      <c r="K21" s="34"/>
-      <c r="L21" s="34"/>
+      <c r="A21" s="31"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="33"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="33"/>
+      <c r="F21" s="33"/>
+      <c r="G21" s="33"/>
+      <c r="H21" s="33"/>
+      <c r="I21" s="33"/>
+      <c r="J21" s="33"/>
+      <c r="K21" s="33"/>
+      <c r="L21" s="33"/>
     </row>
     <row r="22" spans="1:18">
       <c r="A22" s="18" t="s">
@@ -2025,24 +2013,24 @@
       </c>
     </row>
     <row r="23" spans="1:18" ht="4.5" customHeight="1">
-      <c r="A23" s="32"/>
-      <c r="B23" s="33"/>
-      <c r="C23" s="34"/>
-      <c r="D23" s="34"/>
-      <c r="E23" s="34"/>
-      <c r="F23" s="34"/>
-      <c r="G23" s="34"/>
-      <c r="H23" s="34"/>
-      <c r="I23" s="34"/>
-      <c r="J23" s="34"/>
-      <c r="K23" s="34"/>
-      <c r="L23" s="34"/>
+      <c r="A23" s="31"/>
+      <c r="B23" s="32"/>
+      <c r="C23" s="33"/>
+      <c r="D23" s="33"/>
+      <c r="E23" s="33"/>
+      <c r="F23" s="33"/>
+      <c r="G23" s="33"/>
+      <c r="H23" s="33"/>
+      <c r="I23" s="33"/>
+      <c r="J23" s="33"/>
+      <c r="K23" s="33"/>
+      <c r="L23" s="33"/>
     </row>
     <row r="24" spans="1:18">
       <c r="A24" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="B24" s="36"/>
+      <c r="B24" s="35"/>
       <c r="C24" s="8"/>
       <c r="D24" s="5"/>
       <c r="E24" s="6"/>
@@ -2076,18 +2064,18 @@
       <c r="L25" s="7"/>
     </row>
     <row r="26" spans="1:18" ht="4.5" customHeight="1" thickBot="1">
-      <c r="A26" s="32"/>
-      <c r="B26" s="33"/>
-      <c r="C26" s="34"/>
-      <c r="D26" s="34"/>
-      <c r="E26" s="34"/>
-      <c r="F26" s="34"/>
-      <c r="G26" s="34"/>
-      <c r="H26" s="34"/>
-      <c r="I26" s="34"/>
-      <c r="J26" s="34"/>
-      <c r="K26" s="34"/>
-      <c r="L26" s="34"/>
+      <c r="A26" s="31"/>
+      <c r="B26" s="32"/>
+      <c r="C26" s="33"/>
+      <c r="D26" s="33"/>
+      <c r="E26" s="33"/>
+      <c r="F26" s="33"/>
+      <c r="G26" s="33"/>
+      <c r="H26" s="33"/>
+      <c r="I26" s="33"/>
+      <c r="J26" s="33"/>
+      <c r="K26" s="33"/>
+      <c r="L26" s="33"/>
     </row>
     <row r="27" spans="1:18" ht="15.75" thickBot="1">
       <c r="A27" s="24"/>
@@ -2108,13 +2096,13 @@
       <c r="L27" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="N27" s="91" t="s">
+      <c r="N27" s="44" t="s">
         <v>83</v>
       </c>
-      <c r="O27" s="91"/>
-      <c r="P27" s="91"/>
-      <c r="Q27" s="91"/>
-      <c r="R27" s="91"/>
+      <c r="O27" s="44"/>
+      <c r="P27" s="44"/>
+      <c r="Q27" s="44"/>
+      <c r="R27" s="44"/>
     </row>
     <row r="28" spans="1:18" ht="15.75" thickBot="1">
       <c r="A28" s="57" t="s">
@@ -2130,21 +2118,21 @@
       <c r="I28" s="55"/>
       <c r="J28" s="55"/>
       <c r="K28" s="56"/>
-      <c r="L28" s="38"/>
+      <c r="L28" s="37"/>
     </row>
     <row r="29" spans="1:18" ht="4.5" customHeight="1">
-      <c r="A29" s="32"/>
-      <c r="B29" s="33"/>
-      <c r="C29" s="34"/>
-      <c r="D29" s="34"/>
-      <c r="E29" s="34"/>
-      <c r="F29" s="34"/>
-      <c r="G29" s="34"/>
-      <c r="H29" s="34"/>
-      <c r="I29" s="34"/>
-      <c r="J29" s="34"/>
-      <c r="K29" s="34"/>
-      <c r="L29" s="34"/>
+      <c r="A29" s="31"/>
+      <c r="B29" s="32"/>
+      <c r="C29" s="33"/>
+      <c r="D29" s="33"/>
+      <c r="E29" s="33"/>
+      <c r="F29" s="33"/>
+      <c r="G29" s="33"/>
+      <c r="H29" s="33"/>
+      <c r="I29" s="33"/>
+      <c r="J29" s="33"/>
+      <c r="K29" s="33"/>
+      <c r="L29" s="33"/>
     </row>
     <row r="30" spans="1:18" ht="15.75" thickBot="1">
       <c r="A30" s="63" t="s">
@@ -2163,7 +2151,7 @@
       <c r="L30" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="M30" s="37"/>
+      <c r="M30" s="36"/>
     </row>
     <row r="31" spans="1:18" ht="15.75" thickBot="1">
       <c r="A31" s="63" t="s">
@@ -2182,7 +2170,7 @@
       <c r="J31" s="73"/>
       <c r="K31" s="73"/>
       <c r="L31" s="74"/>
-      <c r="M31" s="37"/>
+      <c r="M31" s="36"/>
     </row>
     <row r="32" spans="1:18" ht="16.5" thickBot="1">
       <c r="A32" s="67" t="s">
@@ -2198,7 +2186,7 @@
       <c r="I32" s="60"/>
       <c r="J32" s="60"/>
       <c r="K32" s="61"/>
-      <c r="M32" s="37"/>
+      <c r="M32" s="36"/>
     </row>
     <row r="33" spans="1:13" ht="30.75" customHeight="1" thickBot="1">
       <c r="A33" s="65" t="s">
@@ -2216,20 +2204,20 @@
       <c r="I33" s="78"/>
       <c r="J33" s="78"/>
       <c r="K33" s="79"/>
-      <c r="M33" s="37"/>
+      <c r="M33" s="36"/>
     </row>
     <row r="34" spans="1:13" ht="4.5" customHeight="1" thickBot="1">
-      <c r="A34" s="32"/>
-      <c r="B34" s="33"/>
-      <c r="C34" s="43"/>
-      <c r="D34" s="43"/>
-      <c r="E34" s="43"/>
-      <c r="F34" s="43"/>
-      <c r="G34" s="43"/>
-      <c r="H34" s="34"/>
-      <c r="I34" s="34"/>
-      <c r="J34" s="34"/>
-      <c r="K34" s="34"/>
+      <c r="A34" s="31"/>
+      <c r="B34" s="32"/>
+      <c r="C34" s="42"/>
+      <c r="D34" s="42"/>
+      <c r="E34" s="42"/>
+      <c r="F34" s="42"/>
+      <c r="G34" s="42"/>
+      <c r="H34" s="33"/>
+      <c r="I34" s="33"/>
+      <c r="J34" s="33"/>
+      <c r="K34" s="33"/>
     </row>
     <row r="35" spans="1:13" ht="15.75" thickBot="1">
       <c r="A35" s="63" t="s">
@@ -2245,7 +2233,7 @@
       <c r="I35" s="70"/>
       <c r="J35" s="70"/>
       <c r="K35" s="71"/>
-      <c r="M35" s="37"/>
+      <c r="M35" s="36"/>
     </row>
     <row r="36" spans="1:13" ht="15.75" thickBot="1">
       <c r="A36" s="63" t="s">
@@ -2261,7 +2249,7 @@
       <c r="I36" s="70"/>
       <c r="J36" s="70"/>
       <c r="K36" s="71"/>
-      <c r="M36" s="37"/>
+      <c r="M36" s="36"/>
     </row>
     <row r="37" spans="1:13" ht="15.75" thickBot="1">
       <c r="A37" s="63" t="s">
@@ -2277,7 +2265,7 @@
       <c r="I37" s="70"/>
       <c r="J37" s="70"/>
       <c r="K37" s="71"/>
-      <c r="M37" s="37"/>
+      <c r="M37" s="36"/>
     </row>
     <row r="38" spans="1:13" ht="15.75" thickBot="1"/>
     <row r="39" spans="1:13" ht="15.75" thickBot="1">
@@ -2298,7 +2286,7 @@
         <v>23</v>
       </c>
       <c r="D40" s="88"/>
-      <c r="E40" s="31"/>
+      <c r="E40" s="30"/>
     </row>
     <row r="41" spans="1:13">
       <c r="A41" s="15" t="s">
@@ -2320,7 +2308,7 @@
         <v>69</v>
       </c>
       <c r="D42" s="76"/>
-      <c r="E42" s="44"/>
+      <c r="E42" s="43"/>
     </row>
     <row r="43" spans="1:13" ht="15.75" thickBot="1"/>
     <row r="44" spans="1:13">
@@ -2340,7 +2328,7 @@
       <c r="L44" s="90"/>
     </row>
     <row r="45" spans="1:13">
-      <c r="A45" s="39" t="s">
+      <c r="A45" s="38" t="s">
         <v>38</v>
       </c>
       <c r="B45" s="83" t="s">
@@ -2358,7 +2346,7 @@
       <c r="L45" s="83"/>
     </row>
     <row r="46" spans="1:13" ht="15" customHeight="1">
-      <c r="A46" s="39" t="s">
+      <c r="A46" s="38" t="s">
         <v>32</v>
       </c>
       <c r="B46" s="83" t="s">
@@ -2376,7 +2364,7 @@
       <c r="L46" s="83"/>
     </row>
     <row r="47" spans="1:13">
-      <c r="A47" s="39" t="s">
+      <c r="A47" s="38" t="s">
         <v>33</v>
       </c>
       <c r="B47" s="83" t="s">
@@ -2394,7 +2382,7 @@
       <c r="L47" s="83"/>
     </row>
     <row r="48" spans="1:13">
-      <c r="A48" s="39" t="s">
+      <c r="A48" s="38" t="s">
         <v>34</v>
       </c>
       <c r="B48" s="83" t="s">
@@ -2412,7 +2400,7 @@
       <c r="L48" s="83"/>
     </row>
     <row r="49" spans="1:12">
-      <c r="A49" s="39" t="s">
+      <c r="A49" s="38" t="s">
         <v>54</v>
       </c>
       <c r="B49" s="83" t="s">
@@ -2430,7 +2418,7 @@
       <c r="L49" s="83"/>
     </row>
     <row r="50" spans="1:12">
-      <c r="A50" s="39" t="s">
+      <c r="A50" s="38" t="s">
         <v>52</v>
       </c>
       <c r="B50" s="83" t="s">
@@ -2448,7 +2436,7 @@
       <c r="L50" s="83"/>
     </row>
     <row r="51" spans="1:12">
-      <c r="A51" s="39" t="s">
+      <c r="A51" s="38" t="s">
         <v>53</v>
       </c>
       <c r="B51" s="83" t="s">
@@ -2466,13 +2454,13 @@
       <c r="L51" s="83"/>
     </row>
     <row r="52" spans="1:12">
-      <c r="C52" s="37"/>
+      <c r="C52" s="36"/>
     </row>
     <row r="53" spans="1:12">
-      <c r="C53" s="37"/>
+      <c r="C53" s="36"/>
     </row>
     <row r="54" spans="1:12">
-      <c r="B54" s="37"/>
+      <c r="B54" s="36"/>
     </row>
   </sheetData>
   <sortState ref="A24:K25">

</xml_diff>

<commit_message>
creados los componentes roleposition y degree. Ambos comparten muchas similitudes en modelos y logicas
</commit_message>
<xml_diff>
--- a/Cuadro-de-estado.xlsx
+++ b/Cuadro-de-estado.xlsx
@@ -1125,6 +1125,129 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="10" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1139,129 +1262,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1564,7 +1564,7 @@
   <dimension ref="A1:T54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1581,40 +1581,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="23.25">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="88" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="47"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47"/>
+      <c r="B1" s="88"/>
+      <c r="C1" s="88"/>
+      <c r="D1" s="88"/>
+      <c r="E1" s="88"/>
+      <c r="F1" s="88"/>
+      <c r="G1" s="88"/>
+      <c r="H1" s="88"/>
+      <c r="I1" s="88"/>
+      <c r="J1" s="88"/>
+      <c r="K1" s="88"/>
+      <c r="L1" s="88"/>
     </row>
     <row r="2" spans="1:20" ht="15.75" thickBot="1"/>
     <row r="3" spans="1:20" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="89" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="50" t="s">
+      <c r="B3" s="90"/>
+      <c r="C3" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="52"/>
-      <c r="H3" s="50" t="s">
+      <c r="D3" s="81"/>
+      <c r="E3" s="81"/>
+      <c r="F3" s="81"/>
+      <c r="G3" s="83"/>
+      <c r="H3" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="51"/>
-      <c r="J3" s="53"/>
-      <c r="K3" s="52"/>
+      <c r="I3" s="81"/>
+      <c r="J3" s="82"/>
+      <c r="K3" s="83"/>
       <c r="L3" s="21" t="s">
         <v>4</v>
       </c>
@@ -1696,15 +1696,15 @@
       <c r="J6" s="4"/>
       <c r="K6" s="5"/>
       <c r="L6" s="4"/>
-      <c r="N6" s="45" t="s">
+      <c r="N6" s="86" t="s">
         <v>70</v>
       </c>
-      <c r="O6" s="46"/>
-      <c r="P6" s="46"/>
-      <c r="Q6" s="46"/>
-      <c r="R6" s="46"/>
-      <c r="S6" s="46"/>
-      <c r="T6" s="46"/>
+      <c r="O6" s="87"/>
+      <c r="P6" s="87"/>
+      <c r="Q6" s="87"/>
+      <c r="R6" s="87"/>
+      <c r="S6" s="87"/>
+      <c r="T6" s="87"/>
     </row>
     <row r="7" spans="1:20" ht="4.5" customHeight="1">
       <c r="A7" s="31"/>
@@ -1838,11 +1838,11 @@
       <c r="E13" s="5"/>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
       <c r="K13" s="7"/>
-      <c r="L13" s="6"/>
+      <c r="L13" s="5"/>
     </row>
     <row r="14" spans="1:20">
       <c r="A14" s="39" t="s">
@@ -1890,7 +1890,7 @@
       <c r="B16" s="6"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
-      <c r="E16" s="6"/>
+      <c r="E16" s="5"/>
       <c r="F16" s="8"/>
       <c r="G16" s="7"/>
       <c r="H16" s="6"/>
@@ -1914,14 +1914,14 @@
       </c>
       <c r="C17" s="16"/>
       <c r="D17" s="8"/>
-      <c r="E17" s="6"/>
+      <c r="E17" s="5"/>
       <c r="F17" s="8"/>
       <c r="G17" s="7"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
       <c r="K17" s="7"/>
-      <c r="L17" s="4"/>
+      <c r="L17" s="6"/>
       <c r="N17" t="s">
         <v>79</v>
       </c>
@@ -2080,19 +2080,19 @@
     <row r="27" spans="1:18" ht="15.75" thickBot="1">
       <c r="A27" s="24"/>
       <c r="B27" s="26"/>
-      <c r="C27" s="50" t="s">
+      <c r="C27" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="51"/>
-      <c r="E27" s="51"/>
-      <c r="F27" s="51"/>
-      <c r="G27" s="52"/>
-      <c r="H27" s="50" t="s">
+      <c r="D27" s="81"/>
+      <c r="E27" s="81"/>
+      <c r="F27" s="81"/>
+      <c r="G27" s="83"/>
+      <c r="H27" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="I27" s="51"/>
-      <c r="J27" s="53"/>
-      <c r="K27" s="52"/>
+      <c r="I27" s="81"/>
+      <c r="J27" s="82"/>
+      <c r="K27" s="83"/>
       <c r="L27" s="21" t="s">
         <v>4</v>
       </c>
@@ -2105,19 +2105,19 @@
       <c r="R27" s="44"/>
     </row>
     <row r="28" spans="1:18" ht="15.75" thickBot="1">
-      <c r="A28" s="57" t="s">
+      <c r="A28" s="84" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="58"/>
-      <c r="C28" s="54"/>
-      <c r="D28" s="55"/>
-      <c r="E28" s="55"/>
-      <c r="F28" s="55"/>
-      <c r="G28" s="56"/>
-      <c r="H28" s="54"/>
-      <c r="I28" s="55"/>
-      <c r="J28" s="55"/>
-      <c r="K28" s="56"/>
+      <c r="B28" s="85"/>
+      <c r="C28" s="77"/>
+      <c r="D28" s="78"/>
+      <c r="E28" s="78"/>
+      <c r="F28" s="78"/>
+      <c r="G28" s="79"/>
+      <c r="H28" s="77"/>
+      <c r="I28" s="78"/>
+      <c r="J28" s="78"/>
+      <c r="K28" s="79"/>
       <c r="L28" s="37"/>
     </row>
     <row r="29" spans="1:18" ht="4.5" customHeight="1">
@@ -2135,75 +2135,75 @@
       <c r="L29" s="33"/>
     </row>
     <row r="30" spans="1:18" ht="15.75" thickBot="1">
-      <c r="A30" s="63" t="s">
+      <c r="A30" s="53" t="s">
         <v>40</v>
       </c>
-      <c r="B30" s="64"/>
-      <c r="C30" s="59"/>
-      <c r="D30" s="60"/>
-      <c r="E30" s="60"/>
-      <c r="F30" s="60"/>
-      <c r="G30" s="61"/>
-      <c r="H30" s="62"/>
-      <c r="I30" s="60"/>
-      <c r="J30" s="60"/>
-      <c r="K30" s="61"/>
+      <c r="B30" s="54"/>
+      <c r="C30" s="66"/>
+      <c r="D30" s="67"/>
+      <c r="E30" s="67"/>
+      <c r="F30" s="67"/>
+      <c r="G30" s="68"/>
+      <c r="H30" s="69"/>
+      <c r="I30" s="67"/>
+      <c r="J30" s="67"/>
+      <c r="K30" s="68"/>
       <c r="L30" s="22" t="s">
         <v>5</v>
       </c>
       <c r="M30" s="36"/>
     </row>
     <row r="31" spans="1:18" ht="15.75" thickBot="1">
-      <c r="A31" s="63" t="s">
+      <c r="A31" s="53" t="s">
         <v>62</v>
       </c>
-      <c r="B31" s="64"/>
-      <c r="C31" s="69"/>
-      <c r="D31" s="70"/>
-      <c r="E31" s="70"/>
-      <c r="F31" s="70"/>
-      <c r="G31" s="71"/>
-      <c r="H31" s="72" t="s">
+      <c r="B31" s="54"/>
+      <c r="C31" s="63"/>
+      <c r="D31" s="64"/>
+      <c r="E31" s="64"/>
+      <c r="F31" s="64"/>
+      <c r="G31" s="65"/>
+      <c r="H31" s="74" t="s">
         <v>61</v>
       </c>
-      <c r="I31" s="73"/>
-      <c r="J31" s="73"/>
-      <c r="K31" s="73"/>
-      <c r="L31" s="74"/>
+      <c r="I31" s="75"/>
+      <c r="J31" s="75"/>
+      <c r="K31" s="75"/>
+      <c r="L31" s="76"/>
       <c r="M31" s="36"/>
     </row>
     <row r="32" spans="1:18" ht="16.5" thickBot="1">
-      <c r="A32" s="67" t="s">
+      <c r="A32" s="72" t="s">
         <v>64</v>
       </c>
-      <c r="B32" s="68"/>
-      <c r="C32" s="59"/>
-      <c r="D32" s="60"/>
-      <c r="E32" s="60"/>
-      <c r="F32" s="60"/>
-      <c r="G32" s="61"/>
-      <c r="H32" s="62"/>
-      <c r="I32" s="60"/>
-      <c r="J32" s="60"/>
-      <c r="K32" s="61"/>
+      <c r="B32" s="73"/>
+      <c r="C32" s="66"/>
+      <c r="D32" s="67"/>
+      <c r="E32" s="67"/>
+      <c r="F32" s="67"/>
+      <c r="G32" s="68"/>
+      <c r="H32" s="69"/>
+      <c r="I32" s="67"/>
+      <c r="J32" s="67"/>
+      <c r="K32" s="68"/>
       <c r="M32" s="36"/>
     </row>
     <row r="33" spans="1:13" ht="30.75" customHeight="1" thickBot="1">
-      <c r="A33" s="65" t="s">
+      <c r="A33" s="70" t="s">
         <v>36</v>
       </c>
-      <c r="B33" s="66"/>
-      <c r="C33" s="80" t="s">
+      <c r="B33" s="71"/>
+      <c r="C33" s="60" t="s">
         <v>63</v>
       </c>
-      <c r="D33" s="81"/>
-      <c r="E33" s="81"/>
-      <c r="F33" s="81"/>
-      <c r="G33" s="82"/>
-      <c r="H33" s="77"/>
-      <c r="I33" s="78"/>
-      <c r="J33" s="78"/>
-      <c r="K33" s="79"/>
+      <c r="D33" s="61"/>
+      <c r="E33" s="61"/>
+      <c r="F33" s="61"/>
+      <c r="G33" s="62"/>
+      <c r="H33" s="57"/>
+      <c r="I33" s="58"/>
+      <c r="J33" s="58"/>
+      <c r="K33" s="59"/>
       <c r="M33" s="36"/>
     </row>
     <row r="34" spans="1:13" ht="4.5" customHeight="1" thickBot="1">
@@ -2220,72 +2220,72 @@
       <c r="K34" s="33"/>
     </row>
     <row r="35" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A35" s="63" t="s">
+      <c r="A35" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="64"/>
-      <c r="C35" s="69"/>
-      <c r="D35" s="70"/>
-      <c r="E35" s="70"/>
-      <c r="F35" s="70"/>
-      <c r="G35" s="71"/>
-      <c r="H35" s="69"/>
-      <c r="I35" s="70"/>
-      <c r="J35" s="70"/>
-      <c r="K35" s="71"/>
+      <c r="B35" s="54"/>
+      <c r="C35" s="63"/>
+      <c r="D35" s="64"/>
+      <c r="E35" s="64"/>
+      <c r="F35" s="64"/>
+      <c r="G35" s="65"/>
+      <c r="H35" s="63"/>
+      <c r="I35" s="64"/>
+      <c r="J35" s="64"/>
+      <c r="K35" s="65"/>
       <c r="M35" s="36"/>
     </row>
     <row r="36" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A36" s="63" t="s">
+      <c r="A36" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="64"/>
-      <c r="C36" s="69"/>
-      <c r="D36" s="70"/>
-      <c r="E36" s="70"/>
-      <c r="F36" s="70"/>
-      <c r="G36" s="71"/>
-      <c r="H36" s="69"/>
-      <c r="I36" s="70"/>
-      <c r="J36" s="70"/>
-      <c r="K36" s="71"/>
+      <c r="B36" s="54"/>
+      <c r="C36" s="63"/>
+      <c r="D36" s="64"/>
+      <c r="E36" s="64"/>
+      <c r="F36" s="64"/>
+      <c r="G36" s="65"/>
+      <c r="H36" s="63"/>
+      <c r="I36" s="64"/>
+      <c r="J36" s="64"/>
+      <c r="K36" s="65"/>
       <c r="M36" s="36"/>
     </row>
     <row r="37" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A37" s="63" t="s">
+      <c r="A37" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="B37" s="64"/>
-      <c r="C37" s="69"/>
-      <c r="D37" s="70"/>
-      <c r="E37" s="70"/>
-      <c r="F37" s="70"/>
-      <c r="G37" s="71"/>
-      <c r="H37" s="69"/>
-      <c r="I37" s="70"/>
-      <c r="J37" s="70"/>
-      <c r="K37" s="71"/>
+      <c r="B37" s="54"/>
+      <c r="C37" s="63"/>
+      <c r="D37" s="64"/>
+      <c r="E37" s="64"/>
+      <c r="F37" s="64"/>
+      <c r="G37" s="65"/>
+      <c r="H37" s="63"/>
+      <c r="I37" s="64"/>
+      <c r="J37" s="64"/>
+      <c r="K37" s="65"/>
       <c r="M37" s="36"/>
     </row>
     <row r="38" spans="1:13" ht="15.75" thickBot="1"/>
     <row r="39" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A39" s="84" t="s">
+      <c r="A39" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="B39" s="85"/>
-      <c r="C39" s="85"/>
-      <c r="D39" s="85"/>
-      <c r="E39" s="86"/>
+      <c r="B39" s="47"/>
+      <c r="C39" s="47"/>
+      <c r="D39" s="47"/>
+      <c r="E39" s="48"/>
     </row>
     <row r="40" spans="1:13">
       <c r="A40" s="14" t="s">
         <v>26</v>
       </c>
       <c r="B40" s="13"/>
-      <c r="C40" s="87" t="s">
+      <c r="C40" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="D40" s="88"/>
+      <c r="D40" s="50"/>
       <c r="E40" s="30"/>
     </row>
     <row r="41" spans="1:13">
@@ -2293,10 +2293,10 @@
         <v>22</v>
       </c>
       <c r="B41" s="5"/>
-      <c r="C41" s="87" t="s">
+      <c r="C41" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="D41" s="88"/>
+      <c r="D41" s="50"/>
       <c r="E41" s="8"/>
     </row>
     <row r="42" spans="1:13">
@@ -2304,154 +2304,154 @@
         <v>25</v>
       </c>
       <c r="B42" s="6"/>
-      <c r="C42" s="75" t="s">
+      <c r="C42" s="55" t="s">
         <v>69</v>
       </c>
-      <c r="D42" s="76"/>
+      <c r="D42" s="56"/>
       <c r="E42" s="43"/>
     </row>
     <row r="43" spans="1:13" ht="15.75" thickBot="1"/>
     <row r="44" spans="1:13">
-      <c r="A44" s="89" t="s">
+      <c r="A44" s="51" t="s">
         <v>37</v>
       </c>
-      <c r="B44" s="90"/>
-      <c r="C44" s="90"/>
-      <c r="D44" s="90"/>
-      <c r="E44" s="90"/>
-      <c r="F44" s="90"/>
-      <c r="G44" s="90"/>
-      <c r="H44" s="90"/>
-      <c r="I44" s="90"/>
-      <c r="J44" s="90"/>
-      <c r="K44" s="90"/>
-      <c r="L44" s="90"/>
+      <c r="B44" s="52"/>
+      <c r="C44" s="52"/>
+      <c r="D44" s="52"/>
+      <c r="E44" s="52"/>
+      <c r="F44" s="52"/>
+      <c r="G44" s="52"/>
+      <c r="H44" s="52"/>
+      <c r="I44" s="52"/>
+      <c r="J44" s="52"/>
+      <c r="K44" s="52"/>
+      <c r="L44" s="52"/>
     </row>
     <row r="45" spans="1:13">
       <c r="A45" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="B45" s="83" t="s">
+      <c r="B45" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="C45" s="83"/>
-      <c r="D45" s="83"/>
-      <c r="E45" s="83"/>
-      <c r="F45" s="83"/>
-      <c r="G45" s="83"/>
-      <c r="H45" s="83"/>
-      <c r="I45" s="83"/>
-      <c r="J45" s="83"/>
-      <c r="K45" s="83"/>
-      <c r="L45" s="83"/>
+      <c r="C45" s="45"/>
+      <c r="D45" s="45"/>
+      <c r="E45" s="45"/>
+      <c r="F45" s="45"/>
+      <c r="G45" s="45"/>
+      <c r="H45" s="45"/>
+      <c r="I45" s="45"/>
+      <c r="J45" s="45"/>
+      <c r="K45" s="45"/>
+      <c r="L45" s="45"/>
     </row>
     <row r="46" spans="1:13" ht="15" customHeight="1">
       <c r="A46" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="B46" s="83" t="s">
+      <c r="B46" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="C46" s="83"/>
-      <c r="D46" s="83"/>
-      <c r="E46" s="83"/>
-      <c r="F46" s="83"/>
-      <c r="G46" s="83"/>
-      <c r="H46" s="83"/>
-      <c r="I46" s="83"/>
-      <c r="J46" s="83"/>
-      <c r="K46" s="83"/>
-      <c r="L46" s="83"/>
+      <c r="C46" s="45"/>
+      <c r="D46" s="45"/>
+      <c r="E46" s="45"/>
+      <c r="F46" s="45"/>
+      <c r="G46" s="45"/>
+      <c r="H46" s="45"/>
+      <c r="I46" s="45"/>
+      <c r="J46" s="45"/>
+      <c r="K46" s="45"/>
+      <c r="L46" s="45"/>
     </row>
     <row r="47" spans="1:13">
       <c r="A47" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="B47" s="83" t="s">
+      <c r="B47" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="C47" s="83"/>
-      <c r="D47" s="83"/>
-      <c r="E47" s="83"/>
-      <c r="F47" s="83"/>
-      <c r="G47" s="83"/>
-      <c r="H47" s="83"/>
-      <c r="I47" s="83"/>
-      <c r="J47" s="83"/>
-      <c r="K47" s="83"/>
-      <c r="L47" s="83"/>
+      <c r="C47" s="45"/>
+      <c r="D47" s="45"/>
+      <c r="E47" s="45"/>
+      <c r="F47" s="45"/>
+      <c r="G47" s="45"/>
+      <c r="H47" s="45"/>
+      <c r="I47" s="45"/>
+      <c r="J47" s="45"/>
+      <c r="K47" s="45"/>
+      <c r="L47" s="45"/>
     </row>
     <row r="48" spans="1:13">
       <c r="A48" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="B48" s="83" t="s">
+      <c r="B48" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="C48" s="83"/>
-      <c r="D48" s="83"/>
-      <c r="E48" s="83"/>
-      <c r="F48" s="83"/>
-      <c r="G48" s="83"/>
-      <c r="H48" s="83"/>
-      <c r="I48" s="83"/>
-      <c r="J48" s="83"/>
-      <c r="K48" s="83"/>
-      <c r="L48" s="83"/>
+      <c r="C48" s="45"/>
+      <c r="D48" s="45"/>
+      <c r="E48" s="45"/>
+      <c r="F48" s="45"/>
+      <c r="G48" s="45"/>
+      <c r="H48" s="45"/>
+      <c r="I48" s="45"/>
+      <c r="J48" s="45"/>
+      <c r="K48" s="45"/>
+      <c r="L48" s="45"/>
     </row>
     <row r="49" spans="1:12">
       <c r="A49" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="B49" s="83" t="s">
+      <c r="B49" s="45" t="s">
         <v>35</v>
       </c>
-      <c r="C49" s="83"/>
-      <c r="D49" s="83"/>
-      <c r="E49" s="83"/>
-      <c r="F49" s="83"/>
-      <c r="G49" s="83"/>
-      <c r="H49" s="83"/>
-      <c r="I49" s="83"/>
-      <c r="J49" s="83"/>
-      <c r="K49" s="83"/>
-      <c r="L49" s="83"/>
+      <c r="C49" s="45"/>
+      <c r="D49" s="45"/>
+      <c r="E49" s="45"/>
+      <c r="F49" s="45"/>
+      <c r="G49" s="45"/>
+      <c r="H49" s="45"/>
+      <c r="I49" s="45"/>
+      <c r="J49" s="45"/>
+      <c r="K49" s="45"/>
+      <c r="L49" s="45"/>
     </row>
     <row r="50" spans="1:12">
       <c r="A50" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="B50" s="83" t="s">
+      <c r="B50" s="45" t="s">
         <v>56</v>
       </c>
-      <c r="C50" s="83"/>
-      <c r="D50" s="83"/>
-      <c r="E50" s="83"/>
-      <c r="F50" s="83"/>
-      <c r="G50" s="83"/>
-      <c r="H50" s="83"/>
-      <c r="I50" s="83"/>
-      <c r="J50" s="83"/>
-      <c r="K50" s="83"/>
-      <c r="L50" s="83"/>
+      <c r="C50" s="45"/>
+      <c r="D50" s="45"/>
+      <c r="E50" s="45"/>
+      <c r="F50" s="45"/>
+      <c r="G50" s="45"/>
+      <c r="H50" s="45"/>
+      <c r="I50" s="45"/>
+      <c r="J50" s="45"/>
+      <c r="K50" s="45"/>
+      <c r="L50" s="45"/>
     </row>
     <row r="51" spans="1:12">
       <c r="A51" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="B51" s="83" t="s">
+      <c r="B51" s="45" t="s">
         <v>55</v>
       </c>
-      <c r="C51" s="83"/>
-      <c r="D51" s="83"/>
-      <c r="E51" s="83"/>
-      <c r="F51" s="83"/>
-      <c r="G51" s="83"/>
-      <c r="H51" s="83"/>
-      <c r="I51" s="83"/>
-      <c r="J51" s="83"/>
-      <c r="K51" s="83"/>
-      <c r="L51" s="83"/>
+      <c r="C51" s="45"/>
+      <c r="D51" s="45"/>
+      <c r="E51" s="45"/>
+      <c r="F51" s="45"/>
+      <c r="G51" s="45"/>
+      <c r="H51" s="45"/>
+      <c r="I51" s="45"/>
+      <c r="J51" s="45"/>
+      <c r="K51" s="45"/>
+      <c r="L51" s="45"/>
     </row>
     <row r="52" spans="1:12">
       <c r="C52" s="36"/>
@@ -2467,17 +2467,26 @@
     <sortCondition ref="A3"/>
   </sortState>
   <mergeCells count="43">
-    <mergeCell ref="B50:L50"/>
-    <mergeCell ref="B51:L51"/>
-    <mergeCell ref="A39:E39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="B45:L45"/>
-    <mergeCell ref="A44:L44"/>
-    <mergeCell ref="B46:L46"/>
-    <mergeCell ref="B47:L47"/>
-    <mergeCell ref="B48:L48"/>
-    <mergeCell ref="B49:L49"/>
+    <mergeCell ref="N6:T6"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="H27:K27"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="H28:K28"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="H30:K30"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="H32:K32"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="H31:L31"/>
     <mergeCell ref="A35:B35"/>
     <mergeCell ref="A36:B36"/>
     <mergeCell ref="A37:B37"/>
@@ -2490,26 +2499,17 @@
     <mergeCell ref="C35:G35"/>
     <mergeCell ref="C36:G36"/>
     <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="H30:K30"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="H32:K32"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="H31:L31"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="H28:K28"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="N6:T6"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="H27:K27"/>
+    <mergeCell ref="B50:L50"/>
+    <mergeCell ref="B51:L51"/>
+    <mergeCell ref="A39:E39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="B45:L45"/>
+    <mergeCell ref="A44:L44"/>
+    <mergeCell ref="B46:L46"/>
+    <mergeCell ref="B47:L47"/>
+    <mergeCell ref="B48:L48"/>
+    <mergeCell ref="B49:L49"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="P4" r:id="rId1"/>

</xml_diff>

<commit_message>
Agregado el componente roleposition, funcionalidad, estilo, validaciones form. Tambien se corrigio texto de las ventanas modelas frente a una eliminacion, cambio en la leyenda
</commit_message>
<xml_diff>
--- a/Cuadro-de-estado.xlsx
+++ b/Cuadro-de-estado.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="87">
   <si>
     <t>BACKEND</t>
   </si>
@@ -355,6 +355,12 @@
   </si>
   <si>
     <t>Phone, socialNetwork</t>
+  </si>
+  <si>
+    <t>Existe un error que arroja consola this.itemParaBorrar</t>
+  </si>
+  <si>
+    <t>En los Getter de los Form, hay que eliminar espacios de los string</t>
   </si>
 </sst>
 </file>
@@ -1039,7 +1045,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1097,7 +1103,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1125,6 +1130,120 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1148,120 +1267,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1564,7 +1569,7 @@
   <dimension ref="A1:T54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="N33" sqref="N33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1581,40 +1586,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="23.25">
-      <c r="A1" s="88" t="s">
+      <c r="A1" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="88"/>
-      <c r="C1" s="88"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="88"/>
-      <c r="F1" s="88"/>
-      <c r="G1" s="88"/>
-      <c r="H1" s="88"/>
-      <c r="I1" s="88"/>
-      <c r="J1" s="88"/>
-      <c r="K1" s="88"/>
-      <c r="L1" s="88"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
     </row>
     <row r="2" spans="1:20" ht="15.75" thickBot="1"/>
     <row r="3" spans="1:20" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="89" t="s">
+      <c r="A3" s="47" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="90"/>
-      <c r="C3" s="80" t="s">
+      <c r="B3" s="48"/>
+      <c r="C3" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="81"/>
-      <c r="E3" s="81"/>
-      <c r="F3" s="81"/>
-      <c r="G3" s="83"/>
-      <c r="H3" s="80" t="s">
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="81"/>
-      <c r="J3" s="82"/>
-      <c r="K3" s="83"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="52"/>
+      <c r="K3" s="51"/>
       <c r="L3" s="21" t="s">
         <v>4</v>
       </c>
@@ -1656,26 +1661,26 @@
       <c r="L4" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="N4" s="40" t="s">
+      <c r="N4" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="P4" s="41" t="s">
+      <c r="P4" s="40" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="4.5" customHeight="1">
-      <c r="A5" s="31"/>
-      <c r="B5" s="32"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
-      <c r="I5" s="33"/>
-      <c r="J5" s="33"/>
-      <c r="K5" s="33"/>
-      <c r="L5" s="33"/>
+      <c r="A5" s="30"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="32"/>
+      <c r="I5" s="32"/>
+      <c r="J5" s="32"/>
+      <c r="K5" s="32"/>
+      <c r="L5" s="32"/>
     </row>
     <row r="6" spans="1:20">
       <c r="A6" s="18" t="s">
@@ -1696,29 +1701,29 @@
       <c r="J6" s="4"/>
       <c r="K6" s="5"/>
       <c r="L6" s="4"/>
-      <c r="N6" s="86" t="s">
+      <c r="N6" s="44" t="s">
         <v>70</v>
       </c>
-      <c r="O6" s="87"/>
-      <c r="P6" s="87"/>
-      <c r="Q6" s="87"/>
-      <c r="R6" s="87"/>
-      <c r="S6" s="87"/>
-      <c r="T6" s="87"/>
+      <c r="O6" s="45"/>
+      <c r="P6" s="45"/>
+      <c r="Q6" s="45"/>
+      <c r="R6" s="45"/>
+      <c r="S6" s="45"/>
+      <c r="T6" s="45"/>
     </row>
     <row r="7" spans="1:20" ht="4.5" customHeight="1">
-      <c r="A7" s="31"/>
-      <c r="B7" s="32"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="33"/>
-      <c r="I7" s="33"/>
-      <c r="J7" s="33"/>
-      <c r="K7" s="33"/>
-      <c r="L7" s="33"/>
+      <c r="A7" s="30"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="32"/>
+      <c r="J7" s="32"/>
+      <c r="K7" s="32"/>
+      <c r="L7" s="32"/>
     </row>
     <row r="8" spans="1:20">
       <c r="A8" s="18" t="s">
@@ -1749,7 +1754,7 @@
       <c r="S8" s="6"/>
     </row>
     <row r="9" spans="1:20">
-      <c r="A9" s="29" t="s">
+      <c r="A9" s="28" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="19" t="s">
@@ -1763,7 +1768,7 @@
       <c r="H9" s="13"/>
       <c r="I9" s="13"/>
       <c r="J9" s="4"/>
-      <c r="K9" s="30"/>
+      <c r="K9" s="29"/>
       <c r="L9" s="4"/>
       <c r="O9" s="6" t="s">
         <v>78</v>
@@ -1813,21 +1818,21 @@
       </c>
     </row>
     <row r="12" spans="1:20" ht="4.5" customHeight="1">
-      <c r="A12" s="31"/>
-      <c r="B12" s="32"/>
-      <c r="C12" s="33"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="33"/>
-      <c r="G12" s="33"/>
-      <c r="H12" s="33"/>
-      <c r="I12" s="33"/>
-      <c r="J12" s="33"/>
-      <c r="K12" s="33"/>
-      <c r="L12" s="33"/>
+      <c r="A12" s="30"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="32"/>
+      <c r="J12" s="32"/>
+      <c r="K12" s="32"/>
+      <c r="L12" s="32"/>
     </row>
     <row r="13" spans="1:20">
-      <c r="A13" s="39" t="s">
+      <c r="A13" s="38" t="s">
         <v>30</v>
       </c>
       <c r="B13" s="25" t="s">
@@ -1836,7 +1841,7 @@
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
-      <c r="F13" s="7"/>
+      <c r="F13" s="5"/>
       <c r="G13" s="7"/>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
@@ -1845,21 +1850,21 @@
       <c r="L13" s="5"/>
     </row>
     <row r="14" spans="1:20">
-      <c r="A14" s="39" t="s">
+      <c r="A14" s="38" t="s">
         <v>18</v>
       </c>
       <c r="B14" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="27"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
       <c r="E14" s="5"/>
-      <c r="F14" s="27"/>
+      <c r="F14" s="5"/>
       <c r="G14" s="7"/>
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
-      <c r="K14" s="28"/>
+      <c r="K14" s="27"/>
       <c r="L14" s="6"/>
       <c r="N14" t="s">
         <v>80</v>
@@ -1884,7 +1889,7 @@
       <c r="L15" s="6"/>
     </row>
     <row r="16" spans="1:20">
-      <c r="A16" s="39" t="s">
+      <c r="A16" s="38" t="s">
         <v>9</v>
       </c>
       <c r="B16" s="6"/>
@@ -1905,7 +1910,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="17" spans="1:18">
+    <row r="17" spans="1:19">
       <c r="A17" s="18" t="s">
         <v>47</v>
       </c>
@@ -1926,22 +1931,22 @@
         <v>79</v>
       </c>
     </row>
-    <row r="18" spans="1:18" ht="4.5" customHeight="1">
-      <c r="A18" s="31"/>
-      <c r="B18" s="32"/>
-      <c r="C18" s="33"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="33"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
-      <c r="J18" s="33"/>
-      <c r="K18" s="33"/>
-      <c r="L18" s="33"/>
-    </row>
-    <row r="19" spans="1:18">
-      <c r="A19" s="39" t="s">
+    <row r="18" spans="1:19" ht="4.5" customHeight="1">
+      <c r="A18" s="30"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="32"/>
+      <c r="J18" s="32"/>
+      <c r="K18" s="32"/>
+      <c r="L18" s="32"/>
+    </row>
+    <row r="19" spans="1:19">
+      <c r="A19" s="38" t="s">
         <v>16</v>
       </c>
       <c r="B19" s="25" t="s">
@@ -1956,13 +1961,13 @@
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
       <c r="K19" s="7"/>
-      <c r="L19" s="34"/>
+      <c r="L19" s="33"/>
       <c r="O19" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="1:18">
-      <c r="A20" s="39" t="s">
+    <row r="20" spans="1:19">
+      <c r="A20" s="38" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="25" t="s">
@@ -1977,23 +1982,23 @@
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
       <c r="K20" s="7"/>
-      <c r="L20" s="34"/>
-    </row>
-    <row r="21" spans="1:18" ht="4.5" customHeight="1">
-      <c r="A21" s="31"/>
-      <c r="B21" s="32"/>
-      <c r="C21" s="33"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="33"/>
-      <c r="F21" s="33"/>
-      <c r="G21" s="33"/>
-      <c r="H21" s="33"/>
-      <c r="I21" s="33"/>
-      <c r="J21" s="33"/>
-      <c r="K21" s="33"/>
-      <c r="L21" s="33"/>
-    </row>
-    <row r="22" spans="1:18">
+      <c r="L20" s="33"/>
+    </row>
+    <row r="21" spans="1:19" ht="4.5" customHeight="1">
+      <c r="A21" s="30"/>
+      <c r="B21" s="31"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="32"/>
+      <c r="H21" s="32"/>
+      <c r="I21" s="32"/>
+      <c r="J21" s="32"/>
+      <c r="K21" s="32"/>
+      <c r="L21" s="32"/>
+    </row>
+    <row r="22" spans="1:19">
       <c r="A22" s="18" t="s">
         <v>49</v>
       </c>
@@ -2012,25 +2017,25 @@
         <v>81</v>
       </c>
     </row>
-    <row r="23" spans="1:18" ht="4.5" customHeight="1">
-      <c r="A23" s="31"/>
-      <c r="B23" s="32"/>
-      <c r="C23" s="33"/>
-      <c r="D23" s="33"/>
-      <c r="E23" s="33"/>
-      <c r="F23" s="33"/>
-      <c r="G23" s="33"/>
-      <c r="H23" s="33"/>
-      <c r="I23" s="33"/>
-      <c r="J23" s="33"/>
-      <c r="K23" s="33"/>
-      <c r="L23" s="33"/>
-    </row>
-    <row r="24" spans="1:18">
+    <row r="23" spans="1:19" ht="4.5" customHeight="1">
+      <c r="A23" s="30"/>
+      <c r="B23" s="31"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="32"/>
+      <c r="G23" s="32"/>
+      <c r="H23" s="32"/>
+      <c r="I23" s="32"/>
+      <c r="J23" s="32"/>
+      <c r="K23" s="32"/>
+      <c r="L23" s="32"/>
+    </row>
+    <row r="24" spans="1:19">
       <c r="A24" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="B24" s="35"/>
+      <c r="B24" s="34"/>
       <c r="C24" s="8"/>
       <c r="D24" s="5"/>
       <c r="E24" s="6"/>
@@ -2045,7 +2050,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="25" spans="1:18">
+    <row r="25" spans="1:19">
       <c r="A25" s="18" t="s">
         <v>51</v>
       </c>
@@ -2063,240 +2068,255 @@
       <c r="K25" s="7"/>
       <c r="L25" s="7"/>
     </row>
-    <row r="26" spans="1:18" ht="4.5" customHeight="1" thickBot="1">
-      <c r="A26" s="31"/>
-      <c r="B26" s="32"/>
-      <c r="C26" s="33"/>
-      <c r="D26" s="33"/>
-      <c r="E26" s="33"/>
-      <c r="F26" s="33"/>
-      <c r="G26" s="33"/>
-      <c r="H26" s="33"/>
-      <c r="I26" s="33"/>
-      <c r="J26" s="33"/>
-      <c r="K26" s="33"/>
-      <c r="L26" s="33"/>
-    </row>
-    <row r="27" spans="1:18" ht="15.75" thickBot="1">
+    <row r="26" spans="1:19" ht="4.5" customHeight="1" thickBot="1">
+      <c r="A26" s="30"/>
+      <c r="B26" s="31"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="32"/>
+      <c r="G26" s="32"/>
+      <c r="H26" s="32"/>
+      <c r="I26" s="32"/>
+      <c r="J26" s="32"/>
+      <c r="K26" s="32"/>
+      <c r="L26" s="32"/>
+    </row>
+    <row r="27" spans="1:19" ht="15.75" thickBot="1">
       <c r="A27" s="24"/>
       <c r="B27" s="26"/>
-      <c r="C27" s="80" t="s">
+      <c r="C27" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="81"/>
-      <c r="E27" s="81"/>
-      <c r="F27" s="81"/>
-      <c r="G27" s="83"/>
-      <c r="H27" s="80" t="s">
+      <c r="D27" s="50"/>
+      <c r="E27" s="50"/>
+      <c r="F27" s="50"/>
+      <c r="G27" s="51"/>
+      <c r="H27" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="I27" s="81"/>
-      <c r="J27" s="82"/>
-      <c r="K27" s="83"/>
+      <c r="I27" s="50"/>
+      <c r="J27" s="52"/>
+      <c r="K27" s="51"/>
       <c r="L27" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="N27" s="44" t="s">
+      <c r="N27" s="43" t="s">
         <v>83</v>
       </c>
-      <c r="O27" s="44"/>
-      <c r="P27" s="44"/>
-      <c r="Q27" s="44"/>
-      <c r="R27" s="44"/>
-    </row>
-    <row r="28" spans="1:18" ht="15.75" thickBot="1">
-      <c r="A28" s="84" t="s">
+      <c r="O27" s="43"/>
+      <c r="P27" s="43"/>
+      <c r="Q27" s="43"/>
+      <c r="R27" s="43"/>
+    </row>
+    <row r="28" spans="1:19" ht="15.75" thickBot="1">
+      <c r="A28" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="85"/>
-      <c r="C28" s="77"/>
-      <c r="D28" s="78"/>
-      <c r="E28" s="78"/>
-      <c r="F28" s="78"/>
-      <c r="G28" s="79"/>
-      <c r="H28" s="77"/>
-      <c r="I28" s="78"/>
-      <c r="J28" s="78"/>
-      <c r="K28" s="79"/>
-      <c r="L28" s="37"/>
-    </row>
-    <row r="29" spans="1:18" ht="4.5" customHeight="1">
-      <c r="A29" s="31"/>
-      <c r="B29" s="32"/>
-      <c r="C29" s="33"/>
-      <c r="D29" s="33"/>
-      <c r="E29" s="33"/>
-      <c r="F29" s="33"/>
-      <c r="G29" s="33"/>
-      <c r="H29" s="33"/>
-      <c r="I29" s="33"/>
-      <c r="J29" s="33"/>
-      <c r="K29" s="33"/>
-      <c r="L29" s="33"/>
-    </row>
-    <row r="30" spans="1:18" ht="15.75" thickBot="1">
-      <c r="A30" s="53" t="s">
+      <c r="B28" s="57"/>
+      <c r="C28" s="53"/>
+      <c r="D28" s="54"/>
+      <c r="E28" s="54"/>
+      <c r="F28" s="54"/>
+      <c r="G28" s="55"/>
+      <c r="H28" s="53"/>
+      <c r="I28" s="54"/>
+      <c r="J28" s="54"/>
+      <c r="K28" s="55"/>
+      <c r="L28" s="36"/>
+    </row>
+    <row r="29" spans="1:19" ht="4.5" customHeight="1">
+      <c r="A29" s="30"/>
+      <c r="B29" s="31"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="32"/>
+      <c r="G29" s="32"/>
+      <c r="H29" s="32"/>
+      <c r="I29" s="32"/>
+      <c r="J29" s="32"/>
+      <c r="K29" s="32"/>
+      <c r="L29" s="32"/>
+    </row>
+    <row r="30" spans="1:19" ht="15.75" thickBot="1">
+      <c r="A30" s="62" t="s">
         <v>40</v>
       </c>
-      <c r="B30" s="54"/>
-      <c r="C30" s="66"/>
-      <c r="D30" s="67"/>
-      <c r="E30" s="67"/>
-      <c r="F30" s="67"/>
-      <c r="G30" s="68"/>
-      <c r="H30" s="69"/>
-      <c r="I30" s="67"/>
-      <c r="J30" s="67"/>
-      <c r="K30" s="68"/>
+      <c r="B30" s="63"/>
+      <c r="C30" s="58"/>
+      <c r="D30" s="59"/>
+      <c r="E30" s="59"/>
+      <c r="F30" s="59"/>
+      <c r="G30" s="60"/>
+      <c r="H30" s="61"/>
+      <c r="I30" s="59"/>
+      <c r="J30" s="59"/>
+      <c r="K30" s="60"/>
       <c r="L30" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="M30" s="36"/>
-    </row>
-    <row r="31" spans="1:18" ht="15.75" thickBot="1">
-      <c r="A31" s="53" t="s">
+      <c r="M30" s="35"/>
+      <c r="N30" s="43" t="s">
+        <v>85</v>
+      </c>
+      <c r="O30" s="43"/>
+      <c r="P30" s="43"/>
+      <c r="Q30" s="43"/>
+      <c r="R30" s="43"/>
+    </row>
+    <row r="31" spans="1:19" ht="15.75" thickBot="1">
+      <c r="A31" s="62" t="s">
         <v>62</v>
       </c>
-      <c r="B31" s="54"/>
-      <c r="C31" s="63"/>
-      <c r="D31" s="64"/>
-      <c r="E31" s="64"/>
-      <c r="F31" s="64"/>
-      <c r="G31" s="65"/>
-      <c r="H31" s="74" t="s">
+      <c r="B31" s="63"/>
+      <c r="C31" s="68"/>
+      <c r="D31" s="69"/>
+      <c r="E31" s="69"/>
+      <c r="F31" s="69"/>
+      <c r="G31" s="70"/>
+      <c r="H31" s="71" t="s">
         <v>61</v>
       </c>
-      <c r="I31" s="75"/>
-      <c r="J31" s="75"/>
-      <c r="K31" s="75"/>
-      <c r="L31" s="76"/>
-      <c r="M31" s="36"/>
-    </row>
-    <row r="32" spans="1:18" ht="16.5" thickBot="1">
-      <c r="A32" s="72" t="s">
+      <c r="I31" s="72"/>
+      <c r="J31" s="72"/>
+      <c r="K31" s="72"/>
+      <c r="L31" s="73"/>
+      <c r="M31" s="35"/>
+    </row>
+    <row r="32" spans="1:19" ht="16.5" thickBot="1">
+      <c r="A32" s="66" t="s">
         <v>64</v>
       </c>
-      <c r="B32" s="73"/>
-      <c r="C32" s="66"/>
-      <c r="D32" s="67"/>
-      <c r="E32" s="67"/>
-      <c r="F32" s="67"/>
-      <c r="G32" s="68"/>
-      <c r="H32" s="69"/>
-      <c r="I32" s="67"/>
-      <c r="J32" s="67"/>
-      <c r="K32" s="68"/>
-      <c r="M32" s="36"/>
+      <c r="B32" s="67"/>
+      <c r="C32" s="58"/>
+      <c r="D32" s="59"/>
+      <c r="E32" s="59"/>
+      <c r="F32" s="59"/>
+      <c r="G32" s="60"/>
+      <c r="H32" s="61"/>
+      <c r="I32" s="59"/>
+      <c r="J32" s="59"/>
+      <c r="K32" s="60"/>
+      <c r="M32" s="35"/>
+      <c r="N32" s="43" t="s">
+        <v>86</v>
+      </c>
+      <c r="O32" s="43"/>
+      <c r="P32" s="43"/>
+      <c r="Q32" s="43"/>
+      <c r="R32" s="43"/>
+      <c r="S32" s="43"/>
     </row>
     <row r="33" spans="1:13" ht="30.75" customHeight="1" thickBot="1">
-      <c r="A33" s="70" t="s">
+      <c r="A33" s="64" t="s">
         <v>36</v>
       </c>
-      <c r="B33" s="71"/>
-      <c r="C33" s="60" t="s">
+      <c r="B33" s="65"/>
+      <c r="C33" s="79" t="s">
         <v>63</v>
       </c>
-      <c r="D33" s="61"/>
-      <c r="E33" s="61"/>
-      <c r="F33" s="61"/>
-      <c r="G33" s="62"/>
-      <c r="H33" s="57"/>
-      <c r="I33" s="58"/>
-      <c r="J33" s="58"/>
-      <c r="K33" s="59"/>
-      <c r="M33" s="36"/>
+      <c r="D33" s="80"/>
+      <c r="E33" s="80"/>
+      <c r="F33" s="80"/>
+      <c r="G33" s="81"/>
+      <c r="H33" s="76"/>
+      <c r="I33" s="77"/>
+      <c r="J33" s="77"/>
+      <c r="K33" s="78"/>
+      <c r="M33" s="35"/>
     </row>
     <row r="34" spans="1:13" ht="4.5" customHeight="1" thickBot="1">
-      <c r="A34" s="31"/>
-      <c r="B34" s="32"/>
-      <c r="C34" s="42"/>
-      <c r="D34" s="42"/>
-      <c r="E34" s="42"/>
-      <c r="F34" s="42"/>
-      <c r="G34" s="42"/>
-      <c r="H34" s="33"/>
-      <c r="I34" s="33"/>
-      <c r="J34" s="33"/>
-      <c r="K34" s="33"/>
+      <c r="A34" s="30"/>
+      <c r="B34" s="31"/>
+      <c r="C34" s="41"/>
+      <c r="D34" s="41"/>
+      <c r="E34" s="41"/>
+      <c r="F34" s="41"/>
+      <c r="G34" s="41"/>
+      <c r="H34" s="32"/>
+      <c r="I34" s="32"/>
+      <c r="J34" s="32"/>
+      <c r="K34" s="32"/>
     </row>
     <row r="35" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A35" s="53" t="s">
+      <c r="A35" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="54"/>
-      <c r="C35" s="63"/>
-      <c r="D35" s="64"/>
-      <c r="E35" s="64"/>
-      <c r="F35" s="64"/>
-      <c r="G35" s="65"/>
-      <c r="H35" s="63"/>
-      <c r="I35" s="64"/>
-      <c r="J35" s="64"/>
-      <c r="K35" s="65"/>
-      <c r="M35" s="36"/>
+      <c r="B35" s="63"/>
+      <c r="C35" s="68"/>
+      <c r="D35" s="69"/>
+      <c r="E35" s="69"/>
+      <c r="F35" s="69"/>
+      <c r="G35" s="70"/>
+      <c r="H35" s="68"/>
+      <c r="I35" s="69"/>
+      <c r="J35" s="69"/>
+      <c r="K35" s="70"/>
+      <c r="M35" s="35"/>
     </row>
     <row r="36" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A36" s="53" t="s">
+      <c r="A36" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="54"/>
-      <c r="C36" s="63"/>
-      <c r="D36" s="64"/>
-      <c r="E36" s="64"/>
-      <c r="F36" s="64"/>
-      <c r="G36" s="65"/>
-      <c r="H36" s="63"/>
-      <c r="I36" s="64"/>
-      <c r="J36" s="64"/>
-      <c r="K36" s="65"/>
-      <c r="M36" s="36"/>
+      <c r="B36" s="63"/>
+      <c r="C36" s="68"/>
+      <c r="D36" s="69"/>
+      <c r="E36" s="69"/>
+      <c r="F36" s="69"/>
+      <c r="G36" s="70"/>
+      <c r="H36" s="68"/>
+      <c r="I36" s="69"/>
+      <c r="J36" s="69"/>
+      <c r="K36" s="70"/>
+      <c r="M36" s="35"/>
     </row>
     <row r="37" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A37" s="53" t="s">
+      <c r="A37" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="B37" s="54"/>
-      <c r="C37" s="63"/>
-      <c r="D37" s="64"/>
-      <c r="E37" s="64"/>
-      <c r="F37" s="64"/>
-      <c r="G37" s="65"/>
-      <c r="H37" s="63"/>
-      <c r="I37" s="64"/>
-      <c r="J37" s="64"/>
-      <c r="K37" s="65"/>
-      <c r="M37" s="36"/>
+      <c r="B37" s="63"/>
+      <c r="C37" s="68"/>
+      <c r="D37" s="69"/>
+      <c r="E37" s="69"/>
+      <c r="F37" s="69"/>
+      <c r="G37" s="70"/>
+      <c r="H37" s="68"/>
+      <c r="I37" s="69"/>
+      <c r="J37" s="69"/>
+      <c r="K37" s="70"/>
+      <c r="M37" s="35"/>
     </row>
     <row r="38" spans="1:13" ht="15.75" thickBot="1"/>
     <row r="39" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A39" s="46" t="s">
+      <c r="A39" s="83" t="s">
         <v>27</v>
       </c>
-      <c r="B39" s="47"/>
-      <c r="C39" s="47"/>
-      <c r="D39" s="47"/>
-      <c r="E39" s="48"/>
+      <c r="B39" s="84"/>
+      <c r="C39" s="84"/>
+      <c r="D39" s="84"/>
+      <c r="E39" s="85"/>
     </row>
     <row r="40" spans="1:13">
       <c r="A40" s="14" t="s">
         <v>26</v>
       </c>
       <c r="B40" s="13"/>
-      <c r="C40" s="49" t="s">
+      <c r="C40" s="86" t="s">
         <v>23</v>
       </c>
-      <c r="D40" s="50"/>
-      <c r="E40" s="30"/>
+      <c r="D40" s="87"/>
+      <c r="E40" s="29"/>
     </row>
     <row r="41" spans="1:13">
       <c r="A41" s="15" t="s">
         <v>22</v>
       </c>
       <c r="B41" s="5"/>
-      <c r="C41" s="49" t="s">
+      <c r="C41" s="86" t="s">
         <v>24</v>
       </c>
-      <c r="D41" s="50"/>
+      <c r="D41" s="87"/>
       <c r="E41" s="8"/>
     </row>
     <row r="42" spans="1:13">
@@ -2304,189 +2324,180 @@
         <v>25</v>
       </c>
       <c r="B42" s="6"/>
-      <c r="C42" s="55" t="s">
+      <c r="C42" s="74" t="s">
         <v>69</v>
       </c>
-      <c r="D42" s="56"/>
-      <c r="E42" s="43"/>
+      <c r="D42" s="75"/>
+      <c r="E42" s="42"/>
     </row>
     <row r="43" spans="1:13" ht="15.75" thickBot="1"/>
     <row r="44" spans="1:13">
-      <c r="A44" s="51" t="s">
+      <c r="A44" s="88" t="s">
         <v>37</v>
       </c>
-      <c r="B44" s="52"/>
-      <c r="C44" s="52"/>
-      <c r="D44" s="52"/>
-      <c r="E44" s="52"/>
-      <c r="F44" s="52"/>
-      <c r="G44" s="52"/>
-      <c r="H44" s="52"/>
-      <c r="I44" s="52"/>
-      <c r="J44" s="52"/>
-      <c r="K44" s="52"/>
-      <c r="L44" s="52"/>
+      <c r="B44" s="89"/>
+      <c r="C44" s="89"/>
+      <c r="D44" s="89"/>
+      <c r="E44" s="89"/>
+      <c r="F44" s="89"/>
+      <c r="G44" s="89"/>
+      <c r="H44" s="89"/>
+      <c r="I44" s="89"/>
+      <c r="J44" s="89"/>
+      <c r="K44" s="89"/>
+      <c r="L44" s="89"/>
     </row>
     <row r="45" spans="1:13">
-      <c r="A45" s="38" t="s">
+      <c r="A45" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="B45" s="45" t="s">
+      <c r="B45" s="82" t="s">
         <v>57</v>
       </c>
-      <c r="C45" s="45"/>
-      <c r="D45" s="45"/>
-      <c r="E45" s="45"/>
-      <c r="F45" s="45"/>
-      <c r="G45" s="45"/>
-      <c r="H45" s="45"/>
-      <c r="I45" s="45"/>
-      <c r="J45" s="45"/>
-      <c r="K45" s="45"/>
-      <c r="L45" s="45"/>
+      <c r="C45" s="82"/>
+      <c r="D45" s="82"/>
+      <c r="E45" s="82"/>
+      <c r="F45" s="82"/>
+      <c r="G45" s="82"/>
+      <c r="H45" s="82"/>
+      <c r="I45" s="82"/>
+      <c r="J45" s="82"/>
+      <c r="K45" s="82"/>
+      <c r="L45" s="82"/>
     </row>
     <row r="46" spans="1:13" ht="15" customHeight="1">
-      <c r="A46" s="38" t="s">
+      <c r="A46" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="B46" s="45" t="s">
+      <c r="B46" s="82" t="s">
         <v>58</v>
       </c>
-      <c r="C46" s="45"/>
-      <c r="D46" s="45"/>
-      <c r="E46" s="45"/>
-      <c r="F46" s="45"/>
-      <c r="G46" s="45"/>
-      <c r="H46" s="45"/>
-      <c r="I46" s="45"/>
-      <c r="J46" s="45"/>
-      <c r="K46" s="45"/>
-      <c r="L46" s="45"/>
+      <c r="C46" s="82"/>
+      <c r="D46" s="82"/>
+      <c r="E46" s="82"/>
+      <c r="F46" s="82"/>
+      <c r="G46" s="82"/>
+      <c r="H46" s="82"/>
+      <c r="I46" s="82"/>
+      <c r="J46" s="82"/>
+      <c r="K46" s="82"/>
+      <c r="L46" s="82"/>
     </row>
     <row r="47" spans="1:13">
-      <c r="A47" s="38" t="s">
+      <c r="A47" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="B47" s="45" t="s">
+      <c r="B47" s="82" t="s">
         <v>59</v>
       </c>
-      <c r="C47" s="45"/>
-      <c r="D47" s="45"/>
-      <c r="E47" s="45"/>
-      <c r="F47" s="45"/>
-      <c r="G47" s="45"/>
-      <c r="H47" s="45"/>
-      <c r="I47" s="45"/>
-      <c r="J47" s="45"/>
-      <c r="K47" s="45"/>
-      <c r="L47" s="45"/>
+      <c r="C47" s="82"/>
+      <c r="D47" s="82"/>
+      <c r="E47" s="82"/>
+      <c r="F47" s="82"/>
+      <c r="G47" s="82"/>
+      <c r="H47" s="82"/>
+      <c r="I47" s="82"/>
+      <c r="J47" s="82"/>
+      <c r="K47" s="82"/>
+      <c r="L47" s="82"/>
     </row>
     <row r="48" spans="1:13">
-      <c r="A48" s="38" t="s">
+      <c r="A48" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="B48" s="45" t="s">
+      <c r="B48" s="82" t="s">
         <v>46</v>
       </c>
-      <c r="C48" s="45"/>
-      <c r="D48" s="45"/>
-      <c r="E48" s="45"/>
-      <c r="F48" s="45"/>
-      <c r="G48" s="45"/>
-      <c r="H48" s="45"/>
-      <c r="I48" s="45"/>
-      <c r="J48" s="45"/>
-      <c r="K48" s="45"/>
-      <c r="L48" s="45"/>
+      <c r="C48" s="82"/>
+      <c r="D48" s="82"/>
+      <c r="E48" s="82"/>
+      <c r="F48" s="82"/>
+      <c r="G48" s="82"/>
+      <c r="H48" s="82"/>
+      <c r="I48" s="82"/>
+      <c r="J48" s="82"/>
+      <c r="K48" s="82"/>
+      <c r="L48" s="82"/>
     </row>
     <row r="49" spans="1:12">
-      <c r="A49" s="38" t="s">
+      <c r="A49" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="B49" s="45" t="s">
+      <c r="B49" s="82" t="s">
         <v>35</v>
       </c>
-      <c r="C49" s="45"/>
-      <c r="D49" s="45"/>
-      <c r="E49" s="45"/>
-      <c r="F49" s="45"/>
-      <c r="G49" s="45"/>
-      <c r="H49" s="45"/>
-      <c r="I49" s="45"/>
-      <c r="J49" s="45"/>
-      <c r="K49" s="45"/>
-      <c r="L49" s="45"/>
+      <c r="C49" s="82"/>
+      <c r="D49" s="82"/>
+      <c r="E49" s="82"/>
+      <c r="F49" s="82"/>
+      <c r="G49" s="82"/>
+      <c r="H49" s="82"/>
+      <c r="I49" s="82"/>
+      <c r="J49" s="82"/>
+      <c r="K49" s="82"/>
+      <c r="L49" s="82"/>
     </row>
     <row r="50" spans="1:12">
-      <c r="A50" s="38" t="s">
+      <c r="A50" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="B50" s="45" t="s">
+      <c r="B50" s="82" t="s">
         <v>56</v>
       </c>
-      <c r="C50" s="45"/>
-      <c r="D50" s="45"/>
-      <c r="E50" s="45"/>
-      <c r="F50" s="45"/>
-      <c r="G50" s="45"/>
-      <c r="H50" s="45"/>
-      <c r="I50" s="45"/>
-      <c r="J50" s="45"/>
-      <c r="K50" s="45"/>
-      <c r="L50" s="45"/>
+      <c r="C50" s="82"/>
+      <c r="D50" s="82"/>
+      <c r="E50" s="82"/>
+      <c r="F50" s="82"/>
+      <c r="G50" s="82"/>
+      <c r="H50" s="82"/>
+      <c r="I50" s="82"/>
+      <c r="J50" s="82"/>
+      <c r="K50" s="82"/>
+      <c r="L50" s="82"/>
     </row>
     <row r="51" spans="1:12">
-      <c r="A51" s="38" t="s">
+      <c r="A51" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="B51" s="45" t="s">
+      <c r="B51" s="82" t="s">
         <v>55</v>
       </c>
-      <c r="C51" s="45"/>
-      <c r="D51" s="45"/>
-      <c r="E51" s="45"/>
-      <c r="F51" s="45"/>
-      <c r="G51" s="45"/>
-      <c r="H51" s="45"/>
-      <c r="I51" s="45"/>
-      <c r="J51" s="45"/>
-      <c r="K51" s="45"/>
-      <c r="L51" s="45"/>
+      <c r="C51" s="82"/>
+      <c r="D51" s="82"/>
+      <c r="E51" s="82"/>
+      <c r="F51" s="82"/>
+      <c r="G51" s="82"/>
+      <c r="H51" s="82"/>
+      <c r="I51" s="82"/>
+      <c r="J51" s="82"/>
+      <c r="K51" s="82"/>
+      <c r="L51" s="82"/>
     </row>
     <row r="52" spans="1:12">
-      <c r="C52" s="36"/>
+      <c r="C52" s="35"/>
     </row>
     <row r="53" spans="1:12">
-      <c r="C53" s="36"/>
+      <c r="C53" s="35"/>
     </row>
     <row r="54" spans="1:12">
-      <c r="B54" s="36"/>
+      <c r="B54" s="35"/>
     </row>
   </sheetData>
   <sortState ref="A24:K25">
     <sortCondition ref="A3"/>
   </sortState>
   <mergeCells count="43">
-    <mergeCell ref="N6:T6"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="H27:K27"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="H28:K28"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="H30:K30"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="H32:K32"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="H31:L31"/>
+    <mergeCell ref="B50:L50"/>
+    <mergeCell ref="B51:L51"/>
+    <mergeCell ref="A39:E39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="B45:L45"/>
+    <mergeCell ref="A44:L44"/>
+    <mergeCell ref="B46:L46"/>
+    <mergeCell ref="B47:L47"/>
+    <mergeCell ref="B48:L48"/>
+    <mergeCell ref="B49:L49"/>
     <mergeCell ref="A35:B35"/>
     <mergeCell ref="A36:B36"/>
     <mergeCell ref="A37:B37"/>
@@ -2499,17 +2510,26 @@
     <mergeCell ref="C35:G35"/>
     <mergeCell ref="C36:G36"/>
     <mergeCell ref="C37:G37"/>
-    <mergeCell ref="B50:L50"/>
-    <mergeCell ref="B51:L51"/>
-    <mergeCell ref="A39:E39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="B45:L45"/>
-    <mergeCell ref="A44:L44"/>
-    <mergeCell ref="B46:L46"/>
-    <mergeCell ref="B47:L47"/>
-    <mergeCell ref="B48:L48"/>
-    <mergeCell ref="B49:L49"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="H30:K30"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="H32:K32"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="H31:L31"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="H28:K28"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="N6:T6"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="H27:K27"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="P4" r:id="rId1"/>

</xml_diff>

<commit_message>
Idem con el componente Degree, se corrigieron en el backend clases para el matcheo con el frontend de los componentes Organization, Roleposition, Degree
</commit_message>
<xml_diff>
--- a/Cuadro-de-estado.xlsx
+++ b/Cuadro-de-estado.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="86">
   <si>
     <t>BACKEND</t>
   </si>
@@ -340,9 +340,6 @@
   </si>
   <si>
     <t>Agregar atributo en Person, con la url de ubicación de google.maps</t>
-  </si>
-  <si>
-    <t>Entity Organization, Degree no tienen filtro por Person</t>
   </si>
   <si>
     <t>La consulta traeria a todas y cualquier modificacion</t>
@@ -620,7 +617,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="34">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -907,19 +904,6 @@
       </left>
       <right/>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -1045,7 +1029,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1103,7 +1087,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1112,7 +1095,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1130,7 +1113,130 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1139,134 +1245,11 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1569,7 +1552,7 @@
   <dimension ref="A1:T54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="N33" sqref="N33"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1586,40 +1569,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="23.25">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="86" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
+      <c r="B1" s="86"/>
+      <c r="C1" s="86"/>
+      <c r="D1" s="86"/>
+      <c r="E1" s="86"/>
+      <c r="F1" s="86"/>
+      <c r="G1" s="86"/>
+      <c r="H1" s="86"/>
+      <c r="I1" s="86"/>
+      <c r="J1" s="86"/>
+      <c r="K1" s="86"/>
+      <c r="L1" s="86"/>
     </row>
     <row r="2" spans="1:20" ht="15.75" thickBot="1"/>
     <row r="3" spans="1:20" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="87" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="48"/>
-      <c r="C3" s="49" t="s">
+      <c r="B3" s="88"/>
+      <c r="C3" s="78" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="49" t="s">
+      <c r="D3" s="79"/>
+      <c r="E3" s="79"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="81"/>
+      <c r="H3" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="50"/>
-      <c r="J3" s="52"/>
-      <c r="K3" s="51"/>
+      <c r="I3" s="79"/>
+      <c r="J3" s="80"/>
+      <c r="K3" s="81"/>
       <c r="L3" s="21" t="s">
         <v>4</v>
       </c>
@@ -1661,26 +1644,26 @@
       <c r="L4" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="N4" s="39" t="s">
+      <c r="N4" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="P4" s="40" t="s">
+      <c r="P4" s="39" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="4.5" customHeight="1">
-      <c r="A5" s="30"/>
-      <c r="B5" s="31"/>
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="32"/>
-      <c r="I5" s="32"/>
-      <c r="J5" s="32"/>
-      <c r="K5" s="32"/>
-      <c r="L5" s="32"/>
+      <c r="A5" s="29"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="31"/>
+      <c r="J5" s="31"/>
+      <c r="K5" s="31"/>
+      <c r="L5" s="31"/>
     </row>
     <row r="6" spans="1:20">
       <c r="A6" s="18" t="s">
@@ -1690,7 +1673,7 @@
         <v>14</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="13"/>
@@ -1701,29 +1684,29 @@
       <c r="J6" s="4"/>
       <c r="K6" s="5"/>
       <c r="L6" s="4"/>
-      <c r="N6" s="44" t="s">
+      <c r="N6" s="84" t="s">
         <v>70</v>
       </c>
-      <c r="O6" s="45"/>
-      <c r="P6" s="45"/>
-      <c r="Q6" s="45"/>
-      <c r="R6" s="45"/>
-      <c r="S6" s="45"/>
-      <c r="T6" s="45"/>
+      <c r="O6" s="85"/>
+      <c r="P6" s="85"/>
+      <c r="Q6" s="85"/>
+      <c r="R6" s="85"/>
+      <c r="S6" s="85"/>
+      <c r="T6" s="85"/>
     </row>
     <row r="7" spans="1:20" ht="4.5" customHeight="1">
-      <c r="A7" s="30"/>
-      <c r="B7" s="31"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32"/>
-      <c r="I7" s="32"/>
-      <c r="J7" s="32"/>
-      <c r="K7" s="32"/>
-      <c r="L7" s="32"/>
+      <c r="A7" s="29"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="31"/>
     </row>
     <row r="8" spans="1:20">
       <c r="A8" s="18" t="s">
@@ -1754,7 +1737,7 @@
       <c r="S8" s="6"/>
     </row>
     <row r="9" spans="1:20">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="27" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="19" t="s">
@@ -1768,7 +1751,7 @@
       <c r="H9" s="13"/>
       <c r="I9" s="13"/>
       <c r="J9" s="4"/>
-      <c r="K9" s="29"/>
+      <c r="K9" s="28"/>
       <c r="L9" s="4"/>
       <c r="O9" s="6" t="s">
         <v>78</v>
@@ -1818,21 +1801,21 @@
       </c>
     </row>
     <row r="12" spans="1:20" ht="4.5" customHeight="1">
-      <c r="A12" s="30"/>
-      <c r="B12" s="31"/>
-      <c r="C12" s="32"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="32"/>
-      <c r="I12" s="32"/>
-      <c r="J12" s="32"/>
-      <c r="K12" s="32"/>
-      <c r="L12" s="32"/>
+      <c r="A12" s="29"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="31"/>
+      <c r="I12" s="31"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="31"/>
+      <c r="L12" s="31"/>
     </row>
     <row r="13" spans="1:20">
-      <c r="A13" s="38" t="s">
+      <c r="A13" s="37" t="s">
         <v>30</v>
       </c>
       <c r="B13" s="25" t="s">
@@ -1850,7 +1833,7 @@
       <c r="L13" s="5"/>
     </row>
     <row r="14" spans="1:20">
-      <c r="A14" s="38" t="s">
+      <c r="A14" s="37" t="s">
         <v>18</v>
       </c>
       <c r="B14" s="25" t="s">
@@ -1861,14 +1844,11 @@
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
       <c r="G14" s="7"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="27"/>
-      <c r="L14" s="6"/>
-      <c r="N14" t="s">
-        <v>80</v>
-      </c>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="5"/>
     </row>
     <row r="15" spans="1:20">
       <c r="A15" s="18" t="s">
@@ -1882,27 +1862,29 @@
       <c r="E15" s="5"/>
       <c r="F15" s="16"/>
       <c r="G15" s="7"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
       <c r="K15" s="7"/>
-      <c r="L15" s="6"/>
+      <c r="L15" s="5"/>
     </row>
     <row r="16" spans="1:20">
-      <c r="A16" s="38" t="s">
+      <c r="A16" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
+      <c r="B16" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
       <c r="E16" s="5"/>
-      <c r="F16" s="8"/>
+      <c r="F16" s="5"/>
       <c r="G16" s="7"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
       <c r="K16" s="7"/>
-      <c r="L16" s="6"/>
+      <c r="L16" s="5"/>
       <c r="N16" t="s">
         <v>75</v>
       </c>
@@ -1932,21 +1914,21 @@
       </c>
     </row>
     <row r="18" spans="1:19" ht="4.5" customHeight="1">
-      <c r="A18" s="30"/>
-      <c r="B18" s="31"/>
-      <c r="C18" s="32"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="32"/>
-      <c r="H18" s="32"/>
-      <c r="I18" s="32"/>
-      <c r="J18" s="32"/>
-      <c r="K18" s="32"/>
-      <c r="L18" s="32"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="30"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="31"/>
+      <c r="G18" s="31"/>
+      <c r="H18" s="31"/>
+      <c r="I18" s="31"/>
+      <c r="J18" s="31"/>
+      <c r="K18" s="31"/>
+      <c r="L18" s="31"/>
     </row>
     <row r="19" spans="1:19">
-      <c r="A19" s="38" t="s">
+      <c r="A19" s="37" t="s">
         <v>16</v>
       </c>
       <c r="B19" s="25" t="s">
@@ -1961,13 +1943,13 @@
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
       <c r="K19" s="7"/>
-      <c r="L19" s="33"/>
+      <c r="L19" s="32"/>
       <c r="O19" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="20" spans="1:19">
-      <c r="A20" s="38" t="s">
+      <c r="A20" s="37" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="25" t="s">
@@ -1982,21 +1964,21 @@
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
       <c r="K20" s="7"/>
-      <c r="L20" s="33"/>
+      <c r="L20" s="32"/>
     </row>
     <row r="21" spans="1:19" ht="4.5" customHeight="1">
-      <c r="A21" s="30"/>
-      <c r="B21" s="31"/>
-      <c r="C21" s="32"/>
-      <c r="D21" s="32"/>
-      <c r="E21" s="32"/>
-      <c r="F21" s="32"/>
-      <c r="G21" s="32"/>
-      <c r="H21" s="32"/>
-      <c r="I21" s="32"/>
-      <c r="J21" s="32"/>
-      <c r="K21" s="32"/>
-      <c r="L21" s="32"/>
+      <c r="A21" s="29"/>
+      <c r="B21" s="30"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="31"/>
+      <c r="G21" s="31"/>
+      <c r="H21" s="31"/>
+      <c r="I21" s="31"/>
+      <c r="J21" s="31"/>
+      <c r="K21" s="31"/>
+      <c r="L21" s="31"/>
     </row>
     <row r="22" spans="1:19">
       <c r="A22" s="18" t="s">
@@ -2014,28 +1996,28 @@
       <c r="K22" s="7"/>
       <c r="L22" s="4"/>
       <c r="O22" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:19" ht="4.5" customHeight="1">
-      <c r="A23" s="30"/>
-      <c r="B23" s="31"/>
-      <c r="C23" s="32"/>
-      <c r="D23" s="32"/>
-      <c r="E23" s="32"/>
-      <c r="F23" s="32"/>
-      <c r="G23" s="32"/>
-      <c r="H23" s="32"/>
-      <c r="I23" s="32"/>
-      <c r="J23" s="32"/>
-      <c r="K23" s="32"/>
-      <c r="L23" s="32"/>
+      <c r="A23" s="29"/>
+      <c r="B23" s="30"/>
+      <c r="C23" s="31"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="31"/>
+      <c r="G23" s="31"/>
+      <c r="H23" s="31"/>
+      <c r="I23" s="31"/>
+      <c r="J23" s="31"/>
+      <c r="K23" s="31"/>
+      <c r="L23" s="31"/>
     </row>
     <row r="24" spans="1:19">
       <c r="A24" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="B24" s="34"/>
+      <c r="B24" s="33"/>
       <c r="C24" s="8"/>
       <c r="D24" s="5"/>
       <c r="E24" s="6"/>
@@ -2047,7 +2029,7 @@
       <c r="K24" s="7"/>
       <c r="L24" s="4"/>
       <c r="O24" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="25" spans="1:19">
@@ -2069,254 +2051,254 @@
       <c r="L25" s="7"/>
     </row>
     <row r="26" spans="1:19" ht="4.5" customHeight="1" thickBot="1">
-      <c r="A26" s="30"/>
-      <c r="B26" s="31"/>
-      <c r="C26" s="32"/>
-      <c r="D26" s="32"/>
-      <c r="E26" s="32"/>
-      <c r="F26" s="32"/>
-      <c r="G26" s="32"/>
-      <c r="H26" s="32"/>
-      <c r="I26" s="32"/>
-      <c r="J26" s="32"/>
-      <c r="K26" s="32"/>
-      <c r="L26" s="32"/>
+      <c r="A26" s="29"/>
+      <c r="B26" s="30"/>
+      <c r="C26" s="31"/>
+      <c r="D26" s="31"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="31"/>
+      <c r="G26" s="31"/>
+      <c r="H26" s="31"/>
+      <c r="I26" s="31"/>
+      <c r="J26" s="31"/>
+      <c r="K26" s="31"/>
+      <c r="L26" s="31"/>
     </row>
     <row r="27" spans="1:19" ht="15.75" thickBot="1">
       <c r="A27" s="24"/>
       <c r="B27" s="26"/>
-      <c r="C27" s="49" t="s">
+      <c r="C27" s="78" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="50"/>
-      <c r="E27" s="50"/>
-      <c r="F27" s="50"/>
-      <c r="G27" s="51"/>
-      <c r="H27" s="49" t="s">
+      <c r="D27" s="79"/>
+      <c r="E27" s="79"/>
+      <c r="F27" s="79"/>
+      <c r="G27" s="81"/>
+      <c r="H27" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="I27" s="50"/>
-      <c r="J27" s="52"/>
-      <c r="K27" s="51"/>
+      <c r="I27" s="79"/>
+      <c r="J27" s="80"/>
+      <c r="K27" s="81"/>
       <c r="L27" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="N27" s="43" t="s">
-        <v>83</v>
-      </c>
-      <c r="O27" s="43"/>
-      <c r="P27" s="43"/>
-      <c r="Q27" s="43"/>
-      <c r="R27" s="43"/>
+      <c r="N27" s="42" t="s">
+        <v>82</v>
+      </c>
+      <c r="O27" s="42"/>
+      <c r="P27" s="42"/>
+      <c r="Q27" s="42"/>
+      <c r="R27" s="42"/>
     </row>
     <row r="28" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A28" s="56" t="s">
+      <c r="A28" s="82" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="57"/>
-      <c r="C28" s="53"/>
-      <c r="D28" s="54"/>
-      <c r="E28" s="54"/>
-      <c r="F28" s="54"/>
-      <c r="G28" s="55"/>
-      <c r="H28" s="53"/>
-      <c r="I28" s="54"/>
-      <c r="J28" s="54"/>
-      <c r="K28" s="55"/>
-      <c r="L28" s="36"/>
+      <c r="B28" s="83"/>
+      <c r="C28" s="75"/>
+      <c r="D28" s="76"/>
+      <c r="E28" s="76"/>
+      <c r="F28" s="76"/>
+      <c r="G28" s="77"/>
+      <c r="H28" s="75"/>
+      <c r="I28" s="76"/>
+      <c r="J28" s="76"/>
+      <c r="K28" s="77"/>
+      <c r="L28" s="35"/>
     </row>
     <row r="29" spans="1:19" ht="4.5" customHeight="1">
-      <c r="A29" s="30"/>
-      <c r="B29" s="31"/>
-      <c r="C29" s="32"/>
-      <c r="D29" s="32"/>
-      <c r="E29" s="32"/>
-      <c r="F29" s="32"/>
-      <c r="G29" s="32"/>
-      <c r="H29" s="32"/>
-      <c r="I29" s="32"/>
-      <c r="J29" s="32"/>
-      <c r="K29" s="32"/>
-      <c r="L29" s="32"/>
+      <c r="A29" s="29"/>
+      <c r="B29" s="30"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="31"/>
+      <c r="G29" s="31"/>
+      <c r="H29" s="31"/>
+      <c r="I29" s="31"/>
+      <c r="J29" s="31"/>
+      <c r="K29" s="31"/>
+      <c r="L29" s="31"/>
     </row>
     <row r="30" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A30" s="62" t="s">
+      <c r="A30" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="B30" s="63"/>
-      <c r="C30" s="58"/>
-      <c r="D30" s="59"/>
-      <c r="E30" s="59"/>
-      <c r="F30" s="59"/>
-      <c r="G30" s="60"/>
-      <c r="H30" s="61"/>
-      <c r="I30" s="59"/>
-      <c r="J30" s="59"/>
-      <c r="K30" s="60"/>
+      <c r="B30" s="52"/>
+      <c r="C30" s="64"/>
+      <c r="D30" s="65"/>
+      <c r="E30" s="65"/>
+      <c r="F30" s="65"/>
+      <c r="G30" s="66"/>
+      <c r="H30" s="67"/>
+      <c r="I30" s="65"/>
+      <c r="J30" s="65"/>
+      <c r="K30" s="66"/>
       <c r="L30" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="M30" s="35"/>
-      <c r="N30" s="43" t="s">
+      <c r="M30" s="34"/>
+      <c r="N30" s="42" t="s">
+        <v>84</v>
+      </c>
+      <c r="O30" s="42"/>
+      <c r="P30" s="42"/>
+      <c r="Q30" s="42"/>
+      <c r="R30" s="42"/>
+    </row>
+    <row r="31" spans="1:19" ht="15.75" thickBot="1">
+      <c r="A31" s="51" t="s">
+        <v>62</v>
+      </c>
+      <c r="B31" s="52"/>
+      <c r="C31" s="61"/>
+      <c r="D31" s="62"/>
+      <c r="E31" s="62"/>
+      <c r="F31" s="62"/>
+      <c r="G31" s="63"/>
+      <c r="H31" s="72" t="s">
+        <v>61</v>
+      </c>
+      <c r="I31" s="73"/>
+      <c r="J31" s="73"/>
+      <c r="K31" s="73"/>
+      <c r="L31" s="74"/>
+      <c r="M31" s="34"/>
+    </row>
+    <row r="32" spans="1:19" ht="16.5" thickBot="1">
+      <c r="A32" s="70" t="s">
+        <v>64</v>
+      </c>
+      <c r="B32" s="71"/>
+      <c r="C32" s="64"/>
+      <c r="D32" s="65"/>
+      <c r="E32" s="65"/>
+      <c r="F32" s="65"/>
+      <c r="G32" s="66"/>
+      <c r="H32" s="67"/>
+      <c r="I32" s="65"/>
+      <c r="J32" s="65"/>
+      <c r="K32" s="66"/>
+      <c r="M32" s="34"/>
+      <c r="N32" s="42" t="s">
         <v>85</v>
       </c>
-      <c r="O30" s="43"/>
-      <c r="P30" s="43"/>
-      <c r="Q30" s="43"/>
-      <c r="R30" s="43"/>
-    </row>
-    <row r="31" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A31" s="62" t="s">
-        <v>62</v>
-      </c>
-      <c r="B31" s="63"/>
-      <c r="C31" s="68"/>
-      <c r="D31" s="69"/>
-      <c r="E31" s="69"/>
-      <c r="F31" s="69"/>
-      <c r="G31" s="70"/>
-      <c r="H31" s="71" t="s">
-        <v>61</v>
-      </c>
-      <c r="I31" s="72"/>
-      <c r="J31" s="72"/>
-      <c r="K31" s="72"/>
-      <c r="L31" s="73"/>
-      <c r="M31" s="35"/>
-    </row>
-    <row r="32" spans="1:19" ht="16.5" thickBot="1">
-      <c r="A32" s="66" t="s">
-        <v>64</v>
-      </c>
-      <c r="B32" s="67"/>
-      <c r="C32" s="58"/>
-      <c r="D32" s="59"/>
-      <c r="E32" s="59"/>
-      <c r="F32" s="59"/>
-      <c r="G32" s="60"/>
-      <c r="H32" s="61"/>
-      <c r="I32" s="59"/>
-      <c r="J32" s="59"/>
-      <c r="K32" s="60"/>
-      <c r="M32" s="35"/>
-      <c r="N32" s="43" t="s">
-        <v>86</v>
-      </c>
-      <c r="O32" s="43"/>
-      <c r="P32" s="43"/>
-      <c r="Q32" s="43"/>
-      <c r="R32" s="43"/>
-      <c r="S32" s="43"/>
+      <c r="O32" s="42"/>
+      <c r="P32" s="42"/>
+      <c r="Q32" s="42"/>
+      <c r="R32" s="42"/>
+      <c r="S32" s="42"/>
     </row>
     <row r="33" spans="1:13" ht="30.75" customHeight="1" thickBot="1">
-      <c r="A33" s="64" t="s">
+      <c r="A33" s="68" t="s">
         <v>36</v>
       </c>
-      <c r="B33" s="65"/>
-      <c r="C33" s="79" t="s">
+      <c r="B33" s="69"/>
+      <c r="C33" s="58" t="s">
         <v>63</v>
       </c>
-      <c r="D33" s="80"/>
-      <c r="E33" s="80"/>
-      <c r="F33" s="80"/>
-      <c r="G33" s="81"/>
-      <c r="H33" s="76"/>
-      <c r="I33" s="77"/>
-      <c r="J33" s="77"/>
-      <c r="K33" s="78"/>
-      <c r="M33" s="35"/>
+      <c r="D33" s="59"/>
+      <c r="E33" s="59"/>
+      <c r="F33" s="59"/>
+      <c r="G33" s="60"/>
+      <c r="H33" s="55"/>
+      <c r="I33" s="56"/>
+      <c r="J33" s="56"/>
+      <c r="K33" s="57"/>
+      <c r="M33" s="34"/>
     </row>
     <row r="34" spans="1:13" ht="4.5" customHeight="1" thickBot="1">
-      <c r="A34" s="30"/>
-      <c r="B34" s="31"/>
-      <c r="C34" s="41"/>
-      <c r="D34" s="41"/>
-      <c r="E34" s="41"/>
-      <c r="F34" s="41"/>
-      <c r="G34" s="41"/>
-      <c r="H34" s="32"/>
-      <c r="I34" s="32"/>
-      <c r="J34" s="32"/>
-      <c r="K34" s="32"/>
+      <c r="A34" s="29"/>
+      <c r="B34" s="30"/>
+      <c r="C34" s="40"/>
+      <c r="D34" s="40"/>
+      <c r="E34" s="40"/>
+      <c r="F34" s="40"/>
+      <c r="G34" s="40"/>
+      <c r="H34" s="31"/>
+      <c r="I34" s="31"/>
+      <c r="J34" s="31"/>
+      <c r="K34" s="31"/>
     </row>
     <row r="35" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A35" s="62" t="s">
+      <c r="A35" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="63"/>
-      <c r="C35" s="68"/>
-      <c r="D35" s="69"/>
-      <c r="E35" s="69"/>
-      <c r="F35" s="69"/>
-      <c r="G35" s="70"/>
-      <c r="H35" s="68"/>
-      <c r="I35" s="69"/>
-      <c r="J35" s="69"/>
-      <c r="K35" s="70"/>
-      <c r="M35" s="35"/>
+      <c r="B35" s="52"/>
+      <c r="C35" s="61"/>
+      <c r="D35" s="62"/>
+      <c r="E35" s="62"/>
+      <c r="F35" s="62"/>
+      <c r="G35" s="63"/>
+      <c r="H35" s="61"/>
+      <c r="I35" s="62"/>
+      <c r="J35" s="62"/>
+      <c r="K35" s="63"/>
+      <c r="M35" s="34"/>
     </row>
     <row r="36" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A36" s="62" t="s">
+      <c r="A36" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="63"/>
-      <c r="C36" s="68"/>
-      <c r="D36" s="69"/>
-      <c r="E36" s="69"/>
-      <c r="F36" s="69"/>
-      <c r="G36" s="70"/>
-      <c r="H36" s="68"/>
-      <c r="I36" s="69"/>
-      <c r="J36" s="69"/>
-      <c r="K36" s="70"/>
-      <c r="M36" s="35"/>
+      <c r="B36" s="52"/>
+      <c r="C36" s="61"/>
+      <c r="D36" s="62"/>
+      <c r="E36" s="62"/>
+      <c r="F36" s="62"/>
+      <c r="G36" s="63"/>
+      <c r="H36" s="61"/>
+      <c r="I36" s="62"/>
+      <c r="J36" s="62"/>
+      <c r="K36" s="63"/>
+      <c r="M36" s="34"/>
     </row>
     <row r="37" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A37" s="62" t="s">
+      <c r="A37" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="B37" s="63"/>
-      <c r="C37" s="68"/>
-      <c r="D37" s="69"/>
-      <c r="E37" s="69"/>
-      <c r="F37" s="69"/>
-      <c r="G37" s="70"/>
-      <c r="H37" s="68"/>
-      <c r="I37" s="69"/>
-      <c r="J37" s="69"/>
-      <c r="K37" s="70"/>
-      <c r="M37" s="35"/>
+      <c r="B37" s="52"/>
+      <c r="C37" s="61"/>
+      <c r="D37" s="62"/>
+      <c r="E37" s="62"/>
+      <c r="F37" s="62"/>
+      <c r="G37" s="63"/>
+      <c r="H37" s="61"/>
+      <c r="I37" s="62"/>
+      <c r="J37" s="62"/>
+      <c r="K37" s="63"/>
+      <c r="M37" s="34"/>
     </row>
     <row r="38" spans="1:13" ht="15.75" thickBot="1"/>
     <row r="39" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A39" s="83" t="s">
+      <c r="A39" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="B39" s="84"/>
-      <c r="C39" s="84"/>
-      <c r="D39" s="84"/>
-      <c r="E39" s="85"/>
+      <c r="B39" s="45"/>
+      <c r="C39" s="45"/>
+      <c r="D39" s="45"/>
+      <c r="E39" s="46"/>
     </row>
     <row r="40" spans="1:13">
       <c r="A40" s="14" t="s">
         <v>26</v>
       </c>
       <c r="B40" s="13"/>
-      <c r="C40" s="86" t="s">
+      <c r="C40" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="D40" s="87"/>
-      <c r="E40" s="29"/>
+      <c r="D40" s="48"/>
+      <c r="E40" s="28"/>
     </row>
     <row r="41" spans="1:13">
       <c r="A41" s="15" t="s">
         <v>22</v>
       </c>
       <c r="B41" s="5"/>
-      <c r="C41" s="86" t="s">
+      <c r="C41" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="D41" s="87"/>
+      <c r="D41" s="48"/>
       <c r="E41" s="8"/>
     </row>
     <row r="42" spans="1:13">
@@ -2324,180 +2306,189 @@
         <v>25</v>
       </c>
       <c r="B42" s="6"/>
-      <c r="C42" s="74" t="s">
+      <c r="C42" s="53" t="s">
         <v>69</v>
       </c>
-      <c r="D42" s="75"/>
-      <c r="E42" s="42"/>
+      <c r="D42" s="54"/>
+      <c r="E42" s="41"/>
     </row>
     <row r="43" spans="1:13" ht="15.75" thickBot="1"/>
     <row r="44" spans="1:13">
-      <c r="A44" s="88" t="s">
+      <c r="A44" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="B44" s="89"/>
-      <c r="C44" s="89"/>
-      <c r="D44" s="89"/>
-      <c r="E44" s="89"/>
-      <c r="F44" s="89"/>
-      <c r="G44" s="89"/>
-      <c r="H44" s="89"/>
-      <c r="I44" s="89"/>
-      <c r="J44" s="89"/>
-      <c r="K44" s="89"/>
-      <c r="L44" s="89"/>
+      <c r="B44" s="50"/>
+      <c r="C44" s="50"/>
+      <c r="D44" s="50"/>
+      <c r="E44" s="50"/>
+      <c r="F44" s="50"/>
+      <c r="G44" s="50"/>
+      <c r="H44" s="50"/>
+      <c r="I44" s="50"/>
+      <c r="J44" s="50"/>
+      <c r="K44" s="50"/>
+      <c r="L44" s="50"/>
     </row>
     <row r="45" spans="1:13">
-      <c r="A45" s="37" t="s">
+      <c r="A45" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="B45" s="82" t="s">
+      <c r="B45" s="43" t="s">
         <v>57</v>
       </c>
-      <c r="C45" s="82"/>
-      <c r="D45" s="82"/>
-      <c r="E45" s="82"/>
-      <c r="F45" s="82"/>
-      <c r="G45" s="82"/>
-      <c r="H45" s="82"/>
-      <c r="I45" s="82"/>
-      <c r="J45" s="82"/>
-      <c r="K45" s="82"/>
-      <c r="L45" s="82"/>
+      <c r="C45" s="43"/>
+      <c r="D45" s="43"/>
+      <c r="E45" s="43"/>
+      <c r="F45" s="43"/>
+      <c r="G45" s="43"/>
+      <c r="H45" s="43"/>
+      <c r="I45" s="43"/>
+      <c r="J45" s="43"/>
+      <c r="K45" s="43"/>
+      <c r="L45" s="43"/>
     </row>
     <row r="46" spans="1:13" ht="15" customHeight="1">
-      <c r="A46" s="37" t="s">
+      <c r="A46" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="B46" s="82" t="s">
+      <c r="B46" s="43" t="s">
         <v>58</v>
       </c>
-      <c r="C46" s="82"/>
-      <c r="D46" s="82"/>
-      <c r="E46" s="82"/>
-      <c r="F46" s="82"/>
-      <c r="G46" s="82"/>
-      <c r="H46" s="82"/>
-      <c r="I46" s="82"/>
-      <c r="J46" s="82"/>
-      <c r="K46" s="82"/>
-      <c r="L46" s="82"/>
+      <c r="C46" s="43"/>
+      <c r="D46" s="43"/>
+      <c r="E46" s="43"/>
+      <c r="F46" s="43"/>
+      <c r="G46" s="43"/>
+      <c r="H46" s="43"/>
+      <c r="I46" s="43"/>
+      <c r="J46" s="43"/>
+      <c r="K46" s="43"/>
+      <c r="L46" s="43"/>
     </row>
     <row r="47" spans="1:13">
-      <c r="A47" s="37" t="s">
+      <c r="A47" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="B47" s="82" t="s">
+      <c r="B47" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="C47" s="82"/>
-      <c r="D47" s="82"/>
-      <c r="E47" s="82"/>
-      <c r="F47" s="82"/>
-      <c r="G47" s="82"/>
-      <c r="H47" s="82"/>
-      <c r="I47" s="82"/>
-      <c r="J47" s="82"/>
-      <c r="K47" s="82"/>
-      <c r="L47" s="82"/>
+      <c r="C47" s="43"/>
+      <c r="D47" s="43"/>
+      <c r="E47" s="43"/>
+      <c r="F47" s="43"/>
+      <c r="G47" s="43"/>
+      <c r="H47" s="43"/>
+      <c r="I47" s="43"/>
+      <c r="J47" s="43"/>
+      <c r="K47" s="43"/>
+      <c r="L47" s="43"/>
     </row>
     <row r="48" spans="1:13">
-      <c r="A48" s="37" t="s">
+      <c r="A48" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="B48" s="82" t="s">
+      <c r="B48" s="43" t="s">
         <v>46</v>
       </c>
-      <c r="C48" s="82"/>
-      <c r="D48" s="82"/>
-      <c r="E48" s="82"/>
-      <c r="F48" s="82"/>
-      <c r="G48" s="82"/>
-      <c r="H48" s="82"/>
-      <c r="I48" s="82"/>
-      <c r="J48" s="82"/>
-      <c r="K48" s="82"/>
-      <c r="L48" s="82"/>
+      <c r="C48" s="43"/>
+      <c r="D48" s="43"/>
+      <c r="E48" s="43"/>
+      <c r="F48" s="43"/>
+      <c r="G48" s="43"/>
+      <c r="H48" s="43"/>
+      <c r="I48" s="43"/>
+      <c r="J48" s="43"/>
+      <c r="K48" s="43"/>
+      <c r="L48" s="43"/>
     </row>
     <row r="49" spans="1:12">
-      <c r="A49" s="37" t="s">
+      <c r="A49" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="B49" s="82" t="s">
+      <c r="B49" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="C49" s="82"/>
-      <c r="D49" s="82"/>
-      <c r="E49" s="82"/>
-      <c r="F49" s="82"/>
-      <c r="G49" s="82"/>
-      <c r="H49" s="82"/>
-      <c r="I49" s="82"/>
-      <c r="J49" s="82"/>
-      <c r="K49" s="82"/>
-      <c r="L49" s="82"/>
+      <c r="C49" s="43"/>
+      <c r="D49" s="43"/>
+      <c r="E49" s="43"/>
+      <c r="F49" s="43"/>
+      <c r="G49" s="43"/>
+      <c r="H49" s="43"/>
+      <c r="I49" s="43"/>
+      <c r="J49" s="43"/>
+      <c r="K49" s="43"/>
+      <c r="L49" s="43"/>
     </row>
     <row r="50" spans="1:12">
-      <c r="A50" s="37" t="s">
+      <c r="A50" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="B50" s="82" t="s">
+      <c r="B50" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="C50" s="82"/>
-      <c r="D50" s="82"/>
-      <c r="E50" s="82"/>
-      <c r="F50" s="82"/>
-      <c r="G50" s="82"/>
-      <c r="H50" s="82"/>
-      <c r="I50" s="82"/>
-      <c r="J50" s="82"/>
-      <c r="K50" s="82"/>
-      <c r="L50" s="82"/>
+      <c r="C50" s="43"/>
+      <c r="D50" s="43"/>
+      <c r="E50" s="43"/>
+      <c r="F50" s="43"/>
+      <c r="G50" s="43"/>
+      <c r="H50" s="43"/>
+      <c r="I50" s="43"/>
+      <c r="J50" s="43"/>
+      <c r="K50" s="43"/>
+      <c r="L50" s="43"/>
     </row>
     <row r="51" spans="1:12">
-      <c r="A51" s="37" t="s">
+      <c r="A51" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="B51" s="82" t="s">
+      <c r="B51" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="C51" s="82"/>
-      <c r="D51" s="82"/>
-      <c r="E51" s="82"/>
-      <c r="F51" s="82"/>
-      <c r="G51" s="82"/>
-      <c r="H51" s="82"/>
-      <c r="I51" s="82"/>
-      <c r="J51" s="82"/>
-      <c r="K51" s="82"/>
-      <c r="L51" s="82"/>
+      <c r="C51" s="43"/>
+      <c r="D51" s="43"/>
+      <c r="E51" s="43"/>
+      <c r="F51" s="43"/>
+      <c r="G51" s="43"/>
+      <c r="H51" s="43"/>
+      <c r="I51" s="43"/>
+      <c r="J51" s="43"/>
+      <c r="K51" s="43"/>
+      <c r="L51" s="43"/>
     </row>
     <row r="52" spans="1:12">
-      <c r="C52" s="35"/>
+      <c r="C52" s="34"/>
     </row>
     <row r="53" spans="1:12">
-      <c r="C53" s="35"/>
+      <c r="C53" s="34"/>
     </row>
     <row r="54" spans="1:12">
-      <c r="B54" s="35"/>
+      <c r="B54" s="34"/>
     </row>
   </sheetData>
   <sortState ref="A24:K25">
     <sortCondition ref="A3"/>
   </sortState>
   <mergeCells count="43">
-    <mergeCell ref="B50:L50"/>
-    <mergeCell ref="B51:L51"/>
-    <mergeCell ref="A39:E39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="B45:L45"/>
-    <mergeCell ref="A44:L44"/>
-    <mergeCell ref="B46:L46"/>
-    <mergeCell ref="B47:L47"/>
-    <mergeCell ref="B48:L48"/>
-    <mergeCell ref="B49:L49"/>
+    <mergeCell ref="N6:T6"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="H27:K27"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="H28:K28"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="H30:K30"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="H32:K32"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="H31:L31"/>
     <mergeCell ref="A35:B35"/>
     <mergeCell ref="A36:B36"/>
     <mergeCell ref="A37:B37"/>
@@ -2510,26 +2501,17 @@
     <mergeCell ref="C35:G35"/>
     <mergeCell ref="C36:G36"/>
     <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="H30:K30"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="H32:K32"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="H31:L31"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="H28:K28"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="N6:T6"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="H27:K27"/>
+    <mergeCell ref="B50:L50"/>
+    <mergeCell ref="B51:L51"/>
+    <mergeCell ref="A39:E39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="B45:L45"/>
+    <mergeCell ref="A44:L44"/>
+    <mergeCell ref="B46:L46"/>
+    <mergeCell ref="B47:L47"/>
+    <mergeCell ref="B48:L48"/>
+    <mergeCell ref="B49:L49"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="P4" r:id="rId1"/>

</xml_diff>

<commit_message>
Adaptaciones en las clases DTO para el matcheo con el frontend y excluir informacion, clases Degree, LaboralCarrer, Organization, RolePosition, Studie. Tambien hubo arreglos en el metodo GET para listar segun person id
</commit_message>
<xml_diff>
--- a/Cuadro-de-estado.xlsx
+++ b/Cuadro-de-estado.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="86">
   <si>
     <t>BACKEND</t>
   </si>
@@ -342,22 +342,22 @@
     <t>Agregar atributo en Person, con la url de ubicación de google.maps</t>
   </si>
   <si>
-    <t>La consulta traeria a todas y cualquier modificacion</t>
-  </si>
-  <si>
-    <t>alteraria a todos los Portfolios.</t>
-  </si>
-  <si>
     <t>Aún existen componentes/servicios que apuntan a mock-data</t>
   </si>
   <si>
-    <t>Phone, socialNetwork</t>
-  </si>
-  <si>
     <t>Existe un error que arroja consola this.itemParaBorrar</t>
   </si>
   <si>
     <t>En los Getter de los Form, hay que eliminar espacios de los string</t>
+  </si>
+  <si>
+    <t>modal</t>
+  </si>
+  <si>
+    <t>Integridad, al borrar Organization, RolePosition, etc…. Verificar que no lo tengan otros en sus relaciones</t>
+  </si>
+  <si>
+    <t>En el controller de Person tiene regla de negocio que debe pasar al Service</t>
   </si>
 </sst>
 </file>
@@ -537,7 +537,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -600,12 +600,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1029,7 +1023,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1103,16 +1097,129 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1137,119 +1244,16 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1552,7 +1556,7 @@
   <dimension ref="A1:T54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1569,40 +1573,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="23.25">
-      <c r="A1" s="86" t="s">
+      <c r="A1" s="44" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="86"/>
-      <c r="C1" s="86"/>
-      <c r="D1" s="86"/>
-      <c r="E1" s="86"/>
-      <c r="F1" s="86"/>
-      <c r="G1" s="86"/>
-      <c r="H1" s="86"/>
-      <c r="I1" s="86"/>
-      <c r="J1" s="86"/>
-      <c r="K1" s="86"/>
-      <c r="L1" s="86"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
     </row>
     <row r="2" spans="1:20" ht="15.75" thickBot="1"/>
     <row r="3" spans="1:20" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="87" t="s">
+      <c r="A3" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="88"/>
-      <c r="C3" s="78" t="s">
+      <c r="B3" s="46"/>
+      <c r="C3" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="79"/>
-      <c r="E3" s="79"/>
-      <c r="F3" s="79"/>
-      <c r="G3" s="81"/>
-      <c r="H3" s="78" t="s">
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="79"/>
-      <c r="J3" s="80"/>
-      <c r="K3" s="81"/>
+      <c r="I3" s="48"/>
+      <c r="J3" s="50"/>
+      <c r="K3" s="49"/>
       <c r="L3" s="21" t="s">
         <v>4</v>
       </c>
@@ -1644,10 +1648,10 @@
       <c r="L4" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="N4" s="38" t="s">
+      <c r="N4" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="P4" s="39" t="s">
+      <c r="P4" s="38" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1672,10 +1676,10 @@
       <c r="B6" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="6"/>
+      <c r="D6" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="D6" s="6"/>
       <c r="E6" s="13"/>
       <c r="F6" s="6"/>
       <c r="G6" s="7"/>
@@ -1684,15 +1688,15 @@
       <c r="J6" s="4"/>
       <c r="K6" s="5"/>
       <c r="L6" s="4"/>
-      <c r="N6" s="84" t="s">
+      <c r="N6" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="O6" s="85"/>
-      <c r="P6" s="85"/>
-      <c r="Q6" s="85"/>
-      <c r="R6" s="85"/>
-      <c r="S6" s="85"/>
-      <c r="T6" s="85"/>
+      <c r="O6" s="43"/>
+      <c r="P6" s="43"/>
+      <c r="Q6" s="43"/>
+      <c r="R6" s="43"/>
+      <c r="S6" s="43"/>
+      <c r="T6" s="43"/>
     </row>
     <row r="7" spans="1:20" ht="4.5" customHeight="1">
       <c r="A7" s="29"/>
@@ -1815,40 +1819,47 @@
       <c r="L12" s="31"/>
     </row>
     <row r="13" spans="1:20">
-      <c r="A13" s="37" t="s">
+      <c r="A13" s="88" t="s">
         <v>30</v>
       </c>
       <c r="B13" s="25" t="s">
         <v>13</v>
       </c>
       <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
+      <c r="D13" s="90" t="s">
+        <v>83</v>
+      </c>
+      <c r="E13" s="13"/>
       <c r="F13" s="5"/>
       <c r="G13" s="7"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
       <c r="K13" s="7"/>
-      <c r="L13" s="5"/>
+      <c r="L13" s="4"/>
     </row>
     <row r="14" spans="1:20">
-      <c r="A14" s="37" t="s">
+      <c r="A14" s="88" t="s">
         <v>18</v>
       </c>
       <c r="B14" s="25" t="s">
         <v>13</v>
       </c>
       <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
+      <c r="D14" s="90" t="s">
+        <v>83</v>
+      </c>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
       <c r="G14" s="7"/>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
+      <c r="J14" s="4"/>
       <c r="K14" s="7"/>
       <c r="L14" s="5"/>
+      <c r="N14" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="15" spans="1:20">
       <c r="A15" s="18" t="s">
@@ -1858,31 +1869,33 @@
         <v>12</v>
       </c>
       <c r="C15" s="5"/>
-      <c r="D15" s="16"/>
+      <c r="D15" s="91"/>
       <c r="E15" s="5"/>
       <c r="F15" s="16"/>
       <c r="G15" s="7"/>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
+      <c r="J15" s="4"/>
       <c r="K15" s="7"/>
       <c r="L15" s="5"/>
     </row>
     <row r="16" spans="1:20">
-      <c r="A16" s="37" t="s">
+      <c r="A16" s="88" t="s">
         <v>9</v>
       </c>
       <c r="B16" s="25" t="s">
         <v>13</v>
       </c>
       <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
+      <c r="D16" s="90" t="s">
+        <v>83</v>
+      </c>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
       <c r="G16" s="7"/>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
+      <c r="J16" s="4"/>
       <c r="K16" s="7"/>
       <c r="L16" s="5"/>
       <c r="N16" t="s">
@@ -1899,25 +1912,22 @@
       <c r="B17" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="16"/>
-      <c r="D17" s="8"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="91"/>
       <c r="E17" s="5"/>
-      <c r="F17" s="8"/>
+      <c r="F17" s="16"/>
       <c r="G17" s="7"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="4"/>
       <c r="K17" s="7"/>
-      <c r="L17" s="6"/>
-      <c r="N17" t="s">
-        <v>79</v>
-      </c>
+      <c r="L17" s="5"/>
     </row>
     <row r="18" spans="1:19" ht="4.5" customHeight="1">
       <c r="A18" s="29"/>
       <c r="B18" s="30"/>
       <c r="C18" s="31"/>
-      <c r="D18" s="31"/>
+      <c r="D18" s="30"/>
       <c r="E18" s="31"/>
       <c r="F18" s="31"/>
       <c r="G18" s="31"/>
@@ -1928,14 +1938,16 @@
       <c r="L18" s="31"/>
     </row>
     <row r="19" spans="1:19">
-      <c r="A19" s="37" t="s">
+      <c r="A19" s="89" t="s">
         <v>16</v>
       </c>
       <c r="B19" s="25" t="s">
         <v>13</v>
       </c>
       <c r="C19" s="16"/>
-      <c r="D19" s="8"/>
+      <c r="D19" s="92" t="s">
+        <v>83</v>
+      </c>
       <c r="E19" s="6"/>
       <c r="F19" s="8"/>
       <c r="G19" s="7"/>
@@ -1944,19 +1956,21 @@
       <c r="J19" s="4"/>
       <c r="K19" s="7"/>
       <c r="L19" s="32"/>
-      <c r="O19" t="s">
-        <v>77</v>
+      <c r="N19" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:19">
-      <c r="A20" s="37" t="s">
+      <c r="A20" s="89" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="25" t="s">
         <v>13</v>
       </c>
       <c r="C20" s="16"/>
-      <c r="D20" s="8"/>
+      <c r="D20" s="92" t="s">
+        <v>83</v>
+      </c>
       <c r="E20" s="6"/>
       <c r="F20" s="8"/>
       <c r="G20" s="7"/>
@@ -1981,7 +1995,7 @@
       <c r="L21" s="31"/>
     </row>
     <row r="22" spans="1:19">
-      <c r="A22" s="18" t="s">
+      <c r="A22" s="89" t="s">
         <v>49</v>
       </c>
       <c r="B22" s="20"/>
@@ -1995,9 +2009,6 @@
       <c r="J22" s="4"/>
       <c r="K22" s="7"/>
       <c r="L22" s="4"/>
-      <c r="O22" t="s">
-        <v>80</v>
-      </c>
     </row>
     <row r="23" spans="1:19" ht="4.5" customHeight="1">
       <c r="A23" s="29"/>
@@ -2014,7 +2025,7 @@
       <c r="L23" s="31"/>
     </row>
     <row r="24" spans="1:19">
-      <c r="A24" s="18" t="s">
+      <c r="A24" s="89" t="s">
         <v>50</v>
       </c>
       <c r="B24" s="33"/>
@@ -2028,12 +2039,12 @@
       <c r="J24" s="4"/>
       <c r="K24" s="7"/>
       <c r="L24" s="4"/>
-      <c r="O24" t="s">
-        <v>81</v>
+      <c r="N24" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="25" spans="1:19">
-      <c r="A25" s="18" t="s">
+      <c r="A25" s="89" t="s">
         <v>51</v>
       </c>
       <c r="B25" s="25" t="s">
@@ -2067,44 +2078,44 @@
     <row r="27" spans="1:19" ht="15.75" thickBot="1">
       <c r="A27" s="24"/>
       <c r="B27" s="26"/>
-      <c r="C27" s="78" t="s">
+      <c r="C27" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="79"/>
-      <c r="E27" s="79"/>
-      <c r="F27" s="79"/>
-      <c r="G27" s="81"/>
-      <c r="H27" s="78" t="s">
+      <c r="D27" s="48"/>
+      <c r="E27" s="48"/>
+      <c r="F27" s="48"/>
+      <c r="G27" s="49"/>
+      <c r="H27" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="I27" s="79"/>
-      <c r="J27" s="80"/>
-      <c r="K27" s="81"/>
+      <c r="I27" s="48"/>
+      <c r="J27" s="50"/>
+      <c r="K27" s="49"/>
       <c r="L27" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="N27" s="42" t="s">
-        <v>82</v>
-      </c>
-      <c r="O27" s="42"/>
-      <c r="P27" s="42"/>
-      <c r="Q27" s="42"/>
-      <c r="R27" s="42"/>
+      <c r="N27" s="41" t="s">
+        <v>80</v>
+      </c>
+      <c r="O27" s="41"/>
+      <c r="P27" s="41"/>
+      <c r="Q27" s="41"/>
+      <c r="R27" s="41"/>
     </row>
     <row r="28" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A28" s="82" t="s">
+      <c r="A28" s="54" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="83"/>
-      <c r="C28" s="75"/>
-      <c r="D28" s="76"/>
-      <c r="E28" s="76"/>
-      <c r="F28" s="76"/>
-      <c r="G28" s="77"/>
-      <c r="H28" s="75"/>
-      <c r="I28" s="76"/>
-      <c r="J28" s="76"/>
-      <c r="K28" s="77"/>
+      <c r="B28" s="55"/>
+      <c r="C28" s="51"/>
+      <c r="D28" s="52"/>
+      <c r="E28" s="52"/>
+      <c r="F28" s="52"/>
+      <c r="G28" s="53"/>
+      <c r="H28" s="51"/>
+      <c r="I28" s="52"/>
+      <c r="J28" s="52"/>
+      <c r="K28" s="53"/>
       <c r="L28" s="35"/>
     </row>
     <row r="29" spans="1:19" ht="4.5" customHeight="1">
@@ -2122,338 +2133,346 @@
       <c r="L29" s="31"/>
     </row>
     <row r="30" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A30" s="51" t="s">
+      <c r="A30" s="60" t="s">
         <v>40</v>
       </c>
-      <c r="B30" s="52"/>
-      <c r="C30" s="64"/>
-      <c r="D30" s="65"/>
-      <c r="E30" s="65"/>
-      <c r="F30" s="65"/>
-      <c r="G30" s="66"/>
-      <c r="H30" s="67"/>
-      <c r="I30" s="65"/>
-      <c r="J30" s="65"/>
-      <c r="K30" s="66"/>
+      <c r="B30" s="61"/>
+      <c r="C30" s="56"/>
+      <c r="D30" s="57"/>
+      <c r="E30" s="57"/>
+      <c r="F30" s="57"/>
+      <c r="G30" s="58"/>
+      <c r="H30" s="59"/>
+      <c r="I30" s="57"/>
+      <c r="J30" s="57"/>
+      <c r="K30" s="58"/>
       <c r="L30" s="22" t="s">
         <v>5</v>
       </c>
       <c r="M30" s="34"/>
-      <c r="N30" s="42" t="s">
-        <v>84</v>
-      </c>
-      <c r="O30" s="42"/>
-      <c r="P30" s="42"/>
-      <c r="Q30" s="42"/>
-      <c r="R30" s="42"/>
+      <c r="N30" s="41" t="s">
+        <v>81</v>
+      </c>
+      <c r="O30" s="41"/>
+      <c r="P30" s="41"/>
+      <c r="Q30" s="41"/>
+      <c r="R30" s="41"/>
     </row>
     <row r="31" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A31" s="51" t="s">
+      <c r="A31" s="60" t="s">
         <v>62</v>
       </c>
-      <c r="B31" s="52"/>
-      <c r="C31" s="61"/>
-      <c r="D31" s="62"/>
-      <c r="E31" s="62"/>
-      <c r="F31" s="62"/>
-      <c r="G31" s="63"/>
-      <c r="H31" s="72" t="s">
+      <c r="B31" s="61"/>
+      <c r="C31" s="66"/>
+      <c r="D31" s="67"/>
+      <c r="E31" s="67"/>
+      <c r="F31" s="67"/>
+      <c r="G31" s="68"/>
+      <c r="H31" s="69" t="s">
         <v>61</v>
       </c>
-      <c r="I31" s="73"/>
-      <c r="J31" s="73"/>
-      <c r="K31" s="73"/>
-      <c r="L31" s="74"/>
+      <c r="I31" s="70"/>
+      <c r="J31" s="70"/>
+      <c r="K31" s="70"/>
+      <c r="L31" s="71"/>
       <c r="M31" s="34"/>
     </row>
     <row r="32" spans="1:19" ht="16.5" thickBot="1">
-      <c r="A32" s="70" t="s">
+      <c r="A32" s="64" t="s">
         <v>64</v>
       </c>
-      <c r="B32" s="71"/>
-      <c r="C32" s="64"/>
-      <c r="D32" s="65"/>
-      <c r="E32" s="65"/>
-      <c r="F32" s="65"/>
-      <c r="G32" s="66"/>
-      <c r="H32" s="67"/>
-      <c r="I32" s="65"/>
-      <c r="J32" s="65"/>
-      <c r="K32" s="66"/>
+      <c r="B32" s="65"/>
+      <c r="C32" s="56"/>
+      <c r="D32" s="57"/>
+      <c r="E32" s="57"/>
+      <c r="F32" s="57"/>
+      <c r="G32" s="58"/>
+      <c r="H32" s="59"/>
+      <c r="I32" s="57"/>
+      <c r="J32" s="57"/>
+      <c r="K32" s="58"/>
       <c r="M32" s="34"/>
-      <c r="N32" s="42" t="s">
-        <v>85</v>
-      </c>
-      <c r="O32" s="42"/>
-      <c r="P32" s="42"/>
-      <c r="Q32" s="42"/>
-      <c r="R32" s="42"/>
-      <c r="S32" s="42"/>
-    </row>
-    <row r="33" spans="1:13" ht="30.75" customHeight="1" thickBot="1">
-      <c r="A33" s="68" t="s">
+      <c r="N32" s="41" t="s">
+        <v>82</v>
+      </c>
+      <c r="O32" s="41"/>
+      <c r="P32" s="41"/>
+      <c r="Q32" s="41"/>
+      <c r="R32" s="41"/>
+      <c r="S32" s="41"/>
+    </row>
+    <row r="33" spans="1:19" ht="30.75" customHeight="1" thickBot="1">
+      <c r="A33" s="62" t="s">
         <v>36</v>
       </c>
-      <c r="B33" s="69"/>
-      <c r="C33" s="58" t="s">
+      <c r="B33" s="63"/>
+      <c r="C33" s="77" t="s">
         <v>63</v>
       </c>
-      <c r="D33" s="59"/>
-      <c r="E33" s="59"/>
-      <c r="F33" s="59"/>
-      <c r="G33" s="60"/>
-      <c r="H33" s="55"/>
-      <c r="I33" s="56"/>
-      <c r="J33" s="56"/>
-      <c r="K33" s="57"/>
+      <c r="D33" s="78"/>
+      <c r="E33" s="78"/>
+      <c r="F33" s="78"/>
+      <c r="G33" s="79"/>
+      <c r="H33" s="74"/>
+      <c r="I33" s="75"/>
+      <c r="J33" s="75"/>
+      <c r="K33" s="76"/>
       <c r="M33" s="34"/>
     </row>
-    <row r="34" spans="1:13" ht="4.5" customHeight="1" thickBot="1">
+    <row r="34" spans="1:19" ht="4.5" customHeight="1" thickBot="1">
       <c r="A34" s="29"/>
       <c r="B34" s="30"/>
-      <c r="C34" s="40"/>
-      <c r="D34" s="40"/>
-      <c r="E34" s="40"/>
-      <c r="F34" s="40"/>
-      <c r="G34" s="40"/>
+      <c r="C34" s="39"/>
+      <c r="D34" s="39"/>
+      <c r="E34" s="39"/>
+      <c r="F34" s="39"/>
+      <c r="G34" s="39"/>
       <c r="H34" s="31"/>
       <c r="I34" s="31"/>
       <c r="J34" s="31"/>
       <c r="K34" s="31"/>
     </row>
-    <row r="35" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A35" s="51" t="s">
+    <row r="35" spans="1:19" ht="15.75" thickBot="1">
+      <c r="A35" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="52"/>
-      <c r="C35" s="61"/>
-      <c r="D35" s="62"/>
-      <c r="E35" s="62"/>
-      <c r="F35" s="62"/>
-      <c r="G35" s="63"/>
-      <c r="H35" s="61"/>
-      <c r="I35" s="62"/>
-      <c r="J35" s="62"/>
-      <c r="K35" s="63"/>
+      <c r="B35" s="61"/>
+      <c r="C35" s="66"/>
+      <c r="D35" s="67"/>
+      <c r="E35" s="67"/>
+      <c r="F35" s="67"/>
+      <c r="G35" s="68"/>
+      <c r="H35" s="66"/>
+      <c r="I35" s="67"/>
+      <c r="J35" s="67"/>
+      <c r="K35" s="68"/>
       <c r="M35" s="34"/>
-    </row>
-    <row r="36" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A36" s="51" t="s">
+      <c r="N35" s="41" t="s">
+        <v>85</v>
+      </c>
+      <c r="O35" s="41"/>
+      <c r="P35" s="41"/>
+      <c r="Q35" s="41"/>
+      <c r="R35" s="41"/>
+      <c r="S35" s="41"/>
+    </row>
+    <row r="36" spans="1:19" ht="15.75" thickBot="1">
+      <c r="A36" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="52"/>
-      <c r="C36" s="61"/>
-      <c r="D36" s="62"/>
-      <c r="E36" s="62"/>
-      <c r="F36" s="62"/>
-      <c r="G36" s="63"/>
-      <c r="H36" s="61"/>
-      <c r="I36" s="62"/>
-      <c r="J36" s="62"/>
-      <c r="K36" s="63"/>
+      <c r="B36" s="61"/>
+      <c r="C36" s="66"/>
+      <c r="D36" s="67"/>
+      <c r="E36" s="67"/>
+      <c r="F36" s="67"/>
+      <c r="G36" s="68"/>
+      <c r="H36" s="66"/>
+      <c r="I36" s="67"/>
+      <c r="J36" s="67"/>
+      <c r="K36" s="68"/>
       <c r="M36" s="34"/>
     </row>
-    <row r="37" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A37" s="51" t="s">
+    <row r="37" spans="1:19" ht="15.75" thickBot="1">
+      <c r="A37" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="B37" s="52"/>
-      <c r="C37" s="61"/>
-      <c r="D37" s="62"/>
-      <c r="E37" s="62"/>
-      <c r="F37" s="62"/>
-      <c r="G37" s="63"/>
-      <c r="H37" s="61"/>
-      <c r="I37" s="62"/>
-      <c r="J37" s="62"/>
-      <c r="K37" s="63"/>
+      <c r="B37" s="61"/>
+      <c r="C37" s="66"/>
+      <c r="D37" s="67"/>
+      <c r="E37" s="67"/>
+      <c r="F37" s="67"/>
+      <c r="G37" s="68"/>
+      <c r="H37" s="66"/>
+      <c r="I37" s="67"/>
+      <c r="J37" s="67"/>
+      <c r="K37" s="68"/>
       <c r="M37" s="34"/>
     </row>
-    <row r="38" spans="1:13" ht="15.75" thickBot="1"/>
-    <row r="39" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A39" s="44" t="s">
+    <row r="38" spans="1:19" ht="15.75" thickBot="1"/>
+    <row r="39" spans="1:19" ht="15.75" thickBot="1">
+      <c r="A39" s="81" t="s">
         <v>27</v>
       </c>
-      <c r="B39" s="45"/>
-      <c r="C39" s="45"/>
-      <c r="D39" s="45"/>
-      <c r="E39" s="46"/>
-    </row>
-    <row r="40" spans="1:13">
+      <c r="B39" s="82"/>
+      <c r="C39" s="82"/>
+      <c r="D39" s="82"/>
+      <c r="E39" s="83"/>
+    </row>
+    <row r="40" spans="1:19">
       <c r="A40" s="14" t="s">
         <v>26</v>
       </c>
       <c r="B40" s="13"/>
-      <c r="C40" s="47" t="s">
+      <c r="C40" s="84" t="s">
         <v>23</v>
       </c>
-      <c r="D40" s="48"/>
+      <c r="D40" s="85"/>
       <c r="E40" s="28"/>
     </row>
-    <row r="41" spans="1:13">
+    <row r="41" spans="1:19">
       <c r="A41" s="15" t="s">
         <v>22</v>
       </c>
       <c r="B41" s="5"/>
-      <c r="C41" s="47" t="s">
+      <c r="C41" s="84" t="s">
         <v>24</v>
       </c>
-      <c r="D41" s="48"/>
+      <c r="D41" s="85"/>
       <c r="E41" s="8"/>
     </row>
-    <row r="42" spans="1:13">
+    <row r="42" spans="1:19">
       <c r="A42" s="15" t="s">
         <v>25</v>
       </c>
       <c r="B42" s="6"/>
-      <c r="C42" s="53" t="s">
+      <c r="C42" s="72" t="s">
         <v>69</v>
       </c>
-      <c r="D42" s="54"/>
-      <c r="E42" s="41"/>
-    </row>
-    <row r="43" spans="1:13" ht="15.75" thickBot="1"/>
-    <row r="44" spans="1:13">
-      <c r="A44" s="49" t="s">
+      <c r="D42" s="73"/>
+      <c r="E42" s="40"/>
+    </row>
+    <row r="43" spans="1:19" ht="15.75" thickBot="1"/>
+    <row r="44" spans="1:19">
+      <c r="A44" s="86" t="s">
         <v>37</v>
       </c>
-      <c r="B44" s="50"/>
-      <c r="C44" s="50"/>
-      <c r="D44" s="50"/>
-      <c r="E44" s="50"/>
-      <c r="F44" s="50"/>
-      <c r="G44" s="50"/>
-      <c r="H44" s="50"/>
-      <c r="I44" s="50"/>
-      <c r="J44" s="50"/>
-      <c r="K44" s="50"/>
-      <c r="L44" s="50"/>
-    </row>
-    <row r="45" spans="1:13">
+      <c r="B44" s="87"/>
+      <c r="C44" s="87"/>
+      <c r="D44" s="87"/>
+      <c r="E44" s="87"/>
+      <c r="F44" s="87"/>
+      <c r="G44" s="87"/>
+      <c r="H44" s="87"/>
+      <c r="I44" s="87"/>
+      <c r="J44" s="87"/>
+      <c r="K44" s="87"/>
+      <c r="L44" s="87"/>
+    </row>
+    <row r="45" spans="1:19">
       <c r="A45" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="B45" s="43" t="s">
+      <c r="B45" s="80" t="s">
         <v>57</v>
       </c>
-      <c r="C45" s="43"/>
-      <c r="D45" s="43"/>
-      <c r="E45" s="43"/>
-      <c r="F45" s="43"/>
-      <c r="G45" s="43"/>
-      <c r="H45" s="43"/>
-      <c r="I45" s="43"/>
-      <c r="J45" s="43"/>
-      <c r="K45" s="43"/>
-      <c r="L45" s="43"/>
-    </row>
-    <row r="46" spans="1:13" ht="15" customHeight="1">
+      <c r="C45" s="80"/>
+      <c r="D45" s="80"/>
+      <c r="E45" s="80"/>
+      <c r="F45" s="80"/>
+      <c r="G45" s="80"/>
+      <c r="H45" s="80"/>
+      <c r="I45" s="80"/>
+      <c r="J45" s="80"/>
+      <c r="K45" s="80"/>
+      <c r="L45" s="80"/>
+    </row>
+    <row r="46" spans="1:19" ht="15" customHeight="1">
       <c r="A46" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="B46" s="43" t="s">
+      <c r="B46" s="80" t="s">
         <v>58</v>
       </c>
-      <c r="C46" s="43"/>
-      <c r="D46" s="43"/>
-      <c r="E46" s="43"/>
-      <c r="F46" s="43"/>
-      <c r="G46" s="43"/>
-      <c r="H46" s="43"/>
-      <c r="I46" s="43"/>
-      <c r="J46" s="43"/>
-      <c r="K46" s="43"/>
-      <c r="L46" s="43"/>
-    </row>
-    <row r="47" spans="1:13">
+      <c r="C46" s="80"/>
+      <c r="D46" s="80"/>
+      <c r="E46" s="80"/>
+      <c r="F46" s="80"/>
+      <c r="G46" s="80"/>
+      <c r="H46" s="80"/>
+      <c r="I46" s="80"/>
+      <c r="J46" s="80"/>
+      <c r="K46" s="80"/>
+      <c r="L46" s="80"/>
+    </row>
+    <row r="47" spans="1:19">
       <c r="A47" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="B47" s="43" t="s">
+      <c r="B47" s="80" t="s">
         <v>59</v>
       </c>
-      <c r="C47" s="43"/>
-      <c r="D47" s="43"/>
-      <c r="E47" s="43"/>
-      <c r="F47" s="43"/>
-      <c r="G47" s="43"/>
-      <c r="H47" s="43"/>
-      <c r="I47" s="43"/>
-      <c r="J47" s="43"/>
-      <c r="K47" s="43"/>
-      <c r="L47" s="43"/>
-    </row>
-    <row r="48" spans="1:13">
+      <c r="C47" s="80"/>
+      <c r="D47" s="80"/>
+      <c r="E47" s="80"/>
+      <c r="F47" s="80"/>
+      <c r="G47" s="80"/>
+      <c r="H47" s="80"/>
+      <c r="I47" s="80"/>
+      <c r="J47" s="80"/>
+      <c r="K47" s="80"/>
+      <c r="L47" s="80"/>
+    </row>
+    <row r="48" spans="1:19">
       <c r="A48" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="B48" s="43" t="s">
+      <c r="B48" s="80" t="s">
         <v>46</v>
       </c>
-      <c r="C48" s="43"/>
-      <c r="D48" s="43"/>
-      <c r="E48" s="43"/>
-      <c r="F48" s="43"/>
-      <c r="G48" s="43"/>
-      <c r="H48" s="43"/>
-      <c r="I48" s="43"/>
-      <c r="J48" s="43"/>
-      <c r="K48" s="43"/>
-      <c r="L48" s="43"/>
+      <c r="C48" s="80"/>
+      <c r="D48" s="80"/>
+      <c r="E48" s="80"/>
+      <c r="F48" s="80"/>
+      <c r="G48" s="80"/>
+      <c r="H48" s="80"/>
+      <c r="I48" s="80"/>
+      <c r="J48" s="80"/>
+      <c r="K48" s="80"/>
+      <c r="L48" s="80"/>
     </row>
     <row r="49" spans="1:12">
       <c r="A49" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="B49" s="43" t="s">
+      <c r="B49" s="80" t="s">
         <v>35</v>
       </c>
-      <c r="C49" s="43"/>
-      <c r="D49" s="43"/>
-      <c r="E49" s="43"/>
-      <c r="F49" s="43"/>
-      <c r="G49" s="43"/>
-      <c r="H49" s="43"/>
-      <c r="I49" s="43"/>
-      <c r="J49" s="43"/>
-      <c r="K49" s="43"/>
-      <c r="L49" s="43"/>
+      <c r="C49" s="80"/>
+      <c r="D49" s="80"/>
+      <c r="E49" s="80"/>
+      <c r="F49" s="80"/>
+      <c r="G49" s="80"/>
+      <c r="H49" s="80"/>
+      <c r="I49" s="80"/>
+      <c r="J49" s="80"/>
+      <c r="K49" s="80"/>
+      <c r="L49" s="80"/>
     </row>
     <row r="50" spans="1:12">
       <c r="A50" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="B50" s="43" t="s">
+      <c r="B50" s="80" t="s">
         <v>56</v>
       </c>
-      <c r="C50" s="43"/>
-      <c r="D50" s="43"/>
-      <c r="E50" s="43"/>
-      <c r="F50" s="43"/>
-      <c r="G50" s="43"/>
-      <c r="H50" s="43"/>
-      <c r="I50" s="43"/>
-      <c r="J50" s="43"/>
-      <c r="K50" s="43"/>
-      <c r="L50" s="43"/>
+      <c r="C50" s="80"/>
+      <c r="D50" s="80"/>
+      <c r="E50" s="80"/>
+      <c r="F50" s="80"/>
+      <c r="G50" s="80"/>
+      <c r="H50" s="80"/>
+      <c r="I50" s="80"/>
+      <c r="J50" s="80"/>
+      <c r="K50" s="80"/>
+      <c r="L50" s="80"/>
     </row>
     <row r="51" spans="1:12">
       <c r="A51" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="B51" s="43" t="s">
+      <c r="B51" s="80" t="s">
         <v>55</v>
       </c>
-      <c r="C51" s="43"/>
-      <c r="D51" s="43"/>
-      <c r="E51" s="43"/>
-      <c r="F51" s="43"/>
-      <c r="G51" s="43"/>
-      <c r="H51" s="43"/>
-      <c r="I51" s="43"/>
-      <c r="J51" s="43"/>
-      <c r="K51" s="43"/>
-      <c r="L51" s="43"/>
+      <c r="C51" s="80"/>
+      <c r="D51" s="80"/>
+      <c r="E51" s="80"/>
+      <c r="F51" s="80"/>
+      <c r="G51" s="80"/>
+      <c r="H51" s="80"/>
+      <c r="I51" s="80"/>
+      <c r="J51" s="80"/>
+      <c r="K51" s="80"/>
+      <c r="L51" s="80"/>
     </row>
     <row r="52" spans="1:12">
       <c r="C52" s="34"/>
@@ -2469,26 +2488,17 @@
     <sortCondition ref="A3"/>
   </sortState>
   <mergeCells count="43">
-    <mergeCell ref="N6:T6"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="H27:K27"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="H28:K28"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="H30:K30"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="H32:K32"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="H31:L31"/>
+    <mergeCell ref="B50:L50"/>
+    <mergeCell ref="B51:L51"/>
+    <mergeCell ref="A39:E39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="B45:L45"/>
+    <mergeCell ref="A44:L44"/>
+    <mergeCell ref="B46:L46"/>
+    <mergeCell ref="B47:L47"/>
+    <mergeCell ref="B48:L48"/>
+    <mergeCell ref="B49:L49"/>
     <mergeCell ref="A35:B35"/>
     <mergeCell ref="A36:B36"/>
     <mergeCell ref="A37:B37"/>
@@ -2501,17 +2511,26 @@
     <mergeCell ref="C35:G35"/>
     <mergeCell ref="C36:G36"/>
     <mergeCell ref="C37:G37"/>
-    <mergeCell ref="B50:L50"/>
-    <mergeCell ref="B51:L51"/>
-    <mergeCell ref="A39:E39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="B45:L45"/>
-    <mergeCell ref="A44:L44"/>
-    <mergeCell ref="B46:L46"/>
-    <mergeCell ref="B47:L47"/>
-    <mergeCell ref="B48:L48"/>
-    <mergeCell ref="B49:L49"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="H30:K30"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="H32:K32"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="H31:L31"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="H28:K28"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="N6:T6"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="H27:K27"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="P4" r:id="rId1"/>

</xml_diff>

<commit_message>
actualizado cuadro de estado, y cambio en studie-form-component
</commit_message>
<xml_diff>
--- a/Cuadro-de-estado.xlsx
+++ b/Cuadro-de-estado.xlsx
@@ -354,10 +354,10 @@
     <t>modal</t>
   </si>
   <si>
-    <t>Integridad, al borrar Organization, RolePosition, etc…. Verificar que no lo tengan otros en sus relaciones</t>
-  </si>
-  <si>
     <t>En el controller de Person tiene regla de negocio que debe pasar al Service</t>
+  </si>
+  <si>
+    <t>Integridad, al borrar Organization, RolePosition, Degree. Ojo con la relacion en LaboralCareer y Studie</t>
   </si>
 </sst>
 </file>
@@ -1023,7 +1023,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1106,144 +1106,6 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1254,6 +1116,147 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1556,7 +1559,7 @@
   <dimension ref="A1:T54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1573,40 +1576,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="23.25">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="90" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
+      <c r="B1" s="90"/>
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="90"/>
+      <c r="F1" s="90"/>
+      <c r="G1" s="90"/>
+      <c r="H1" s="90"/>
+      <c r="I1" s="90"/>
+      <c r="J1" s="90"/>
+      <c r="K1" s="90"/>
+      <c r="L1" s="90"/>
     </row>
     <row r="2" spans="1:20" ht="15.75" thickBot="1"/>
     <row r="3" spans="1:20" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="91" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="46"/>
-      <c r="C3" s="47" t="s">
+      <c r="B3" s="92"/>
+      <c r="C3" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="49"/>
-      <c r="H3" s="47" t="s">
+      <c r="D3" s="83"/>
+      <c r="E3" s="83"/>
+      <c r="F3" s="83"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="82" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="48"/>
-      <c r="J3" s="50"/>
-      <c r="K3" s="49"/>
+      <c r="I3" s="83"/>
+      <c r="J3" s="84"/>
+      <c r="K3" s="85"/>
       <c r="L3" s="21" t="s">
         <v>4</v>
       </c>
@@ -1688,15 +1691,15 @@
       <c r="J6" s="4"/>
       <c r="K6" s="5"/>
       <c r="L6" s="4"/>
-      <c r="N6" s="42" t="s">
+      <c r="N6" s="88" t="s">
         <v>70</v>
       </c>
-      <c r="O6" s="43"/>
-      <c r="P6" s="43"/>
-      <c r="Q6" s="43"/>
-      <c r="R6" s="43"/>
-      <c r="S6" s="43"/>
-      <c r="T6" s="43"/>
+      <c r="O6" s="89"/>
+      <c r="P6" s="89"/>
+      <c r="Q6" s="89"/>
+      <c r="R6" s="89"/>
+      <c r="S6" s="89"/>
+      <c r="T6" s="89"/>
     </row>
     <row r="7" spans="1:20" ht="4.5" customHeight="1">
       <c r="A7" s="29"/>
@@ -1819,14 +1822,14 @@
       <c r="L12" s="31"/>
     </row>
     <row r="13" spans="1:20">
-      <c r="A13" s="88" t="s">
+      <c r="A13" s="42" t="s">
         <v>30</v>
       </c>
       <c r="B13" s="25" t="s">
         <v>13</v>
       </c>
       <c r="C13" s="5"/>
-      <c r="D13" s="90" t="s">
+      <c r="D13" s="44" t="s">
         <v>83</v>
       </c>
       <c r="E13" s="13"/>
@@ -1839,14 +1842,14 @@
       <c r="L13" s="4"/>
     </row>
     <row r="14" spans="1:20">
-      <c r="A14" s="88" t="s">
+      <c r="A14" s="42" t="s">
         <v>18</v>
       </c>
       <c r="B14" s="25" t="s">
         <v>13</v>
       </c>
       <c r="C14" s="5"/>
-      <c r="D14" s="90" t="s">
+      <c r="D14" s="44" t="s">
         <v>83</v>
       </c>
       <c r="E14" s="5"/>
@@ -1857,9 +1860,14 @@
       <c r="J14" s="4"/>
       <c r="K14" s="7"/>
       <c r="L14" s="5"/>
-      <c r="N14" t="s">
-        <v>84</v>
-      </c>
+      <c r="N14" s="93" t="s">
+        <v>85</v>
+      </c>
+      <c r="O14" s="93"/>
+      <c r="P14" s="93"/>
+      <c r="Q14" s="93"/>
+      <c r="R14" s="93"/>
+      <c r="S14" s="93"/>
     </row>
     <row r="15" spans="1:20">
       <c r="A15" s="18" t="s">
@@ -1869,7 +1877,7 @@
         <v>12</v>
       </c>
       <c r="C15" s="5"/>
-      <c r="D15" s="91"/>
+      <c r="D15" s="45"/>
       <c r="E15" s="5"/>
       <c r="F15" s="16"/>
       <c r="G15" s="7"/>
@@ -1878,16 +1886,22 @@
       <c r="J15" s="4"/>
       <c r="K15" s="7"/>
       <c r="L15" s="5"/>
+      <c r="N15" s="93"/>
+      <c r="O15" s="93"/>
+      <c r="P15" s="93"/>
+      <c r="Q15" s="93"/>
+      <c r="R15" s="93"/>
+      <c r="S15" s="93"/>
     </row>
     <row r="16" spans="1:20">
-      <c r="A16" s="88" t="s">
+      <c r="A16" s="42" t="s">
         <v>9</v>
       </c>
       <c r="B16" s="25" t="s">
         <v>13</v>
       </c>
       <c r="C16" s="5"/>
-      <c r="D16" s="90" t="s">
+      <c r="D16" s="44" t="s">
         <v>83</v>
       </c>
       <c r="E16" s="5"/>
@@ -1898,12 +1912,6 @@
       <c r="J16" s="4"/>
       <c r="K16" s="7"/>
       <c r="L16" s="5"/>
-      <c r="N16" t="s">
-        <v>75</v>
-      </c>
-      <c r="O16" t="s">
-        <v>76</v>
-      </c>
     </row>
     <row r="17" spans="1:19">
       <c r="A17" s="18" t="s">
@@ -1913,7 +1921,7 @@
         <v>12</v>
       </c>
       <c r="C17" s="5"/>
-      <c r="D17" s="91"/>
+      <c r="D17" s="45"/>
       <c r="E17" s="5"/>
       <c r="F17" s="16"/>
       <c r="G17" s="7"/>
@@ -1938,14 +1946,14 @@
       <c r="L18" s="31"/>
     </row>
     <row r="19" spans="1:19">
-      <c r="A19" s="89" t="s">
+      <c r="A19" s="43" t="s">
         <v>16</v>
       </c>
       <c r="B19" s="25" t="s">
         <v>13</v>
       </c>
       <c r="C19" s="16"/>
-      <c r="D19" s="92" t="s">
+      <c r="D19" s="46" t="s">
         <v>83</v>
       </c>
       <c r="E19" s="6"/>
@@ -1961,14 +1969,14 @@
       </c>
     </row>
     <row r="20" spans="1:19">
-      <c r="A20" s="89" t="s">
+      <c r="A20" s="43" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="25" t="s">
         <v>13</v>
       </c>
       <c r="C20" s="16"/>
-      <c r="D20" s="92" t="s">
+      <c r="D20" s="46" t="s">
         <v>83</v>
       </c>
       <c r="E20" s="6"/>
@@ -1995,7 +2003,7 @@
       <c r="L21" s="31"/>
     </row>
     <row r="22" spans="1:19">
-      <c r="A22" s="89" t="s">
+      <c r="A22" s="43" t="s">
         <v>49</v>
       </c>
       <c r="B22" s="20"/>
@@ -2025,7 +2033,7 @@
       <c r="L23" s="31"/>
     </row>
     <row r="24" spans="1:19">
-      <c r="A24" s="89" t="s">
+      <c r="A24" s="43" t="s">
         <v>50</v>
       </c>
       <c r="B24" s="33"/>
@@ -2040,11 +2048,14 @@
       <c r="K24" s="7"/>
       <c r="L24" s="4"/>
       <c r="N24" t="s">
-        <v>77</v>
+        <v>75</v>
+      </c>
+      <c r="O24" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="25" spans="1:19">
-      <c r="A25" s="89" t="s">
+      <c r="A25" s="43" t="s">
         <v>51</v>
       </c>
       <c r="B25" s="25" t="s">
@@ -2060,6 +2071,9 @@
       <c r="J25" s="7"/>
       <c r="K25" s="7"/>
       <c r="L25" s="7"/>
+      <c r="N25" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="26" spans="1:19" ht="4.5" customHeight="1" thickBot="1">
       <c r="A26" s="29"/>
@@ -2078,19 +2092,19 @@
     <row r="27" spans="1:19" ht="15.75" thickBot="1">
       <c r="A27" s="24"/>
       <c r="B27" s="26"/>
-      <c r="C27" s="47" t="s">
+      <c r="C27" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="48"/>
-      <c r="E27" s="48"/>
-      <c r="F27" s="48"/>
-      <c r="G27" s="49"/>
-      <c r="H27" s="47" t="s">
+      <c r="D27" s="83"/>
+      <c r="E27" s="83"/>
+      <c r="F27" s="83"/>
+      <c r="G27" s="85"/>
+      <c r="H27" s="82" t="s">
         <v>0</v>
       </c>
-      <c r="I27" s="48"/>
-      <c r="J27" s="50"/>
-      <c r="K27" s="49"/>
+      <c r="I27" s="83"/>
+      <c r="J27" s="84"/>
+      <c r="K27" s="85"/>
       <c r="L27" s="21" t="s">
         <v>4</v>
       </c>
@@ -2103,20 +2117,27 @@
       <c r="R27" s="41"/>
     </row>
     <row r="28" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A28" s="54" t="s">
+      <c r="A28" s="86" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="55"/>
-      <c r="C28" s="51"/>
-      <c r="D28" s="52"/>
-      <c r="E28" s="52"/>
-      <c r="F28" s="52"/>
-      <c r="G28" s="53"/>
-      <c r="H28" s="51"/>
-      <c r="I28" s="52"/>
-      <c r="J28" s="52"/>
-      <c r="K28" s="53"/>
+      <c r="B28" s="87"/>
+      <c r="C28" s="79"/>
+      <c r="D28" s="80"/>
+      <c r="E28" s="80"/>
+      <c r="F28" s="80"/>
+      <c r="G28" s="81"/>
+      <c r="H28" s="79"/>
+      <c r="I28" s="80"/>
+      <c r="J28" s="80"/>
+      <c r="K28" s="81"/>
       <c r="L28" s="35"/>
+      <c r="N28" s="41" t="s">
+        <v>81</v>
+      </c>
+      <c r="O28" s="41"/>
+      <c r="P28" s="41"/>
+      <c r="Q28" s="41"/>
+      <c r="R28" s="41"/>
     </row>
     <row r="29" spans="1:19" ht="4.5" customHeight="1">
       <c r="A29" s="29"/>
@@ -2133,67 +2154,68 @@
       <c r="L29" s="31"/>
     </row>
     <row r="30" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A30" s="60" t="s">
+      <c r="A30" s="55" t="s">
         <v>40</v>
       </c>
-      <c r="B30" s="61"/>
-      <c r="C30" s="56"/>
-      <c r="D30" s="57"/>
-      <c r="E30" s="57"/>
-      <c r="F30" s="57"/>
-      <c r="G30" s="58"/>
-      <c r="H30" s="59"/>
-      <c r="I30" s="57"/>
-      <c r="J30" s="57"/>
-      <c r="K30" s="58"/>
+      <c r="B30" s="56"/>
+      <c r="C30" s="68"/>
+      <c r="D30" s="69"/>
+      <c r="E30" s="69"/>
+      <c r="F30" s="69"/>
+      <c r="G30" s="70"/>
+      <c r="H30" s="71"/>
+      <c r="I30" s="69"/>
+      <c r="J30" s="69"/>
+      <c r="K30" s="70"/>
       <c r="L30" s="22" t="s">
         <v>5</v>
       </c>
       <c r="M30" s="34"/>
       <c r="N30" s="41" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="O30" s="41"/>
       <c r="P30" s="41"/>
       <c r="Q30" s="41"/>
       <c r="R30" s="41"/>
+      <c r="S30" s="41"/>
     </row>
     <row r="31" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A31" s="60" t="s">
+      <c r="A31" s="55" t="s">
         <v>62</v>
       </c>
-      <c r="B31" s="61"/>
-      <c r="C31" s="66"/>
-      <c r="D31" s="67"/>
-      <c r="E31" s="67"/>
-      <c r="F31" s="67"/>
-      <c r="G31" s="68"/>
-      <c r="H31" s="69" t="s">
+      <c r="B31" s="56"/>
+      <c r="C31" s="65"/>
+      <c r="D31" s="66"/>
+      <c r="E31" s="66"/>
+      <c r="F31" s="66"/>
+      <c r="G31" s="67"/>
+      <c r="H31" s="76" t="s">
         <v>61</v>
       </c>
-      <c r="I31" s="70"/>
-      <c r="J31" s="70"/>
-      <c r="K31" s="70"/>
-      <c r="L31" s="71"/>
+      <c r="I31" s="77"/>
+      <c r="J31" s="77"/>
+      <c r="K31" s="77"/>
+      <c r="L31" s="78"/>
       <c r="M31" s="34"/>
     </row>
     <row r="32" spans="1:19" ht="16.5" thickBot="1">
-      <c r="A32" s="64" t="s">
+      <c r="A32" s="74" t="s">
         <v>64</v>
       </c>
-      <c r="B32" s="65"/>
-      <c r="C32" s="56"/>
-      <c r="D32" s="57"/>
-      <c r="E32" s="57"/>
-      <c r="F32" s="57"/>
-      <c r="G32" s="58"/>
-      <c r="H32" s="59"/>
-      <c r="I32" s="57"/>
-      <c r="J32" s="57"/>
-      <c r="K32" s="58"/>
+      <c r="B32" s="75"/>
+      <c r="C32" s="68"/>
+      <c r="D32" s="69"/>
+      <c r="E32" s="69"/>
+      <c r="F32" s="69"/>
+      <c r="G32" s="70"/>
+      <c r="H32" s="71"/>
+      <c r="I32" s="69"/>
+      <c r="J32" s="69"/>
+      <c r="K32" s="70"/>
       <c r="M32" s="34"/>
       <c r="N32" s="41" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="O32" s="41"/>
       <c r="P32" s="41"/>
@@ -2201,25 +2223,25 @@
       <c r="R32" s="41"/>
       <c r="S32" s="41"/>
     </row>
-    <row r="33" spans="1:19" ht="30.75" customHeight="1" thickBot="1">
-      <c r="A33" s="62" t="s">
+    <row r="33" spans="1:13" ht="30.75" customHeight="1" thickBot="1">
+      <c r="A33" s="72" t="s">
         <v>36</v>
       </c>
-      <c r="B33" s="63"/>
-      <c r="C33" s="77" t="s">
+      <c r="B33" s="73"/>
+      <c r="C33" s="62" t="s">
         <v>63</v>
       </c>
-      <c r="D33" s="78"/>
-      <c r="E33" s="78"/>
-      <c r="F33" s="78"/>
-      <c r="G33" s="79"/>
-      <c r="H33" s="74"/>
-      <c r="I33" s="75"/>
-      <c r="J33" s="75"/>
-      <c r="K33" s="76"/>
+      <c r="D33" s="63"/>
+      <c r="E33" s="63"/>
+      <c r="F33" s="63"/>
+      <c r="G33" s="64"/>
+      <c r="H33" s="59"/>
+      <c r="I33" s="60"/>
+      <c r="J33" s="60"/>
+      <c r="K33" s="61"/>
       <c r="M33" s="34"/>
     </row>
-    <row r="34" spans="1:19" ht="4.5" customHeight="1" thickBot="1">
+    <row r="34" spans="1:13" ht="4.5" customHeight="1" thickBot="1">
       <c r="A34" s="29"/>
       <c r="B34" s="30"/>
       <c r="C34" s="39"/>
@@ -2232,247 +2254,239 @@
       <c r="J34" s="31"/>
       <c r="K34" s="31"/>
     </row>
-    <row r="35" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A35" s="60" t="s">
+    <row r="35" spans="1:13" ht="15.75" thickBot="1">
+      <c r="A35" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="61"/>
-      <c r="C35" s="66"/>
-      <c r="D35" s="67"/>
-      <c r="E35" s="67"/>
-      <c r="F35" s="67"/>
-      <c r="G35" s="68"/>
-      <c r="H35" s="66"/>
-      <c r="I35" s="67"/>
-      <c r="J35" s="67"/>
-      <c r="K35" s="68"/>
+      <c r="B35" s="56"/>
+      <c r="C35" s="65"/>
+      <c r="D35" s="66"/>
+      <c r="E35" s="66"/>
+      <c r="F35" s="66"/>
+      <c r="G35" s="67"/>
+      <c r="H35" s="65"/>
+      <c r="I35" s="66"/>
+      <c r="J35" s="66"/>
+      <c r="K35" s="67"/>
       <c r="M35" s="34"/>
-      <c r="N35" s="41" t="s">
-        <v>85</v>
-      </c>
-      <c r="O35" s="41"/>
-      <c r="P35" s="41"/>
-      <c r="Q35" s="41"/>
-      <c r="R35" s="41"/>
-      <c r="S35" s="41"/>
-    </row>
-    <row r="36" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A36" s="60" t="s">
+    </row>
+    <row r="36" spans="1:13" ht="15.75" thickBot="1">
+      <c r="A36" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="61"/>
-      <c r="C36" s="66"/>
-      <c r="D36" s="67"/>
-      <c r="E36" s="67"/>
-      <c r="F36" s="67"/>
-      <c r="G36" s="68"/>
-      <c r="H36" s="66"/>
-      <c r="I36" s="67"/>
-      <c r="J36" s="67"/>
-      <c r="K36" s="68"/>
+      <c r="B36" s="56"/>
+      <c r="C36" s="65"/>
+      <c r="D36" s="66"/>
+      <c r="E36" s="66"/>
+      <c r="F36" s="66"/>
+      <c r="G36" s="67"/>
+      <c r="H36" s="65"/>
+      <c r="I36" s="66"/>
+      <c r="J36" s="66"/>
+      <c r="K36" s="67"/>
       <c r="M36" s="34"/>
     </row>
-    <row r="37" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A37" s="60" t="s">
+    <row r="37" spans="1:13" ht="15.75" thickBot="1">
+      <c r="A37" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="B37" s="61"/>
-      <c r="C37" s="66"/>
-      <c r="D37" s="67"/>
-      <c r="E37" s="67"/>
-      <c r="F37" s="67"/>
-      <c r="G37" s="68"/>
-      <c r="H37" s="66"/>
-      <c r="I37" s="67"/>
-      <c r="J37" s="67"/>
-      <c r="K37" s="68"/>
+      <c r="B37" s="56"/>
+      <c r="C37" s="65"/>
+      <c r="D37" s="66"/>
+      <c r="E37" s="66"/>
+      <c r="F37" s="66"/>
+      <c r="G37" s="67"/>
+      <c r="H37" s="65"/>
+      <c r="I37" s="66"/>
+      <c r="J37" s="66"/>
+      <c r="K37" s="67"/>
       <c r="M37" s="34"/>
     </row>
-    <row r="38" spans="1:19" ht="15.75" thickBot="1"/>
-    <row r="39" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A39" s="81" t="s">
+    <row r="38" spans="1:13" ht="15.75" thickBot="1"/>
+    <row r="39" spans="1:13" ht="15.75" thickBot="1">
+      <c r="A39" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="B39" s="82"/>
-      <c r="C39" s="82"/>
-      <c r="D39" s="82"/>
-      <c r="E39" s="83"/>
-    </row>
-    <row r="40" spans="1:19">
+      <c r="B39" s="49"/>
+      <c r="C39" s="49"/>
+      <c r="D39" s="49"/>
+      <c r="E39" s="50"/>
+    </row>
+    <row r="40" spans="1:13">
       <c r="A40" s="14" t="s">
         <v>26</v>
       </c>
       <c r="B40" s="13"/>
-      <c r="C40" s="84" t="s">
+      <c r="C40" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="D40" s="85"/>
+      <c r="D40" s="52"/>
       <c r="E40" s="28"/>
     </row>
-    <row r="41" spans="1:19">
+    <row r="41" spans="1:13">
       <c r="A41" s="15" t="s">
         <v>22</v>
       </c>
       <c r="B41" s="5"/>
-      <c r="C41" s="84" t="s">
+      <c r="C41" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="D41" s="85"/>
+      <c r="D41" s="52"/>
       <c r="E41" s="8"/>
     </row>
-    <row r="42" spans="1:19">
+    <row r="42" spans="1:13">
       <c r="A42" s="15" t="s">
         <v>25</v>
       </c>
       <c r="B42" s="6"/>
-      <c r="C42" s="72" t="s">
+      <c r="C42" s="57" t="s">
         <v>69</v>
       </c>
-      <c r="D42" s="73"/>
+      <c r="D42" s="58"/>
       <c r="E42" s="40"/>
     </row>
-    <row r="43" spans="1:19" ht="15.75" thickBot="1"/>
-    <row r="44" spans="1:19">
-      <c r="A44" s="86" t="s">
+    <row r="43" spans="1:13" ht="15.75" thickBot="1"/>
+    <row r="44" spans="1:13">
+      <c r="A44" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="B44" s="87"/>
-      <c r="C44" s="87"/>
-      <c r="D44" s="87"/>
-      <c r="E44" s="87"/>
-      <c r="F44" s="87"/>
-      <c r="G44" s="87"/>
-      <c r="H44" s="87"/>
-      <c r="I44" s="87"/>
-      <c r="J44" s="87"/>
-      <c r="K44" s="87"/>
-      <c r="L44" s="87"/>
-    </row>
-    <row r="45" spans="1:19">
+      <c r="B44" s="54"/>
+      <c r="C44" s="54"/>
+      <c r="D44" s="54"/>
+      <c r="E44" s="54"/>
+      <c r="F44" s="54"/>
+      <c r="G44" s="54"/>
+      <c r="H44" s="54"/>
+      <c r="I44" s="54"/>
+      <c r="J44" s="54"/>
+      <c r="K44" s="54"/>
+      <c r="L44" s="54"/>
+    </row>
+    <row r="45" spans="1:13">
       <c r="A45" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="B45" s="80" t="s">
+      <c r="B45" s="47" t="s">
         <v>57</v>
       </c>
-      <c r="C45" s="80"/>
-      <c r="D45" s="80"/>
-      <c r="E45" s="80"/>
-      <c r="F45" s="80"/>
-      <c r="G45" s="80"/>
-      <c r="H45" s="80"/>
-      <c r="I45" s="80"/>
-      <c r="J45" s="80"/>
-      <c r="K45" s="80"/>
-      <c r="L45" s="80"/>
-    </row>
-    <row r="46" spans="1:19" ht="15" customHeight="1">
+      <c r="C45" s="47"/>
+      <c r="D45" s="47"/>
+      <c r="E45" s="47"/>
+      <c r="F45" s="47"/>
+      <c r="G45" s="47"/>
+      <c r="H45" s="47"/>
+      <c r="I45" s="47"/>
+      <c r="J45" s="47"/>
+      <c r="K45" s="47"/>
+      <c r="L45" s="47"/>
+    </row>
+    <row r="46" spans="1:13" ht="15" customHeight="1">
       <c r="A46" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="B46" s="80" t="s">
+      <c r="B46" s="47" t="s">
         <v>58</v>
       </c>
-      <c r="C46" s="80"/>
-      <c r="D46" s="80"/>
-      <c r="E46" s="80"/>
-      <c r="F46" s="80"/>
-      <c r="G46" s="80"/>
-      <c r="H46" s="80"/>
-      <c r="I46" s="80"/>
-      <c r="J46" s="80"/>
-      <c r="K46" s="80"/>
-      <c r="L46" s="80"/>
-    </row>
-    <row r="47" spans="1:19">
+      <c r="C46" s="47"/>
+      <c r="D46" s="47"/>
+      <c r="E46" s="47"/>
+      <c r="F46" s="47"/>
+      <c r="G46" s="47"/>
+      <c r="H46" s="47"/>
+      <c r="I46" s="47"/>
+      <c r="J46" s="47"/>
+      <c r="K46" s="47"/>
+      <c r="L46" s="47"/>
+    </row>
+    <row r="47" spans="1:13">
       <c r="A47" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="B47" s="80" t="s">
+      <c r="B47" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="C47" s="80"/>
-      <c r="D47" s="80"/>
-      <c r="E47" s="80"/>
-      <c r="F47" s="80"/>
-      <c r="G47" s="80"/>
-      <c r="H47" s="80"/>
-      <c r="I47" s="80"/>
-      <c r="J47" s="80"/>
-      <c r="K47" s="80"/>
-      <c r="L47" s="80"/>
-    </row>
-    <row r="48" spans="1:19">
+      <c r="C47" s="47"/>
+      <c r="D47" s="47"/>
+      <c r="E47" s="47"/>
+      <c r="F47" s="47"/>
+      <c r="G47" s="47"/>
+      <c r="H47" s="47"/>
+      <c r="I47" s="47"/>
+      <c r="J47" s="47"/>
+      <c r="K47" s="47"/>
+      <c r="L47" s="47"/>
+    </row>
+    <row r="48" spans="1:13">
       <c r="A48" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="B48" s="80" t="s">
+      <c r="B48" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="C48" s="80"/>
-      <c r="D48" s="80"/>
-      <c r="E48" s="80"/>
-      <c r="F48" s="80"/>
-      <c r="G48" s="80"/>
-      <c r="H48" s="80"/>
-      <c r="I48" s="80"/>
-      <c r="J48" s="80"/>
-      <c r="K48" s="80"/>
-      <c r="L48" s="80"/>
+      <c r="C48" s="47"/>
+      <c r="D48" s="47"/>
+      <c r="E48" s="47"/>
+      <c r="F48" s="47"/>
+      <c r="G48" s="47"/>
+      <c r="H48" s="47"/>
+      <c r="I48" s="47"/>
+      <c r="J48" s="47"/>
+      <c r="K48" s="47"/>
+      <c r="L48" s="47"/>
     </row>
     <row r="49" spans="1:12">
       <c r="A49" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="B49" s="80" t="s">
+      <c r="B49" s="47" t="s">
         <v>35</v>
       </c>
-      <c r="C49" s="80"/>
-      <c r="D49" s="80"/>
-      <c r="E49" s="80"/>
-      <c r="F49" s="80"/>
-      <c r="G49" s="80"/>
-      <c r="H49" s="80"/>
-      <c r="I49" s="80"/>
-      <c r="J49" s="80"/>
-      <c r="K49" s="80"/>
-      <c r="L49" s="80"/>
+      <c r="C49" s="47"/>
+      <c r="D49" s="47"/>
+      <c r="E49" s="47"/>
+      <c r="F49" s="47"/>
+      <c r="G49" s="47"/>
+      <c r="H49" s="47"/>
+      <c r="I49" s="47"/>
+      <c r="J49" s="47"/>
+      <c r="K49" s="47"/>
+      <c r="L49" s="47"/>
     </row>
     <row r="50" spans="1:12">
       <c r="A50" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="B50" s="80" t="s">
+      <c r="B50" s="47" t="s">
         <v>56</v>
       </c>
-      <c r="C50" s="80"/>
-      <c r="D50" s="80"/>
-      <c r="E50" s="80"/>
-      <c r="F50" s="80"/>
-      <c r="G50" s="80"/>
-      <c r="H50" s="80"/>
-      <c r="I50" s="80"/>
-      <c r="J50" s="80"/>
-      <c r="K50" s="80"/>
-      <c r="L50" s="80"/>
+      <c r="C50" s="47"/>
+      <c r="D50" s="47"/>
+      <c r="E50" s="47"/>
+      <c r="F50" s="47"/>
+      <c r="G50" s="47"/>
+      <c r="H50" s="47"/>
+      <c r="I50" s="47"/>
+      <c r="J50" s="47"/>
+      <c r="K50" s="47"/>
+      <c r="L50" s="47"/>
     </row>
     <row r="51" spans="1:12">
       <c r="A51" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="B51" s="80" t="s">
+      <c r="B51" s="47" t="s">
         <v>55</v>
       </c>
-      <c r="C51" s="80"/>
-      <c r="D51" s="80"/>
-      <c r="E51" s="80"/>
-      <c r="F51" s="80"/>
-      <c r="G51" s="80"/>
-      <c r="H51" s="80"/>
-      <c r="I51" s="80"/>
-      <c r="J51" s="80"/>
-      <c r="K51" s="80"/>
-      <c r="L51" s="80"/>
+      <c r="C51" s="47"/>
+      <c r="D51" s="47"/>
+      <c r="E51" s="47"/>
+      <c r="F51" s="47"/>
+      <c r="G51" s="47"/>
+      <c r="H51" s="47"/>
+      <c r="I51" s="47"/>
+      <c r="J51" s="47"/>
+      <c r="K51" s="47"/>
+      <c r="L51" s="47"/>
     </row>
     <row r="52" spans="1:12">
       <c r="C52" s="34"/>
@@ -2487,18 +2501,28 @@
   <sortState ref="A24:K25">
     <sortCondition ref="A3"/>
   </sortState>
-  <mergeCells count="43">
-    <mergeCell ref="B50:L50"/>
-    <mergeCell ref="B51:L51"/>
-    <mergeCell ref="A39:E39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="B45:L45"/>
-    <mergeCell ref="A44:L44"/>
-    <mergeCell ref="B46:L46"/>
-    <mergeCell ref="B47:L47"/>
-    <mergeCell ref="B48:L48"/>
-    <mergeCell ref="B49:L49"/>
+  <mergeCells count="44">
+    <mergeCell ref="N6:T6"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="H27:K27"/>
+    <mergeCell ref="N14:S15"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="H28:K28"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="H30:K30"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="H32:K32"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="H31:L31"/>
     <mergeCell ref="A35:B35"/>
     <mergeCell ref="A36:B36"/>
     <mergeCell ref="A37:B37"/>
@@ -2511,26 +2535,17 @@
     <mergeCell ref="C35:G35"/>
     <mergeCell ref="C36:G36"/>
     <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="H30:K30"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="H32:K32"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="H31:L31"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="H28:K28"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="N6:T6"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="H27:K27"/>
+    <mergeCell ref="B50:L50"/>
+    <mergeCell ref="B51:L51"/>
+    <mergeCell ref="A39:E39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="B45:L45"/>
+    <mergeCell ref="A44:L44"/>
+    <mergeCell ref="B46:L46"/>
+    <mergeCell ref="B47:L47"/>
+    <mergeCell ref="B48:L48"/>
+    <mergeCell ref="B49:L49"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="P4" r:id="rId1"/>

</xml_diff>

<commit_message>
Usando el servicio api del backen en localhost para DEgree, Hardskill, Interest, Person. Hubo correcciones en los controller del backend, DeleteMapping. Se detectaron varios errores en el frontEnd, Registrado en cuadro de estado
</commit_message>
<xml_diff>
--- a/Cuadro-de-estado.xlsx
+++ b/Cuadro-de-estado.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="88">
   <si>
     <t>BACKEND</t>
   </si>
@@ -345,9 +345,6 @@
     <t>Aún existen componentes/servicios que apuntan a mock-data</t>
   </si>
   <si>
-    <t>Existe un error que arroja consola this.itemParaBorrar</t>
-  </si>
-  <si>
     <t>En los Getter de los Form, hay que eliminar espacios de los string</t>
   </si>
   <si>
@@ -358,6 +355,15 @@
   </si>
   <si>
     <t>Integridad, al borrar Organization, RolePosition, Degree. Ojo con la relacion en LaboralCareer y Studie</t>
+  </si>
+  <si>
+    <t>En cada componente, vuelve a buscar la informacion a la DB, ¿está bien?</t>
+  </si>
+  <si>
+    <t>No actualiza codigo JS de los widgets al dar de alta un hard o soft skill</t>
+  </si>
+  <si>
+    <t>Existe un error que arroja consola this.itemParaBorrar (sin error en softskill p.ej)</t>
   </si>
 </sst>
 </file>
@@ -1023,7 +1029,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1105,7 +1111,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1117,6 +1122,123 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1141,122 +1263,11 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1559,7 +1570,7 @@
   <dimension ref="A1:T54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1576,40 +1587,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="23.25">
-      <c r="A1" s="90" t="s">
+      <c r="A1" s="48" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="90"/>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="90"/>
-      <c r="G1" s="90"/>
-      <c r="H1" s="90"/>
-      <c r="I1" s="90"/>
-      <c r="J1" s="90"/>
-      <c r="K1" s="90"/>
-      <c r="L1" s="90"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
+      <c r="L1" s="48"/>
     </row>
     <row r="2" spans="1:20" ht="15.75" thickBot="1"/>
     <row r="3" spans="1:20" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="91" t="s">
+      <c r="A3" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="92"/>
-      <c r="C3" s="82" t="s">
+      <c r="B3" s="50"/>
+      <c r="C3" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="83"/>
-      <c r="E3" s="83"/>
-      <c r="F3" s="83"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="82" t="s">
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="83"/>
-      <c r="J3" s="84"/>
-      <c r="K3" s="85"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="53"/>
       <c r="L3" s="21" t="s">
         <v>4</v>
       </c>
@@ -1681,25 +1692,25 @@
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E6" s="13"/>
       <c r="F6" s="6"/>
-      <c r="G6" s="7"/>
+      <c r="G6" s="5"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
       <c r="K6" s="5"/>
       <c r="L6" s="4"/>
-      <c r="N6" s="88" t="s">
+      <c r="N6" s="46" t="s">
         <v>70</v>
       </c>
-      <c r="O6" s="89"/>
-      <c r="P6" s="89"/>
-      <c r="Q6" s="89"/>
-      <c r="R6" s="89"/>
-      <c r="S6" s="89"/>
-      <c r="T6" s="89"/>
+      <c r="O6" s="47"/>
+      <c r="P6" s="47"/>
+      <c r="Q6" s="47"/>
+      <c r="R6" s="47"/>
+      <c r="S6" s="47"/>
+      <c r="T6" s="47"/>
     </row>
     <row r="7" spans="1:20" ht="4.5" customHeight="1">
       <c r="A7" s="29"/>
@@ -1726,7 +1737,7 @@
       <c r="D8" s="13"/>
       <c r="E8" s="13"/>
       <c r="F8" s="13"/>
-      <c r="G8" s="7"/>
+      <c r="G8" s="5"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
@@ -1754,7 +1765,7 @@
       <c r="D9" s="13"/>
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
-      <c r="G9" s="7"/>
+      <c r="G9" s="5"/>
       <c r="H9" s="13"/>
       <c r="I9" s="13"/>
       <c r="J9" s="4"/>
@@ -1776,7 +1787,7 @@
       <c r="D10" s="13"/>
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
-      <c r="G10" s="7"/>
+      <c r="G10" s="5"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
@@ -1822,15 +1833,15 @@
       <c r="L12" s="31"/>
     </row>
     <row r="13" spans="1:20">
-      <c r="A13" s="42" t="s">
+      <c r="A13" s="41" t="s">
         <v>30</v>
       </c>
       <c r="B13" s="25" t="s">
         <v>13</v>
       </c>
       <c r="C13" s="5"/>
-      <c r="D13" s="44" t="s">
-        <v>83</v>
+      <c r="D13" s="43" t="s">
+        <v>82</v>
       </c>
       <c r="E13" s="13"/>
       <c r="F13" s="5"/>
@@ -1842,15 +1853,15 @@
       <c r="L13" s="4"/>
     </row>
     <row r="14" spans="1:20">
-      <c r="A14" s="42" t="s">
+      <c r="A14" s="41" t="s">
         <v>18</v>
       </c>
       <c r="B14" s="25" t="s">
         <v>13</v>
       </c>
       <c r="C14" s="5"/>
-      <c r="D14" s="44" t="s">
-        <v>83</v>
+      <c r="D14" s="43" t="s">
+        <v>82</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
@@ -1860,14 +1871,14 @@
       <c r="J14" s="4"/>
       <c r="K14" s="7"/>
       <c r="L14" s="5"/>
-      <c r="N14" s="93" t="s">
-        <v>85</v>
-      </c>
-      <c r="O14" s="93"/>
-      <c r="P14" s="93"/>
-      <c r="Q14" s="93"/>
-      <c r="R14" s="93"/>
-      <c r="S14" s="93"/>
+      <c r="N14" s="55" t="s">
+        <v>84</v>
+      </c>
+      <c r="O14" s="55"/>
+      <c r="P14" s="55"/>
+      <c r="Q14" s="55"/>
+      <c r="R14" s="55"/>
+      <c r="S14" s="55"/>
     </row>
     <row r="15" spans="1:20">
       <c r="A15" s="18" t="s">
@@ -1877,7 +1888,7 @@
         <v>12</v>
       </c>
       <c r="C15" s="5"/>
-      <c r="D15" s="45"/>
+      <c r="D15" s="44"/>
       <c r="E15" s="5"/>
       <c r="F15" s="16"/>
       <c r="G15" s="7"/>
@@ -1886,23 +1897,23 @@
       <c r="J15" s="4"/>
       <c r="K15" s="7"/>
       <c r="L15" s="5"/>
-      <c r="N15" s="93"/>
-      <c r="O15" s="93"/>
-      <c r="P15" s="93"/>
-      <c r="Q15" s="93"/>
-      <c r="R15" s="93"/>
-      <c r="S15" s="93"/>
+      <c r="N15" s="55"/>
+      <c r="O15" s="55"/>
+      <c r="P15" s="55"/>
+      <c r="Q15" s="55"/>
+      <c r="R15" s="55"/>
+      <c r="S15" s="55"/>
     </row>
     <row r="16" spans="1:20">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="41" t="s">
         <v>9</v>
       </c>
       <c r="B16" s="25" t="s">
         <v>13</v>
       </c>
       <c r="C16" s="5"/>
-      <c r="D16" s="44" t="s">
-        <v>83</v>
+      <c r="D16" s="43" t="s">
+        <v>82</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
@@ -1921,7 +1932,7 @@
         <v>12</v>
       </c>
       <c r="C17" s="5"/>
-      <c r="D17" s="45"/>
+      <c r="D17" s="44"/>
       <c r="E17" s="5"/>
       <c r="F17" s="16"/>
       <c r="G17" s="7"/>
@@ -1946,15 +1957,15 @@
       <c r="L18" s="31"/>
     </row>
     <row r="19" spans="1:19">
-      <c r="A19" s="43" t="s">
+      <c r="A19" s="42" t="s">
         <v>16</v>
       </c>
       <c r="B19" s="25" t="s">
         <v>13</v>
       </c>
       <c r="C19" s="16"/>
-      <c r="D19" s="46" t="s">
-        <v>83</v>
+      <c r="D19" s="45" t="s">
+        <v>82</v>
       </c>
       <c r="E19" s="6"/>
       <c r="F19" s="8"/>
@@ -1969,15 +1980,15 @@
       </c>
     </row>
     <row r="20" spans="1:19">
-      <c r="A20" s="43" t="s">
+      <c r="A20" s="42" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="25" t="s">
         <v>13</v>
       </c>
       <c r="C20" s="16"/>
-      <c r="D20" s="46" t="s">
-        <v>83</v>
+      <c r="D20" s="45" t="s">
+        <v>82</v>
       </c>
       <c r="E20" s="6"/>
       <c r="F20" s="8"/>
@@ -2003,7 +2014,7 @@
       <c r="L21" s="31"/>
     </row>
     <row r="22" spans="1:19">
-      <c r="A22" s="43" t="s">
+      <c r="A22" s="42" t="s">
         <v>49</v>
       </c>
       <c r="B22" s="20"/>
@@ -2033,7 +2044,7 @@
       <c r="L23" s="31"/>
     </row>
     <row r="24" spans="1:19">
-      <c r="A24" s="43" t="s">
+      <c r="A24" s="42" t="s">
         <v>50</v>
       </c>
       <c r="B24" s="33"/>
@@ -2055,7 +2066,7 @@
       </c>
     </row>
     <row r="25" spans="1:19">
-      <c r="A25" s="43" t="s">
+      <c r="A25" s="42" t="s">
         <v>51</v>
       </c>
       <c r="B25" s="25" t="s">
@@ -2092,52 +2103,54 @@
     <row r="27" spans="1:19" ht="15.75" thickBot="1">
       <c r="A27" s="24"/>
       <c r="B27" s="26"/>
-      <c r="C27" s="82" t="s">
+      <c r="C27" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="83"/>
-      <c r="E27" s="83"/>
-      <c r="F27" s="83"/>
-      <c r="G27" s="85"/>
-      <c r="H27" s="82" t="s">
+      <c r="D27" s="52"/>
+      <c r="E27" s="52"/>
+      <c r="F27" s="52"/>
+      <c r="G27" s="53"/>
+      <c r="H27" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="I27" s="83"/>
-      <c r="J27" s="84"/>
-      <c r="K27" s="85"/>
+      <c r="I27" s="52"/>
+      <c r="J27" s="54"/>
+      <c r="K27" s="53"/>
       <c r="L27" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="N27" s="41" t="s">
-        <v>80</v>
-      </c>
-      <c r="O27" s="41"/>
-      <c r="P27" s="41"/>
-      <c r="Q27" s="41"/>
-      <c r="R27" s="41"/>
+      <c r="N27" s="94" t="s">
+        <v>87</v>
+      </c>
+      <c r="O27" s="94"/>
+      <c r="P27" s="94"/>
+      <c r="Q27" s="94"/>
+      <c r="R27" s="94"/>
+      <c r="S27" s="94"/>
     </row>
     <row r="28" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A28" s="86" t="s">
+      <c r="A28" s="59" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="87"/>
-      <c r="C28" s="79"/>
-      <c r="D28" s="80"/>
-      <c r="E28" s="80"/>
-      <c r="F28" s="80"/>
-      <c r="G28" s="81"/>
-      <c r="H28" s="79"/>
-      <c r="I28" s="80"/>
-      <c r="J28" s="80"/>
-      <c r="K28" s="81"/>
+      <c r="B28" s="60"/>
+      <c r="C28" s="56"/>
+      <c r="D28" s="57"/>
+      <c r="E28" s="57"/>
+      <c r="F28" s="57"/>
+      <c r="G28" s="58"/>
+      <c r="H28" s="56"/>
+      <c r="I28" s="57"/>
+      <c r="J28" s="57"/>
+      <c r="K28" s="58"/>
       <c r="L28" s="35"/>
-      <c r="N28" s="41" t="s">
-        <v>81</v>
-      </c>
-      <c r="O28" s="41"/>
-      <c r="P28" s="41"/>
-      <c r="Q28" s="41"/>
-      <c r="R28" s="41"/>
+      <c r="N28" s="94" t="s">
+        <v>86</v>
+      </c>
+      <c r="O28" s="94"/>
+      <c r="P28" s="94"/>
+      <c r="Q28" s="94"/>
+      <c r="R28" s="94"/>
+      <c r="S28" s="94"/>
     </row>
     <row r="29" spans="1:19" ht="4.5" customHeight="1">
       <c r="A29" s="29"/>
@@ -2154,94 +2167,102 @@
       <c r="L29" s="31"/>
     </row>
     <row r="30" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A30" s="55" t="s">
+      <c r="A30" s="65" t="s">
         <v>40</v>
       </c>
-      <c r="B30" s="56"/>
-      <c r="C30" s="68"/>
-      <c r="D30" s="69"/>
-      <c r="E30" s="69"/>
-      <c r="F30" s="69"/>
-      <c r="G30" s="70"/>
-      <c r="H30" s="71"/>
-      <c r="I30" s="69"/>
-      <c r="J30" s="69"/>
-      <c r="K30" s="70"/>
+      <c r="B30" s="66"/>
+      <c r="C30" s="61"/>
+      <c r="D30" s="62"/>
+      <c r="E30" s="62"/>
+      <c r="F30" s="62"/>
+      <c r="G30" s="63"/>
+      <c r="H30" s="64"/>
+      <c r="I30" s="62"/>
+      <c r="J30" s="62"/>
+      <c r="K30" s="63"/>
       <c r="L30" s="22" t="s">
         <v>5</v>
       </c>
       <c r="M30" s="34"/>
-      <c r="N30" s="41" t="s">
-        <v>82</v>
-      </c>
-      <c r="O30" s="41"/>
-      <c r="P30" s="41"/>
-      <c r="Q30" s="41"/>
-      <c r="R30" s="41"/>
-      <c r="S30" s="41"/>
+      <c r="N30" s="93" t="s">
+        <v>85</v>
+      </c>
+      <c r="O30" s="93"/>
+      <c r="P30" s="93"/>
+      <c r="Q30" s="93"/>
+      <c r="R30" s="93"/>
+      <c r="S30" s="93"/>
     </row>
     <row r="31" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A31" s="55" t="s">
+      <c r="A31" s="65" t="s">
         <v>62</v>
       </c>
-      <c r="B31" s="56"/>
-      <c r="C31" s="65"/>
-      <c r="D31" s="66"/>
-      <c r="E31" s="66"/>
-      <c r="F31" s="66"/>
-      <c r="G31" s="67"/>
-      <c r="H31" s="76" t="s">
+      <c r="B31" s="66"/>
+      <c r="C31" s="71"/>
+      <c r="D31" s="72"/>
+      <c r="E31" s="72"/>
+      <c r="F31" s="72"/>
+      <c r="G31" s="73"/>
+      <c r="H31" s="74" t="s">
         <v>61</v>
       </c>
-      <c r="I31" s="77"/>
-      <c r="J31" s="77"/>
-      <c r="K31" s="77"/>
-      <c r="L31" s="78"/>
+      <c r="I31" s="75"/>
+      <c r="J31" s="75"/>
+      <c r="K31" s="75"/>
+      <c r="L31" s="76"/>
       <c r="M31" s="34"/>
+      <c r="N31" s="93" t="s">
+        <v>80</v>
+      </c>
+      <c r="O31" s="93"/>
+      <c r="P31" s="93"/>
+      <c r="Q31" s="93"/>
+      <c r="R31" s="93"/>
+      <c r="S31" s="93"/>
     </row>
     <row r="32" spans="1:19" ht="16.5" thickBot="1">
-      <c r="A32" s="74" t="s">
+      <c r="A32" s="69" t="s">
         <v>64</v>
       </c>
-      <c r="B32" s="75"/>
-      <c r="C32" s="68"/>
-      <c r="D32" s="69"/>
-      <c r="E32" s="69"/>
-      <c r="F32" s="69"/>
-      <c r="G32" s="70"/>
-      <c r="H32" s="71"/>
-      <c r="I32" s="69"/>
-      <c r="J32" s="69"/>
-      <c r="K32" s="70"/>
+      <c r="B32" s="70"/>
+      <c r="C32" s="61"/>
+      <c r="D32" s="62"/>
+      <c r="E32" s="62"/>
+      <c r="F32" s="62"/>
+      <c r="G32" s="63"/>
+      <c r="H32" s="64"/>
+      <c r="I32" s="62"/>
+      <c r="J32" s="62"/>
+      <c r="K32" s="63"/>
       <c r="M32" s="34"/>
-      <c r="N32" s="41" t="s">
-        <v>84</v>
-      </c>
-      <c r="O32" s="41"/>
-      <c r="P32" s="41"/>
-      <c r="Q32" s="41"/>
-      <c r="R32" s="41"/>
-      <c r="S32" s="41"/>
-    </row>
-    <row r="33" spans="1:13" ht="30.75" customHeight="1" thickBot="1">
-      <c r="A33" s="72" t="s">
+    </row>
+    <row r="33" spans="1:19" ht="30.75" customHeight="1" thickBot="1">
+      <c r="A33" s="67" t="s">
         <v>36</v>
       </c>
-      <c r="B33" s="73"/>
-      <c r="C33" s="62" t="s">
+      <c r="B33" s="68"/>
+      <c r="C33" s="82" t="s">
         <v>63</v>
       </c>
-      <c r="D33" s="63"/>
-      <c r="E33" s="63"/>
-      <c r="F33" s="63"/>
-      <c r="G33" s="64"/>
-      <c r="H33" s="59"/>
-      <c r="I33" s="60"/>
-      <c r="J33" s="60"/>
-      <c r="K33" s="61"/>
+      <c r="D33" s="83"/>
+      <c r="E33" s="83"/>
+      <c r="F33" s="83"/>
+      <c r="G33" s="84"/>
+      <c r="H33" s="79"/>
+      <c r="I33" s="80"/>
+      <c r="J33" s="80"/>
+      <c r="K33" s="81"/>
       <c r="M33" s="34"/>
-    </row>
-    <row r="34" spans="1:13" ht="4.5" customHeight="1" thickBot="1">
+      <c r="N33" s="93" t="s">
+        <v>81</v>
+      </c>
+      <c r="O33" s="93"/>
+      <c r="P33" s="93"/>
+      <c r="Q33" s="93"/>
+      <c r="R33" s="93"/>
+      <c r="S33" s="93"/>
+    </row>
+    <row r="34" spans="1:19" ht="4.5" customHeight="1" thickBot="1">
       <c r="A34" s="29"/>
       <c r="B34" s="30"/>
       <c r="C34" s="39"/>
@@ -2254,239 +2275,247 @@
       <c r="J34" s="31"/>
       <c r="K34" s="31"/>
     </row>
-    <row r="35" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A35" s="55" t="s">
+    <row r="35" spans="1:19" ht="15.75" thickBot="1">
+      <c r="A35" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="56"/>
-      <c r="C35" s="65"/>
-      <c r="D35" s="66"/>
-      <c r="E35" s="66"/>
-      <c r="F35" s="66"/>
-      <c r="G35" s="67"/>
-      <c r="H35" s="65"/>
-      <c r="I35" s="66"/>
-      <c r="J35" s="66"/>
-      <c r="K35" s="67"/>
+      <c r="B35" s="66"/>
+      <c r="C35" s="71"/>
+      <c r="D35" s="72"/>
+      <c r="E35" s="72"/>
+      <c r="F35" s="72"/>
+      <c r="G35" s="73"/>
+      <c r="H35" s="71"/>
+      <c r="I35" s="72"/>
+      <c r="J35" s="72"/>
+      <c r="K35" s="73"/>
       <c r="M35" s="34"/>
-    </row>
-    <row r="36" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A36" s="55" t="s">
+      <c r="N35" s="93" t="s">
+        <v>83</v>
+      </c>
+      <c r="O35" s="93"/>
+      <c r="P35" s="93"/>
+      <c r="Q35" s="93"/>
+      <c r="R35" s="93"/>
+      <c r="S35" s="93"/>
+    </row>
+    <row r="36" spans="1:19" ht="15.75" thickBot="1">
+      <c r="A36" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="56"/>
-      <c r="C36" s="65"/>
-      <c r="D36" s="66"/>
-      <c r="E36" s="66"/>
-      <c r="F36" s="66"/>
-      <c r="G36" s="67"/>
-      <c r="H36" s="65"/>
-      <c r="I36" s="66"/>
-      <c r="J36" s="66"/>
-      <c r="K36" s="67"/>
+      <c r="B36" s="66"/>
+      <c r="C36" s="71"/>
+      <c r="D36" s="72"/>
+      <c r="E36" s="72"/>
+      <c r="F36" s="72"/>
+      <c r="G36" s="73"/>
+      <c r="H36" s="71"/>
+      <c r="I36" s="72"/>
+      <c r="J36" s="72"/>
+      <c r="K36" s="73"/>
       <c r="M36" s="34"/>
     </row>
-    <row r="37" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A37" s="55" t="s">
+    <row r="37" spans="1:19" ht="15.75" thickBot="1">
+      <c r="A37" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="B37" s="56"/>
-      <c r="C37" s="65"/>
-      <c r="D37" s="66"/>
-      <c r="E37" s="66"/>
-      <c r="F37" s="66"/>
-      <c r="G37" s="67"/>
-      <c r="H37" s="65"/>
-      <c r="I37" s="66"/>
-      <c r="J37" s="66"/>
-      <c r="K37" s="67"/>
+      <c r="B37" s="66"/>
+      <c r="C37" s="71"/>
+      <c r="D37" s="72"/>
+      <c r="E37" s="72"/>
+      <c r="F37" s="72"/>
+      <c r="G37" s="73"/>
+      <c r="H37" s="71"/>
+      <c r="I37" s="72"/>
+      <c r="J37" s="72"/>
+      <c r="K37" s="73"/>
       <c r="M37" s="34"/>
     </row>
-    <row r="38" spans="1:13" ht="15.75" thickBot="1"/>
-    <row r="39" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A39" s="48" t="s">
+    <row r="38" spans="1:19" ht="15.75" thickBot="1"/>
+    <row r="39" spans="1:19" ht="15.75" thickBot="1">
+      <c r="A39" s="86" t="s">
         <v>27</v>
       </c>
-      <c r="B39" s="49"/>
-      <c r="C39" s="49"/>
-      <c r="D39" s="49"/>
-      <c r="E39" s="50"/>
-    </row>
-    <row r="40" spans="1:13">
+      <c r="B39" s="87"/>
+      <c r="C39" s="87"/>
+      <c r="D39" s="87"/>
+      <c r="E39" s="88"/>
+    </row>
+    <row r="40" spans="1:19">
       <c r="A40" s="14" t="s">
         <v>26</v>
       </c>
       <c r="B40" s="13"/>
-      <c r="C40" s="51" t="s">
+      <c r="C40" s="89" t="s">
         <v>23</v>
       </c>
-      <c r="D40" s="52"/>
+      <c r="D40" s="90"/>
       <c r="E40" s="28"/>
     </row>
-    <row r="41" spans="1:13">
+    <row r="41" spans="1:19">
       <c r="A41" s="15" t="s">
         <v>22</v>
       </c>
       <c r="B41" s="5"/>
-      <c r="C41" s="51" t="s">
+      <c r="C41" s="89" t="s">
         <v>24</v>
       </c>
-      <c r="D41" s="52"/>
+      <c r="D41" s="90"/>
       <c r="E41" s="8"/>
     </row>
-    <row r="42" spans="1:13">
+    <row r="42" spans="1:19">
       <c r="A42" s="15" t="s">
         <v>25</v>
       </c>
       <c r="B42" s="6"/>
-      <c r="C42" s="57" t="s">
+      <c r="C42" s="77" t="s">
         <v>69</v>
       </c>
-      <c r="D42" s="58"/>
+      <c r="D42" s="78"/>
       <c r="E42" s="40"/>
     </row>
-    <row r="43" spans="1:13" ht="15.75" thickBot="1"/>
-    <row r="44" spans="1:13">
-      <c r="A44" s="53" t="s">
+    <row r="43" spans="1:19" ht="15.75" thickBot="1"/>
+    <row r="44" spans="1:19">
+      <c r="A44" s="91" t="s">
         <v>37</v>
       </c>
-      <c r="B44" s="54"/>
-      <c r="C44" s="54"/>
-      <c r="D44" s="54"/>
-      <c r="E44" s="54"/>
-      <c r="F44" s="54"/>
-      <c r="G44" s="54"/>
-      <c r="H44" s="54"/>
-      <c r="I44" s="54"/>
-      <c r="J44" s="54"/>
-      <c r="K44" s="54"/>
-      <c r="L44" s="54"/>
-    </row>
-    <row r="45" spans="1:13">
+      <c r="B44" s="92"/>
+      <c r="C44" s="92"/>
+      <c r="D44" s="92"/>
+      <c r="E44" s="92"/>
+      <c r="F44" s="92"/>
+      <c r="G44" s="92"/>
+      <c r="H44" s="92"/>
+      <c r="I44" s="92"/>
+      <c r="J44" s="92"/>
+      <c r="K44" s="92"/>
+      <c r="L44" s="92"/>
+    </row>
+    <row r="45" spans="1:19">
       <c r="A45" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="B45" s="47" t="s">
+      <c r="B45" s="85" t="s">
         <v>57</v>
       </c>
-      <c r="C45" s="47"/>
-      <c r="D45" s="47"/>
-      <c r="E45" s="47"/>
-      <c r="F45" s="47"/>
-      <c r="G45" s="47"/>
-      <c r="H45" s="47"/>
-      <c r="I45" s="47"/>
-      <c r="J45" s="47"/>
-      <c r="K45" s="47"/>
-      <c r="L45" s="47"/>
-    </row>
-    <row r="46" spans="1:13" ht="15" customHeight="1">
+      <c r="C45" s="85"/>
+      <c r="D45" s="85"/>
+      <c r="E45" s="85"/>
+      <c r="F45" s="85"/>
+      <c r="G45" s="85"/>
+      <c r="H45" s="85"/>
+      <c r="I45" s="85"/>
+      <c r="J45" s="85"/>
+      <c r="K45" s="85"/>
+      <c r="L45" s="85"/>
+    </row>
+    <row r="46" spans="1:19" ht="15" customHeight="1">
       <c r="A46" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="B46" s="47" t="s">
+      <c r="B46" s="85" t="s">
         <v>58</v>
       </c>
-      <c r="C46" s="47"/>
-      <c r="D46" s="47"/>
-      <c r="E46" s="47"/>
-      <c r="F46" s="47"/>
-      <c r="G46" s="47"/>
-      <c r="H46" s="47"/>
-      <c r="I46" s="47"/>
-      <c r="J46" s="47"/>
-      <c r="K46" s="47"/>
-      <c r="L46" s="47"/>
-    </row>
-    <row r="47" spans="1:13">
+      <c r="C46" s="85"/>
+      <c r="D46" s="85"/>
+      <c r="E46" s="85"/>
+      <c r="F46" s="85"/>
+      <c r="G46" s="85"/>
+      <c r="H46" s="85"/>
+      <c r="I46" s="85"/>
+      <c r="J46" s="85"/>
+      <c r="K46" s="85"/>
+      <c r="L46" s="85"/>
+    </row>
+    <row r="47" spans="1:19">
       <c r="A47" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="B47" s="47" t="s">
+      <c r="B47" s="85" t="s">
         <v>59</v>
       </c>
-      <c r="C47" s="47"/>
-      <c r="D47" s="47"/>
-      <c r="E47" s="47"/>
-      <c r="F47" s="47"/>
-      <c r="G47" s="47"/>
-      <c r="H47" s="47"/>
-      <c r="I47" s="47"/>
-      <c r="J47" s="47"/>
-      <c r="K47" s="47"/>
-      <c r="L47" s="47"/>
-    </row>
-    <row r="48" spans="1:13">
+      <c r="C47" s="85"/>
+      <c r="D47" s="85"/>
+      <c r="E47" s="85"/>
+      <c r="F47" s="85"/>
+      <c r="G47" s="85"/>
+      <c r="H47" s="85"/>
+      <c r="I47" s="85"/>
+      <c r="J47" s="85"/>
+      <c r="K47" s="85"/>
+      <c r="L47" s="85"/>
+    </row>
+    <row r="48" spans="1:19">
       <c r="A48" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="B48" s="47" t="s">
+      <c r="B48" s="85" t="s">
         <v>46</v>
       </c>
-      <c r="C48" s="47"/>
-      <c r="D48" s="47"/>
-      <c r="E48" s="47"/>
-      <c r="F48" s="47"/>
-      <c r="G48" s="47"/>
-      <c r="H48" s="47"/>
-      <c r="I48" s="47"/>
-      <c r="J48" s="47"/>
-      <c r="K48" s="47"/>
-      <c r="L48" s="47"/>
+      <c r="C48" s="85"/>
+      <c r="D48" s="85"/>
+      <c r="E48" s="85"/>
+      <c r="F48" s="85"/>
+      <c r="G48" s="85"/>
+      <c r="H48" s="85"/>
+      <c r="I48" s="85"/>
+      <c r="J48" s="85"/>
+      <c r="K48" s="85"/>
+      <c r="L48" s="85"/>
     </row>
     <row r="49" spans="1:12">
       <c r="A49" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="B49" s="47" t="s">
+      <c r="B49" s="85" t="s">
         <v>35</v>
       </c>
-      <c r="C49" s="47"/>
-      <c r="D49" s="47"/>
-      <c r="E49" s="47"/>
-      <c r="F49" s="47"/>
-      <c r="G49" s="47"/>
-      <c r="H49" s="47"/>
-      <c r="I49" s="47"/>
-      <c r="J49" s="47"/>
-      <c r="K49" s="47"/>
-      <c r="L49" s="47"/>
+      <c r="C49" s="85"/>
+      <c r="D49" s="85"/>
+      <c r="E49" s="85"/>
+      <c r="F49" s="85"/>
+      <c r="G49" s="85"/>
+      <c r="H49" s="85"/>
+      <c r="I49" s="85"/>
+      <c r="J49" s="85"/>
+      <c r="K49" s="85"/>
+      <c r="L49" s="85"/>
     </row>
     <row r="50" spans="1:12">
       <c r="A50" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="B50" s="47" t="s">
+      <c r="B50" s="85" t="s">
         <v>56</v>
       </c>
-      <c r="C50" s="47"/>
-      <c r="D50" s="47"/>
-      <c r="E50" s="47"/>
-      <c r="F50" s="47"/>
-      <c r="G50" s="47"/>
-      <c r="H50" s="47"/>
-      <c r="I50" s="47"/>
-      <c r="J50" s="47"/>
-      <c r="K50" s="47"/>
-      <c r="L50" s="47"/>
+      <c r="C50" s="85"/>
+      <c r="D50" s="85"/>
+      <c r="E50" s="85"/>
+      <c r="F50" s="85"/>
+      <c r="G50" s="85"/>
+      <c r="H50" s="85"/>
+      <c r="I50" s="85"/>
+      <c r="J50" s="85"/>
+      <c r="K50" s="85"/>
+      <c r="L50" s="85"/>
     </row>
     <row r="51" spans="1:12">
       <c r="A51" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="B51" s="47" t="s">
+      <c r="B51" s="85" t="s">
         <v>55</v>
       </c>
-      <c r="C51" s="47"/>
-      <c r="D51" s="47"/>
-      <c r="E51" s="47"/>
-      <c r="F51" s="47"/>
-      <c r="G51" s="47"/>
-      <c r="H51" s="47"/>
-      <c r="I51" s="47"/>
-      <c r="J51" s="47"/>
-      <c r="K51" s="47"/>
-      <c r="L51" s="47"/>
+      <c r="C51" s="85"/>
+      <c r="D51" s="85"/>
+      <c r="E51" s="85"/>
+      <c r="F51" s="85"/>
+      <c r="G51" s="85"/>
+      <c r="H51" s="85"/>
+      <c r="I51" s="85"/>
+      <c r="J51" s="85"/>
+      <c r="K51" s="85"/>
+      <c r="L51" s="85"/>
     </row>
     <row r="52" spans="1:12">
       <c r="C52" s="34"/>
@@ -2501,28 +2530,23 @@
   <sortState ref="A24:K25">
     <sortCondition ref="A3"/>
   </sortState>
-  <mergeCells count="44">
-    <mergeCell ref="N6:T6"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="H27:K27"/>
-    <mergeCell ref="N14:S15"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="H28:K28"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="H30:K30"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="H32:K32"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="H31:L31"/>
+  <mergeCells count="50">
+    <mergeCell ref="N27:S27"/>
+    <mergeCell ref="N33:S33"/>
+    <mergeCell ref="N35:S35"/>
+    <mergeCell ref="N30:S30"/>
+    <mergeCell ref="N28:S28"/>
+    <mergeCell ref="B50:L50"/>
+    <mergeCell ref="B51:L51"/>
+    <mergeCell ref="A39:E39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="B45:L45"/>
+    <mergeCell ref="A44:L44"/>
+    <mergeCell ref="B46:L46"/>
+    <mergeCell ref="B47:L47"/>
+    <mergeCell ref="B48:L48"/>
+    <mergeCell ref="B49:L49"/>
     <mergeCell ref="A35:B35"/>
     <mergeCell ref="A36:B36"/>
     <mergeCell ref="A37:B37"/>
@@ -2535,17 +2559,28 @@
     <mergeCell ref="C35:G35"/>
     <mergeCell ref="C36:G36"/>
     <mergeCell ref="C37:G37"/>
-    <mergeCell ref="B50:L50"/>
-    <mergeCell ref="B51:L51"/>
-    <mergeCell ref="A39:E39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="B45:L45"/>
-    <mergeCell ref="A44:L44"/>
-    <mergeCell ref="B46:L46"/>
-    <mergeCell ref="B47:L47"/>
-    <mergeCell ref="B48:L48"/>
-    <mergeCell ref="B49:L49"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="H30:K30"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="H32:K32"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="H31:L31"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="H28:K28"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="N6:T6"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="H27:K27"/>
+    <mergeCell ref="N14:S15"/>
+    <mergeCell ref="N31:S31"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="P4" r:id="rId1"/>

</xml_diff>

<commit_message>
Finalizada la integracion con el backend, ahora data.service utiliza la API del backend, se detectaron errores en el frontend turante el testing del uso de los servicios API
</commit_message>
<xml_diff>
--- a/Cuadro-de-estado.xlsx
+++ b/Cuadro-de-estado.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="95">
   <si>
     <t>BACKEND</t>
   </si>
@@ -365,12 +365,33 @@
   <si>
     <t>Existe un error que arroja consola this.itemParaBorrar (sin error en softskill p.ej)</t>
   </si>
+  <si>
+    <t xml:space="preserve"> item ParaBorrar</t>
+  </si>
+  <si>
+    <t>no muestra altas</t>
+  </si>
+  <si>
+    <t>add widget</t>
+  </si>
+  <si>
+    <t>Test en Front</t>
+  </si>
+  <si>
+    <t>Errores DETECTADOS</t>
+  </si>
+  <si>
+    <t>Si no tiene URL no debiera mostrar -VISITAR-</t>
+  </si>
+  <si>
+    <t>Input photoPath</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="23">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -542,6 +563,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="13">
     <fill>
@@ -1029,7 +1057,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1122,6 +1150,135 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1137,137 +1294,21 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1567,10 +1608,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:T54"/>
+  <dimension ref="A1:U54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1586,46 +1627,50 @@
     <col min="10" max="12" width="7.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="23.25">
-      <c r="A1" s="48" t="s">
+    <row r="1" spans="1:21" ht="23.25">
+      <c r="A1" s="91" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48"/>
-      <c r="L1" s="48"/>
-    </row>
-    <row r="2" spans="1:20" ht="15.75" thickBot="1"/>
-    <row r="3" spans="1:20" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="49" t="s">
+      <c r="B1" s="91"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="91"/>
+      <c r="G1" s="91"/>
+      <c r="H1" s="91"/>
+      <c r="I1" s="91"/>
+      <c r="J1" s="91"/>
+      <c r="K1" s="91"/>
+      <c r="L1" s="91"/>
+    </row>
+    <row r="2" spans="1:21" ht="15.75" thickBot="1"/>
+    <row r="3" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1">
+      <c r="A3" s="92" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="50"/>
-      <c r="C3" s="51" t="s">
+      <c r="B3" s="93"/>
+      <c r="C3" s="83" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="51" t="s">
+      <c r="D3" s="84"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="84"/>
+      <c r="G3" s="86"/>
+      <c r="H3" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="52"/>
-      <c r="J3" s="54"/>
-      <c r="K3" s="53"/>
+      <c r="I3" s="84"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="86"/>
       <c r="L3" s="21" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" s="3" customFormat="1" ht="40.5" customHeight="1" thickBot="1">
+      <c r="M3" s="96" t="s">
+        <v>91</v>
+      </c>
+      <c r="N3" s="90"/>
+    </row>
+    <row r="4" spans="1:21" s="3" customFormat="1" ht="40.5" customHeight="1" thickBot="1">
       <c r="A4" s="17" t="s">
         <v>29</v>
       </c>
@@ -1662,14 +1707,18 @@
       <c r="L4" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="N4" s="37" t="s">
+      <c r="M4" s="98" t="s">
+        <v>92</v>
+      </c>
+      <c r="N4" s="99"/>
+      <c r="O4" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="P4" s="38" t="s">
+      <c r="Q4" s="38" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="4.5" customHeight="1">
+    <row r="5" spans="1:21" ht="4.5" customHeight="1">
       <c r="A5" s="29"/>
       <c r="B5" s="30"/>
       <c r="C5" s="31"/>
@@ -1683,7 +1732,7 @@
       <c r="K5" s="31"/>
       <c r="L5" s="31"/>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:21">
       <c r="A6" s="18" t="s">
         <v>15</v>
       </c>
@@ -1702,17 +1751,20 @@
       <c r="J6" s="4"/>
       <c r="K6" s="5"/>
       <c r="L6" s="4"/>
-      <c r="N6" s="46" t="s">
+      <c r="M6" s="95" t="s">
+        <v>94</v>
+      </c>
+      <c r="O6" s="89" t="s">
         <v>70</v>
       </c>
-      <c r="O6" s="47"/>
-      <c r="P6" s="47"/>
-      <c r="Q6" s="47"/>
-      <c r="R6" s="47"/>
-      <c r="S6" s="47"/>
-      <c r="T6" s="47"/>
-    </row>
-    <row r="7" spans="1:20" ht="4.5" customHeight="1">
+      <c r="P6" s="90"/>
+      <c r="Q6" s="90"/>
+      <c r="R6" s="90"/>
+      <c r="S6" s="90"/>
+      <c r="T6" s="90"/>
+      <c r="U6" s="90"/>
+    </row>
+    <row r="7" spans="1:21" ht="4.5" customHeight="1">
       <c r="A7" s="29"/>
       <c r="B7" s="30"/>
       <c r="C7" s="31"/>
@@ -1726,7 +1778,7 @@
       <c r="K7" s="31"/>
       <c r="L7" s="31"/>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:21">
       <c r="A8" s="18" t="s">
         <v>11</v>
       </c>
@@ -1743,18 +1795,24 @@
       <c r="J8" s="4"/>
       <c r="K8" s="7"/>
       <c r="L8" s="4"/>
-      <c r="N8" s="6" t="s">
+      <c r="M8" s="95" t="s">
+        <v>88</v>
+      </c>
+      <c r="N8" s="95" t="s">
+        <v>90</v>
+      </c>
+      <c r="O8" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="O8" s="6" t="s">
+      <c r="P8" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="P8" s="6"/>
       <c r="Q8" s="6"/>
       <c r="R8" s="6"/>
       <c r="S8" s="6"/>
-    </row>
-    <row r="9" spans="1:20">
+      <c r="T8" s="6"/>
+    </row>
+    <row r="9" spans="1:21">
       <c r="A9" s="27" t="s">
         <v>10</v>
       </c>
@@ -1771,12 +1829,18 @@
       <c r="J9" s="4"/>
       <c r="K9" s="28"/>
       <c r="L9" s="4"/>
-      <c r="O9" s="6" t="s">
+      <c r="M9" s="95" t="s">
+        <v>88</v>
+      </c>
+      <c r="N9" s="95" t="s">
+        <v>90</v>
+      </c>
+      <c r="P9" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="P9" s="6"/>
-    </row>
-    <row r="10" spans="1:20">
+      <c r="Q9" s="6"/>
+    </row>
+    <row r="10" spans="1:21">
       <c r="A10" s="18" t="s">
         <v>20</v>
       </c>
@@ -1794,7 +1858,7 @@
       <c r="K10" s="7"/>
       <c r="L10" s="4"/>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:21">
       <c r="A11" s="18" t="s">
         <v>17</v>
       </c>
@@ -1805,20 +1869,23 @@
       <c r="D11" s="13"/>
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
-      <c r="G11" s="7"/>
+      <c r="G11" s="5"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
       <c r="K11" s="7"/>
       <c r="L11" s="4"/>
-      <c r="N11" t="s">
+      <c r="N11" s="95" t="s">
+        <v>89</v>
+      </c>
+      <c r="O11" t="s">
         <v>73</v>
       </c>
-      <c r="O11" t="s">
+      <c r="P11" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="4.5" customHeight="1">
+    <row r="12" spans="1:21" ht="4.5" customHeight="1">
       <c r="A12" s="29"/>
       <c r="B12" s="30"/>
       <c r="C12" s="31"/>
@@ -1832,7 +1899,7 @@
       <c r="K12" s="31"/>
       <c r="L12" s="31"/>
     </row>
-    <row r="13" spans="1:20">
+    <row r="13" spans="1:21">
       <c r="A13" s="41" t="s">
         <v>30</v>
       </c>
@@ -1845,14 +1912,17 @@
       </c>
       <c r="E13" s="13"/>
       <c r="F13" s="5"/>
-      <c r="G13" s="7"/>
+      <c r="G13" s="5"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
       <c r="K13" s="7"/>
       <c r="L13" s="4"/>
-    </row>
-    <row r="14" spans="1:20">
+      <c r="N13" s="95" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21">
       <c r="A14" s="41" t="s">
         <v>18</v>
       </c>
@@ -1865,22 +1935,25 @@
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
-      <c r="G14" s="7"/>
+      <c r="G14" s="5"/>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
       <c r="J14" s="4"/>
       <c r="K14" s="7"/>
-      <c r="L14" s="5"/>
-      <c r="N14" s="55" t="s">
+      <c r="L14" s="4"/>
+      <c r="N14" s="95" t="s">
+        <v>89</v>
+      </c>
+      <c r="O14" s="94" t="s">
         <v>84</v>
       </c>
-      <c r="O14" s="55"/>
-      <c r="P14" s="55"/>
-      <c r="Q14" s="55"/>
-      <c r="R14" s="55"/>
-      <c r="S14" s="55"/>
-    </row>
-    <row r="15" spans="1:20">
+      <c r="P14" s="94"/>
+      <c r="Q14" s="94"/>
+      <c r="R14" s="94"/>
+      <c r="S14" s="94"/>
+      <c r="T14" s="94"/>
+    </row>
+    <row r="15" spans="1:21">
       <c r="A15" s="18" t="s">
         <v>48</v>
       </c>
@@ -1891,20 +1964,26 @@
       <c r="D15" s="44"/>
       <c r="E15" s="5"/>
       <c r="F15" s="16"/>
-      <c r="G15" s="7"/>
+      <c r="G15" s="5"/>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
       <c r="J15" s="4"/>
       <c r="K15" s="7"/>
-      <c r="L15" s="5"/>
-      <c r="N15" s="55"/>
-      <c r="O15" s="55"/>
-      <c r="P15" s="55"/>
-      <c r="Q15" s="55"/>
-      <c r="R15" s="55"/>
-      <c r="S15" s="55"/>
-    </row>
-    <row r="16" spans="1:20">
+      <c r="L15" s="4"/>
+      <c r="M15" s="95" t="s">
+        <v>88</v>
+      </c>
+      <c r="N15" s="95" t="s">
+        <v>89</v>
+      </c>
+      <c r="O15" s="94"/>
+      <c r="P15" s="94"/>
+      <c r="Q15" s="94"/>
+      <c r="R15" s="94"/>
+      <c r="S15" s="94"/>
+      <c r="T15" s="94"/>
+    </row>
+    <row r="16" spans="1:21">
       <c r="A16" s="41" t="s">
         <v>9</v>
       </c>
@@ -1917,14 +1996,17 @@
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
-      <c r="G16" s="7"/>
+      <c r="G16" s="5"/>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
       <c r="J16" s="4"/>
       <c r="K16" s="7"/>
-      <c r="L16" s="5"/>
-    </row>
-    <row r="17" spans="1:19">
+      <c r="L16" s="4"/>
+      <c r="N16" s="95" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20">
       <c r="A17" s="18" t="s">
         <v>47</v>
       </c>
@@ -1935,14 +2017,17 @@
       <c r="D17" s="44"/>
       <c r="E17" s="5"/>
       <c r="F17" s="16"/>
-      <c r="G17" s="7"/>
+      <c r="G17" s="5"/>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
       <c r="J17" s="4"/>
       <c r="K17" s="7"/>
-      <c r="L17" s="5"/>
-    </row>
-    <row r="18" spans="1:19" ht="4.5" customHeight="1">
+      <c r="L17" s="4"/>
+      <c r="N17" s="95" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" ht="4.5" customHeight="1">
       <c r="A18" s="29"/>
       <c r="B18" s="30"/>
       <c r="C18" s="31"/>
@@ -1956,7 +2041,7 @@
       <c r="K18" s="31"/>
       <c r="L18" s="31"/>
     </row>
-    <row r="19" spans="1:19">
+    <row r="19" spans="1:20">
       <c r="A19" s="42" t="s">
         <v>16</v>
       </c>
@@ -1975,11 +2060,11 @@
       <c r="J19" s="4"/>
       <c r="K19" s="7"/>
       <c r="L19" s="32"/>
-      <c r="N19" t="s">
+      <c r="O19" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="20" spans="1:19">
+    <row r="20" spans="1:20">
       <c r="A20" s="42" t="s">
         <v>19</v>
       </c>
@@ -1999,7 +2084,7 @@
       <c r="K20" s="7"/>
       <c r="L20" s="32"/>
     </row>
-    <row r="21" spans="1:19" ht="4.5" customHeight="1">
+    <row r="21" spans="1:20" ht="4.5" customHeight="1">
       <c r="A21" s="29"/>
       <c r="B21" s="30"/>
       <c r="C21" s="31"/>
@@ -2013,7 +2098,7 @@
       <c r="K21" s="31"/>
       <c r="L21" s="31"/>
     </row>
-    <row r="22" spans="1:19">
+    <row r="22" spans="1:20">
       <c r="A22" s="42" t="s">
         <v>49</v>
       </c>
@@ -2029,7 +2114,7 @@
       <c r="K22" s="7"/>
       <c r="L22" s="4"/>
     </row>
-    <row r="23" spans="1:19" ht="4.5" customHeight="1">
+    <row r="23" spans="1:20" ht="4.5" customHeight="1">
       <c r="A23" s="29"/>
       <c r="B23" s="30"/>
       <c r="C23" s="31"/>
@@ -2043,7 +2128,7 @@
       <c r="K23" s="31"/>
       <c r="L23" s="31"/>
     </row>
-    <row r="24" spans="1:19">
+    <row r="24" spans="1:20">
       <c r="A24" s="42" t="s">
         <v>50</v>
       </c>
@@ -2058,14 +2143,14 @@
       <c r="J24" s="4"/>
       <c r="K24" s="7"/>
       <c r="L24" s="4"/>
-      <c r="N24" t="s">
+      <c r="O24" t="s">
         <v>75</v>
       </c>
-      <c r="O24" t="s">
+      <c r="P24" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="25" spans="1:19">
+    <row r="25" spans="1:20">
       <c r="A25" s="42" t="s">
         <v>51</v>
       </c>
@@ -2082,11 +2167,11 @@
       <c r="J25" s="7"/>
       <c r="K25" s="7"/>
       <c r="L25" s="7"/>
-      <c r="N25" t="s">
+      <c r="O25" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="26" spans="1:19" ht="4.5" customHeight="1" thickBot="1">
+    <row r="26" spans="1:20" ht="4.5" customHeight="1" thickBot="1">
       <c r="A26" s="29"/>
       <c r="B26" s="30"/>
       <c r="C26" s="31"/>
@@ -2100,59 +2185,59 @@
       <c r="K26" s="31"/>
       <c r="L26" s="31"/>
     </row>
-    <row r="27" spans="1:19" ht="15.75" thickBot="1">
+    <row r="27" spans="1:20" ht="15.75" thickBot="1">
       <c r="A27" s="24"/>
       <c r="B27" s="26"/>
-      <c r="C27" s="51" t="s">
+      <c r="C27" s="83" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="52"/>
-      <c r="E27" s="52"/>
-      <c r="F27" s="52"/>
-      <c r="G27" s="53"/>
-      <c r="H27" s="51" t="s">
+      <c r="D27" s="84"/>
+      <c r="E27" s="84"/>
+      <c r="F27" s="84"/>
+      <c r="G27" s="86"/>
+      <c r="H27" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="I27" s="52"/>
-      <c r="J27" s="54"/>
-      <c r="K27" s="53"/>
+      <c r="I27" s="84"/>
+      <c r="J27" s="85"/>
+      <c r="K27" s="86"/>
       <c r="L27" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="N27" s="94" t="s">
+      <c r="O27" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="O27" s="94"/>
-      <c r="P27" s="94"/>
-      <c r="Q27" s="94"/>
-      <c r="R27" s="94"/>
-      <c r="S27" s="94"/>
-    </row>
-    <row r="28" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A28" s="59" t="s">
+      <c r="P27" s="46"/>
+      <c r="Q27" s="46"/>
+      <c r="R27" s="46"/>
+      <c r="S27" s="46"/>
+      <c r="T27" s="46"/>
+    </row>
+    <row r="28" spans="1:20" ht="15.75" thickBot="1">
+      <c r="A28" s="87" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="60"/>
-      <c r="C28" s="56"/>
-      <c r="D28" s="57"/>
-      <c r="E28" s="57"/>
-      <c r="F28" s="57"/>
-      <c r="G28" s="58"/>
-      <c r="H28" s="56"/>
-      <c r="I28" s="57"/>
-      <c r="J28" s="57"/>
-      <c r="K28" s="58"/>
+      <c r="B28" s="88"/>
+      <c r="C28" s="80"/>
+      <c r="D28" s="81"/>
+      <c r="E28" s="81"/>
+      <c r="F28" s="81"/>
+      <c r="G28" s="82"/>
+      <c r="H28" s="80"/>
+      <c r="I28" s="81"/>
+      <c r="J28" s="81"/>
+      <c r="K28" s="82"/>
       <c r="L28" s="35"/>
-      <c r="N28" s="94" t="s">
+      <c r="O28" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="O28" s="94"/>
-      <c r="P28" s="94"/>
-      <c r="Q28" s="94"/>
-      <c r="R28" s="94"/>
-      <c r="S28" s="94"/>
-    </row>
-    <row r="29" spans="1:19" ht="4.5" customHeight="1">
+      <c r="P28" s="46"/>
+      <c r="Q28" s="46"/>
+      <c r="R28" s="46"/>
+      <c r="S28" s="46"/>
+      <c r="T28" s="46"/>
+    </row>
+    <row r="29" spans="1:20" ht="4.5" customHeight="1">
       <c r="A29" s="29"/>
       <c r="B29" s="30"/>
       <c r="C29" s="31"/>
@@ -2166,103 +2251,107 @@
       <c r="K29" s="31"/>
       <c r="L29" s="31"/>
     </row>
-    <row r="30" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A30" s="65" t="s">
+    <row r="30" spans="1:20" ht="15.75" thickBot="1">
+      <c r="A30" s="56" t="s">
         <v>40</v>
       </c>
-      <c r="B30" s="66"/>
-      <c r="C30" s="61"/>
-      <c r="D30" s="62"/>
-      <c r="E30" s="62"/>
-      <c r="F30" s="62"/>
-      <c r="G30" s="63"/>
-      <c r="H30" s="64"/>
-      <c r="I30" s="62"/>
-      <c r="J30" s="62"/>
-      <c r="K30" s="63"/>
+      <c r="B30" s="57"/>
+      <c r="C30" s="69"/>
+      <c r="D30" s="70"/>
+      <c r="E30" s="70"/>
+      <c r="F30" s="70"/>
+      <c r="G30" s="71"/>
+      <c r="H30" s="72"/>
+      <c r="I30" s="70"/>
+      <c r="J30" s="70"/>
+      <c r="K30" s="71"/>
       <c r="L30" s="22" t="s">
         <v>5</v>
       </c>
       <c r="M30" s="34"/>
-      <c r="N30" s="93" t="s">
+      <c r="N30" s="34"/>
+      <c r="O30" s="47" t="s">
         <v>85</v>
       </c>
-      <c r="O30" s="93"/>
-      <c r="P30" s="93"/>
-      <c r="Q30" s="93"/>
-      <c r="R30" s="93"/>
-      <c r="S30" s="93"/>
-    </row>
-    <row r="31" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A31" s="65" t="s">
+      <c r="P30" s="47"/>
+      <c r="Q30" s="47"/>
+      <c r="R30" s="47"/>
+      <c r="S30" s="47"/>
+      <c r="T30" s="47"/>
+    </row>
+    <row r="31" spans="1:20" ht="15.75" thickBot="1">
+      <c r="A31" s="56" t="s">
         <v>62</v>
       </c>
-      <c r="B31" s="66"/>
-      <c r="C31" s="71"/>
-      <c r="D31" s="72"/>
-      <c r="E31" s="72"/>
-      <c r="F31" s="72"/>
-      <c r="G31" s="73"/>
-      <c r="H31" s="74" t="s">
+      <c r="B31" s="57"/>
+      <c r="C31" s="66"/>
+      <c r="D31" s="67"/>
+      <c r="E31" s="67"/>
+      <c r="F31" s="67"/>
+      <c r="G31" s="68"/>
+      <c r="H31" s="77" t="s">
         <v>61</v>
       </c>
-      <c r="I31" s="75"/>
-      <c r="J31" s="75"/>
-      <c r="K31" s="75"/>
-      <c r="L31" s="76"/>
+      <c r="I31" s="78"/>
+      <c r="J31" s="78"/>
+      <c r="K31" s="78"/>
+      <c r="L31" s="79"/>
       <c r="M31" s="34"/>
-      <c r="N31" s="93" t="s">
+      <c r="N31" s="34"/>
+      <c r="O31" s="47" t="s">
         <v>80</v>
       </c>
-      <c r="O31" s="93"/>
-      <c r="P31" s="93"/>
-      <c r="Q31" s="93"/>
-      <c r="R31" s="93"/>
-      <c r="S31" s="93"/>
-    </row>
-    <row r="32" spans="1:19" ht="16.5" thickBot="1">
-      <c r="A32" s="69" t="s">
+      <c r="P31" s="47"/>
+      <c r="Q31" s="47"/>
+      <c r="R31" s="47"/>
+      <c r="S31" s="47"/>
+      <c r="T31" s="47"/>
+    </row>
+    <row r="32" spans="1:20" ht="16.5" thickBot="1">
+      <c r="A32" s="75" t="s">
         <v>64</v>
       </c>
-      <c r="B32" s="70"/>
-      <c r="C32" s="61"/>
-      <c r="D32" s="62"/>
-      <c r="E32" s="62"/>
-      <c r="F32" s="62"/>
-      <c r="G32" s="63"/>
-      <c r="H32" s="64"/>
-      <c r="I32" s="62"/>
-      <c r="J32" s="62"/>
-      <c r="K32" s="63"/>
+      <c r="B32" s="76"/>
+      <c r="C32" s="69"/>
+      <c r="D32" s="70"/>
+      <c r="E32" s="70"/>
+      <c r="F32" s="70"/>
+      <c r="G32" s="71"/>
+      <c r="H32" s="72"/>
+      <c r="I32" s="70"/>
+      <c r="J32" s="70"/>
+      <c r="K32" s="71"/>
       <c r="M32" s="34"/>
-    </row>
-    <row r="33" spans="1:19" ht="30.75" customHeight="1" thickBot="1">
-      <c r="A33" s="67" t="s">
+      <c r="N32" s="34"/>
+    </row>
+    <row r="33" spans="1:20" ht="30.75" customHeight="1" thickBot="1">
+      <c r="A33" s="73" t="s">
         <v>36</v>
       </c>
-      <c r="B33" s="68"/>
-      <c r="C33" s="82" t="s">
+      <c r="B33" s="74"/>
+      <c r="C33" s="63" t="s">
         <v>63</v>
       </c>
-      <c r="D33" s="83"/>
-      <c r="E33" s="83"/>
-      <c r="F33" s="83"/>
-      <c r="G33" s="84"/>
-      <c r="H33" s="79"/>
-      <c r="I33" s="80"/>
-      <c r="J33" s="80"/>
-      <c r="K33" s="81"/>
+      <c r="D33" s="64"/>
+      <c r="E33" s="64"/>
+      <c r="F33" s="64"/>
+      <c r="G33" s="65"/>
+      <c r="H33" s="60"/>
+      <c r="I33" s="61"/>
+      <c r="J33" s="61"/>
+      <c r="K33" s="62"/>
       <c r="M33" s="34"/>
-      <c r="N33" s="93" t="s">
+      <c r="N33" s="34"/>
+      <c r="O33" s="97" t="s">
         <v>81</v>
       </c>
-      <c r="O33" s="93"/>
-      <c r="P33" s="93"/>
-      <c r="Q33" s="93"/>
-      <c r="R33" s="93"/>
-      <c r="S33" s="93"/>
-    </row>
-    <row r="34" spans="1:19" ht="4.5" customHeight="1" thickBot="1">
+      <c r="P33" s="97"/>
+      <c r="Q33" s="97"/>
+      <c r="R33" s="97"/>
+      <c r="S33" s="97"/>
+      <c r="T33" s="97"/>
+    </row>
+    <row r="34" spans="1:20" ht="4.5" customHeight="1" thickBot="1">
       <c r="A34" s="29"/>
       <c r="B34" s="30"/>
       <c r="C34" s="39"/>
@@ -2275,247 +2364,258 @@
       <c r="J34" s="31"/>
       <c r="K34" s="31"/>
     </row>
-    <row r="35" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A35" s="65" t="s">
+    <row r="35" spans="1:20" ht="15.75" thickBot="1">
+      <c r="A35" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="66"/>
-      <c r="C35" s="71"/>
-      <c r="D35" s="72"/>
-      <c r="E35" s="72"/>
-      <c r="F35" s="72"/>
-      <c r="G35" s="73"/>
-      <c r="H35" s="71"/>
-      <c r="I35" s="72"/>
-      <c r="J35" s="72"/>
-      <c r="K35" s="73"/>
+      <c r="B35" s="57"/>
+      <c r="C35" s="66"/>
+      <c r="D35" s="67"/>
+      <c r="E35" s="67"/>
+      <c r="F35" s="67"/>
+      <c r="G35" s="68"/>
+      <c r="H35" s="66"/>
+      <c r="I35" s="67"/>
+      <c r="J35" s="67"/>
+      <c r="K35" s="68"/>
       <c r="M35" s="34"/>
-      <c r="N35" s="93" t="s">
+      <c r="N35" s="34"/>
+      <c r="O35" s="47" t="s">
         <v>83</v>
       </c>
-      <c r="O35" s="93"/>
-      <c r="P35" s="93"/>
-      <c r="Q35" s="93"/>
-      <c r="R35" s="93"/>
-      <c r="S35" s="93"/>
-    </row>
-    <row r="36" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A36" s="65" t="s">
+      <c r="P35" s="47"/>
+      <c r="Q35" s="47"/>
+      <c r="R35" s="47"/>
+      <c r="S35" s="47"/>
+      <c r="T35" s="47"/>
+    </row>
+    <row r="36" spans="1:20" ht="15.75" thickBot="1">
+      <c r="A36" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="66"/>
-      <c r="C36" s="71"/>
-      <c r="D36" s="72"/>
-      <c r="E36" s="72"/>
-      <c r="F36" s="72"/>
-      <c r="G36" s="73"/>
-      <c r="H36" s="71"/>
-      <c r="I36" s="72"/>
-      <c r="J36" s="72"/>
-      <c r="K36" s="73"/>
+      <c r="B36" s="57"/>
+      <c r="C36" s="66"/>
+      <c r="D36" s="67"/>
+      <c r="E36" s="67"/>
+      <c r="F36" s="67"/>
+      <c r="G36" s="68"/>
+      <c r="H36" s="66"/>
+      <c r="I36" s="67"/>
+      <c r="J36" s="67"/>
+      <c r="K36" s="68"/>
       <c r="M36" s="34"/>
-    </row>
-    <row r="37" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A37" s="65" t="s">
+      <c r="N36" s="34"/>
+    </row>
+    <row r="37" spans="1:20" ht="15.75" thickBot="1">
+      <c r="A37" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="B37" s="66"/>
-      <c r="C37" s="71"/>
-      <c r="D37" s="72"/>
-      <c r="E37" s="72"/>
-      <c r="F37" s="72"/>
-      <c r="G37" s="73"/>
-      <c r="H37" s="71"/>
-      <c r="I37" s="72"/>
-      <c r="J37" s="72"/>
-      <c r="K37" s="73"/>
+      <c r="B37" s="57"/>
+      <c r="C37" s="66"/>
+      <c r="D37" s="67"/>
+      <c r="E37" s="67"/>
+      <c r="F37" s="67"/>
+      <c r="G37" s="68"/>
+      <c r="H37" s="66"/>
+      <c r="I37" s="67"/>
+      <c r="J37" s="67"/>
+      <c r="K37" s="68"/>
       <c r="M37" s="34"/>
-    </row>
-    <row r="38" spans="1:19" ht="15.75" thickBot="1"/>
-    <row r="39" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A39" s="86" t="s">
+      <c r="N37" s="34"/>
+      <c r="O37" s="46" t="s">
+        <v>93</v>
+      </c>
+      <c r="P37" s="46"/>
+      <c r="Q37" s="46"/>
+      <c r="R37" s="46"/>
+      <c r="S37" s="46"/>
+      <c r="T37" s="46"/>
+    </row>
+    <row r="38" spans="1:20" ht="15.75" thickBot="1"/>
+    <row r="39" spans="1:20" ht="15.75" thickBot="1">
+      <c r="A39" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="B39" s="87"/>
-      <c r="C39" s="87"/>
-      <c r="D39" s="87"/>
-      <c r="E39" s="88"/>
-    </row>
-    <row r="40" spans="1:19">
+      <c r="B39" s="50"/>
+      <c r="C39" s="50"/>
+      <c r="D39" s="50"/>
+      <c r="E39" s="51"/>
+    </row>
+    <row r="40" spans="1:20">
       <c r="A40" s="14" t="s">
         <v>26</v>
       </c>
       <c r="B40" s="13"/>
-      <c r="C40" s="89" t="s">
+      <c r="C40" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="D40" s="90"/>
+      <c r="D40" s="53"/>
       <c r="E40" s="28"/>
     </row>
-    <row r="41" spans="1:19">
+    <row r="41" spans="1:20">
       <c r="A41" s="15" t="s">
         <v>22</v>
       </c>
       <c r="B41" s="5"/>
-      <c r="C41" s="89" t="s">
+      <c r="C41" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="D41" s="90"/>
+      <c r="D41" s="53"/>
       <c r="E41" s="8"/>
     </row>
-    <row r="42" spans="1:19">
+    <row r="42" spans="1:20">
       <c r="A42" s="15" t="s">
         <v>25</v>
       </c>
       <c r="B42" s="6"/>
-      <c r="C42" s="77" t="s">
+      <c r="C42" s="58" t="s">
         <v>69</v>
       </c>
-      <c r="D42" s="78"/>
+      <c r="D42" s="59"/>
       <c r="E42" s="40"/>
     </row>
-    <row r="43" spans="1:19" ht="15.75" thickBot="1"/>
-    <row r="44" spans="1:19">
-      <c r="A44" s="91" t="s">
+    <row r="43" spans="1:20" ht="15.75" thickBot="1"/>
+    <row r="44" spans="1:20">
+      <c r="A44" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="B44" s="92"/>
-      <c r="C44" s="92"/>
-      <c r="D44" s="92"/>
-      <c r="E44" s="92"/>
-      <c r="F44" s="92"/>
-      <c r="G44" s="92"/>
-      <c r="H44" s="92"/>
-      <c r="I44" s="92"/>
-      <c r="J44" s="92"/>
-      <c r="K44" s="92"/>
-      <c r="L44" s="92"/>
-    </row>
-    <row r="45" spans="1:19">
+      <c r="B44" s="55"/>
+      <c r="C44" s="55"/>
+      <c r="D44" s="55"/>
+      <c r="E44" s="55"/>
+      <c r="F44" s="55"/>
+      <c r="G44" s="55"/>
+      <c r="H44" s="55"/>
+      <c r="I44" s="55"/>
+      <c r="J44" s="55"/>
+      <c r="K44" s="55"/>
+      <c r="L44" s="55"/>
+    </row>
+    <row r="45" spans="1:20">
       <c r="A45" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="B45" s="85" t="s">
+      <c r="B45" s="48" t="s">
         <v>57</v>
       </c>
-      <c r="C45" s="85"/>
-      <c r="D45" s="85"/>
-      <c r="E45" s="85"/>
-      <c r="F45" s="85"/>
-      <c r="G45" s="85"/>
-      <c r="H45" s="85"/>
-      <c r="I45" s="85"/>
-      <c r="J45" s="85"/>
-      <c r="K45" s="85"/>
-      <c r="L45" s="85"/>
-    </row>
-    <row r="46" spans="1:19" ht="15" customHeight="1">
+      <c r="C45" s="48"/>
+      <c r="D45" s="48"/>
+      <c r="E45" s="48"/>
+      <c r="F45" s="48"/>
+      <c r="G45" s="48"/>
+      <c r="H45" s="48"/>
+      <c r="I45" s="48"/>
+      <c r="J45" s="48"/>
+      <c r="K45" s="48"/>
+      <c r="L45" s="48"/>
+    </row>
+    <row r="46" spans="1:20" ht="15" customHeight="1">
       <c r="A46" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="B46" s="85" t="s">
+      <c r="B46" s="48" t="s">
         <v>58</v>
       </c>
-      <c r="C46" s="85"/>
-      <c r="D46" s="85"/>
-      <c r="E46" s="85"/>
-      <c r="F46" s="85"/>
-      <c r="G46" s="85"/>
-      <c r="H46" s="85"/>
-      <c r="I46" s="85"/>
-      <c r="J46" s="85"/>
-      <c r="K46" s="85"/>
-      <c r="L46" s="85"/>
-    </row>
-    <row r="47" spans="1:19">
+      <c r="C46" s="48"/>
+      <c r="D46" s="48"/>
+      <c r="E46" s="48"/>
+      <c r="F46" s="48"/>
+      <c r="G46" s="48"/>
+      <c r="H46" s="48"/>
+      <c r="I46" s="48"/>
+      <c r="J46" s="48"/>
+      <c r="K46" s="48"/>
+      <c r="L46" s="48"/>
+    </row>
+    <row r="47" spans="1:20">
       <c r="A47" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="B47" s="85" t="s">
+      <c r="B47" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="C47" s="85"/>
-      <c r="D47" s="85"/>
-      <c r="E47" s="85"/>
-      <c r="F47" s="85"/>
-      <c r="G47" s="85"/>
-      <c r="H47" s="85"/>
-      <c r="I47" s="85"/>
-      <c r="J47" s="85"/>
-      <c r="K47" s="85"/>
-      <c r="L47" s="85"/>
-    </row>
-    <row r="48" spans="1:19">
+      <c r="C47" s="48"/>
+      <c r="D47" s="48"/>
+      <c r="E47" s="48"/>
+      <c r="F47" s="48"/>
+      <c r="G47" s="48"/>
+      <c r="H47" s="48"/>
+      <c r="I47" s="48"/>
+      <c r="J47" s="48"/>
+      <c r="K47" s="48"/>
+      <c r="L47" s="48"/>
+    </row>
+    <row r="48" spans="1:20">
       <c r="A48" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="B48" s="85" t="s">
+      <c r="B48" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="C48" s="85"/>
-      <c r="D48" s="85"/>
-      <c r="E48" s="85"/>
-      <c r="F48" s="85"/>
-      <c r="G48" s="85"/>
-      <c r="H48" s="85"/>
-      <c r="I48" s="85"/>
-      <c r="J48" s="85"/>
-      <c r="K48" s="85"/>
-      <c r="L48" s="85"/>
+      <c r="C48" s="48"/>
+      <c r="D48" s="48"/>
+      <c r="E48" s="48"/>
+      <c r="F48" s="48"/>
+      <c r="G48" s="48"/>
+      <c r="H48" s="48"/>
+      <c r="I48" s="48"/>
+      <c r="J48" s="48"/>
+      <c r="K48" s="48"/>
+      <c r="L48" s="48"/>
     </row>
     <row r="49" spans="1:12">
       <c r="A49" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="B49" s="85" t="s">
+      <c r="B49" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="C49" s="85"/>
-      <c r="D49" s="85"/>
-      <c r="E49" s="85"/>
-      <c r="F49" s="85"/>
-      <c r="G49" s="85"/>
-      <c r="H49" s="85"/>
-      <c r="I49" s="85"/>
-      <c r="J49" s="85"/>
-      <c r="K49" s="85"/>
-      <c r="L49" s="85"/>
+      <c r="C49" s="48"/>
+      <c r="D49" s="48"/>
+      <c r="E49" s="48"/>
+      <c r="F49" s="48"/>
+      <c r="G49" s="48"/>
+      <c r="H49" s="48"/>
+      <c r="I49" s="48"/>
+      <c r="J49" s="48"/>
+      <c r="K49" s="48"/>
+      <c r="L49" s="48"/>
     </row>
     <row r="50" spans="1:12">
       <c r="A50" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="B50" s="85" t="s">
+      <c r="B50" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="C50" s="85"/>
-      <c r="D50" s="85"/>
-      <c r="E50" s="85"/>
-      <c r="F50" s="85"/>
-      <c r="G50" s="85"/>
-      <c r="H50" s="85"/>
-      <c r="I50" s="85"/>
-      <c r="J50" s="85"/>
-      <c r="K50" s="85"/>
-      <c r="L50" s="85"/>
+      <c r="C50" s="48"/>
+      <c r="D50" s="48"/>
+      <c r="E50" s="48"/>
+      <c r="F50" s="48"/>
+      <c r="G50" s="48"/>
+      <c r="H50" s="48"/>
+      <c r="I50" s="48"/>
+      <c r="J50" s="48"/>
+      <c r="K50" s="48"/>
+      <c r="L50" s="48"/>
     </row>
     <row r="51" spans="1:12">
       <c r="A51" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="B51" s="85" t="s">
+      <c r="B51" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="C51" s="85"/>
-      <c r="D51" s="85"/>
-      <c r="E51" s="85"/>
-      <c r="F51" s="85"/>
-      <c r="G51" s="85"/>
-      <c r="H51" s="85"/>
-      <c r="I51" s="85"/>
-      <c r="J51" s="85"/>
-      <c r="K51" s="85"/>
-      <c r="L51" s="85"/>
+      <c r="C51" s="48"/>
+      <c r="D51" s="48"/>
+      <c r="E51" s="48"/>
+      <c r="F51" s="48"/>
+      <c r="G51" s="48"/>
+      <c r="H51" s="48"/>
+      <c r="I51" s="48"/>
+      <c r="J51" s="48"/>
+      <c r="K51" s="48"/>
+      <c r="L51" s="48"/>
     </row>
     <row r="52" spans="1:12">
       <c r="C52" s="34"/>
@@ -2530,23 +2630,31 @@
   <sortState ref="A24:K25">
     <sortCondition ref="A3"/>
   </sortState>
-  <mergeCells count="50">
-    <mergeCell ref="N27:S27"/>
-    <mergeCell ref="N33:S33"/>
-    <mergeCell ref="N35:S35"/>
-    <mergeCell ref="N30:S30"/>
-    <mergeCell ref="N28:S28"/>
-    <mergeCell ref="B50:L50"/>
-    <mergeCell ref="B51:L51"/>
-    <mergeCell ref="A39:E39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="B45:L45"/>
-    <mergeCell ref="A44:L44"/>
-    <mergeCell ref="B46:L46"/>
-    <mergeCell ref="B47:L47"/>
-    <mergeCell ref="B48:L48"/>
-    <mergeCell ref="B49:L49"/>
+  <mergeCells count="53">
+    <mergeCell ref="O37:T37"/>
+    <mergeCell ref="O6:U6"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="H27:K27"/>
+    <mergeCell ref="O14:T15"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="H28:K28"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="H30:K30"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="H32:K32"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="H31:L31"/>
     <mergeCell ref="A35:B35"/>
     <mergeCell ref="A36:B36"/>
     <mergeCell ref="A37:B37"/>
@@ -2559,31 +2667,26 @@
     <mergeCell ref="C35:G35"/>
     <mergeCell ref="C36:G36"/>
     <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="H30:K30"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="H32:K32"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="H31:L31"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="H28:K28"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="N6:T6"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="H27:K27"/>
-    <mergeCell ref="N14:S15"/>
-    <mergeCell ref="N31:S31"/>
+    <mergeCell ref="B50:L50"/>
+    <mergeCell ref="B51:L51"/>
+    <mergeCell ref="A39:E39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="B45:L45"/>
+    <mergeCell ref="A44:L44"/>
+    <mergeCell ref="B46:L46"/>
+    <mergeCell ref="B47:L47"/>
+    <mergeCell ref="B48:L48"/>
+    <mergeCell ref="B49:L49"/>
+    <mergeCell ref="O27:T27"/>
+    <mergeCell ref="O33:T33"/>
+    <mergeCell ref="O35:T35"/>
+    <mergeCell ref="O30:T30"/>
+    <mergeCell ref="O28:T28"/>
+    <mergeCell ref="O31:T31"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="P4" r:id="rId1"/>
+    <hyperlink ref="Q4" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.51" right="0.35" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="89" orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
Los errores detectados en el front durante el testing del funcionamiento de la conexion entre back-front, se resolvió corrigiendo los valores de retornos de las clases java -Controller, Iservice, Service-, se necesito la instancia guardada en la DB para mostrarla en el front
</commit_message>
<xml_diff>
--- a/Cuadro-de-estado.xlsx
+++ b/Cuadro-de-estado.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="27255" windowHeight="13050"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="22350" windowHeight="9885"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="94">
   <si>
     <t>BACKEND</t>
   </si>
@@ -285,12 +285,6 @@
     <t>ESTADO DEL PROYECTO Y ORDEN PARA AVANZAR</t>
   </si>
   <si>
-    <t>Sin interface</t>
-  </si>
-  <si>
-    <t>Interface RESPONSIVA</t>
-  </si>
-  <si>
     <t>Reutilizar componentes (p.e atributos de person, skills, etc.) Modules, componentes para pruebas</t>
   </si>
   <si>
@@ -369,12 +363,6 @@
     <t xml:space="preserve"> item ParaBorrar</t>
   </si>
   <si>
-    <t>no muestra altas</t>
-  </si>
-  <si>
-    <t>add widget</t>
-  </si>
-  <si>
     <t>Test en Front</t>
   </si>
   <si>
@@ -385,6 +373,15 @@
   </si>
   <si>
     <t>Input photoPath</t>
+  </si>
+  <si>
+    <t>interfaz RESPONSIVA</t>
+  </si>
+  <si>
+    <t>Sin interfaz</t>
+  </si>
+  <si>
+    <t>https://www.arquitecturajava.com/angular-select-y-todas-sus-opciones/</t>
   </si>
 </sst>
 </file>
@@ -1057,7 +1054,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1150,166 +1147,167 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1611,7 +1609,7 @@
   <dimension ref="A1:U54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1628,47 +1626,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="50" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="91"/>
-      <c r="G1" s="91"/>
-      <c r="H1" s="91"/>
-      <c r="I1" s="91"/>
-      <c r="J1" s="91"/>
-      <c r="K1" s="91"/>
-      <c r="L1" s="91"/>
-    </row>
-    <row r="2" spans="1:21" ht="15.75" thickBot="1"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="50"/>
+      <c r="L1" s="50"/>
+    </row>
+    <row r="2" spans="1:21" ht="18" thickBot="1">
+      <c r="O2" s="100" t="s">
+        <v>93</v>
+      </c>
+    </row>
     <row r="3" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="92" t="s">
+      <c r="A3" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="93"/>
-      <c r="C3" s="83" t="s">
+      <c r="B3" s="52"/>
+      <c r="C3" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="84"/>
-      <c r="E3" s="84"/>
-      <c r="F3" s="84"/>
-      <c r="G3" s="86"/>
-      <c r="H3" s="83" t="s">
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="84"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="86"/>
+      <c r="I3" s="54"/>
+      <c r="J3" s="56"/>
+      <c r="K3" s="55"/>
       <c r="L3" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="96" t="s">
-        <v>91</v>
-      </c>
-      <c r="N3" s="90"/>
+      <c r="M3" s="58" t="s">
+        <v>87</v>
+      </c>
+      <c r="N3" s="49"/>
     </row>
     <row r="4" spans="1:21" s="3" customFormat="1" ht="40.5" customHeight="1" thickBot="1">
       <c r="A4" s="17" t="s">
@@ -1684,10 +1686,10 @@
         <v>3</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G4" s="11" t="s">
         <v>44</v>
@@ -1707,15 +1709,15 @@
       <c r="L4" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="M4" s="98" t="s">
-        <v>92</v>
-      </c>
-      <c r="N4" s="99"/>
+      <c r="M4" s="59" t="s">
+        <v>88</v>
+      </c>
+      <c r="N4" s="60"/>
       <c r="O4" s="37" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="Q4" s="38" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="4.5" customHeight="1">
@@ -1741,7 +1743,7 @@
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E6" s="13"/>
       <c r="F6" s="6"/>
@@ -1751,18 +1753,18 @@
       <c r="J6" s="4"/>
       <c r="K6" s="5"/>
       <c r="L6" s="4"/>
-      <c r="M6" s="95" t="s">
-        <v>94</v>
-      </c>
-      <c r="O6" s="89" t="s">
-        <v>70</v>
-      </c>
-      <c r="P6" s="90"/>
-      <c r="Q6" s="90"/>
-      <c r="R6" s="90"/>
-      <c r="S6" s="90"/>
-      <c r="T6" s="90"/>
-      <c r="U6" s="90"/>
+      <c r="M6" s="46" t="s">
+        <v>90</v>
+      </c>
+      <c r="O6" s="48" t="s">
+        <v>68</v>
+      </c>
+      <c r="P6" s="49"/>
+      <c r="Q6" s="49"/>
+      <c r="R6" s="49"/>
+      <c r="S6" s="49"/>
+      <c r="T6" s="49"/>
+      <c r="U6" s="49"/>
     </row>
     <row r="7" spans="1:21" ht="4.5" customHeight="1">
       <c r="A7" s="29"/>
@@ -1795,17 +1797,14 @@
       <c r="J8" s="4"/>
       <c r="K8" s="7"/>
       <c r="L8" s="4"/>
-      <c r="M8" s="95" t="s">
-        <v>88</v>
-      </c>
-      <c r="N8" s="95" t="s">
-        <v>90</v>
+      <c r="M8" s="46" t="s">
+        <v>86</v>
       </c>
       <c r="O8" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="P8" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="Q8" s="6"/>
       <c r="R8" s="6"/>
@@ -1829,14 +1828,11 @@
       <c r="J9" s="4"/>
       <c r="K9" s="28"/>
       <c r="L9" s="4"/>
-      <c r="M9" s="95" t="s">
-        <v>88</v>
-      </c>
-      <c r="N9" s="95" t="s">
-        <v>90</v>
+      <c r="M9" s="46" t="s">
+        <v>86</v>
       </c>
       <c r="P9" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="Q9" s="6"/>
     </row>
@@ -1875,14 +1871,11 @@
       <c r="J11" s="4"/>
       <c r="K11" s="7"/>
       <c r="L11" s="4"/>
-      <c r="N11" s="95" t="s">
-        <v>89</v>
-      </c>
       <c r="O11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="P11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="4.5" customHeight="1">
@@ -1908,7 +1901,7 @@
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="43" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E13" s="13"/>
       <c r="F13" s="5"/>
@@ -1918,9 +1911,6 @@
       <c r="J13" s="4"/>
       <c r="K13" s="7"/>
       <c r="L13" s="4"/>
-      <c r="N13" s="95" t="s">
-        <v>89</v>
-      </c>
     </row>
     <row r="14" spans="1:21">
       <c r="A14" s="41" t="s">
@@ -1931,7 +1921,7 @@
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="43" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
@@ -1941,17 +1931,14 @@
       <c r="J14" s="4"/>
       <c r="K14" s="7"/>
       <c r="L14" s="4"/>
-      <c r="N14" s="95" t="s">
-        <v>89</v>
-      </c>
-      <c r="O14" s="94" t="s">
-        <v>84</v>
-      </c>
-      <c r="P14" s="94"/>
-      <c r="Q14" s="94"/>
-      <c r="R14" s="94"/>
-      <c r="S14" s="94"/>
-      <c r="T14" s="94"/>
+      <c r="O14" s="57" t="s">
+        <v>82</v>
+      </c>
+      <c r="P14" s="57"/>
+      <c r="Q14" s="57"/>
+      <c r="R14" s="57"/>
+      <c r="S14" s="57"/>
+      <c r="T14" s="57"/>
     </row>
     <row r="15" spans="1:21">
       <c r="A15" s="18" t="s">
@@ -1970,18 +1957,15 @@
       <c r="J15" s="4"/>
       <c r="K15" s="7"/>
       <c r="L15" s="4"/>
-      <c r="M15" s="95" t="s">
-        <v>88</v>
-      </c>
-      <c r="N15" s="95" t="s">
-        <v>89</v>
-      </c>
-      <c r="O15" s="94"/>
-      <c r="P15" s="94"/>
-      <c r="Q15" s="94"/>
-      <c r="R15" s="94"/>
-      <c r="S15" s="94"/>
-      <c r="T15" s="94"/>
+      <c r="M15" s="46" t="s">
+        <v>86</v>
+      </c>
+      <c r="O15" s="57"/>
+      <c r="P15" s="57"/>
+      <c r="Q15" s="57"/>
+      <c r="R15" s="57"/>
+      <c r="S15" s="57"/>
+      <c r="T15" s="57"/>
     </row>
     <row r="16" spans="1:21">
       <c r="A16" s="41" t="s">
@@ -1992,7 +1976,7 @@
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="43" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
@@ -2002,9 +1986,6 @@
       <c r="J16" s="4"/>
       <c r="K16" s="7"/>
       <c r="L16" s="4"/>
-      <c r="N16" s="95" t="s">
-        <v>89</v>
-      </c>
     </row>
     <row r="17" spans="1:20">
       <c r="A17" s="18" t="s">
@@ -2023,9 +2004,6 @@
       <c r="J17" s="4"/>
       <c r="K17" s="7"/>
       <c r="L17" s="4"/>
-      <c r="N17" s="95" t="s">
-        <v>89</v>
-      </c>
     </row>
     <row r="18" spans="1:20" ht="4.5" customHeight="1">
       <c r="A18" s="29"/>
@@ -2050,7 +2028,7 @@
       </c>
       <c r="C19" s="16"/>
       <c r="D19" s="45" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E19" s="6"/>
       <c r="F19" s="8"/>
@@ -2061,7 +2039,7 @@
       <c r="K19" s="7"/>
       <c r="L19" s="32"/>
       <c r="O19" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20" spans="1:20">
@@ -2073,7 +2051,7 @@
       </c>
       <c r="C20" s="16"/>
       <c r="D20" s="45" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E20" s="6"/>
       <c r="F20" s="8"/>
@@ -2144,10 +2122,10 @@
       <c r="K24" s="7"/>
       <c r="L24" s="4"/>
       <c r="O24" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="P24" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:20">
@@ -2168,7 +2146,7 @@
       <c r="K25" s="7"/>
       <c r="L25" s="7"/>
       <c r="O25" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="26" spans="1:20" ht="4.5" customHeight="1" thickBot="1">
@@ -2188,54 +2166,54 @@
     <row r="27" spans="1:20" ht="15.75" thickBot="1">
       <c r="A27" s="24"/>
       <c r="B27" s="26"/>
-      <c r="C27" s="83" t="s">
+      <c r="C27" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="84"/>
-      <c r="E27" s="84"/>
-      <c r="F27" s="84"/>
-      <c r="G27" s="86"/>
-      <c r="H27" s="83" t="s">
+      <c r="D27" s="54"/>
+      <c r="E27" s="54"/>
+      <c r="F27" s="54"/>
+      <c r="G27" s="55"/>
+      <c r="H27" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="I27" s="84"/>
-      <c r="J27" s="85"/>
-      <c r="K27" s="86"/>
+      <c r="I27" s="54"/>
+      <c r="J27" s="56"/>
+      <c r="K27" s="55"/>
       <c r="L27" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="O27" s="46" t="s">
-        <v>87</v>
-      </c>
-      <c r="P27" s="46"/>
-      <c r="Q27" s="46"/>
-      <c r="R27" s="46"/>
-      <c r="S27" s="46"/>
-      <c r="T27" s="46"/>
+      <c r="O27" s="47" t="s">
+        <v>85</v>
+      </c>
+      <c r="P27" s="47"/>
+      <c r="Q27" s="47"/>
+      <c r="R27" s="47"/>
+      <c r="S27" s="47"/>
+      <c r="T27" s="47"/>
     </row>
     <row r="28" spans="1:20" ht="15.75" thickBot="1">
-      <c r="A28" s="87" t="s">
+      <c r="A28" s="64" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="88"/>
-      <c r="C28" s="80"/>
-      <c r="D28" s="81"/>
-      <c r="E28" s="81"/>
-      <c r="F28" s="81"/>
-      <c r="G28" s="82"/>
-      <c r="H28" s="80"/>
-      <c r="I28" s="81"/>
-      <c r="J28" s="81"/>
-      <c r="K28" s="82"/>
+      <c r="B28" s="65"/>
+      <c r="C28" s="61"/>
+      <c r="D28" s="62"/>
+      <c r="E28" s="62"/>
+      <c r="F28" s="62"/>
+      <c r="G28" s="63"/>
+      <c r="H28" s="61"/>
+      <c r="I28" s="62"/>
+      <c r="J28" s="62"/>
+      <c r="K28" s="63"/>
       <c r="L28" s="35"/>
-      <c r="O28" s="46" t="s">
-        <v>86</v>
-      </c>
-      <c r="P28" s="46"/>
-      <c r="Q28" s="46"/>
-      <c r="R28" s="46"/>
-      <c r="S28" s="46"/>
-      <c r="T28" s="46"/>
+      <c r="O28" s="47" t="s">
+        <v>84</v>
+      </c>
+      <c r="P28" s="47"/>
+      <c r="Q28" s="47"/>
+      <c r="R28" s="47"/>
+      <c r="S28" s="47"/>
+      <c r="T28" s="47"/>
     </row>
     <row r="29" spans="1:20" ht="4.5" customHeight="1">
       <c r="A29" s="29"/>
@@ -2252,104 +2230,104 @@
       <c r="L29" s="31"/>
     </row>
     <row r="30" spans="1:20" ht="15.75" thickBot="1">
-      <c r="A30" s="56" t="s">
+      <c r="A30" s="70" t="s">
         <v>40</v>
       </c>
-      <c r="B30" s="57"/>
-      <c r="C30" s="69"/>
-      <c r="D30" s="70"/>
-      <c r="E30" s="70"/>
-      <c r="F30" s="70"/>
-      <c r="G30" s="71"/>
-      <c r="H30" s="72"/>
-      <c r="I30" s="70"/>
-      <c r="J30" s="70"/>
-      <c r="K30" s="71"/>
+      <c r="B30" s="71"/>
+      <c r="C30" s="66"/>
+      <c r="D30" s="67"/>
+      <c r="E30" s="67"/>
+      <c r="F30" s="67"/>
+      <c r="G30" s="68"/>
+      <c r="H30" s="69"/>
+      <c r="I30" s="67"/>
+      <c r="J30" s="67"/>
+      <c r="K30" s="68"/>
       <c r="L30" s="22" t="s">
         <v>5</v>
       </c>
       <c r="M30" s="34"/>
       <c r="N30" s="34"/>
-      <c r="O30" s="47" t="s">
-        <v>85</v>
-      </c>
-      <c r="P30" s="47"/>
-      <c r="Q30" s="47"/>
-      <c r="R30" s="47"/>
-      <c r="S30" s="47"/>
-      <c r="T30" s="47"/>
+      <c r="O30" s="99" t="s">
+        <v>83</v>
+      </c>
+      <c r="P30" s="99"/>
+      <c r="Q30" s="99"/>
+      <c r="R30" s="99"/>
+      <c r="S30" s="99"/>
+      <c r="T30" s="99"/>
     </row>
     <row r="31" spans="1:20" ht="15.75" thickBot="1">
-      <c r="A31" s="56" t="s">
-        <v>62</v>
-      </c>
-      <c r="B31" s="57"/>
-      <c r="C31" s="66"/>
-      <c r="D31" s="67"/>
-      <c r="E31" s="67"/>
-      <c r="F31" s="67"/>
-      <c r="G31" s="68"/>
-      <c r="H31" s="77" t="s">
-        <v>61</v>
-      </c>
-      <c r="I31" s="78"/>
-      <c r="J31" s="78"/>
-      <c r="K31" s="78"/>
-      <c r="L31" s="79"/>
+      <c r="A31" s="70" t="s">
+        <v>91</v>
+      </c>
+      <c r="B31" s="71"/>
+      <c r="C31" s="76"/>
+      <c r="D31" s="77"/>
+      <c r="E31" s="77"/>
+      <c r="F31" s="77"/>
+      <c r="G31" s="78"/>
+      <c r="H31" s="79" t="s">
+        <v>92</v>
+      </c>
+      <c r="I31" s="80"/>
+      <c r="J31" s="80"/>
+      <c r="K31" s="80"/>
+      <c r="L31" s="81"/>
       <c r="M31" s="34"/>
       <c r="N31" s="34"/>
-      <c r="O31" s="47" t="s">
-        <v>80</v>
-      </c>
-      <c r="P31" s="47"/>
-      <c r="Q31" s="47"/>
-      <c r="R31" s="47"/>
-      <c r="S31" s="47"/>
-      <c r="T31" s="47"/>
+      <c r="O31" s="99" t="s">
+        <v>78</v>
+      </c>
+      <c r="P31" s="99"/>
+      <c r="Q31" s="99"/>
+      <c r="R31" s="99"/>
+      <c r="S31" s="99"/>
+      <c r="T31" s="99"/>
     </row>
     <row r="32" spans="1:20" ht="16.5" thickBot="1">
-      <c r="A32" s="75" t="s">
-        <v>64</v>
-      </c>
-      <c r="B32" s="76"/>
-      <c r="C32" s="69"/>
-      <c r="D32" s="70"/>
-      <c r="E32" s="70"/>
-      <c r="F32" s="70"/>
-      <c r="G32" s="71"/>
-      <c r="H32" s="72"/>
-      <c r="I32" s="70"/>
-      <c r="J32" s="70"/>
-      <c r="K32" s="71"/>
+      <c r="A32" s="74" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" s="75"/>
+      <c r="C32" s="66"/>
+      <c r="D32" s="67"/>
+      <c r="E32" s="67"/>
+      <c r="F32" s="67"/>
+      <c r="G32" s="68"/>
+      <c r="H32" s="69"/>
+      <c r="I32" s="67"/>
+      <c r="J32" s="67"/>
+      <c r="K32" s="68"/>
       <c r="M32" s="34"/>
       <c r="N32" s="34"/>
     </row>
     <row r="33" spans="1:20" ht="30.75" customHeight="1" thickBot="1">
-      <c r="A33" s="73" t="s">
+      <c r="A33" s="72" t="s">
         <v>36</v>
       </c>
-      <c r="B33" s="74"/>
-      <c r="C33" s="63" t="s">
-        <v>63</v>
-      </c>
-      <c r="D33" s="64"/>
-      <c r="E33" s="64"/>
-      <c r="F33" s="64"/>
-      <c r="G33" s="65"/>
-      <c r="H33" s="60"/>
-      <c r="I33" s="61"/>
-      <c r="J33" s="61"/>
-      <c r="K33" s="62"/>
+      <c r="B33" s="73"/>
+      <c r="C33" s="87" t="s">
+        <v>61</v>
+      </c>
+      <c r="D33" s="88"/>
+      <c r="E33" s="88"/>
+      <c r="F33" s="88"/>
+      <c r="G33" s="89"/>
+      <c r="H33" s="84"/>
+      <c r="I33" s="85"/>
+      <c r="J33" s="85"/>
+      <c r="K33" s="86"/>
       <c r="M33" s="34"/>
       <c r="N33" s="34"/>
-      <c r="O33" s="97" t="s">
-        <v>81</v>
-      </c>
-      <c r="P33" s="97"/>
-      <c r="Q33" s="97"/>
-      <c r="R33" s="97"/>
-      <c r="S33" s="97"/>
-      <c r="T33" s="97"/>
+      <c r="O33" s="98" t="s">
+        <v>79</v>
+      </c>
+      <c r="P33" s="98"/>
+      <c r="Q33" s="98"/>
+      <c r="R33" s="98"/>
+      <c r="S33" s="98"/>
+      <c r="T33" s="98"/>
     </row>
     <row r="34" spans="1:20" ht="4.5" customHeight="1" thickBot="1">
       <c r="A34" s="29"/>
@@ -2365,91 +2343,91 @@
       <c r="K34" s="31"/>
     </row>
     <row r="35" spans="1:20" ht="15.75" thickBot="1">
-      <c r="A35" s="56" t="s">
-        <v>6</v>
-      </c>
-      <c r="B35" s="57"/>
-      <c r="C35" s="66"/>
-      <c r="D35" s="67"/>
-      <c r="E35" s="67"/>
-      <c r="F35" s="67"/>
-      <c r="G35" s="68"/>
-      <c r="H35" s="66"/>
-      <c r="I35" s="67"/>
-      <c r="J35" s="67"/>
-      <c r="K35" s="68"/>
+      <c r="A35" s="70" t="s">
+        <v>7</v>
+      </c>
+      <c r="B35" s="71"/>
+      <c r="C35" s="76"/>
+      <c r="D35" s="77"/>
+      <c r="E35" s="77"/>
+      <c r="F35" s="77"/>
+      <c r="G35" s="78"/>
+      <c r="H35" s="76"/>
+      <c r="I35" s="77"/>
+      <c r="J35" s="77"/>
+      <c r="K35" s="78"/>
       <c r="M35" s="34"/>
       <c r="N35" s="34"/>
-      <c r="O35" s="47" t="s">
-        <v>83</v>
-      </c>
-      <c r="P35" s="47"/>
-      <c r="Q35" s="47"/>
-      <c r="R35" s="47"/>
-      <c r="S35" s="47"/>
-      <c r="T35" s="47"/>
+      <c r="O35" s="99" t="s">
+        <v>81</v>
+      </c>
+      <c r="P35" s="99"/>
+      <c r="Q35" s="99"/>
+      <c r="R35" s="99"/>
+      <c r="S35" s="99"/>
+      <c r="T35" s="99"/>
     </row>
     <row r="36" spans="1:20" ht="15.75" thickBot="1">
-      <c r="A36" s="56" t="s">
-        <v>7</v>
-      </c>
-      <c r="B36" s="57"/>
-      <c r="C36" s="66"/>
-      <c r="D36" s="67"/>
-      <c r="E36" s="67"/>
-      <c r="F36" s="67"/>
-      <c r="G36" s="68"/>
-      <c r="H36" s="66"/>
-      <c r="I36" s="67"/>
-      <c r="J36" s="67"/>
-      <c r="K36" s="68"/>
+      <c r="A36" s="70" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36" s="71"/>
+      <c r="C36" s="76"/>
+      <c r="D36" s="77"/>
+      <c r="E36" s="77"/>
+      <c r="F36" s="77"/>
+      <c r="G36" s="78"/>
+      <c r="H36" s="76"/>
+      <c r="I36" s="77"/>
+      <c r="J36" s="77"/>
+      <c r="K36" s="78"/>
       <c r="M36" s="34"/>
       <c r="N36" s="34"/>
     </row>
     <row r="37" spans="1:20" ht="15.75" thickBot="1">
-      <c r="A37" s="56" t="s">
+      <c r="A37" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="B37" s="57"/>
-      <c r="C37" s="66"/>
-      <c r="D37" s="67"/>
-      <c r="E37" s="67"/>
-      <c r="F37" s="67"/>
-      <c r="G37" s="68"/>
-      <c r="H37" s="66"/>
-      <c r="I37" s="67"/>
-      <c r="J37" s="67"/>
-      <c r="K37" s="68"/>
+      <c r="B37" s="71"/>
+      <c r="C37" s="76"/>
+      <c r="D37" s="77"/>
+      <c r="E37" s="77"/>
+      <c r="F37" s="77"/>
+      <c r="G37" s="78"/>
+      <c r="H37" s="76"/>
+      <c r="I37" s="77"/>
+      <c r="J37" s="77"/>
+      <c r="K37" s="78"/>
       <c r="M37" s="34"/>
       <c r="N37" s="34"/>
-      <c r="O37" s="46" t="s">
-        <v>93</v>
-      </c>
-      <c r="P37" s="46"/>
-      <c r="Q37" s="46"/>
-      <c r="R37" s="46"/>
-      <c r="S37" s="46"/>
-      <c r="T37" s="46"/>
+      <c r="O37" s="47" t="s">
+        <v>89</v>
+      </c>
+      <c r="P37" s="47"/>
+      <c r="Q37" s="47"/>
+      <c r="R37" s="47"/>
+      <c r="S37" s="47"/>
+      <c r="T37" s="47"/>
     </row>
     <row r="38" spans="1:20" ht="15.75" thickBot="1"/>
     <row r="39" spans="1:20" ht="15.75" thickBot="1">
-      <c r="A39" s="49" t="s">
+      <c r="A39" s="91" t="s">
         <v>27</v>
       </c>
-      <c r="B39" s="50"/>
-      <c r="C39" s="50"/>
-      <c r="D39" s="50"/>
-      <c r="E39" s="51"/>
+      <c r="B39" s="92"/>
+      <c r="C39" s="92"/>
+      <c r="D39" s="92"/>
+      <c r="E39" s="93"/>
     </row>
     <row r="40" spans="1:20">
       <c r="A40" s="14" t="s">
         <v>26</v>
       </c>
       <c r="B40" s="13"/>
-      <c r="C40" s="52" t="s">
+      <c r="C40" s="94" t="s">
         <v>23</v>
       </c>
-      <c r="D40" s="53"/>
+      <c r="D40" s="95"/>
       <c r="E40" s="28"/>
     </row>
     <row r="41" spans="1:20">
@@ -2457,10 +2435,10 @@
         <v>22</v>
       </c>
       <c r="B41" s="5"/>
-      <c r="C41" s="52" t="s">
+      <c r="C41" s="94" t="s">
         <v>24</v>
       </c>
-      <c r="D41" s="53"/>
+      <c r="D41" s="95"/>
       <c r="E41" s="8"/>
     </row>
     <row r="42" spans="1:20">
@@ -2468,154 +2446,154 @@
         <v>25</v>
       </c>
       <c r="B42" s="6"/>
-      <c r="C42" s="58" t="s">
-        <v>69</v>
-      </c>
-      <c r="D42" s="59"/>
+      <c r="C42" s="82" t="s">
+        <v>67</v>
+      </c>
+      <c r="D42" s="83"/>
       <c r="E42" s="40"/>
     </row>
     <row r="43" spans="1:20" ht="15.75" thickBot="1"/>
     <row r="44" spans="1:20">
-      <c r="A44" s="54" t="s">
+      <c r="A44" s="96" t="s">
         <v>37</v>
       </c>
-      <c r="B44" s="55"/>
-      <c r="C44" s="55"/>
-      <c r="D44" s="55"/>
-      <c r="E44" s="55"/>
-      <c r="F44" s="55"/>
-      <c r="G44" s="55"/>
-      <c r="H44" s="55"/>
-      <c r="I44" s="55"/>
-      <c r="J44" s="55"/>
-      <c r="K44" s="55"/>
-      <c r="L44" s="55"/>
+      <c r="B44" s="97"/>
+      <c r="C44" s="97"/>
+      <c r="D44" s="97"/>
+      <c r="E44" s="97"/>
+      <c r="F44" s="97"/>
+      <c r="G44" s="97"/>
+      <c r="H44" s="97"/>
+      <c r="I44" s="97"/>
+      <c r="J44" s="97"/>
+      <c r="K44" s="97"/>
+      <c r="L44" s="97"/>
     </row>
     <row r="45" spans="1:20">
       <c r="A45" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="B45" s="48" t="s">
+      <c r="B45" s="90" t="s">
         <v>57</v>
       </c>
-      <c r="C45" s="48"/>
-      <c r="D45" s="48"/>
-      <c r="E45" s="48"/>
-      <c r="F45" s="48"/>
-      <c r="G45" s="48"/>
-      <c r="H45" s="48"/>
-      <c r="I45" s="48"/>
-      <c r="J45" s="48"/>
-      <c r="K45" s="48"/>
-      <c r="L45" s="48"/>
+      <c r="C45" s="90"/>
+      <c r="D45" s="90"/>
+      <c r="E45" s="90"/>
+      <c r="F45" s="90"/>
+      <c r="G45" s="90"/>
+      <c r="H45" s="90"/>
+      <c r="I45" s="90"/>
+      <c r="J45" s="90"/>
+      <c r="K45" s="90"/>
+      <c r="L45" s="90"/>
     </row>
     <row r="46" spans="1:20" ht="15" customHeight="1">
       <c r="A46" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="B46" s="48" t="s">
+      <c r="B46" s="90" t="s">
         <v>58</v>
       </c>
-      <c r="C46" s="48"/>
-      <c r="D46" s="48"/>
-      <c r="E46" s="48"/>
-      <c r="F46" s="48"/>
-      <c r="G46" s="48"/>
-      <c r="H46" s="48"/>
-      <c r="I46" s="48"/>
-      <c r="J46" s="48"/>
-      <c r="K46" s="48"/>
-      <c r="L46" s="48"/>
+      <c r="C46" s="90"/>
+      <c r="D46" s="90"/>
+      <c r="E46" s="90"/>
+      <c r="F46" s="90"/>
+      <c r="G46" s="90"/>
+      <c r="H46" s="90"/>
+      <c r="I46" s="90"/>
+      <c r="J46" s="90"/>
+      <c r="K46" s="90"/>
+      <c r="L46" s="90"/>
     </row>
     <row r="47" spans="1:20">
       <c r="A47" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="B47" s="48" t="s">
+      <c r="B47" s="90" t="s">
         <v>59</v>
       </c>
-      <c r="C47" s="48"/>
-      <c r="D47" s="48"/>
-      <c r="E47" s="48"/>
-      <c r="F47" s="48"/>
-      <c r="G47" s="48"/>
-      <c r="H47" s="48"/>
-      <c r="I47" s="48"/>
-      <c r="J47" s="48"/>
-      <c r="K47" s="48"/>
-      <c r="L47" s="48"/>
+      <c r="C47" s="90"/>
+      <c r="D47" s="90"/>
+      <c r="E47" s="90"/>
+      <c r="F47" s="90"/>
+      <c r="G47" s="90"/>
+      <c r="H47" s="90"/>
+      <c r="I47" s="90"/>
+      <c r="J47" s="90"/>
+      <c r="K47" s="90"/>
+      <c r="L47" s="90"/>
     </row>
     <row r="48" spans="1:20">
       <c r="A48" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="B48" s="48" t="s">
+      <c r="B48" s="90" t="s">
         <v>46</v>
       </c>
-      <c r="C48" s="48"/>
-      <c r="D48" s="48"/>
-      <c r="E48" s="48"/>
-      <c r="F48" s="48"/>
-      <c r="G48" s="48"/>
-      <c r="H48" s="48"/>
-      <c r="I48" s="48"/>
-      <c r="J48" s="48"/>
-      <c r="K48" s="48"/>
-      <c r="L48" s="48"/>
+      <c r="C48" s="90"/>
+      <c r="D48" s="90"/>
+      <c r="E48" s="90"/>
+      <c r="F48" s="90"/>
+      <c r="G48" s="90"/>
+      <c r="H48" s="90"/>
+      <c r="I48" s="90"/>
+      <c r="J48" s="90"/>
+      <c r="K48" s="90"/>
+      <c r="L48" s="90"/>
     </row>
     <row r="49" spans="1:12">
       <c r="A49" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="B49" s="48" t="s">
+      <c r="B49" s="90" t="s">
         <v>35</v>
       </c>
-      <c r="C49" s="48"/>
-      <c r="D49" s="48"/>
-      <c r="E49" s="48"/>
-      <c r="F49" s="48"/>
-      <c r="G49" s="48"/>
-      <c r="H49" s="48"/>
-      <c r="I49" s="48"/>
-      <c r="J49" s="48"/>
-      <c r="K49" s="48"/>
-      <c r="L49" s="48"/>
+      <c r="C49" s="90"/>
+      <c r="D49" s="90"/>
+      <c r="E49" s="90"/>
+      <c r="F49" s="90"/>
+      <c r="G49" s="90"/>
+      <c r="H49" s="90"/>
+      <c r="I49" s="90"/>
+      <c r="J49" s="90"/>
+      <c r="K49" s="90"/>
+      <c r="L49" s="90"/>
     </row>
     <row r="50" spans="1:12">
       <c r="A50" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="B50" s="48" t="s">
+      <c r="B50" s="90" t="s">
         <v>56</v>
       </c>
-      <c r="C50" s="48"/>
-      <c r="D50" s="48"/>
-      <c r="E50" s="48"/>
-      <c r="F50" s="48"/>
-      <c r="G50" s="48"/>
-      <c r="H50" s="48"/>
-      <c r="I50" s="48"/>
-      <c r="J50" s="48"/>
-      <c r="K50" s="48"/>
-      <c r="L50" s="48"/>
+      <c r="C50" s="90"/>
+      <c r="D50" s="90"/>
+      <c r="E50" s="90"/>
+      <c r="F50" s="90"/>
+      <c r="G50" s="90"/>
+      <c r="H50" s="90"/>
+      <c r="I50" s="90"/>
+      <c r="J50" s="90"/>
+      <c r="K50" s="90"/>
+      <c r="L50" s="90"/>
     </row>
     <row r="51" spans="1:12">
       <c r="A51" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="B51" s="48" t="s">
+      <c r="B51" s="90" t="s">
         <v>55</v>
       </c>
-      <c r="C51" s="48"/>
-      <c r="D51" s="48"/>
-      <c r="E51" s="48"/>
-      <c r="F51" s="48"/>
-      <c r="G51" s="48"/>
-      <c r="H51" s="48"/>
-      <c r="I51" s="48"/>
-      <c r="J51" s="48"/>
-      <c r="K51" s="48"/>
-      <c r="L51" s="48"/>
+      <c r="C51" s="90"/>
+      <c r="D51" s="90"/>
+      <c r="E51" s="90"/>
+      <c r="F51" s="90"/>
+      <c r="G51" s="90"/>
+      <c r="H51" s="90"/>
+      <c r="I51" s="90"/>
+      <c r="J51" s="90"/>
+      <c r="K51" s="90"/>
+      <c r="L51" s="90"/>
     </row>
     <row r="52" spans="1:12">
       <c r="C52" s="34"/>
@@ -2631,6 +2609,43 @@
     <sortCondition ref="A3"/>
   </sortState>
   <mergeCells count="53">
+    <mergeCell ref="O27:T27"/>
+    <mergeCell ref="O33:T33"/>
+    <mergeCell ref="O35:T35"/>
+    <mergeCell ref="O30:T30"/>
+    <mergeCell ref="O28:T28"/>
+    <mergeCell ref="O31:T31"/>
+    <mergeCell ref="B50:L50"/>
+    <mergeCell ref="B51:L51"/>
+    <mergeCell ref="A39:E39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="B45:L45"/>
+    <mergeCell ref="A44:L44"/>
+    <mergeCell ref="B46:L46"/>
+    <mergeCell ref="B47:L47"/>
+    <mergeCell ref="B48:L48"/>
+    <mergeCell ref="B49:L49"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="H33:K33"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="H35:K35"/>
+    <mergeCell ref="H36:K36"/>
+    <mergeCell ref="H37:K37"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="H32:K32"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="H31:L31"/>
     <mergeCell ref="O37:T37"/>
     <mergeCell ref="O6:U6"/>
     <mergeCell ref="A1:L1"/>
@@ -2647,49 +2662,13 @@
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="C30:G30"/>
     <mergeCell ref="H30:K30"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="H32:K32"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="H31:L31"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="H33:K33"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="H35:K35"/>
-    <mergeCell ref="H36:K36"/>
-    <mergeCell ref="H37:K37"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="B50:L50"/>
-    <mergeCell ref="B51:L51"/>
-    <mergeCell ref="A39:E39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="B45:L45"/>
-    <mergeCell ref="A44:L44"/>
-    <mergeCell ref="B46:L46"/>
-    <mergeCell ref="B47:L47"/>
-    <mergeCell ref="B48:L48"/>
-    <mergeCell ref="B49:L49"/>
-    <mergeCell ref="O27:T27"/>
-    <mergeCell ref="O33:T33"/>
-    <mergeCell ref="O35:T35"/>
-    <mergeCell ref="O30:T30"/>
-    <mergeCell ref="O28:T28"/>
-    <mergeCell ref="O31:T31"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="Q4" r:id="rId1"/>
+    <hyperlink ref="O2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.51" right="0.35" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="89" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" scale="89" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
arreglados los bugs detectados en el testing. Resta evaluar declarar como privada / let la variable itemParaBorrar
</commit_message>
<xml_diff>
--- a/Cuadro-de-estado.xlsx
+++ b/Cuadro-de-estado.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="94">
   <si>
     <t>BACKEND</t>
   </si>
@@ -354,15 +354,6 @@
     <t>En cada componente, vuelve a buscar la informacion a la DB, ¿está bien?</t>
   </si>
   <si>
-    <t>No actualiza codigo JS de los widgets al dar de alta un hard o soft skill</t>
-  </si>
-  <si>
-    <t>Existe un error que arroja consola this.itemParaBorrar (sin error en softskill p.ej)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> item ParaBorrar</t>
-  </si>
-  <si>
     <t>Test en Front</t>
   </si>
   <si>
@@ -382,6 +373,15 @@
   </si>
   <si>
     <t>https://www.arquitecturajava.com/angular-select-y-todas-sus-opciones/</t>
+  </si>
+  <si>
+    <t>Corregir el :hover sobre los widget</t>
+  </si>
+  <si>
+    <t>declarar como privada/let this.itemParaBorrar</t>
+  </si>
+  <si>
+    <t>Si está en mostrar form, no habilitar modificar datos grales</t>
   </si>
 </sst>
 </file>
@@ -1148,9 +1148,112 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1205,109 +1308,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1609,7 +1609,7 @@
   <dimension ref="A1:U54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1626,51 +1626,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="85" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50"/>
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="85"/>
+      <c r="H1" s="85"/>
+      <c r="I1" s="85"/>
+      <c r="J1" s="85"/>
+      <c r="K1" s="85"/>
+      <c r="L1" s="85"/>
     </row>
     <row r="2" spans="1:21" ht="18" thickBot="1">
-      <c r="O2" s="100" t="s">
-        <v>93</v>
+      <c r="O2" s="47" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="86" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="52"/>
-      <c r="C3" s="53" t="s">
+      <c r="B3" s="87"/>
+      <c r="C3" s="88" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="54"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="55"/>
-      <c r="H3" s="53" t="s">
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="90"/>
+      <c r="H3" s="88" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="54"/>
-      <c r="J3" s="56"/>
-      <c r="K3" s="55"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="91"/>
+      <c r="K3" s="90"/>
       <c r="L3" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="58" t="s">
-        <v>87</v>
-      </c>
-      <c r="N3" s="49"/>
+      <c r="M3" s="93" t="s">
+        <v>84</v>
+      </c>
+      <c r="N3" s="84"/>
     </row>
     <row r="4" spans="1:21" s="3" customFormat="1" ht="40.5" customHeight="1" thickBot="1">
       <c r="A4" s="17" t="s">
@@ -1709,10 +1709,10 @@
       <c r="L4" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="M4" s="59" t="s">
-        <v>88</v>
-      </c>
-      <c r="N4" s="60"/>
+      <c r="M4" s="94" t="s">
+        <v>85</v>
+      </c>
+      <c r="N4" s="95"/>
       <c r="O4" s="37" t="s">
         <v>64</v>
       </c>
@@ -1754,17 +1754,17 @@
       <c r="K6" s="5"/>
       <c r="L6" s="4"/>
       <c r="M6" s="46" t="s">
-        <v>90</v>
-      </c>
-      <c r="O6" s="48" t="s">
+        <v>87</v>
+      </c>
+      <c r="O6" s="83" t="s">
         <v>68</v>
       </c>
-      <c r="P6" s="49"/>
-      <c r="Q6" s="49"/>
-      <c r="R6" s="49"/>
-      <c r="S6" s="49"/>
-      <c r="T6" s="49"/>
-      <c r="U6" s="49"/>
+      <c r="P6" s="84"/>
+      <c r="Q6" s="84"/>
+      <c r="R6" s="84"/>
+      <c r="S6" s="84"/>
+      <c r="T6" s="84"/>
+      <c r="U6" s="84"/>
     </row>
     <row r="7" spans="1:21" ht="4.5" customHeight="1">
       <c r="A7" s="29"/>
@@ -1797,9 +1797,6 @@
       <c r="J8" s="4"/>
       <c r="K8" s="7"/>
       <c r="L8" s="4"/>
-      <c r="M8" s="46" t="s">
-        <v>86</v>
-      </c>
       <c r="O8" s="6" t="s">
         <v>69</v>
       </c>
@@ -1828,9 +1825,6 @@
       <c r="J9" s="4"/>
       <c r="K9" s="28"/>
       <c r="L9" s="4"/>
-      <c r="M9" s="46" t="s">
-        <v>86</v>
-      </c>
       <c r="P9" s="6" t="s">
         <v>76</v>
       </c>
@@ -1931,14 +1925,14 @@
       <c r="J14" s="4"/>
       <c r="K14" s="7"/>
       <c r="L14" s="4"/>
-      <c r="O14" s="57" t="s">
+      <c r="O14" s="92" t="s">
         <v>82</v>
       </c>
-      <c r="P14" s="57"/>
-      <c r="Q14" s="57"/>
-      <c r="R14" s="57"/>
-      <c r="S14" s="57"/>
-      <c r="T14" s="57"/>
+      <c r="P14" s="92"/>
+      <c r="Q14" s="92"/>
+      <c r="R14" s="92"/>
+      <c r="S14" s="92"/>
+      <c r="T14" s="92"/>
     </row>
     <row r="15" spans="1:21">
       <c r="A15" s="18" t="s">
@@ -1957,15 +1951,12 @@
       <c r="J15" s="4"/>
       <c r="K15" s="7"/>
       <c r="L15" s="4"/>
-      <c r="M15" s="46" t="s">
-        <v>86</v>
-      </c>
-      <c r="O15" s="57"/>
-      <c r="P15" s="57"/>
-      <c r="Q15" s="57"/>
-      <c r="R15" s="57"/>
-      <c r="S15" s="57"/>
-      <c r="T15" s="57"/>
+      <c r="O15" s="92"/>
+      <c r="P15" s="92"/>
+      <c r="Q15" s="92"/>
+      <c r="R15" s="92"/>
+      <c r="S15" s="92"/>
+      <c r="T15" s="92"/>
     </row>
     <row r="16" spans="1:21">
       <c r="A16" s="41" t="s">
@@ -1986,8 +1977,14 @@
       <c r="J16" s="4"/>
       <c r="K16" s="7"/>
       <c r="L16" s="4"/>
-    </row>
-    <row r="17" spans="1:20">
+      <c r="O16" t="s">
+        <v>73</v>
+      </c>
+      <c r="P16" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19">
       <c r="A17" s="18" t="s">
         <v>47</v>
       </c>
@@ -2004,8 +2001,11 @@
       <c r="J17" s="4"/>
       <c r="K17" s="7"/>
       <c r="L17" s="4"/>
-    </row>
-    <row r="18" spans="1:20" ht="4.5" customHeight="1">
+      <c r="O17" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" ht="4.5" customHeight="1">
       <c r="A18" s="29"/>
       <c r="B18" s="30"/>
       <c r="C18" s="31"/>
@@ -2019,7 +2019,7 @@
       <c r="K18" s="31"/>
       <c r="L18" s="31"/>
     </row>
-    <row r="19" spans="1:20">
+    <row r="19" spans="1:19">
       <c r="A19" s="42" t="s">
         <v>16</v>
       </c>
@@ -2042,7 +2042,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="1:20">
+    <row r="20" spans="1:19">
       <c r="A20" s="42" t="s">
         <v>19</v>
       </c>
@@ -2062,7 +2062,7 @@
       <c r="K20" s="7"/>
       <c r="L20" s="32"/>
     </row>
-    <row r="21" spans="1:20" ht="4.5" customHeight="1">
+    <row r="21" spans="1:19" ht="4.5" customHeight="1">
       <c r="A21" s="29"/>
       <c r="B21" s="30"/>
       <c r="C21" s="31"/>
@@ -2076,7 +2076,7 @@
       <c r="K21" s="31"/>
       <c r="L21" s="31"/>
     </row>
-    <row r="22" spans="1:20">
+    <row r="22" spans="1:19">
       <c r="A22" s="42" t="s">
         <v>49</v>
       </c>
@@ -2092,7 +2092,7 @@
       <c r="K22" s="7"/>
       <c r="L22" s="4"/>
     </row>
-    <row r="23" spans="1:20" ht="4.5" customHeight="1">
+    <row r="23" spans="1:19" ht="4.5" customHeight="1">
       <c r="A23" s="29"/>
       <c r="B23" s="30"/>
       <c r="C23" s="31"/>
@@ -2106,7 +2106,7 @@
       <c r="K23" s="31"/>
       <c r="L23" s="31"/>
     </row>
-    <row r="24" spans="1:20">
+    <row r="24" spans="1:19">
       <c r="A24" s="42" t="s">
         <v>50</v>
       </c>
@@ -2121,14 +2121,8 @@
       <c r="J24" s="4"/>
       <c r="K24" s="7"/>
       <c r="L24" s="4"/>
-      <c r="O24" t="s">
-        <v>73</v>
-      </c>
-      <c r="P24" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20">
+    </row>
+    <row r="25" spans="1:19">
       <c r="A25" s="42" t="s">
         <v>51</v>
       </c>
@@ -2145,11 +2139,8 @@
       <c r="J25" s="7"/>
       <c r="K25" s="7"/>
       <c r="L25" s="7"/>
-      <c r="O25" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="26" spans="1:20" ht="4.5" customHeight="1" thickBot="1">
+    </row>
+    <row r="26" spans="1:19" ht="4.5" customHeight="1" thickBot="1">
       <c r="A26" s="29"/>
       <c r="B26" s="30"/>
       <c r="C26" s="31"/>
@@ -2163,59 +2154,59 @@
       <c r="K26" s="31"/>
       <c r="L26" s="31"/>
     </row>
-    <row r="27" spans="1:20" ht="15.75" thickBot="1">
+    <row r="27" spans="1:19" ht="15.75" thickBot="1">
       <c r="A27" s="24"/>
       <c r="B27" s="26"/>
-      <c r="C27" s="53" t="s">
+      <c r="C27" s="88" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="54"/>
-      <c r="E27" s="54"/>
-      <c r="F27" s="54"/>
-      <c r="G27" s="55"/>
-      <c r="H27" s="53" t="s">
+      <c r="D27" s="89"/>
+      <c r="E27" s="89"/>
+      <c r="F27" s="89"/>
+      <c r="G27" s="90"/>
+      <c r="H27" s="88" t="s">
         <v>0</v>
       </c>
-      <c r="I27" s="54"/>
-      <c r="J27" s="56"/>
-      <c r="K27" s="55"/>
+      <c r="I27" s="89"/>
+      <c r="J27" s="91"/>
+      <c r="K27" s="90"/>
       <c r="L27" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="O27" s="47" t="s">
-        <v>85</v>
-      </c>
-      <c r="P27" s="47"/>
-      <c r="Q27" s="47"/>
-      <c r="R27" s="47"/>
-      <c r="S27" s="47"/>
-      <c r="T27" s="47"/>
-    </row>
-    <row r="28" spans="1:20" ht="15.75" thickBot="1">
-      <c r="A28" s="64" t="s">
+      <c r="N27" s="48" t="s">
+        <v>92</v>
+      </c>
+      <c r="O27" s="48"/>
+      <c r="P27" s="48"/>
+      <c r="Q27" s="48"/>
+      <c r="R27" s="48"/>
+      <c r="S27" s="48"/>
+    </row>
+    <row r="28" spans="1:19" ht="15.75" thickBot="1">
+      <c r="A28" s="99" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="65"/>
-      <c r="C28" s="61"/>
-      <c r="D28" s="62"/>
-      <c r="E28" s="62"/>
-      <c r="F28" s="62"/>
-      <c r="G28" s="63"/>
-      <c r="H28" s="61"/>
-      <c r="I28" s="62"/>
-      <c r="J28" s="62"/>
-      <c r="K28" s="63"/>
+      <c r="B28" s="100"/>
+      <c r="C28" s="96"/>
+      <c r="D28" s="97"/>
+      <c r="E28" s="97"/>
+      <c r="F28" s="97"/>
+      <c r="G28" s="98"/>
+      <c r="H28" s="96"/>
+      <c r="I28" s="97"/>
+      <c r="J28" s="97"/>
+      <c r="K28" s="98"/>
       <c r="L28" s="35"/>
-      <c r="O28" s="47" t="s">
-        <v>84</v>
-      </c>
-      <c r="P28" s="47"/>
-      <c r="Q28" s="47"/>
-      <c r="R28" s="47"/>
-      <c r="S28" s="47"/>
-      <c r="T28" s="47"/>
-    </row>
-    <row r="29" spans="1:20" ht="4.5" customHeight="1">
+      <c r="N28" s="50" t="s">
+        <v>91</v>
+      </c>
+      <c r="O28" s="50"/>
+      <c r="P28" s="50"/>
+      <c r="Q28" s="50"/>
+      <c r="R28" s="50"/>
+      <c r="S28" s="50"/>
+    </row>
+    <row r="29" spans="1:19" ht="4.5" customHeight="1">
       <c r="A29" s="29"/>
       <c r="B29" s="30"/>
       <c r="C29" s="31"/>
@@ -2229,107 +2220,103 @@
       <c r="K29" s="31"/>
       <c r="L29" s="31"/>
     </row>
-    <row r="30" spans="1:20" ht="15.75" thickBot="1">
-      <c r="A30" s="70" t="s">
+    <row r="30" spans="1:19" ht="15.75" thickBot="1">
+      <c r="A30" s="59" t="s">
         <v>40</v>
       </c>
-      <c r="B30" s="71"/>
-      <c r="C30" s="66"/>
-      <c r="D30" s="67"/>
-      <c r="E30" s="67"/>
-      <c r="F30" s="67"/>
-      <c r="G30" s="68"/>
-      <c r="H30" s="69"/>
-      <c r="I30" s="67"/>
-      <c r="J30" s="67"/>
-      <c r="K30" s="68"/>
+      <c r="B30" s="60"/>
+      <c r="C30" s="76"/>
+      <c r="D30" s="77"/>
+      <c r="E30" s="77"/>
+      <c r="F30" s="77"/>
+      <c r="G30" s="78"/>
+      <c r="H30" s="79"/>
+      <c r="I30" s="77"/>
+      <c r="J30" s="77"/>
+      <c r="K30" s="78"/>
       <c r="L30" s="22" t="s">
         <v>5</v>
       </c>
       <c r="M30" s="34"/>
-      <c r="N30" s="34"/>
-      <c r="O30" s="99" t="s">
+      <c r="N30" s="50" t="s">
         <v>83</v>
       </c>
-      <c r="P30" s="99"/>
-      <c r="Q30" s="99"/>
-      <c r="R30" s="99"/>
-      <c r="S30" s="99"/>
-      <c r="T30" s="99"/>
-    </row>
-    <row r="31" spans="1:20" ht="15.75" thickBot="1">
-      <c r="A31" s="70" t="s">
-        <v>91</v>
-      </c>
-      <c r="B31" s="71"/>
-      <c r="C31" s="76"/>
-      <c r="D31" s="77"/>
-      <c r="E31" s="77"/>
-      <c r="F31" s="77"/>
-      <c r="G31" s="78"/>
-      <c r="H31" s="79" t="s">
-        <v>92</v>
-      </c>
-      <c r="I31" s="80"/>
-      <c r="J31" s="80"/>
-      <c r="K31" s="80"/>
-      <c r="L31" s="81"/>
+      <c r="O30" s="50"/>
+      <c r="P30" s="50"/>
+      <c r="Q30" s="50"/>
+      <c r="R30" s="50"/>
+      <c r="S30" s="50"/>
+    </row>
+    <row r="31" spans="1:19" ht="15.75" thickBot="1">
+      <c r="A31" s="59" t="s">
+        <v>88</v>
+      </c>
+      <c r="B31" s="60"/>
+      <c r="C31" s="69"/>
+      <c r="D31" s="70"/>
+      <c r="E31" s="70"/>
+      <c r="F31" s="70"/>
+      <c r="G31" s="71"/>
+      <c r="H31" s="80" t="s">
+        <v>89</v>
+      </c>
+      <c r="I31" s="81"/>
+      <c r="J31" s="81"/>
+      <c r="K31" s="81"/>
+      <c r="L31" s="82"/>
       <c r="M31" s="34"/>
-      <c r="N31" s="34"/>
-      <c r="O31" s="99" t="s">
+      <c r="N31" s="50" t="s">
         <v>78</v>
       </c>
-      <c r="P31" s="99"/>
-      <c r="Q31" s="99"/>
-      <c r="R31" s="99"/>
-      <c r="S31" s="99"/>
-      <c r="T31" s="99"/>
-    </row>
-    <row r="32" spans="1:20" ht="16.5" thickBot="1">
+      <c r="O31" s="50"/>
+      <c r="P31" s="50"/>
+      <c r="Q31" s="50"/>
+      <c r="R31" s="50"/>
+      <c r="S31" s="50"/>
+    </row>
+    <row r="32" spans="1:19" ht="16.5" thickBot="1">
       <c r="A32" s="74" t="s">
         <v>62</v>
       </c>
       <c r="B32" s="75"/>
-      <c r="C32" s="66"/>
-      <c r="D32" s="67"/>
-      <c r="E32" s="67"/>
-      <c r="F32" s="67"/>
-      <c r="G32" s="68"/>
-      <c r="H32" s="69"/>
-      <c r="I32" s="67"/>
-      <c r="J32" s="67"/>
-      <c r="K32" s="68"/>
+      <c r="C32" s="76"/>
+      <c r="D32" s="77"/>
+      <c r="E32" s="77"/>
+      <c r="F32" s="77"/>
+      <c r="G32" s="78"/>
+      <c r="H32" s="79"/>
+      <c r="I32" s="77"/>
+      <c r="J32" s="77"/>
+      <c r="K32" s="78"/>
       <c r="M32" s="34"/>
-      <c r="N32" s="34"/>
-    </row>
-    <row r="33" spans="1:20" ht="30.75" customHeight="1" thickBot="1">
+    </row>
+    <row r="33" spans="1:19" ht="30.75" customHeight="1" thickBot="1">
       <c r="A33" s="72" t="s">
         <v>36</v>
       </c>
       <c r="B33" s="73"/>
-      <c r="C33" s="87" t="s">
+      <c r="C33" s="66" t="s">
         <v>61</v>
       </c>
-      <c r="D33" s="88"/>
-      <c r="E33" s="88"/>
-      <c r="F33" s="88"/>
-      <c r="G33" s="89"/>
-      <c r="H33" s="84"/>
-      <c r="I33" s="85"/>
-      <c r="J33" s="85"/>
-      <c r="K33" s="86"/>
+      <c r="D33" s="67"/>
+      <c r="E33" s="67"/>
+      <c r="F33" s="67"/>
+      <c r="G33" s="68"/>
+      <c r="H33" s="63"/>
+      <c r="I33" s="64"/>
+      <c r="J33" s="64"/>
+      <c r="K33" s="65"/>
       <c r="M33" s="34"/>
-      <c r="N33" s="34"/>
-      <c r="O33" s="98" t="s">
+      <c r="N33" s="49" t="s">
         <v>79</v>
       </c>
-      <c r="P33" s="98"/>
-      <c r="Q33" s="98"/>
-      <c r="R33" s="98"/>
-      <c r="S33" s="98"/>
-      <c r="T33" s="98"/>
-    </row>
-    <row r="34" spans="1:20" ht="4.5" customHeight="1" thickBot="1">
+      <c r="O33" s="49"/>
+      <c r="P33" s="49"/>
+      <c r="Q33" s="49"/>
+      <c r="R33" s="49"/>
+      <c r="S33" s="49"/>
+    </row>
+    <row r="34" spans="1:19" ht="4.5" customHeight="1" thickBot="1">
       <c r="A34" s="29"/>
       <c r="B34" s="30"/>
       <c r="C34" s="39"/>
@@ -2342,258 +2329,264 @@
       <c r="J34" s="31"/>
       <c r="K34" s="31"/>
     </row>
-    <row r="35" spans="1:20" ht="15.75" thickBot="1">
-      <c r="A35" s="70" t="s">
+    <row r="35" spans="1:19" ht="15.75" thickBot="1">
+      <c r="A35" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="B35" s="71"/>
-      <c r="C35" s="76"/>
-      <c r="D35" s="77"/>
-      <c r="E35" s="77"/>
-      <c r="F35" s="77"/>
-      <c r="G35" s="78"/>
-      <c r="H35" s="76"/>
-      <c r="I35" s="77"/>
-      <c r="J35" s="77"/>
-      <c r="K35" s="78"/>
+      <c r="B35" s="60"/>
+      <c r="C35" s="69"/>
+      <c r="D35" s="70"/>
+      <c r="E35" s="70"/>
+      <c r="F35" s="70"/>
+      <c r="G35" s="71"/>
+      <c r="H35" s="69"/>
+      <c r="I35" s="70"/>
+      <c r="J35" s="70"/>
+      <c r="K35" s="71"/>
       <c r="M35" s="34"/>
-      <c r="N35" s="34"/>
-      <c r="O35" s="99" t="s">
+      <c r="N35" s="50" t="s">
         <v>81</v>
       </c>
-      <c r="P35" s="99"/>
-      <c r="Q35" s="99"/>
-      <c r="R35" s="99"/>
-      <c r="S35" s="99"/>
-      <c r="T35" s="99"/>
-    </row>
-    <row r="36" spans="1:20" ht="15.75" thickBot="1">
-      <c r="A36" s="70" t="s">
+      <c r="O35" s="50"/>
+      <c r="P35" s="50"/>
+      <c r="Q35" s="50"/>
+      <c r="R35" s="50"/>
+      <c r="S35" s="50"/>
+    </row>
+    <row r="36" spans="1:19" ht="15.75" thickBot="1">
+      <c r="A36" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="B36" s="71"/>
-      <c r="C36" s="76"/>
-      <c r="D36" s="77"/>
-      <c r="E36" s="77"/>
-      <c r="F36" s="77"/>
-      <c r="G36" s="78"/>
-      <c r="H36" s="76"/>
-      <c r="I36" s="77"/>
-      <c r="J36" s="77"/>
-      <c r="K36" s="78"/>
+      <c r="B36" s="60"/>
+      <c r="C36" s="69"/>
+      <c r="D36" s="70"/>
+      <c r="E36" s="70"/>
+      <c r="F36" s="70"/>
+      <c r="G36" s="71"/>
+      <c r="H36" s="69"/>
+      <c r="I36" s="70"/>
+      <c r="J36" s="70"/>
+      <c r="K36" s="71"/>
       <c r="M36" s="34"/>
-      <c r="N36" s="34"/>
-    </row>
-    <row r="37" spans="1:20" ht="15.75" thickBot="1">
-      <c r="A37" s="70" t="s">
+      <c r="N36" s="48" t="s">
+        <v>86</v>
+      </c>
+      <c r="O36" s="48"/>
+      <c r="P36" s="48"/>
+      <c r="Q36" s="48"/>
+      <c r="R36" s="48"/>
+      <c r="S36" s="48"/>
+    </row>
+    <row r="37" spans="1:19" ht="15.75" thickBot="1">
+      <c r="A37" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="B37" s="71"/>
-      <c r="C37" s="76"/>
-      <c r="D37" s="77"/>
-      <c r="E37" s="77"/>
-      <c r="F37" s="77"/>
-      <c r="G37" s="78"/>
-      <c r="H37" s="76"/>
-      <c r="I37" s="77"/>
-      <c r="J37" s="77"/>
-      <c r="K37" s="78"/>
+      <c r="B37" s="60"/>
+      <c r="C37" s="69"/>
+      <c r="D37" s="70"/>
+      <c r="E37" s="70"/>
+      <c r="F37" s="70"/>
+      <c r="G37" s="71"/>
+      <c r="H37" s="69"/>
+      <c r="I37" s="70"/>
+      <c r="J37" s="70"/>
+      <c r="K37" s="71"/>
       <c r="M37" s="34"/>
-      <c r="N37" s="34"/>
-      <c r="O37" s="47" t="s">
-        <v>89</v>
-      </c>
-      <c r="P37" s="47"/>
-      <c r="Q37" s="47"/>
-      <c r="R37" s="47"/>
-      <c r="S37" s="47"/>
-      <c r="T37" s="47"/>
-    </row>
-    <row r="38" spans="1:20" ht="15.75" thickBot="1"/>
-    <row r="39" spans="1:20" ht="15.75" thickBot="1">
-      <c r="A39" s="91" t="s">
+    </row>
+    <row r="38" spans="1:19" ht="15.75" thickBot="1">
+      <c r="N38" s="48" t="s">
+        <v>93</v>
+      </c>
+      <c r="O38" s="48"/>
+      <c r="P38" s="48"/>
+      <c r="Q38" s="48"/>
+      <c r="R38" s="48"/>
+      <c r="S38" s="48"/>
+    </row>
+    <row r="39" spans="1:19" ht="15.75" thickBot="1">
+      <c r="A39" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="B39" s="92"/>
-      <c r="C39" s="92"/>
-      <c r="D39" s="92"/>
-      <c r="E39" s="93"/>
-    </row>
-    <row r="40" spans="1:20">
+      <c r="B39" s="53"/>
+      <c r="C39" s="53"/>
+      <c r="D39" s="53"/>
+      <c r="E39" s="54"/>
+    </row>
+    <row r="40" spans="1:19">
       <c r="A40" s="14" t="s">
         <v>26</v>
       </c>
       <c r="B40" s="13"/>
-      <c r="C40" s="94" t="s">
+      <c r="C40" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="D40" s="95"/>
+      <c r="D40" s="56"/>
       <c r="E40" s="28"/>
     </row>
-    <row r="41" spans="1:20">
+    <row r="41" spans="1:19">
       <c r="A41" s="15" t="s">
         <v>22</v>
       </c>
       <c r="B41" s="5"/>
-      <c r="C41" s="94" t="s">
+      <c r="C41" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="D41" s="95"/>
+      <c r="D41" s="56"/>
       <c r="E41" s="8"/>
     </row>
-    <row r="42" spans="1:20">
+    <row r="42" spans="1:19">
       <c r="A42" s="15" t="s">
         <v>25</v>
       </c>
       <c r="B42" s="6"/>
-      <c r="C42" s="82" t="s">
+      <c r="C42" s="61" t="s">
         <v>67</v>
       </c>
-      <c r="D42" s="83"/>
+      <c r="D42" s="62"/>
       <c r="E42" s="40"/>
     </row>
-    <row r="43" spans="1:20" ht="15.75" thickBot="1"/>
-    <row r="44" spans="1:20">
-      <c r="A44" s="96" t="s">
+    <row r="43" spans="1:19" ht="15.75" thickBot="1"/>
+    <row r="44" spans="1:19">
+      <c r="A44" s="57" t="s">
         <v>37</v>
       </c>
-      <c r="B44" s="97"/>
-      <c r="C44" s="97"/>
-      <c r="D44" s="97"/>
-      <c r="E44" s="97"/>
-      <c r="F44" s="97"/>
-      <c r="G44" s="97"/>
-      <c r="H44" s="97"/>
-      <c r="I44" s="97"/>
-      <c r="J44" s="97"/>
-      <c r="K44" s="97"/>
-      <c r="L44" s="97"/>
-    </row>
-    <row r="45" spans="1:20">
+      <c r="B44" s="58"/>
+      <c r="C44" s="58"/>
+      <c r="D44" s="58"/>
+      <c r="E44" s="58"/>
+      <c r="F44" s="58"/>
+      <c r="G44" s="58"/>
+      <c r="H44" s="58"/>
+      <c r="I44" s="58"/>
+      <c r="J44" s="58"/>
+      <c r="K44" s="58"/>
+      <c r="L44" s="58"/>
+    </row>
+    <row r="45" spans="1:19">
       <c r="A45" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="B45" s="90" t="s">
+      <c r="B45" s="51" t="s">
         <v>57</v>
       </c>
-      <c r="C45" s="90"/>
-      <c r="D45" s="90"/>
-      <c r="E45" s="90"/>
-      <c r="F45" s="90"/>
-      <c r="G45" s="90"/>
-      <c r="H45" s="90"/>
-      <c r="I45" s="90"/>
-      <c r="J45" s="90"/>
-      <c r="K45" s="90"/>
-      <c r="L45" s="90"/>
-    </row>
-    <row r="46" spans="1:20" ht="15" customHeight="1">
+      <c r="C45" s="51"/>
+      <c r="D45" s="51"/>
+      <c r="E45" s="51"/>
+      <c r="F45" s="51"/>
+      <c r="G45" s="51"/>
+      <c r="H45" s="51"/>
+      <c r="I45" s="51"/>
+      <c r="J45" s="51"/>
+      <c r="K45" s="51"/>
+      <c r="L45" s="51"/>
+    </row>
+    <row r="46" spans="1:19" ht="15" customHeight="1">
       <c r="A46" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="B46" s="90" t="s">
+      <c r="B46" s="51" t="s">
         <v>58</v>
       </c>
-      <c r="C46" s="90"/>
-      <c r="D46" s="90"/>
-      <c r="E46" s="90"/>
-      <c r="F46" s="90"/>
-      <c r="G46" s="90"/>
-      <c r="H46" s="90"/>
-      <c r="I46" s="90"/>
-      <c r="J46" s="90"/>
-      <c r="K46" s="90"/>
-      <c r="L46" s="90"/>
-    </row>
-    <row r="47" spans="1:20">
+      <c r="C46" s="51"/>
+      <c r="D46" s="51"/>
+      <c r="E46" s="51"/>
+      <c r="F46" s="51"/>
+      <c r="G46" s="51"/>
+      <c r="H46" s="51"/>
+      <c r="I46" s="51"/>
+      <c r="J46" s="51"/>
+      <c r="K46" s="51"/>
+      <c r="L46" s="51"/>
+    </row>
+    <row r="47" spans="1:19">
       <c r="A47" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="B47" s="90" t="s">
+      <c r="B47" s="51" t="s">
         <v>59</v>
       </c>
-      <c r="C47" s="90"/>
-      <c r="D47" s="90"/>
-      <c r="E47" s="90"/>
-      <c r="F47" s="90"/>
-      <c r="G47" s="90"/>
-      <c r="H47" s="90"/>
-      <c r="I47" s="90"/>
-      <c r="J47" s="90"/>
-      <c r="K47" s="90"/>
-      <c r="L47" s="90"/>
-    </row>
-    <row r="48" spans="1:20">
+      <c r="C47" s="51"/>
+      <c r="D47" s="51"/>
+      <c r="E47" s="51"/>
+      <c r="F47" s="51"/>
+      <c r="G47" s="51"/>
+      <c r="H47" s="51"/>
+      <c r="I47" s="51"/>
+      <c r="J47" s="51"/>
+      <c r="K47" s="51"/>
+      <c r="L47" s="51"/>
+    </row>
+    <row r="48" spans="1:19">
       <c r="A48" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="B48" s="90" t="s">
+      <c r="B48" s="51" t="s">
         <v>46</v>
       </c>
-      <c r="C48" s="90"/>
-      <c r="D48" s="90"/>
-      <c r="E48" s="90"/>
-      <c r="F48" s="90"/>
-      <c r="G48" s="90"/>
-      <c r="H48" s="90"/>
-      <c r="I48" s="90"/>
-      <c r="J48" s="90"/>
-      <c r="K48" s="90"/>
-      <c r="L48" s="90"/>
+      <c r="C48" s="51"/>
+      <c r="D48" s="51"/>
+      <c r="E48" s="51"/>
+      <c r="F48" s="51"/>
+      <c r="G48" s="51"/>
+      <c r="H48" s="51"/>
+      <c r="I48" s="51"/>
+      <c r="J48" s="51"/>
+      <c r="K48" s="51"/>
+      <c r="L48" s="51"/>
     </row>
     <row r="49" spans="1:12">
       <c r="A49" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="B49" s="90" t="s">
+      <c r="B49" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="C49" s="90"/>
-      <c r="D49" s="90"/>
-      <c r="E49" s="90"/>
-      <c r="F49" s="90"/>
-      <c r="G49" s="90"/>
-      <c r="H49" s="90"/>
-      <c r="I49" s="90"/>
-      <c r="J49" s="90"/>
-      <c r="K49" s="90"/>
-      <c r="L49" s="90"/>
+      <c r="C49" s="51"/>
+      <c r="D49" s="51"/>
+      <c r="E49" s="51"/>
+      <c r="F49" s="51"/>
+      <c r="G49" s="51"/>
+      <c r="H49" s="51"/>
+      <c r="I49" s="51"/>
+      <c r="J49" s="51"/>
+      <c r="K49" s="51"/>
+      <c r="L49" s="51"/>
     </row>
     <row r="50" spans="1:12">
       <c r="A50" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="B50" s="90" t="s">
+      <c r="B50" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="C50" s="90"/>
-      <c r="D50" s="90"/>
-      <c r="E50" s="90"/>
-      <c r="F50" s="90"/>
-      <c r="G50" s="90"/>
-      <c r="H50" s="90"/>
-      <c r="I50" s="90"/>
-      <c r="J50" s="90"/>
-      <c r="K50" s="90"/>
-      <c r="L50" s="90"/>
+      <c r="C50" s="51"/>
+      <c r="D50" s="51"/>
+      <c r="E50" s="51"/>
+      <c r="F50" s="51"/>
+      <c r="G50" s="51"/>
+      <c r="H50" s="51"/>
+      <c r="I50" s="51"/>
+      <c r="J50" s="51"/>
+      <c r="K50" s="51"/>
+      <c r="L50" s="51"/>
     </row>
     <row r="51" spans="1:12">
       <c r="A51" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="B51" s="90" t="s">
+      <c r="B51" s="51" t="s">
         <v>55</v>
       </c>
-      <c r="C51" s="90"/>
-      <c r="D51" s="90"/>
-      <c r="E51" s="90"/>
-      <c r="F51" s="90"/>
-      <c r="G51" s="90"/>
-      <c r="H51" s="90"/>
-      <c r="I51" s="90"/>
-      <c r="J51" s="90"/>
-      <c r="K51" s="90"/>
-      <c r="L51" s="90"/>
+      <c r="C51" s="51"/>
+      <c r="D51" s="51"/>
+      <c r="E51" s="51"/>
+      <c r="F51" s="51"/>
+      <c r="G51" s="51"/>
+      <c r="H51" s="51"/>
+      <c r="I51" s="51"/>
+      <c r="J51" s="51"/>
+      <c r="K51" s="51"/>
+      <c r="L51" s="51"/>
     </row>
     <row r="52" spans="1:12">
       <c r="C52" s="34"/>
@@ -2608,45 +2601,9 @@
   <sortState ref="A24:K25">
     <sortCondition ref="A3"/>
   </sortState>
-  <mergeCells count="53">
-    <mergeCell ref="O27:T27"/>
-    <mergeCell ref="O33:T33"/>
-    <mergeCell ref="O35:T35"/>
-    <mergeCell ref="O30:T30"/>
-    <mergeCell ref="O28:T28"/>
-    <mergeCell ref="O31:T31"/>
-    <mergeCell ref="B50:L50"/>
-    <mergeCell ref="B51:L51"/>
-    <mergeCell ref="A39:E39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="B45:L45"/>
-    <mergeCell ref="A44:L44"/>
-    <mergeCell ref="B46:L46"/>
-    <mergeCell ref="B47:L47"/>
-    <mergeCell ref="B48:L48"/>
-    <mergeCell ref="B49:L49"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="H33:K33"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="H35:K35"/>
-    <mergeCell ref="H36:K36"/>
-    <mergeCell ref="H37:K37"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="H32:K32"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="H31:L31"/>
-    <mergeCell ref="O37:T37"/>
+  <mergeCells count="54">
+    <mergeCell ref="N38:S38"/>
+    <mergeCell ref="N36:S36"/>
     <mergeCell ref="O6:U6"/>
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="A3:B3"/>
@@ -2662,6 +2619,43 @@
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="C30:G30"/>
     <mergeCell ref="H30:K30"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="H32:K32"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="H31:L31"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="H33:K33"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="H35:K35"/>
+    <mergeCell ref="H36:K36"/>
+    <mergeCell ref="H37:K37"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="B50:L50"/>
+    <mergeCell ref="B51:L51"/>
+    <mergeCell ref="A39:E39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="B45:L45"/>
+    <mergeCell ref="A44:L44"/>
+    <mergeCell ref="B46:L46"/>
+    <mergeCell ref="B47:L47"/>
+    <mergeCell ref="B48:L48"/>
+    <mergeCell ref="B49:L49"/>
+    <mergeCell ref="N27:S27"/>
+    <mergeCell ref="N33:S33"/>
+    <mergeCell ref="N35:S35"/>
+    <mergeCell ref="N30:S30"/>
+    <mergeCell ref="N28:S28"/>
+    <mergeCell ref="N31:S31"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="Q4" r:id="rId1"/>

</xml_diff>

<commit_message>
existe error al crear archivo .jar, es el mismo error que se genera en el despliegue, claramente es la imagen de un compilado que no puede encontrar la clase Main del proyecto, sin embargo desde netbeans corre bien, usando la DB subida a clever-cloud
</commit_message>
<xml_diff>
--- a/Cuadro-de-estado.xlsx
+++ b/Cuadro-de-estado.xlsx
@@ -1054,7 +1054,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1124,7 +1124,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1152,161 +1151,161 @@
     <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1609,7 +1608,7 @@
   <dimension ref="A1:U54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1626,51 +1625,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25">
-      <c r="A1" s="85" t="s">
+      <c r="A1" s="50" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="85"/>
-      <c r="C1" s="85"/>
-      <c r="D1" s="85"/>
-      <c r="E1" s="85"/>
-      <c r="F1" s="85"/>
-      <c r="G1" s="85"/>
-      <c r="H1" s="85"/>
-      <c r="I1" s="85"/>
-      <c r="J1" s="85"/>
-      <c r="K1" s="85"/>
-      <c r="L1" s="85"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="50"/>
+      <c r="L1" s="50"/>
     </row>
     <row r="2" spans="1:21" ht="18" thickBot="1">
-      <c r="O2" s="47" t="s">
+      <c r="O2" s="46" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="86" t="s">
+      <c r="A3" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="87"/>
-      <c r="C3" s="88" t="s">
+      <c r="B3" s="52"/>
+      <c r="C3" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="90"/>
-      <c r="H3" s="88" t="s">
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="89"/>
-      <c r="J3" s="91"/>
-      <c r="K3" s="90"/>
+      <c r="I3" s="54"/>
+      <c r="J3" s="56"/>
+      <c r="K3" s="55"/>
       <c r="L3" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="93" t="s">
+      <c r="M3" s="58" t="s">
         <v>84</v>
       </c>
-      <c r="N3" s="84"/>
+      <c r="N3" s="49"/>
     </row>
     <row r="4" spans="1:21" s="3" customFormat="1" ht="40.5" customHeight="1" thickBot="1">
       <c r="A4" s="17" t="s">
@@ -1709,14 +1708,14 @@
       <c r="L4" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="M4" s="94" t="s">
+      <c r="M4" s="59" t="s">
         <v>85</v>
       </c>
-      <c r="N4" s="95"/>
-      <c r="O4" s="37" t="s">
+      <c r="N4" s="60"/>
+      <c r="O4" s="36" t="s">
         <v>64</v>
       </c>
-      <c r="Q4" s="38" t="s">
+      <c r="Q4" s="37" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1753,18 +1752,18 @@
       <c r="J6" s="4"/>
       <c r="K6" s="5"/>
       <c r="L6" s="4"/>
-      <c r="M6" s="46" t="s">
+      <c r="M6" s="45" t="s">
         <v>87</v>
       </c>
-      <c r="O6" s="83" t="s">
+      <c r="O6" s="48" t="s">
         <v>68</v>
       </c>
-      <c r="P6" s="84"/>
-      <c r="Q6" s="84"/>
-      <c r="R6" s="84"/>
-      <c r="S6" s="84"/>
-      <c r="T6" s="84"/>
-      <c r="U6" s="84"/>
+      <c r="P6" s="49"/>
+      <c r="Q6" s="49"/>
+      <c r="R6" s="49"/>
+      <c r="S6" s="49"/>
+      <c r="T6" s="49"/>
+      <c r="U6" s="49"/>
     </row>
     <row r="7" spans="1:21" ht="4.5" customHeight="1">
       <c r="A7" s="29"/>
@@ -1887,14 +1886,14 @@
       <c r="L12" s="31"/>
     </row>
     <row r="13" spans="1:21">
-      <c r="A13" s="41" t="s">
+      <c r="A13" s="40" t="s">
         <v>30</v>
       </c>
       <c r="B13" s="25" t="s">
         <v>13</v>
       </c>
       <c r="C13" s="5"/>
-      <c r="D13" s="43" t="s">
+      <c r="D13" s="42" t="s">
         <v>80</v>
       </c>
       <c r="E13" s="13"/>
@@ -1907,14 +1906,14 @@
       <c r="L13" s="4"/>
     </row>
     <row r="14" spans="1:21">
-      <c r="A14" s="41" t="s">
+      <c r="A14" s="40" t="s">
         <v>18</v>
       </c>
       <c r="B14" s="25" t="s">
         <v>13</v>
       </c>
       <c r="C14" s="5"/>
-      <c r="D14" s="43" t="s">
+      <c r="D14" s="42" t="s">
         <v>80</v>
       </c>
       <c r="E14" s="5"/>
@@ -1925,14 +1924,14 @@
       <c r="J14" s="4"/>
       <c r="K14" s="7"/>
       <c r="L14" s="4"/>
-      <c r="O14" s="92" t="s">
+      <c r="O14" s="57" t="s">
         <v>82</v>
       </c>
-      <c r="P14" s="92"/>
-      <c r="Q14" s="92"/>
-      <c r="R14" s="92"/>
-      <c r="S14" s="92"/>
-      <c r="T14" s="92"/>
+      <c r="P14" s="57"/>
+      <c r="Q14" s="57"/>
+      <c r="R14" s="57"/>
+      <c r="S14" s="57"/>
+      <c r="T14" s="57"/>
     </row>
     <row r="15" spans="1:21">
       <c r="A15" s="18" t="s">
@@ -1942,7 +1941,7 @@
         <v>12</v>
       </c>
       <c r="C15" s="5"/>
-      <c r="D15" s="44"/>
+      <c r="D15" s="43"/>
       <c r="E15" s="5"/>
       <c r="F15" s="16"/>
       <c r="G15" s="5"/>
@@ -1951,22 +1950,22 @@
       <c r="J15" s="4"/>
       <c r="K15" s="7"/>
       <c r="L15" s="4"/>
-      <c r="O15" s="92"/>
-      <c r="P15" s="92"/>
-      <c r="Q15" s="92"/>
-      <c r="R15" s="92"/>
-      <c r="S15" s="92"/>
-      <c r="T15" s="92"/>
+      <c r="O15" s="57"/>
+      <c r="P15" s="57"/>
+      <c r="Q15" s="57"/>
+      <c r="R15" s="57"/>
+      <c r="S15" s="57"/>
+      <c r="T15" s="57"/>
     </row>
     <row r="16" spans="1:21">
-      <c r="A16" s="41" t="s">
+      <c r="A16" s="40" t="s">
         <v>9</v>
       </c>
       <c r="B16" s="25" t="s">
         <v>13</v>
       </c>
       <c r="C16" s="5"/>
-      <c r="D16" s="43" t="s">
+      <c r="D16" s="42" t="s">
         <v>80</v>
       </c>
       <c r="E16" s="5"/>
@@ -1992,7 +1991,7 @@
         <v>12</v>
       </c>
       <c r="C17" s="5"/>
-      <c r="D17" s="44"/>
+      <c r="D17" s="43"/>
       <c r="E17" s="5"/>
       <c r="F17" s="16"/>
       <c r="G17" s="5"/>
@@ -2020,14 +2019,14 @@
       <c r="L18" s="31"/>
     </row>
     <row r="19" spans="1:19">
-      <c r="A19" s="42" t="s">
+      <c r="A19" s="41" t="s">
         <v>16</v>
       </c>
       <c r="B19" s="25" t="s">
         <v>13</v>
       </c>
       <c r="C19" s="16"/>
-      <c r="D19" s="45" t="s">
+      <c r="D19" s="44" t="s">
         <v>80</v>
       </c>
       <c r="E19" s="6"/>
@@ -2043,14 +2042,14 @@
       </c>
     </row>
     <row r="20" spans="1:19">
-      <c r="A20" s="42" t="s">
+      <c r="A20" s="41" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="25" t="s">
         <v>13</v>
       </c>
       <c r="C20" s="16"/>
-      <c r="D20" s="45" t="s">
+      <c r="D20" s="44" t="s">
         <v>80</v>
       </c>
       <c r="E20" s="6"/>
@@ -2077,7 +2076,7 @@
       <c r="L21" s="31"/>
     </row>
     <row r="22" spans="1:19">
-      <c r="A22" s="42" t="s">
+      <c r="A22" s="41" t="s">
         <v>49</v>
       </c>
       <c r="B22" s="20"/>
@@ -2107,7 +2106,7 @@
       <c r="L23" s="31"/>
     </row>
     <row r="24" spans="1:19">
-      <c r="A24" s="42" t="s">
+      <c r="A24" s="41" t="s">
         <v>50</v>
       </c>
       <c r="B24" s="33"/>
@@ -2123,7 +2122,7 @@
       <c r="L24" s="4"/>
     </row>
     <row r="25" spans="1:19">
-      <c r="A25" s="42" t="s">
+      <c r="A25" s="41" t="s">
         <v>51</v>
       </c>
       <c r="B25" s="25" t="s">
@@ -2157,54 +2156,54 @@
     <row r="27" spans="1:19" ht="15.75" thickBot="1">
       <c r="A27" s="24"/>
       <c r="B27" s="26"/>
-      <c r="C27" s="88" t="s">
+      <c r="C27" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="89"/>
-      <c r="E27" s="89"/>
-      <c r="F27" s="89"/>
-      <c r="G27" s="90"/>
-      <c r="H27" s="88" t="s">
+      <c r="D27" s="54"/>
+      <c r="E27" s="54"/>
+      <c r="F27" s="54"/>
+      <c r="G27" s="55"/>
+      <c r="H27" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="I27" s="89"/>
-      <c r="J27" s="91"/>
-      <c r="K27" s="90"/>
+      <c r="I27" s="54"/>
+      <c r="J27" s="56"/>
+      <c r="K27" s="55"/>
       <c r="L27" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="N27" s="48" t="s">
+      <c r="N27" s="47" t="s">
         <v>92</v>
       </c>
-      <c r="O27" s="48"/>
-      <c r="P27" s="48"/>
-      <c r="Q27" s="48"/>
-      <c r="R27" s="48"/>
-      <c r="S27" s="48"/>
+      <c r="O27" s="47"/>
+      <c r="P27" s="47"/>
+      <c r="Q27" s="47"/>
+      <c r="R27" s="47"/>
+      <c r="S27" s="47"/>
     </row>
     <row r="28" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A28" s="99" t="s">
+      <c r="A28" s="64" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="100"/>
-      <c r="C28" s="96"/>
-      <c r="D28" s="97"/>
-      <c r="E28" s="97"/>
-      <c r="F28" s="97"/>
-      <c r="G28" s="98"/>
-      <c r="H28" s="96"/>
-      <c r="I28" s="97"/>
-      <c r="J28" s="97"/>
-      <c r="K28" s="98"/>
-      <c r="L28" s="35"/>
-      <c r="N28" s="50" t="s">
+      <c r="B28" s="65"/>
+      <c r="C28" s="61"/>
+      <c r="D28" s="62"/>
+      <c r="E28" s="62"/>
+      <c r="F28" s="62"/>
+      <c r="G28" s="63"/>
+      <c r="H28" s="61"/>
+      <c r="I28" s="62"/>
+      <c r="J28" s="62"/>
+      <c r="K28" s="63"/>
+      <c r="L28" s="4"/>
+      <c r="N28" s="99" t="s">
         <v>91</v>
       </c>
-      <c r="O28" s="50"/>
-      <c r="P28" s="50"/>
-      <c r="Q28" s="50"/>
-      <c r="R28" s="50"/>
-      <c r="S28" s="50"/>
+      <c r="O28" s="99"/>
+      <c r="P28" s="99"/>
+      <c r="Q28" s="99"/>
+      <c r="R28" s="99"/>
+      <c r="S28" s="99"/>
     </row>
     <row r="29" spans="1:19" ht="4.5" customHeight="1">
       <c r="A29" s="29"/>
@@ -2221,73 +2220,73 @@
       <c r="L29" s="31"/>
     </row>
     <row r="30" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A30" s="59" t="s">
+      <c r="A30" s="70" t="s">
         <v>40</v>
       </c>
-      <c r="B30" s="60"/>
-      <c r="C30" s="76"/>
-      <c r="D30" s="77"/>
-      <c r="E30" s="77"/>
-      <c r="F30" s="77"/>
-      <c r="G30" s="78"/>
-      <c r="H30" s="79"/>
-      <c r="I30" s="77"/>
-      <c r="J30" s="77"/>
-      <c r="K30" s="78"/>
+      <c r="B30" s="71"/>
+      <c r="C30" s="66"/>
+      <c r="D30" s="67"/>
+      <c r="E30" s="67"/>
+      <c r="F30" s="67"/>
+      <c r="G30" s="68"/>
+      <c r="H30" s="69"/>
+      <c r="I30" s="67"/>
+      <c r="J30" s="67"/>
+      <c r="K30" s="68"/>
       <c r="L30" s="22" t="s">
         <v>5</v>
       </c>
       <c r="M30" s="34"/>
-      <c r="N30" s="50" t="s">
+      <c r="N30" s="99" t="s">
         <v>83</v>
       </c>
-      <c r="O30" s="50"/>
-      <c r="P30" s="50"/>
-      <c r="Q30" s="50"/>
-      <c r="R30" s="50"/>
-      <c r="S30" s="50"/>
+      <c r="O30" s="99"/>
+      <c r="P30" s="99"/>
+      <c r="Q30" s="99"/>
+      <c r="R30" s="99"/>
+      <c r="S30" s="99"/>
     </row>
     <row r="31" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A31" s="59" t="s">
+      <c r="A31" s="70" t="s">
         <v>88</v>
       </c>
-      <c r="B31" s="60"/>
-      <c r="C31" s="69"/>
-      <c r="D31" s="70"/>
-      <c r="E31" s="70"/>
-      <c r="F31" s="70"/>
-      <c r="G31" s="71"/>
-      <c r="H31" s="80" t="s">
+      <c r="B31" s="71"/>
+      <c r="C31" s="76"/>
+      <c r="D31" s="77"/>
+      <c r="E31" s="77"/>
+      <c r="F31" s="77"/>
+      <c r="G31" s="78"/>
+      <c r="H31" s="79" t="s">
         <v>89</v>
       </c>
-      <c r="I31" s="81"/>
-      <c r="J31" s="81"/>
-      <c r="K31" s="81"/>
-      <c r="L31" s="82"/>
+      <c r="I31" s="80"/>
+      <c r="J31" s="80"/>
+      <c r="K31" s="80"/>
+      <c r="L31" s="81"/>
       <c r="M31" s="34"/>
-      <c r="N31" s="50" t="s">
+      <c r="N31" s="99" t="s">
         <v>78</v>
       </c>
-      <c r="O31" s="50"/>
-      <c r="P31" s="50"/>
-      <c r="Q31" s="50"/>
-      <c r="R31" s="50"/>
-      <c r="S31" s="50"/>
+      <c r="O31" s="99"/>
+      <c r="P31" s="99"/>
+      <c r="Q31" s="99"/>
+      <c r="R31" s="99"/>
+      <c r="S31" s="99"/>
     </row>
     <row r="32" spans="1:19" ht="16.5" thickBot="1">
       <c r="A32" s="74" t="s">
         <v>62</v>
       </c>
       <c r="B32" s="75"/>
-      <c r="C32" s="76"/>
-      <c r="D32" s="77"/>
-      <c r="E32" s="77"/>
-      <c r="F32" s="77"/>
-      <c r="G32" s="78"/>
-      <c r="H32" s="79"/>
-      <c r="I32" s="77"/>
-      <c r="J32" s="77"/>
-      <c r="K32" s="78"/>
+      <c r="C32" s="66"/>
+      <c r="D32" s="67"/>
+      <c r="E32" s="67"/>
+      <c r="F32" s="67"/>
+      <c r="G32" s="68"/>
+      <c r="H32" s="69"/>
+      <c r="I32" s="67"/>
+      <c r="J32" s="67"/>
+      <c r="K32" s="68"/>
       <c r="M32" s="34"/>
     </row>
     <row r="33" spans="1:19" ht="30.75" customHeight="1" thickBot="1">
@@ -2295,132 +2294,132 @@
         <v>36</v>
       </c>
       <c r="B33" s="73"/>
-      <c r="C33" s="66" t="s">
+      <c r="C33" s="87" t="s">
         <v>61</v>
       </c>
-      <c r="D33" s="67"/>
-      <c r="E33" s="67"/>
-      <c r="F33" s="67"/>
-      <c r="G33" s="68"/>
-      <c r="H33" s="63"/>
-      <c r="I33" s="64"/>
-      <c r="J33" s="64"/>
-      <c r="K33" s="65"/>
+      <c r="D33" s="88"/>
+      <c r="E33" s="88"/>
+      <c r="F33" s="88"/>
+      <c r="G33" s="89"/>
+      <c r="H33" s="84"/>
+      <c r="I33" s="85"/>
+      <c r="J33" s="85"/>
+      <c r="K33" s="86"/>
       <c r="M33" s="34"/>
-      <c r="N33" s="49" t="s">
+      <c r="N33" s="98" t="s">
         <v>79</v>
       </c>
-      <c r="O33" s="49"/>
-      <c r="P33" s="49"/>
-      <c r="Q33" s="49"/>
-      <c r="R33" s="49"/>
-      <c r="S33" s="49"/>
+      <c r="O33" s="98"/>
+      <c r="P33" s="98"/>
+      <c r="Q33" s="98"/>
+      <c r="R33" s="98"/>
+      <c r="S33" s="98"/>
     </row>
     <row r="34" spans="1:19" ht="4.5" customHeight="1" thickBot="1">
       <c r="A34" s="29"/>
       <c r="B34" s="30"/>
-      <c r="C34" s="39"/>
-      <c r="D34" s="39"/>
-      <c r="E34" s="39"/>
-      <c r="F34" s="39"/>
-      <c r="G34" s="39"/>
+      <c r="C34" s="38"/>
+      <c r="D34" s="38"/>
+      <c r="E34" s="38"/>
+      <c r="F34" s="38"/>
+      <c r="G34" s="38"/>
       <c r="H34" s="31"/>
       <c r="I34" s="31"/>
       <c r="J34" s="31"/>
       <c r="K34" s="31"/>
     </row>
     <row r="35" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A35" s="59" t="s">
+      <c r="A35" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="B35" s="60"/>
-      <c r="C35" s="69"/>
-      <c r="D35" s="70"/>
-      <c r="E35" s="70"/>
-      <c r="F35" s="70"/>
-      <c r="G35" s="71"/>
-      <c r="H35" s="69"/>
-      <c r="I35" s="70"/>
-      <c r="J35" s="70"/>
-      <c r="K35" s="71"/>
+      <c r="B35" s="71"/>
+      <c r="C35" s="76"/>
+      <c r="D35" s="77"/>
+      <c r="E35" s="77"/>
+      <c r="F35" s="77"/>
+      <c r="G35" s="78"/>
+      <c r="H35" s="76"/>
+      <c r="I35" s="77"/>
+      <c r="J35" s="77"/>
+      <c r="K35" s="78"/>
       <c r="M35" s="34"/>
-      <c r="N35" s="50" t="s">
+      <c r="N35" s="99" t="s">
         <v>81</v>
       </c>
-      <c r="O35" s="50"/>
-      <c r="P35" s="50"/>
-      <c r="Q35" s="50"/>
-      <c r="R35" s="50"/>
-      <c r="S35" s="50"/>
+      <c r="O35" s="99"/>
+      <c r="P35" s="99"/>
+      <c r="Q35" s="99"/>
+      <c r="R35" s="99"/>
+      <c r="S35" s="99"/>
     </row>
     <row r="36" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A36" s="59" t="s">
+      <c r="A36" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="B36" s="60"/>
-      <c r="C36" s="69"/>
-      <c r="D36" s="70"/>
-      <c r="E36" s="70"/>
-      <c r="F36" s="70"/>
-      <c r="G36" s="71"/>
-      <c r="H36" s="69"/>
-      <c r="I36" s="70"/>
-      <c r="J36" s="70"/>
-      <c r="K36" s="71"/>
+      <c r="B36" s="71"/>
+      <c r="C36" s="76"/>
+      <c r="D36" s="77"/>
+      <c r="E36" s="77"/>
+      <c r="F36" s="77"/>
+      <c r="G36" s="78"/>
+      <c r="H36" s="76"/>
+      <c r="I36" s="77"/>
+      <c r="J36" s="77"/>
+      <c r="K36" s="78"/>
       <c r="M36" s="34"/>
-      <c r="N36" s="48" t="s">
+      <c r="N36" s="47" t="s">
         <v>86</v>
       </c>
-      <c r="O36" s="48"/>
-      <c r="P36" s="48"/>
-      <c r="Q36" s="48"/>
-      <c r="R36" s="48"/>
-      <c r="S36" s="48"/>
+      <c r="O36" s="47"/>
+      <c r="P36" s="47"/>
+      <c r="Q36" s="47"/>
+      <c r="R36" s="47"/>
+      <c r="S36" s="47"/>
     </row>
     <row r="37" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A37" s="59" t="s">
+      <c r="A37" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="B37" s="60"/>
-      <c r="C37" s="69"/>
-      <c r="D37" s="70"/>
-      <c r="E37" s="70"/>
-      <c r="F37" s="70"/>
-      <c r="G37" s="71"/>
-      <c r="H37" s="69"/>
-      <c r="I37" s="70"/>
-      <c r="J37" s="70"/>
-      <c r="K37" s="71"/>
+      <c r="B37" s="71"/>
+      <c r="C37" s="76"/>
+      <c r="D37" s="77"/>
+      <c r="E37" s="77"/>
+      <c r="F37" s="77"/>
+      <c r="G37" s="78"/>
+      <c r="H37" s="76"/>
+      <c r="I37" s="77"/>
+      <c r="J37" s="77"/>
+      <c r="K37" s="78"/>
       <c r="M37" s="34"/>
     </row>
     <row r="38" spans="1:19" ht="15.75" thickBot="1">
-      <c r="N38" s="48" t="s">
+      <c r="N38" s="47" t="s">
         <v>93</v>
       </c>
-      <c r="O38" s="48"/>
-      <c r="P38" s="48"/>
-      <c r="Q38" s="48"/>
-      <c r="R38" s="48"/>
-      <c r="S38" s="48"/>
+      <c r="O38" s="47"/>
+      <c r="P38" s="47"/>
+      <c r="Q38" s="47"/>
+      <c r="R38" s="47"/>
+      <c r="S38" s="47"/>
     </row>
     <row r="39" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A39" s="52" t="s">
+      <c r="A39" s="91" t="s">
         <v>27</v>
       </c>
-      <c r="B39" s="53"/>
-      <c r="C39" s="53"/>
-      <c r="D39" s="53"/>
-      <c r="E39" s="54"/>
+      <c r="B39" s="92"/>
+      <c r="C39" s="92"/>
+      <c r="D39" s="92"/>
+      <c r="E39" s="93"/>
     </row>
     <row r="40" spans="1:19">
       <c r="A40" s="14" t="s">
         <v>26</v>
       </c>
       <c r="B40" s="13"/>
-      <c r="C40" s="55" t="s">
+      <c r="C40" s="94" t="s">
         <v>23</v>
       </c>
-      <c r="D40" s="56"/>
+      <c r="D40" s="95"/>
       <c r="E40" s="28"/>
     </row>
     <row r="41" spans="1:19">
@@ -2428,10 +2427,10 @@
         <v>22</v>
       </c>
       <c r="B41" s="5"/>
-      <c r="C41" s="55" t="s">
+      <c r="C41" s="94" t="s">
         <v>24</v>
       </c>
-      <c r="D41" s="56"/>
+      <c r="D41" s="95"/>
       <c r="E41" s="8"/>
     </row>
     <row r="42" spans="1:19">
@@ -2439,154 +2438,154 @@
         <v>25</v>
       </c>
       <c r="B42" s="6"/>
-      <c r="C42" s="61" t="s">
+      <c r="C42" s="82" t="s">
         <v>67</v>
       </c>
-      <c r="D42" s="62"/>
-      <c r="E42" s="40"/>
+      <c r="D42" s="83"/>
+      <c r="E42" s="39"/>
     </row>
     <row r="43" spans="1:19" ht="15.75" thickBot="1"/>
     <row r="44" spans="1:19">
-      <c r="A44" s="57" t="s">
+      <c r="A44" s="96" t="s">
         <v>37</v>
       </c>
-      <c r="B44" s="58"/>
-      <c r="C44" s="58"/>
-      <c r="D44" s="58"/>
-      <c r="E44" s="58"/>
-      <c r="F44" s="58"/>
-      <c r="G44" s="58"/>
-      <c r="H44" s="58"/>
-      <c r="I44" s="58"/>
-      <c r="J44" s="58"/>
-      <c r="K44" s="58"/>
-      <c r="L44" s="58"/>
+      <c r="B44" s="97"/>
+      <c r="C44" s="97"/>
+      <c r="D44" s="97"/>
+      <c r="E44" s="97"/>
+      <c r="F44" s="97"/>
+      <c r="G44" s="97"/>
+      <c r="H44" s="97"/>
+      <c r="I44" s="97"/>
+      <c r="J44" s="97"/>
+      <c r="K44" s="97"/>
+      <c r="L44" s="97"/>
     </row>
     <row r="45" spans="1:19">
-      <c r="A45" s="36" t="s">
+      <c r="A45" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="B45" s="51" t="s">
+      <c r="B45" s="90" t="s">
         <v>57</v>
       </c>
-      <c r="C45" s="51"/>
-      <c r="D45" s="51"/>
-      <c r="E45" s="51"/>
-      <c r="F45" s="51"/>
-      <c r="G45" s="51"/>
-      <c r="H45" s="51"/>
-      <c r="I45" s="51"/>
-      <c r="J45" s="51"/>
-      <c r="K45" s="51"/>
-      <c r="L45" s="51"/>
+      <c r="C45" s="90"/>
+      <c r="D45" s="90"/>
+      <c r="E45" s="90"/>
+      <c r="F45" s="90"/>
+      <c r="G45" s="90"/>
+      <c r="H45" s="90"/>
+      <c r="I45" s="90"/>
+      <c r="J45" s="90"/>
+      <c r="K45" s="90"/>
+      <c r="L45" s="90"/>
     </row>
     <row r="46" spans="1:19" ht="15" customHeight="1">
-      <c r="A46" s="36" t="s">
+      <c r="A46" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="B46" s="51" t="s">
+      <c r="B46" s="90" t="s">
         <v>58</v>
       </c>
-      <c r="C46" s="51"/>
-      <c r="D46" s="51"/>
-      <c r="E46" s="51"/>
-      <c r="F46" s="51"/>
-      <c r="G46" s="51"/>
-      <c r="H46" s="51"/>
-      <c r="I46" s="51"/>
-      <c r="J46" s="51"/>
-      <c r="K46" s="51"/>
-      <c r="L46" s="51"/>
+      <c r="C46" s="90"/>
+      <c r="D46" s="90"/>
+      <c r="E46" s="90"/>
+      <c r="F46" s="90"/>
+      <c r="G46" s="90"/>
+      <c r="H46" s="90"/>
+      <c r="I46" s="90"/>
+      <c r="J46" s="90"/>
+      <c r="K46" s="90"/>
+      <c r="L46" s="90"/>
     </row>
     <row r="47" spans="1:19">
-      <c r="A47" s="36" t="s">
+      <c r="A47" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="B47" s="51" t="s">
+      <c r="B47" s="90" t="s">
         <v>59</v>
       </c>
-      <c r="C47" s="51"/>
-      <c r="D47" s="51"/>
-      <c r="E47" s="51"/>
-      <c r="F47" s="51"/>
-      <c r="G47" s="51"/>
-      <c r="H47" s="51"/>
-      <c r="I47" s="51"/>
-      <c r="J47" s="51"/>
-      <c r="K47" s="51"/>
-      <c r="L47" s="51"/>
+      <c r="C47" s="90"/>
+      <c r="D47" s="90"/>
+      <c r="E47" s="90"/>
+      <c r="F47" s="90"/>
+      <c r="G47" s="90"/>
+      <c r="H47" s="90"/>
+      <c r="I47" s="90"/>
+      <c r="J47" s="90"/>
+      <c r="K47" s="90"/>
+      <c r="L47" s="90"/>
     </row>
     <row r="48" spans="1:19">
-      <c r="A48" s="36" t="s">
+      <c r="A48" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="B48" s="51" t="s">
+      <c r="B48" s="90" t="s">
         <v>46</v>
       </c>
-      <c r="C48" s="51"/>
-      <c r="D48" s="51"/>
-      <c r="E48" s="51"/>
-      <c r="F48" s="51"/>
-      <c r="G48" s="51"/>
-      <c r="H48" s="51"/>
-      <c r="I48" s="51"/>
-      <c r="J48" s="51"/>
-      <c r="K48" s="51"/>
-      <c r="L48" s="51"/>
+      <c r="C48" s="90"/>
+      <c r="D48" s="90"/>
+      <c r="E48" s="90"/>
+      <c r="F48" s="90"/>
+      <c r="G48" s="90"/>
+      <c r="H48" s="90"/>
+      <c r="I48" s="90"/>
+      <c r="J48" s="90"/>
+      <c r="K48" s="90"/>
+      <c r="L48" s="90"/>
     </row>
     <row r="49" spans="1:12">
-      <c r="A49" s="36" t="s">
+      <c r="A49" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="B49" s="51" t="s">
+      <c r="B49" s="90" t="s">
         <v>35</v>
       </c>
-      <c r="C49" s="51"/>
-      <c r="D49" s="51"/>
-      <c r="E49" s="51"/>
-      <c r="F49" s="51"/>
-      <c r="G49" s="51"/>
-      <c r="H49" s="51"/>
-      <c r="I49" s="51"/>
-      <c r="J49" s="51"/>
-      <c r="K49" s="51"/>
-      <c r="L49" s="51"/>
+      <c r="C49" s="90"/>
+      <c r="D49" s="90"/>
+      <c r="E49" s="90"/>
+      <c r="F49" s="90"/>
+      <c r="G49" s="90"/>
+      <c r="H49" s="90"/>
+      <c r="I49" s="90"/>
+      <c r="J49" s="90"/>
+      <c r="K49" s="90"/>
+      <c r="L49" s="90"/>
     </row>
     <row r="50" spans="1:12">
-      <c r="A50" s="36" t="s">
+      <c r="A50" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="B50" s="51" t="s">
+      <c r="B50" s="90" t="s">
         <v>56</v>
       </c>
-      <c r="C50" s="51"/>
-      <c r="D50" s="51"/>
-      <c r="E50" s="51"/>
-      <c r="F50" s="51"/>
-      <c r="G50" s="51"/>
-      <c r="H50" s="51"/>
-      <c r="I50" s="51"/>
-      <c r="J50" s="51"/>
-      <c r="K50" s="51"/>
-      <c r="L50" s="51"/>
+      <c r="C50" s="90"/>
+      <c r="D50" s="90"/>
+      <c r="E50" s="90"/>
+      <c r="F50" s="90"/>
+      <c r="G50" s="90"/>
+      <c r="H50" s="90"/>
+      <c r="I50" s="90"/>
+      <c r="J50" s="90"/>
+      <c r="K50" s="90"/>
+      <c r="L50" s="90"/>
     </row>
     <row r="51" spans="1:12">
-      <c r="A51" s="36" t="s">
+      <c r="A51" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="B51" s="51" t="s">
+      <c r="B51" s="90" t="s">
         <v>55</v>
       </c>
-      <c r="C51" s="51"/>
-      <c r="D51" s="51"/>
-      <c r="E51" s="51"/>
-      <c r="F51" s="51"/>
-      <c r="G51" s="51"/>
-      <c r="H51" s="51"/>
-      <c r="I51" s="51"/>
-      <c r="J51" s="51"/>
-      <c r="K51" s="51"/>
-      <c r="L51" s="51"/>
+      <c r="C51" s="90"/>
+      <c r="D51" s="90"/>
+      <c r="E51" s="90"/>
+      <c r="F51" s="90"/>
+      <c r="G51" s="90"/>
+      <c r="H51" s="90"/>
+      <c r="I51" s="90"/>
+      <c r="J51" s="90"/>
+      <c r="K51" s="90"/>
+      <c r="L51" s="90"/>
     </row>
     <row r="52" spans="1:12">
       <c r="C52" s="34"/>
@@ -2602,6 +2601,44 @@
     <sortCondition ref="A3"/>
   </sortState>
   <mergeCells count="54">
+    <mergeCell ref="N27:S27"/>
+    <mergeCell ref="N33:S33"/>
+    <mergeCell ref="N35:S35"/>
+    <mergeCell ref="N30:S30"/>
+    <mergeCell ref="N28:S28"/>
+    <mergeCell ref="N31:S31"/>
+    <mergeCell ref="B50:L50"/>
+    <mergeCell ref="B51:L51"/>
+    <mergeCell ref="A39:E39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="B45:L45"/>
+    <mergeCell ref="A44:L44"/>
+    <mergeCell ref="B46:L46"/>
+    <mergeCell ref="B47:L47"/>
+    <mergeCell ref="B48:L48"/>
+    <mergeCell ref="B49:L49"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="H33:K33"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="H35:K35"/>
+    <mergeCell ref="H36:K36"/>
+    <mergeCell ref="H37:K37"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="H30:K30"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="H32:K32"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="H31:L31"/>
     <mergeCell ref="N38:S38"/>
     <mergeCell ref="N36:S36"/>
     <mergeCell ref="O6:U6"/>
@@ -2618,44 +2655,6 @@
     <mergeCell ref="C3:G3"/>
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="C30:G30"/>
-    <mergeCell ref="H30:K30"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="H32:K32"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="H31:L31"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="H33:K33"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="H35:K35"/>
-    <mergeCell ref="H36:K36"/>
-    <mergeCell ref="H37:K37"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="B50:L50"/>
-    <mergeCell ref="B51:L51"/>
-    <mergeCell ref="A39:E39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="B45:L45"/>
-    <mergeCell ref="A44:L44"/>
-    <mergeCell ref="B46:L46"/>
-    <mergeCell ref="B47:L47"/>
-    <mergeCell ref="B48:L48"/>
-    <mergeCell ref="B49:L49"/>
-    <mergeCell ref="N27:S27"/>
-    <mergeCell ref="N33:S33"/>
-    <mergeCell ref="N35:S35"/>
-    <mergeCell ref="N30:S30"/>
-    <mergeCell ref="N28:S28"/>
-    <mergeCell ref="N31:S31"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="Q4" r:id="rId1"/>

</xml_diff>

<commit_message>
actualizado cuadro de estado
</commit_message>
<xml_diff>
--- a/Cuadro-de-estado.xlsx
+++ b/Cuadro-de-estado.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="95">
   <si>
     <t>BACKEND</t>
   </si>
@@ -382,6 +382,9 @@
   </si>
   <si>
     <t>Si está en mostrar form, no habilitar modificar datos grales</t>
+  </si>
+  <si>
+    <t>showBtnAction debe ser un servicio dentro de ui.service</t>
   </si>
 </sst>
 </file>
@@ -1151,6 +1154,108 @@
     <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1204,108 +1309,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1608,7 +1611,7 @@
   <dimension ref="A1:U54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1625,20 +1628,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="84" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50"/>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="84"/>
+      <c r="K1" s="84"/>
+      <c r="L1" s="84"/>
     </row>
     <row r="2" spans="1:21" ht="18" thickBot="1">
       <c r="O2" s="46" t="s">
@@ -1646,30 +1649,30 @@
       </c>
     </row>
     <row r="3" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="85" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="52"/>
-      <c r="C3" s="53" t="s">
+      <c r="B3" s="86"/>
+      <c r="C3" s="87" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="54"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="55"/>
-      <c r="H3" s="53" t="s">
+      <c r="D3" s="88"/>
+      <c r="E3" s="88"/>
+      <c r="F3" s="88"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="54"/>
-      <c r="J3" s="56"/>
-      <c r="K3" s="55"/>
+      <c r="I3" s="88"/>
+      <c r="J3" s="90"/>
+      <c r="K3" s="89"/>
       <c r="L3" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="58" t="s">
+      <c r="M3" s="92" t="s">
         <v>84</v>
       </c>
-      <c r="N3" s="49"/>
+      <c r="N3" s="83"/>
     </row>
     <row r="4" spans="1:21" s="3" customFormat="1" ht="40.5" customHeight="1" thickBot="1">
       <c r="A4" s="17" t="s">
@@ -1708,10 +1711,10 @@
       <c r="L4" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="M4" s="59" t="s">
+      <c r="M4" s="93" t="s">
         <v>85</v>
       </c>
-      <c r="N4" s="60"/>
+      <c r="N4" s="94"/>
       <c r="O4" s="36" t="s">
         <v>64</v>
       </c>
@@ -1755,15 +1758,15 @@
       <c r="M6" s="45" t="s">
         <v>87</v>
       </c>
-      <c r="O6" s="48" t="s">
+      <c r="O6" s="82" t="s">
         <v>68</v>
       </c>
-      <c r="P6" s="49"/>
-      <c r="Q6" s="49"/>
-      <c r="R6" s="49"/>
-      <c r="S6" s="49"/>
-      <c r="T6" s="49"/>
-      <c r="U6" s="49"/>
+      <c r="P6" s="83"/>
+      <c r="Q6" s="83"/>
+      <c r="R6" s="83"/>
+      <c r="S6" s="83"/>
+      <c r="T6" s="83"/>
+      <c r="U6" s="83"/>
     </row>
     <row r="7" spans="1:21" ht="4.5" customHeight="1">
       <c r="A7" s="29"/>
@@ -1924,14 +1927,14 @@
       <c r="J14" s="4"/>
       <c r="K14" s="7"/>
       <c r="L14" s="4"/>
-      <c r="O14" s="57" t="s">
+      <c r="O14" s="91" t="s">
         <v>82</v>
       </c>
-      <c r="P14" s="57"/>
-      <c r="Q14" s="57"/>
-      <c r="R14" s="57"/>
-      <c r="S14" s="57"/>
-      <c r="T14" s="57"/>
+      <c r="P14" s="91"/>
+      <c r="Q14" s="91"/>
+      <c r="R14" s="91"/>
+      <c r="S14" s="91"/>
+      <c r="T14" s="91"/>
     </row>
     <row r="15" spans="1:21">
       <c r="A15" s="18" t="s">
@@ -1950,12 +1953,12 @@
       <c r="J15" s="4"/>
       <c r="K15" s="7"/>
       <c r="L15" s="4"/>
-      <c r="O15" s="57"/>
-      <c r="P15" s="57"/>
-      <c r="Q15" s="57"/>
-      <c r="R15" s="57"/>
-      <c r="S15" s="57"/>
-      <c r="T15" s="57"/>
+      <c r="O15" s="91"/>
+      <c r="P15" s="91"/>
+      <c r="Q15" s="91"/>
+      <c r="R15" s="91"/>
+      <c r="S15" s="91"/>
+      <c r="T15" s="91"/>
     </row>
     <row r="16" spans="1:21">
       <c r="A16" s="40" t="s">
@@ -2120,6 +2123,14 @@
       <c r="J24" s="4"/>
       <c r="K24" s="7"/>
       <c r="L24" s="4"/>
+      <c r="N24" s="47" t="s">
+        <v>94</v>
+      </c>
+      <c r="O24" s="47"/>
+      <c r="P24" s="47"/>
+      <c r="Q24" s="47"/>
+      <c r="R24" s="47"/>
+      <c r="S24" s="47"/>
     </row>
     <row r="25" spans="1:19">
       <c r="A25" s="41" t="s">
@@ -2156,19 +2167,19 @@
     <row r="27" spans="1:19" ht="15.75" thickBot="1">
       <c r="A27" s="24"/>
       <c r="B27" s="26"/>
-      <c r="C27" s="53" t="s">
+      <c r="C27" s="87" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="54"/>
-      <c r="E27" s="54"/>
-      <c r="F27" s="54"/>
-      <c r="G27" s="55"/>
-      <c r="H27" s="53" t="s">
+      <c r="D27" s="88"/>
+      <c r="E27" s="88"/>
+      <c r="F27" s="88"/>
+      <c r="G27" s="89"/>
+      <c r="H27" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="I27" s="54"/>
-      <c r="J27" s="56"/>
-      <c r="K27" s="55"/>
+      <c r="I27" s="88"/>
+      <c r="J27" s="90"/>
+      <c r="K27" s="89"/>
       <c r="L27" s="21" t="s">
         <v>4</v>
       </c>
@@ -2182,28 +2193,28 @@
       <c r="S27" s="47"/>
     </row>
     <row r="28" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A28" s="64" t="s">
+      <c r="A28" s="98" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="65"/>
-      <c r="C28" s="61"/>
-      <c r="D28" s="62"/>
-      <c r="E28" s="62"/>
-      <c r="F28" s="62"/>
-      <c r="G28" s="63"/>
-      <c r="H28" s="61"/>
-      <c r="I28" s="62"/>
-      <c r="J28" s="62"/>
-      <c r="K28" s="63"/>
+      <c r="B28" s="99"/>
+      <c r="C28" s="95"/>
+      <c r="D28" s="96"/>
+      <c r="E28" s="96"/>
+      <c r="F28" s="96"/>
+      <c r="G28" s="97"/>
+      <c r="H28" s="95"/>
+      <c r="I28" s="96"/>
+      <c r="J28" s="96"/>
+      <c r="K28" s="97"/>
       <c r="L28" s="4"/>
-      <c r="N28" s="99" t="s">
+      <c r="N28" s="49" t="s">
         <v>91</v>
       </c>
-      <c r="O28" s="99"/>
-      <c r="P28" s="99"/>
-      <c r="Q28" s="99"/>
-      <c r="R28" s="99"/>
-      <c r="S28" s="99"/>
+      <c r="O28" s="49"/>
+      <c r="P28" s="49"/>
+      <c r="Q28" s="49"/>
+      <c r="R28" s="49"/>
+      <c r="S28" s="49"/>
     </row>
     <row r="29" spans="1:19" ht="4.5" customHeight="1">
       <c r="A29" s="29"/>
@@ -2220,42 +2231,42 @@
       <c r="L29" s="31"/>
     </row>
     <row r="30" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A30" s="70" t="s">
+      <c r="A30" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="B30" s="71"/>
-      <c r="C30" s="66"/>
-      <c r="D30" s="67"/>
-      <c r="E30" s="67"/>
-      <c r="F30" s="67"/>
-      <c r="G30" s="68"/>
-      <c r="H30" s="69"/>
-      <c r="I30" s="67"/>
-      <c r="J30" s="67"/>
-      <c r="K30" s="68"/>
+      <c r="B30" s="59"/>
+      <c r="C30" s="78"/>
+      <c r="D30" s="72"/>
+      <c r="E30" s="72"/>
+      <c r="F30" s="72"/>
+      <c r="G30" s="73"/>
+      <c r="H30" s="71"/>
+      <c r="I30" s="72"/>
+      <c r="J30" s="72"/>
+      <c r="K30" s="73"/>
       <c r="L30" s="22" t="s">
         <v>5</v>
       </c>
       <c r="M30" s="34"/>
-      <c r="N30" s="99" t="s">
+      <c r="N30" s="49" t="s">
         <v>83</v>
       </c>
-      <c r="O30" s="99"/>
-      <c r="P30" s="99"/>
-      <c r="Q30" s="99"/>
-      <c r="R30" s="99"/>
-      <c r="S30" s="99"/>
+      <c r="O30" s="49"/>
+      <c r="P30" s="49"/>
+      <c r="Q30" s="49"/>
+      <c r="R30" s="49"/>
+      <c r="S30" s="49"/>
     </row>
     <row r="31" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A31" s="70" t="s">
+      <c r="A31" s="58" t="s">
         <v>88</v>
       </c>
-      <c r="B31" s="71"/>
-      <c r="C31" s="76"/>
-      <c r="D31" s="77"/>
-      <c r="E31" s="77"/>
-      <c r="F31" s="77"/>
-      <c r="G31" s="78"/>
+      <c r="B31" s="59"/>
+      <c r="C31" s="68"/>
+      <c r="D31" s="69"/>
+      <c r="E31" s="69"/>
+      <c r="F31" s="69"/>
+      <c r="G31" s="70"/>
       <c r="H31" s="79" t="s">
         <v>89</v>
       </c>
@@ -2264,56 +2275,56 @@
       <c r="K31" s="80"/>
       <c r="L31" s="81"/>
       <c r="M31" s="34"/>
-      <c r="N31" s="99" t="s">
+      <c r="N31" s="49" t="s">
         <v>78</v>
       </c>
-      <c r="O31" s="99"/>
-      <c r="P31" s="99"/>
-      <c r="Q31" s="99"/>
-      <c r="R31" s="99"/>
-      <c r="S31" s="99"/>
+      <c r="O31" s="49"/>
+      <c r="P31" s="49"/>
+      <c r="Q31" s="49"/>
+      <c r="R31" s="49"/>
+      <c r="S31" s="49"/>
     </row>
     <row r="32" spans="1:19" ht="16.5" thickBot="1">
-      <c r="A32" s="74" t="s">
+      <c r="A32" s="76" t="s">
         <v>62</v>
       </c>
-      <c r="B32" s="75"/>
-      <c r="C32" s="66"/>
-      <c r="D32" s="67"/>
-      <c r="E32" s="67"/>
-      <c r="F32" s="67"/>
-      <c r="G32" s="68"/>
-      <c r="H32" s="69"/>
-      <c r="I32" s="67"/>
-      <c r="J32" s="67"/>
-      <c r="K32" s="68"/>
+      <c r="B32" s="77"/>
+      <c r="C32" s="78"/>
+      <c r="D32" s="72"/>
+      <c r="E32" s="72"/>
+      <c r="F32" s="72"/>
+      <c r="G32" s="73"/>
+      <c r="H32" s="71"/>
+      <c r="I32" s="72"/>
+      <c r="J32" s="72"/>
+      <c r="K32" s="73"/>
       <c r="M32" s="34"/>
     </row>
     <row r="33" spans="1:19" ht="30.75" customHeight="1" thickBot="1">
-      <c r="A33" s="72" t="s">
+      <c r="A33" s="74" t="s">
         <v>36</v>
       </c>
-      <c r="B33" s="73"/>
-      <c r="C33" s="87" t="s">
+      <c r="B33" s="75"/>
+      <c r="C33" s="65" t="s">
         <v>61</v>
       </c>
-      <c r="D33" s="88"/>
-      <c r="E33" s="88"/>
-      <c r="F33" s="88"/>
-      <c r="G33" s="89"/>
-      <c r="H33" s="84"/>
-      <c r="I33" s="85"/>
-      <c r="J33" s="85"/>
-      <c r="K33" s="86"/>
+      <c r="D33" s="66"/>
+      <c r="E33" s="66"/>
+      <c r="F33" s="66"/>
+      <c r="G33" s="67"/>
+      <c r="H33" s="62"/>
+      <c r="I33" s="63"/>
+      <c r="J33" s="63"/>
+      <c r="K33" s="64"/>
       <c r="M33" s="34"/>
-      <c r="N33" s="98" t="s">
+      <c r="N33" s="48" t="s">
         <v>79</v>
       </c>
-      <c r="O33" s="98"/>
-      <c r="P33" s="98"/>
-      <c r="Q33" s="98"/>
-      <c r="R33" s="98"/>
-      <c r="S33" s="98"/>
+      <c r="O33" s="48"/>
+      <c r="P33" s="48"/>
+      <c r="Q33" s="48"/>
+      <c r="R33" s="48"/>
+      <c r="S33" s="48"/>
     </row>
     <row r="34" spans="1:19" ht="4.5" customHeight="1" thickBot="1">
       <c r="A34" s="29"/>
@@ -2329,43 +2340,43 @@
       <c r="K34" s="31"/>
     </row>
     <row r="35" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A35" s="70" t="s">
+      <c r="A35" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="B35" s="71"/>
-      <c r="C35" s="76"/>
-      <c r="D35" s="77"/>
-      <c r="E35" s="77"/>
-      <c r="F35" s="77"/>
-      <c r="G35" s="78"/>
-      <c r="H35" s="76"/>
-      <c r="I35" s="77"/>
-      <c r="J35" s="77"/>
-      <c r="K35" s="78"/>
+      <c r="B35" s="59"/>
+      <c r="C35" s="68"/>
+      <c r="D35" s="69"/>
+      <c r="E35" s="69"/>
+      <c r="F35" s="69"/>
+      <c r="G35" s="70"/>
+      <c r="H35" s="68"/>
+      <c r="I35" s="69"/>
+      <c r="J35" s="69"/>
+      <c r="K35" s="70"/>
       <c r="M35" s="34"/>
-      <c r="N35" s="99" t="s">
+      <c r="N35" s="49" t="s">
         <v>81</v>
       </c>
-      <c r="O35" s="99"/>
-      <c r="P35" s="99"/>
-      <c r="Q35" s="99"/>
-      <c r="R35" s="99"/>
-      <c r="S35" s="99"/>
+      <c r="O35" s="49"/>
+      <c r="P35" s="49"/>
+      <c r="Q35" s="49"/>
+      <c r="R35" s="49"/>
+      <c r="S35" s="49"/>
     </row>
     <row r="36" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A36" s="70" t="s">
+      <c r="A36" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="B36" s="71"/>
-      <c r="C36" s="76"/>
-      <c r="D36" s="77"/>
-      <c r="E36" s="77"/>
-      <c r="F36" s="77"/>
-      <c r="G36" s="78"/>
-      <c r="H36" s="76"/>
-      <c r="I36" s="77"/>
-      <c r="J36" s="77"/>
-      <c r="K36" s="78"/>
+      <c r="B36" s="59"/>
+      <c r="C36" s="68"/>
+      <c r="D36" s="69"/>
+      <c r="E36" s="69"/>
+      <c r="F36" s="69"/>
+      <c r="G36" s="70"/>
+      <c r="H36" s="68"/>
+      <c r="I36" s="69"/>
+      <c r="J36" s="69"/>
+      <c r="K36" s="70"/>
       <c r="M36" s="34"/>
       <c r="N36" s="47" t="s">
         <v>86</v>
@@ -2377,19 +2388,19 @@
       <c r="S36" s="47"/>
     </row>
     <row r="37" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A37" s="70" t="s">
+      <c r="A37" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="B37" s="71"/>
-      <c r="C37" s="76"/>
-      <c r="D37" s="77"/>
-      <c r="E37" s="77"/>
-      <c r="F37" s="77"/>
-      <c r="G37" s="78"/>
-      <c r="H37" s="76"/>
-      <c r="I37" s="77"/>
-      <c r="J37" s="77"/>
-      <c r="K37" s="78"/>
+      <c r="B37" s="59"/>
+      <c r="C37" s="68"/>
+      <c r="D37" s="69"/>
+      <c r="E37" s="69"/>
+      <c r="F37" s="69"/>
+      <c r="G37" s="70"/>
+      <c r="H37" s="68"/>
+      <c r="I37" s="69"/>
+      <c r="J37" s="69"/>
+      <c r="K37" s="70"/>
       <c r="M37" s="34"/>
     </row>
     <row r="38" spans="1:19" ht="15.75" thickBot="1">
@@ -2403,23 +2414,23 @@
       <c r="S38" s="47"/>
     </row>
     <row r="39" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A39" s="91" t="s">
+      <c r="A39" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="B39" s="92"/>
-      <c r="C39" s="92"/>
-      <c r="D39" s="92"/>
-      <c r="E39" s="93"/>
+      <c r="B39" s="52"/>
+      <c r="C39" s="52"/>
+      <c r="D39" s="52"/>
+      <c r="E39" s="53"/>
     </row>
     <row r="40" spans="1:19">
       <c r="A40" s="14" t="s">
         <v>26</v>
       </c>
       <c r="B40" s="13"/>
-      <c r="C40" s="94" t="s">
+      <c r="C40" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="D40" s="95"/>
+      <c r="D40" s="55"/>
       <c r="E40" s="28"/>
     </row>
     <row r="41" spans="1:19">
@@ -2427,10 +2438,10 @@
         <v>22</v>
       </c>
       <c r="B41" s="5"/>
-      <c r="C41" s="94" t="s">
+      <c r="C41" s="54" t="s">
         <v>24</v>
       </c>
-      <c r="D41" s="95"/>
+      <c r="D41" s="55"/>
       <c r="E41" s="8"/>
     </row>
     <row r="42" spans="1:19">
@@ -2438,154 +2449,154 @@
         <v>25</v>
       </c>
       <c r="B42" s="6"/>
-      <c r="C42" s="82" t="s">
+      <c r="C42" s="60" t="s">
         <v>67</v>
       </c>
-      <c r="D42" s="83"/>
+      <c r="D42" s="61"/>
       <c r="E42" s="39"/>
     </row>
     <row r="43" spans="1:19" ht="15.75" thickBot="1"/>
     <row r="44" spans="1:19">
-      <c r="A44" s="96" t="s">
+      <c r="A44" s="56" t="s">
         <v>37</v>
       </c>
-      <c r="B44" s="97"/>
-      <c r="C44" s="97"/>
-      <c r="D44" s="97"/>
-      <c r="E44" s="97"/>
-      <c r="F44" s="97"/>
-      <c r="G44" s="97"/>
-      <c r="H44" s="97"/>
-      <c r="I44" s="97"/>
-      <c r="J44" s="97"/>
-      <c r="K44" s="97"/>
-      <c r="L44" s="97"/>
+      <c r="B44" s="57"/>
+      <c r="C44" s="57"/>
+      <c r="D44" s="57"/>
+      <c r="E44" s="57"/>
+      <c r="F44" s="57"/>
+      <c r="G44" s="57"/>
+      <c r="H44" s="57"/>
+      <c r="I44" s="57"/>
+      <c r="J44" s="57"/>
+      <c r="K44" s="57"/>
+      <c r="L44" s="57"/>
     </row>
     <row r="45" spans="1:19">
       <c r="A45" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="B45" s="90" t="s">
+      <c r="B45" s="50" t="s">
         <v>57</v>
       </c>
-      <c r="C45" s="90"/>
-      <c r="D45" s="90"/>
-      <c r="E45" s="90"/>
-      <c r="F45" s="90"/>
-      <c r="G45" s="90"/>
-      <c r="H45" s="90"/>
-      <c r="I45" s="90"/>
-      <c r="J45" s="90"/>
-      <c r="K45" s="90"/>
-      <c r="L45" s="90"/>
+      <c r="C45" s="50"/>
+      <c r="D45" s="50"/>
+      <c r="E45" s="50"/>
+      <c r="F45" s="50"/>
+      <c r="G45" s="50"/>
+      <c r="H45" s="50"/>
+      <c r="I45" s="50"/>
+      <c r="J45" s="50"/>
+      <c r="K45" s="50"/>
+      <c r="L45" s="50"/>
     </row>
     <row r="46" spans="1:19" ht="15" customHeight="1">
       <c r="A46" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="B46" s="90" t="s">
+      <c r="B46" s="50" t="s">
         <v>58</v>
       </c>
-      <c r="C46" s="90"/>
-      <c r="D46" s="90"/>
-      <c r="E46" s="90"/>
-      <c r="F46" s="90"/>
-      <c r="G46" s="90"/>
-      <c r="H46" s="90"/>
-      <c r="I46" s="90"/>
-      <c r="J46" s="90"/>
-      <c r="K46" s="90"/>
-      <c r="L46" s="90"/>
+      <c r="C46" s="50"/>
+      <c r="D46" s="50"/>
+      <c r="E46" s="50"/>
+      <c r="F46" s="50"/>
+      <c r="G46" s="50"/>
+      <c r="H46" s="50"/>
+      <c r="I46" s="50"/>
+      <c r="J46" s="50"/>
+      <c r="K46" s="50"/>
+      <c r="L46" s="50"/>
     </row>
     <row r="47" spans="1:19">
       <c r="A47" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="B47" s="90" t="s">
+      <c r="B47" s="50" t="s">
         <v>59</v>
       </c>
-      <c r="C47" s="90"/>
-      <c r="D47" s="90"/>
-      <c r="E47" s="90"/>
-      <c r="F47" s="90"/>
-      <c r="G47" s="90"/>
-      <c r="H47" s="90"/>
-      <c r="I47" s="90"/>
-      <c r="J47" s="90"/>
-      <c r="K47" s="90"/>
-      <c r="L47" s="90"/>
+      <c r="C47" s="50"/>
+      <c r="D47" s="50"/>
+      <c r="E47" s="50"/>
+      <c r="F47" s="50"/>
+      <c r="G47" s="50"/>
+      <c r="H47" s="50"/>
+      <c r="I47" s="50"/>
+      <c r="J47" s="50"/>
+      <c r="K47" s="50"/>
+      <c r="L47" s="50"/>
     </row>
     <row r="48" spans="1:19">
       <c r="A48" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="B48" s="90" t="s">
+      <c r="B48" s="50" t="s">
         <v>46</v>
       </c>
-      <c r="C48" s="90"/>
-      <c r="D48" s="90"/>
-      <c r="E48" s="90"/>
-      <c r="F48" s="90"/>
-      <c r="G48" s="90"/>
-      <c r="H48" s="90"/>
-      <c r="I48" s="90"/>
-      <c r="J48" s="90"/>
-      <c r="K48" s="90"/>
-      <c r="L48" s="90"/>
+      <c r="C48" s="50"/>
+      <c r="D48" s="50"/>
+      <c r="E48" s="50"/>
+      <c r="F48" s="50"/>
+      <c r="G48" s="50"/>
+      <c r="H48" s="50"/>
+      <c r="I48" s="50"/>
+      <c r="J48" s="50"/>
+      <c r="K48" s="50"/>
+      <c r="L48" s="50"/>
     </row>
     <row r="49" spans="1:12">
       <c r="A49" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="B49" s="90" t="s">
+      <c r="B49" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="C49" s="90"/>
-      <c r="D49" s="90"/>
-      <c r="E49" s="90"/>
-      <c r="F49" s="90"/>
-      <c r="G49" s="90"/>
-      <c r="H49" s="90"/>
-      <c r="I49" s="90"/>
-      <c r="J49" s="90"/>
-      <c r="K49" s="90"/>
-      <c r="L49" s="90"/>
+      <c r="C49" s="50"/>
+      <c r="D49" s="50"/>
+      <c r="E49" s="50"/>
+      <c r="F49" s="50"/>
+      <c r="G49" s="50"/>
+      <c r="H49" s="50"/>
+      <c r="I49" s="50"/>
+      <c r="J49" s="50"/>
+      <c r="K49" s="50"/>
+      <c r="L49" s="50"/>
     </row>
     <row r="50" spans="1:12">
       <c r="A50" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="B50" s="90" t="s">
+      <c r="B50" s="50" t="s">
         <v>56</v>
       </c>
-      <c r="C50" s="90"/>
-      <c r="D50" s="90"/>
-      <c r="E50" s="90"/>
-      <c r="F50" s="90"/>
-      <c r="G50" s="90"/>
-      <c r="H50" s="90"/>
-      <c r="I50" s="90"/>
-      <c r="J50" s="90"/>
-      <c r="K50" s="90"/>
-      <c r="L50" s="90"/>
+      <c r="C50" s="50"/>
+      <c r="D50" s="50"/>
+      <c r="E50" s="50"/>
+      <c r="F50" s="50"/>
+      <c r="G50" s="50"/>
+      <c r="H50" s="50"/>
+      <c r="I50" s="50"/>
+      <c r="J50" s="50"/>
+      <c r="K50" s="50"/>
+      <c r="L50" s="50"/>
     </row>
     <row r="51" spans="1:12">
       <c r="A51" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="B51" s="90" t="s">
+      <c r="B51" s="50" t="s">
         <v>55</v>
       </c>
-      <c r="C51" s="90"/>
-      <c r="D51" s="90"/>
-      <c r="E51" s="90"/>
-      <c r="F51" s="90"/>
-      <c r="G51" s="90"/>
-      <c r="H51" s="90"/>
-      <c r="I51" s="90"/>
-      <c r="J51" s="90"/>
-      <c r="K51" s="90"/>
-      <c r="L51" s="90"/>
+      <c r="C51" s="50"/>
+      <c r="D51" s="50"/>
+      <c r="E51" s="50"/>
+      <c r="F51" s="50"/>
+      <c r="G51" s="50"/>
+      <c r="H51" s="50"/>
+      <c r="I51" s="50"/>
+      <c r="J51" s="50"/>
+      <c r="K51" s="50"/>
+      <c r="L51" s="50"/>
     </row>
     <row r="52" spans="1:12">
       <c r="C52" s="34"/>
@@ -2600,45 +2611,8 @@
   <sortState ref="A24:K25">
     <sortCondition ref="A3"/>
   </sortState>
-  <mergeCells count="54">
-    <mergeCell ref="N27:S27"/>
-    <mergeCell ref="N33:S33"/>
-    <mergeCell ref="N35:S35"/>
-    <mergeCell ref="N30:S30"/>
-    <mergeCell ref="N28:S28"/>
-    <mergeCell ref="N31:S31"/>
-    <mergeCell ref="B50:L50"/>
-    <mergeCell ref="B51:L51"/>
-    <mergeCell ref="A39:E39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="B45:L45"/>
-    <mergeCell ref="A44:L44"/>
-    <mergeCell ref="B46:L46"/>
-    <mergeCell ref="B47:L47"/>
-    <mergeCell ref="B48:L48"/>
-    <mergeCell ref="B49:L49"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="H33:K33"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="H35:K35"/>
-    <mergeCell ref="H36:K36"/>
-    <mergeCell ref="H37:K37"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="H30:K30"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="H32:K32"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="H31:L31"/>
+  <mergeCells count="55">
+    <mergeCell ref="N24:S24"/>
     <mergeCell ref="N38:S38"/>
     <mergeCell ref="N36:S36"/>
     <mergeCell ref="O6:U6"/>
@@ -2655,6 +2629,44 @@
     <mergeCell ref="C3:G3"/>
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="C30:G30"/>
+    <mergeCell ref="H30:K30"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="H32:K32"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="H31:L31"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="H33:K33"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="H35:K35"/>
+    <mergeCell ref="H36:K36"/>
+    <mergeCell ref="H37:K37"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="B50:L50"/>
+    <mergeCell ref="B51:L51"/>
+    <mergeCell ref="A39:E39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="B45:L45"/>
+    <mergeCell ref="A44:L44"/>
+    <mergeCell ref="B46:L46"/>
+    <mergeCell ref="B47:L47"/>
+    <mergeCell ref="B48:L48"/>
+    <mergeCell ref="B49:L49"/>
+    <mergeCell ref="N27:S27"/>
+    <mergeCell ref="N33:S33"/>
+    <mergeCell ref="N35:S35"/>
+    <mergeCell ref="N30:S30"/>
+    <mergeCell ref="N28:S28"/>
+    <mergeCell ref="N31:S31"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="Q4" r:id="rId1"/>

</xml_diff>

<commit_message>
Backend, limpiado el cache, complilado y empaquetado con maven desde el prompt. FrontEnd creado componente para emitir alertas en ventana modal
</commit_message>
<xml_diff>
--- a/Cuadro-de-estado.xlsx
+++ b/Cuadro-de-estado.xlsx
@@ -282,9 +282,6 @@
     <t>Funcionando en localHost, se obtienen los JSON y se actualiza en la Base de Datos</t>
   </si>
   <si>
-    <t>ESTADO DEL PROYECTO Y ORDEN PARA AVANZAR</t>
-  </si>
-  <si>
     <t>Reutilizar componentes (p.e atributos de person, skills, etc.) Modules, componentes para pruebas</t>
   </si>
   <si>
@@ -385,6 +382,9 @@
   </si>
   <si>
     <t>showBtnAction debe ser un servicio dentro de ui.service</t>
+  </si>
+  <si>
+    <t>ESTADO DEL PROYECTO Y PRIORIDADES</t>
   </si>
 </sst>
 </file>
@@ -1154,161 +1154,161 @@
     <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1611,7 +1611,7 @@
   <dimension ref="A1:U54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1628,51 +1628,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25">
-      <c r="A1" s="84" t="s">
-        <v>60</v>
-      </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
-      <c r="F1" s="84"/>
-      <c r="G1" s="84"/>
-      <c r="H1" s="84"/>
-      <c r="I1" s="84"/>
-      <c r="J1" s="84"/>
-      <c r="K1" s="84"/>
-      <c r="L1" s="84"/>
+      <c r="A1" s="50" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="50"/>
+      <c r="L1" s="50"/>
     </row>
     <row r="2" spans="1:21" ht="18" thickBot="1">
       <c r="O2" s="46" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="85" t="s">
+      <c r="A3" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="86"/>
-      <c r="C3" s="87" t="s">
+      <c r="B3" s="52"/>
+      <c r="C3" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="88"/>
-      <c r="E3" s="88"/>
-      <c r="F3" s="88"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="87" t="s">
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="88"/>
-      <c r="J3" s="90"/>
-      <c r="K3" s="89"/>
+      <c r="I3" s="54"/>
+      <c r="J3" s="56"/>
+      <c r="K3" s="55"/>
       <c r="L3" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="92" t="s">
-        <v>84</v>
-      </c>
-      <c r="N3" s="83"/>
+      <c r="M3" s="58" t="s">
+        <v>83</v>
+      </c>
+      <c r="N3" s="49"/>
     </row>
     <row r="4" spans="1:21" s="3" customFormat="1" ht="40.5" customHeight="1" thickBot="1">
       <c r="A4" s="17" t="s">
@@ -1688,10 +1688,10 @@
         <v>3</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G4" s="11" t="s">
         <v>44</v>
@@ -1711,15 +1711,15 @@
       <c r="L4" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="M4" s="93" t="s">
-        <v>85</v>
-      </c>
-      <c r="N4" s="94"/>
+      <c r="M4" s="59" t="s">
+        <v>84</v>
+      </c>
+      <c r="N4" s="60"/>
       <c r="O4" s="36" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q4" s="37" t="s">
         <v>64</v>
-      </c>
-      <c r="Q4" s="37" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="4.5" customHeight="1">
@@ -1745,7 +1745,7 @@
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E6" s="13"/>
       <c r="F6" s="6"/>
@@ -1756,17 +1756,17 @@
       <c r="K6" s="5"/>
       <c r="L6" s="4"/>
       <c r="M6" s="45" t="s">
-        <v>87</v>
-      </c>
-      <c r="O6" s="82" t="s">
-        <v>68</v>
-      </c>
-      <c r="P6" s="83"/>
-      <c r="Q6" s="83"/>
-      <c r="R6" s="83"/>
-      <c r="S6" s="83"/>
-      <c r="T6" s="83"/>
-      <c r="U6" s="83"/>
+        <v>86</v>
+      </c>
+      <c r="O6" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="P6" s="49"/>
+      <c r="Q6" s="49"/>
+      <c r="R6" s="49"/>
+      <c r="S6" s="49"/>
+      <c r="T6" s="49"/>
+      <c r="U6" s="49"/>
     </row>
     <row r="7" spans="1:21" ht="4.5" customHeight="1">
       <c r="A7" s="29"/>
@@ -1800,10 +1800,10 @@
       <c r="K8" s="7"/>
       <c r="L8" s="4"/>
       <c r="O8" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="P8" s="6" t="s">
         <v>69</v>
-      </c>
-      <c r="P8" s="6" t="s">
-        <v>70</v>
       </c>
       <c r="Q8" s="6"/>
       <c r="R8" s="6"/>
@@ -1828,7 +1828,7 @@
       <c r="K9" s="28"/>
       <c r="L9" s="4"/>
       <c r="P9" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Q9" s="6"/>
     </row>
@@ -1868,10 +1868,10 @@
       <c r="K11" s="7"/>
       <c r="L11" s="4"/>
       <c r="O11" t="s">
+        <v>70</v>
+      </c>
+      <c r="P11" t="s">
         <v>71</v>
-      </c>
-      <c r="P11" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="4.5" customHeight="1">
@@ -1897,7 +1897,7 @@
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="42" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E13" s="13"/>
       <c r="F13" s="5"/>
@@ -1917,7 +1917,7 @@
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="42" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
@@ -1927,14 +1927,14 @@
       <c r="J14" s="4"/>
       <c r="K14" s="7"/>
       <c r="L14" s="4"/>
-      <c r="O14" s="91" t="s">
-        <v>82</v>
-      </c>
-      <c r="P14" s="91"/>
-      <c r="Q14" s="91"/>
-      <c r="R14" s="91"/>
-      <c r="S14" s="91"/>
-      <c r="T14" s="91"/>
+      <c r="O14" s="57" t="s">
+        <v>81</v>
+      </c>
+      <c r="P14" s="57"/>
+      <c r="Q14" s="57"/>
+      <c r="R14" s="57"/>
+      <c r="S14" s="57"/>
+      <c r="T14" s="57"/>
     </row>
     <row r="15" spans="1:21">
       <c r="A15" s="18" t="s">
@@ -1953,12 +1953,12 @@
       <c r="J15" s="4"/>
       <c r="K15" s="7"/>
       <c r="L15" s="4"/>
-      <c r="O15" s="91"/>
-      <c r="P15" s="91"/>
-      <c r="Q15" s="91"/>
-      <c r="R15" s="91"/>
-      <c r="S15" s="91"/>
-      <c r="T15" s="91"/>
+      <c r="O15" s="57"/>
+      <c r="P15" s="57"/>
+      <c r="Q15" s="57"/>
+      <c r="R15" s="57"/>
+      <c r="S15" s="57"/>
+      <c r="T15" s="57"/>
     </row>
     <row r="16" spans="1:21">
       <c r="A16" s="40" t="s">
@@ -1969,7 +1969,7 @@
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="42" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
@@ -1980,10 +1980,10 @@
       <c r="K16" s="7"/>
       <c r="L16" s="4"/>
       <c r="O16" t="s">
+        <v>72</v>
+      </c>
+      <c r="P16" t="s">
         <v>73</v>
-      </c>
-      <c r="P16" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:19">
@@ -2004,7 +2004,7 @@
       <c r="K17" s="7"/>
       <c r="L17" s="4"/>
       <c r="O17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:19" ht="4.5" customHeight="1">
@@ -2030,7 +2030,7 @@
       </c>
       <c r="C19" s="16"/>
       <c r="D19" s="44" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E19" s="6"/>
       <c r="F19" s="8"/>
@@ -2041,7 +2041,7 @@
       <c r="K19" s="7"/>
       <c r="L19" s="32"/>
       <c r="O19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:19">
@@ -2053,7 +2053,7 @@
       </c>
       <c r="C20" s="16"/>
       <c r="D20" s="44" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E20" s="6"/>
       <c r="F20" s="8"/>
@@ -2124,7 +2124,7 @@
       <c r="K24" s="7"/>
       <c r="L24" s="4"/>
       <c r="N24" s="47" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="O24" s="47"/>
       <c r="P24" s="47"/>
@@ -2167,24 +2167,24 @@
     <row r="27" spans="1:19" ht="15.75" thickBot="1">
       <c r="A27" s="24"/>
       <c r="B27" s="26"/>
-      <c r="C27" s="87" t="s">
+      <c r="C27" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="88"/>
-      <c r="E27" s="88"/>
-      <c r="F27" s="88"/>
-      <c r="G27" s="89"/>
-      <c r="H27" s="87" t="s">
+      <c r="D27" s="54"/>
+      <c r="E27" s="54"/>
+      <c r="F27" s="54"/>
+      <c r="G27" s="55"/>
+      <c r="H27" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="I27" s="88"/>
-      <c r="J27" s="90"/>
-      <c r="K27" s="89"/>
+      <c r="I27" s="54"/>
+      <c r="J27" s="56"/>
+      <c r="K27" s="55"/>
       <c r="L27" s="21" t="s">
         <v>4</v>
       </c>
       <c r="N27" s="47" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="O27" s="47"/>
       <c r="P27" s="47"/>
@@ -2193,28 +2193,28 @@
       <c r="S27" s="47"/>
     </row>
     <row r="28" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A28" s="98" t="s">
+      <c r="A28" s="64" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="99"/>
-      <c r="C28" s="95"/>
-      <c r="D28" s="96"/>
-      <c r="E28" s="96"/>
-      <c r="F28" s="96"/>
-      <c r="G28" s="97"/>
-      <c r="H28" s="95"/>
-      <c r="I28" s="96"/>
-      <c r="J28" s="96"/>
-      <c r="K28" s="97"/>
+      <c r="B28" s="65"/>
+      <c r="C28" s="61"/>
+      <c r="D28" s="62"/>
+      <c r="E28" s="62"/>
+      <c r="F28" s="62"/>
+      <c r="G28" s="63"/>
+      <c r="H28" s="61"/>
+      <c r="I28" s="62"/>
+      <c r="J28" s="62"/>
+      <c r="K28" s="63"/>
       <c r="L28" s="4"/>
-      <c r="N28" s="49" t="s">
-        <v>91</v>
-      </c>
-      <c r="O28" s="49"/>
-      <c r="P28" s="49"/>
-      <c r="Q28" s="49"/>
-      <c r="R28" s="49"/>
-      <c r="S28" s="49"/>
+      <c r="N28" s="99" t="s">
+        <v>90</v>
+      </c>
+      <c r="O28" s="99"/>
+      <c r="P28" s="99"/>
+      <c r="Q28" s="99"/>
+      <c r="R28" s="99"/>
+      <c r="S28" s="99"/>
     </row>
     <row r="29" spans="1:19" ht="4.5" customHeight="1">
       <c r="A29" s="29"/>
@@ -2231,100 +2231,100 @@
       <c r="L29" s="31"/>
     </row>
     <row r="30" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A30" s="58" t="s">
+      <c r="A30" s="70" t="s">
         <v>40</v>
       </c>
-      <c r="B30" s="59"/>
-      <c r="C30" s="78"/>
-      <c r="D30" s="72"/>
-      <c r="E30" s="72"/>
-      <c r="F30" s="72"/>
-      <c r="G30" s="73"/>
-      <c r="H30" s="71"/>
-      <c r="I30" s="72"/>
-      <c r="J30" s="72"/>
-      <c r="K30" s="73"/>
+      <c r="B30" s="71"/>
+      <c r="C30" s="66"/>
+      <c r="D30" s="67"/>
+      <c r="E30" s="67"/>
+      <c r="F30" s="67"/>
+      <c r="G30" s="68"/>
+      <c r="H30" s="69"/>
+      <c r="I30" s="67"/>
+      <c r="J30" s="67"/>
+      <c r="K30" s="68"/>
       <c r="L30" s="22" t="s">
         <v>5</v>
       </c>
       <c r="M30" s="34"/>
-      <c r="N30" s="49" t="s">
-        <v>83</v>
-      </c>
-      <c r="O30" s="49"/>
-      <c r="P30" s="49"/>
-      <c r="Q30" s="49"/>
-      <c r="R30" s="49"/>
-      <c r="S30" s="49"/>
+      <c r="N30" s="99" t="s">
+        <v>82</v>
+      </c>
+      <c r="O30" s="99"/>
+      <c r="P30" s="99"/>
+      <c r="Q30" s="99"/>
+      <c r="R30" s="99"/>
+      <c r="S30" s="99"/>
     </row>
     <row r="31" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A31" s="58" t="s">
+      <c r="A31" s="70" t="s">
+        <v>87</v>
+      </c>
+      <c r="B31" s="71"/>
+      <c r="C31" s="76"/>
+      <c r="D31" s="77"/>
+      <c r="E31" s="77"/>
+      <c r="F31" s="77"/>
+      <c r="G31" s="78"/>
+      <c r="H31" s="79" t="s">
         <v>88</v>
-      </c>
-      <c r="B31" s="59"/>
-      <c r="C31" s="68"/>
-      <c r="D31" s="69"/>
-      <c r="E31" s="69"/>
-      <c r="F31" s="69"/>
-      <c r="G31" s="70"/>
-      <c r="H31" s="79" t="s">
-        <v>89</v>
       </c>
       <c r="I31" s="80"/>
       <c r="J31" s="80"/>
       <c r="K31" s="80"/>
       <c r="L31" s="81"/>
       <c r="M31" s="34"/>
-      <c r="N31" s="49" t="s">
+      <c r="N31" s="99" t="s">
+        <v>77</v>
+      </c>
+      <c r="O31" s="99"/>
+      <c r="P31" s="99"/>
+      <c r="Q31" s="99"/>
+      <c r="R31" s="99"/>
+      <c r="S31" s="99"/>
+    </row>
+    <row r="32" spans="1:19" ht="16.5" thickBot="1">
+      <c r="A32" s="74" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32" s="75"/>
+      <c r="C32" s="66"/>
+      <c r="D32" s="67"/>
+      <c r="E32" s="67"/>
+      <c r="F32" s="67"/>
+      <c r="G32" s="68"/>
+      <c r="H32" s="69"/>
+      <c r="I32" s="67"/>
+      <c r="J32" s="67"/>
+      <c r="K32" s="68"/>
+      <c r="M32" s="34"/>
+    </row>
+    <row r="33" spans="1:19" ht="30.75" customHeight="1" thickBot="1">
+      <c r="A33" s="72" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" s="73"/>
+      <c r="C33" s="87" t="s">
+        <v>60</v>
+      </c>
+      <c r="D33" s="88"/>
+      <c r="E33" s="88"/>
+      <c r="F33" s="88"/>
+      <c r="G33" s="89"/>
+      <c r="H33" s="84"/>
+      <c r="I33" s="85"/>
+      <c r="J33" s="85"/>
+      <c r="K33" s="86"/>
+      <c r="M33" s="34"/>
+      <c r="N33" s="98" t="s">
         <v>78</v>
       </c>
-      <c r="O31" s="49"/>
-      <c r="P31" s="49"/>
-      <c r="Q31" s="49"/>
-      <c r="R31" s="49"/>
-      <c r="S31" s="49"/>
-    </row>
-    <row r="32" spans="1:19" ht="16.5" thickBot="1">
-      <c r="A32" s="76" t="s">
-        <v>62</v>
-      </c>
-      <c r="B32" s="77"/>
-      <c r="C32" s="78"/>
-      <c r="D32" s="72"/>
-      <c r="E32" s="72"/>
-      <c r="F32" s="72"/>
-      <c r="G32" s="73"/>
-      <c r="H32" s="71"/>
-      <c r="I32" s="72"/>
-      <c r="J32" s="72"/>
-      <c r="K32" s="73"/>
-      <c r="M32" s="34"/>
-    </row>
-    <row r="33" spans="1:19" ht="30.75" customHeight="1" thickBot="1">
-      <c r="A33" s="74" t="s">
-        <v>36</v>
-      </c>
-      <c r="B33" s="75"/>
-      <c r="C33" s="65" t="s">
-        <v>61</v>
-      </c>
-      <c r="D33" s="66"/>
-      <c r="E33" s="66"/>
-      <c r="F33" s="66"/>
-      <c r="G33" s="67"/>
-      <c r="H33" s="62"/>
-      <c r="I33" s="63"/>
-      <c r="J33" s="63"/>
-      <c r="K33" s="64"/>
-      <c r="M33" s="34"/>
-      <c r="N33" s="48" t="s">
-        <v>79</v>
-      </c>
-      <c r="O33" s="48"/>
-      <c r="P33" s="48"/>
-      <c r="Q33" s="48"/>
-      <c r="R33" s="48"/>
-      <c r="S33" s="48"/>
+      <c r="O33" s="98"/>
+      <c r="P33" s="98"/>
+      <c r="Q33" s="98"/>
+      <c r="R33" s="98"/>
+      <c r="S33" s="98"/>
     </row>
     <row r="34" spans="1:19" ht="4.5" customHeight="1" thickBot="1">
       <c r="A34" s="29"/>
@@ -2340,46 +2340,46 @@
       <c r="K34" s="31"/>
     </row>
     <row r="35" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A35" s="58" t="s">
+      <c r="A35" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="B35" s="59"/>
-      <c r="C35" s="68"/>
-      <c r="D35" s="69"/>
-      <c r="E35" s="69"/>
-      <c r="F35" s="69"/>
-      <c r="G35" s="70"/>
-      <c r="H35" s="68"/>
-      <c r="I35" s="69"/>
-      <c r="J35" s="69"/>
-      <c r="K35" s="70"/>
+      <c r="B35" s="71"/>
+      <c r="C35" s="76"/>
+      <c r="D35" s="77"/>
+      <c r="E35" s="77"/>
+      <c r="F35" s="77"/>
+      <c r="G35" s="78"/>
+      <c r="H35" s="76"/>
+      <c r="I35" s="77"/>
+      <c r="J35" s="77"/>
+      <c r="K35" s="78"/>
       <c r="M35" s="34"/>
-      <c r="N35" s="49" t="s">
-        <v>81</v>
-      </c>
-      <c r="O35" s="49"/>
-      <c r="P35" s="49"/>
-      <c r="Q35" s="49"/>
-      <c r="R35" s="49"/>
-      <c r="S35" s="49"/>
+      <c r="N35" s="99" t="s">
+        <v>80</v>
+      </c>
+      <c r="O35" s="99"/>
+      <c r="P35" s="99"/>
+      <c r="Q35" s="99"/>
+      <c r="R35" s="99"/>
+      <c r="S35" s="99"/>
     </row>
     <row r="36" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A36" s="58" t="s">
+      <c r="A36" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="B36" s="59"/>
-      <c r="C36" s="68"/>
-      <c r="D36" s="69"/>
-      <c r="E36" s="69"/>
-      <c r="F36" s="69"/>
-      <c r="G36" s="70"/>
-      <c r="H36" s="68"/>
-      <c r="I36" s="69"/>
-      <c r="J36" s="69"/>
-      <c r="K36" s="70"/>
+      <c r="B36" s="71"/>
+      <c r="C36" s="76"/>
+      <c r="D36" s="77"/>
+      <c r="E36" s="77"/>
+      <c r="F36" s="77"/>
+      <c r="G36" s="78"/>
+      <c r="H36" s="76"/>
+      <c r="I36" s="77"/>
+      <c r="J36" s="77"/>
+      <c r="K36" s="78"/>
       <c r="M36" s="34"/>
       <c r="N36" s="47" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="O36" s="47"/>
       <c r="P36" s="47"/>
@@ -2388,24 +2388,24 @@
       <c r="S36" s="47"/>
     </row>
     <row r="37" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A37" s="58" t="s">
+      <c r="A37" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="B37" s="59"/>
-      <c r="C37" s="68"/>
-      <c r="D37" s="69"/>
-      <c r="E37" s="69"/>
-      <c r="F37" s="69"/>
-      <c r="G37" s="70"/>
-      <c r="H37" s="68"/>
-      <c r="I37" s="69"/>
-      <c r="J37" s="69"/>
-      <c r="K37" s="70"/>
+      <c r="B37" s="71"/>
+      <c r="C37" s="76"/>
+      <c r="D37" s="77"/>
+      <c r="E37" s="77"/>
+      <c r="F37" s="77"/>
+      <c r="G37" s="78"/>
+      <c r="H37" s="76"/>
+      <c r="I37" s="77"/>
+      <c r="J37" s="77"/>
+      <c r="K37" s="78"/>
       <c r="M37" s="34"/>
     </row>
     <row r="38" spans="1:19" ht="15.75" thickBot="1">
       <c r="N38" s="47" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="O38" s="47"/>
       <c r="P38" s="47"/>
@@ -2414,23 +2414,23 @@
       <c r="S38" s="47"/>
     </row>
     <row r="39" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A39" s="51" t="s">
+      <c r="A39" s="91" t="s">
         <v>27</v>
       </c>
-      <c r="B39" s="52"/>
-      <c r="C39" s="52"/>
-      <c r="D39" s="52"/>
-      <c r="E39" s="53"/>
+      <c r="B39" s="92"/>
+      <c r="C39" s="92"/>
+      <c r="D39" s="92"/>
+      <c r="E39" s="93"/>
     </row>
     <row r="40" spans="1:19">
       <c r="A40" s="14" t="s">
         <v>26</v>
       </c>
       <c r="B40" s="13"/>
-      <c r="C40" s="54" t="s">
+      <c r="C40" s="94" t="s">
         <v>23</v>
       </c>
-      <c r="D40" s="55"/>
+      <c r="D40" s="95"/>
       <c r="E40" s="28"/>
     </row>
     <row r="41" spans="1:19">
@@ -2438,10 +2438,10 @@
         <v>22</v>
       </c>
       <c r="B41" s="5"/>
-      <c r="C41" s="54" t="s">
+      <c r="C41" s="94" t="s">
         <v>24</v>
       </c>
-      <c r="D41" s="55"/>
+      <c r="D41" s="95"/>
       <c r="E41" s="8"/>
     </row>
     <row r="42" spans="1:19">
@@ -2449,154 +2449,154 @@
         <v>25</v>
       </c>
       <c r="B42" s="6"/>
-      <c r="C42" s="60" t="s">
-        <v>67</v>
-      </c>
-      <c r="D42" s="61"/>
+      <c r="C42" s="82" t="s">
+        <v>66</v>
+      </c>
+      <c r="D42" s="83"/>
       <c r="E42" s="39"/>
     </row>
     <row r="43" spans="1:19" ht="15.75" thickBot="1"/>
     <row r="44" spans="1:19">
-      <c r="A44" s="56" t="s">
+      <c r="A44" s="96" t="s">
         <v>37</v>
       </c>
-      <c r="B44" s="57"/>
-      <c r="C44" s="57"/>
-      <c r="D44" s="57"/>
-      <c r="E44" s="57"/>
-      <c r="F44" s="57"/>
-      <c r="G44" s="57"/>
-      <c r="H44" s="57"/>
-      <c r="I44" s="57"/>
-      <c r="J44" s="57"/>
-      <c r="K44" s="57"/>
-      <c r="L44" s="57"/>
+      <c r="B44" s="97"/>
+      <c r="C44" s="97"/>
+      <c r="D44" s="97"/>
+      <c r="E44" s="97"/>
+      <c r="F44" s="97"/>
+      <c r="G44" s="97"/>
+      <c r="H44" s="97"/>
+      <c r="I44" s="97"/>
+      <c r="J44" s="97"/>
+      <c r="K44" s="97"/>
+      <c r="L44" s="97"/>
     </row>
     <row r="45" spans="1:19">
       <c r="A45" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="B45" s="50" t="s">
+      <c r="B45" s="90" t="s">
         <v>57</v>
       </c>
-      <c r="C45" s="50"/>
-      <c r="D45" s="50"/>
-      <c r="E45" s="50"/>
-      <c r="F45" s="50"/>
-      <c r="G45" s="50"/>
-      <c r="H45" s="50"/>
-      <c r="I45" s="50"/>
-      <c r="J45" s="50"/>
-      <c r="K45" s="50"/>
-      <c r="L45" s="50"/>
+      <c r="C45" s="90"/>
+      <c r="D45" s="90"/>
+      <c r="E45" s="90"/>
+      <c r="F45" s="90"/>
+      <c r="G45" s="90"/>
+      <c r="H45" s="90"/>
+      <c r="I45" s="90"/>
+      <c r="J45" s="90"/>
+      <c r="K45" s="90"/>
+      <c r="L45" s="90"/>
     </row>
     <row r="46" spans="1:19" ht="15" customHeight="1">
       <c r="A46" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="B46" s="50" t="s">
+      <c r="B46" s="90" t="s">
         <v>58</v>
       </c>
-      <c r="C46" s="50"/>
-      <c r="D46" s="50"/>
-      <c r="E46" s="50"/>
-      <c r="F46" s="50"/>
-      <c r="G46" s="50"/>
-      <c r="H46" s="50"/>
-      <c r="I46" s="50"/>
-      <c r="J46" s="50"/>
-      <c r="K46" s="50"/>
-      <c r="L46" s="50"/>
+      <c r="C46" s="90"/>
+      <c r="D46" s="90"/>
+      <c r="E46" s="90"/>
+      <c r="F46" s="90"/>
+      <c r="G46" s="90"/>
+      <c r="H46" s="90"/>
+      <c r="I46" s="90"/>
+      <c r="J46" s="90"/>
+      <c r="K46" s="90"/>
+      <c r="L46" s="90"/>
     </row>
     <row r="47" spans="1:19">
       <c r="A47" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="B47" s="50" t="s">
+      <c r="B47" s="90" t="s">
         <v>59</v>
       </c>
-      <c r="C47" s="50"/>
-      <c r="D47" s="50"/>
-      <c r="E47" s="50"/>
-      <c r="F47" s="50"/>
-      <c r="G47" s="50"/>
-      <c r="H47" s="50"/>
-      <c r="I47" s="50"/>
-      <c r="J47" s="50"/>
-      <c r="K47" s="50"/>
-      <c r="L47" s="50"/>
+      <c r="C47" s="90"/>
+      <c r="D47" s="90"/>
+      <c r="E47" s="90"/>
+      <c r="F47" s="90"/>
+      <c r="G47" s="90"/>
+      <c r="H47" s="90"/>
+      <c r="I47" s="90"/>
+      <c r="J47" s="90"/>
+      <c r="K47" s="90"/>
+      <c r="L47" s="90"/>
     </row>
     <row r="48" spans="1:19">
       <c r="A48" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="B48" s="50" t="s">
+      <c r="B48" s="90" t="s">
         <v>46</v>
       </c>
-      <c r="C48" s="50"/>
-      <c r="D48" s="50"/>
-      <c r="E48" s="50"/>
-      <c r="F48" s="50"/>
-      <c r="G48" s="50"/>
-      <c r="H48" s="50"/>
-      <c r="I48" s="50"/>
-      <c r="J48" s="50"/>
-      <c r="K48" s="50"/>
-      <c r="L48" s="50"/>
+      <c r="C48" s="90"/>
+      <c r="D48" s="90"/>
+      <c r="E48" s="90"/>
+      <c r="F48" s="90"/>
+      <c r="G48" s="90"/>
+      <c r="H48" s="90"/>
+      <c r="I48" s="90"/>
+      <c r="J48" s="90"/>
+      <c r="K48" s="90"/>
+      <c r="L48" s="90"/>
     </row>
     <row r="49" spans="1:12">
       <c r="A49" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="B49" s="50" t="s">
+      <c r="B49" s="90" t="s">
         <v>35</v>
       </c>
-      <c r="C49" s="50"/>
-      <c r="D49" s="50"/>
-      <c r="E49" s="50"/>
-      <c r="F49" s="50"/>
-      <c r="G49" s="50"/>
-      <c r="H49" s="50"/>
-      <c r="I49" s="50"/>
-      <c r="J49" s="50"/>
-      <c r="K49" s="50"/>
-      <c r="L49" s="50"/>
+      <c r="C49" s="90"/>
+      <c r="D49" s="90"/>
+      <c r="E49" s="90"/>
+      <c r="F49" s="90"/>
+      <c r="G49" s="90"/>
+      <c r="H49" s="90"/>
+      <c r="I49" s="90"/>
+      <c r="J49" s="90"/>
+      <c r="K49" s="90"/>
+      <c r="L49" s="90"/>
     </row>
     <row r="50" spans="1:12">
       <c r="A50" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="B50" s="50" t="s">
+      <c r="B50" s="90" t="s">
         <v>56</v>
       </c>
-      <c r="C50" s="50"/>
-      <c r="D50" s="50"/>
-      <c r="E50" s="50"/>
-      <c r="F50" s="50"/>
-      <c r="G50" s="50"/>
-      <c r="H50" s="50"/>
-      <c r="I50" s="50"/>
-      <c r="J50" s="50"/>
-      <c r="K50" s="50"/>
-      <c r="L50" s="50"/>
+      <c r="C50" s="90"/>
+      <c r="D50" s="90"/>
+      <c r="E50" s="90"/>
+      <c r="F50" s="90"/>
+      <c r="G50" s="90"/>
+      <c r="H50" s="90"/>
+      <c r="I50" s="90"/>
+      <c r="J50" s="90"/>
+      <c r="K50" s="90"/>
+      <c r="L50" s="90"/>
     </row>
     <row r="51" spans="1:12">
       <c r="A51" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="B51" s="50" t="s">
+      <c r="B51" s="90" t="s">
         <v>55</v>
       </c>
-      <c r="C51" s="50"/>
-      <c r="D51" s="50"/>
-      <c r="E51" s="50"/>
-      <c r="F51" s="50"/>
-      <c r="G51" s="50"/>
-      <c r="H51" s="50"/>
-      <c r="I51" s="50"/>
-      <c r="J51" s="50"/>
-      <c r="K51" s="50"/>
-      <c r="L51" s="50"/>
+      <c r="C51" s="90"/>
+      <c r="D51" s="90"/>
+      <c r="E51" s="90"/>
+      <c r="F51" s="90"/>
+      <c r="G51" s="90"/>
+      <c r="H51" s="90"/>
+      <c r="I51" s="90"/>
+      <c r="J51" s="90"/>
+      <c r="K51" s="90"/>
+      <c r="L51" s="90"/>
     </row>
     <row r="52" spans="1:12">
       <c r="C52" s="34"/>
@@ -2612,6 +2612,45 @@
     <sortCondition ref="A3"/>
   </sortState>
   <mergeCells count="55">
+    <mergeCell ref="N27:S27"/>
+    <mergeCell ref="N33:S33"/>
+    <mergeCell ref="N35:S35"/>
+    <mergeCell ref="N30:S30"/>
+    <mergeCell ref="N28:S28"/>
+    <mergeCell ref="N31:S31"/>
+    <mergeCell ref="B50:L50"/>
+    <mergeCell ref="B51:L51"/>
+    <mergeCell ref="A39:E39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="B45:L45"/>
+    <mergeCell ref="A44:L44"/>
+    <mergeCell ref="B46:L46"/>
+    <mergeCell ref="B47:L47"/>
+    <mergeCell ref="B48:L48"/>
+    <mergeCell ref="B49:L49"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="H33:K33"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="H35:K35"/>
+    <mergeCell ref="H36:K36"/>
+    <mergeCell ref="H37:K37"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="H30:K30"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="H32:K32"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="H31:L31"/>
     <mergeCell ref="N24:S24"/>
     <mergeCell ref="N38:S38"/>
     <mergeCell ref="N36:S36"/>
@@ -2628,45 +2667,6 @@
     <mergeCell ref="H3:K3"/>
     <mergeCell ref="C3:G3"/>
     <mergeCell ref="A28:B28"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="H30:K30"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="H32:K32"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="H31:L31"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="H33:K33"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="H35:K35"/>
-    <mergeCell ref="H36:K36"/>
-    <mergeCell ref="H37:K37"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="B50:L50"/>
-    <mergeCell ref="B51:L51"/>
-    <mergeCell ref="A39:E39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="B45:L45"/>
-    <mergeCell ref="A44:L44"/>
-    <mergeCell ref="B46:L46"/>
-    <mergeCell ref="B47:L47"/>
-    <mergeCell ref="B48:L48"/>
-    <mergeCell ref="B49:L49"/>
-    <mergeCell ref="N27:S27"/>
-    <mergeCell ref="N33:S33"/>
-    <mergeCell ref="N35:S35"/>
-    <mergeCell ref="N30:S30"/>
-    <mergeCell ref="N28:S28"/>
-    <mergeCell ref="N31:S31"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="Q4" r:id="rId1"/>

</xml_diff>

<commit_message>
encarado el componente de trayectoria y formacion, con componentes de organizacion, perfil y grado de estudio, está sin terminar, problemas cal cerrar el 2do formulario, problemas de variable showbtnaction
</commit_message>
<xml_diff>
--- a/Cuadro-de-estado.xlsx
+++ b/Cuadro-de-estado.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="94">
   <si>
     <t>BACKEND</t>
   </si>
@@ -337,9 +337,6 @@
   </si>
   <si>
     <t>En los Getter de los Form, hay que eliminar espacios de los string</t>
-  </si>
-  <si>
-    <t>modal</t>
   </si>
   <si>
     <t>En el controller de Person tiene regla de negocio que debe pasar al Service</t>
@@ -1154,6 +1151,108 @@
     <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1207,108 +1306,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1611,7 +1608,7 @@
   <dimension ref="A1:U54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1628,51 +1625,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25">
-      <c r="A1" s="50" t="s">
-        <v>94</v>
-      </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50"/>
+      <c r="A1" s="84" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="84"/>
+      <c r="K1" s="84"/>
+      <c r="L1" s="84"/>
     </row>
     <row r="2" spans="1:21" ht="18" thickBot="1">
       <c r="O2" s="46" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="85" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="52"/>
-      <c r="C3" s="53" t="s">
+      <c r="B3" s="86"/>
+      <c r="C3" s="87" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="54"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="55"/>
-      <c r="H3" s="53" t="s">
+      <c r="D3" s="88"/>
+      <c r="E3" s="88"/>
+      <c r="F3" s="88"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="54"/>
-      <c r="J3" s="56"/>
-      <c r="K3" s="55"/>
+      <c r="I3" s="88"/>
+      <c r="J3" s="90"/>
+      <c r="K3" s="89"/>
       <c r="L3" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="58" t="s">
-        <v>83</v>
-      </c>
-      <c r="N3" s="49"/>
+      <c r="M3" s="92" t="s">
+        <v>82</v>
+      </c>
+      <c r="N3" s="83"/>
     </row>
     <row r="4" spans="1:21" s="3" customFormat="1" ht="40.5" customHeight="1" thickBot="1">
       <c r="A4" s="17" t="s">
@@ -1711,10 +1708,10 @@
       <c r="L4" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="M4" s="59" t="s">
-        <v>84</v>
-      </c>
-      <c r="N4" s="60"/>
+      <c r="M4" s="93" t="s">
+        <v>83</v>
+      </c>
+      <c r="N4" s="94"/>
       <c r="O4" s="36" t="s">
         <v>63</v>
       </c>
@@ -1744,9 +1741,7 @@
         <v>14</v>
       </c>
       <c r="C6" s="6"/>
-      <c r="D6" s="6" t="s">
-        <v>79</v>
-      </c>
+      <c r="D6" s="6"/>
       <c r="E6" s="13"/>
       <c r="F6" s="6"/>
       <c r="G6" s="5"/>
@@ -1756,17 +1751,17 @@
       <c r="K6" s="5"/>
       <c r="L6" s="4"/>
       <c r="M6" s="45" t="s">
-        <v>86</v>
-      </c>
-      <c r="O6" s="48" t="s">
+        <v>85</v>
+      </c>
+      <c r="O6" s="82" t="s">
         <v>67</v>
       </c>
-      <c r="P6" s="49"/>
-      <c r="Q6" s="49"/>
-      <c r="R6" s="49"/>
-      <c r="S6" s="49"/>
-      <c r="T6" s="49"/>
-      <c r="U6" s="49"/>
+      <c r="P6" s="83"/>
+      <c r="Q6" s="83"/>
+      <c r="R6" s="83"/>
+      <c r="S6" s="83"/>
+      <c r="T6" s="83"/>
+      <c r="U6" s="83"/>
     </row>
     <row r="7" spans="1:21" ht="4.5" customHeight="1">
       <c r="A7" s="29"/>
@@ -1896,9 +1891,7 @@
         <v>13</v>
       </c>
       <c r="C13" s="5"/>
-      <c r="D13" s="42" t="s">
-        <v>79</v>
-      </c>
+      <c r="D13" s="42"/>
       <c r="E13" s="13"/>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
@@ -1916,9 +1909,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="5"/>
-      <c r="D14" s="42" t="s">
-        <v>79</v>
-      </c>
+      <c r="D14" s="42"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
@@ -1927,14 +1918,14 @@
       <c r="J14" s="4"/>
       <c r="K14" s="7"/>
       <c r="L14" s="4"/>
-      <c r="O14" s="57" t="s">
-        <v>81</v>
-      </c>
-      <c r="P14" s="57"/>
-      <c r="Q14" s="57"/>
-      <c r="R14" s="57"/>
-      <c r="S14" s="57"/>
-      <c r="T14" s="57"/>
+      <c r="O14" s="91" t="s">
+        <v>80</v>
+      </c>
+      <c r="P14" s="91"/>
+      <c r="Q14" s="91"/>
+      <c r="R14" s="91"/>
+      <c r="S14" s="91"/>
+      <c r="T14" s="91"/>
     </row>
     <row r="15" spans="1:21">
       <c r="A15" s="18" t="s">
@@ -1944,21 +1935,21 @@
         <v>12</v>
       </c>
       <c r="C15" s="5"/>
-      <c r="D15" s="43"/>
+      <c r="D15" s="5"/>
       <c r="E15" s="5"/>
-      <c r="F15" s="16"/>
+      <c r="F15" s="5"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
       <c r="J15" s="4"/>
       <c r="K15" s="7"/>
       <c r="L15" s="4"/>
-      <c r="O15" s="57"/>
-      <c r="P15" s="57"/>
-      <c r="Q15" s="57"/>
-      <c r="R15" s="57"/>
-      <c r="S15" s="57"/>
-      <c r="T15" s="57"/>
+      <c r="O15" s="91"/>
+      <c r="P15" s="91"/>
+      <c r="Q15" s="91"/>
+      <c r="R15" s="91"/>
+      <c r="S15" s="91"/>
+      <c r="T15" s="91"/>
     </row>
     <row r="16" spans="1:21">
       <c r="A16" s="40" t="s">
@@ -1968,9 +1959,7 @@
         <v>13</v>
       </c>
       <c r="C16" s="5"/>
-      <c r="D16" s="42" t="s">
-        <v>79</v>
-      </c>
+      <c r="D16" s="42"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
@@ -2029,9 +2018,7 @@
         <v>13</v>
       </c>
       <c r="C19" s="16"/>
-      <c r="D19" s="44" t="s">
-        <v>79</v>
-      </c>
+      <c r="D19" s="44"/>
       <c r="E19" s="6"/>
       <c r="F19" s="8"/>
       <c r="G19" s="7"/>
@@ -2052,9 +2039,7 @@
         <v>13</v>
       </c>
       <c r="C20" s="16"/>
-      <c r="D20" s="44" t="s">
-        <v>79</v>
-      </c>
+      <c r="D20" s="44"/>
       <c r="E20" s="6"/>
       <c r="F20" s="8"/>
       <c r="G20" s="7"/>
@@ -2124,7 +2109,7 @@
       <c r="K24" s="7"/>
       <c r="L24" s="4"/>
       <c r="N24" s="47" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="O24" s="47"/>
       <c r="P24" s="47"/>
@@ -2167,24 +2152,24 @@
     <row r="27" spans="1:19" ht="15.75" thickBot="1">
       <c r="A27" s="24"/>
       <c r="B27" s="26"/>
-      <c r="C27" s="53" t="s">
+      <c r="C27" s="87" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="54"/>
-      <c r="E27" s="54"/>
-      <c r="F27" s="54"/>
-      <c r="G27" s="55"/>
-      <c r="H27" s="53" t="s">
+      <c r="D27" s="88"/>
+      <c r="E27" s="88"/>
+      <c r="F27" s="88"/>
+      <c r="G27" s="89"/>
+      <c r="H27" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="I27" s="54"/>
-      <c r="J27" s="56"/>
-      <c r="K27" s="55"/>
+      <c r="I27" s="88"/>
+      <c r="J27" s="90"/>
+      <c r="K27" s="89"/>
       <c r="L27" s="21" t="s">
         <v>4</v>
       </c>
       <c r="N27" s="47" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="O27" s="47"/>
       <c r="P27" s="47"/>
@@ -2193,28 +2178,28 @@
       <c r="S27" s="47"/>
     </row>
     <row r="28" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A28" s="64" t="s">
+      <c r="A28" s="98" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="65"/>
-      <c r="C28" s="61"/>
-      <c r="D28" s="62"/>
-      <c r="E28" s="62"/>
-      <c r="F28" s="62"/>
-      <c r="G28" s="63"/>
-      <c r="H28" s="61"/>
-      <c r="I28" s="62"/>
-      <c r="J28" s="62"/>
-      <c r="K28" s="63"/>
+      <c r="B28" s="99"/>
+      <c r="C28" s="95"/>
+      <c r="D28" s="96"/>
+      <c r="E28" s="96"/>
+      <c r="F28" s="96"/>
+      <c r="G28" s="97"/>
+      <c r="H28" s="95"/>
+      <c r="I28" s="96"/>
+      <c r="J28" s="96"/>
+      <c r="K28" s="97"/>
       <c r="L28" s="4"/>
-      <c r="N28" s="99" t="s">
-        <v>90</v>
-      </c>
-      <c r="O28" s="99"/>
-      <c r="P28" s="99"/>
-      <c r="Q28" s="99"/>
-      <c r="R28" s="99"/>
-      <c r="S28" s="99"/>
+      <c r="N28" s="49" t="s">
+        <v>89</v>
+      </c>
+      <c r="O28" s="49"/>
+      <c r="P28" s="49"/>
+      <c r="Q28" s="49"/>
+      <c r="R28" s="49"/>
+      <c r="S28" s="49"/>
     </row>
     <row r="29" spans="1:19" ht="4.5" customHeight="1">
       <c r="A29" s="29"/>
@@ -2231,100 +2216,100 @@
       <c r="L29" s="31"/>
     </row>
     <row r="30" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A30" s="70" t="s">
+      <c r="A30" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="B30" s="71"/>
-      <c r="C30" s="66"/>
-      <c r="D30" s="67"/>
-      <c r="E30" s="67"/>
-      <c r="F30" s="67"/>
-      <c r="G30" s="68"/>
-      <c r="H30" s="69"/>
-      <c r="I30" s="67"/>
-      <c r="J30" s="67"/>
-      <c r="K30" s="68"/>
+      <c r="B30" s="59"/>
+      <c r="C30" s="71"/>
+      <c r="D30" s="72"/>
+      <c r="E30" s="72"/>
+      <c r="F30" s="72"/>
+      <c r="G30" s="73"/>
+      <c r="H30" s="74"/>
+      <c r="I30" s="72"/>
+      <c r="J30" s="72"/>
+      <c r="K30" s="73"/>
       <c r="L30" s="22" t="s">
         <v>5</v>
       </c>
       <c r="M30" s="34"/>
-      <c r="N30" s="99" t="s">
-        <v>82</v>
-      </c>
-      <c r="O30" s="99"/>
-      <c r="P30" s="99"/>
-      <c r="Q30" s="99"/>
-      <c r="R30" s="99"/>
-      <c r="S30" s="99"/>
+      <c r="N30" s="49" t="s">
+        <v>81</v>
+      </c>
+      <c r="O30" s="49"/>
+      <c r="P30" s="49"/>
+      <c r="Q30" s="49"/>
+      <c r="R30" s="49"/>
+      <c r="S30" s="49"/>
     </row>
     <row r="31" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A31" s="70" t="s">
+      <c r="A31" s="58" t="s">
+        <v>86</v>
+      </c>
+      <c r="B31" s="59"/>
+      <c r="C31" s="68"/>
+      <c r="D31" s="69"/>
+      <c r="E31" s="69"/>
+      <c r="F31" s="69"/>
+      <c r="G31" s="70"/>
+      <c r="H31" s="79" t="s">
         <v>87</v>
-      </c>
-      <c r="B31" s="71"/>
-      <c r="C31" s="76"/>
-      <c r="D31" s="77"/>
-      <c r="E31" s="77"/>
-      <c r="F31" s="77"/>
-      <c r="G31" s="78"/>
-      <c r="H31" s="79" t="s">
-        <v>88</v>
       </c>
       <c r="I31" s="80"/>
       <c r="J31" s="80"/>
       <c r="K31" s="80"/>
       <c r="L31" s="81"/>
       <c r="M31" s="34"/>
-      <c r="N31" s="99" t="s">
+      <c r="N31" s="49" t="s">
         <v>77</v>
       </c>
-      <c r="O31" s="99"/>
-      <c r="P31" s="99"/>
-      <c r="Q31" s="99"/>
-      <c r="R31" s="99"/>
-      <c r="S31" s="99"/>
+      <c r="O31" s="49"/>
+      <c r="P31" s="49"/>
+      <c r="Q31" s="49"/>
+      <c r="R31" s="49"/>
+      <c r="S31" s="49"/>
     </row>
     <row r="32" spans="1:19" ht="16.5" thickBot="1">
-      <c r="A32" s="74" t="s">
+      <c r="A32" s="77" t="s">
         <v>61</v>
       </c>
-      <c r="B32" s="75"/>
-      <c r="C32" s="66"/>
-      <c r="D32" s="67"/>
-      <c r="E32" s="67"/>
-      <c r="F32" s="67"/>
-      <c r="G32" s="68"/>
-      <c r="H32" s="69"/>
-      <c r="I32" s="67"/>
-      <c r="J32" s="67"/>
-      <c r="K32" s="68"/>
+      <c r="B32" s="78"/>
+      <c r="C32" s="71"/>
+      <c r="D32" s="72"/>
+      <c r="E32" s="72"/>
+      <c r="F32" s="72"/>
+      <c r="G32" s="73"/>
+      <c r="H32" s="74"/>
+      <c r="I32" s="72"/>
+      <c r="J32" s="72"/>
+      <c r="K32" s="73"/>
       <c r="M32" s="34"/>
     </row>
     <row r="33" spans="1:19" ht="30.75" customHeight="1" thickBot="1">
-      <c r="A33" s="72" t="s">
+      <c r="A33" s="75" t="s">
         <v>36</v>
       </c>
-      <c r="B33" s="73"/>
-      <c r="C33" s="87" t="s">
+      <c r="B33" s="76"/>
+      <c r="C33" s="65" t="s">
         <v>60</v>
       </c>
-      <c r="D33" s="88"/>
-      <c r="E33" s="88"/>
-      <c r="F33" s="88"/>
-      <c r="G33" s="89"/>
-      <c r="H33" s="84"/>
-      <c r="I33" s="85"/>
-      <c r="J33" s="85"/>
-      <c r="K33" s="86"/>
+      <c r="D33" s="66"/>
+      <c r="E33" s="66"/>
+      <c r="F33" s="66"/>
+      <c r="G33" s="67"/>
+      <c r="H33" s="62"/>
+      <c r="I33" s="63"/>
+      <c r="J33" s="63"/>
+      <c r="K33" s="64"/>
       <c r="M33" s="34"/>
-      <c r="N33" s="98" t="s">
+      <c r="N33" s="48" t="s">
         <v>78</v>
       </c>
-      <c r="O33" s="98"/>
-      <c r="P33" s="98"/>
-      <c r="Q33" s="98"/>
-      <c r="R33" s="98"/>
-      <c r="S33" s="98"/>
+      <c r="O33" s="48"/>
+      <c r="P33" s="48"/>
+      <c r="Q33" s="48"/>
+      <c r="R33" s="48"/>
+      <c r="S33" s="48"/>
     </row>
     <row r="34" spans="1:19" ht="4.5" customHeight="1" thickBot="1">
       <c r="A34" s="29"/>
@@ -2340,46 +2325,46 @@
       <c r="K34" s="31"/>
     </row>
     <row r="35" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A35" s="70" t="s">
+      <c r="A35" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="B35" s="71"/>
-      <c r="C35" s="76"/>
-      <c r="D35" s="77"/>
-      <c r="E35" s="77"/>
-      <c r="F35" s="77"/>
-      <c r="G35" s="78"/>
-      <c r="H35" s="76"/>
-      <c r="I35" s="77"/>
-      <c r="J35" s="77"/>
-      <c r="K35" s="78"/>
+      <c r="B35" s="59"/>
+      <c r="C35" s="68"/>
+      <c r="D35" s="69"/>
+      <c r="E35" s="69"/>
+      <c r="F35" s="69"/>
+      <c r="G35" s="70"/>
+      <c r="H35" s="68"/>
+      <c r="I35" s="69"/>
+      <c r="J35" s="69"/>
+      <c r="K35" s="70"/>
       <c r="M35" s="34"/>
-      <c r="N35" s="99" t="s">
-        <v>80</v>
-      </c>
-      <c r="O35" s="99"/>
-      <c r="P35" s="99"/>
-      <c r="Q35" s="99"/>
-      <c r="R35" s="99"/>
-      <c r="S35" s="99"/>
+      <c r="N35" s="49" t="s">
+        <v>79</v>
+      </c>
+      <c r="O35" s="49"/>
+      <c r="P35" s="49"/>
+      <c r="Q35" s="49"/>
+      <c r="R35" s="49"/>
+      <c r="S35" s="49"/>
     </row>
     <row r="36" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A36" s="70" t="s">
+      <c r="A36" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="B36" s="71"/>
-      <c r="C36" s="76"/>
-      <c r="D36" s="77"/>
-      <c r="E36" s="77"/>
-      <c r="F36" s="77"/>
-      <c r="G36" s="78"/>
-      <c r="H36" s="76"/>
-      <c r="I36" s="77"/>
-      <c r="J36" s="77"/>
-      <c r="K36" s="78"/>
+      <c r="B36" s="59"/>
+      <c r="C36" s="68"/>
+      <c r="D36" s="69"/>
+      <c r="E36" s="69"/>
+      <c r="F36" s="69"/>
+      <c r="G36" s="70"/>
+      <c r="H36" s="68"/>
+      <c r="I36" s="69"/>
+      <c r="J36" s="69"/>
+      <c r="K36" s="70"/>
       <c r="M36" s="34"/>
       <c r="N36" s="47" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="O36" s="47"/>
       <c r="P36" s="47"/>
@@ -2388,24 +2373,24 @@
       <c r="S36" s="47"/>
     </row>
     <row r="37" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A37" s="70" t="s">
+      <c r="A37" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="B37" s="71"/>
-      <c r="C37" s="76"/>
-      <c r="D37" s="77"/>
-      <c r="E37" s="77"/>
-      <c r="F37" s="77"/>
-      <c r="G37" s="78"/>
-      <c r="H37" s="76"/>
-      <c r="I37" s="77"/>
-      <c r="J37" s="77"/>
-      <c r="K37" s="78"/>
+      <c r="B37" s="59"/>
+      <c r="C37" s="68"/>
+      <c r="D37" s="69"/>
+      <c r="E37" s="69"/>
+      <c r="F37" s="69"/>
+      <c r="G37" s="70"/>
+      <c r="H37" s="68"/>
+      <c r="I37" s="69"/>
+      <c r="J37" s="69"/>
+      <c r="K37" s="70"/>
       <c r="M37" s="34"/>
     </row>
     <row r="38" spans="1:19" ht="15.75" thickBot="1">
       <c r="N38" s="47" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="O38" s="47"/>
       <c r="P38" s="47"/>
@@ -2414,23 +2399,23 @@
       <c r="S38" s="47"/>
     </row>
     <row r="39" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A39" s="91" t="s">
+      <c r="A39" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="B39" s="92"/>
-      <c r="C39" s="92"/>
-      <c r="D39" s="92"/>
-      <c r="E39" s="93"/>
+      <c r="B39" s="52"/>
+      <c r="C39" s="52"/>
+      <c r="D39" s="52"/>
+      <c r="E39" s="53"/>
     </row>
     <row r="40" spans="1:19">
       <c r="A40" s="14" t="s">
         <v>26</v>
       </c>
       <c r="B40" s="13"/>
-      <c r="C40" s="94" t="s">
+      <c r="C40" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="D40" s="95"/>
+      <c r="D40" s="55"/>
       <c r="E40" s="28"/>
     </row>
     <row r="41" spans="1:19">
@@ -2438,10 +2423,10 @@
         <v>22</v>
       </c>
       <c r="B41" s="5"/>
-      <c r="C41" s="94" t="s">
+      <c r="C41" s="54" t="s">
         <v>24</v>
       </c>
-      <c r="D41" s="95"/>
+      <c r="D41" s="55"/>
       <c r="E41" s="8"/>
     </row>
     <row r="42" spans="1:19">
@@ -2449,154 +2434,154 @@
         <v>25</v>
       </c>
       <c r="B42" s="6"/>
-      <c r="C42" s="82" t="s">
+      <c r="C42" s="60" t="s">
         <v>66</v>
       </c>
-      <c r="D42" s="83"/>
+      <c r="D42" s="61"/>
       <c r="E42" s="39"/>
     </row>
     <row r="43" spans="1:19" ht="15.75" thickBot="1"/>
     <row r="44" spans="1:19">
-      <c r="A44" s="96" t="s">
+      <c r="A44" s="56" t="s">
         <v>37</v>
       </c>
-      <c r="B44" s="97"/>
-      <c r="C44" s="97"/>
-      <c r="D44" s="97"/>
-      <c r="E44" s="97"/>
-      <c r="F44" s="97"/>
-      <c r="G44" s="97"/>
-      <c r="H44" s="97"/>
-      <c r="I44" s="97"/>
-      <c r="J44" s="97"/>
-      <c r="K44" s="97"/>
-      <c r="L44" s="97"/>
+      <c r="B44" s="57"/>
+      <c r="C44" s="57"/>
+      <c r="D44" s="57"/>
+      <c r="E44" s="57"/>
+      <c r="F44" s="57"/>
+      <c r="G44" s="57"/>
+      <c r="H44" s="57"/>
+      <c r="I44" s="57"/>
+      <c r="J44" s="57"/>
+      <c r="K44" s="57"/>
+      <c r="L44" s="57"/>
     </row>
     <row r="45" spans="1:19">
       <c r="A45" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="B45" s="90" t="s">
+      <c r="B45" s="50" t="s">
         <v>57</v>
       </c>
-      <c r="C45" s="90"/>
-      <c r="D45" s="90"/>
-      <c r="E45" s="90"/>
-      <c r="F45" s="90"/>
-      <c r="G45" s="90"/>
-      <c r="H45" s="90"/>
-      <c r="I45" s="90"/>
-      <c r="J45" s="90"/>
-      <c r="K45" s="90"/>
-      <c r="L45" s="90"/>
+      <c r="C45" s="50"/>
+      <c r="D45" s="50"/>
+      <c r="E45" s="50"/>
+      <c r="F45" s="50"/>
+      <c r="G45" s="50"/>
+      <c r="H45" s="50"/>
+      <c r="I45" s="50"/>
+      <c r="J45" s="50"/>
+      <c r="K45" s="50"/>
+      <c r="L45" s="50"/>
     </row>
     <row r="46" spans="1:19" ht="15" customHeight="1">
       <c r="A46" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="B46" s="90" t="s">
+      <c r="B46" s="50" t="s">
         <v>58</v>
       </c>
-      <c r="C46" s="90"/>
-      <c r="D46" s="90"/>
-      <c r="E46" s="90"/>
-      <c r="F46" s="90"/>
-      <c r="G46" s="90"/>
-      <c r="H46" s="90"/>
-      <c r="I46" s="90"/>
-      <c r="J46" s="90"/>
-      <c r="K46" s="90"/>
-      <c r="L46" s="90"/>
+      <c r="C46" s="50"/>
+      <c r="D46" s="50"/>
+      <c r="E46" s="50"/>
+      <c r="F46" s="50"/>
+      <c r="G46" s="50"/>
+      <c r="H46" s="50"/>
+      <c r="I46" s="50"/>
+      <c r="J46" s="50"/>
+      <c r="K46" s="50"/>
+      <c r="L46" s="50"/>
     </row>
     <row r="47" spans="1:19">
       <c r="A47" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="B47" s="90" t="s">
+      <c r="B47" s="50" t="s">
         <v>59</v>
       </c>
-      <c r="C47" s="90"/>
-      <c r="D47" s="90"/>
-      <c r="E47" s="90"/>
-      <c r="F47" s="90"/>
-      <c r="G47" s="90"/>
-      <c r="H47" s="90"/>
-      <c r="I47" s="90"/>
-      <c r="J47" s="90"/>
-      <c r="K47" s="90"/>
-      <c r="L47" s="90"/>
+      <c r="C47" s="50"/>
+      <c r="D47" s="50"/>
+      <c r="E47" s="50"/>
+      <c r="F47" s="50"/>
+      <c r="G47" s="50"/>
+      <c r="H47" s="50"/>
+      <c r="I47" s="50"/>
+      <c r="J47" s="50"/>
+      <c r="K47" s="50"/>
+      <c r="L47" s="50"/>
     </row>
     <row r="48" spans="1:19">
       <c r="A48" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="B48" s="90" t="s">
+      <c r="B48" s="50" t="s">
         <v>46</v>
       </c>
-      <c r="C48" s="90"/>
-      <c r="D48" s="90"/>
-      <c r="E48" s="90"/>
-      <c r="F48" s="90"/>
-      <c r="G48" s="90"/>
-      <c r="H48" s="90"/>
-      <c r="I48" s="90"/>
-      <c r="J48" s="90"/>
-      <c r="K48" s="90"/>
-      <c r="L48" s="90"/>
+      <c r="C48" s="50"/>
+      <c r="D48" s="50"/>
+      <c r="E48" s="50"/>
+      <c r="F48" s="50"/>
+      <c r="G48" s="50"/>
+      <c r="H48" s="50"/>
+      <c r="I48" s="50"/>
+      <c r="J48" s="50"/>
+      <c r="K48" s="50"/>
+      <c r="L48" s="50"/>
     </row>
     <row r="49" spans="1:12">
       <c r="A49" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="B49" s="90" t="s">
+      <c r="B49" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="C49" s="90"/>
-      <c r="D49" s="90"/>
-      <c r="E49" s="90"/>
-      <c r="F49" s="90"/>
-      <c r="G49" s="90"/>
-      <c r="H49" s="90"/>
-      <c r="I49" s="90"/>
-      <c r="J49" s="90"/>
-      <c r="K49" s="90"/>
-      <c r="L49" s="90"/>
+      <c r="C49" s="50"/>
+      <c r="D49" s="50"/>
+      <c r="E49" s="50"/>
+      <c r="F49" s="50"/>
+      <c r="G49" s="50"/>
+      <c r="H49" s="50"/>
+      <c r="I49" s="50"/>
+      <c r="J49" s="50"/>
+      <c r="K49" s="50"/>
+      <c r="L49" s="50"/>
     </row>
     <row r="50" spans="1:12">
       <c r="A50" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="B50" s="90" t="s">
+      <c r="B50" s="50" t="s">
         <v>56</v>
       </c>
-      <c r="C50" s="90"/>
-      <c r="D50" s="90"/>
-      <c r="E50" s="90"/>
-      <c r="F50" s="90"/>
-      <c r="G50" s="90"/>
-      <c r="H50" s="90"/>
-      <c r="I50" s="90"/>
-      <c r="J50" s="90"/>
-      <c r="K50" s="90"/>
-      <c r="L50" s="90"/>
+      <c r="C50" s="50"/>
+      <c r="D50" s="50"/>
+      <c r="E50" s="50"/>
+      <c r="F50" s="50"/>
+      <c r="G50" s="50"/>
+      <c r="H50" s="50"/>
+      <c r="I50" s="50"/>
+      <c r="J50" s="50"/>
+      <c r="K50" s="50"/>
+      <c r="L50" s="50"/>
     </row>
     <row r="51" spans="1:12">
       <c r="A51" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="B51" s="90" t="s">
+      <c r="B51" s="50" t="s">
         <v>55</v>
       </c>
-      <c r="C51" s="90"/>
-      <c r="D51" s="90"/>
-      <c r="E51" s="90"/>
-      <c r="F51" s="90"/>
-      <c r="G51" s="90"/>
-      <c r="H51" s="90"/>
-      <c r="I51" s="90"/>
-      <c r="J51" s="90"/>
-      <c r="K51" s="90"/>
-      <c r="L51" s="90"/>
+      <c r="C51" s="50"/>
+      <c r="D51" s="50"/>
+      <c r="E51" s="50"/>
+      <c r="F51" s="50"/>
+      <c r="G51" s="50"/>
+      <c r="H51" s="50"/>
+      <c r="I51" s="50"/>
+      <c r="J51" s="50"/>
+      <c r="K51" s="50"/>
+      <c r="L51" s="50"/>
     </row>
     <row r="52" spans="1:12">
       <c r="C52" s="34"/>
@@ -2612,45 +2597,6 @@
     <sortCondition ref="A3"/>
   </sortState>
   <mergeCells count="55">
-    <mergeCell ref="N27:S27"/>
-    <mergeCell ref="N33:S33"/>
-    <mergeCell ref="N35:S35"/>
-    <mergeCell ref="N30:S30"/>
-    <mergeCell ref="N28:S28"/>
-    <mergeCell ref="N31:S31"/>
-    <mergeCell ref="B50:L50"/>
-    <mergeCell ref="B51:L51"/>
-    <mergeCell ref="A39:E39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="B45:L45"/>
-    <mergeCell ref="A44:L44"/>
-    <mergeCell ref="B46:L46"/>
-    <mergeCell ref="B47:L47"/>
-    <mergeCell ref="B48:L48"/>
-    <mergeCell ref="B49:L49"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="H33:K33"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="H35:K35"/>
-    <mergeCell ref="H36:K36"/>
-    <mergeCell ref="H37:K37"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="H30:K30"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="H32:K32"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="H31:L31"/>
     <mergeCell ref="N24:S24"/>
     <mergeCell ref="N38:S38"/>
     <mergeCell ref="N36:S36"/>
@@ -2667,6 +2613,45 @@
     <mergeCell ref="H3:K3"/>
     <mergeCell ref="C3:G3"/>
     <mergeCell ref="A28:B28"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="H30:K30"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="H32:K32"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="H31:L31"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="H33:K33"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="H35:K35"/>
+    <mergeCell ref="H36:K36"/>
+    <mergeCell ref="H37:K37"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="B50:L50"/>
+    <mergeCell ref="B51:L51"/>
+    <mergeCell ref="A39:E39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="B45:L45"/>
+    <mergeCell ref="A44:L44"/>
+    <mergeCell ref="B46:L46"/>
+    <mergeCell ref="B47:L47"/>
+    <mergeCell ref="B48:L48"/>
+    <mergeCell ref="B49:L49"/>
+    <mergeCell ref="N27:S27"/>
+    <mergeCell ref="N33:S33"/>
+    <mergeCell ref="N35:S35"/>
+    <mergeCell ref="N30:S30"/>
+    <mergeCell ref="N28:S28"/>
+    <mergeCell ref="N31:S31"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="Q4" r:id="rId1"/>

</xml_diff>

<commit_message>
refactorizado de las clases en el backend, ahora funciona el archivo.jar desde consola, pero falta acomodar dentro de netbeans, que ahora es quien arroja el error de no encontrar la clase main
</commit_message>
<xml_diff>
--- a/Cuadro-de-estado.xlsx
+++ b/Cuadro-de-estado.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="95">
   <si>
     <t>BACKEND</t>
   </si>
@@ -383,12 +383,18 @@
   <si>
     <t>ESTADO DEL PROYECTO Y PRIORIDADES</t>
   </si>
+  <si>
+    <t>Dias faltantes</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="24">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
+  </numFmts>
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -567,8 +573,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -641,6 +672,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="33">
     <border>
@@ -1047,14 +1084,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="43" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1151,165 +1189,176 @@
     <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="13" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+    <cellStyle name="Millares" xfId="2" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1608,7 +1657,7 @@
   <dimension ref="A1:U54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1625,51 +1674,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25">
-      <c r="A1" s="84" t="s">
+      <c r="A1" s="50" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
-      <c r="F1" s="84"/>
-      <c r="G1" s="84"/>
-      <c r="H1" s="84"/>
-      <c r="I1" s="84"/>
-      <c r="J1" s="84"/>
-      <c r="K1" s="84"/>
-      <c r="L1" s="84"/>
-    </row>
-    <row r="2" spans="1:21" ht="18" thickBot="1">
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="50"/>
+      <c r="L1" s="50"/>
+    </row>
+    <row r="2" spans="1:21" ht="19.5" thickBot="1">
+      <c r="A2" s="101">
+        <f ca="1">M2-TODAY()-1</f>
+        <v>49</v>
+      </c>
+      <c r="B2" s="102" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" s="103"/>
+      <c r="M2" s="100">
+        <v>45011</v>
+      </c>
       <c r="O2" s="46" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="85" t="s">
+      <c r="A3" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="86"/>
-      <c r="C3" s="87" t="s">
+      <c r="B3" s="52"/>
+      <c r="C3" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="88"/>
-      <c r="E3" s="88"/>
-      <c r="F3" s="88"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="87" t="s">
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="88"/>
-      <c r="J3" s="90"/>
-      <c r="K3" s="89"/>
+      <c r="I3" s="54"/>
+      <c r="J3" s="56"/>
+      <c r="K3" s="55"/>
       <c r="L3" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="92" t="s">
+      <c r="M3" s="58" t="s">
         <v>82</v>
       </c>
-      <c r="N3" s="83"/>
+      <c r="N3" s="49"/>
     </row>
     <row r="4" spans="1:21" s="3" customFormat="1" ht="40.5" customHeight="1" thickBot="1">
       <c r="A4" s="17" t="s">
@@ -1708,10 +1768,10 @@
       <c r="L4" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="M4" s="93" t="s">
+      <c r="M4" s="59" t="s">
         <v>83</v>
       </c>
-      <c r="N4" s="94"/>
+      <c r="N4" s="60"/>
       <c r="O4" s="36" t="s">
         <v>63</v>
       </c>
@@ -1753,15 +1813,15 @@
       <c r="M6" s="45" t="s">
         <v>85</v>
       </c>
-      <c r="O6" s="82" t="s">
+      <c r="O6" s="48" t="s">
         <v>67</v>
       </c>
-      <c r="P6" s="83"/>
-      <c r="Q6" s="83"/>
-      <c r="R6" s="83"/>
-      <c r="S6" s="83"/>
-      <c r="T6" s="83"/>
-      <c r="U6" s="83"/>
+      <c r="P6" s="49"/>
+      <c r="Q6" s="49"/>
+      <c r="R6" s="49"/>
+      <c r="S6" s="49"/>
+      <c r="T6" s="49"/>
+      <c r="U6" s="49"/>
     </row>
     <row r="7" spans="1:21" ht="4.5" customHeight="1">
       <c r="A7" s="29"/>
@@ -1918,14 +1978,14 @@
       <c r="J14" s="4"/>
       <c r="K14" s="7"/>
       <c r="L14" s="4"/>
-      <c r="O14" s="91" t="s">
+      <c r="O14" s="57" t="s">
         <v>80</v>
       </c>
-      <c r="P14" s="91"/>
-      <c r="Q14" s="91"/>
-      <c r="R14" s="91"/>
-      <c r="S14" s="91"/>
-      <c r="T14" s="91"/>
+      <c r="P14" s="57"/>
+      <c r="Q14" s="57"/>
+      <c r="R14" s="57"/>
+      <c r="S14" s="57"/>
+      <c r="T14" s="57"/>
     </row>
     <row r="15" spans="1:21">
       <c r="A15" s="18" t="s">
@@ -1944,12 +2004,12 @@
       <c r="J15" s="4"/>
       <c r="K15" s="7"/>
       <c r="L15" s="4"/>
-      <c r="O15" s="91"/>
-      <c r="P15" s="91"/>
-      <c r="Q15" s="91"/>
-      <c r="R15" s="91"/>
-      <c r="S15" s="91"/>
-      <c r="T15" s="91"/>
+      <c r="O15" s="57"/>
+      <c r="P15" s="57"/>
+      <c r="Q15" s="57"/>
+      <c r="R15" s="57"/>
+      <c r="S15" s="57"/>
+      <c r="T15" s="57"/>
     </row>
     <row r="16" spans="1:21">
       <c r="A16" s="40" t="s">
@@ -2152,19 +2212,19 @@
     <row r="27" spans="1:19" ht="15.75" thickBot="1">
       <c r="A27" s="24"/>
       <c r="B27" s="26"/>
-      <c r="C27" s="87" t="s">
+      <c r="C27" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="88"/>
-      <c r="E27" s="88"/>
-      <c r="F27" s="88"/>
-      <c r="G27" s="89"/>
-      <c r="H27" s="87" t="s">
+      <c r="D27" s="54"/>
+      <c r="E27" s="54"/>
+      <c r="F27" s="54"/>
+      <c r="G27" s="55"/>
+      <c r="H27" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="I27" s="88"/>
-      <c r="J27" s="90"/>
-      <c r="K27" s="89"/>
+      <c r="I27" s="54"/>
+      <c r="J27" s="56"/>
+      <c r="K27" s="55"/>
       <c r="L27" s="21" t="s">
         <v>4</v>
       </c>
@@ -2178,28 +2238,28 @@
       <c r="S27" s="47"/>
     </row>
     <row r="28" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A28" s="98" t="s">
+      <c r="A28" s="64" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="99"/>
-      <c r="C28" s="95"/>
-      <c r="D28" s="96"/>
-      <c r="E28" s="96"/>
-      <c r="F28" s="96"/>
-      <c r="G28" s="97"/>
-      <c r="H28" s="95"/>
-      <c r="I28" s="96"/>
-      <c r="J28" s="96"/>
-      <c r="K28" s="97"/>
+      <c r="B28" s="65"/>
+      <c r="C28" s="61"/>
+      <c r="D28" s="62"/>
+      <c r="E28" s="62"/>
+      <c r="F28" s="62"/>
+      <c r="G28" s="63"/>
+      <c r="H28" s="61"/>
+      <c r="I28" s="62"/>
+      <c r="J28" s="62"/>
+      <c r="K28" s="63"/>
       <c r="L28" s="4"/>
-      <c r="N28" s="49" t="s">
+      <c r="N28" s="99" t="s">
         <v>89</v>
       </c>
-      <c r="O28" s="49"/>
-      <c r="P28" s="49"/>
-      <c r="Q28" s="49"/>
-      <c r="R28" s="49"/>
-      <c r="S28" s="49"/>
+      <c r="O28" s="99"/>
+      <c r="P28" s="99"/>
+      <c r="Q28" s="99"/>
+      <c r="R28" s="99"/>
+      <c r="S28" s="99"/>
     </row>
     <row r="29" spans="1:19" ht="4.5" customHeight="1">
       <c r="A29" s="29"/>
@@ -2216,42 +2276,42 @@
       <c r="L29" s="31"/>
     </row>
     <row r="30" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A30" s="58" t="s">
+      <c r="A30" s="70" t="s">
         <v>40</v>
       </c>
-      <c r="B30" s="59"/>
-      <c r="C30" s="71"/>
-      <c r="D30" s="72"/>
-      <c r="E30" s="72"/>
-      <c r="F30" s="72"/>
-      <c r="G30" s="73"/>
-      <c r="H30" s="74"/>
-      <c r="I30" s="72"/>
-      <c r="J30" s="72"/>
-      <c r="K30" s="73"/>
+      <c r="B30" s="71"/>
+      <c r="C30" s="66"/>
+      <c r="D30" s="67"/>
+      <c r="E30" s="67"/>
+      <c r="F30" s="67"/>
+      <c r="G30" s="68"/>
+      <c r="H30" s="69"/>
+      <c r="I30" s="67"/>
+      <c r="J30" s="67"/>
+      <c r="K30" s="68"/>
       <c r="L30" s="22" t="s">
         <v>5</v>
       </c>
       <c r="M30" s="34"/>
-      <c r="N30" s="49" t="s">
+      <c r="N30" s="99" t="s">
         <v>81</v>
       </c>
-      <c r="O30" s="49"/>
-      <c r="P30" s="49"/>
-      <c r="Q30" s="49"/>
-      <c r="R30" s="49"/>
-      <c r="S30" s="49"/>
+      <c r="O30" s="99"/>
+      <c r="P30" s="99"/>
+      <c r="Q30" s="99"/>
+      <c r="R30" s="99"/>
+      <c r="S30" s="99"/>
     </row>
     <row r="31" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A31" s="58" t="s">
+      <c r="A31" s="70" t="s">
         <v>86</v>
       </c>
-      <c r="B31" s="59"/>
-      <c r="C31" s="68"/>
-      <c r="D31" s="69"/>
-      <c r="E31" s="69"/>
-      <c r="F31" s="69"/>
-      <c r="G31" s="70"/>
+      <c r="B31" s="71"/>
+      <c r="C31" s="76"/>
+      <c r="D31" s="77"/>
+      <c r="E31" s="77"/>
+      <c r="F31" s="77"/>
+      <c r="G31" s="78"/>
       <c r="H31" s="79" t="s">
         <v>87</v>
       </c>
@@ -2260,56 +2320,56 @@
       <c r="K31" s="80"/>
       <c r="L31" s="81"/>
       <c r="M31" s="34"/>
-      <c r="N31" s="49" t="s">
+      <c r="N31" s="99" t="s">
         <v>77</v>
       </c>
-      <c r="O31" s="49"/>
-      <c r="P31" s="49"/>
-      <c r="Q31" s="49"/>
-      <c r="R31" s="49"/>
-      <c r="S31" s="49"/>
+      <c r="O31" s="99"/>
+      <c r="P31" s="99"/>
+      <c r="Q31" s="99"/>
+      <c r="R31" s="99"/>
+      <c r="S31" s="99"/>
     </row>
     <row r="32" spans="1:19" ht="16.5" thickBot="1">
-      <c r="A32" s="77" t="s">
+      <c r="A32" s="74" t="s">
         <v>61</v>
       </c>
-      <c r="B32" s="78"/>
-      <c r="C32" s="71"/>
-      <c r="D32" s="72"/>
-      <c r="E32" s="72"/>
-      <c r="F32" s="72"/>
-      <c r="G32" s="73"/>
-      <c r="H32" s="74"/>
-      <c r="I32" s="72"/>
-      <c r="J32" s="72"/>
-      <c r="K32" s="73"/>
+      <c r="B32" s="75"/>
+      <c r="C32" s="66"/>
+      <c r="D32" s="67"/>
+      <c r="E32" s="67"/>
+      <c r="F32" s="67"/>
+      <c r="G32" s="68"/>
+      <c r="H32" s="69"/>
+      <c r="I32" s="67"/>
+      <c r="J32" s="67"/>
+      <c r="K32" s="68"/>
       <c r="M32" s="34"/>
     </row>
     <row r="33" spans="1:19" ht="30.75" customHeight="1" thickBot="1">
-      <c r="A33" s="75" t="s">
+      <c r="A33" s="72" t="s">
         <v>36</v>
       </c>
-      <c r="B33" s="76"/>
-      <c r="C33" s="65" t="s">
+      <c r="B33" s="73"/>
+      <c r="C33" s="87" t="s">
         <v>60</v>
       </c>
-      <c r="D33" s="66"/>
-      <c r="E33" s="66"/>
-      <c r="F33" s="66"/>
-      <c r="G33" s="67"/>
-      <c r="H33" s="62"/>
-      <c r="I33" s="63"/>
-      <c r="J33" s="63"/>
-      <c r="K33" s="64"/>
+      <c r="D33" s="88"/>
+      <c r="E33" s="88"/>
+      <c r="F33" s="88"/>
+      <c r="G33" s="89"/>
+      <c r="H33" s="84"/>
+      <c r="I33" s="85"/>
+      <c r="J33" s="85"/>
+      <c r="K33" s="86"/>
       <c r="M33" s="34"/>
-      <c r="N33" s="48" t="s">
+      <c r="N33" s="98" t="s">
         <v>78</v>
       </c>
-      <c r="O33" s="48"/>
-      <c r="P33" s="48"/>
-      <c r="Q33" s="48"/>
-      <c r="R33" s="48"/>
-      <c r="S33" s="48"/>
+      <c r="O33" s="98"/>
+      <c r="P33" s="98"/>
+      <c r="Q33" s="98"/>
+      <c r="R33" s="98"/>
+      <c r="S33" s="98"/>
     </row>
     <row r="34" spans="1:19" ht="4.5" customHeight="1" thickBot="1">
       <c r="A34" s="29"/>
@@ -2325,43 +2385,43 @@
       <c r="K34" s="31"/>
     </row>
     <row r="35" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A35" s="58" t="s">
+      <c r="A35" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="B35" s="59"/>
-      <c r="C35" s="68"/>
-      <c r="D35" s="69"/>
-      <c r="E35" s="69"/>
-      <c r="F35" s="69"/>
-      <c r="G35" s="70"/>
-      <c r="H35" s="68"/>
-      <c r="I35" s="69"/>
-      <c r="J35" s="69"/>
-      <c r="K35" s="70"/>
+      <c r="B35" s="71"/>
+      <c r="C35" s="76"/>
+      <c r="D35" s="77"/>
+      <c r="E35" s="77"/>
+      <c r="F35" s="77"/>
+      <c r="G35" s="78"/>
+      <c r="H35" s="76"/>
+      <c r="I35" s="77"/>
+      <c r="J35" s="77"/>
+      <c r="K35" s="78"/>
       <c r="M35" s="34"/>
-      <c r="N35" s="49" t="s">
+      <c r="N35" s="99" t="s">
         <v>79</v>
       </c>
-      <c r="O35" s="49"/>
-      <c r="P35" s="49"/>
-      <c r="Q35" s="49"/>
-      <c r="R35" s="49"/>
-      <c r="S35" s="49"/>
+      <c r="O35" s="99"/>
+      <c r="P35" s="99"/>
+      <c r="Q35" s="99"/>
+      <c r="R35" s="99"/>
+      <c r="S35" s="99"/>
     </row>
     <row r="36" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A36" s="58" t="s">
+      <c r="A36" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="B36" s="59"/>
-      <c r="C36" s="68"/>
-      <c r="D36" s="69"/>
-      <c r="E36" s="69"/>
-      <c r="F36" s="69"/>
-      <c r="G36" s="70"/>
-      <c r="H36" s="68"/>
-      <c r="I36" s="69"/>
-      <c r="J36" s="69"/>
-      <c r="K36" s="70"/>
+      <c r="B36" s="71"/>
+      <c r="C36" s="76"/>
+      <c r="D36" s="77"/>
+      <c r="E36" s="77"/>
+      <c r="F36" s="77"/>
+      <c r="G36" s="78"/>
+      <c r="H36" s="76"/>
+      <c r="I36" s="77"/>
+      <c r="J36" s="77"/>
+      <c r="K36" s="78"/>
       <c r="M36" s="34"/>
       <c r="N36" s="47" t="s">
         <v>84</v>
@@ -2373,19 +2433,19 @@
       <c r="S36" s="47"/>
     </row>
     <row r="37" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A37" s="58" t="s">
+      <c r="A37" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="B37" s="59"/>
-      <c r="C37" s="68"/>
-      <c r="D37" s="69"/>
-      <c r="E37" s="69"/>
-      <c r="F37" s="69"/>
-      <c r="G37" s="70"/>
-      <c r="H37" s="68"/>
-      <c r="I37" s="69"/>
-      <c r="J37" s="69"/>
-      <c r="K37" s="70"/>
+      <c r="B37" s="71"/>
+      <c r="C37" s="76"/>
+      <c r="D37" s="77"/>
+      <c r="E37" s="77"/>
+      <c r="F37" s="77"/>
+      <c r="G37" s="78"/>
+      <c r="H37" s="76"/>
+      <c r="I37" s="77"/>
+      <c r="J37" s="77"/>
+      <c r="K37" s="78"/>
       <c r="M37" s="34"/>
     </row>
     <row r="38" spans="1:19" ht="15.75" thickBot="1">
@@ -2399,23 +2459,23 @@
       <c r="S38" s="47"/>
     </row>
     <row r="39" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A39" s="51" t="s">
+      <c r="A39" s="91" t="s">
         <v>27</v>
       </c>
-      <c r="B39" s="52"/>
-      <c r="C39" s="52"/>
-      <c r="D39" s="52"/>
-      <c r="E39" s="53"/>
+      <c r="B39" s="92"/>
+      <c r="C39" s="92"/>
+      <c r="D39" s="92"/>
+      <c r="E39" s="93"/>
     </row>
     <row r="40" spans="1:19">
       <c r="A40" s="14" t="s">
         <v>26</v>
       </c>
       <c r="B40" s="13"/>
-      <c r="C40" s="54" t="s">
+      <c r="C40" s="94" t="s">
         <v>23</v>
       </c>
-      <c r="D40" s="55"/>
+      <c r="D40" s="95"/>
       <c r="E40" s="28"/>
     </row>
     <row r="41" spans="1:19">
@@ -2423,10 +2483,10 @@
         <v>22</v>
       </c>
       <c r="B41" s="5"/>
-      <c r="C41" s="54" t="s">
+      <c r="C41" s="94" t="s">
         <v>24</v>
       </c>
-      <c r="D41" s="55"/>
+      <c r="D41" s="95"/>
       <c r="E41" s="8"/>
     </row>
     <row r="42" spans="1:19">
@@ -2434,154 +2494,154 @@
         <v>25</v>
       </c>
       <c r="B42" s="6"/>
-      <c r="C42" s="60" t="s">
+      <c r="C42" s="82" t="s">
         <v>66</v>
       </c>
-      <c r="D42" s="61"/>
+      <c r="D42" s="83"/>
       <c r="E42" s="39"/>
     </row>
     <row r="43" spans="1:19" ht="15.75" thickBot="1"/>
     <row r="44" spans="1:19">
-      <c r="A44" s="56" t="s">
+      <c r="A44" s="96" t="s">
         <v>37</v>
       </c>
-      <c r="B44" s="57"/>
-      <c r="C44" s="57"/>
-      <c r="D44" s="57"/>
-      <c r="E44" s="57"/>
-      <c r="F44" s="57"/>
-      <c r="G44" s="57"/>
-      <c r="H44" s="57"/>
-      <c r="I44" s="57"/>
-      <c r="J44" s="57"/>
-      <c r="K44" s="57"/>
-      <c r="L44" s="57"/>
+      <c r="B44" s="97"/>
+      <c r="C44" s="97"/>
+      <c r="D44" s="97"/>
+      <c r="E44" s="97"/>
+      <c r="F44" s="97"/>
+      <c r="G44" s="97"/>
+      <c r="H44" s="97"/>
+      <c r="I44" s="97"/>
+      <c r="J44" s="97"/>
+      <c r="K44" s="97"/>
+      <c r="L44" s="97"/>
     </row>
     <row r="45" spans="1:19">
       <c r="A45" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="B45" s="50" t="s">
+      <c r="B45" s="90" t="s">
         <v>57</v>
       </c>
-      <c r="C45" s="50"/>
-      <c r="D45" s="50"/>
-      <c r="E45" s="50"/>
-      <c r="F45" s="50"/>
-      <c r="G45" s="50"/>
-      <c r="H45" s="50"/>
-      <c r="I45" s="50"/>
-      <c r="J45" s="50"/>
-      <c r="K45" s="50"/>
-      <c r="L45" s="50"/>
+      <c r="C45" s="90"/>
+      <c r="D45" s="90"/>
+      <c r="E45" s="90"/>
+      <c r="F45" s="90"/>
+      <c r="G45" s="90"/>
+      <c r="H45" s="90"/>
+      <c r="I45" s="90"/>
+      <c r="J45" s="90"/>
+      <c r="K45" s="90"/>
+      <c r="L45" s="90"/>
     </row>
     <row r="46" spans="1:19" ht="15" customHeight="1">
       <c r="A46" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="B46" s="50" t="s">
+      <c r="B46" s="90" t="s">
         <v>58</v>
       </c>
-      <c r="C46" s="50"/>
-      <c r="D46" s="50"/>
-      <c r="E46" s="50"/>
-      <c r="F46" s="50"/>
-      <c r="G46" s="50"/>
-      <c r="H46" s="50"/>
-      <c r="I46" s="50"/>
-      <c r="J46" s="50"/>
-      <c r="K46" s="50"/>
-      <c r="L46" s="50"/>
+      <c r="C46" s="90"/>
+      <c r="D46" s="90"/>
+      <c r="E46" s="90"/>
+      <c r="F46" s="90"/>
+      <c r="G46" s="90"/>
+      <c r="H46" s="90"/>
+      <c r="I46" s="90"/>
+      <c r="J46" s="90"/>
+      <c r="K46" s="90"/>
+      <c r="L46" s="90"/>
     </row>
     <row r="47" spans="1:19">
       <c r="A47" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="B47" s="50" t="s">
+      <c r="B47" s="90" t="s">
         <v>59</v>
       </c>
-      <c r="C47" s="50"/>
-      <c r="D47" s="50"/>
-      <c r="E47" s="50"/>
-      <c r="F47" s="50"/>
-      <c r="G47" s="50"/>
-      <c r="H47" s="50"/>
-      <c r="I47" s="50"/>
-      <c r="J47" s="50"/>
-      <c r="K47" s="50"/>
-      <c r="L47" s="50"/>
+      <c r="C47" s="90"/>
+      <c r="D47" s="90"/>
+      <c r="E47" s="90"/>
+      <c r="F47" s="90"/>
+      <c r="G47" s="90"/>
+      <c r="H47" s="90"/>
+      <c r="I47" s="90"/>
+      <c r="J47" s="90"/>
+      <c r="K47" s="90"/>
+      <c r="L47" s="90"/>
     </row>
     <row r="48" spans="1:19">
       <c r="A48" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="B48" s="50" t="s">
+      <c r="B48" s="90" t="s">
         <v>46</v>
       </c>
-      <c r="C48" s="50"/>
-      <c r="D48" s="50"/>
-      <c r="E48" s="50"/>
-      <c r="F48" s="50"/>
-      <c r="G48" s="50"/>
-      <c r="H48" s="50"/>
-      <c r="I48" s="50"/>
-      <c r="J48" s="50"/>
-      <c r="K48" s="50"/>
-      <c r="L48" s="50"/>
+      <c r="C48" s="90"/>
+      <c r="D48" s="90"/>
+      <c r="E48" s="90"/>
+      <c r="F48" s="90"/>
+      <c r="G48" s="90"/>
+      <c r="H48" s="90"/>
+      <c r="I48" s="90"/>
+      <c r="J48" s="90"/>
+      <c r="K48" s="90"/>
+      <c r="L48" s="90"/>
     </row>
     <row r="49" spans="1:12">
       <c r="A49" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="B49" s="50" t="s">
+      <c r="B49" s="90" t="s">
         <v>35</v>
       </c>
-      <c r="C49" s="50"/>
-      <c r="D49" s="50"/>
-      <c r="E49" s="50"/>
-      <c r="F49" s="50"/>
-      <c r="G49" s="50"/>
-      <c r="H49" s="50"/>
-      <c r="I49" s="50"/>
-      <c r="J49" s="50"/>
-      <c r="K49" s="50"/>
-      <c r="L49" s="50"/>
+      <c r="C49" s="90"/>
+      <c r="D49" s="90"/>
+      <c r="E49" s="90"/>
+      <c r="F49" s="90"/>
+      <c r="G49" s="90"/>
+      <c r="H49" s="90"/>
+      <c r="I49" s="90"/>
+      <c r="J49" s="90"/>
+      <c r="K49" s="90"/>
+      <c r="L49" s="90"/>
     </row>
     <row r="50" spans="1:12">
       <c r="A50" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="B50" s="50" t="s">
+      <c r="B50" s="90" t="s">
         <v>56</v>
       </c>
-      <c r="C50" s="50"/>
-      <c r="D50" s="50"/>
-      <c r="E50" s="50"/>
-      <c r="F50" s="50"/>
-      <c r="G50" s="50"/>
-      <c r="H50" s="50"/>
-      <c r="I50" s="50"/>
-      <c r="J50" s="50"/>
-      <c r="K50" s="50"/>
-      <c r="L50" s="50"/>
+      <c r="C50" s="90"/>
+      <c r="D50" s="90"/>
+      <c r="E50" s="90"/>
+      <c r="F50" s="90"/>
+      <c r="G50" s="90"/>
+      <c r="H50" s="90"/>
+      <c r="I50" s="90"/>
+      <c r="J50" s="90"/>
+      <c r="K50" s="90"/>
+      <c r="L50" s="90"/>
     </row>
     <row r="51" spans="1:12">
       <c r="A51" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="B51" s="50" t="s">
+      <c r="B51" s="90" t="s">
         <v>55</v>
       </c>
-      <c r="C51" s="50"/>
-      <c r="D51" s="50"/>
-      <c r="E51" s="50"/>
-      <c r="F51" s="50"/>
-      <c r="G51" s="50"/>
-      <c r="H51" s="50"/>
-      <c r="I51" s="50"/>
-      <c r="J51" s="50"/>
-      <c r="K51" s="50"/>
-      <c r="L51" s="50"/>
+      <c r="C51" s="90"/>
+      <c r="D51" s="90"/>
+      <c r="E51" s="90"/>
+      <c r="F51" s="90"/>
+      <c r="G51" s="90"/>
+      <c r="H51" s="90"/>
+      <c r="I51" s="90"/>
+      <c r="J51" s="90"/>
+      <c r="K51" s="90"/>
+      <c r="L51" s="90"/>
     </row>
     <row r="52" spans="1:12">
       <c r="C52" s="34"/>
@@ -2597,6 +2657,45 @@
     <sortCondition ref="A3"/>
   </sortState>
   <mergeCells count="55">
+    <mergeCell ref="N27:S27"/>
+    <mergeCell ref="N33:S33"/>
+    <mergeCell ref="N35:S35"/>
+    <mergeCell ref="N30:S30"/>
+    <mergeCell ref="N28:S28"/>
+    <mergeCell ref="N31:S31"/>
+    <mergeCell ref="B50:L50"/>
+    <mergeCell ref="B51:L51"/>
+    <mergeCell ref="A39:E39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="B45:L45"/>
+    <mergeCell ref="A44:L44"/>
+    <mergeCell ref="B46:L46"/>
+    <mergeCell ref="B47:L47"/>
+    <mergeCell ref="B48:L48"/>
+    <mergeCell ref="B49:L49"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="H33:K33"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="H35:K35"/>
+    <mergeCell ref="H36:K36"/>
+    <mergeCell ref="H37:K37"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="H30:K30"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="H32:K32"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="H31:L31"/>
     <mergeCell ref="N24:S24"/>
     <mergeCell ref="N38:S38"/>
     <mergeCell ref="N36:S36"/>
@@ -2613,45 +2712,6 @@
     <mergeCell ref="H3:K3"/>
     <mergeCell ref="C3:G3"/>
     <mergeCell ref="A28:B28"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="H30:K30"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="H32:K32"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="H31:L31"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="H33:K33"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="H35:K35"/>
-    <mergeCell ref="H36:K36"/>
-    <mergeCell ref="H37:K37"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="B50:L50"/>
-    <mergeCell ref="B51:L51"/>
-    <mergeCell ref="A39:E39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="B45:L45"/>
-    <mergeCell ref="A44:L44"/>
-    <mergeCell ref="B46:L46"/>
-    <mergeCell ref="B47:L47"/>
-    <mergeCell ref="B48:L48"/>
-    <mergeCell ref="B49:L49"/>
-    <mergeCell ref="N27:S27"/>
-    <mergeCell ref="N33:S33"/>
-    <mergeCell ref="N35:S35"/>
-    <mergeCell ref="N30:S30"/>
-    <mergeCell ref="N28:S28"/>
-    <mergeCell ref="N31:S31"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="Q4" r:id="rId1"/>

</xml_diff>

<commit_message>
Preparando entorno para despliegue en Firebase
</commit_message>
<xml_diff>
--- a/Cuadro-de-estado.xlsx
+++ b/Cuadro-de-estado.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="99">
   <si>
     <t>BACKEND</t>
   </si>
@@ -385,6 +385,18 @@
   </si>
   <si>
     <t>Dias faltantes</t>
+  </si>
+  <si>
+    <t>koyeb</t>
+  </si>
+  <si>
+    <t>clever-cloud</t>
+  </si>
+  <si>
+    <t>firebase</t>
+  </si>
+  <si>
+    <t>Upload file</t>
   </si>
 </sst>
 </file>
@@ -679,7 +691,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="33">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -1081,6 +1093,43 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -1092,7 +1141,7 @@
     </xf>
     <xf numFmtId="43" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1186,6 +1235,19 @@
     </xf>
     <xf numFmtId="0" fontId="23" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="13" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1229,13 +1291,22 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1345,16 +1416,6 @@
     <xf numFmtId="0" fontId="22" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="13" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1657,7 +1718,7 @@
   <dimension ref="A1:U54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="O14" sqref="O14:T15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1674,31 +1735,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="55" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
+      <c r="L1" s="55"/>
     </row>
     <row r="2" spans="1:21" ht="19.5" thickBot="1">
-      <c r="A2" s="101">
+      <c r="A2" s="48">
         <f ca="1">M2-TODAY()-1</f>
-        <v>49</v>
-      </c>
-      <c r="B2" s="102" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="49" t="s">
         <v>94</v>
       </c>
-      <c r="C2" s="103"/>
-      <c r="M2" s="100">
+      <c r="C2" s="50"/>
+      <c r="M2" s="47">
         <v>45011</v>
       </c>
       <c r="O2" s="46" t="s">
@@ -1706,30 +1767,30 @@
       </c>
     </row>
     <row r="3" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="56" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="52"/>
-      <c r="C3" s="53" t="s">
+      <c r="B3" s="57"/>
+      <c r="C3" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="54"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="55"/>
-      <c r="H3" s="53" t="s">
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="59"/>
+      <c r="G3" s="60"/>
+      <c r="H3" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="54"/>
-      <c r="J3" s="56"/>
-      <c r="K3" s="55"/>
+      <c r="I3" s="59"/>
+      <c r="J3" s="61"/>
+      <c r="K3" s="60"/>
       <c r="L3" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="58" t="s">
+      <c r="M3" s="63" t="s">
         <v>82</v>
       </c>
-      <c r="N3" s="49"/>
+      <c r="N3" s="54"/>
     </row>
     <row r="4" spans="1:21" s="3" customFormat="1" ht="40.5" customHeight="1" thickBot="1">
       <c r="A4" s="17" t="s">
@@ -1768,10 +1829,10 @@
       <c r="L4" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="M4" s="59" t="s">
+      <c r="M4" s="64" t="s">
         <v>83</v>
       </c>
-      <c r="N4" s="60"/>
+      <c r="N4" s="65"/>
       <c r="O4" s="36" t="s">
         <v>63</v>
       </c>
@@ -1813,15 +1874,15 @@
       <c r="M6" s="45" t="s">
         <v>85</v>
       </c>
-      <c r="O6" s="48" t="s">
+      <c r="O6" s="53" t="s">
         <v>67</v>
       </c>
-      <c r="P6" s="49"/>
-      <c r="Q6" s="49"/>
-      <c r="R6" s="49"/>
-      <c r="S6" s="49"/>
-      <c r="T6" s="49"/>
-      <c r="U6" s="49"/>
+      <c r="P6" s="54"/>
+      <c r="Q6" s="54"/>
+      <c r="R6" s="54"/>
+      <c r="S6" s="54"/>
+      <c r="T6" s="54"/>
+      <c r="U6" s="54"/>
     </row>
     <row r="7" spans="1:21" ht="4.5" customHeight="1">
       <c r="A7" s="29"/>
@@ -1960,6 +2021,9 @@
       <c r="J13" s="4"/>
       <c r="K13" s="7"/>
       <c r="L13" s="4"/>
+      <c r="O13" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="14" spans="1:21">
       <c r="A14" s="40" t="s">
@@ -1978,14 +2042,14 @@
       <c r="J14" s="4"/>
       <c r="K14" s="7"/>
       <c r="L14" s="4"/>
-      <c r="O14" s="57" t="s">
+      <c r="O14" s="62" t="s">
         <v>80</v>
       </c>
-      <c r="P14" s="57"/>
-      <c r="Q14" s="57"/>
-      <c r="R14" s="57"/>
-      <c r="S14" s="57"/>
-      <c r="T14" s="57"/>
+      <c r="P14" s="62"/>
+      <c r="Q14" s="62"/>
+      <c r="R14" s="62"/>
+      <c r="S14" s="62"/>
+      <c r="T14" s="62"/>
     </row>
     <row r="15" spans="1:21">
       <c r="A15" s="18" t="s">
@@ -2004,12 +2068,12 @@
       <c r="J15" s="4"/>
       <c r="K15" s="7"/>
       <c r="L15" s="4"/>
-      <c r="O15" s="57"/>
-      <c r="P15" s="57"/>
-      <c r="Q15" s="57"/>
-      <c r="R15" s="57"/>
-      <c r="S15" s="57"/>
-      <c r="T15" s="57"/>
+      <c r="O15" s="62"/>
+      <c r="P15" s="62"/>
+      <c r="Q15" s="62"/>
+      <c r="R15" s="62"/>
+      <c r="S15" s="62"/>
+      <c r="T15" s="62"/>
     </row>
     <row r="16" spans="1:21">
       <c r="A16" s="40" t="s">
@@ -2168,14 +2232,14 @@
       <c r="J24" s="4"/>
       <c r="K24" s="7"/>
       <c r="L24" s="4"/>
-      <c r="N24" s="47" t="s">
+      <c r="N24" s="52" t="s">
         <v>92</v>
       </c>
-      <c r="O24" s="47"/>
-      <c r="P24" s="47"/>
-      <c r="Q24" s="47"/>
-      <c r="R24" s="47"/>
-      <c r="S24" s="47"/>
+      <c r="O24" s="52"/>
+      <c r="P24" s="52"/>
+      <c r="Q24" s="52"/>
+      <c r="R24" s="52"/>
+      <c r="S24" s="52"/>
     </row>
     <row r="25" spans="1:19">
       <c r="A25" s="41" t="s">
@@ -2212,54 +2276,60 @@
     <row r="27" spans="1:19" ht="15.75" thickBot="1">
       <c r="A27" s="24"/>
       <c r="B27" s="26"/>
-      <c r="C27" s="53" t="s">
+      <c r="C27" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="54"/>
-      <c r="E27" s="54"/>
-      <c r="F27" s="54"/>
-      <c r="G27" s="55"/>
-      <c r="H27" s="53" t="s">
+      <c r="D27" s="59"/>
+      <c r="E27" s="59"/>
+      <c r="F27" s="59"/>
+      <c r="G27" s="60"/>
+      <c r="H27" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="I27" s="54"/>
-      <c r="J27" s="56"/>
-      <c r="K27" s="55"/>
+      <c r="I27" s="59"/>
+      <c r="J27" s="61"/>
+      <c r="K27" s="60"/>
       <c r="L27" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="N27" s="47" t="s">
+      <c r="N27" s="52" t="s">
         <v>90</v>
       </c>
-      <c r="O27" s="47"/>
-      <c r="P27" s="47"/>
-      <c r="Q27" s="47"/>
-      <c r="R27" s="47"/>
-      <c r="S27" s="47"/>
-    </row>
-    <row r="28" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A28" s="64" t="s">
+      <c r="O27" s="52"/>
+      <c r="P27" s="52"/>
+      <c r="Q27" s="52"/>
+      <c r="R27" s="52"/>
+      <c r="S27" s="52"/>
+    </row>
+    <row r="28" spans="1:19" ht="30.75" thickBot="1">
+      <c r="A28" s="72" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="65"/>
-      <c r="C28" s="61"/>
-      <c r="D28" s="62"/>
-      <c r="E28" s="62"/>
-      <c r="F28" s="62"/>
-      <c r="G28" s="63"/>
-      <c r="H28" s="61"/>
-      <c r="I28" s="62"/>
-      <c r="J28" s="62"/>
-      <c r="K28" s="63"/>
-      <c r="L28" s="4"/>
-      <c r="N28" s="99" t="s">
+      <c r="B28" s="73"/>
+      <c r="C28" s="66" t="s">
+        <v>97</v>
+      </c>
+      <c r="D28" s="67"/>
+      <c r="E28" s="67"/>
+      <c r="F28" s="67"/>
+      <c r="G28" s="68"/>
+      <c r="H28" s="69" t="s">
+        <v>95</v>
+      </c>
+      <c r="I28" s="70"/>
+      <c r="J28" s="70"/>
+      <c r="K28" s="71"/>
+      <c r="L28" s="51" t="s">
+        <v>96</v>
+      </c>
+      <c r="N28" s="107" t="s">
         <v>89</v>
       </c>
-      <c r="O28" s="99"/>
-      <c r="P28" s="99"/>
-      <c r="Q28" s="99"/>
-      <c r="R28" s="99"/>
-      <c r="S28" s="99"/>
+      <c r="O28" s="107"/>
+      <c r="P28" s="107"/>
+      <c r="Q28" s="107"/>
+      <c r="R28" s="107"/>
+      <c r="S28" s="107"/>
     </row>
     <row r="29" spans="1:19" ht="4.5" customHeight="1">
       <c r="A29" s="29"/>
@@ -2276,100 +2346,100 @@
       <c r="L29" s="31"/>
     </row>
     <row r="30" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A30" s="70" t="s">
+      <c r="A30" s="78" t="s">
         <v>40</v>
       </c>
-      <c r="B30" s="71"/>
-      <c r="C30" s="66"/>
-      <c r="D30" s="67"/>
-      <c r="E30" s="67"/>
-      <c r="F30" s="67"/>
-      <c r="G30" s="68"/>
-      <c r="H30" s="69"/>
-      <c r="I30" s="67"/>
-      <c r="J30" s="67"/>
-      <c r="K30" s="68"/>
+      <c r="B30" s="79"/>
+      <c r="C30" s="74"/>
+      <c r="D30" s="75"/>
+      <c r="E30" s="75"/>
+      <c r="F30" s="75"/>
+      <c r="G30" s="76"/>
+      <c r="H30" s="77"/>
+      <c r="I30" s="75"/>
+      <c r="J30" s="75"/>
+      <c r="K30" s="76"/>
       <c r="L30" s="22" t="s">
         <v>5</v>
       </c>
       <c r="M30" s="34"/>
-      <c r="N30" s="99" t="s">
+      <c r="N30" s="107" t="s">
         <v>81</v>
       </c>
-      <c r="O30" s="99"/>
-      <c r="P30" s="99"/>
-      <c r="Q30" s="99"/>
-      <c r="R30" s="99"/>
-      <c r="S30" s="99"/>
+      <c r="O30" s="107"/>
+      <c r="P30" s="107"/>
+      <c r="Q30" s="107"/>
+      <c r="R30" s="107"/>
+      <c r="S30" s="107"/>
     </row>
     <row r="31" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A31" s="70" t="s">
+      <c r="A31" s="78" t="s">
         <v>86</v>
       </c>
-      <c r="B31" s="71"/>
-      <c r="C31" s="76"/>
-      <c r="D31" s="77"/>
-      <c r="E31" s="77"/>
-      <c r="F31" s="77"/>
-      <c r="G31" s="78"/>
-      <c r="H31" s="79" t="s">
+      <c r="B31" s="79"/>
+      <c r="C31" s="84"/>
+      <c r="D31" s="85"/>
+      <c r="E31" s="85"/>
+      <c r="F31" s="85"/>
+      <c r="G31" s="86"/>
+      <c r="H31" s="87" t="s">
         <v>87</v>
       </c>
-      <c r="I31" s="80"/>
-      <c r="J31" s="80"/>
-      <c r="K31" s="80"/>
-      <c r="L31" s="81"/>
+      <c r="I31" s="88"/>
+      <c r="J31" s="88"/>
+      <c r="K31" s="88"/>
+      <c r="L31" s="89"/>
       <c r="M31" s="34"/>
-      <c r="N31" s="99" t="s">
+      <c r="N31" s="107" t="s">
         <v>77</v>
       </c>
-      <c r="O31" s="99"/>
-      <c r="P31" s="99"/>
-      <c r="Q31" s="99"/>
-      <c r="R31" s="99"/>
-      <c r="S31" s="99"/>
+      <c r="O31" s="107"/>
+      <c r="P31" s="107"/>
+      <c r="Q31" s="107"/>
+      <c r="R31" s="107"/>
+      <c r="S31" s="107"/>
     </row>
     <row r="32" spans="1:19" ht="16.5" thickBot="1">
-      <c r="A32" s="74" t="s">
+      <c r="A32" s="82" t="s">
         <v>61</v>
       </c>
-      <c r="B32" s="75"/>
-      <c r="C32" s="66"/>
-      <c r="D32" s="67"/>
-      <c r="E32" s="67"/>
-      <c r="F32" s="67"/>
-      <c r="G32" s="68"/>
-      <c r="H32" s="69"/>
-      <c r="I32" s="67"/>
-      <c r="J32" s="67"/>
-      <c r="K32" s="68"/>
+      <c r="B32" s="83"/>
+      <c r="C32" s="74"/>
+      <c r="D32" s="75"/>
+      <c r="E32" s="75"/>
+      <c r="F32" s="75"/>
+      <c r="G32" s="76"/>
+      <c r="H32" s="77"/>
+      <c r="I32" s="75"/>
+      <c r="J32" s="75"/>
+      <c r="K32" s="76"/>
       <c r="M32" s="34"/>
     </row>
     <row r="33" spans="1:19" ht="30.75" customHeight="1" thickBot="1">
-      <c r="A33" s="72" t="s">
+      <c r="A33" s="80" t="s">
         <v>36</v>
       </c>
-      <c r="B33" s="73"/>
-      <c r="C33" s="87" t="s">
+      <c r="B33" s="81"/>
+      <c r="C33" s="95" t="s">
         <v>60</v>
       </c>
-      <c r="D33" s="88"/>
-      <c r="E33" s="88"/>
-      <c r="F33" s="88"/>
-      <c r="G33" s="89"/>
-      <c r="H33" s="84"/>
-      <c r="I33" s="85"/>
-      <c r="J33" s="85"/>
-      <c r="K33" s="86"/>
+      <c r="D33" s="96"/>
+      <c r="E33" s="96"/>
+      <c r="F33" s="96"/>
+      <c r="G33" s="97"/>
+      <c r="H33" s="92"/>
+      <c r="I33" s="93"/>
+      <c r="J33" s="93"/>
+      <c r="K33" s="94"/>
       <c r="M33" s="34"/>
-      <c r="N33" s="98" t="s">
+      <c r="N33" s="106" t="s">
         <v>78</v>
       </c>
-      <c r="O33" s="98"/>
-      <c r="P33" s="98"/>
-      <c r="Q33" s="98"/>
-      <c r="R33" s="98"/>
-      <c r="S33" s="98"/>
+      <c r="O33" s="106"/>
+      <c r="P33" s="106"/>
+      <c r="Q33" s="106"/>
+      <c r="R33" s="106"/>
+      <c r="S33" s="106"/>
     </row>
     <row r="34" spans="1:19" ht="4.5" customHeight="1" thickBot="1">
       <c r="A34" s="29"/>
@@ -2385,97 +2455,97 @@
       <c r="K34" s="31"/>
     </row>
     <row r="35" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A35" s="70" t="s">
+      <c r="A35" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="B35" s="71"/>
-      <c r="C35" s="76"/>
-      <c r="D35" s="77"/>
-      <c r="E35" s="77"/>
-      <c r="F35" s="77"/>
-      <c r="G35" s="78"/>
-      <c r="H35" s="76"/>
-      <c r="I35" s="77"/>
-      <c r="J35" s="77"/>
-      <c r="K35" s="78"/>
+      <c r="B35" s="79"/>
+      <c r="C35" s="84"/>
+      <c r="D35" s="85"/>
+      <c r="E35" s="85"/>
+      <c r="F35" s="85"/>
+      <c r="G35" s="86"/>
+      <c r="H35" s="84"/>
+      <c r="I35" s="85"/>
+      <c r="J35" s="85"/>
+      <c r="K35" s="86"/>
       <c r="M35" s="34"/>
-      <c r="N35" s="99" t="s">
+      <c r="N35" s="107" t="s">
         <v>79</v>
       </c>
-      <c r="O35" s="99"/>
-      <c r="P35" s="99"/>
-      <c r="Q35" s="99"/>
-      <c r="R35" s="99"/>
-      <c r="S35" s="99"/>
+      <c r="O35" s="107"/>
+      <c r="P35" s="107"/>
+      <c r="Q35" s="107"/>
+      <c r="R35" s="107"/>
+      <c r="S35" s="107"/>
     </row>
     <row r="36" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A36" s="70" t="s">
+      <c r="A36" s="78" t="s">
         <v>6</v>
       </c>
-      <c r="B36" s="71"/>
-      <c r="C36" s="76"/>
-      <c r="D36" s="77"/>
-      <c r="E36" s="77"/>
-      <c r="F36" s="77"/>
-      <c r="G36" s="78"/>
-      <c r="H36" s="76"/>
-      <c r="I36" s="77"/>
-      <c r="J36" s="77"/>
-      <c r="K36" s="78"/>
+      <c r="B36" s="79"/>
+      <c r="C36" s="84"/>
+      <c r="D36" s="85"/>
+      <c r="E36" s="85"/>
+      <c r="F36" s="85"/>
+      <c r="G36" s="86"/>
+      <c r="H36" s="84"/>
+      <c r="I36" s="85"/>
+      <c r="J36" s="85"/>
+      <c r="K36" s="86"/>
       <c r="M36" s="34"/>
-      <c r="N36" s="47" t="s">
+      <c r="N36" s="52" t="s">
         <v>84</v>
       </c>
-      <c r="O36" s="47"/>
-      <c r="P36" s="47"/>
-      <c r="Q36" s="47"/>
-      <c r="R36" s="47"/>
-      <c r="S36" s="47"/>
+      <c r="O36" s="52"/>
+      <c r="P36" s="52"/>
+      <c r="Q36" s="52"/>
+      <c r="R36" s="52"/>
+      <c r="S36" s="52"/>
     </row>
     <row r="37" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A37" s="70" t="s">
+      <c r="A37" s="78" t="s">
         <v>8</v>
       </c>
-      <c r="B37" s="71"/>
-      <c r="C37" s="76"/>
-      <c r="D37" s="77"/>
-      <c r="E37" s="77"/>
-      <c r="F37" s="77"/>
-      <c r="G37" s="78"/>
-      <c r="H37" s="76"/>
-      <c r="I37" s="77"/>
-      <c r="J37" s="77"/>
-      <c r="K37" s="78"/>
+      <c r="B37" s="79"/>
+      <c r="C37" s="84"/>
+      <c r="D37" s="85"/>
+      <c r="E37" s="85"/>
+      <c r="F37" s="85"/>
+      <c r="G37" s="86"/>
+      <c r="H37" s="84"/>
+      <c r="I37" s="85"/>
+      <c r="J37" s="85"/>
+      <c r="K37" s="86"/>
       <c r="M37" s="34"/>
     </row>
     <row r="38" spans="1:19" ht="15.75" thickBot="1">
-      <c r="N38" s="47" t="s">
+      <c r="N38" s="52" t="s">
         <v>91</v>
       </c>
-      <c r="O38" s="47"/>
-      <c r="P38" s="47"/>
-      <c r="Q38" s="47"/>
-      <c r="R38" s="47"/>
-      <c r="S38" s="47"/>
+      <c r="O38" s="52"/>
+      <c r="P38" s="52"/>
+      <c r="Q38" s="52"/>
+      <c r="R38" s="52"/>
+      <c r="S38" s="52"/>
     </row>
     <row r="39" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A39" s="91" t="s">
+      <c r="A39" s="99" t="s">
         <v>27</v>
       </c>
-      <c r="B39" s="92"/>
-      <c r="C39" s="92"/>
-      <c r="D39" s="92"/>
-      <c r="E39" s="93"/>
+      <c r="B39" s="100"/>
+      <c r="C39" s="100"/>
+      <c r="D39" s="100"/>
+      <c r="E39" s="101"/>
     </row>
     <row r="40" spans="1:19">
       <c r="A40" s="14" t="s">
         <v>26</v>
       </c>
       <c r="B40" s="13"/>
-      <c r="C40" s="94" t="s">
+      <c r="C40" s="102" t="s">
         <v>23</v>
       </c>
-      <c r="D40" s="95"/>
+      <c r="D40" s="103"/>
       <c r="E40" s="28"/>
     </row>
     <row r="41" spans="1:19">
@@ -2483,10 +2553,10 @@
         <v>22</v>
       </c>
       <c r="B41" s="5"/>
-      <c r="C41" s="94" t="s">
+      <c r="C41" s="102" t="s">
         <v>24</v>
       </c>
-      <c r="D41" s="95"/>
+      <c r="D41" s="103"/>
       <c r="E41" s="8"/>
     </row>
     <row r="42" spans="1:19">
@@ -2494,154 +2564,154 @@
         <v>25</v>
       </c>
       <c r="B42" s="6"/>
-      <c r="C42" s="82" t="s">
+      <c r="C42" s="90" t="s">
         <v>66</v>
       </c>
-      <c r="D42" s="83"/>
+      <c r="D42" s="91"/>
       <c r="E42" s="39"/>
     </row>
     <row r="43" spans="1:19" ht="15.75" thickBot="1"/>
     <row r="44" spans="1:19">
-      <c r="A44" s="96" t="s">
+      <c r="A44" s="104" t="s">
         <v>37</v>
       </c>
-      <c r="B44" s="97"/>
-      <c r="C44" s="97"/>
-      <c r="D44" s="97"/>
-      <c r="E44" s="97"/>
-      <c r="F44" s="97"/>
-      <c r="G44" s="97"/>
-      <c r="H44" s="97"/>
-      <c r="I44" s="97"/>
-      <c r="J44" s="97"/>
-      <c r="K44" s="97"/>
-      <c r="L44" s="97"/>
+      <c r="B44" s="105"/>
+      <c r="C44" s="105"/>
+      <c r="D44" s="105"/>
+      <c r="E44" s="105"/>
+      <c r="F44" s="105"/>
+      <c r="G44" s="105"/>
+      <c r="H44" s="105"/>
+      <c r="I44" s="105"/>
+      <c r="J44" s="105"/>
+      <c r="K44" s="105"/>
+      <c r="L44" s="105"/>
     </row>
     <row r="45" spans="1:19">
       <c r="A45" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="B45" s="90" t="s">
+      <c r="B45" s="98" t="s">
         <v>57</v>
       </c>
-      <c r="C45" s="90"/>
-      <c r="D45" s="90"/>
-      <c r="E45" s="90"/>
-      <c r="F45" s="90"/>
-      <c r="G45" s="90"/>
-      <c r="H45" s="90"/>
-      <c r="I45" s="90"/>
-      <c r="J45" s="90"/>
-      <c r="K45" s="90"/>
-      <c r="L45" s="90"/>
+      <c r="C45" s="98"/>
+      <c r="D45" s="98"/>
+      <c r="E45" s="98"/>
+      <c r="F45" s="98"/>
+      <c r="G45" s="98"/>
+      <c r="H45" s="98"/>
+      <c r="I45" s="98"/>
+      <c r="J45" s="98"/>
+      <c r="K45" s="98"/>
+      <c r="L45" s="98"/>
     </row>
     <row r="46" spans="1:19" ht="15" customHeight="1">
       <c r="A46" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="B46" s="90" t="s">
+      <c r="B46" s="98" t="s">
         <v>58</v>
       </c>
-      <c r="C46" s="90"/>
-      <c r="D46" s="90"/>
-      <c r="E46" s="90"/>
-      <c r="F46" s="90"/>
-      <c r="G46" s="90"/>
-      <c r="H46" s="90"/>
-      <c r="I46" s="90"/>
-      <c r="J46" s="90"/>
-      <c r="K46" s="90"/>
-      <c r="L46" s="90"/>
+      <c r="C46" s="98"/>
+      <c r="D46" s="98"/>
+      <c r="E46" s="98"/>
+      <c r="F46" s="98"/>
+      <c r="G46" s="98"/>
+      <c r="H46" s="98"/>
+      <c r="I46" s="98"/>
+      <c r="J46" s="98"/>
+      <c r="K46" s="98"/>
+      <c r="L46" s="98"/>
     </row>
     <row r="47" spans="1:19">
       <c r="A47" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="B47" s="90" t="s">
+      <c r="B47" s="98" t="s">
         <v>59</v>
       </c>
-      <c r="C47" s="90"/>
-      <c r="D47" s="90"/>
-      <c r="E47" s="90"/>
-      <c r="F47" s="90"/>
-      <c r="G47" s="90"/>
-      <c r="H47" s="90"/>
-      <c r="I47" s="90"/>
-      <c r="J47" s="90"/>
-      <c r="K47" s="90"/>
-      <c r="L47" s="90"/>
+      <c r="C47" s="98"/>
+      <c r="D47" s="98"/>
+      <c r="E47" s="98"/>
+      <c r="F47" s="98"/>
+      <c r="G47" s="98"/>
+      <c r="H47" s="98"/>
+      <c r="I47" s="98"/>
+      <c r="J47" s="98"/>
+      <c r="K47" s="98"/>
+      <c r="L47" s="98"/>
     </row>
     <row r="48" spans="1:19">
       <c r="A48" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="B48" s="90" t="s">
+      <c r="B48" s="98" t="s">
         <v>46</v>
       </c>
-      <c r="C48" s="90"/>
-      <c r="D48" s="90"/>
-      <c r="E48" s="90"/>
-      <c r="F48" s="90"/>
-      <c r="G48" s="90"/>
-      <c r="H48" s="90"/>
-      <c r="I48" s="90"/>
-      <c r="J48" s="90"/>
-      <c r="K48" s="90"/>
-      <c r="L48" s="90"/>
+      <c r="C48" s="98"/>
+      <c r="D48" s="98"/>
+      <c r="E48" s="98"/>
+      <c r="F48" s="98"/>
+      <c r="G48" s="98"/>
+      <c r="H48" s="98"/>
+      <c r="I48" s="98"/>
+      <c r="J48" s="98"/>
+      <c r="K48" s="98"/>
+      <c r="L48" s="98"/>
     </row>
     <row r="49" spans="1:12">
       <c r="A49" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="B49" s="90" t="s">
+      <c r="B49" s="98" t="s">
         <v>35</v>
       </c>
-      <c r="C49" s="90"/>
-      <c r="D49" s="90"/>
-      <c r="E49" s="90"/>
-      <c r="F49" s="90"/>
-      <c r="G49" s="90"/>
-      <c r="H49" s="90"/>
-      <c r="I49" s="90"/>
-      <c r="J49" s="90"/>
-      <c r="K49" s="90"/>
-      <c r="L49" s="90"/>
+      <c r="C49" s="98"/>
+      <c r="D49" s="98"/>
+      <c r="E49" s="98"/>
+      <c r="F49" s="98"/>
+      <c r="G49" s="98"/>
+      <c r="H49" s="98"/>
+      <c r="I49" s="98"/>
+      <c r="J49" s="98"/>
+      <c r="K49" s="98"/>
+      <c r="L49" s="98"/>
     </row>
     <row r="50" spans="1:12">
       <c r="A50" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="B50" s="90" t="s">
+      <c r="B50" s="98" t="s">
         <v>56</v>
       </c>
-      <c r="C50" s="90"/>
-      <c r="D50" s="90"/>
-      <c r="E50" s="90"/>
-      <c r="F50" s="90"/>
-      <c r="G50" s="90"/>
-      <c r="H50" s="90"/>
-      <c r="I50" s="90"/>
-      <c r="J50" s="90"/>
-      <c r="K50" s="90"/>
-      <c r="L50" s="90"/>
+      <c r="C50" s="98"/>
+      <c r="D50" s="98"/>
+      <c r="E50" s="98"/>
+      <c r="F50" s="98"/>
+      <c r="G50" s="98"/>
+      <c r="H50" s="98"/>
+      <c r="I50" s="98"/>
+      <c r="J50" s="98"/>
+      <c r="K50" s="98"/>
+      <c r="L50" s="98"/>
     </row>
     <row r="51" spans="1:12">
       <c r="A51" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="B51" s="90" t="s">
+      <c r="B51" s="98" t="s">
         <v>55</v>
       </c>
-      <c r="C51" s="90"/>
-      <c r="D51" s="90"/>
-      <c r="E51" s="90"/>
-      <c r="F51" s="90"/>
-      <c r="G51" s="90"/>
-      <c r="H51" s="90"/>
-      <c r="I51" s="90"/>
-      <c r="J51" s="90"/>
-      <c r="K51" s="90"/>
-      <c r="L51" s="90"/>
+      <c r="C51" s="98"/>
+      <c r="D51" s="98"/>
+      <c r="E51" s="98"/>
+      <c r="F51" s="98"/>
+      <c r="G51" s="98"/>
+      <c r="H51" s="98"/>
+      <c r="I51" s="98"/>
+      <c r="J51" s="98"/>
+      <c r="K51" s="98"/>
+      <c r="L51" s="98"/>
     </row>
     <row r="52" spans="1:12">
       <c r="C52" s="34"/>

</xml_diff>

<commit_message>
configuraciones para despliegue en firebase, nuevo paquete de distribucion, configuracion de variable de entorno prod/dev para el builder y el run dev
</commit_message>
<xml_diff>
--- a/Cuadro-de-estado.xlsx
+++ b/Cuadro-de-estado.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="110">
   <si>
     <t>BACKEND</t>
   </si>
@@ -34,9 +34,6 @@
   </si>
   <si>
     <t>DER</t>
-  </si>
-  <si>
-    <t>LOGGIN</t>
   </si>
   <si>
     <t>TOKEN</t>
@@ -397,6 +394,42 @@
   </si>
   <si>
     <t>Upload file</t>
+  </si>
+  <si>
+    <t>Las Card init, las está tomando del archivo .json</t>
+  </si>
+  <si>
+    <t>LOGIN</t>
+  </si>
+  <si>
+    <t>https://portfolio-frontend-wdr.web.app/</t>
+  </si>
+  <si>
+    <t>FrontEnd</t>
+  </si>
+  <si>
+    <t>BackEnd</t>
+  </si>
+  <si>
+    <t>https://yoprogramo-waldrom68.koyeb.app</t>
+  </si>
+  <si>
+    <t>https://api.clever-cloud.com/v2/session/login</t>
+  </si>
+  <si>
+    <t>Montreal Canada</t>
+  </si>
+  <si>
+    <t>https://www.koyeb.com/</t>
+  </si>
+  <si>
+    <t>Frankfurt Alemania</t>
+  </si>
+  <si>
+    <t>https://firebase.google.com</t>
+  </si>
+  <si>
+    <t>US-central</t>
   </si>
 </sst>
 </file>
@@ -691,7 +724,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="36">
+  <borders count="37">
     <border>
       <left/>
       <right/>
@@ -1122,6 +1155,19 @@
     <border>
       <left/>
       <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="medium">
@@ -1141,7 +1187,7 @@
     </xf>
     <xf numFmtId="43" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1251,6 +1297,90 @@
     <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1290,15 +1420,6 @@
     <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1314,107 +1435,33 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1717,8 +1764,8 @@
   </sheetPr>
   <dimension ref="A1:U54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14:T15"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="N54" sqref="N54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1735,20 +1782,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25">
-      <c r="A1" s="55" t="s">
-        <v>93</v>
-      </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="55"/>
-      <c r="K1" s="55"/>
-      <c r="L1" s="55"/>
+      <c r="A1" s="83" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" s="83"/>
+      <c r="C1" s="83"/>
+      <c r="D1" s="83"/>
+      <c r="E1" s="83"/>
+      <c r="F1" s="83"/>
+      <c r="G1" s="83"/>
+      <c r="H1" s="83"/>
+      <c r="I1" s="83"/>
+      <c r="J1" s="83"/>
+      <c r="K1" s="83"/>
+      <c r="L1" s="83"/>
     </row>
     <row r="2" spans="1:21" ht="19.5" thickBot="1">
       <c r="A2" s="48">
@@ -1756,88 +1803,88 @@
         <v>43</v>
       </c>
       <c r="B2" s="49" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C2" s="50"/>
       <c r="M2" s="47">
         <v>45011</v>
       </c>
       <c r="O2" s="46" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="56" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" s="57"/>
-      <c r="C3" s="58" t="s">
+      <c r="A3" s="84" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="85"/>
+      <c r="C3" s="86" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="59"/>
-      <c r="E3" s="59"/>
-      <c r="F3" s="59"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="58" t="s">
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="88"/>
+      <c r="H3" s="86" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="59"/>
-      <c r="J3" s="61"/>
-      <c r="K3" s="60"/>
+      <c r="I3" s="87"/>
+      <c r="J3" s="89"/>
+      <c r="K3" s="88"/>
       <c r="L3" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="63" t="s">
-        <v>82</v>
-      </c>
-      <c r="N3" s="54"/>
+      <c r="M3" s="91" t="s">
+        <v>81</v>
+      </c>
+      <c r="N3" s="82"/>
     </row>
     <row r="4" spans="1:21" s="3" customFormat="1" ht="40.5" customHeight="1" thickBot="1">
       <c r="A4" s="17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>3</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H4" s="9" t="s">
         <v>1</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J4" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K4" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L4" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="M4" s="64" t="s">
-        <v>83</v>
-      </c>
-      <c r="N4" s="65"/>
+        <v>27</v>
+      </c>
+      <c r="M4" s="92" t="s">
+        <v>82</v>
+      </c>
+      <c r="N4" s="93"/>
       <c r="O4" s="36" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q4" s="37" t="s">
         <v>63</v>
-      </c>
-      <c r="Q4" s="37" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="4.5" customHeight="1">
@@ -1856,10 +1903,10 @@
     </row>
     <row r="6" spans="1:21">
       <c r="A6" s="18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
@@ -1872,17 +1919,17 @@
       <c r="K6" s="5"/>
       <c r="L6" s="4"/>
       <c r="M6" s="45" t="s">
-        <v>85</v>
-      </c>
-      <c r="O6" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="P6" s="54"/>
-      <c r="Q6" s="54"/>
-      <c r="R6" s="54"/>
-      <c r="S6" s="54"/>
-      <c r="T6" s="54"/>
-      <c r="U6" s="54"/>
+        <v>84</v>
+      </c>
+      <c r="O6" s="81" t="s">
+        <v>66</v>
+      </c>
+      <c r="P6" s="82"/>
+      <c r="Q6" s="82"/>
+      <c r="R6" s="82"/>
+      <c r="S6" s="82"/>
+      <c r="T6" s="82"/>
+      <c r="U6" s="82"/>
     </row>
     <row r="7" spans="1:21" ht="4.5" customHeight="1">
       <c r="A7" s="29"/>
@@ -1900,10 +1947,10 @@
     </row>
     <row r="8" spans="1:21">
       <c r="A8" s="18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="13"/>
@@ -1916,10 +1963,10 @@
       <c r="K8" s="7"/>
       <c r="L8" s="4"/>
       <c r="O8" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="P8" s="6" t="s">
         <v>68</v>
-      </c>
-      <c r="P8" s="6" t="s">
-        <v>69</v>
       </c>
       <c r="Q8" s="6"/>
       <c r="R8" s="6"/>
@@ -1928,10 +1975,10 @@
     </row>
     <row r="9" spans="1:21">
       <c r="A9" s="27" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
@@ -1944,16 +1991,16 @@
       <c r="K9" s="28"/>
       <c r="L9" s="4"/>
       <c r="P9" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="Q9" s="6"/>
     </row>
     <row r="10" spans="1:21">
       <c r="A10" s="18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" s="13"/>
       <c r="D10" s="13"/>
@@ -1968,10 +2015,10 @@
     </row>
     <row r="11" spans="1:21">
       <c r="A11" s="18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
@@ -1984,10 +2031,10 @@
       <c r="K11" s="7"/>
       <c r="L11" s="4"/>
       <c r="O11" t="s">
+        <v>69</v>
+      </c>
+      <c r="P11" t="s">
         <v>70</v>
-      </c>
-      <c r="P11" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="4.5" customHeight="1">
@@ -2006,10 +2053,10 @@
     </row>
     <row r="13" spans="1:21">
       <c r="A13" s="40" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="42"/>
@@ -2022,15 +2069,15 @@
       <c r="K13" s="7"/>
       <c r="L13" s="4"/>
       <c r="O13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:21">
       <c r="A14" s="40" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="42"/>
@@ -2042,21 +2089,21 @@
       <c r="J14" s="4"/>
       <c r="K14" s="7"/>
       <c r="L14" s="4"/>
-      <c r="O14" s="62" t="s">
-        <v>80</v>
-      </c>
-      <c r="P14" s="62"/>
-      <c r="Q14" s="62"/>
-      <c r="R14" s="62"/>
-      <c r="S14" s="62"/>
-      <c r="T14" s="62"/>
+      <c r="O14" s="90" t="s">
+        <v>79</v>
+      </c>
+      <c r="P14" s="90"/>
+      <c r="Q14" s="90"/>
+      <c r="R14" s="90"/>
+      <c r="S14" s="90"/>
+      <c r="T14" s="90"/>
     </row>
     <row r="15" spans="1:21">
       <c r="A15" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
@@ -2068,19 +2115,19 @@
       <c r="J15" s="4"/>
       <c r="K15" s="7"/>
       <c r="L15" s="4"/>
-      <c r="O15" s="62"/>
-      <c r="P15" s="62"/>
-      <c r="Q15" s="62"/>
-      <c r="R15" s="62"/>
-      <c r="S15" s="62"/>
-      <c r="T15" s="62"/>
+      <c r="O15" s="90"/>
+      <c r="P15" s="90"/>
+      <c r="Q15" s="90"/>
+      <c r="R15" s="90"/>
+      <c r="S15" s="90"/>
+      <c r="T15" s="90"/>
     </row>
     <row r="16" spans="1:21">
       <c r="A16" s="40" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="42"/>
@@ -2093,18 +2140,18 @@
       <c r="K16" s="7"/>
       <c r="L16" s="4"/>
       <c r="O16" t="s">
+        <v>71</v>
+      </c>
+      <c r="P16" t="s">
         <v>72</v>
-      </c>
-      <c r="P16" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:19">
       <c r="A17" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="43"/>
@@ -2117,7 +2164,7 @@
       <c r="K17" s="7"/>
       <c r="L17" s="4"/>
       <c r="O17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:19" ht="4.5" customHeight="1">
@@ -2136,10 +2183,10 @@
     </row>
     <row r="19" spans="1:19">
       <c r="A19" s="41" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B19" s="25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C19" s="16"/>
       <c r="D19" s="44"/>
@@ -2152,15 +2199,15 @@
       <c r="K19" s="7"/>
       <c r="L19" s="32"/>
       <c r="O19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:19">
       <c r="A20" s="41" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C20" s="16"/>
       <c r="D20" s="44"/>
@@ -2189,7 +2236,7 @@
     </row>
     <row r="22" spans="1:19">
       <c r="A22" s="41" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B22" s="20"/>
       <c r="C22" s="16"/>
@@ -2219,7 +2266,7 @@
     </row>
     <row r="24" spans="1:19">
       <c r="A24" s="41" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B24" s="33"/>
       <c r="C24" s="8"/>
@@ -2233,7 +2280,7 @@
       <c r="K24" s="7"/>
       <c r="L24" s="4"/>
       <c r="N24" s="52" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="O24" s="52"/>
       <c r="P24" s="52"/>
@@ -2243,10 +2290,10 @@
     </row>
     <row r="25" spans="1:19">
       <c r="A25" s="41" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B25" s="25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C25" s="23"/>
       <c r="D25" s="8"/>
@@ -2276,24 +2323,24 @@
     <row r="27" spans="1:19" ht="15.75" thickBot="1">
       <c r="A27" s="24"/>
       <c r="B27" s="26"/>
-      <c r="C27" s="58" t="s">
+      <c r="C27" s="86" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="59"/>
-      <c r="E27" s="59"/>
-      <c r="F27" s="59"/>
-      <c r="G27" s="60"/>
-      <c r="H27" s="58" t="s">
+      <c r="D27" s="87"/>
+      <c r="E27" s="87"/>
+      <c r="F27" s="87"/>
+      <c r="G27" s="88"/>
+      <c r="H27" s="86" t="s">
         <v>0</v>
       </c>
-      <c r="I27" s="59"/>
-      <c r="J27" s="61"/>
-      <c r="K27" s="60"/>
+      <c r="I27" s="87"/>
+      <c r="J27" s="89"/>
+      <c r="K27" s="88"/>
       <c r="L27" s="21" t="s">
         <v>4</v>
       </c>
       <c r="N27" s="52" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="O27" s="52"/>
       <c r="P27" s="52"/>
@@ -2301,35 +2348,35 @@
       <c r="R27" s="52"/>
       <c r="S27" s="52"/>
     </row>
-    <row r="28" spans="1:19" ht="30.75" thickBot="1">
-      <c r="A28" s="72" t="s">
-        <v>31</v>
-      </c>
-      <c r="B28" s="73"/>
-      <c r="C28" s="66" t="s">
-        <v>97</v>
-      </c>
-      <c r="D28" s="67"/>
-      <c r="E28" s="67"/>
-      <c r="F28" s="67"/>
-      <c r="G28" s="68"/>
-      <c r="H28" s="69" t="s">
+    <row r="28" spans="1:19" ht="30">
+      <c r="A28" s="97" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="98"/>
+      <c r="C28" s="99" t="s">
+        <v>96</v>
+      </c>
+      <c r="D28" s="100"/>
+      <c r="E28" s="100"/>
+      <c r="F28" s="100"/>
+      <c r="G28" s="101"/>
+      <c r="H28" s="94" t="s">
+        <v>94</v>
+      </c>
+      <c r="I28" s="95"/>
+      <c r="J28" s="95"/>
+      <c r="K28" s="96"/>
+      <c r="L28" s="51" t="s">
         <v>95</v>
       </c>
-      <c r="I28" s="70"/>
-      <c r="J28" s="70"/>
-      <c r="K28" s="71"/>
-      <c r="L28" s="51" t="s">
-        <v>96</v>
-      </c>
-      <c r="N28" s="107" t="s">
-        <v>89</v>
-      </c>
-      <c r="O28" s="107"/>
-      <c r="P28" s="107"/>
-      <c r="Q28" s="107"/>
-      <c r="R28" s="107"/>
-      <c r="S28" s="107"/>
+      <c r="N28" s="54" t="s">
+        <v>88</v>
+      </c>
+      <c r="O28" s="54"/>
+      <c r="P28" s="54"/>
+      <c r="Q28" s="54"/>
+      <c r="R28" s="54"/>
+      <c r="S28" s="54"/>
     </row>
     <row r="29" spans="1:19" ht="4.5" customHeight="1">
       <c r="A29" s="29"/>
@@ -2346,10 +2393,10 @@
       <c r="L29" s="31"/>
     </row>
     <row r="30" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A30" s="78" t="s">
-        <v>40</v>
-      </c>
-      <c r="B30" s="79"/>
+      <c r="A30" s="103" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" s="104"/>
       <c r="C30" s="74"/>
       <c r="D30" s="75"/>
       <c r="E30" s="75"/>
@@ -2363,47 +2410,47 @@
         <v>5</v>
       </c>
       <c r="M30" s="34"/>
-      <c r="N30" s="107" t="s">
-        <v>81</v>
-      </c>
-      <c r="O30" s="107"/>
-      <c r="P30" s="107"/>
-      <c r="Q30" s="107"/>
-      <c r="R30" s="107"/>
-      <c r="S30" s="107"/>
+      <c r="N30" s="54" t="s">
+        <v>80</v>
+      </c>
+      <c r="O30" s="54"/>
+      <c r="P30" s="54"/>
+      <c r="Q30" s="54"/>
+      <c r="R30" s="54"/>
+      <c r="S30" s="54"/>
     </row>
     <row r="31" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A31" s="78" t="s">
+      <c r="A31" s="103" t="s">
+        <v>85</v>
+      </c>
+      <c r="B31" s="104"/>
+      <c r="C31" s="99"/>
+      <c r="D31" s="100"/>
+      <c r="E31" s="100"/>
+      <c r="F31" s="100"/>
+      <c r="G31" s="101"/>
+      <c r="H31" s="78" t="s">
         <v>86</v>
       </c>
-      <c r="B31" s="79"/>
-      <c r="C31" s="84"/>
-      <c r="D31" s="85"/>
-      <c r="E31" s="85"/>
-      <c r="F31" s="85"/>
-      <c r="G31" s="86"/>
-      <c r="H31" s="87" t="s">
-        <v>87</v>
-      </c>
-      <c r="I31" s="88"/>
-      <c r="J31" s="88"/>
-      <c r="K31" s="88"/>
-      <c r="L31" s="89"/>
+      <c r="I31" s="79"/>
+      <c r="J31" s="79"/>
+      <c r="K31" s="79"/>
+      <c r="L31" s="80"/>
       <c r="M31" s="34"/>
-      <c r="N31" s="107" t="s">
-        <v>77</v>
-      </c>
-      <c r="O31" s="107"/>
-      <c r="P31" s="107"/>
-      <c r="Q31" s="107"/>
-      <c r="R31" s="107"/>
-      <c r="S31" s="107"/>
+      <c r="N31" s="54" t="s">
+        <v>76</v>
+      </c>
+      <c r="O31" s="54"/>
+      <c r="P31" s="54"/>
+      <c r="Q31" s="54"/>
+      <c r="R31" s="54"/>
+      <c r="S31" s="54"/>
     </row>
     <row r="32" spans="1:19" ht="16.5" thickBot="1">
-      <c r="A32" s="82" t="s">
-        <v>61</v>
-      </c>
-      <c r="B32" s="83"/>
+      <c r="A32" s="105" t="s">
+        <v>60</v>
+      </c>
+      <c r="B32" s="106"/>
       <c r="C32" s="74"/>
       <c r="D32" s="75"/>
       <c r="E32" s="75"/>
@@ -2416,30 +2463,30 @@
       <c r="M32" s="34"/>
     </row>
     <row r="33" spans="1:19" ht="30.75" customHeight="1" thickBot="1">
-      <c r="A33" s="80" t="s">
-        <v>36</v>
-      </c>
-      <c r="B33" s="81"/>
-      <c r="C33" s="95" t="s">
-        <v>60</v>
-      </c>
-      <c r="D33" s="96"/>
-      <c r="E33" s="96"/>
-      <c r="F33" s="96"/>
-      <c r="G33" s="97"/>
-      <c r="H33" s="92"/>
-      <c r="I33" s="93"/>
-      <c r="J33" s="93"/>
-      <c r="K33" s="94"/>
+      <c r="A33" s="107" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33" s="108"/>
+      <c r="C33" s="68" t="s">
+        <v>59</v>
+      </c>
+      <c r="D33" s="69"/>
+      <c r="E33" s="69"/>
+      <c r="F33" s="69"/>
+      <c r="G33" s="70"/>
+      <c r="H33" s="65"/>
+      <c r="I33" s="66"/>
+      <c r="J33" s="66"/>
+      <c r="K33" s="67"/>
       <c r="M33" s="34"/>
-      <c r="N33" s="106" t="s">
-        <v>78</v>
-      </c>
-      <c r="O33" s="106"/>
-      <c r="P33" s="106"/>
-      <c r="Q33" s="106"/>
-      <c r="R33" s="106"/>
-      <c r="S33" s="106"/>
+      <c r="N33" s="53" t="s">
+        <v>77</v>
+      </c>
+      <c r="O33" s="53"/>
+      <c r="P33" s="53"/>
+      <c r="Q33" s="53"/>
+      <c r="R33" s="53"/>
+      <c r="S33" s="53"/>
     </row>
     <row r="34" spans="1:19" ht="4.5" customHeight="1" thickBot="1">
       <c r="A34" s="29"/>
@@ -2455,46 +2502,46 @@
       <c r="K34" s="31"/>
     </row>
     <row r="35" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A35" s="78" t="s">
-        <v>7</v>
-      </c>
-      <c r="B35" s="79"/>
-      <c r="C35" s="84"/>
-      <c r="D35" s="85"/>
-      <c r="E35" s="85"/>
-      <c r="F35" s="85"/>
-      <c r="G35" s="86"/>
-      <c r="H35" s="84"/>
-      <c r="I35" s="85"/>
-      <c r="J35" s="85"/>
-      <c r="K35" s="86"/>
+      <c r="A35" s="103" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="104"/>
+      <c r="C35" s="71"/>
+      <c r="D35" s="72"/>
+      <c r="E35" s="72"/>
+      <c r="F35" s="72"/>
+      <c r="G35" s="73"/>
+      <c r="H35" s="71"/>
+      <c r="I35" s="72"/>
+      <c r="J35" s="72"/>
+      <c r="K35" s="73"/>
       <c r="M35" s="34"/>
-      <c r="N35" s="107" t="s">
-        <v>79</v>
-      </c>
-      <c r="O35" s="107"/>
-      <c r="P35" s="107"/>
-      <c r="Q35" s="107"/>
-      <c r="R35" s="107"/>
-      <c r="S35" s="107"/>
+      <c r="N35" s="54" t="s">
+        <v>78</v>
+      </c>
+      <c r="O35" s="54"/>
+      <c r="P35" s="54"/>
+      <c r="Q35" s="54"/>
+      <c r="R35" s="54"/>
+      <c r="S35" s="54"/>
     </row>
     <row r="36" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A36" s="78" t="s">
-        <v>6</v>
-      </c>
-      <c r="B36" s="79"/>
-      <c r="C36" s="84"/>
-      <c r="D36" s="85"/>
-      <c r="E36" s="85"/>
-      <c r="F36" s="85"/>
-      <c r="G36" s="86"/>
-      <c r="H36" s="84"/>
-      <c r="I36" s="85"/>
-      <c r="J36" s="85"/>
-      <c r="K36" s="86"/>
+      <c r="A36" s="103" t="s">
+        <v>99</v>
+      </c>
+      <c r="B36" s="104"/>
+      <c r="C36" s="71"/>
+      <c r="D36" s="72"/>
+      <c r="E36" s="72"/>
+      <c r="F36" s="72"/>
+      <c r="G36" s="73"/>
+      <c r="H36" s="71"/>
+      <c r="I36" s="72"/>
+      <c r="J36" s="72"/>
+      <c r="K36" s="73"/>
       <c r="M36" s="34"/>
       <c r="N36" s="52" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O36" s="52"/>
       <c r="P36" s="52"/>
@@ -2503,24 +2550,24 @@
       <c r="S36" s="52"/>
     </row>
     <row r="37" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A37" s="78" t="s">
-        <v>8</v>
-      </c>
-      <c r="B37" s="79"/>
-      <c r="C37" s="84"/>
-      <c r="D37" s="85"/>
-      <c r="E37" s="85"/>
-      <c r="F37" s="85"/>
-      <c r="G37" s="86"/>
-      <c r="H37" s="84"/>
-      <c r="I37" s="85"/>
-      <c r="J37" s="85"/>
-      <c r="K37" s="86"/>
+      <c r="A37" s="103" t="s">
+        <v>7</v>
+      </c>
+      <c r="B37" s="104"/>
+      <c r="C37" s="71"/>
+      <c r="D37" s="72"/>
+      <c r="E37" s="72"/>
+      <c r="F37" s="72"/>
+      <c r="G37" s="73"/>
+      <c r="H37" s="71"/>
+      <c r="I37" s="72"/>
+      <c r="J37" s="72"/>
+      <c r="K37" s="73"/>
       <c r="M37" s="34"/>
     </row>
     <row r="38" spans="1:19" ht="15.75" thickBot="1">
       <c r="N38" s="52" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="O38" s="52"/>
       <c r="P38" s="52"/>
@@ -2529,197 +2576,234 @@
       <c r="S38" s="52"/>
     </row>
     <row r="39" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A39" s="99" t="s">
-        <v>27</v>
-      </c>
-      <c r="B39" s="100"/>
-      <c r="C39" s="100"/>
-      <c r="D39" s="100"/>
-      <c r="E39" s="101"/>
+      <c r="A39" s="56" t="s">
+        <v>26</v>
+      </c>
+      <c r="B39" s="57"/>
+      <c r="C39" s="57"/>
+      <c r="D39" s="57"/>
+      <c r="E39" s="58"/>
     </row>
     <row r="40" spans="1:19">
       <c r="A40" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B40" s="13"/>
-      <c r="C40" s="102" t="s">
-        <v>23</v>
-      </c>
-      <c r="D40" s="103"/>
+      <c r="C40" s="59" t="s">
+        <v>22</v>
+      </c>
+      <c r="D40" s="60"/>
       <c r="E40" s="28"/>
+      <c r="N40" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="41" spans="1:19">
       <c r="A41" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B41" s="5"/>
-      <c r="C41" s="102" t="s">
-        <v>24</v>
-      </c>
-      <c r="D41" s="103"/>
+      <c r="C41" s="59" t="s">
+        <v>23</v>
+      </c>
+      <c r="D41" s="60"/>
       <c r="E41" s="8"/>
     </row>
     <row r="42" spans="1:19">
       <c r="A42" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B42" s="6"/>
-      <c r="C42" s="90" t="s">
-        <v>66</v>
-      </c>
-      <c r="D42" s="91"/>
+      <c r="C42" s="63" t="s">
+        <v>65</v>
+      </c>
+      <c r="D42" s="64"/>
       <c r="E42" s="39"/>
     </row>
-    <row r="43" spans="1:19" ht="15.75" thickBot="1"/>
+    <row r="43" spans="1:19" ht="18" thickBot="1">
+      <c r="N43" s="102" t="s">
+        <v>4</v>
+      </c>
+      <c r="O43" s="46" t="s">
+        <v>104</v>
+      </c>
+    </row>
     <row r="44" spans="1:19">
-      <c r="A44" s="104" t="s">
-        <v>37</v>
-      </c>
-      <c r="B44" s="105"/>
-      <c r="C44" s="105"/>
-      <c r="D44" s="105"/>
-      <c r="E44" s="105"/>
-      <c r="F44" s="105"/>
-      <c r="G44" s="105"/>
-      <c r="H44" s="105"/>
-      <c r="I44" s="105"/>
-      <c r="J44" s="105"/>
-      <c r="K44" s="105"/>
-      <c r="L44" s="105"/>
+      <c r="A44" s="61" t="s">
+        <v>36</v>
+      </c>
+      <c r="B44" s="62"/>
+      <c r="C44" s="62"/>
+      <c r="D44" s="62"/>
+      <c r="E44" s="62"/>
+      <c r="F44" s="62"/>
+      <c r="G44" s="62"/>
+      <c r="H44" s="62"/>
+      <c r="I44" s="62"/>
+      <c r="J44" s="62"/>
+      <c r="K44" s="62"/>
+      <c r="L44" s="62"/>
+      <c r="O44" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="45" spans="1:19">
       <c r="A45" s="35" t="s">
-        <v>38</v>
-      </c>
-      <c r="B45" s="98" t="s">
-        <v>57</v>
-      </c>
-      <c r="C45" s="98"/>
-      <c r="D45" s="98"/>
-      <c r="E45" s="98"/>
-      <c r="F45" s="98"/>
-      <c r="G45" s="98"/>
-      <c r="H45" s="98"/>
-      <c r="I45" s="98"/>
-      <c r="J45" s="98"/>
-      <c r="K45" s="98"/>
-      <c r="L45" s="98"/>
+        <v>37</v>
+      </c>
+      <c r="B45" s="55" t="s">
+        <v>56</v>
+      </c>
+      <c r="C45" s="55"/>
+      <c r="D45" s="55"/>
+      <c r="E45" s="55"/>
+      <c r="F45" s="55"/>
+      <c r="G45" s="55"/>
+      <c r="H45" s="55"/>
+      <c r="I45" s="55"/>
+      <c r="J45" s="55"/>
+      <c r="K45" s="55"/>
+      <c r="L45" s="55"/>
     </row>
     <row r="46" spans="1:19" ht="15" customHeight="1">
       <c r="A46" s="35" t="s">
-        <v>32</v>
-      </c>
-      <c r="B46" s="98" t="s">
-        <v>58</v>
-      </c>
-      <c r="C46" s="98"/>
-      <c r="D46" s="98"/>
-      <c r="E46" s="98"/>
-      <c r="F46" s="98"/>
-      <c r="G46" s="98"/>
-      <c r="H46" s="98"/>
-      <c r="I46" s="98"/>
-      <c r="J46" s="98"/>
-      <c r="K46" s="98"/>
-      <c r="L46" s="98"/>
+        <v>31</v>
+      </c>
+      <c r="B46" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="C46" s="55"/>
+      <c r="D46" s="55"/>
+      <c r="E46" s="55"/>
+      <c r="F46" s="55"/>
+      <c r="G46" s="55"/>
+      <c r="H46" s="55"/>
+      <c r="I46" s="55"/>
+      <c r="J46" s="55"/>
+      <c r="K46" s="55"/>
+      <c r="L46" s="55"/>
+      <c r="N46" s="102" t="s">
+        <v>102</v>
+      </c>
+      <c r="O46" s="46" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="47" spans="1:19">
       <c r="A47" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="B47" s="98" t="s">
-        <v>59</v>
-      </c>
-      <c r="C47" s="98"/>
-      <c r="D47" s="98"/>
-      <c r="E47" s="98"/>
-      <c r="F47" s="98"/>
-      <c r="G47" s="98"/>
-      <c r="H47" s="98"/>
-      <c r="I47" s="98"/>
-      <c r="J47" s="98"/>
-      <c r="K47" s="98"/>
-      <c r="L47" s="98"/>
+        <v>32</v>
+      </c>
+      <c r="B47" s="55" t="s">
+        <v>58</v>
+      </c>
+      <c r="C47" s="55"/>
+      <c r="D47" s="55"/>
+      <c r="E47" s="55"/>
+      <c r="F47" s="55"/>
+      <c r="G47" s="55"/>
+      <c r="H47" s="55"/>
+      <c r="I47" s="55"/>
+      <c r="J47" s="55"/>
+      <c r="K47" s="55"/>
+      <c r="L47" s="55"/>
+      <c r="O47" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="48" spans="1:19">
       <c r="A48" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="B48" s="55" t="s">
+        <v>45</v>
+      </c>
+      <c r="C48" s="55"/>
+      <c r="D48" s="55"/>
+      <c r="E48" s="55"/>
+      <c r="F48" s="55"/>
+      <c r="G48" s="55"/>
+      <c r="H48" s="55"/>
+      <c r="I48" s="55"/>
+      <c r="J48" s="55"/>
+      <c r="K48" s="55"/>
+      <c r="L48" s="55"/>
+      <c r="O48" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15">
+      <c r="A49" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="B49" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="B48" s="98" t="s">
-        <v>46</v>
-      </c>
-      <c r="C48" s="98"/>
-      <c r="D48" s="98"/>
-      <c r="E48" s="98"/>
-      <c r="F48" s="98"/>
-      <c r="G48" s="98"/>
-      <c r="H48" s="98"/>
-      <c r="I48" s="98"/>
-      <c r="J48" s="98"/>
-      <c r="K48" s="98"/>
-      <c r="L48" s="98"/>
-    </row>
-    <row r="49" spans="1:12">
-      <c r="A49" s="35" t="s">
+      <c r="C49" s="55"/>
+      <c r="D49" s="55"/>
+      <c r="E49" s="55"/>
+      <c r="F49" s="55"/>
+      <c r="G49" s="55"/>
+      <c r="H49" s="55"/>
+      <c r="I49" s="55"/>
+      <c r="J49" s="55"/>
+      <c r="K49" s="55"/>
+      <c r="L49" s="55"/>
+    </row>
+    <row r="50" spans="1:15" ht="17.25">
+      <c r="A50" s="35" t="s">
+        <v>51</v>
+      </c>
+      <c r="B50" s="55" t="s">
+        <v>55</v>
+      </c>
+      <c r="C50" s="55"/>
+      <c r="D50" s="55"/>
+      <c r="E50" s="55"/>
+      <c r="F50" s="55"/>
+      <c r="G50" s="55"/>
+      <c r="H50" s="55"/>
+      <c r="I50" s="55"/>
+      <c r="J50" s="55"/>
+      <c r="K50" s="55"/>
+      <c r="L50" s="55"/>
+      <c r="N50" s="102" t="s">
+        <v>101</v>
+      </c>
+      <c r="O50" s="46" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15">
+      <c r="A51" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="B51" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="B49" s="98" t="s">
-        <v>35</v>
-      </c>
-      <c r="C49" s="98"/>
-      <c r="D49" s="98"/>
-      <c r="E49" s="98"/>
-      <c r="F49" s="98"/>
-      <c r="G49" s="98"/>
-      <c r="H49" s="98"/>
-      <c r="I49" s="98"/>
-      <c r="J49" s="98"/>
-      <c r="K49" s="98"/>
-      <c r="L49" s="98"/>
-    </row>
-    <row r="50" spans="1:12">
-      <c r="A50" s="35" t="s">
-        <v>52</v>
-      </c>
-      <c r="B50" s="98" t="s">
-        <v>56</v>
-      </c>
-      <c r="C50" s="98"/>
-      <c r="D50" s="98"/>
-      <c r="E50" s="98"/>
-      <c r="F50" s="98"/>
-      <c r="G50" s="98"/>
-      <c r="H50" s="98"/>
-      <c r="I50" s="98"/>
-      <c r="J50" s="98"/>
-      <c r="K50" s="98"/>
-      <c r="L50" s="98"/>
-    </row>
-    <row r="51" spans="1:12">
-      <c r="A51" s="35" t="s">
-        <v>53</v>
-      </c>
-      <c r="B51" s="98" t="s">
-        <v>55</v>
-      </c>
-      <c r="C51" s="98"/>
-      <c r="D51" s="98"/>
-      <c r="E51" s="98"/>
-      <c r="F51" s="98"/>
-      <c r="G51" s="98"/>
-      <c r="H51" s="98"/>
-      <c r="I51" s="98"/>
-      <c r="J51" s="98"/>
-      <c r="K51" s="98"/>
-      <c r="L51" s="98"/>
-    </row>
-    <row r="52" spans="1:12">
+      <c r="C51" s="55"/>
+      <c r="D51" s="55"/>
+      <c r="E51" s="55"/>
+      <c r="F51" s="55"/>
+      <c r="G51" s="55"/>
+      <c r="H51" s="55"/>
+      <c r="I51" s="55"/>
+      <c r="J51" s="55"/>
+      <c r="K51" s="55"/>
+      <c r="L51" s="55"/>
+      <c r="O51" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15">
       <c r="C52" s="34"/>
-    </row>
-    <row r="53" spans="1:12">
+      <c r="O52" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15">
       <c r="C53" s="34"/>
     </row>
-    <row r="54" spans="1:12">
+    <row r="54" spans="1:15">
       <c r="B54" s="34"/>
     </row>
   </sheetData>
@@ -2727,45 +2811,6 @@
     <sortCondition ref="A3"/>
   </sortState>
   <mergeCells count="55">
-    <mergeCell ref="N27:S27"/>
-    <mergeCell ref="N33:S33"/>
-    <mergeCell ref="N35:S35"/>
-    <mergeCell ref="N30:S30"/>
-    <mergeCell ref="N28:S28"/>
-    <mergeCell ref="N31:S31"/>
-    <mergeCell ref="B50:L50"/>
-    <mergeCell ref="B51:L51"/>
-    <mergeCell ref="A39:E39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="B45:L45"/>
-    <mergeCell ref="A44:L44"/>
-    <mergeCell ref="B46:L46"/>
-    <mergeCell ref="B47:L47"/>
-    <mergeCell ref="B48:L48"/>
-    <mergeCell ref="B49:L49"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="H33:K33"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="H35:K35"/>
-    <mergeCell ref="H36:K36"/>
-    <mergeCell ref="H37:K37"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="H30:K30"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="H32:K32"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="H31:L31"/>
     <mergeCell ref="N24:S24"/>
     <mergeCell ref="N38:S38"/>
     <mergeCell ref="N36:S36"/>
@@ -2782,13 +2827,55 @@
     <mergeCell ref="H3:K3"/>
     <mergeCell ref="C3:G3"/>
     <mergeCell ref="A28:B28"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="H30:K30"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="H32:K32"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="H31:L31"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="H33:K33"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="H35:K35"/>
+    <mergeCell ref="H36:K36"/>
+    <mergeCell ref="H37:K37"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="B50:L50"/>
+    <mergeCell ref="B51:L51"/>
+    <mergeCell ref="A39:E39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="B45:L45"/>
+    <mergeCell ref="A44:L44"/>
+    <mergeCell ref="B46:L46"/>
+    <mergeCell ref="B47:L47"/>
+    <mergeCell ref="B48:L48"/>
+    <mergeCell ref="B49:L49"/>
+    <mergeCell ref="N27:S27"/>
+    <mergeCell ref="N33:S33"/>
+    <mergeCell ref="N35:S35"/>
+    <mergeCell ref="N30:S30"/>
+    <mergeCell ref="N28:S28"/>
+    <mergeCell ref="N31:S31"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="Q4" r:id="rId1"/>
     <hyperlink ref="O2" r:id="rId2"/>
+    <hyperlink ref="O50" r:id="rId3"/>
+    <hyperlink ref="O46" r:id="rId4"/>
+    <hyperlink ref="O43" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.51" right="0.35" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="89" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" scale="89" orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Actualizado el cuadro de estado y el archivo proyectoportfolio.md. Se aclara que Interest component y los servicios del token ya cuentan con control de excepciones basico
</commit_message>
<xml_diff>
--- a/Cuadro-de-estado.xlsx
+++ b/Cuadro-de-estado.xlsx
@@ -8,15 +8,16 @@
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
-    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
+    <sheet name="Test" sheetId="4" r:id="rId2"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId3"/>
+    <sheet name="Hoja3" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="119">
   <si>
     <t>BACKEND</t>
   </si>
@@ -369,9 +370,6 @@
     <t>Corregir el :hover sobre los widget</t>
   </si>
   <si>
-    <t>declarar como privada/let this.itemParaBorrar</t>
-  </si>
-  <si>
     <t>Si está en mostrar form, no habilitar modificar datos grales</t>
   </si>
   <si>
@@ -423,13 +421,43 @@
     <t>https://www.koyeb.com/</t>
   </si>
   <si>
-    <t>Frankfurt Alemania</t>
-  </si>
-  <si>
     <t>https://firebase.google.com</t>
   </si>
   <si>
     <t>US-central</t>
+  </si>
+  <si>
+    <t>Washington US</t>
+  </si>
+  <si>
+    <t>USER</t>
+  </si>
+  <si>
+    <t>ADMIN</t>
+  </si>
+  <si>
+    <t>ELIMINACION</t>
+  </si>
+  <si>
+    <t>MODIFICACION</t>
+  </si>
+  <si>
+    <t>ALTA</t>
+  </si>
+  <si>
+    <t>MAIN</t>
+  </si>
+  <si>
+    <t>LISTADO</t>
+  </si>
+  <si>
+    <t>CRUD</t>
+  </si>
+  <si>
+    <t>INTERESES</t>
+  </si>
+  <si>
+    <t>OK</t>
   </si>
 </sst>
 </file>
@@ -439,7 +467,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -643,6 +671,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="14">
     <fill>
@@ -724,7 +759,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="37">
+  <borders count="38">
     <border>
       <left/>
       <right/>
@@ -1174,6 +1209,19 @@
         <color indexed="64"/>
       </top>
       <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -1187,7 +1235,7 @@
     </xf>
     <xf numFmtId="43" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1294,175 +1342,198 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1764,8 +1835,8 @@
   </sheetPr>
   <dimension ref="A1:U54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="N54" sqref="N54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1782,28 +1853,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25">
-      <c r="A1" s="83" t="s">
-        <v>92</v>
-      </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
-      <c r="E1" s="83"/>
-      <c r="F1" s="83"/>
-      <c r="G1" s="83"/>
-      <c r="H1" s="83"/>
-      <c r="I1" s="83"/>
-      <c r="J1" s="83"/>
-      <c r="K1" s="83"/>
-      <c r="L1" s="83"/>
+      <c r="A1" s="56" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="56"/>
     </row>
     <row r="2" spans="1:21" ht="19.5" thickBot="1">
       <c r="A2" s="48">
         <f ca="1">M2-TODAY()-1</f>
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B2" s="49" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C2" s="50"/>
       <c r="M2" s="47">
@@ -1814,30 +1885,30 @@
       </c>
     </row>
     <row r="3" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="84" t="s">
+      <c r="A3" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="85"/>
-      <c r="C3" s="86" t="s">
+      <c r="B3" s="58"/>
+      <c r="C3" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="88"/>
-      <c r="H3" s="86" t="s">
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="87"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="88"/>
+      <c r="I3" s="60"/>
+      <c r="J3" s="62"/>
+      <c r="K3" s="61"/>
       <c r="L3" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="91" t="s">
+      <c r="M3" s="64" t="s">
         <v>81</v>
       </c>
-      <c r="N3" s="82"/>
+      <c r="N3" s="55"/>
     </row>
     <row r="4" spans="1:21" s="3" customFormat="1" ht="40.5" customHeight="1" thickBot="1">
       <c r="A4" s="17" t="s">
@@ -1876,10 +1947,10 @@
       <c r="L4" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="M4" s="92" t="s">
+      <c r="M4" s="65" t="s">
         <v>82</v>
       </c>
-      <c r="N4" s="93"/>
+      <c r="N4" s="66"/>
       <c r="O4" s="36" t="s">
         <v>62</v>
       </c>
@@ -1909,10 +1980,10 @@
         <v>13</v>
       </c>
       <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
+      <c r="D6" s="5"/>
       <c r="E6" s="13"/>
       <c r="F6" s="6"/>
-      <c r="G6" s="5"/>
+      <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
@@ -1921,15 +1992,15 @@
       <c r="M6" s="45" t="s">
         <v>84</v>
       </c>
-      <c r="O6" s="81" t="s">
+      <c r="O6" s="54" t="s">
         <v>66</v>
       </c>
-      <c r="P6" s="82"/>
-      <c r="Q6" s="82"/>
-      <c r="R6" s="82"/>
-      <c r="S6" s="82"/>
-      <c r="T6" s="82"/>
-      <c r="U6" s="82"/>
+      <c r="P6" s="55"/>
+      <c r="Q6" s="55"/>
+      <c r="R6" s="55"/>
+      <c r="S6" s="55"/>
+      <c r="T6" s="55"/>
+      <c r="U6" s="55"/>
     </row>
     <row r="7" spans="1:21" ht="4.5" customHeight="1">
       <c r="A7" s="29"/>
@@ -1956,7 +2027,7 @@
       <c r="D8" s="13"/>
       <c r="E8" s="13"/>
       <c r="F8" s="13"/>
-      <c r="G8" s="5"/>
+      <c r="G8" s="4"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
@@ -1984,7 +2055,7 @@
       <c r="D9" s="13"/>
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
-      <c r="G9" s="5"/>
+      <c r="G9" s="4"/>
       <c r="H9" s="13"/>
       <c r="I9" s="13"/>
       <c r="J9" s="4"/>
@@ -2006,7 +2077,7 @@
       <c r="D10" s="13"/>
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
-      <c r="G10" s="5"/>
+      <c r="G10" s="4"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
@@ -2024,7 +2095,7 @@
       <c r="D11" s="13"/>
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
-      <c r="G11" s="5"/>
+      <c r="G11" s="4"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
@@ -2062,14 +2133,14 @@
       <c r="D13" s="42"/>
       <c r="E13" s="13"/>
       <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
+      <c r="G13" s="4"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
       <c r="K13" s="7"/>
       <c r="L13" s="4"/>
       <c r="O13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:21">
@@ -2083,20 +2154,20 @@
       <c r="D14" s="42"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
       <c r="J14" s="4"/>
       <c r="K14" s="7"/>
       <c r="L14" s="4"/>
-      <c r="O14" s="90" t="s">
+      <c r="O14" s="63" t="s">
         <v>79</v>
       </c>
-      <c r="P14" s="90"/>
-      <c r="Q14" s="90"/>
-      <c r="R14" s="90"/>
-      <c r="S14" s="90"/>
-      <c r="T14" s="90"/>
+      <c r="P14" s="63"/>
+      <c r="Q14" s="63"/>
+      <c r="R14" s="63"/>
+      <c r="S14" s="63"/>
+      <c r="T14" s="63"/>
     </row>
     <row r="15" spans="1:21">
       <c r="A15" s="18" t="s">
@@ -2109,18 +2180,18 @@
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
       <c r="J15" s="4"/>
       <c r="K15" s="7"/>
       <c r="L15" s="4"/>
-      <c r="O15" s="90"/>
-      <c r="P15" s="90"/>
-      <c r="Q15" s="90"/>
-      <c r="R15" s="90"/>
-      <c r="S15" s="90"/>
-      <c r="T15" s="90"/>
+      <c r="O15" s="63"/>
+      <c r="P15" s="63"/>
+      <c r="Q15" s="63"/>
+      <c r="R15" s="63"/>
+      <c r="S15" s="63"/>
+      <c r="T15" s="63"/>
     </row>
     <row r="16" spans="1:21">
       <c r="A16" s="40" t="s">
@@ -2133,9 +2204,9 @@
       <c r="D16" s="42"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
       <c r="J16" s="4"/>
       <c r="K16" s="7"/>
       <c r="L16" s="4"/>
@@ -2157,9 +2228,9 @@
       <c r="D17" s="43"/>
       <c r="E17" s="5"/>
       <c r="F17" s="16"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
       <c r="J17" s="4"/>
       <c r="K17" s="7"/>
       <c r="L17" s="4"/>
@@ -2243,7 +2314,7 @@
       <c r="D22" s="8"/>
       <c r="E22" s="6"/>
       <c r="F22" s="8"/>
-      <c r="G22" s="7"/>
+      <c r="G22" s="4"/>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
@@ -2279,14 +2350,14 @@
       <c r="J24" s="4"/>
       <c r="K24" s="7"/>
       <c r="L24" s="4"/>
-      <c r="N24" s="52" t="s">
-        <v>91</v>
-      </c>
-      <c r="O24" s="52"/>
-      <c r="P24" s="52"/>
-      <c r="Q24" s="52"/>
-      <c r="R24" s="52"/>
-      <c r="S24" s="52"/>
+      <c r="N24" s="53" t="s">
+        <v>90</v>
+      </c>
+      <c r="O24" s="53"/>
+      <c r="P24" s="53"/>
+      <c r="Q24" s="53"/>
+      <c r="R24" s="53"/>
+      <c r="S24" s="53"/>
     </row>
     <row r="25" spans="1:19">
       <c r="A25" s="41" t="s">
@@ -2323,60 +2394,58 @@
     <row r="27" spans="1:19" ht="15.75" thickBot="1">
       <c r="A27" s="24"/>
       <c r="B27" s="26"/>
-      <c r="C27" s="86" t="s">
+      <c r="C27" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="87"/>
-      <c r="E27" s="87"/>
-      <c r="F27" s="87"/>
-      <c r="G27" s="88"/>
-      <c r="H27" s="86" t="s">
+      <c r="D27" s="60"/>
+      <c r="E27" s="60"/>
+      <c r="F27" s="60"/>
+      <c r="G27" s="61"/>
+      <c r="H27" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="I27" s="87"/>
-      <c r="J27" s="89"/>
-      <c r="K27" s="88"/>
+      <c r="I27" s="60"/>
+      <c r="J27" s="62"/>
+      <c r="K27" s="61"/>
       <c r="L27" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="N27" s="52" t="s">
-        <v>89</v>
-      </c>
-      <c r="O27" s="52"/>
-      <c r="P27" s="52"/>
-      <c r="Q27" s="52"/>
-      <c r="R27" s="52"/>
-      <c r="S27" s="52"/>
+      <c r="N27" s="53"/>
+      <c r="O27" s="53"/>
+      <c r="P27" s="53"/>
+      <c r="Q27" s="53"/>
+      <c r="R27" s="53"/>
+      <c r="S27" s="53"/>
     </row>
     <row r="28" spans="1:19" ht="30">
-      <c r="A28" s="97" t="s">
+      <c r="A28" s="73" t="s">
         <v>30</v>
       </c>
-      <c r="B28" s="98"/>
-      <c r="C28" s="99" t="s">
-        <v>96</v>
-      </c>
-      <c r="D28" s="100"/>
-      <c r="E28" s="100"/>
-      <c r="F28" s="100"/>
-      <c r="G28" s="101"/>
-      <c r="H28" s="94" t="s">
+      <c r="B28" s="74"/>
+      <c r="C28" s="67" t="s">
+        <v>95</v>
+      </c>
+      <c r="D28" s="68"/>
+      <c r="E28" s="68"/>
+      <c r="F28" s="68"/>
+      <c r="G28" s="69"/>
+      <c r="H28" s="70" t="s">
+        <v>93</v>
+      </c>
+      <c r="I28" s="71"/>
+      <c r="J28" s="71"/>
+      <c r="K28" s="72"/>
+      <c r="L28" s="51" t="s">
         <v>94</v>
       </c>
-      <c r="I28" s="95"/>
-      <c r="J28" s="95"/>
-      <c r="K28" s="96"/>
-      <c r="L28" s="51" t="s">
-        <v>95</v>
-      </c>
-      <c r="N28" s="54" t="s">
+      <c r="N28" s="114" t="s">
         <v>88</v>
       </c>
-      <c r="O28" s="54"/>
-      <c r="P28" s="54"/>
-      <c r="Q28" s="54"/>
-      <c r="R28" s="54"/>
-      <c r="S28" s="54"/>
+      <c r="O28" s="114"/>
+      <c r="P28" s="114"/>
+      <c r="Q28" s="114"/>
+      <c r="R28" s="114"/>
+      <c r="S28" s="114"/>
     </row>
     <row r="29" spans="1:19" ht="4.5" customHeight="1">
       <c r="A29" s="29"/>
@@ -2393,100 +2462,100 @@
       <c r="L29" s="31"/>
     </row>
     <row r="30" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A30" s="103" t="s">
+      <c r="A30" s="79" t="s">
         <v>39</v>
       </c>
-      <c r="B30" s="104"/>
-      <c r="C30" s="74"/>
-      <c r="D30" s="75"/>
-      <c r="E30" s="75"/>
-      <c r="F30" s="75"/>
-      <c r="G30" s="76"/>
-      <c r="H30" s="77"/>
-      <c r="I30" s="75"/>
-      <c r="J30" s="75"/>
-      <c r="K30" s="76"/>
+      <c r="B30" s="80"/>
+      <c r="C30" s="75"/>
+      <c r="D30" s="76"/>
+      <c r="E30" s="76"/>
+      <c r="F30" s="76"/>
+      <c r="G30" s="77"/>
+      <c r="H30" s="78"/>
+      <c r="I30" s="76"/>
+      <c r="J30" s="76"/>
+      <c r="K30" s="77"/>
       <c r="L30" s="22" t="s">
         <v>5</v>
       </c>
       <c r="M30" s="34"/>
-      <c r="N30" s="54" t="s">
+      <c r="N30" s="114" t="s">
         <v>80</v>
       </c>
-      <c r="O30" s="54"/>
-      <c r="P30" s="54"/>
-      <c r="Q30" s="54"/>
-      <c r="R30" s="54"/>
-      <c r="S30" s="54"/>
+      <c r="O30" s="114"/>
+      <c r="P30" s="114"/>
+      <c r="Q30" s="114"/>
+      <c r="R30" s="114"/>
+      <c r="S30" s="114"/>
     </row>
     <row r="31" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A31" s="103" t="s">
+      <c r="A31" s="79" t="s">
         <v>85</v>
       </c>
-      <c r="B31" s="104"/>
-      <c r="C31" s="99"/>
-      <c r="D31" s="100"/>
-      <c r="E31" s="100"/>
-      <c r="F31" s="100"/>
-      <c r="G31" s="101"/>
-      <c r="H31" s="78" t="s">
+      <c r="B31" s="80"/>
+      <c r="C31" s="67"/>
+      <c r="D31" s="68"/>
+      <c r="E31" s="68"/>
+      <c r="F31" s="68"/>
+      <c r="G31" s="69"/>
+      <c r="H31" s="85" t="s">
         <v>86</v>
       </c>
-      <c r="I31" s="79"/>
-      <c r="J31" s="79"/>
-      <c r="K31" s="79"/>
-      <c r="L31" s="80"/>
+      <c r="I31" s="86"/>
+      <c r="J31" s="86"/>
+      <c r="K31" s="86"/>
+      <c r="L31" s="87"/>
       <c r="M31" s="34"/>
-      <c r="N31" s="54" t="s">
+      <c r="N31" s="114" t="s">
         <v>76</v>
       </c>
-      <c r="O31" s="54"/>
-      <c r="P31" s="54"/>
-      <c r="Q31" s="54"/>
-      <c r="R31" s="54"/>
-      <c r="S31" s="54"/>
+      <c r="O31" s="114"/>
+      <c r="P31" s="114"/>
+      <c r="Q31" s="114"/>
+      <c r="R31" s="114"/>
+      <c r="S31" s="114"/>
     </row>
     <row r="32" spans="1:19" ht="16.5" thickBot="1">
-      <c r="A32" s="105" t="s">
+      <c r="A32" s="83" t="s">
         <v>60</v>
       </c>
-      <c r="B32" s="106"/>
-      <c r="C32" s="74"/>
-      <c r="D32" s="75"/>
-      <c r="E32" s="75"/>
-      <c r="F32" s="75"/>
-      <c r="G32" s="76"/>
-      <c r="H32" s="77"/>
-      <c r="I32" s="75"/>
-      <c r="J32" s="75"/>
-      <c r="K32" s="76"/>
+      <c r="B32" s="84"/>
+      <c r="C32" s="75"/>
+      <c r="D32" s="76"/>
+      <c r="E32" s="76"/>
+      <c r="F32" s="76"/>
+      <c r="G32" s="77"/>
+      <c r="H32" s="78"/>
+      <c r="I32" s="76"/>
+      <c r="J32" s="76"/>
+      <c r="K32" s="77"/>
       <c r="M32" s="34"/>
     </row>
     <row r="33" spans="1:19" ht="30.75" customHeight="1" thickBot="1">
-      <c r="A33" s="107" t="s">
+      <c r="A33" s="81" t="s">
         <v>35</v>
       </c>
-      <c r="B33" s="108"/>
-      <c r="C33" s="68" t="s">
+      <c r="B33" s="82"/>
+      <c r="C33" s="93" t="s">
         <v>59</v>
       </c>
-      <c r="D33" s="69"/>
-      <c r="E33" s="69"/>
-      <c r="F33" s="69"/>
-      <c r="G33" s="70"/>
-      <c r="H33" s="65"/>
-      <c r="I33" s="66"/>
-      <c r="J33" s="66"/>
-      <c r="K33" s="67"/>
+      <c r="D33" s="94"/>
+      <c r="E33" s="94"/>
+      <c r="F33" s="94"/>
+      <c r="G33" s="95"/>
+      <c r="H33" s="90"/>
+      <c r="I33" s="91"/>
+      <c r="J33" s="91"/>
+      <c r="K33" s="92"/>
       <c r="M33" s="34"/>
-      <c r="N33" s="53" t="s">
+      <c r="N33" s="113" t="s">
         <v>77</v>
       </c>
-      <c r="O33" s="53"/>
-      <c r="P33" s="53"/>
-      <c r="Q33" s="53"/>
-      <c r="R33" s="53"/>
-      <c r="S33" s="53"/>
+      <c r="O33" s="113"/>
+      <c r="P33" s="113"/>
+      <c r="Q33" s="113"/>
+      <c r="R33" s="113"/>
+      <c r="S33" s="113"/>
     </row>
     <row r="34" spans="1:19" ht="4.5" customHeight="1" thickBot="1">
       <c r="A34" s="29"/>
@@ -2502,100 +2571,100 @@
       <c r="K34" s="31"/>
     </row>
     <row r="35" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A35" s="103" t="s">
+      <c r="A35" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="104"/>
-      <c r="C35" s="71"/>
-      <c r="D35" s="72"/>
-      <c r="E35" s="72"/>
-      <c r="F35" s="72"/>
-      <c r="G35" s="73"/>
-      <c r="H35" s="71"/>
-      <c r="I35" s="72"/>
-      <c r="J35" s="72"/>
-      <c r="K35" s="73"/>
+      <c r="B35" s="80"/>
+      <c r="C35" s="102"/>
+      <c r="D35" s="103"/>
+      <c r="E35" s="103"/>
+      <c r="F35" s="103"/>
+      <c r="G35" s="104"/>
+      <c r="H35" s="96"/>
+      <c r="I35" s="97"/>
+      <c r="J35" s="97"/>
+      <c r="K35" s="98"/>
       <c r="M35" s="34"/>
-      <c r="N35" s="54" t="s">
+      <c r="N35" s="114" t="s">
         <v>78</v>
       </c>
-      <c r="O35" s="54"/>
-      <c r="P35" s="54"/>
-      <c r="Q35" s="54"/>
-      <c r="R35" s="54"/>
-      <c r="S35" s="54"/>
+      <c r="O35" s="114"/>
+      <c r="P35" s="114"/>
+      <c r="Q35" s="114"/>
+      <c r="R35" s="114"/>
+      <c r="S35" s="114"/>
     </row>
     <row r="36" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A36" s="103" t="s">
-        <v>99</v>
-      </c>
-      <c r="B36" s="104"/>
-      <c r="C36" s="71"/>
-      <c r="D36" s="72"/>
-      <c r="E36" s="72"/>
-      <c r="F36" s="72"/>
-      <c r="G36" s="73"/>
-      <c r="H36" s="71"/>
-      <c r="I36" s="72"/>
-      <c r="J36" s="72"/>
-      <c r="K36" s="73"/>
+      <c r="A36" s="79" t="s">
+        <v>98</v>
+      </c>
+      <c r="B36" s="80"/>
+      <c r="C36" s="102"/>
+      <c r="D36" s="103"/>
+      <c r="E36" s="103"/>
+      <c r="F36" s="103"/>
+      <c r="G36" s="104"/>
+      <c r="H36" s="96"/>
+      <c r="I36" s="97"/>
+      <c r="J36" s="97"/>
+      <c r="K36" s="98"/>
       <c r="M36" s="34"/>
-      <c r="N36" s="52" t="s">
+      <c r="N36" s="53" t="s">
         <v>83</v>
       </c>
-      <c r="O36" s="52"/>
-      <c r="P36" s="52"/>
-      <c r="Q36" s="52"/>
-      <c r="R36" s="52"/>
-      <c r="S36" s="52"/>
+      <c r="O36" s="53"/>
+      <c r="P36" s="53"/>
+      <c r="Q36" s="53"/>
+      <c r="R36" s="53"/>
+      <c r="S36" s="53"/>
     </row>
     <row r="37" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A37" s="103" t="s">
+      <c r="A37" s="79" t="s">
         <v>7</v>
       </c>
-      <c r="B37" s="104"/>
-      <c r="C37" s="71"/>
-      <c r="D37" s="72"/>
-      <c r="E37" s="72"/>
-      <c r="F37" s="72"/>
-      <c r="G37" s="73"/>
-      <c r="H37" s="71"/>
-      <c r="I37" s="72"/>
-      <c r="J37" s="72"/>
-      <c r="K37" s="73"/>
+      <c r="B37" s="80"/>
+      <c r="C37" s="99"/>
+      <c r="D37" s="100"/>
+      <c r="E37" s="100"/>
+      <c r="F37" s="100"/>
+      <c r="G37" s="101"/>
+      <c r="H37" s="99"/>
+      <c r="I37" s="100"/>
+      <c r="J37" s="100"/>
+      <c r="K37" s="101"/>
       <c r="M37" s="34"/>
     </row>
     <row r="38" spans="1:19" ht="15.75" thickBot="1">
-      <c r="N38" s="52" t="s">
-        <v>90</v>
-      </c>
-      <c r="O38" s="52"/>
-      <c r="P38" s="52"/>
-      <c r="Q38" s="52"/>
-      <c r="R38" s="52"/>
-      <c r="S38" s="52"/>
+      <c r="N38" s="53" t="s">
+        <v>89</v>
+      </c>
+      <c r="O38" s="53"/>
+      <c r="P38" s="53"/>
+      <c r="Q38" s="53"/>
+      <c r="R38" s="53"/>
+      <c r="S38" s="53"/>
     </row>
     <row r="39" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A39" s="56" t="s">
+      <c r="A39" s="106" t="s">
         <v>26</v>
       </c>
-      <c r="B39" s="57"/>
-      <c r="C39" s="57"/>
-      <c r="D39" s="57"/>
-      <c r="E39" s="58"/>
+      <c r="B39" s="107"/>
+      <c r="C39" s="107"/>
+      <c r="D39" s="107"/>
+      <c r="E39" s="108"/>
     </row>
     <row r="40" spans="1:19">
       <c r="A40" s="14" t="s">
         <v>25</v>
       </c>
       <c r="B40" s="13"/>
-      <c r="C40" s="59" t="s">
+      <c r="C40" s="109" t="s">
         <v>22</v>
       </c>
-      <c r="D40" s="60"/>
+      <c r="D40" s="110"/>
       <c r="E40" s="28"/>
       <c r="N40" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="41" spans="1:19">
@@ -2603,10 +2672,10 @@
         <v>21</v>
       </c>
       <c r="B41" s="5"/>
-      <c r="C41" s="59" t="s">
+      <c r="C41" s="109" t="s">
         <v>23</v>
       </c>
-      <c r="D41" s="60"/>
+      <c r="D41" s="110"/>
       <c r="E41" s="8"/>
     </row>
     <row r="42" spans="1:19">
@@ -2614,190 +2683,190 @@
         <v>24</v>
       </c>
       <c r="B42" s="6"/>
-      <c r="C42" s="63" t="s">
+      <c r="C42" s="88" t="s">
         <v>65</v>
       </c>
-      <c r="D42" s="64"/>
+      <c r="D42" s="89"/>
       <c r="E42" s="39"/>
     </row>
     <row r="43" spans="1:19" ht="18" thickBot="1">
-      <c r="N43" s="102" t="s">
+      <c r="N43" s="52" t="s">
         <v>4</v>
       </c>
       <c r="O43" s="46" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19">
+      <c r="A44" s="111" t="s">
+        <v>36</v>
+      </c>
+      <c r="B44" s="112"/>
+      <c r="C44" s="112"/>
+      <c r="D44" s="112"/>
+      <c r="E44" s="112"/>
+      <c r="F44" s="112"/>
+      <c r="G44" s="112"/>
+      <c r="H44" s="112"/>
+      <c r="I44" s="112"/>
+      <c r="J44" s="112"/>
+      <c r="K44" s="112"/>
+      <c r="L44" s="112"/>
+      <c r="O44" t="s">
         <v>104</v>
-      </c>
-    </row>
-    <row r="44" spans="1:19">
-      <c r="A44" s="61" t="s">
-        <v>36</v>
-      </c>
-      <c r="B44" s="62"/>
-      <c r="C44" s="62"/>
-      <c r="D44" s="62"/>
-      <c r="E44" s="62"/>
-      <c r="F44" s="62"/>
-      <c r="G44" s="62"/>
-      <c r="H44" s="62"/>
-      <c r="I44" s="62"/>
-      <c r="J44" s="62"/>
-      <c r="K44" s="62"/>
-      <c r="L44" s="62"/>
-      <c r="O44" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="45" spans="1:19">
       <c r="A45" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="B45" s="55" t="s">
+      <c r="B45" s="105" t="s">
         <v>56</v>
       </c>
-      <c r="C45" s="55"/>
-      <c r="D45" s="55"/>
-      <c r="E45" s="55"/>
-      <c r="F45" s="55"/>
-      <c r="G45" s="55"/>
-      <c r="H45" s="55"/>
-      <c r="I45" s="55"/>
-      <c r="J45" s="55"/>
-      <c r="K45" s="55"/>
-      <c r="L45" s="55"/>
+      <c r="C45" s="105"/>
+      <c r="D45" s="105"/>
+      <c r="E45" s="105"/>
+      <c r="F45" s="105"/>
+      <c r="G45" s="105"/>
+      <c r="H45" s="105"/>
+      <c r="I45" s="105"/>
+      <c r="J45" s="105"/>
+      <c r="K45" s="105"/>
+      <c r="L45" s="105"/>
     </row>
     <row r="46" spans="1:19" ht="15" customHeight="1">
       <c r="A46" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="B46" s="55" t="s">
+      <c r="B46" s="105" t="s">
         <v>57</v>
       </c>
-      <c r="C46" s="55"/>
-      <c r="D46" s="55"/>
-      <c r="E46" s="55"/>
-      <c r="F46" s="55"/>
-      <c r="G46" s="55"/>
-      <c r="H46" s="55"/>
-      <c r="I46" s="55"/>
-      <c r="J46" s="55"/>
-      <c r="K46" s="55"/>
-      <c r="L46" s="55"/>
-      <c r="N46" s="102" t="s">
+      <c r="C46" s="105"/>
+      <c r="D46" s="105"/>
+      <c r="E46" s="105"/>
+      <c r="F46" s="105"/>
+      <c r="G46" s="105"/>
+      <c r="H46" s="105"/>
+      <c r="I46" s="105"/>
+      <c r="J46" s="105"/>
+      <c r="K46" s="105"/>
+      <c r="L46" s="105"/>
+      <c r="N46" s="52" t="s">
+        <v>101</v>
+      </c>
+      <c r="O46" s="46" t="s">
         <v>102</v>
       </c>
-      <c r="O46" s="46" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="47" spans="1:19">
+    </row>
+    <row r="47" spans="1:19" ht="17.25">
       <c r="A47" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="B47" s="55" t="s">
+      <c r="B47" s="105" t="s">
         <v>58</v>
       </c>
-      <c r="C47" s="55"/>
-      <c r="D47" s="55"/>
-      <c r="E47" s="55"/>
-      <c r="F47" s="55"/>
-      <c r="G47" s="55"/>
-      <c r="H47" s="55"/>
-      <c r="I47" s="55"/>
-      <c r="J47" s="55"/>
-      <c r="K47" s="55"/>
-      <c r="L47" s="55"/>
-      <c r="O47" t="s">
-        <v>106</v>
+      <c r="C47" s="105"/>
+      <c r="D47" s="105"/>
+      <c r="E47" s="105"/>
+      <c r="F47" s="105"/>
+      <c r="G47" s="105"/>
+      <c r="H47" s="105"/>
+      <c r="I47" s="105"/>
+      <c r="J47" s="105"/>
+      <c r="K47" s="105"/>
+      <c r="L47" s="105"/>
+      <c r="O47" s="46" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="48" spans="1:19">
       <c r="A48" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="B48" s="55" t="s">
+      <c r="B48" s="105" t="s">
         <v>45</v>
       </c>
-      <c r="C48" s="55"/>
-      <c r="D48" s="55"/>
-      <c r="E48" s="55"/>
-      <c r="F48" s="55"/>
-      <c r="G48" s="55"/>
-      <c r="H48" s="55"/>
-      <c r="I48" s="55"/>
-      <c r="J48" s="55"/>
-      <c r="K48" s="55"/>
-      <c r="L48" s="55"/>
+      <c r="C48" s="105"/>
+      <c r="D48" s="105"/>
+      <c r="E48" s="105"/>
+      <c r="F48" s="105"/>
+      <c r="G48" s="105"/>
+      <c r="H48" s="105"/>
+      <c r="I48" s="105"/>
+      <c r="J48" s="105"/>
+      <c r="K48" s="105"/>
+      <c r="L48" s="105"/>
       <c r="O48" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="49" spans="1:15">
       <c r="A49" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="B49" s="55" t="s">
+      <c r="B49" s="105" t="s">
         <v>34</v>
       </c>
-      <c r="C49" s="55"/>
-      <c r="D49" s="55"/>
-      <c r="E49" s="55"/>
-      <c r="F49" s="55"/>
-      <c r="G49" s="55"/>
-      <c r="H49" s="55"/>
-      <c r="I49" s="55"/>
-      <c r="J49" s="55"/>
-      <c r="K49" s="55"/>
-      <c r="L49" s="55"/>
+      <c r="C49" s="105"/>
+      <c r="D49" s="105"/>
+      <c r="E49" s="105"/>
+      <c r="F49" s="105"/>
+      <c r="G49" s="105"/>
+      <c r="H49" s="105"/>
+      <c r="I49" s="105"/>
+      <c r="J49" s="105"/>
+      <c r="K49" s="105"/>
+      <c r="L49" s="105"/>
     </row>
     <row r="50" spans="1:15" ht="17.25">
       <c r="A50" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="B50" s="55" t="s">
+      <c r="B50" s="105" t="s">
         <v>55</v>
       </c>
-      <c r="C50" s="55"/>
-      <c r="D50" s="55"/>
-      <c r="E50" s="55"/>
-      <c r="F50" s="55"/>
-      <c r="G50" s="55"/>
-      <c r="H50" s="55"/>
-      <c r="I50" s="55"/>
-      <c r="J50" s="55"/>
-      <c r="K50" s="55"/>
-      <c r="L50" s="55"/>
-      <c r="N50" s="102" t="s">
-        <v>101</v>
+      <c r="C50" s="105"/>
+      <c r="D50" s="105"/>
+      <c r="E50" s="105"/>
+      <c r="F50" s="105"/>
+      <c r="G50" s="105"/>
+      <c r="H50" s="105"/>
+      <c r="I50" s="105"/>
+      <c r="J50" s="105"/>
+      <c r="K50" s="105"/>
+      <c r="L50" s="105"/>
+      <c r="N50" s="52" t="s">
+        <v>100</v>
       </c>
       <c r="O50" s="46" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="51" spans="1:15">
       <c r="A51" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="B51" s="55" t="s">
+      <c r="B51" s="105" t="s">
         <v>54</v>
       </c>
-      <c r="C51" s="55"/>
-      <c r="D51" s="55"/>
-      <c r="E51" s="55"/>
-      <c r="F51" s="55"/>
-      <c r="G51" s="55"/>
-      <c r="H51" s="55"/>
-      <c r="I51" s="55"/>
-      <c r="J51" s="55"/>
-      <c r="K51" s="55"/>
-      <c r="L51" s="55"/>
+      <c r="C51" s="105"/>
+      <c r="D51" s="105"/>
+      <c r="E51" s="105"/>
+      <c r="F51" s="105"/>
+      <c r="G51" s="105"/>
+      <c r="H51" s="105"/>
+      <c r="I51" s="105"/>
+      <c r="J51" s="105"/>
+      <c r="K51" s="105"/>
+      <c r="L51" s="105"/>
       <c r="O51" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="52" spans="1:15">
       <c r="C52" s="34"/>
       <c r="O52" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="53" spans="1:15">
@@ -2811,6 +2880,45 @@
     <sortCondition ref="A3"/>
   </sortState>
   <mergeCells count="55">
+    <mergeCell ref="N27:S27"/>
+    <mergeCell ref="N33:S33"/>
+    <mergeCell ref="N35:S35"/>
+    <mergeCell ref="N30:S30"/>
+    <mergeCell ref="N28:S28"/>
+    <mergeCell ref="N31:S31"/>
+    <mergeCell ref="B50:L50"/>
+    <mergeCell ref="B51:L51"/>
+    <mergeCell ref="A39:E39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="B45:L45"/>
+    <mergeCell ref="A44:L44"/>
+    <mergeCell ref="B46:L46"/>
+    <mergeCell ref="B47:L47"/>
+    <mergeCell ref="B48:L48"/>
+    <mergeCell ref="B49:L49"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="H33:K33"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="H35:K35"/>
+    <mergeCell ref="H36:K36"/>
+    <mergeCell ref="H37:K37"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="H30:K30"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="H32:K32"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="H31:L31"/>
     <mergeCell ref="N24:S24"/>
     <mergeCell ref="N38:S38"/>
     <mergeCell ref="N36:S36"/>
@@ -2827,45 +2935,6 @@
     <mergeCell ref="H3:K3"/>
     <mergeCell ref="C3:G3"/>
     <mergeCell ref="A28:B28"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="H30:K30"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="H32:K32"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="H31:L31"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="H33:K33"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="H35:K35"/>
-    <mergeCell ref="H36:K36"/>
-    <mergeCell ref="H37:K37"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="B50:L50"/>
-    <mergeCell ref="B51:L51"/>
-    <mergeCell ref="A39:E39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="B45:L45"/>
-    <mergeCell ref="A44:L44"/>
-    <mergeCell ref="B46:L46"/>
-    <mergeCell ref="B47:L47"/>
-    <mergeCell ref="B48:L48"/>
-    <mergeCell ref="B49:L49"/>
-    <mergeCell ref="N27:S27"/>
-    <mergeCell ref="N33:S33"/>
-    <mergeCell ref="N35:S35"/>
-    <mergeCell ref="N30:S30"/>
-    <mergeCell ref="N28:S28"/>
-    <mergeCell ref="N31:S31"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="Q4" r:id="rId1"/>
@@ -2873,21 +2942,145 @@
     <hyperlink ref="O50" r:id="rId3"/>
     <hyperlink ref="O46" r:id="rId4"/>
     <hyperlink ref="O43" r:id="rId5"/>
+    <hyperlink ref="O47" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.51" right="0.35" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="89" orientation="portrait" r:id="rId6"/>
+  <pageSetup paperSize="9" scale="89" orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A3:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="11.42578125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="116" t="s">
+        <v>116</v>
+      </c>
+      <c r="B4" s="116"/>
+      <c r="C4" s="116" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="116" t="s">
+        <v>115</v>
+      </c>
+      <c r="E4" s="116" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="115" t="s">
+        <v>113</v>
+      </c>
+      <c r="B5" s="115" t="s">
+        <v>110</v>
+      </c>
+      <c r="C5" s="116"/>
+      <c r="D5" s="116"/>
+      <c r="E5" s="116"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="115"/>
+      <c r="B6" s="115" t="s">
+        <v>109</v>
+      </c>
+      <c r="C6" s="116" t="s">
+        <v>118</v>
+      </c>
+      <c r="D6" s="116" t="s">
+        <v>118</v>
+      </c>
+      <c r="E6" s="116" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="115"/>
+      <c r="B7" s="115"/>
+      <c r="C7" s="116"/>
+      <c r="D7" s="116"/>
+      <c r="E7" s="116"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="115" t="s">
+        <v>112</v>
+      </c>
+      <c r="B8" s="115" t="s">
+        <v>110</v>
+      </c>
+      <c r="C8" s="116"/>
+      <c r="D8" s="116"/>
+      <c r="E8" s="116"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="115"/>
+      <c r="B9" s="115" t="s">
+        <v>109</v>
+      </c>
+      <c r="C9" s="116" t="s">
+        <v>118</v>
+      </c>
+      <c r="D9" s="116" t="s">
+        <v>118</v>
+      </c>
+      <c r="E9" s="116" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="115"/>
+      <c r="B10" s="115"/>
+      <c r="C10" s="116"/>
+      <c r="D10" s="116"/>
+      <c r="E10" s="116"/>
+    </row>
+    <row r="11" spans="1:6" ht="15.75">
+      <c r="A11" s="115" t="s">
+        <v>111</v>
+      </c>
+      <c r="B11" s="115" t="s">
+        <v>110</v>
+      </c>
+      <c r="C11" s="116"/>
+      <c r="D11" s="116"/>
+      <c r="E11" s="116"/>
+      <c r="F11" s="117"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="115"/>
+      <c r="B12" s="115" t="s">
+        <v>109</v>
+      </c>
+      <c r="C12" s="116" t="s">
+        <v>118</v>
+      </c>
+      <c r="D12" s="116" t="s">
+        <v>118</v>
+      </c>
+      <c r="E12" s="116" t="s">
+        <v>118</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2901,4 +3094,16 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Componentes Hardskill e Interes con control de excepcion y validacion de integridad. Ya compatible con el backend
</commit_message>
<xml_diff>
--- a/Cuadro-de-estado.xlsx
+++ b/Cuadro-de-estado.xlsx
@@ -1235,7 +1235,7 @@
     </xf>
     <xf numFmtId="43" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1273,9 +1273,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1300,7 +1297,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1343,9 +1339,134 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1386,15 +1507,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1403,137 +1515,26 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1836,7 +1837,7 @@
   <dimension ref="A1:U54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P20" sqref="P20"/>
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1853,62 +1854,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="97" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="56"/>
-      <c r="L1" s="56"/>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
+      <c r="G1" s="97"/>
+      <c r="H1" s="97"/>
+      <c r="I1" s="97"/>
+      <c r="J1" s="97"/>
+      <c r="K1" s="97"/>
+      <c r="L1" s="97"/>
     </row>
     <row r="2" spans="1:21" ht="19.5" thickBot="1">
-      <c r="A2" s="48">
+      <c r="A2" s="46">
         <f ca="1">M2-TODAY()-1</f>
-        <v>33</v>
-      </c>
-      <c r="B2" s="49" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="47" t="s">
         <v>92</v>
       </c>
-      <c r="C2" s="50"/>
-      <c r="M2" s="47">
+      <c r="C2" s="48"/>
+      <c r="M2" s="45">
         <v>45011</v>
       </c>
-      <c r="O2" s="46" t="s">
+      <c r="O2" s="44" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="98" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="58"/>
-      <c r="C3" s="59" t="s">
+      <c r="B3" s="99"/>
+      <c r="C3" s="100" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="61"/>
-      <c r="H3" s="59" t="s">
+      <c r="D3" s="101"/>
+      <c r="E3" s="101"/>
+      <c r="F3" s="101"/>
+      <c r="G3" s="102"/>
+      <c r="H3" s="100" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="60"/>
-      <c r="J3" s="62"/>
-      <c r="K3" s="61"/>
-      <c r="L3" s="21" t="s">
+      <c r="I3" s="101"/>
+      <c r="J3" s="103"/>
+      <c r="K3" s="102"/>
+      <c r="L3" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="64" t="s">
+      <c r="M3" s="105" t="s">
         <v>81</v>
       </c>
-      <c r="N3" s="55"/>
+      <c r="N3" s="96"/>
     </row>
     <row r="4" spans="1:21" s="3" customFormat="1" ht="40.5" customHeight="1" thickBot="1">
       <c r="A4" s="17" t="s">
@@ -1947,36 +1948,36 @@
       <c r="L4" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="M4" s="65" t="s">
+      <c r="M4" s="106" t="s">
         <v>82</v>
       </c>
-      <c r="N4" s="66"/>
-      <c r="O4" s="36" t="s">
+      <c r="N4" s="107"/>
+      <c r="O4" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="Q4" s="37" t="s">
+      <c r="Q4" s="35" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="4.5" customHeight="1">
-      <c r="A5" s="29"/>
-      <c r="B5" s="30"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="31"/>
-      <c r="I5" s="31"/>
-      <c r="J5" s="31"/>
-      <c r="K5" s="31"/>
-      <c r="L5" s="31"/>
+      <c r="A5" s="28"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="30"/>
+      <c r="K5" s="30"/>
+      <c r="L5" s="30"/>
     </row>
     <row r="6" spans="1:21">
       <c r="A6" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="24" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="6"/>
@@ -1989,38 +1990,38 @@
       <c r="J6" s="4"/>
       <c r="K6" s="5"/>
       <c r="L6" s="4"/>
-      <c r="M6" s="45" t="s">
+      <c r="M6" s="43" t="s">
         <v>84</v>
       </c>
-      <c r="O6" s="54" t="s">
+      <c r="O6" s="95" t="s">
         <v>66</v>
       </c>
-      <c r="P6" s="55"/>
-      <c r="Q6" s="55"/>
-      <c r="R6" s="55"/>
-      <c r="S6" s="55"/>
-      <c r="T6" s="55"/>
-      <c r="U6" s="55"/>
+      <c r="P6" s="96"/>
+      <c r="Q6" s="96"/>
+      <c r="R6" s="96"/>
+      <c r="S6" s="96"/>
+      <c r="T6" s="96"/>
+      <c r="U6" s="96"/>
     </row>
     <row r="7" spans="1:21" ht="4.5" customHeight="1">
-      <c r="A7" s="29"/>
-      <c r="B7" s="30"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="31"/>
-      <c r="J7" s="31"/>
-      <c r="K7" s="31"/>
-      <c r="L7" s="31"/>
+      <c r="A7" s="28"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="30"/>
+      <c r="I7" s="30"/>
+      <c r="J7" s="30"/>
+      <c r="K7" s="30"/>
+      <c r="L7" s="30"/>
     </row>
     <row r="8" spans="1:21">
       <c r="A8" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="24" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="13"/>
@@ -2031,7 +2032,7 @@
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
-      <c r="K8" s="7"/>
+      <c r="K8" s="4"/>
       <c r="L8" s="4"/>
       <c r="O8" s="6" t="s">
         <v>67</v>
@@ -2045,10 +2046,10 @@
       <c r="T8" s="6"/>
     </row>
     <row r="9" spans="1:21">
-      <c r="A9" s="27" t="s">
+      <c r="A9" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="24" t="s">
         <v>12</v>
       </c>
       <c r="C9" s="13"/>
@@ -2056,10 +2057,10 @@
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
       <c r="G9" s="4"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
       <c r="J9" s="4"/>
-      <c r="K9" s="28"/>
+      <c r="K9" s="4"/>
       <c r="L9" s="4"/>
       <c r="P9" s="6" t="s">
         <v>74</v>
@@ -2070,17 +2071,17 @@
       <c r="A10" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="25" t="s">
+      <c r="B10" s="116" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
       <c r="K10" s="7"/>
       <c r="L10" s="4"/>
     </row>
@@ -2088,17 +2089,17 @@
       <c r="A11" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="116" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
       <c r="K11" s="7"/>
       <c r="L11" s="4"/>
       <c r="O11" t="s">
@@ -2109,34 +2110,34 @@
       </c>
     </row>
     <row r="12" spans="1:21" ht="4.5" customHeight="1">
-      <c r="A12" s="29"/>
-      <c r="B12" s="30"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="31"/>
-      <c r="G12" s="31"/>
-      <c r="H12" s="31"/>
-      <c r="I12" s="31"/>
-      <c r="J12" s="31"/>
-      <c r="K12" s="31"/>
-      <c r="L12" s="31"/>
+      <c r="A12" s="28"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="30"/>
+      <c r="J12" s="30"/>
+      <c r="K12" s="30"/>
+      <c r="L12" s="30"/>
     </row>
     <row r="13" spans="1:21">
-      <c r="A13" s="40" t="s">
+      <c r="A13" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="25" t="s">
+      <c r="B13" s="116" t="s">
         <v>12</v>
       </c>
       <c r="C13" s="5"/>
-      <c r="D13" s="42"/>
-      <c r="E13" s="13"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="114"/>
       <c r="F13" s="5"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
       <c r="K13" s="7"/>
       <c r="L13" s="4"/>
       <c r="O13" t="s">
@@ -2144,70 +2145,70 @@
       </c>
     </row>
     <row r="14" spans="1:21">
-      <c r="A14" s="40" t="s">
+      <c r="A14" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="25" t="s">
+      <c r="B14" s="116" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="5"/>
-      <c r="D14" s="42"/>
+      <c r="D14" s="40"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
       <c r="K14" s="7"/>
       <c r="L14" s="4"/>
-      <c r="O14" s="63" t="s">
+      <c r="O14" s="104" t="s">
         <v>79</v>
       </c>
-      <c r="P14" s="63"/>
-      <c r="Q14" s="63"/>
-      <c r="R14" s="63"/>
-      <c r="S14" s="63"/>
-      <c r="T14" s="63"/>
+      <c r="P14" s="104"/>
+      <c r="Q14" s="104"/>
+      <c r="R14" s="104"/>
+      <c r="S14" s="104"/>
+      <c r="T14" s="104"/>
     </row>
     <row r="15" spans="1:21">
       <c r="A15" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="B15" s="25" t="s">
+      <c r="B15" s="116" t="s">
         <v>11</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
       <c r="K15" s="7"/>
       <c r="L15" s="4"/>
-      <c r="O15" s="63"/>
-      <c r="P15" s="63"/>
-      <c r="Q15" s="63"/>
-      <c r="R15" s="63"/>
-      <c r="S15" s="63"/>
-      <c r="T15" s="63"/>
+      <c r="O15" s="104"/>
+      <c r="P15" s="104"/>
+      <c r="Q15" s="104"/>
+      <c r="R15" s="104"/>
+      <c r="S15" s="104"/>
+      <c r="T15" s="104"/>
     </row>
     <row r="16" spans="1:21">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="25" t="s">
+      <c r="B16" s="116" t="s">
         <v>12</v>
       </c>
       <c r="C16" s="5"/>
-      <c r="D16" s="42"/>
+      <c r="D16" s="40"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
       <c r="K16" s="7"/>
       <c r="L16" s="4"/>
       <c r="O16" t="s">
@@ -2221,17 +2222,17 @@
       <c r="A17" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="B17" s="25" t="s">
+      <c r="B17" s="116" t="s">
         <v>11</v>
       </c>
       <c r="C17" s="5"/>
-      <c r="D17" s="43"/>
+      <c r="D17" s="41"/>
       <c r="E17" s="5"/>
       <c r="F17" s="16"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
       <c r="K17" s="7"/>
       <c r="L17" s="4"/>
       <c r="O17" t="s">
@@ -2239,134 +2240,134 @@
       </c>
     </row>
     <row r="18" spans="1:19" ht="4.5" customHeight="1">
-      <c r="A18" s="29"/>
-      <c r="B18" s="30"/>
-      <c r="C18" s="31"/>
-      <c r="D18" s="30"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="31"/>
-      <c r="G18" s="31"/>
-      <c r="H18" s="31"/>
-      <c r="I18" s="31"/>
-      <c r="J18" s="31"/>
-      <c r="K18" s="31"/>
-      <c r="L18" s="31"/>
+      <c r="A18" s="28"/>
+      <c r="B18" s="29"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="30"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="30"/>
+      <c r="J18" s="30"/>
+      <c r="K18" s="30"/>
+      <c r="L18" s="30"/>
     </row>
     <row r="19" spans="1:19">
-      <c r="A19" s="41" t="s">
+      <c r="A19" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="25" t="s">
+      <c r="B19" s="24" t="s">
         <v>12</v>
       </c>
       <c r="C19" s="16"/>
-      <c r="D19" s="44"/>
+      <c r="D19" s="42"/>
       <c r="E19" s="6"/>
       <c r="F19" s="8"/>
       <c r="G19" s="7"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
       <c r="K19" s="7"/>
-      <c r="L19" s="32"/>
+      <c r="L19" s="115"/>
       <c r="O19" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:19">
-      <c r="A20" s="41" t="s">
+      <c r="A20" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="25" t="s">
+      <c r="B20" s="24" t="s">
         <v>12</v>
       </c>
       <c r="C20" s="16"/>
-      <c r="D20" s="44"/>
+      <c r="D20" s="42"/>
       <c r="E20" s="6"/>
       <c r="F20" s="8"/>
       <c r="G20" s="7"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
       <c r="K20" s="7"/>
-      <c r="L20" s="32"/>
+      <c r="L20" s="115"/>
     </row>
     <row r="21" spans="1:19" ht="4.5" customHeight="1">
-      <c r="A21" s="29"/>
-      <c r="B21" s="30"/>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="31"/>
-      <c r="G21" s="31"/>
-      <c r="H21" s="31"/>
-      <c r="I21" s="31"/>
-      <c r="J21" s="31"/>
-      <c r="K21" s="31"/>
-      <c r="L21" s="31"/>
+      <c r="A21" s="28"/>
+      <c r="B21" s="29"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="30"/>
+      <c r="I21" s="30"/>
+      <c r="J21" s="30"/>
+      <c r="K21" s="30"/>
+      <c r="L21" s="30"/>
     </row>
     <row r="22" spans="1:19">
-      <c r="A22" s="41" t="s">
+      <c r="A22" s="39" t="s">
         <v>48</v>
       </c>
-      <c r="B22" s="20"/>
+      <c r="B22" s="19"/>
       <c r="C22" s="16"/>
       <c r="D22" s="8"/>
       <c r="E22" s="6"/>
       <c r="F22" s="8"/>
       <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
       <c r="K22" s="7"/>
       <c r="L22" s="4"/>
     </row>
     <row r="23" spans="1:19" ht="4.5" customHeight="1">
-      <c r="A23" s="29"/>
-      <c r="B23" s="30"/>
-      <c r="C23" s="31"/>
-      <c r="D23" s="31"/>
-      <c r="E23" s="31"/>
-      <c r="F23" s="31"/>
-      <c r="G23" s="31"/>
-      <c r="H23" s="31"/>
-      <c r="I23" s="31"/>
-      <c r="J23" s="31"/>
-      <c r="K23" s="31"/>
-      <c r="L23" s="31"/>
+      <c r="A23" s="28"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="30"/>
+      <c r="G23" s="30"/>
+      <c r="H23" s="30"/>
+      <c r="I23" s="30"/>
+      <c r="J23" s="30"/>
+      <c r="K23" s="30"/>
+      <c r="L23" s="30"/>
     </row>
     <row r="24" spans="1:19">
-      <c r="A24" s="41" t="s">
+      <c r="A24" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="B24" s="33"/>
+      <c r="B24" s="31"/>
       <c r="C24" s="8"/>
       <c r="D24" s="5"/>
       <c r="E24" s="6"/>
       <c r="F24" s="8"/>
       <c r="G24" s="7"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
-      <c r="J24" s="4"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
       <c r="K24" s="7"/>
       <c r="L24" s="4"/>
-      <c r="N24" s="53" t="s">
+      <c r="N24" s="54" t="s">
         <v>90</v>
       </c>
-      <c r="O24" s="53"/>
-      <c r="P24" s="53"/>
-      <c r="Q24" s="53"/>
-      <c r="R24" s="53"/>
-      <c r="S24" s="53"/>
+      <c r="O24" s="54"/>
+      <c r="P24" s="54"/>
+      <c r="Q24" s="54"/>
+      <c r="R24" s="54"/>
+      <c r="S24" s="54"/>
     </row>
     <row r="25" spans="1:19">
-      <c r="A25" s="41" t="s">
+      <c r="A25" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="B25" s="25" t="s">
+      <c r="B25" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C25" s="23"/>
+      <c r="C25" s="22"/>
       <c r="D25" s="8"/>
       <c r="E25" s="6"/>
       <c r="F25" s="8"/>
@@ -2378,291 +2379,291 @@
       <c r="L25" s="7"/>
     </row>
     <row r="26" spans="1:19" ht="4.5" customHeight="1" thickBot="1">
-      <c r="A26" s="29"/>
-      <c r="B26" s="30"/>
-      <c r="C26" s="31"/>
-      <c r="D26" s="31"/>
-      <c r="E26" s="31"/>
-      <c r="F26" s="31"/>
-      <c r="G26" s="31"/>
-      <c r="H26" s="31"/>
-      <c r="I26" s="31"/>
-      <c r="J26" s="31"/>
-      <c r="K26" s="31"/>
-      <c r="L26" s="31"/>
+      <c r="A26" s="28"/>
+      <c r="B26" s="29"/>
+      <c r="C26" s="30"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="30"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="30"/>
+      <c r="I26" s="30"/>
+      <c r="J26" s="30"/>
+      <c r="K26" s="30"/>
+      <c r="L26" s="30"/>
     </row>
     <row r="27" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A27" s="24"/>
-      <c r="B27" s="26"/>
-      <c r="C27" s="59" t="s">
+      <c r="A27" s="23"/>
+      <c r="B27" s="25"/>
+      <c r="C27" s="100" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="60"/>
-      <c r="E27" s="60"/>
-      <c r="F27" s="60"/>
-      <c r="G27" s="61"/>
-      <c r="H27" s="59" t="s">
+      <c r="D27" s="101"/>
+      <c r="E27" s="101"/>
+      <c r="F27" s="101"/>
+      <c r="G27" s="102"/>
+      <c r="H27" s="100" t="s">
         <v>0</v>
       </c>
-      <c r="I27" s="60"/>
-      <c r="J27" s="62"/>
-      <c r="K27" s="61"/>
-      <c r="L27" s="21" t="s">
+      <c r="I27" s="101"/>
+      <c r="J27" s="103"/>
+      <c r="K27" s="102"/>
+      <c r="L27" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="N27" s="53"/>
-      <c r="O27" s="53"/>
-      <c r="P27" s="53"/>
-      <c r="Q27" s="53"/>
-      <c r="R27" s="53"/>
-      <c r="S27" s="53"/>
+      <c r="N27" s="54"/>
+      <c r="O27" s="54"/>
+      <c r="P27" s="54"/>
+      <c r="Q27" s="54"/>
+      <c r="R27" s="54"/>
+      <c r="S27" s="54"/>
     </row>
     <row r="28" spans="1:19" ht="30">
-      <c r="A28" s="73" t="s">
+      <c r="A28" s="117" t="s">
         <v>30</v>
       </c>
-      <c r="B28" s="74"/>
-      <c r="C28" s="67" t="s">
+      <c r="B28" s="118"/>
+      <c r="C28" s="89" t="s">
         <v>95</v>
       </c>
-      <c r="D28" s="68"/>
-      <c r="E28" s="68"/>
-      <c r="F28" s="68"/>
-      <c r="G28" s="69"/>
-      <c r="H28" s="70" t="s">
+      <c r="D28" s="90"/>
+      <c r="E28" s="90"/>
+      <c r="F28" s="90"/>
+      <c r="G28" s="91"/>
+      <c r="H28" s="108" t="s">
         <v>93</v>
       </c>
-      <c r="I28" s="71"/>
-      <c r="J28" s="71"/>
-      <c r="K28" s="72"/>
-      <c r="L28" s="51" t="s">
+      <c r="I28" s="109"/>
+      <c r="J28" s="109"/>
+      <c r="K28" s="110"/>
+      <c r="L28" s="49" t="s">
         <v>94</v>
       </c>
-      <c r="N28" s="114" t="s">
+      <c r="N28" s="56" t="s">
         <v>88</v>
       </c>
-      <c r="O28" s="114"/>
-      <c r="P28" s="114"/>
-      <c r="Q28" s="114"/>
-      <c r="R28" s="114"/>
-      <c r="S28" s="114"/>
+      <c r="O28" s="56"/>
+      <c r="P28" s="56"/>
+      <c r="Q28" s="56"/>
+      <c r="R28" s="56"/>
+      <c r="S28" s="56"/>
     </row>
     <row r="29" spans="1:19" ht="4.5" customHeight="1">
-      <c r="A29" s="29"/>
-      <c r="B29" s="30"/>
-      <c r="C29" s="31"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="31"/>
-      <c r="F29" s="31"/>
-      <c r="G29" s="31"/>
-      <c r="H29" s="31"/>
-      <c r="I29" s="31"/>
-      <c r="J29" s="31"/>
-      <c r="K29" s="31"/>
-      <c r="L29" s="31"/>
+      <c r="A29" s="28"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="30"/>
+      <c r="G29" s="30"/>
+      <c r="H29" s="30"/>
+      <c r="I29" s="30"/>
+      <c r="J29" s="30"/>
+      <c r="K29" s="30"/>
+      <c r="L29" s="30"/>
     </row>
     <row r="30" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A30" s="79" t="s">
+      <c r="A30" s="65" t="s">
         <v>39</v>
       </c>
-      <c r="B30" s="80"/>
-      <c r="C30" s="75"/>
-      <c r="D30" s="76"/>
-      <c r="E30" s="76"/>
-      <c r="F30" s="76"/>
-      <c r="G30" s="77"/>
-      <c r="H30" s="78"/>
-      <c r="I30" s="76"/>
-      <c r="J30" s="76"/>
-      <c r="K30" s="77"/>
-      <c r="L30" s="22" t="s">
+      <c r="B30" s="66"/>
+      <c r="C30" s="81"/>
+      <c r="D30" s="82"/>
+      <c r="E30" s="82"/>
+      <c r="F30" s="82"/>
+      <c r="G30" s="83"/>
+      <c r="H30" s="84"/>
+      <c r="I30" s="82"/>
+      <c r="J30" s="82"/>
+      <c r="K30" s="83"/>
+      <c r="L30" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="M30" s="34"/>
-      <c r="N30" s="114" t="s">
+      <c r="M30" s="32"/>
+      <c r="N30" s="56" t="s">
         <v>80</v>
       </c>
-      <c r="O30" s="114"/>
-      <c r="P30" s="114"/>
-      <c r="Q30" s="114"/>
-      <c r="R30" s="114"/>
-      <c r="S30" s="114"/>
+      <c r="O30" s="56"/>
+      <c r="P30" s="56"/>
+      <c r="Q30" s="56"/>
+      <c r="R30" s="56"/>
+      <c r="S30" s="56"/>
     </row>
     <row r="31" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A31" s="79" t="s">
+      <c r="A31" s="65" t="s">
         <v>85</v>
       </c>
-      <c r="B31" s="80"/>
-      <c r="C31" s="67"/>
-      <c r="D31" s="68"/>
-      <c r="E31" s="68"/>
-      <c r="F31" s="68"/>
-      <c r="G31" s="69"/>
-      <c r="H31" s="85" t="s">
+      <c r="B31" s="66"/>
+      <c r="C31" s="89"/>
+      <c r="D31" s="90"/>
+      <c r="E31" s="90"/>
+      <c r="F31" s="90"/>
+      <c r="G31" s="91"/>
+      <c r="H31" s="92" t="s">
         <v>86</v>
       </c>
-      <c r="I31" s="86"/>
-      <c r="J31" s="86"/>
-      <c r="K31" s="86"/>
-      <c r="L31" s="87"/>
-      <c r="M31" s="34"/>
-      <c r="N31" s="114" t="s">
+      <c r="I31" s="93"/>
+      <c r="J31" s="93"/>
+      <c r="K31" s="93"/>
+      <c r="L31" s="94"/>
+      <c r="M31" s="32"/>
+      <c r="N31" s="56" t="s">
         <v>76</v>
       </c>
-      <c r="O31" s="114"/>
-      <c r="P31" s="114"/>
-      <c r="Q31" s="114"/>
-      <c r="R31" s="114"/>
-      <c r="S31" s="114"/>
+      <c r="O31" s="56"/>
+      <c r="P31" s="56"/>
+      <c r="Q31" s="56"/>
+      <c r="R31" s="56"/>
+      <c r="S31" s="56"/>
     </row>
     <row r="32" spans="1:19" ht="16.5" thickBot="1">
-      <c r="A32" s="83" t="s">
+      <c r="A32" s="87" t="s">
         <v>60</v>
       </c>
-      <c r="B32" s="84"/>
-      <c r="C32" s="75"/>
-      <c r="D32" s="76"/>
-      <c r="E32" s="76"/>
-      <c r="F32" s="76"/>
-      <c r="G32" s="77"/>
-      <c r="H32" s="78"/>
-      <c r="I32" s="76"/>
-      <c r="J32" s="76"/>
-      <c r="K32" s="77"/>
-      <c r="M32" s="34"/>
+      <c r="B32" s="88"/>
+      <c r="C32" s="81"/>
+      <c r="D32" s="82"/>
+      <c r="E32" s="82"/>
+      <c r="F32" s="82"/>
+      <c r="G32" s="83"/>
+      <c r="H32" s="84"/>
+      <c r="I32" s="82"/>
+      <c r="J32" s="82"/>
+      <c r="K32" s="83"/>
+      <c r="M32" s="32"/>
     </row>
     <row r="33" spans="1:19" ht="30.75" customHeight="1" thickBot="1">
-      <c r="A33" s="81" t="s">
+      <c r="A33" s="85" t="s">
         <v>35</v>
       </c>
-      <c r="B33" s="82"/>
-      <c r="C33" s="93" t="s">
+      <c r="B33" s="86"/>
+      <c r="C33" s="72" t="s">
         <v>59</v>
       </c>
-      <c r="D33" s="94"/>
-      <c r="E33" s="94"/>
-      <c r="F33" s="94"/>
-      <c r="G33" s="95"/>
-      <c r="H33" s="90"/>
-      <c r="I33" s="91"/>
-      <c r="J33" s="91"/>
-      <c r="K33" s="92"/>
-      <c r="M33" s="34"/>
-      <c r="N33" s="113" t="s">
+      <c r="D33" s="73"/>
+      <c r="E33" s="73"/>
+      <c r="F33" s="73"/>
+      <c r="G33" s="74"/>
+      <c r="H33" s="69"/>
+      <c r="I33" s="70"/>
+      <c r="J33" s="70"/>
+      <c r="K33" s="71"/>
+      <c r="M33" s="32"/>
+      <c r="N33" s="55" t="s">
         <v>77</v>
       </c>
-      <c r="O33" s="113"/>
-      <c r="P33" s="113"/>
-      <c r="Q33" s="113"/>
-      <c r="R33" s="113"/>
-      <c r="S33" s="113"/>
+      <c r="O33" s="55"/>
+      <c r="P33" s="55"/>
+      <c r="Q33" s="55"/>
+      <c r="R33" s="55"/>
+      <c r="S33" s="55"/>
     </row>
     <row r="34" spans="1:19" ht="4.5" customHeight="1" thickBot="1">
-      <c r="A34" s="29"/>
-      <c r="B34" s="30"/>
-      <c r="C34" s="38"/>
-      <c r="D34" s="38"/>
-      <c r="E34" s="38"/>
-      <c r="F34" s="38"/>
-      <c r="G34" s="38"/>
-      <c r="H34" s="31"/>
-      <c r="I34" s="31"/>
-      <c r="J34" s="31"/>
-      <c r="K34" s="31"/>
+      <c r="A34" s="28"/>
+      <c r="B34" s="29"/>
+      <c r="C34" s="36"/>
+      <c r="D34" s="36"/>
+      <c r="E34" s="36"/>
+      <c r="F34" s="36"/>
+      <c r="G34" s="36"/>
+      <c r="H34" s="30"/>
+      <c r="I34" s="30"/>
+      <c r="J34" s="30"/>
+      <c r="K34" s="30"/>
     </row>
     <row r="35" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A35" s="79" t="s">
+      <c r="A35" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="80"/>
-      <c r="C35" s="102"/>
-      <c r="D35" s="103"/>
-      <c r="E35" s="103"/>
-      <c r="F35" s="103"/>
-      <c r="G35" s="104"/>
-      <c r="H35" s="96"/>
-      <c r="I35" s="97"/>
-      <c r="J35" s="97"/>
-      <c r="K35" s="98"/>
-      <c r="M35" s="34"/>
-      <c r="N35" s="114" t="s">
+      <c r="B35" s="66"/>
+      <c r="C35" s="111"/>
+      <c r="D35" s="112"/>
+      <c r="E35" s="112"/>
+      <c r="F35" s="112"/>
+      <c r="G35" s="113"/>
+      <c r="H35" s="75"/>
+      <c r="I35" s="76"/>
+      <c r="J35" s="76"/>
+      <c r="K35" s="77"/>
+      <c r="M35" s="32"/>
+      <c r="N35" s="56" t="s">
         <v>78</v>
       </c>
-      <c r="O35" s="114"/>
-      <c r="P35" s="114"/>
-      <c r="Q35" s="114"/>
-      <c r="R35" s="114"/>
-      <c r="S35" s="114"/>
+      <c r="O35" s="56"/>
+      <c r="P35" s="56"/>
+      <c r="Q35" s="56"/>
+      <c r="R35" s="56"/>
+      <c r="S35" s="56"/>
     </row>
     <row r="36" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A36" s="79" t="s">
+      <c r="A36" s="65" t="s">
         <v>98</v>
       </c>
-      <c r="B36" s="80"/>
-      <c r="C36" s="102"/>
-      <c r="D36" s="103"/>
-      <c r="E36" s="103"/>
-      <c r="F36" s="103"/>
-      <c r="G36" s="104"/>
-      <c r="H36" s="96"/>
-      <c r="I36" s="97"/>
-      <c r="J36" s="97"/>
-      <c r="K36" s="98"/>
-      <c r="M36" s="34"/>
-      <c r="N36" s="53" t="s">
+      <c r="B36" s="66"/>
+      <c r="C36" s="111"/>
+      <c r="D36" s="112"/>
+      <c r="E36" s="112"/>
+      <c r="F36" s="112"/>
+      <c r="G36" s="113"/>
+      <c r="H36" s="75"/>
+      <c r="I36" s="76"/>
+      <c r="J36" s="76"/>
+      <c r="K36" s="77"/>
+      <c r="M36" s="32"/>
+      <c r="N36" s="54" t="s">
         <v>83</v>
       </c>
-      <c r="O36" s="53"/>
-      <c r="P36" s="53"/>
-      <c r="Q36" s="53"/>
-      <c r="R36" s="53"/>
-      <c r="S36" s="53"/>
+      <c r="O36" s="54"/>
+      <c r="P36" s="54"/>
+      <c r="Q36" s="54"/>
+      <c r="R36" s="54"/>
+      <c r="S36" s="54"/>
     </row>
     <row r="37" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A37" s="79" t="s">
+      <c r="A37" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="B37" s="80"/>
-      <c r="C37" s="99"/>
-      <c r="D37" s="100"/>
-      <c r="E37" s="100"/>
-      <c r="F37" s="100"/>
-      <c r="G37" s="101"/>
-      <c r="H37" s="99"/>
-      <c r="I37" s="100"/>
-      <c r="J37" s="100"/>
-      <c r="K37" s="101"/>
-      <c r="M37" s="34"/>
+      <c r="B37" s="66"/>
+      <c r="C37" s="78"/>
+      <c r="D37" s="79"/>
+      <c r="E37" s="79"/>
+      <c r="F37" s="79"/>
+      <c r="G37" s="80"/>
+      <c r="H37" s="78"/>
+      <c r="I37" s="79"/>
+      <c r="J37" s="79"/>
+      <c r="K37" s="80"/>
+      <c r="M37" s="32"/>
     </row>
     <row r="38" spans="1:19" ht="15.75" thickBot="1">
-      <c r="N38" s="53" t="s">
+      <c r="N38" s="54" t="s">
         <v>89</v>
       </c>
-      <c r="O38" s="53"/>
-      <c r="P38" s="53"/>
-      <c r="Q38" s="53"/>
-      <c r="R38" s="53"/>
-      <c r="S38" s="53"/>
+      <c r="O38" s="54"/>
+      <c r="P38" s="54"/>
+      <c r="Q38" s="54"/>
+      <c r="R38" s="54"/>
+      <c r="S38" s="54"/>
     </row>
     <row r="39" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A39" s="106" t="s">
+      <c r="A39" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="B39" s="107"/>
-      <c r="C39" s="107"/>
-      <c r="D39" s="107"/>
-      <c r="E39" s="108"/>
+      <c r="B39" s="59"/>
+      <c r="C39" s="59"/>
+      <c r="D39" s="59"/>
+      <c r="E39" s="60"/>
     </row>
     <row r="40" spans="1:19">
       <c r="A40" s="14" t="s">
         <v>25</v>
       </c>
       <c r="B40" s="13"/>
-      <c r="C40" s="109" t="s">
+      <c r="C40" s="61" t="s">
         <v>22</v>
       </c>
-      <c r="D40" s="110"/>
-      <c r="E40" s="28"/>
+      <c r="D40" s="62"/>
+      <c r="E40" s="27"/>
       <c r="N40" t="s">
         <v>97</v>
       </c>
@@ -2672,10 +2673,10 @@
         <v>21</v>
       </c>
       <c r="B41" s="5"/>
-      <c r="C41" s="109" t="s">
+      <c r="C41" s="61" t="s">
         <v>23</v>
       </c>
-      <c r="D41" s="110"/>
+      <c r="D41" s="62"/>
       <c r="E41" s="8"/>
     </row>
     <row r="42" spans="1:19">
@@ -2683,242 +2684,203 @@
         <v>24</v>
       </c>
       <c r="B42" s="6"/>
-      <c r="C42" s="88" t="s">
+      <c r="C42" s="67" t="s">
         <v>65</v>
       </c>
-      <c r="D42" s="89"/>
-      <c r="E42" s="39"/>
+      <c r="D42" s="68"/>
+      <c r="E42" s="37"/>
     </row>
     <row r="43" spans="1:19" ht="18" thickBot="1">
-      <c r="N43" s="52" t="s">
+      <c r="N43" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="O43" s="46" t="s">
+      <c r="O43" s="44" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="44" spans="1:19">
-      <c r="A44" s="111" t="s">
+      <c r="A44" s="63" t="s">
         <v>36</v>
       </c>
-      <c r="B44" s="112"/>
-      <c r="C44" s="112"/>
-      <c r="D44" s="112"/>
-      <c r="E44" s="112"/>
-      <c r="F44" s="112"/>
-      <c r="G44" s="112"/>
-      <c r="H44" s="112"/>
-      <c r="I44" s="112"/>
-      <c r="J44" s="112"/>
-      <c r="K44" s="112"/>
-      <c r="L44" s="112"/>
+      <c r="B44" s="64"/>
+      <c r="C44" s="64"/>
+      <c r="D44" s="64"/>
+      <c r="E44" s="64"/>
+      <c r="F44" s="64"/>
+      <c r="G44" s="64"/>
+      <c r="H44" s="64"/>
+      <c r="I44" s="64"/>
+      <c r="J44" s="64"/>
+      <c r="K44" s="64"/>
+      <c r="L44" s="64"/>
       <c r="O44" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="45" spans="1:19">
-      <c r="A45" s="35" t="s">
+      <c r="A45" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="B45" s="105" t="s">
+      <c r="B45" s="57" t="s">
         <v>56</v>
       </c>
-      <c r="C45" s="105"/>
-      <c r="D45" s="105"/>
-      <c r="E45" s="105"/>
-      <c r="F45" s="105"/>
-      <c r="G45" s="105"/>
-      <c r="H45" s="105"/>
-      <c r="I45" s="105"/>
-      <c r="J45" s="105"/>
-      <c r="K45" s="105"/>
-      <c r="L45" s="105"/>
+      <c r="C45" s="57"/>
+      <c r="D45" s="57"/>
+      <c r="E45" s="57"/>
+      <c r="F45" s="57"/>
+      <c r="G45" s="57"/>
+      <c r="H45" s="57"/>
+      <c r="I45" s="57"/>
+      <c r="J45" s="57"/>
+      <c r="K45" s="57"/>
+      <c r="L45" s="57"/>
     </row>
     <row r="46" spans="1:19" ht="15" customHeight="1">
-      <c r="A46" s="35" t="s">
+      <c r="A46" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="B46" s="105" t="s">
+      <c r="B46" s="57" t="s">
         <v>57</v>
       </c>
-      <c r="C46" s="105"/>
-      <c r="D46" s="105"/>
-      <c r="E46" s="105"/>
-      <c r="F46" s="105"/>
-      <c r="G46" s="105"/>
-      <c r="H46" s="105"/>
-      <c r="I46" s="105"/>
-      <c r="J46" s="105"/>
-      <c r="K46" s="105"/>
-      <c r="L46" s="105"/>
-      <c r="N46" s="52" t="s">
+      <c r="C46" s="57"/>
+      <c r="D46" s="57"/>
+      <c r="E46" s="57"/>
+      <c r="F46" s="57"/>
+      <c r="G46" s="57"/>
+      <c r="H46" s="57"/>
+      <c r="I46" s="57"/>
+      <c r="J46" s="57"/>
+      <c r="K46" s="57"/>
+      <c r="L46" s="57"/>
+      <c r="N46" s="50" t="s">
         <v>101</v>
       </c>
-      <c r="O46" s="46" t="s">
+      <c r="O46" s="44" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="47" spans="1:19" ht="17.25">
-      <c r="A47" s="35" t="s">
+      <c r="A47" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="B47" s="105" t="s">
+      <c r="B47" s="57" t="s">
         <v>58</v>
       </c>
-      <c r="C47" s="105"/>
-      <c r="D47" s="105"/>
-      <c r="E47" s="105"/>
-      <c r="F47" s="105"/>
-      <c r="G47" s="105"/>
-      <c r="H47" s="105"/>
-      <c r="I47" s="105"/>
-      <c r="J47" s="105"/>
-      <c r="K47" s="105"/>
-      <c r="L47" s="105"/>
-      <c r="O47" s="46" t="s">
+      <c r="C47" s="57"/>
+      <c r="D47" s="57"/>
+      <c r="E47" s="57"/>
+      <c r="F47" s="57"/>
+      <c r="G47" s="57"/>
+      <c r="H47" s="57"/>
+      <c r="I47" s="57"/>
+      <c r="J47" s="57"/>
+      <c r="K47" s="57"/>
+      <c r="L47" s="57"/>
+      <c r="O47" s="44" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="48" spans="1:19">
-      <c r="A48" s="35" t="s">
+      <c r="A48" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="B48" s="105" t="s">
+      <c r="B48" s="57" t="s">
         <v>45</v>
       </c>
-      <c r="C48" s="105"/>
-      <c r="D48" s="105"/>
-      <c r="E48" s="105"/>
-      <c r="F48" s="105"/>
-      <c r="G48" s="105"/>
-      <c r="H48" s="105"/>
-      <c r="I48" s="105"/>
-      <c r="J48" s="105"/>
-      <c r="K48" s="105"/>
-      <c r="L48" s="105"/>
+      <c r="C48" s="57"/>
+      <c r="D48" s="57"/>
+      <c r="E48" s="57"/>
+      <c r="F48" s="57"/>
+      <c r="G48" s="57"/>
+      <c r="H48" s="57"/>
+      <c r="I48" s="57"/>
+      <c r="J48" s="57"/>
+      <c r="K48" s="57"/>
+      <c r="L48" s="57"/>
       <c r="O48" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="49" spans="1:15">
-      <c r="A49" s="35" t="s">
+      <c r="A49" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="B49" s="105" t="s">
+      <c r="B49" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="C49" s="105"/>
-      <c r="D49" s="105"/>
-      <c r="E49" s="105"/>
-      <c r="F49" s="105"/>
-      <c r="G49" s="105"/>
-      <c r="H49" s="105"/>
-      <c r="I49" s="105"/>
-      <c r="J49" s="105"/>
-      <c r="K49" s="105"/>
-      <c r="L49" s="105"/>
+      <c r="C49" s="57"/>
+      <c r="D49" s="57"/>
+      <c r="E49" s="57"/>
+      <c r="F49" s="57"/>
+      <c r="G49" s="57"/>
+      <c r="H49" s="57"/>
+      <c r="I49" s="57"/>
+      <c r="J49" s="57"/>
+      <c r="K49" s="57"/>
+      <c r="L49" s="57"/>
     </row>
     <row r="50" spans="1:15" ht="17.25">
-      <c r="A50" s="35" t="s">
+      <c r="A50" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="B50" s="105" t="s">
+      <c r="B50" s="57" t="s">
         <v>55</v>
       </c>
-      <c r="C50" s="105"/>
-      <c r="D50" s="105"/>
-      <c r="E50" s="105"/>
-      <c r="F50" s="105"/>
-      <c r="G50" s="105"/>
-      <c r="H50" s="105"/>
-      <c r="I50" s="105"/>
-      <c r="J50" s="105"/>
-      <c r="K50" s="105"/>
-      <c r="L50" s="105"/>
-      <c r="N50" s="52" t="s">
+      <c r="C50" s="57"/>
+      <c r="D50" s="57"/>
+      <c r="E50" s="57"/>
+      <c r="F50" s="57"/>
+      <c r="G50" s="57"/>
+      <c r="H50" s="57"/>
+      <c r="I50" s="57"/>
+      <c r="J50" s="57"/>
+      <c r="K50" s="57"/>
+      <c r="L50" s="57"/>
+      <c r="N50" s="50" t="s">
         <v>100</v>
       </c>
-      <c r="O50" s="46" t="s">
+      <c r="O50" s="44" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="51" spans="1:15">
-      <c r="A51" s="35" t="s">
+      <c r="A51" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="B51" s="105" t="s">
+      <c r="B51" s="57" t="s">
         <v>54</v>
       </c>
-      <c r="C51" s="105"/>
-      <c r="D51" s="105"/>
-      <c r="E51" s="105"/>
-      <c r="F51" s="105"/>
-      <c r="G51" s="105"/>
-      <c r="H51" s="105"/>
-      <c r="I51" s="105"/>
-      <c r="J51" s="105"/>
-      <c r="K51" s="105"/>
-      <c r="L51" s="105"/>
+      <c r="C51" s="57"/>
+      <c r="D51" s="57"/>
+      <c r="E51" s="57"/>
+      <c r="F51" s="57"/>
+      <c r="G51" s="57"/>
+      <c r="H51" s="57"/>
+      <c r="I51" s="57"/>
+      <c r="J51" s="57"/>
+      <c r="K51" s="57"/>
+      <c r="L51" s="57"/>
       <c r="O51" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="52" spans="1:15">
-      <c r="C52" s="34"/>
+      <c r="C52" s="32"/>
       <c r="O52" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="53" spans="1:15">
-      <c r="C53" s="34"/>
+      <c r="C53" s="32"/>
     </row>
     <row r="54" spans="1:15">
-      <c r="B54" s="34"/>
+      <c r="B54" s="32"/>
     </row>
   </sheetData>
   <sortState ref="A24:K25">
     <sortCondition ref="A3"/>
   </sortState>
   <mergeCells count="55">
-    <mergeCell ref="N27:S27"/>
-    <mergeCell ref="N33:S33"/>
-    <mergeCell ref="N35:S35"/>
-    <mergeCell ref="N30:S30"/>
-    <mergeCell ref="N28:S28"/>
-    <mergeCell ref="N31:S31"/>
-    <mergeCell ref="B50:L50"/>
-    <mergeCell ref="B51:L51"/>
-    <mergeCell ref="A39:E39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="B45:L45"/>
-    <mergeCell ref="A44:L44"/>
-    <mergeCell ref="B46:L46"/>
-    <mergeCell ref="B47:L47"/>
-    <mergeCell ref="B48:L48"/>
-    <mergeCell ref="B49:L49"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="H33:K33"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="H35:K35"/>
-    <mergeCell ref="H36:K36"/>
-    <mergeCell ref="H37:K37"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="H30:K30"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="H32:K32"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="H31:L31"/>
     <mergeCell ref="N24:S24"/>
     <mergeCell ref="N38:S38"/>
     <mergeCell ref="N36:S36"/>
@@ -2935,6 +2897,45 @@
     <mergeCell ref="H3:K3"/>
     <mergeCell ref="C3:G3"/>
     <mergeCell ref="A28:B28"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="H30:K30"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="H32:K32"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="H31:L31"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="H33:K33"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="H35:K35"/>
+    <mergeCell ref="H36:K36"/>
+    <mergeCell ref="H37:K37"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="B50:L50"/>
+    <mergeCell ref="B51:L51"/>
+    <mergeCell ref="A39:E39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="B45:L45"/>
+    <mergeCell ref="A44:L44"/>
+    <mergeCell ref="B46:L46"/>
+    <mergeCell ref="B47:L47"/>
+    <mergeCell ref="B48:L48"/>
+    <mergeCell ref="B49:L49"/>
+    <mergeCell ref="N27:S27"/>
+    <mergeCell ref="N33:S33"/>
+    <mergeCell ref="N35:S35"/>
+    <mergeCell ref="N30:S30"/>
+    <mergeCell ref="N28:S28"/>
+    <mergeCell ref="N31:S31"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="Q4" r:id="rId1"/>
@@ -2971,110 +2972,110 @@
       <c r="B3" s="1"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="116" t="s">
+      <c r="A4" s="52" t="s">
         <v>116</v>
       </c>
-      <c r="B4" s="116"/>
-      <c r="C4" s="116" t="s">
+      <c r="B4" s="52"/>
+      <c r="C4" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="116" t="s">
+      <c r="D4" s="52" t="s">
         <v>115</v>
       </c>
-      <c r="E4" s="116" t="s">
+      <c r="E4" s="52" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="115" t="s">
+      <c r="A5" s="51" t="s">
         <v>113</v>
       </c>
-      <c r="B5" s="115" t="s">
+      <c r="B5" s="51" t="s">
         <v>110</v>
       </c>
-      <c r="C5" s="116"/>
-      <c r="D5" s="116"/>
-      <c r="E5" s="116"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="115"/>
-      <c r="B6" s="115" t="s">
+      <c r="A6" s="51"/>
+      <c r="B6" s="51" t="s">
         <v>109</v>
       </c>
-      <c r="C6" s="116" t="s">
+      <c r="C6" s="52" t="s">
         <v>118</v>
       </c>
-      <c r="D6" s="116" t="s">
+      <c r="D6" s="52" t="s">
         <v>118</v>
       </c>
-      <c r="E6" s="116" t="s">
+      <c r="E6" s="52" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="115"/>
-      <c r="B7" s="115"/>
-      <c r="C7" s="116"/>
-      <c r="D7" s="116"/>
-      <c r="E7" s="116"/>
+      <c r="A7" s="51"/>
+      <c r="B7" s="51"/>
+      <c r="C7" s="52"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="52"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="115" t="s">
+      <c r="A8" s="51" t="s">
         <v>112</v>
       </c>
-      <c r="B8" s="115" t="s">
+      <c r="B8" s="51" t="s">
         <v>110</v>
       </c>
-      <c r="C8" s="116"/>
-      <c r="D8" s="116"/>
-      <c r="E8" s="116"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="52"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="115"/>
-      <c r="B9" s="115" t="s">
+      <c r="A9" s="51"/>
+      <c r="B9" s="51" t="s">
         <v>109</v>
       </c>
-      <c r="C9" s="116" t="s">
+      <c r="C9" s="52" t="s">
         <v>118</v>
       </c>
-      <c r="D9" s="116" t="s">
+      <c r="D9" s="52" t="s">
         <v>118</v>
       </c>
-      <c r="E9" s="116" t="s">
+      <c r="E9" s="52" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="115"/>
-      <c r="B10" s="115"/>
-      <c r="C10" s="116"/>
-      <c r="D10" s="116"/>
-      <c r="E10" s="116"/>
+      <c r="A10" s="51"/>
+      <c r="B10" s="51"/>
+      <c r="C10" s="52"/>
+      <c r="D10" s="52"/>
+      <c r="E10" s="52"/>
     </row>
     <row r="11" spans="1:6" ht="15.75">
-      <c r="A11" s="115" t="s">
+      <c r="A11" s="51" t="s">
         <v>111</v>
       </c>
-      <c r="B11" s="115" t="s">
+      <c r="B11" s="51" t="s">
         <v>110</v>
       </c>
-      <c r="C11" s="116"/>
-      <c r="D11" s="116"/>
-      <c r="E11" s="116"/>
-      <c r="F11" s="117"/>
+      <c r="C11" s="52"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="52"/>
+      <c r="F11" s="53"/>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="115"/>
-      <c r="B12" s="115" t="s">
+      <c r="A12" s="51"/>
+      <c r="B12" s="51" t="s">
         <v>109</v>
       </c>
-      <c r="C12" s="116" t="s">
+      <c r="C12" s="52" t="s">
         <v>118</v>
       </c>
-      <c r="D12" s="116" t="s">
+      <c r="D12" s="52" t="s">
         <v>118</v>
       </c>
-      <c r="E12" s="116" t="s">
+      <c r="E12" s="52" t="s">
         <v>118</v>
       </c>
     </row>
@@ -3088,7 +3089,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>

</xml_diff>

<commit_message>
Arreglos en Controles de integridad y manejo de excepciones en Softskill, Interest, Project. Correccion del modal de borado, ahora ni usa un servicio, se toma el valor con el modalDialog.afterClosed()
</commit_message>
<xml_diff>
--- a/Cuadro-de-estado.xlsx
+++ b/Cuadro-de-estado.xlsx
@@ -367,9 +367,6 @@
     <t>https://www.arquitecturajava.com/angular-select-y-todas-sus-opciones/</t>
   </si>
   <si>
-    <t>Corregir el :hover sobre los widget</t>
-  </si>
-  <si>
     <t>Si está en mostrar form, no habilitar modificar datos grales</t>
   </si>
   <si>
@@ -394,9 +391,6 @@
     <t>Upload file</t>
   </si>
   <si>
-    <t>Las Card init, las está tomando del archivo .json</t>
-  </si>
-  <si>
     <t>LOGIN</t>
   </si>
   <si>
@@ -458,6 +452,12 @@
   </si>
   <si>
     <t>OK</t>
+  </si>
+  <si>
+    <t>A las Card init, las está tomando del archivo .json</t>
+  </si>
+  <si>
+    <t>Tengo problemas para borrar un alta, despues de su modificacion, lo arrastra incluso a otros componentes, como que es algo que queda pendiente de realizar, pero en verdad ya lo habia borrado la primera vez.</t>
   </si>
 </sst>
 </file>
@@ -1235,7 +1235,7 @@
     </xf>
     <xf numFmtId="43" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="119">
+  <cellXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1344,196 +1344,206 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1837,7 +1847,7 @@
   <dimension ref="A1:U54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1854,28 +1864,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25">
-      <c r="A1" s="97" t="s">
-        <v>91</v>
-      </c>
-      <c r="B1" s="97"/>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
-      <c r="E1" s="97"/>
-      <c r="F1" s="97"/>
-      <c r="G1" s="97"/>
-      <c r="H1" s="97"/>
-      <c r="I1" s="97"/>
-      <c r="J1" s="97"/>
-      <c r="K1" s="97"/>
-      <c r="L1" s="97"/>
+      <c r="A1" s="105" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="105"/>
+      <c r="C1" s="105"/>
+      <c r="D1" s="105"/>
+      <c r="E1" s="105"/>
+      <c r="F1" s="105"/>
+      <c r="G1" s="105"/>
+      <c r="H1" s="105"/>
+      <c r="I1" s="105"/>
+      <c r="J1" s="105"/>
+      <c r="K1" s="105"/>
+      <c r="L1" s="105"/>
     </row>
     <row r="2" spans="1:21" ht="19.5" thickBot="1">
       <c r="A2" s="46">
         <f ca="1">M2-TODAY()-1</f>
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B2" s="47" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C2" s="48"/>
       <c r="M2" s="45">
@@ -1886,30 +1896,30 @@
       </c>
     </row>
     <row r="3" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="98" t="s">
+      <c r="A3" s="106" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="99"/>
-      <c r="C3" s="100" t="s">
+      <c r="B3" s="107"/>
+      <c r="C3" s="108" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="101"/>
-      <c r="E3" s="101"/>
-      <c r="F3" s="101"/>
-      <c r="G3" s="102"/>
-      <c r="H3" s="100" t="s">
+      <c r="D3" s="109"/>
+      <c r="E3" s="109"/>
+      <c r="F3" s="109"/>
+      <c r="G3" s="110"/>
+      <c r="H3" s="108" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="101"/>
-      <c r="J3" s="103"/>
-      <c r="K3" s="102"/>
+      <c r="I3" s="109"/>
+      <c r="J3" s="111"/>
+      <c r="K3" s="110"/>
       <c r="L3" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="105" t="s">
+      <c r="M3" s="113" t="s">
         <v>81</v>
       </c>
-      <c r="N3" s="96"/>
+      <c r="N3" s="104"/>
     </row>
     <row r="4" spans="1:21" s="3" customFormat="1" ht="40.5" customHeight="1" thickBot="1">
       <c r="A4" s="17" t="s">
@@ -1948,10 +1958,10 @@
       <c r="L4" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="M4" s="106" t="s">
+      <c r="M4" s="114" t="s">
         <v>82</v>
       </c>
-      <c r="N4" s="107"/>
+      <c r="N4" s="115"/>
       <c r="O4" s="34" t="s">
         <v>62</v>
       </c>
@@ -1993,15 +2003,15 @@
       <c r="M6" s="43" t="s">
         <v>84</v>
       </c>
-      <c r="O6" s="95" t="s">
+      <c r="O6" s="103" t="s">
         <v>66</v>
       </c>
-      <c r="P6" s="96"/>
-      <c r="Q6" s="96"/>
-      <c r="R6" s="96"/>
-      <c r="S6" s="96"/>
-      <c r="T6" s="96"/>
-      <c r="U6" s="96"/>
+      <c r="P6" s="104"/>
+      <c r="Q6" s="104"/>
+      <c r="R6" s="104"/>
+      <c r="S6" s="104"/>
+      <c r="T6" s="104"/>
+      <c r="U6" s="104"/>
     </row>
     <row r="7" spans="1:21" ht="4.5" customHeight="1">
       <c r="A7" s="28"/>
@@ -2024,10 +2034,10 @@
       <c r="B8" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
@@ -2052,10 +2062,10 @@
       <c r="B9" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
@@ -2071,36 +2081,36 @@
       <c r="A10" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="116" t="s">
+      <c r="B10" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="7"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
       <c r="L10" s="4"/>
     </row>
     <row r="11" spans="1:21">
       <c r="A11" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="116" t="s">
+      <c r="B11" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="7"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
       <c r="L11" s="4"/>
       <c r="O11" t="s">
         <v>69</v>
@@ -2111,28 +2121,28 @@
     </row>
     <row r="12" spans="1:21" ht="4.5" customHeight="1">
       <c r="A12" s="28"/>
-      <c r="B12" s="29"/>
-      <c r="C12" s="30"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="30"/>
-      <c r="H12" s="30"/>
-      <c r="I12" s="30"/>
-      <c r="J12" s="30"/>
-      <c r="K12" s="30"/>
-      <c r="L12" s="30"/>
+      <c r="B12" s="57"/>
+      <c r="C12" s="58"/>
+      <c r="D12" s="58"/>
+      <c r="E12" s="58"/>
+      <c r="F12" s="58"/>
+      <c r="G12" s="58"/>
+      <c r="H12" s="58"/>
+      <c r="I12" s="58"/>
+      <c r="J12" s="58"/>
+      <c r="K12" s="58"/>
+      <c r="L12" s="58"/>
     </row>
     <row r="13" spans="1:21">
       <c r="A13" s="38" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="116" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="56" t="s">
         <v>12</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="40"/>
-      <c r="E13" s="114"/>
+      <c r="E13" s="5"/>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
@@ -2141,19 +2151,22 @@
       <c r="K13" s="7"/>
       <c r="L13" s="4"/>
       <c r="O13" t="s">
-        <v>96</v>
+        <v>71</v>
+      </c>
+      <c r="P13" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:21">
       <c r="A14" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="116" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="56" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="40"/>
-      <c r="E14" s="5"/>
+      <c r="E14" s="54"/>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
@@ -2161,24 +2174,19 @@
       <c r="J14" s="5"/>
       <c r="K14" s="7"/>
       <c r="L14" s="4"/>
-      <c r="O14" s="104" t="s">
-        <v>79</v>
-      </c>
-      <c r="P14" s="104"/>
-      <c r="Q14" s="104"/>
-      <c r="R14" s="104"/>
-      <c r="S14" s="104"/>
-      <c r="T14" s="104"/>
-    </row>
-    <row r="15" spans="1:21">
-      <c r="A15" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="B15" s="116" t="s">
-        <v>11</v>
+      <c r="O14" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" ht="15" customHeight="1">
+      <c r="A15" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="56" t="s">
+        <v>12</v>
       </c>
       <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
+      <c r="D15" s="40"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
@@ -2187,22 +2195,24 @@
       <c r="J15" s="5"/>
       <c r="K15" s="7"/>
       <c r="L15" s="4"/>
-      <c r="O15" s="104"/>
-      <c r="P15" s="104"/>
-      <c r="Q15" s="104"/>
-      <c r="R15" s="104"/>
-      <c r="S15" s="104"/>
-      <c r="T15" s="104"/>
+      <c r="O15" s="112" t="s">
+        <v>79</v>
+      </c>
+      <c r="P15" s="112"/>
+      <c r="Q15" s="112"/>
+      <c r="R15" s="112"/>
+      <c r="S15" s="112"/>
+      <c r="T15" s="121"/>
     </row>
     <row r="16" spans="1:21">
-      <c r="A16" s="38" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" s="116" t="s">
-        <v>12</v>
+      <c r="A16" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="56" t="s">
+        <v>11</v>
       </c>
       <c r="C16" s="5"/>
-      <c r="D16" s="40"/>
+      <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
@@ -2211,18 +2221,18 @@
       <c r="J16" s="5"/>
       <c r="K16" s="7"/>
       <c r="L16" s="4"/>
-      <c r="O16" t="s">
-        <v>71</v>
-      </c>
-      <c r="P16" t="s">
-        <v>72</v>
-      </c>
+      <c r="O16" s="112"/>
+      <c r="P16" s="112"/>
+      <c r="Q16" s="112"/>
+      <c r="R16" s="112"/>
+      <c r="S16" s="112"/>
+      <c r="T16" s="121"/>
     </row>
     <row r="17" spans="1:19">
       <c r="A17" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="B17" s="116" t="s">
+      <c r="B17" s="56" t="s">
         <v>11</v>
       </c>
       <c r="C17" s="5"/>
@@ -2269,7 +2279,7 @@
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
       <c r="K19" s="7"/>
-      <c r="L19" s="115"/>
+      <c r="L19" s="55"/>
       <c r="O19" t="s">
         <v>75</v>
       </c>
@@ -2290,7 +2300,7 @@
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
       <c r="K20" s="7"/>
-      <c r="L20" s="115"/>
+      <c r="L20" s="55"/>
     </row>
     <row r="21" spans="1:19" ht="4.5" customHeight="1">
       <c r="A21" s="28"/>
@@ -2351,14 +2361,14 @@
       <c r="J24" s="5"/>
       <c r="K24" s="7"/>
       <c r="L24" s="4"/>
-      <c r="N24" s="54" t="s">
-        <v>90</v>
-      </c>
-      <c r="O24" s="54"/>
-      <c r="P24" s="54"/>
-      <c r="Q24" s="54"/>
-      <c r="R24" s="54"/>
-      <c r="S24" s="54"/>
+      <c r="N24" s="59" t="s">
+        <v>89</v>
+      </c>
+      <c r="O24" s="59"/>
+      <c r="P24" s="59"/>
+      <c r="Q24" s="59"/>
+      <c r="R24" s="59"/>
+      <c r="S24" s="59"/>
     </row>
     <row r="25" spans="1:19">
       <c r="A25" s="39" t="s">
@@ -2395,58 +2405,58 @@
     <row r="27" spans="1:19" ht="15.75" thickBot="1">
       <c r="A27" s="23"/>
       <c r="B27" s="25"/>
-      <c r="C27" s="100" t="s">
+      <c r="C27" s="108" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="101"/>
-      <c r="E27" s="101"/>
-      <c r="F27" s="101"/>
-      <c r="G27" s="102"/>
-      <c r="H27" s="100" t="s">
+      <c r="D27" s="109"/>
+      <c r="E27" s="109"/>
+      <c r="F27" s="109"/>
+      <c r="G27" s="110"/>
+      <c r="H27" s="108" t="s">
         <v>0</v>
       </c>
-      <c r="I27" s="101"/>
-      <c r="J27" s="103"/>
-      <c r="K27" s="102"/>
+      <c r="I27" s="109"/>
+      <c r="J27" s="111"/>
+      <c r="K27" s="110"/>
       <c r="L27" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="N27" s="54"/>
-      <c r="O27" s="54"/>
-      <c r="P27" s="54"/>
-      <c r="Q27" s="54"/>
-      <c r="R27" s="54"/>
-      <c r="S27" s="54"/>
+      <c r="N27" s="122" t="s">
+        <v>118</v>
+      </c>
+      <c r="O27" s="122"/>
+      <c r="P27" s="122"/>
+      <c r="Q27" s="122"/>
+      <c r="R27" s="122"/>
+      <c r="S27" s="122"/>
     </row>
     <row r="28" spans="1:19" ht="30">
-      <c r="A28" s="117" t="s">
+      <c r="A28" s="119" t="s">
         <v>30</v>
       </c>
-      <c r="B28" s="118"/>
-      <c r="C28" s="89" t="s">
-        <v>95</v>
-      </c>
-      <c r="D28" s="90"/>
-      <c r="E28" s="90"/>
-      <c r="F28" s="90"/>
-      <c r="G28" s="91"/>
-      <c r="H28" s="108" t="s">
+      <c r="B28" s="120"/>
+      <c r="C28" s="97" t="s">
+        <v>94</v>
+      </c>
+      <c r="D28" s="98"/>
+      <c r="E28" s="98"/>
+      <c r="F28" s="98"/>
+      <c r="G28" s="99"/>
+      <c r="H28" s="116" t="s">
+        <v>92</v>
+      </c>
+      <c r="I28" s="117"/>
+      <c r="J28" s="117"/>
+      <c r="K28" s="118"/>
+      <c r="L28" s="49" t="s">
         <v>93</v>
       </c>
-      <c r="I28" s="109"/>
-      <c r="J28" s="109"/>
-      <c r="K28" s="110"/>
-      <c r="L28" s="49" t="s">
-        <v>94</v>
-      </c>
-      <c r="N28" s="56" t="s">
-        <v>88</v>
-      </c>
-      <c r="O28" s="56"/>
-      <c r="P28" s="56"/>
-      <c r="Q28" s="56"/>
-      <c r="R28" s="56"/>
-      <c r="S28" s="56"/>
+      <c r="N28" s="122"/>
+      <c r="O28" s="122"/>
+      <c r="P28" s="122"/>
+      <c r="Q28" s="122"/>
+      <c r="R28" s="122"/>
+      <c r="S28" s="122"/>
     </row>
     <row r="29" spans="1:19" ht="4.5" customHeight="1">
       <c r="A29" s="28"/>
@@ -2463,100 +2473,100 @@
       <c r="L29" s="30"/>
     </row>
     <row r="30" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A30" s="65" t="s">
+      <c r="A30" s="70" t="s">
         <v>39</v>
       </c>
-      <c r="B30" s="66"/>
-      <c r="C30" s="81"/>
-      <c r="D30" s="82"/>
-      <c r="E30" s="82"/>
-      <c r="F30" s="82"/>
-      <c r="G30" s="83"/>
-      <c r="H30" s="84"/>
-      <c r="I30" s="82"/>
-      <c r="J30" s="82"/>
-      <c r="K30" s="83"/>
+      <c r="B30" s="71"/>
+      <c r="C30" s="89"/>
+      <c r="D30" s="90"/>
+      <c r="E30" s="90"/>
+      <c r="F30" s="90"/>
+      <c r="G30" s="91"/>
+      <c r="H30" s="92"/>
+      <c r="I30" s="90"/>
+      <c r="J30" s="90"/>
+      <c r="K30" s="91"/>
       <c r="L30" s="21" t="s">
         <v>5</v>
       </c>
       <c r="M30" s="32"/>
-      <c r="N30" s="56" t="s">
+      <c r="N30" s="61" t="s">
         <v>80</v>
       </c>
-      <c r="O30" s="56"/>
-      <c r="P30" s="56"/>
-      <c r="Q30" s="56"/>
-      <c r="R30" s="56"/>
-      <c r="S30" s="56"/>
+      <c r="O30" s="61"/>
+      <c r="P30" s="61"/>
+      <c r="Q30" s="61"/>
+      <c r="R30" s="61"/>
+      <c r="S30" s="61"/>
     </row>
     <row r="31" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A31" s="65" t="s">
+      <c r="A31" s="70" t="s">
         <v>85</v>
       </c>
-      <c r="B31" s="66"/>
-      <c r="C31" s="89"/>
-      <c r="D31" s="90"/>
-      <c r="E31" s="90"/>
-      <c r="F31" s="90"/>
-      <c r="G31" s="91"/>
-      <c r="H31" s="92" t="s">
+      <c r="B31" s="71"/>
+      <c r="C31" s="97"/>
+      <c r="D31" s="98"/>
+      <c r="E31" s="98"/>
+      <c r="F31" s="98"/>
+      <c r="G31" s="99"/>
+      <c r="H31" s="100" t="s">
         <v>86</v>
       </c>
-      <c r="I31" s="93"/>
-      <c r="J31" s="93"/>
-      <c r="K31" s="93"/>
-      <c r="L31" s="94"/>
+      <c r="I31" s="101"/>
+      <c r="J31" s="101"/>
+      <c r="K31" s="101"/>
+      <c r="L31" s="102"/>
       <c r="M31" s="32"/>
-      <c r="N31" s="56" t="s">
+      <c r="N31" s="61" t="s">
         <v>76</v>
       </c>
-      <c r="O31" s="56"/>
-      <c r="P31" s="56"/>
-      <c r="Q31" s="56"/>
-      <c r="R31" s="56"/>
-      <c r="S31" s="56"/>
+      <c r="O31" s="61"/>
+      <c r="P31" s="61"/>
+      <c r="Q31" s="61"/>
+      <c r="R31" s="61"/>
+      <c r="S31" s="61"/>
     </row>
     <row r="32" spans="1:19" ht="16.5" thickBot="1">
-      <c r="A32" s="87" t="s">
+      <c r="A32" s="95" t="s">
         <v>60</v>
       </c>
-      <c r="B32" s="88"/>
-      <c r="C32" s="81"/>
-      <c r="D32" s="82"/>
-      <c r="E32" s="82"/>
-      <c r="F32" s="82"/>
-      <c r="G32" s="83"/>
-      <c r="H32" s="84"/>
-      <c r="I32" s="82"/>
-      <c r="J32" s="82"/>
-      <c r="K32" s="83"/>
+      <c r="B32" s="96"/>
+      <c r="C32" s="89"/>
+      <c r="D32" s="90"/>
+      <c r="E32" s="90"/>
+      <c r="F32" s="90"/>
+      <c r="G32" s="91"/>
+      <c r="H32" s="92"/>
+      <c r="I32" s="90"/>
+      <c r="J32" s="90"/>
+      <c r="K32" s="91"/>
       <c r="M32" s="32"/>
     </row>
     <row r="33" spans="1:19" ht="30.75" customHeight="1" thickBot="1">
-      <c r="A33" s="85" t="s">
+      <c r="A33" s="93" t="s">
         <v>35</v>
       </c>
-      <c r="B33" s="86"/>
-      <c r="C33" s="72" t="s">
+      <c r="B33" s="94"/>
+      <c r="C33" s="77" t="s">
         <v>59</v>
       </c>
-      <c r="D33" s="73"/>
-      <c r="E33" s="73"/>
-      <c r="F33" s="73"/>
-      <c r="G33" s="74"/>
-      <c r="H33" s="69"/>
-      <c r="I33" s="70"/>
-      <c r="J33" s="70"/>
-      <c r="K33" s="71"/>
+      <c r="D33" s="78"/>
+      <c r="E33" s="78"/>
+      <c r="F33" s="78"/>
+      <c r="G33" s="79"/>
+      <c r="H33" s="74"/>
+      <c r="I33" s="75"/>
+      <c r="J33" s="75"/>
+      <c r="K33" s="76"/>
       <c r="M33" s="32"/>
-      <c r="N33" s="55" t="s">
+      <c r="N33" s="60" t="s">
         <v>77</v>
       </c>
-      <c r="O33" s="55"/>
-      <c r="P33" s="55"/>
-      <c r="Q33" s="55"/>
-      <c r="R33" s="55"/>
-      <c r="S33" s="55"/>
+      <c r="O33" s="60"/>
+      <c r="P33" s="60"/>
+      <c r="Q33" s="60"/>
+      <c r="R33" s="60"/>
+      <c r="S33" s="60"/>
     </row>
     <row r="34" spans="1:19" ht="4.5" customHeight="1" thickBot="1">
       <c r="A34" s="28"/>
@@ -2572,111 +2582,116 @@
       <c r="K34" s="30"/>
     </row>
     <row r="35" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A35" s="65" t="s">
+      <c r="A35" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="66"/>
-      <c r="C35" s="111"/>
-      <c r="D35" s="112"/>
-      <c r="E35" s="112"/>
-      <c r="F35" s="112"/>
-      <c r="G35" s="113"/>
-      <c r="H35" s="75"/>
-      <c r="I35" s="76"/>
-      <c r="J35" s="76"/>
-      <c r="K35" s="77"/>
+      <c r="B35" s="71"/>
+      <c r="C35" s="86"/>
+      <c r="D35" s="87"/>
+      <c r="E35" s="87"/>
+      <c r="F35" s="87"/>
+      <c r="G35" s="88"/>
+      <c r="H35" s="80"/>
+      <c r="I35" s="81"/>
+      <c r="J35" s="81"/>
+      <c r="K35" s="82"/>
       <c r="M35" s="32"/>
-      <c r="N35" s="56" t="s">
+      <c r="N35" s="61" t="s">
         <v>78</v>
       </c>
-      <c r="O35" s="56"/>
-      <c r="P35" s="56"/>
-      <c r="Q35" s="56"/>
-      <c r="R35" s="56"/>
-      <c r="S35" s="56"/>
+      <c r="O35" s="61"/>
+      <c r="P35" s="61"/>
+      <c r="Q35" s="61"/>
+      <c r="R35" s="61"/>
+      <c r="S35" s="61"/>
     </row>
     <row r="36" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A36" s="65" t="s">
-        <v>98</v>
-      </c>
-      <c r="B36" s="66"/>
-      <c r="C36" s="111"/>
-      <c r="D36" s="112"/>
-      <c r="E36" s="112"/>
-      <c r="F36" s="112"/>
-      <c r="G36" s="113"/>
-      <c r="H36" s="75"/>
-      <c r="I36" s="76"/>
-      <c r="J36" s="76"/>
-      <c r="K36" s="77"/>
+      <c r="A36" s="70" t="s">
+        <v>96</v>
+      </c>
+      <c r="B36" s="71"/>
+      <c r="C36" s="86"/>
+      <c r="D36" s="87"/>
+      <c r="E36" s="87"/>
+      <c r="F36" s="87"/>
+      <c r="G36" s="88"/>
+      <c r="H36" s="80"/>
+      <c r="I36" s="81"/>
+      <c r="J36" s="81"/>
+      <c r="K36" s="82"/>
       <c r="M36" s="32"/>
-      <c r="N36" s="54" t="s">
+      <c r="N36" s="59" t="s">
         <v>83</v>
       </c>
-      <c r="O36" s="54"/>
-      <c r="P36" s="54"/>
-      <c r="Q36" s="54"/>
-      <c r="R36" s="54"/>
-      <c r="S36" s="54"/>
+      <c r="O36" s="59"/>
+      <c r="P36" s="59"/>
+      <c r="Q36" s="59"/>
+      <c r="R36" s="59"/>
+      <c r="S36" s="59"/>
     </row>
     <row r="37" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A37" s="65" t="s">
+      <c r="A37" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="B37" s="66"/>
-      <c r="C37" s="78"/>
-      <c r="D37" s="79"/>
-      <c r="E37" s="79"/>
-      <c r="F37" s="79"/>
-      <c r="G37" s="80"/>
-      <c r="H37" s="78"/>
-      <c r="I37" s="79"/>
-      <c r="J37" s="79"/>
-      <c r="K37" s="80"/>
+      <c r="B37" s="71"/>
+      <c r="C37" s="83"/>
+      <c r="D37" s="84"/>
+      <c r="E37" s="84"/>
+      <c r="F37" s="84"/>
+      <c r="G37" s="85"/>
+      <c r="H37" s="83"/>
+      <c r="I37" s="84"/>
+      <c r="J37" s="84"/>
+      <c r="K37" s="85"/>
       <c r="M37" s="32"/>
     </row>
     <row r="38" spans="1:19" ht="15.75" thickBot="1">
-      <c r="N38" s="54" t="s">
-        <v>89</v>
-      </c>
-      <c r="O38" s="54"/>
-      <c r="P38" s="54"/>
-      <c r="Q38" s="54"/>
-      <c r="R38" s="54"/>
-      <c r="S38" s="54"/>
+      <c r="N38" s="59" t="s">
+        <v>88</v>
+      </c>
+      <c r="O38" s="59"/>
+      <c r="P38" s="59"/>
+      <c r="Q38" s="59"/>
+      <c r="R38" s="59"/>
+      <c r="S38" s="59"/>
     </row>
     <row r="39" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A39" s="58" t="s">
+      <c r="A39" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="B39" s="59"/>
-      <c r="C39" s="59"/>
-      <c r="D39" s="59"/>
-      <c r="E39" s="60"/>
+      <c r="B39" s="64"/>
+      <c r="C39" s="64"/>
+      <c r="D39" s="64"/>
+      <c r="E39" s="65"/>
     </row>
     <row r="40" spans="1:19">
       <c r="A40" s="14" t="s">
         <v>25</v>
       </c>
       <c r="B40" s="13"/>
-      <c r="C40" s="61" t="s">
+      <c r="C40" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="D40" s="62"/>
+      <c r="D40" s="67"/>
       <c r="E40" s="27"/>
-      <c r="N40" t="s">
-        <v>97</v>
-      </c>
+      <c r="N40" s="59" t="s">
+        <v>117</v>
+      </c>
+      <c r="O40" s="59"/>
+      <c r="P40" s="59"/>
+      <c r="Q40" s="59"/>
+      <c r="R40" s="59"/>
+      <c r="S40" s="59"/>
     </row>
     <row r="41" spans="1:19">
       <c r="A41" s="15" t="s">
         <v>21</v>
       </c>
       <c r="B41" s="5"/>
-      <c r="C41" s="61" t="s">
+      <c r="C41" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="D41" s="62"/>
+      <c r="D41" s="67"/>
       <c r="E41" s="8"/>
     </row>
     <row r="42" spans="1:19">
@@ -2684,10 +2699,10 @@
         <v>24</v>
       </c>
       <c r="B42" s="6"/>
-      <c r="C42" s="67" t="s">
+      <c r="C42" s="72" t="s">
         <v>65</v>
       </c>
-      <c r="D42" s="68"/>
+      <c r="D42" s="73"/>
       <c r="E42" s="37"/>
     </row>
     <row r="43" spans="1:19" ht="18" thickBot="1">
@@ -2695,179 +2710,179 @@
         <v>4</v>
       </c>
       <c r="O43" s="44" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="44" spans="1:19">
-      <c r="A44" s="63" t="s">
+      <c r="A44" s="68" t="s">
         <v>36</v>
       </c>
-      <c r="B44" s="64"/>
-      <c r="C44" s="64"/>
-      <c r="D44" s="64"/>
-      <c r="E44" s="64"/>
-      <c r="F44" s="64"/>
-      <c r="G44" s="64"/>
-      <c r="H44" s="64"/>
-      <c r="I44" s="64"/>
-      <c r="J44" s="64"/>
-      <c r="K44" s="64"/>
-      <c r="L44" s="64"/>
+      <c r="B44" s="69"/>
+      <c r="C44" s="69"/>
+      <c r="D44" s="69"/>
+      <c r="E44" s="69"/>
+      <c r="F44" s="69"/>
+      <c r="G44" s="69"/>
+      <c r="H44" s="69"/>
+      <c r="I44" s="69"/>
+      <c r="J44" s="69"/>
+      <c r="K44" s="69"/>
+      <c r="L44" s="69"/>
       <c r="O44" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="45" spans="1:19">
       <c r="A45" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="B45" s="57" t="s">
+      <c r="B45" s="62" t="s">
         <v>56</v>
       </c>
-      <c r="C45" s="57"/>
-      <c r="D45" s="57"/>
-      <c r="E45" s="57"/>
-      <c r="F45" s="57"/>
-      <c r="G45" s="57"/>
-      <c r="H45" s="57"/>
-      <c r="I45" s="57"/>
-      <c r="J45" s="57"/>
-      <c r="K45" s="57"/>
-      <c r="L45" s="57"/>
+      <c r="C45" s="62"/>
+      <c r="D45" s="62"/>
+      <c r="E45" s="62"/>
+      <c r="F45" s="62"/>
+      <c r="G45" s="62"/>
+      <c r="H45" s="62"/>
+      <c r="I45" s="62"/>
+      <c r="J45" s="62"/>
+      <c r="K45" s="62"/>
+      <c r="L45" s="62"/>
     </row>
     <row r="46" spans="1:19" ht="15" customHeight="1">
       <c r="A46" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="B46" s="57" t="s">
+      <c r="B46" s="62" t="s">
         <v>57</v>
       </c>
-      <c r="C46" s="57"/>
-      <c r="D46" s="57"/>
-      <c r="E46" s="57"/>
-      <c r="F46" s="57"/>
-      <c r="G46" s="57"/>
-      <c r="H46" s="57"/>
-      <c r="I46" s="57"/>
-      <c r="J46" s="57"/>
-      <c r="K46" s="57"/>
-      <c r="L46" s="57"/>
+      <c r="C46" s="62"/>
+      <c r="D46" s="62"/>
+      <c r="E46" s="62"/>
+      <c r="F46" s="62"/>
+      <c r="G46" s="62"/>
+      <c r="H46" s="62"/>
+      <c r="I46" s="62"/>
+      <c r="J46" s="62"/>
+      <c r="K46" s="62"/>
+      <c r="L46" s="62"/>
       <c r="N46" s="50" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="O46" s="44" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="47" spans="1:19" ht="17.25">
       <c r="A47" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="B47" s="57" t="s">
+      <c r="B47" s="62" t="s">
         <v>58</v>
       </c>
-      <c r="C47" s="57"/>
-      <c r="D47" s="57"/>
-      <c r="E47" s="57"/>
-      <c r="F47" s="57"/>
-      <c r="G47" s="57"/>
-      <c r="H47" s="57"/>
-      <c r="I47" s="57"/>
-      <c r="J47" s="57"/>
-      <c r="K47" s="57"/>
-      <c r="L47" s="57"/>
+      <c r="C47" s="62"/>
+      <c r="D47" s="62"/>
+      <c r="E47" s="62"/>
+      <c r="F47" s="62"/>
+      <c r="G47" s="62"/>
+      <c r="H47" s="62"/>
+      <c r="I47" s="62"/>
+      <c r="J47" s="62"/>
+      <c r="K47" s="62"/>
+      <c r="L47" s="62"/>
       <c r="O47" s="44" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="48" spans="1:19">
       <c r="A48" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="B48" s="57" t="s">
+      <c r="B48" s="62" t="s">
         <v>45</v>
       </c>
-      <c r="C48" s="57"/>
-      <c r="D48" s="57"/>
-      <c r="E48" s="57"/>
-      <c r="F48" s="57"/>
-      <c r="G48" s="57"/>
-      <c r="H48" s="57"/>
-      <c r="I48" s="57"/>
-      <c r="J48" s="57"/>
-      <c r="K48" s="57"/>
-      <c r="L48" s="57"/>
+      <c r="C48" s="62"/>
+      <c r="D48" s="62"/>
+      <c r="E48" s="62"/>
+      <c r="F48" s="62"/>
+      <c r="G48" s="62"/>
+      <c r="H48" s="62"/>
+      <c r="I48" s="62"/>
+      <c r="J48" s="62"/>
+      <c r="K48" s="62"/>
+      <c r="L48" s="62"/>
       <c r="O48" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="49" spans="1:15">
       <c r="A49" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="B49" s="57" t="s">
+      <c r="B49" s="62" t="s">
         <v>34</v>
       </c>
-      <c r="C49" s="57"/>
-      <c r="D49" s="57"/>
-      <c r="E49" s="57"/>
-      <c r="F49" s="57"/>
-      <c r="G49" s="57"/>
-      <c r="H49" s="57"/>
-      <c r="I49" s="57"/>
-      <c r="J49" s="57"/>
-      <c r="K49" s="57"/>
-      <c r="L49" s="57"/>
+      <c r="C49" s="62"/>
+      <c r="D49" s="62"/>
+      <c r="E49" s="62"/>
+      <c r="F49" s="62"/>
+      <c r="G49" s="62"/>
+      <c r="H49" s="62"/>
+      <c r="I49" s="62"/>
+      <c r="J49" s="62"/>
+      <c r="K49" s="62"/>
+      <c r="L49" s="62"/>
     </row>
     <row r="50" spans="1:15" ht="17.25">
       <c r="A50" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="B50" s="57" t="s">
+      <c r="B50" s="62" t="s">
         <v>55</v>
       </c>
-      <c r="C50" s="57"/>
-      <c r="D50" s="57"/>
-      <c r="E50" s="57"/>
-      <c r="F50" s="57"/>
-      <c r="G50" s="57"/>
-      <c r="H50" s="57"/>
-      <c r="I50" s="57"/>
-      <c r="J50" s="57"/>
-      <c r="K50" s="57"/>
-      <c r="L50" s="57"/>
+      <c r="C50" s="62"/>
+      <c r="D50" s="62"/>
+      <c r="E50" s="62"/>
+      <c r="F50" s="62"/>
+      <c r="G50" s="62"/>
+      <c r="H50" s="62"/>
+      <c r="I50" s="62"/>
+      <c r="J50" s="62"/>
+      <c r="K50" s="62"/>
+      <c r="L50" s="62"/>
       <c r="N50" s="50" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="O50" s="44" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="51" spans="1:15">
       <c r="A51" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="B51" s="57" t="s">
+      <c r="B51" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="C51" s="57"/>
-      <c r="D51" s="57"/>
-      <c r="E51" s="57"/>
-      <c r="F51" s="57"/>
-      <c r="G51" s="57"/>
-      <c r="H51" s="57"/>
-      <c r="I51" s="57"/>
-      <c r="J51" s="57"/>
-      <c r="K51" s="57"/>
-      <c r="L51" s="57"/>
+      <c r="C51" s="62"/>
+      <c r="D51" s="62"/>
+      <c r="E51" s="62"/>
+      <c r="F51" s="62"/>
+      <c r="G51" s="62"/>
+      <c r="H51" s="62"/>
+      <c r="I51" s="62"/>
+      <c r="J51" s="62"/>
+      <c r="K51" s="62"/>
+      <c r="L51" s="62"/>
       <c r="O51" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="52" spans="1:15">
       <c r="C52" s="32"/>
       <c r="O52" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="53" spans="1:15">
@@ -2881,6 +2896,8 @@
     <sortCondition ref="A3"/>
   </sortState>
   <mergeCells count="55">
+    <mergeCell ref="O15:S16"/>
+    <mergeCell ref="N27:S28"/>
     <mergeCell ref="N24:S24"/>
     <mergeCell ref="N38:S38"/>
     <mergeCell ref="N36:S36"/>
@@ -2889,7 +2906,6 @@
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C27:G27"/>
     <mergeCell ref="H27:K27"/>
-    <mergeCell ref="O14:T15"/>
     <mergeCell ref="M3:N3"/>
     <mergeCell ref="M4:N4"/>
     <mergeCell ref="C28:G28"/>
@@ -2930,11 +2946,10 @@
     <mergeCell ref="B47:L47"/>
     <mergeCell ref="B48:L48"/>
     <mergeCell ref="B49:L49"/>
-    <mergeCell ref="N27:S27"/>
+    <mergeCell ref="N40:S40"/>
     <mergeCell ref="N33:S33"/>
     <mergeCell ref="N35:S35"/>
     <mergeCell ref="N30:S30"/>
-    <mergeCell ref="N28:S28"/>
     <mergeCell ref="N31:S31"/>
   </mergeCells>
   <hyperlinks>
@@ -2967,31 +2982,31 @@
   <sheetData>
     <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B3" s="1"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="52" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B4" s="52"/>
       <c r="C4" s="52" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="52" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E4" s="52" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="51" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B5" s="51" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C5" s="52"/>
       <c r="D5" s="52"/>
@@ -3000,16 +3015,16 @@
     <row r="6" spans="1:6">
       <c r="A6" s="51"/>
       <c r="B6" s="51" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C6" s="52" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D6" s="52" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E6" s="52" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -3021,10 +3036,10 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="51" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B8" s="51" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C8" s="52"/>
       <c r="D8" s="52"/>
@@ -3033,16 +3048,16 @@
     <row r="9" spans="1:6">
       <c r="A9" s="51"/>
       <c r="B9" s="51" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C9" s="52" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D9" s="52" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E9" s="52" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -3054,10 +3069,10 @@
     </row>
     <row r="11" spans="1:6" ht="15.75">
       <c r="A11" s="51" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B11" s="51" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C11" s="52"/>
       <c r="D11" s="52"/>
@@ -3067,16 +3082,16 @@
     <row r="12" spans="1:6">
       <c r="A12" s="51"/>
       <c r="B12" s="51" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C12" s="52" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D12" s="52" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E12" s="52" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
actualizado cuadro de estado, y el readme
</commit_message>
<xml_diff>
--- a/Cuadro-de-estado.xlsx
+++ b/Cuadro-de-estado.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="118">
   <si>
     <t>BACKEND</t>
   </si>
@@ -328,9 +328,6 @@
     <t>Validation form</t>
   </si>
   <si>
-    <t>Agregar atributo en Person, con la url de ubicación de google.maps</t>
-  </si>
-  <si>
     <t>Aún existen componentes/servicios que apuntan a mock-data</t>
   </si>
   <si>
@@ -457,7 +454,7 @@
     <t>A las Card init, las está tomando del archivo .json</t>
   </si>
   <si>
-    <t>Tengo problemas para borrar un alta, despues de su modificacion, lo arrastra incluso a otros componentes, como que es algo que queda pendiente de realizar, pero en verdad ya lo habia borrado la primera vez.</t>
+    <t>Incorporar en los Form, el atributo url</t>
   </si>
 </sst>
 </file>
@@ -1353,197 +1350,197 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1847,7 +1844,7 @@
   <dimension ref="A1:U54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1864,62 +1861,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25">
-      <c r="A1" s="105" t="s">
-        <v>90</v>
-      </c>
-      <c r="B1" s="105"/>
-      <c r="C1" s="105"/>
-      <c r="D1" s="105"/>
-      <c r="E1" s="105"/>
-      <c r="F1" s="105"/>
-      <c r="G1" s="105"/>
-      <c r="H1" s="105"/>
-      <c r="I1" s="105"/>
-      <c r="J1" s="105"/>
-      <c r="K1" s="105"/>
-      <c r="L1" s="105"/>
+      <c r="A1" s="64" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="64"/>
+      <c r="J1" s="64"/>
+      <c r="K1" s="64"/>
+      <c r="L1" s="64"/>
     </row>
     <row r="2" spans="1:21" ht="19.5" thickBot="1">
       <c r="A2" s="46">
         <f ca="1">M2-TODAY()-1</f>
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="47" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C2" s="48"/>
       <c r="M2" s="45">
         <v>45011</v>
       </c>
       <c r="O2" s="44" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="106" t="s">
+      <c r="A3" s="65" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="107"/>
-      <c r="C3" s="108" t="s">
+      <c r="B3" s="66"/>
+      <c r="C3" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="109"/>
-      <c r="E3" s="109"/>
-      <c r="F3" s="109"/>
-      <c r="G3" s="110"/>
-      <c r="H3" s="108" t="s">
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="68"/>
+      <c r="G3" s="69"/>
+      <c r="H3" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="109"/>
-      <c r="J3" s="111"/>
-      <c r="K3" s="110"/>
+      <c r="I3" s="68"/>
+      <c r="J3" s="70"/>
+      <c r="K3" s="69"/>
       <c r="L3" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="113" t="s">
-        <v>81</v>
-      </c>
-      <c r="N3" s="104"/>
+      <c r="M3" s="71" t="s">
+        <v>80</v>
+      </c>
+      <c r="N3" s="63"/>
     </row>
     <row r="4" spans="1:21" s="3" customFormat="1" ht="40.5" customHeight="1" thickBot="1">
       <c r="A4" s="17" t="s">
@@ -1958,10 +1955,10 @@
       <c r="L4" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="M4" s="114" t="s">
-        <v>82</v>
-      </c>
-      <c r="N4" s="115"/>
+      <c r="M4" s="72" t="s">
+        <v>81</v>
+      </c>
+      <c r="N4" s="73"/>
       <c r="O4" s="34" t="s">
         <v>62</v>
       </c>
@@ -2001,17 +1998,17 @@
       <c r="K6" s="5"/>
       <c r="L6" s="4"/>
       <c r="M6" s="43" t="s">
-        <v>84</v>
-      </c>
-      <c r="O6" s="103" t="s">
+        <v>83</v>
+      </c>
+      <c r="O6" s="62" t="s">
         <v>66</v>
       </c>
-      <c r="P6" s="104"/>
-      <c r="Q6" s="104"/>
-      <c r="R6" s="104"/>
-      <c r="S6" s="104"/>
-      <c r="T6" s="104"/>
-      <c r="U6" s="104"/>
+      <c r="P6" s="63"/>
+      <c r="Q6" s="63"/>
+      <c r="R6" s="63"/>
+      <c r="S6" s="63"/>
+      <c r="T6" s="63"/>
+      <c r="U6" s="63"/>
     </row>
     <row r="7" spans="1:21" ht="4.5" customHeight="1">
       <c r="A7" s="28"/>
@@ -2137,18 +2134,18 @@
       <c r="A13" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="56" t="s">
+      <c r="B13" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="5"/>
+      <c r="C13" s="4"/>
       <c r="D13" s="40"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="7"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
       <c r="L13" s="4"/>
       <c r="O13" t="s">
         <v>71</v>
@@ -2175,7 +2172,7 @@
       <c r="K14" s="7"/>
       <c r="L14" s="4"/>
       <c r="O14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="15" customHeight="1">
@@ -2195,14 +2192,14 @@
       <c r="J15" s="5"/>
       <c r="K15" s="7"/>
       <c r="L15" s="4"/>
-      <c r="O15" s="112" t="s">
-        <v>79</v>
-      </c>
-      <c r="P15" s="112"/>
-      <c r="Q15" s="112"/>
-      <c r="R15" s="112"/>
-      <c r="S15" s="112"/>
-      <c r="T15" s="121"/>
+      <c r="O15" s="60" t="s">
+        <v>78</v>
+      </c>
+      <c r="P15" s="60"/>
+      <c r="Q15" s="60"/>
+      <c r="R15" s="60"/>
+      <c r="S15" s="60"/>
+      <c r="T15" s="59"/>
     </row>
     <row r="16" spans="1:21">
       <c r="A16" s="18" t="s">
@@ -2221,12 +2218,12 @@
       <c r="J16" s="5"/>
       <c r="K16" s="7"/>
       <c r="L16" s="4"/>
-      <c r="O16" s="112"/>
-      <c r="P16" s="112"/>
-      <c r="Q16" s="112"/>
-      <c r="R16" s="112"/>
-      <c r="S16" s="112"/>
-      <c r="T16" s="121"/>
+      <c r="O16" s="60"/>
+      <c r="P16" s="60"/>
+      <c r="Q16" s="60"/>
+      <c r="R16" s="60"/>
+      <c r="S16" s="60"/>
+      <c r="T16" s="59"/>
     </row>
     <row r="17" spans="1:19">
       <c r="A17" s="18" t="s">
@@ -2280,9 +2277,6 @@
       <c r="J19" s="5"/>
       <c r="K19" s="7"/>
       <c r="L19" s="55"/>
-      <c r="O19" t="s">
-        <v>75</v>
-      </c>
     </row>
     <row r="20" spans="1:19">
       <c r="A20" s="39" t="s">
@@ -2361,14 +2355,14 @@
       <c r="J24" s="5"/>
       <c r="K24" s="7"/>
       <c r="L24" s="4"/>
-      <c r="N24" s="59" t="s">
-        <v>89</v>
-      </c>
-      <c r="O24" s="59"/>
-      <c r="P24" s="59"/>
-      <c r="Q24" s="59"/>
-      <c r="R24" s="59"/>
-      <c r="S24" s="59"/>
+      <c r="N24" s="61" t="s">
+        <v>88</v>
+      </c>
+      <c r="O24" s="61"/>
+      <c r="P24" s="61"/>
+      <c r="Q24" s="61"/>
+      <c r="R24" s="61"/>
+      <c r="S24" s="61"/>
     </row>
     <row r="25" spans="1:19">
       <c r="A25" s="39" t="s">
@@ -2405,53 +2399,55 @@
     <row r="27" spans="1:19" ht="15.75" thickBot="1">
       <c r="A27" s="23"/>
       <c r="B27" s="25"/>
-      <c r="C27" s="108" t="s">
+      <c r="C27" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="109"/>
-      <c r="E27" s="109"/>
-      <c r="F27" s="109"/>
-      <c r="G27" s="110"/>
-      <c r="H27" s="108" t="s">
+      <c r="D27" s="68"/>
+      <c r="E27" s="68"/>
+      <c r="F27" s="68"/>
+      <c r="G27" s="69"/>
+      <c r="H27" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="I27" s="109"/>
-      <c r="J27" s="111"/>
-      <c r="K27" s="110"/>
+      <c r="I27" s="68"/>
+      <c r="J27" s="70"/>
+      <c r="K27" s="69"/>
       <c r="L27" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="N27" s="122" t="s">
-        <v>118</v>
-      </c>
-      <c r="O27" s="122"/>
-      <c r="P27" s="122"/>
-      <c r="Q27" s="122"/>
-      <c r="R27" s="122"/>
-      <c r="S27" s="122"/>
+      <c r="N27" s="61" t="s">
+        <v>82</v>
+      </c>
+      <c r="O27" s="61"/>
+      <c r="P27" s="61"/>
+      <c r="Q27" s="61"/>
+      <c r="R27" s="61"/>
+      <c r="S27" s="61"/>
     </row>
     <row r="28" spans="1:19" ht="30">
-      <c r="A28" s="119" t="s">
+      <c r="A28" s="80" t="s">
         <v>30</v>
       </c>
-      <c r="B28" s="120"/>
-      <c r="C28" s="97" t="s">
-        <v>94</v>
-      </c>
-      <c r="D28" s="98"/>
-      <c r="E28" s="98"/>
-      <c r="F28" s="98"/>
-      <c r="G28" s="99"/>
-      <c r="H28" s="116" t="s">
+      <c r="B28" s="81"/>
+      <c r="C28" s="74" t="s">
+        <v>93</v>
+      </c>
+      <c r="D28" s="75"/>
+      <c r="E28" s="75"/>
+      <c r="F28" s="75"/>
+      <c r="G28" s="76"/>
+      <c r="H28" s="77" t="s">
+        <v>91</v>
+      </c>
+      <c r="I28" s="78"/>
+      <c r="J28" s="78"/>
+      <c r="K28" s="79"/>
+      <c r="L28" s="49" t="s">
         <v>92</v>
       </c>
-      <c r="I28" s="117"/>
-      <c r="J28" s="117"/>
-      <c r="K28" s="118"/>
-      <c r="L28" s="49" t="s">
-        <v>93</v>
-      </c>
-      <c r="N28" s="122"/>
+      <c r="N28" s="122" t="s">
+        <v>117</v>
+      </c>
       <c r="O28" s="122"/>
       <c r="P28" s="122"/>
       <c r="Q28" s="122"/>
@@ -2473,100 +2469,100 @@
       <c r="L29" s="30"/>
     </row>
     <row r="30" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A30" s="70" t="s">
+      <c r="A30" s="86" t="s">
         <v>39</v>
       </c>
-      <c r="B30" s="71"/>
-      <c r="C30" s="89"/>
-      <c r="D30" s="90"/>
-      <c r="E30" s="90"/>
-      <c r="F30" s="90"/>
-      <c r="G30" s="91"/>
-      <c r="H30" s="92"/>
-      <c r="I30" s="90"/>
-      <c r="J30" s="90"/>
-      <c r="K30" s="91"/>
+      <c r="B30" s="87"/>
+      <c r="C30" s="82"/>
+      <c r="D30" s="83"/>
+      <c r="E30" s="83"/>
+      <c r="F30" s="83"/>
+      <c r="G30" s="84"/>
+      <c r="H30" s="85"/>
+      <c r="I30" s="83"/>
+      <c r="J30" s="83"/>
+      <c r="K30" s="84"/>
       <c r="L30" s="21" t="s">
         <v>5</v>
       </c>
       <c r="M30" s="32"/>
-      <c r="N30" s="61" t="s">
-        <v>80</v>
-      </c>
-      <c r="O30" s="61"/>
-      <c r="P30" s="61"/>
-      <c r="Q30" s="61"/>
-      <c r="R30" s="61"/>
-      <c r="S30" s="61"/>
+      <c r="N30" s="121" t="s">
+        <v>79</v>
+      </c>
+      <c r="O30" s="121"/>
+      <c r="P30" s="121"/>
+      <c r="Q30" s="121"/>
+      <c r="R30" s="121"/>
+      <c r="S30" s="121"/>
     </row>
     <row r="31" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A31" s="70" t="s">
+      <c r="A31" s="86" t="s">
+        <v>84</v>
+      </c>
+      <c r="B31" s="87"/>
+      <c r="C31" s="74"/>
+      <c r="D31" s="75"/>
+      <c r="E31" s="75"/>
+      <c r="F31" s="75"/>
+      <c r="G31" s="76"/>
+      <c r="H31" s="92" t="s">
         <v>85</v>
       </c>
-      <c r="B31" s="71"/>
-      <c r="C31" s="97"/>
-      <c r="D31" s="98"/>
-      <c r="E31" s="98"/>
-      <c r="F31" s="98"/>
-      <c r="G31" s="99"/>
-      <c r="H31" s="100" t="s">
-        <v>86</v>
-      </c>
-      <c r="I31" s="101"/>
-      <c r="J31" s="101"/>
-      <c r="K31" s="101"/>
-      <c r="L31" s="102"/>
+      <c r="I31" s="93"/>
+      <c r="J31" s="93"/>
+      <c r="K31" s="93"/>
+      <c r="L31" s="94"/>
       <c r="M31" s="32"/>
-      <c r="N31" s="61" t="s">
+      <c r="N31" s="121" t="s">
+        <v>75</v>
+      </c>
+      <c r="O31" s="121"/>
+      <c r="P31" s="121"/>
+      <c r="Q31" s="121"/>
+      <c r="R31" s="121"/>
+      <c r="S31" s="121"/>
+    </row>
+    <row r="32" spans="1:19" ht="16.5" thickBot="1">
+      <c r="A32" s="90" t="s">
+        <v>60</v>
+      </c>
+      <c r="B32" s="91"/>
+      <c r="C32" s="82"/>
+      <c r="D32" s="83"/>
+      <c r="E32" s="83"/>
+      <c r="F32" s="83"/>
+      <c r="G32" s="84"/>
+      <c r="H32" s="85"/>
+      <c r="I32" s="83"/>
+      <c r="J32" s="83"/>
+      <c r="K32" s="84"/>
+      <c r="M32" s="32"/>
+    </row>
+    <row r="33" spans="1:19" ht="30.75" customHeight="1" thickBot="1">
+      <c r="A33" s="88" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33" s="89"/>
+      <c r="C33" s="100" t="s">
+        <v>59</v>
+      </c>
+      <c r="D33" s="101"/>
+      <c r="E33" s="101"/>
+      <c r="F33" s="101"/>
+      <c r="G33" s="102"/>
+      <c r="H33" s="97"/>
+      <c r="I33" s="98"/>
+      <c r="J33" s="98"/>
+      <c r="K33" s="99"/>
+      <c r="M33" s="32"/>
+      <c r="N33" s="120" t="s">
         <v>76</v>
       </c>
-      <c r="O31" s="61"/>
-      <c r="P31" s="61"/>
-      <c r="Q31" s="61"/>
-      <c r="R31" s="61"/>
-      <c r="S31" s="61"/>
-    </row>
-    <row r="32" spans="1:19" ht="16.5" thickBot="1">
-      <c r="A32" s="95" t="s">
-        <v>60</v>
-      </c>
-      <c r="B32" s="96"/>
-      <c r="C32" s="89"/>
-      <c r="D32" s="90"/>
-      <c r="E32" s="90"/>
-      <c r="F32" s="90"/>
-      <c r="G32" s="91"/>
-      <c r="H32" s="92"/>
-      <c r="I32" s="90"/>
-      <c r="J32" s="90"/>
-      <c r="K32" s="91"/>
-      <c r="M32" s="32"/>
-    </row>
-    <row r="33" spans="1:19" ht="30.75" customHeight="1" thickBot="1">
-      <c r="A33" s="93" t="s">
-        <v>35</v>
-      </c>
-      <c r="B33" s="94"/>
-      <c r="C33" s="77" t="s">
-        <v>59</v>
-      </c>
-      <c r="D33" s="78"/>
-      <c r="E33" s="78"/>
-      <c r="F33" s="78"/>
-      <c r="G33" s="79"/>
-      <c r="H33" s="74"/>
-      <c r="I33" s="75"/>
-      <c r="J33" s="75"/>
-      <c r="K33" s="76"/>
-      <c r="M33" s="32"/>
-      <c r="N33" s="60" t="s">
-        <v>77</v>
-      </c>
-      <c r="O33" s="60"/>
-      <c r="P33" s="60"/>
-      <c r="Q33" s="60"/>
-      <c r="R33" s="60"/>
-      <c r="S33" s="60"/>
+      <c r="O33" s="120"/>
+      <c r="P33" s="120"/>
+      <c r="Q33" s="120"/>
+      <c r="R33" s="120"/>
+      <c r="S33" s="120"/>
     </row>
     <row r="34" spans="1:19" ht="4.5" customHeight="1" thickBot="1">
       <c r="A34" s="28"/>
@@ -2582,116 +2578,108 @@
       <c r="K34" s="30"/>
     </row>
     <row r="35" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A35" s="70" t="s">
+      <c r="A35" s="86" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="71"/>
-      <c r="C35" s="86"/>
-      <c r="D35" s="87"/>
-      <c r="E35" s="87"/>
-      <c r="F35" s="87"/>
-      <c r="G35" s="88"/>
-      <c r="H35" s="80"/>
-      <c r="I35" s="81"/>
-      <c r="J35" s="81"/>
-      <c r="K35" s="82"/>
+      <c r="B35" s="87"/>
+      <c r="C35" s="109"/>
+      <c r="D35" s="110"/>
+      <c r="E35" s="110"/>
+      <c r="F35" s="110"/>
+      <c r="G35" s="111"/>
+      <c r="H35" s="103"/>
+      <c r="I35" s="104"/>
+      <c r="J35" s="104"/>
+      <c r="K35" s="105"/>
       <c r="M35" s="32"/>
-      <c r="N35" s="61" t="s">
-        <v>78</v>
-      </c>
-      <c r="O35" s="61"/>
-      <c r="P35" s="61"/>
-      <c r="Q35" s="61"/>
-      <c r="R35" s="61"/>
-      <c r="S35" s="61"/>
     </row>
     <row r="36" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A36" s="70" t="s">
-        <v>96</v>
-      </c>
-      <c r="B36" s="71"/>
-      <c r="C36" s="86"/>
-      <c r="D36" s="87"/>
-      <c r="E36" s="87"/>
-      <c r="F36" s="87"/>
-      <c r="G36" s="88"/>
-      <c r="H36" s="80"/>
-      <c r="I36" s="81"/>
-      <c r="J36" s="81"/>
-      <c r="K36" s="82"/>
+      <c r="A36" s="86" t="s">
+        <v>95</v>
+      </c>
+      <c r="B36" s="87"/>
+      <c r="C36" s="109"/>
+      <c r="D36" s="110"/>
+      <c r="E36" s="110"/>
+      <c r="F36" s="110"/>
+      <c r="G36" s="111"/>
+      <c r="H36" s="103"/>
+      <c r="I36" s="104"/>
+      <c r="J36" s="104"/>
+      <c r="K36" s="105"/>
       <c r="M36" s="32"/>
-      <c r="N36" s="59" t="s">
-        <v>83</v>
-      </c>
-      <c r="O36" s="59"/>
-      <c r="P36" s="59"/>
-      <c r="Q36" s="59"/>
-      <c r="R36" s="59"/>
-      <c r="S36" s="59"/>
+      <c r="N36" s="121" t="s">
+        <v>77</v>
+      </c>
+      <c r="O36" s="121"/>
+      <c r="P36" s="121"/>
+      <c r="Q36" s="121"/>
+      <c r="R36" s="121"/>
+      <c r="S36" s="121"/>
     </row>
     <row r="37" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A37" s="70" t="s">
+      <c r="A37" s="86" t="s">
         <v>7</v>
       </c>
-      <c r="B37" s="71"/>
-      <c r="C37" s="83"/>
-      <c r="D37" s="84"/>
-      <c r="E37" s="84"/>
-      <c r="F37" s="84"/>
-      <c r="G37" s="85"/>
-      <c r="H37" s="83"/>
-      <c r="I37" s="84"/>
-      <c r="J37" s="84"/>
-      <c r="K37" s="85"/>
+      <c r="B37" s="87"/>
+      <c r="C37" s="106"/>
+      <c r="D37" s="107"/>
+      <c r="E37" s="107"/>
+      <c r="F37" s="107"/>
+      <c r="G37" s="108"/>
+      <c r="H37" s="106"/>
+      <c r="I37" s="107"/>
+      <c r="J37" s="107"/>
+      <c r="K37" s="108"/>
       <c r="M37" s="32"/>
     </row>
     <row r="38" spans="1:19" ht="15.75" thickBot="1">
-      <c r="N38" s="59" t="s">
-        <v>88</v>
-      </c>
-      <c r="O38" s="59"/>
-      <c r="P38" s="59"/>
-      <c r="Q38" s="59"/>
-      <c r="R38" s="59"/>
-      <c r="S38" s="59"/>
+      <c r="N38" s="61" t="s">
+        <v>87</v>
+      </c>
+      <c r="O38" s="61"/>
+      <c r="P38" s="61"/>
+      <c r="Q38" s="61"/>
+      <c r="R38" s="61"/>
+      <c r="S38" s="61"/>
     </row>
     <row r="39" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A39" s="63" t="s">
+      <c r="A39" s="113" t="s">
         <v>26</v>
       </c>
-      <c r="B39" s="64"/>
-      <c r="C39" s="64"/>
-      <c r="D39" s="64"/>
-      <c r="E39" s="65"/>
+      <c r="B39" s="114"/>
+      <c r="C39" s="114"/>
+      <c r="D39" s="114"/>
+      <c r="E39" s="115"/>
     </row>
     <row r="40" spans="1:19">
       <c r="A40" s="14" t="s">
         <v>25</v>
       </c>
       <c r="B40" s="13"/>
-      <c r="C40" s="66" t="s">
+      <c r="C40" s="116" t="s">
         <v>22</v>
       </c>
-      <c r="D40" s="67"/>
+      <c r="D40" s="117"/>
       <c r="E40" s="27"/>
-      <c r="N40" s="59" t="s">
-        <v>117</v>
-      </c>
-      <c r="O40" s="59"/>
-      <c r="P40" s="59"/>
-      <c r="Q40" s="59"/>
-      <c r="R40" s="59"/>
-      <c r="S40" s="59"/>
+      <c r="N40" s="61" t="s">
+        <v>116</v>
+      </c>
+      <c r="O40" s="61"/>
+      <c r="P40" s="61"/>
+      <c r="Q40" s="61"/>
+      <c r="R40" s="61"/>
+      <c r="S40" s="61"/>
     </row>
     <row r="41" spans="1:19">
       <c r="A41" s="15" t="s">
         <v>21</v>
       </c>
       <c r="B41" s="5"/>
-      <c r="C41" s="66" t="s">
+      <c r="C41" s="116" t="s">
         <v>23</v>
       </c>
-      <c r="D41" s="67"/>
+      <c r="D41" s="117"/>
       <c r="E41" s="8"/>
     </row>
     <row r="42" spans="1:19">
@@ -2699,10 +2687,10 @@
         <v>24</v>
       </c>
       <c r="B42" s="6"/>
-      <c r="C42" s="72" t="s">
+      <c r="C42" s="95" t="s">
         <v>65</v>
       </c>
-      <c r="D42" s="73"/>
+      <c r="D42" s="96"/>
       <c r="E42" s="37"/>
     </row>
     <row r="43" spans="1:19" ht="18" thickBot="1">
@@ -2710,179 +2698,179 @@
         <v>4</v>
       </c>
       <c r="O43" s="44" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19">
+      <c r="A44" s="118" t="s">
+        <v>36</v>
+      </c>
+      <c r="B44" s="119"/>
+      <c r="C44" s="119"/>
+      <c r="D44" s="119"/>
+      <c r="E44" s="119"/>
+      <c r="F44" s="119"/>
+      <c r="G44" s="119"/>
+      <c r="H44" s="119"/>
+      <c r="I44" s="119"/>
+      <c r="J44" s="119"/>
+      <c r="K44" s="119"/>
+      <c r="L44" s="119"/>
+      <c r="O44" t="s">
         <v>101</v>
-      </c>
-    </row>
-    <row r="44" spans="1:19">
-      <c r="A44" s="68" t="s">
-        <v>36</v>
-      </c>
-      <c r="B44" s="69"/>
-      <c r="C44" s="69"/>
-      <c r="D44" s="69"/>
-      <c r="E44" s="69"/>
-      <c r="F44" s="69"/>
-      <c r="G44" s="69"/>
-      <c r="H44" s="69"/>
-      <c r="I44" s="69"/>
-      <c r="J44" s="69"/>
-      <c r="K44" s="69"/>
-      <c r="L44" s="69"/>
-      <c r="O44" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="45" spans="1:19">
       <c r="A45" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="B45" s="62" t="s">
+      <c r="B45" s="112" t="s">
         <v>56</v>
       </c>
-      <c r="C45" s="62"/>
-      <c r="D45" s="62"/>
-      <c r="E45" s="62"/>
-      <c r="F45" s="62"/>
-      <c r="G45" s="62"/>
-      <c r="H45" s="62"/>
-      <c r="I45" s="62"/>
-      <c r="J45" s="62"/>
-      <c r="K45" s="62"/>
-      <c r="L45" s="62"/>
+      <c r="C45" s="112"/>
+      <c r="D45" s="112"/>
+      <c r="E45" s="112"/>
+      <c r="F45" s="112"/>
+      <c r="G45" s="112"/>
+      <c r="H45" s="112"/>
+      <c r="I45" s="112"/>
+      <c r="J45" s="112"/>
+      <c r="K45" s="112"/>
+      <c r="L45" s="112"/>
     </row>
     <row r="46" spans="1:19" ht="15" customHeight="1">
       <c r="A46" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="B46" s="62" t="s">
+      <c r="B46" s="112" t="s">
         <v>57</v>
       </c>
-      <c r="C46" s="62"/>
-      <c r="D46" s="62"/>
-      <c r="E46" s="62"/>
-      <c r="F46" s="62"/>
-      <c r="G46" s="62"/>
-      <c r="H46" s="62"/>
-      <c r="I46" s="62"/>
-      <c r="J46" s="62"/>
-      <c r="K46" s="62"/>
-      <c r="L46" s="62"/>
+      <c r="C46" s="112"/>
+      <c r="D46" s="112"/>
+      <c r="E46" s="112"/>
+      <c r="F46" s="112"/>
+      <c r="G46" s="112"/>
+      <c r="H46" s="112"/>
+      <c r="I46" s="112"/>
+      <c r="J46" s="112"/>
+      <c r="K46" s="112"/>
+      <c r="L46" s="112"/>
       <c r="N46" s="50" t="s">
+        <v>98</v>
+      </c>
+      <c r="O46" s="44" t="s">
         <v>99</v>
-      </c>
-      <c r="O46" s="44" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="47" spans="1:19" ht="17.25">
       <c r="A47" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="B47" s="62" t="s">
+      <c r="B47" s="112" t="s">
         <v>58</v>
       </c>
-      <c r="C47" s="62"/>
-      <c r="D47" s="62"/>
-      <c r="E47" s="62"/>
-      <c r="F47" s="62"/>
-      <c r="G47" s="62"/>
-      <c r="H47" s="62"/>
-      <c r="I47" s="62"/>
-      <c r="J47" s="62"/>
-      <c r="K47" s="62"/>
-      <c r="L47" s="62"/>
+      <c r="C47" s="112"/>
+      <c r="D47" s="112"/>
+      <c r="E47" s="112"/>
+      <c r="F47" s="112"/>
+      <c r="G47" s="112"/>
+      <c r="H47" s="112"/>
+      <c r="I47" s="112"/>
+      <c r="J47" s="112"/>
+      <c r="K47" s="112"/>
+      <c r="L47" s="112"/>
       <c r="O47" s="44" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="48" spans="1:19">
       <c r="A48" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="B48" s="62" t="s">
+      <c r="B48" s="112" t="s">
         <v>45</v>
       </c>
-      <c r="C48" s="62"/>
-      <c r="D48" s="62"/>
-      <c r="E48" s="62"/>
-      <c r="F48" s="62"/>
-      <c r="G48" s="62"/>
-      <c r="H48" s="62"/>
-      <c r="I48" s="62"/>
-      <c r="J48" s="62"/>
-      <c r="K48" s="62"/>
-      <c r="L48" s="62"/>
+      <c r="C48" s="112"/>
+      <c r="D48" s="112"/>
+      <c r="E48" s="112"/>
+      <c r="F48" s="112"/>
+      <c r="G48" s="112"/>
+      <c r="H48" s="112"/>
+      <c r="I48" s="112"/>
+      <c r="J48" s="112"/>
+      <c r="K48" s="112"/>
+      <c r="L48" s="112"/>
       <c r="O48" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="49" spans="1:15">
       <c r="A49" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="B49" s="62" t="s">
+      <c r="B49" s="112" t="s">
         <v>34</v>
       </c>
-      <c r="C49" s="62"/>
-      <c r="D49" s="62"/>
-      <c r="E49" s="62"/>
-      <c r="F49" s="62"/>
-      <c r="G49" s="62"/>
-      <c r="H49" s="62"/>
-      <c r="I49" s="62"/>
-      <c r="J49" s="62"/>
-      <c r="K49" s="62"/>
-      <c r="L49" s="62"/>
+      <c r="C49" s="112"/>
+      <c r="D49" s="112"/>
+      <c r="E49" s="112"/>
+      <c r="F49" s="112"/>
+      <c r="G49" s="112"/>
+      <c r="H49" s="112"/>
+      <c r="I49" s="112"/>
+      <c r="J49" s="112"/>
+      <c r="K49" s="112"/>
+      <c r="L49" s="112"/>
     </row>
     <row r="50" spans="1:15" ht="17.25">
       <c r="A50" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="B50" s="62" t="s">
+      <c r="B50" s="112" t="s">
         <v>55</v>
       </c>
-      <c r="C50" s="62"/>
-      <c r="D50" s="62"/>
-      <c r="E50" s="62"/>
-      <c r="F50" s="62"/>
-      <c r="G50" s="62"/>
-      <c r="H50" s="62"/>
-      <c r="I50" s="62"/>
-      <c r="J50" s="62"/>
-      <c r="K50" s="62"/>
-      <c r="L50" s="62"/>
+      <c r="C50" s="112"/>
+      <c r="D50" s="112"/>
+      <c r="E50" s="112"/>
+      <c r="F50" s="112"/>
+      <c r="G50" s="112"/>
+      <c r="H50" s="112"/>
+      <c r="I50" s="112"/>
+      <c r="J50" s="112"/>
+      <c r="K50" s="112"/>
+      <c r="L50" s="112"/>
       <c r="N50" s="50" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="O50" s="44" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="51" spans="1:15">
       <c r="A51" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="B51" s="62" t="s">
+      <c r="B51" s="112" t="s">
         <v>54</v>
       </c>
-      <c r="C51" s="62"/>
-      <c r="D51" s="62"/>
-      <c r="E51" s="62"/>
-      <c r="F51" s="62"/>
-      <c r="G51" s="62"/>
-      <c r="H51" s="62"/>
-      <c r="I51" s="62"/>
-      <c r="J51" s="62"/>
-      <c r="K51" s="62"/>
-      <c r="L51" s="62"/>
+      <c r="C51" s="112"/>
+      <c r="D51" s="112"/>
+      <c r="E51" s="112"/>
+      <c r="F51" s="112"/>
+      <c r="G51" s="112"/>
+      <c r="H51" s="112"/>
+      <c r="I51" s="112"/>
+      <c r="J51" s="112"/>
+      <c r="K51" s="112"/>
+      <c r="L51" s="112"/>
       <c r="O51" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="52" spans="1:15">
       <c r="C52" s="32"/>
       <c r="O52" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="53" spans="1:15">
@@ -2896,33 +2884,22 @@
     <sortCondition ref="A3"/>
   </sortState>
   <mergeCells count="55">
-    <mergeCell ref="O15:S16"/>
-    <mergeCell ref="N27:S28"/>
-    <mergeCell ref="N24:S24"/>
-    <mergeCell ref="N38:S38"/>
+    <mergeCell ref="N40:S40"/>
+    <mergeCell ref="N33:S33"/>
     <mergeCell ref="N36:S36"/>
-    <mergeCell ref="O6:U6"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="H27:K27"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="H28:K28"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="H30:K30"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="H32:K32"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="H31:L31"/>
+    <mergeCell ref="N30:S30"/>
+    <mergeCell ref="N31:S31"/>
+    <mergeCell ref="B50:L50"/>
+    <mergeCell ref="B51:L51"/>
+    <mergeCell ref="A39:E39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="B45:L45"/>
+    <mergeCell ref="A44:L44"/>
+    <mergeCell ref="B46:L46"/>
+    <mergeCell ref="B47:L47"/>
+    <mergeCell ref="B48:L48"/>
+    <mergeCell ref="B49:L49"/>
     <mergeCell ref="A35:B35"/>
     <mergeCell ref="A36:B36"/>
     <mergeCell ref="A37:B37"/>
@@ -2935,22 +2912,33 @@
     <mergeCell ref="C35:G35"/>
     <mergeCell ref="C36:G36"/>
     <mergeCell ref="C37:G37"/>
-    <mergeCell ref="B50:L50"/>
-    <mergeCell ref="B51:L51"/>
-    <mergeCell ref="A39:E39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="B45:L45"/>
-    <mergeCell ref="A44:L44"/>
-    <mergeCell ref="B46:L46"/>
-    <mergeCell ref="B47:L47"/>
-    <mergeCell ref="B48:L48"/>
-    <mergeCell ref="B49:L49"/>
-    <mergeCell ref="N40:S40"/>
-    <mergeCell ref="N33:S33"/>
-    <mergeCell ref="N35:S35"/>
-    <mergeCell ref="N30:S30"/>
-    <mergeCell ref="N31:S31"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="H30:K30"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="H32:K32"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="H31:L31"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="H28:K28"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="O6:U6"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="H27:K27"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="O15:S16"/>
+    <mergeCell ref="N24:S24"/>
+    <mergeCell ref="N38:S38"/>
+    <mergeCell ref="N27:S27"/>
+    <mergeCell ref="N28:S28"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="Q4" r:id="rId1"/>
@@ -2982,31 +2970,31 @@
   <sheetData>
     <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B3" s="1"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="52" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B4" s="52"/>
       <c r="C4" s="52" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="52" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E4" s="52" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="51" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B5" s="51" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C5" s="52"/>
       <c r="D5" s="52"/>
@@ -3015,16 +3003,16 @@
     <row r="6" spans="1:6">
       <c r="A6" s="51"/>
       <c r="B6" s="51" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C6" s="52" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D6" s="52" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E6" s="52" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -3036,10 +3024,10 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="51" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B8" s="51" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C8" s="52"/>
       <c r="D8" s="52"/>
@@ -3048,16 +3036,16 @@
     <row r="9" spans="1:6">
       <c r="A9" s="51"/>
       <c r="B9" s="51" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C9" s="52" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D9" s="52" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E9" s="52" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -3069,10 +3057,10 @@
     </row>
     <row r="11" spans="1:6" ht="15.75">
       <c r="A11" s="51" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B11" s="51" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C11" s="52"/>
       <c r="D11" s="52"/>
@@ -3082,16 +3070,16 @@
     <row r="12" spans="1:6">
       <c r="A12" s="51"/>
       <c r="B12" s="51" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C12" s="52" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D12" s="52" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E12" s="52" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Supera el testing los modulos (y submodulos) de Trayactoria laboral y Formacion. Resta validacion de formularios y manejo de fechas
</commit_message>
<xml_diff>
--- a/Cuadro-de-estado.xlsx
+++ b/Cuadro-de-estado.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="119">
   <si>
     <t>BACKEND</t>
   </si>
@@ -89,9 +89,6 @@
   </si>
   <si>
     <t>No iniciado</t>
-  </si>
-  <si>
-    <t>Modificado</t>
   </si>
   <si>
     <t>Verificado</t>
@@ -455,6 +452,12 @@
   </si>
   <si>
     <t>Incorporar en los Form, el atributo url</t>
+  </si>
+  <si>
+    <t>Completando</t>
+  </si>
+  <si>
+    <t>OJO CON LOS GET HTTP, que no hayan desparramados o dobles llamadas</t>
   </si>
 </sst>
 </file>
@@ -676,7 +679,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -755,6 +758,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="38">
     <border>
@@ -1232,7 +1247,7 @@
     </xf>
     <xf numFmtId="43" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1314,9 +1329,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1341,11 +1353,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1353,48 +1361,52 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1449,6 +1461,18 @@
     <xf numFmtId="0" fontId="20" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1500,12 +1524,6 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1539,9 +1557,7 @@
     <xf numFmtId="0" fontId="22" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1844,7 +1860,7 @@
   <dimension ref="A1:U54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1861,109 +1877,109 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="61" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="61"/>
+      <c r="L1" s="61"/>
+    </row>
+    <row r="2" spans="1:21" ht="19.5" thickBot="1">
+      <c r="A2" s="45">
+        <f ca="1">M2-TODAY()-1</f>
+        <v>29</v>
+      </c>
+      <c r="B2" s="46" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
-      <c r="I1" s="64"/>
-      <c r="J1" s="64"/>
-      <c r="K1" s="64"/>
-      <c r="L1" s="64"/>
-    </row>
-    <row r="2" spans="1:21" ht="19.5" thickBot="1">
-      <c r="A2" s="46">
-        <f ca="1">M2-TODAY()-1</f>
-        <v>30</v>
-      </c>
-      <c r="B2" s="47" t="s">
-        <v>90</v>
-      </c>
-      <c r="C2" s="48"/>
-      <c r="M2" s="45">
+      <c r="C2" s="47"/>
+      <c r="M2" s="44">
         <v>45011</v>
       </c>
-      <c r="O2" s="44" t="s">
-        <v>86</v>
+      <c r="O2" s="43" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="65" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" s="66"/>
-      <c r="C3" s="67" t="s">
+      <c r="A3" s="62" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="63"/>
+      <c r="C3" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="69"/>
-      <c r="H3" s="67" t="s">
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="68"/>
-      <c r="J3" s="70"/>
-      <c r="K3" s="69"/>
+      <c r="I3" s="65"/>
+      <c r="J3" s="67"/>
+      <c r="K3" s="66"/>
       <c r="L3" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="71" t="s">
-        <v>80</v>
-      </c>
-      <c r="N3" s="63"/>
+      <c r="M3" s="68" t="s">
+        <v>79</v>
+      </c>
+      <c r="N3" s="60"/>
     </row>
     <row r="4" spans="1:21" s="3" customFormat="1" ht="40.5" customHeight="1" thickBot="1">
       <c r="A4" s="17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" s="17" t="s">
         <v>20</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>3</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H4" s="9" t="s">
         <v>1</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J4" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K4" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L4" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="M4" s="72" t="s">
-        <v>81</v>
-      </c>
-      <c r="N4" s="73"/>
+        <v>26</v>
+      </c>
+      <c r="M4" s="69" t="s">
+        <v>80</v>
+      </c>
+      <c r="N4" s="70"/>
       <c r="O4" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q4" s="35" t="s">
         <v>62</v>
-      </c>
-      <c r="Q4" s="35" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="4.5" customHeight="1">
@@ -1987,28 +2003,28 @@
       <c r="B6" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="6"/>
+      <c r="C6" s="57"/>
       <c r="D6" s="5"/>
       <c r="E6" s="13"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="4"/>
+      <c r="F6" s="57"/>
+      <c r="G6" s="5"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
       <c r="K6" s="5"/>
       <c r="L6" s="4"/>
-      <c r="M6" s="43" t="s">
-        <v>83</v>
-      </c>
-      <c r="O6" s="62" t="s">
-        <v>66</v>
-      </c>
-      <c r="P6" s="63"/>
-      <c r="Q6" s="63"/>
-      <c r="R6" s="63"/>
-      <c r="S6" s="63"/>
-      <c r="T6" s="63"/>
-      <c r="U6" s="63"/>
+      <c r="M6" s="42" t="s">
+        <v>82</v>
+      </c>
+      <c r="O6" s="59" t="s">
+        <v>65</v>
+      </c>
+      <c r="P6" s="60"/>
+      <c r="Q6" s="60"/>
+      <c r="R6" s="60"/>
+      <c r="S6" s="60"/>
+      <c r="T6" s="60"/>
+      <c r="U6" s="60"/>
     </row>
     <row r="7" spans="1:21" ht="4.5" customHeight="1">
       <c r="A7" s="28"/>
@@ -2042,10 +2058,10 @@
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
       <c r="O8" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="P8" s="6" t="s">
         <v>67</v>
-      </c>
-      <c r="P8" s="6" t="s">
-        <v>68</v>
       </c>
       <c r="Q8" s="6"/>
       <c r="R8" s="6"/>
@@ -2070,7 +2086,7 @@
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
       <c r="P9" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q9" s="6"/>
     </row>
@@ -2110,25 +2126,25 @@
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
       <c r="O11" t="s">
+        <v>68</v>
+      </c>
+      <c r="P11" t="s">
         <v>69</v>
-      </c>
-      <c r="P11" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="4.5" customHeight="1">
       <c r="A12" s="28"/>
-      <c r="B12" s="57"/>
-      <c r="C12" s="58"/>
-      <c r="D12" s="58"/>
-      <c r="E12" s="58"/>
-      <c r="F12" s="58"/>
-      <c r="G12" s="58"/>
-      <c r="H12" s="58"/>
-      <c r="I12" s="58"/>
-      <c r="J12" s="58"/>
-      <c r="K12" s="58"/>
-      <c r="L12" s="58"/>
+      <c r="B12" s="54"/>
+      <c r="C12" s="55"/>
+      <c r="D12" s="55"/>
+      <c r="E12" s="55"/>
+      <c r="F12" s="55"/>
+      <c r="G12" s="55"/>
+      <c r="H12" s="55"/>
+      <c r="I12" s="55"/>
+      <c r="J12" s="55"/>
+      <c r="K12" s="55"/>
+      <c r="L12" s="55"/>
     </row>
     <row r="13" spans="1:21">
       <c r="A13" s="38" t="s">
@@ -2145,105 +2161,105 @@
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
+      <c r="K13" s="57"/>
       <c r="L13" s="4"/>
       <c r="O13" t="s">
+        <v>70</v>
+      </c>
+      <c r="P13" t="s">
         <v>71</v>
-      </c>
-      <c r="P13" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:21">
       <c r="A14" s="38" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="56" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="5"/>
+      <c r="C14" s="4"/>
       <c r="D14" s="40"/>
-      <c r="E14" s="54"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="7"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="57"/>
       <c r="L14" s="4"/>
       <c r="O14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="15" customHeight="1">
       <c r="A15" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="56" t="s">
+      <c r="B15" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="5"/>
+      <c r="C15" s="4"/>
       <c r="D15" s="40"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="7"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="57"/>
       <c r="L15" s="4"/>
-      <c r="O15" s="60" t="s">
-        <v>78</v>
-      </c>
-      <c r="P15" s="60"/>
-      <c r="Q15" s="60"/>
-      <c r="R15" s="60"/>
-      <c r="S15" s="60"/>
-      <c r="T15" s="59"/>
+      <c r="O15" s="71" t="s">
+        <v>77</v>
+      </c>
+      <c r="P15" s="71"/>
+      <c r="Q15" s="71"/>
+      <c r="R15" s="71"/>
+      <c r="S15" s="71"/>
+      <c r="T15" s="56"/>
     </row>
     <row r="16" spans="1:21">
       <c r="A16" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="B16" s="56" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="7"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="123"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
       <c r="L16" s="4"/>
-      <c r="O16" s="60"/>
-      <c r="P16" s="60"/>
-      <c r="Q16" s="60"/>
-      <c r="R16" s="60"/>
-      <c r="S16" s="60"/>
-      <c r="T16" s="59"/>
+      <c r="O16" s="71"/>
+      <c r="P16" s="71"/>
+      <c r="Q16" s="71"/>
+      <c r="R16" s="71"/>
+      <c r="S16" s="71"/>
+      <c r="T16" s="56"/>
     </row>
     <row r="17" spans="1:19">
       <c r="A17" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="B17" s="56" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="7"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="123"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
       <c r="L17" s="4"/>
       <c r="O17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:19" ht="4.5" customHeight="1">
@@ -2267,16 +2283,16 @@
       <c r="B19" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="16"/>
-      <c r="D19" s="42"/>
-      <c r="E19" s="6"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="57"/>
       <c r="F19" s="8"/>
       <c r="G19" s="7"/>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
       <c r="K19" s="7"/>
-      <c r="L19" s="55"/>
+      <c r="L19" s="53"/>
     </row>
     <row r="20" spans="1:19">
       <c r="A20" s="39" t="s">
@@ -2285,16 +2301,24 @@
       <c r="B20" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="16"/>
-      <c r="D20" s="42"/>
-      <c r="E20" s="6"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="57"/>
       <c r="F20" s="8"/>
       <c r="G20" s="7"/>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
       <c r="K20" s="7"/>
-      <c r="L20" s="55"/>
+      <c r="L20" s="53"/>
+      <c r="N20" s="72" t="s">
+        <v>118</v>
+      </c>
+      <c r="O20" s="72"/>
+      <c r="P20" s="72"/>
+      <c r="Q20" s="72"/>
+      <c r="R20" s="72"/>
+      <c r="S20" s="72"/>
     </row>
     <row r="21" spans="1:19" ht="4.5" customHeight="1">
       <c r="A21" s="28"/>
@@ -2312,12 +2336,12 @@
     </row>
     <row r="22" spans="1:19">
       <c r="A22" s="39" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B22" s="19"/>
       <c r="C22" s="16"/>
       <c r="D22" s="8"/>
-      <c r="E22" s="6"/>
+      <c r="E22" s="57"/>
       <c r="F22" s="8"/>
       <c r="G22" s="4"/>
       <c r="H22" s="5"/>
@@ -2342,12 +2366,12 @@
     </row>
     <row r="24" spans="1:19">
       <c r="A24" s="39" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B24" s="31"/>
       <c r="C24" s="8"/>
       <c r="D24" s="5"/>
-      <c r="E24" s="6"/>
+      <c r="E24" s="57"/>
       <c r="F24" s="8"/>
       <c r="G24" s="7"/>
       <c r="H24" s="5"/>
@@ -2355,32 +2379,32 @@
       <c r="J24" s="5"/>
       <c r="K24" s="7"/>
       <c r="L24" s="4"/>
-      <c r="N24" s="61" t="s">
-        <v>88</v>
-      </c>
-      <c r="O24" s="61"/>
-      <c r="P24" s="61"/>
-      <c r="Q24" s="61"/>
-      <c r="R24" s="61"/>
-      <c r="S24" s="61"/>
+      <c r="N24" s="72" t="s">
+        <v>87</v>
+      </c>
+      <c r="O24" s="72"/>
+      <c r="P24" s="72"/>
+      <c r="Q24" s="72"/>
+      <c r="R24" s="72"/>
+      <c r="S24" s="72"/>
     </row>
     <row r="25" spans="1:19">
       <c r="A25" s="39" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B25" s="24" t="s">
         <v>12</v>
       </c>
       <c r="C25" s="22"/>
       <c r="D25" s="8"/>
-      <c r="E25" s="6"/>
+      <c r="E25" s="57"/>
       <c r="F25" s="8"/>
       <c r="G25" s="8"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
-      <c r="J25" s="7"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
       <c r="K25" s="7"/>
-      <c r="L25" s="7"/>
+      <c r="L25" s="4"/>
     </row>
     <row r="26" spans="1:19" ht="4.5" customHeight="1" thickBot="1">
       <c r="A26" s="28"/>
@@ -2399,60 +2423,60 @@
     <row r="27" spans="1:19" ht="15.75" thickBot="1">
       <c r="A27" s="23"/>
       <c r="B27" s="25"/>
-      <c r="C27" s="67" t="s">
+      <c r="C27" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="68"/>
-      <c r="E27" s="68"/>
-      <c r="F27" s="68"/>
-      <c r="G27" s="69"/>
-      <c r="H27" s="67" t="s">
+      <c r="D27" s="65"/>
+      <c r="E27" s="65"/>
+      <c r="F27" s="65"/>
+      <c r="G27" s="66"/>
+      <c r="H27" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="I27" s="68"/>
-      <c r="J27" s="70"/>
-      <c r="K27" s="69"/>
+      <c r="I27" s="65"/>
+      <c r="J27" s="67"/>
+      <c r="K27" s="66"/>
       <c r="L27" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="N27" s="61" t="s">
-        <v>82</v>
-      </c>
-      <c r="O27" s="61"/>
-      <c r="P27" s="61"/>
-      <c r="Q27" s="61"/>
-      <c r="R27" s="61"/>
-      <c r="S27" s="61"/>
+      <c r="N27" s="72" t="s">
+        <v>81</v>
+      </c>
+      <c r="O27" s="72"/>
+      <c r="P27" s="72"/>
+      <c r="Q27" s="72"/>
+      <c r="R27" s="72"/>
+      <c r="S27" s="72"/>
     </row>
     <row r="28" spans="1:19" ht="30">
-      <c r="A28" s="80" t="s">
-        <v>30</v>
-      </c>
-      <c r="B28" s="81"/>
-      <c r="C28" s="74" t="s">
-        <v>93</v>
-      </c>
-      <c r="D28" s="75"/>
-      <c r="E28" s="75"/>
-      <c r="F28" s="75"/>
-      <c r="G28" s="76"/>
-      <c r="H28" s="77" t="s">
+      <c r="A28" s="79" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" s="80"/>
+      <c r="C28" s="73" t="s">
+        <v>92</v>
+      </c>
+      <c r="D28" s="74"/>
+      <c r="E28" s="74"/>
+      <c r="F28" s="74"/>
+      <c r="G28" s="75"/>
+      <c r="H28" s="76" t="s">
+        <v>90</v>
+      </c>
+      <c r="I28" s="77"/>
+      <c r="J28" s="77"/>
+      <c r="K28" s="78"/>
+      <c r="L28" s="48" t="s">
         <v>91</v>
       </c>
-      <c r="I28" s="78"/>
-      <c r="J28" s="78"/>
-      <c r="K28" s="79"/>
-      <c r="L28" s="49" t="s">
-        <v>92</v>
-      </c>
-      <c r="N28" s="122" t="s">
-        <v>117</v>
-      </c>
-      <c r="O28" s="122"/>
-      <c r="P28" s="122"/>
-      <c r="Q28" s="122"/>
-      <c r="R28" s="122"/>
-      <c r="S28" s="122"/>
+      <c r="N28" s="58" t="s">
+        <v>116</v>
+      </c>
+      <c r="O28" s="58"/>
+      <c r="P28" s="58"/>
+      <c r="Q28" s="58"/>
+      <c r="R28" s="58"/>
+      <c r="S28" s="58"/>
     </row>
     <row r="29" spans="1:19" ht="4.5" customHeight="1">
       <c r="A29" s="28"/>
@@ -2469,100 +2493,100 @@
       <c r="L29" s="30"/>
     </row>
     <row r="30" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A30" s="86" t="s">
-        <v>39</v>
-      </c>
-      <c r="B30" s="87"/>
-      <c r="C30" s="82"/>
-      <c r="D30" s="83"/>
-      <c r="E30" s="83"/>
-      <c r="F30" s="83"/>
-      <c r="G30" s="84"/>
-      <c r="H30" s="85"/>
-      <c r="I30" s="83"/>
-      <c r="J30" s="83"/>
-      <c r="K30" s="84"/>
+      <c r="A30" s="85" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30" s="86"/>
+      <c r="C30" s="81"/>
+      <c r="D30" s="82"/>
+      <c r="E30" s="82"/>
+      <c r="F30" s="82"/>
+      <c r="G30" s="83"/>
+      <c r="H30" s="84"/>
+      <c r="I30" s="82"/>
+      <c r="J30" s="82"/>
+      <c r="K30" s="83"/>
       <c r="L30" s="21" t="s">
         <v>5</v>
       </c>
       <c r="M30" s="32"/>
-      <c r="N30" s="121" t="s">
-        <v>79</v>
-      </c>
-      <c r="O30" s="121"/>
-      <c r="P30" s="121"/>
-      <c r="Q30" s="121"/>
-      <c r="R30" s="121"/>
-      <c r="S30" s="121"/>
+      <c r="N30" s="122" t="s">
+        <v>78</v>
+      </c>
+      <c r="O30" s="122"/>
+      <c r="P30" s="122"/>
+      <c r="Q30" s="122"/>
+      <c r="R30" s="122"/>
+      <c r="S30" s="122"/>
     </row>
     <row r="31" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A31" s="86" t="s">
+      <c r="A31" s="85" t="s">
+        <v>83</v>
+      </c>
+      <c r="B31" s="86"/>
+      <c r="C31" s="73"/>
+      <c r="D31" s="74"/>
+      <c r="E31" s="74"/>
+      <c r="F31" s="74"/>
+      <c r="G31" s="75"/>
+      <c r="H31" s="95" t="s">
         <v>84</v>
       </c>
-      <c r="B31" s="87"/>
-      <c r="C31" s="74"/>
-      <c r="D31" s="75"/>
-      <c r="E31" s="75"/>
-      <c r="F31" s="75"/>
-      <c r="G31" s="76"/>
-      <c r="H31" s="92" t="s">
-        <v>85</v>
-      </c>
-      <c r="I31" s="93"/>
-      <c r="J31" s="93"/>
-      <c r="K31" s="93"/>
-      <c r="L31" s="94"/>
+      <c r="I31" s="96"/>
+      <c r="J31" s="96"/>
+      <c r="K31" s="96"/>
+      <c r="L31" s="97"/>
       <c r="M31" s="32"/>
-      <c r="N31" s="121" t="s">
+      <c r="N31" s="122" t="s">
+        <v>74</v>
+      </c>
+      <c r="O31" s="122"/>
+      <c r="P31" s="122"/>
+      <c r="Q31" s="122"/>
+      <c r="R31" s="122"/>
+      <c r="S31" s="122"/>
+    </row>
+    <row r="32" spans="1:19" ht="16.5" thickBot="1">
+      <c r="A32" s="89" t="s">
+        <v>59</v>
+      </c>
+      <c r="B32" s="90"/>
+      <c r="C32" s="91"/>
+      <c r="D32" s="92"/>
+      <c r="E32" s="92"/>
+      <c r="F32" s="92"/>
+      <c r="G32" s="93"/>
+      <c r="H32" s="94"/>
+      <c r="I32" s="92"/>
+      <c r="J32" s="92"/>
+      <c r="K32" s="93"/>
+      <c r="M32" s="32"/>
+    </row>
+    <row r="33" spans="1:19" ht="30.75" customHeight="1" thickBot="1">
+      <c r="A33" s="87" t="s">
+        <v>34</v>
+      </c>
+      <c r="B33" s="88"/>
+      <c r="C33" s="103" t="s">
+        <v>58</v>
+      </c>
+      <c r="D33" s="104"/>
+      <c r="E33" s="104"/>
+      <c r="F33" s="104"/>
+      <c r="G33" s="105"/>
+      <c r="H33" s="100"/>
+      <c r="I33" s="101"/>
+      <c r="J33" s="101"/>
+      <c r="K33" s="102"/>
+      <c r="M33" s="32"/>
+      <c r="N33" s="121" t="s">
         <v>75</v>
       </c>
-      <c r="O31" s="121"/>
-      <c r="P31" s="121"/>
-      <c r="Q31" s="121"/>
-      <c r="R31" s="121"/>
-      <c r="S31" s="121"/>
-    </row>
-    <row r="32" spans="1:19" ht="16.5" thickBot="1">
-      <c r="A32" s="90" t="s">
-        <v>60</v>
-      </c>
-      <c r="B32" s="91"/>
-      <c r="C32" s="82"/>
-      <c r="D32" s="83"/>
-      <c r="E32" s="83"/>
-      <c r="F32" s="83"/>
-      <c r="G32" s="84"/>
-      <c r="H32" s="85"/>
-      <c r="I32" s="83"/>
-      <c r="J32" s="83"/>
-      <c r="K32" s="84"/>
-      <c r="M32" s="32"/>
-    </row>
-    <row r="33" spans="1:19" ht="30.75" customHeight="1" thickBot="1">
-      <c r="A33" s="88" t="s">
-        <v>35</v>
-      </c>
-      <c r="B33" s="89"/>
-      <c r="C33" s="100" t="s">
-        <v>59</v>
-      </c>
-      <c r="D33" s="101"/>
-      <c r="E33" s="101"/>
-      <c r="F33" s="101"/>
-      <c r="G33" s="102"/>
-      <c r="H33" s="97"/>
-      <c r="I33" s="98"/>
-      <c r="J33" s="98"/>
-      <c r="K33" s="99"/>
-      <c r="M33" s="32"/>
-      <c r="N33" s="120" t="s">
-        <v>76</v>
-      </c>
-      <c r="O33" s="120"/>
-      <c r="P33" s="120"/>
-      <c r="Q33" s="120"/>
-      <c r="R33" s="120"/>
-      <c r="S33" s="120"/>
+      <c r="O33" s="121"/>
+      <c r="P33" s="121"/>
+      <c r="Q33" s="121"/>
+      <c r="R33" s="121"/>
+      <c r="S33" s="121"/>
     </row>
     <row r="34" spans="1:19" ht="4.5" customHeight="1" thickBot="1">
       <c r="A34" s="28"/>
@@ -2578,299 +2602,299 @@
       <c r="K34" s="30"/>
     </row>
     <row r="35" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A35" s="86" t="s">
+      <c r="A35" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="87"/>
-      <c r="C35" s="109"/>
-      <c r="D35" s="110"/>
-      <c r="E35" s="110"/>
-      <c r="F35" s="110"/>
-      <c r="G35" s="111"/>
-      <c r="H35" s="103"/>
-      <c r="I35" s="104"/>
-      <c r="J35" s="104"/>
-      <c r="K35" s="105"/>
+      <c r="B35" s="86"/>
+      <c r="C35" s="91"/>
+      <c r="D35" s="92"/>
+      <c r="E35" s="92"/>
+      <c r="F35" s="92"/>
+      <c r="G35" s="112"/>
+      <c r="H35" s="106"/>
+      <c r="I35" s="107"/>
+      <c r="J35" s="107"/>
+      <c r="K35" s="108"/>
       <c r="M35" s="32"/>
     </row>
     <row r="36" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A36" s="86" t="s">
-        <v>95</v>
-      </c>
-      <c r="B36" s="87"/>
-      <c r="C36" s="109"/>
-      <c r="D36" s="110"/>
-      <c r="E36" s="110"/>
-      <c r="F36" s="110"/>
-      <c r="G36" s="111"/>
-      <c r="H36" s="103"/>
-      <c r="I36" s="104"/>
-      <c r="J36" s="104"/>
-      <c r="K36" s="105"/>
+      <c r="A36" s="85" t="s">
+        <v>94</v>
+      </c>
+      <c r="B36" s="86"/>
+      <c r="C36" s="91"/>
+      <c r="D36" s="92"/>
+      <c r="E36" s="92"/>
+      <c r="F36" s="92"/>
+      <c r="G36" s="112"/>
+      <c r="H36" s="106"/>
+      <c r="I36" s="107"/>
+      <c r="J36" s="107"/>
+      <c r="K36" s="108"/>
       <c r="M36" s="32"/>
-      <c r="N36" s="121" t="s">
-        <v>77</v>
-      </c>
-      <c r="O36" s="121"/>
-      <c r="P36" s="121"/>
-      <c r="Q36" s="121"/>
-      <c r="R36" s="121"/>
-      <c r="S36" s="121"/>
+      <c r="N36" s="122" t="s">
+        <v>76</v>
+      </c>
+      <c r="O36" s="122"/>
+      <c r="P36" s="122"/>
+      <c r="Q36" s="122"/>
+      <c r="R36" s="122"/>
+      <c r="S36" s="122"/>
     </row>
     <row r="37" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A37" s="86" t="s">
+      <c r="A37" s="85" t="s">
         <v>7</v>
       </c>
-      <c r="B37" s="87"/>
-      <c r="C37" s="106"/>
-      <c r="D37" s="107"/>
-      <c r="E37" s="107"/>
-      <c r="F37" s="107"/>
-      <c r="G37" s="108"/>
-      <c r="H37" s="106"/>
-      <c r="I37" s="107"/>
-      <c r="J37" s="107"/>
-      <c r="K37" s="108"/>
+      <c r="B37" s="86"/>
+      <c r="C37" s="109"/>
+      <c r="D37" s="110"/>
+      <c r="E37" s="110"/>
+      <c r="F37" s="110"/>
+      <c r="G37" s="111"/>
+      <c r="H37" s="109"/>
+      <c r="I37" s="110"/>
+      <c r="J37" s="110"/>
+      <c r="K37" s="111"/>
       <c r="M37" s="32"/>
     </row>
     <row r="38" spans="1:19" ht="15.75" thickBot="1">
-      <c r="N38" s="61" t="s">
-        <v>87</v>
-      </c>
-      <c r="O38" s="61"/>
-      <c r="P38" s="61"/>
-      <c r="Q38" s="61"/>
-      <c r="R38" s="61"/>
-      <c r="S38" s="61"/>
+      <c r="N38" s="72" t="s">
+        <v>86</v>
+      </c>
+      <c r="O38" s="72"/>
+      <c r="P38" s="72"/>
+      <c r="Q38" s="72"/>
+      <c r="R38" s="72"/>
+      <c r="S38" s="72"/>
     </row>
     <row r="39" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A39" s="113" t="s">
-        <v>26</v>
-      </c>
-      <c r="B39" s="114"/>
-      <c r="C39" s="114"/>
-      <c r="D39" s="114"/>
-      <c r="E39" s="115"/>
+      <c r="A39" s="114" t="s">
+        <v>25</v>
+      </c>
+      <c r="B39" s="115"/>
+      <c r="C39" s="115"/>
+      <c r="D39" s="115"/>
+      <c r="E39" s="116"/>
     </row>
     <row r="40" spans="1:19">
       <c r="A40" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B40" s="13"/>
-      <c r="C40" s="116" t="s">
+      <c r="C40" s="117" t="s">
         <v>22</v>
       </c>
-      <c r="D40" s="117"/>
+      <c r="D40" s="118"/>
       <c r="E40" s="27"/>
-      <c r="N40" s="61" t="s">
-        <v>116</v>
-      </c>
-      <c r="O40" s="61"/>
-      <c r="P40" s="61"/>
-      <c r="Q40" s="61"/>
-      <c r="R40" s="61"/>
-      <c r="S40" s="61"/>
+      <c r="N40" s="72" t="s">
+        <v>115</v>
+      </c>
+      <c r="O40" s="72"/>
+      <c r="P40" s="72"/>
+      <c r="Q40" s="72"/>
+      <c r="R40" s="72"/>
+      <c r="S40" s="72"/>
     </row>
     <row r="41" spans="1:19">
       <c r="A41" s="15" t="s">
         <v>21</v>
       </c>
       <c r="B41" s="5"/>
-      <c r="C41" s="116" t="s">
+      <c r="C41" s="117" t="s">
         <v>23</v>
       </c>
-      <c r="D41" s="117"/>
+      <c r="D41" s="118"/>
       <c r="E41" s="8"/>
     </row>
     <row r="42" spans="1:19">
       <c r="A42" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B42" s="6"/>
-      <c r="C42" s="95" t="s">
-        <v>65</v>
-      </c>
-      <c r="D42" s="96"/>
+        <v>117</v>
+      </c>
+      <c r="B42" s="57"/>
+      <c r="C42" s="98" t="s">
+        <v>64</v>
+      </c>
+      <c r="D42" s="99"/>
       <c r="E42" s="37"/>
     </row>
     <row r="43" spans="1:19" ht="18" thickBot="1">
-      <c r="N43" s="50" t="s">
+      <c r="N43" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="O43" s="44" t="s">
+      <c r="O43" s="43" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19">
+      <c r="A44" s="119" t="s">
+        <v>35</v>
+      </c>
+      <c r="B44" s="120"/>
+      <c r="C44" s="120"/>
+      <c r="D44" s="120"/>
+      <c r="E44" s="120"/>
+      <c r="F44" s="120"/>
+      <c r="G44" s="120"/>
+      <c r="H44" s="120"/>
+      <c r="I44" s="120"/>
+      <c r="J44" s="120"/>
+      <c r="K44" s="120"/>
+      <c r="L44" s="120"/>
+      <c r="O44" t="s">
         <v>100</v>
-      </c>
-    </row>
-    <row r="44" spans="1:19">
-      <c r="A44" s="118" t="s">
-        <v>36</v>
-      </c>
-      <c r="B44" s="119"/>
-      <c r="C44" s="119"/>
-      <c r="D44" s="119"/>
-      <c r="E44" s="119"/>
-      <c r="F44" s="119"/>
-      <c r="G44" s="119"/>
-      <c r="H44" s="119"/>
-      <c r="I44" s="119"/>
-      <c r="J44" s="119"/>
-      <c r="K44" s="119"/>
-      <c r="L44" s="119"/>
-      <c r="O44" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="45" spans="1:19">
       <c r="A45" s="33" t="s">
-        <v>37</v>
-      </c>
-      <c r="B45" s="112" t="s">
-        <v>56</v>
-      </c>
-      <c r="C45" s="112"/>
-      <c r="D45" s="112"/>
-      <c r="E45" s="112"/>
-      <c r="F45" s="112"/>
-      <c r="G45" s="112"/>
-      <c r="H45" s="112"/>
-      <c r="I45" s="112"/>
-      <c r="J45" s="112"/>
-      <c r="K45" s="112"/>
-      <c r="L45" s="112"/>
+        <v>36</v>
+      </c>
+      <c r="B45" s="113" t="s">
+        <v>55</v>
+      </c>
+      <c r="C45" s="113"/>
+      <c r="D45" s="113"/>
+      <c r="E45" s="113"/>
+      <c r="F45" s="113"/>
+      <c r="G45" s="113"/>
+      <c r="H45" s="113"/>
+      <c r="I45" s="113"/>
+      <c r="J45" s="113"/>
+      <c r="K45" s="113"/>
+      <c r="L45" s="113"/>
     </row>
     <row r="46" spans="1:19" ht="15" customHeight="1">
       <c r="A46" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="B46" s="112" t="s">
-        <v>57</v>
-      </c>
-      <c r="C46" s="112"/>
-      <c r="D46" s="112"/>
-      <c r="E46" s="112"/>
-      <c r="F46" s="112"/>
-      <c r="G46" s="112"/>
-      <c r="H46" s="112"/>
-      <c r="I46" s="112"/>
-      <c r="J46" s="112"/>
-      <c r="K46" s="112"/>
-      <c r="L46" s="112"/>
-      <c r="N46" s="50" t="s">
+        <v>30</v>
+      </c>
+      <c r="B46" s="113" t="s">
+        <v>56</v>
+      </c>
+      <c r="C46" s="113"/>
+      <c r="D46" s="113"/>
+      <c r="E46" s="113"/>
+      <c r="F46" s="113"/>
+      <c r="G46" s="113"/>
+      <c r="H46" s="113"/>
+      <c r="I46" s="113"/>
+      <c r="J46" s="113"/>
+      <c r="K46" s="113"/>
+      <c r="L46" s="113"/>
+      <c r="N46" s="49" t="s">
+        <v>97</v>
+      </c>
+      <c r="O46" s="43" t="s">
         <v>98</v>
-      </c>
-      <c r="O46" s="44" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="47" spans="1:19" ht="17.25">
       <c r="A47" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B47" s="112" t="s">
-        <v>58</v>
-      </c>
-      <c r="C47" s="112"/>
-      <c r="D47" s="112"/>
-      <c r="E47" s="112"/>
-      <c r="F47" s="112"/>
-      <c r="G47" s="112"/>
-      <c r="H47" s="112"/>
-      <c r="I47" s="112"/>
-      <c r="J47" s="112"/>
-      <c r="K47" s="112"/>
-      <c r="L47" s="112"/>
-      <c r="O47" s="44" t="s">
-        <v>102</v>
+        <v>31</v>
+      </c>
+      <c r="B47" s="113" t="s">
+        <v>57</v>
+      </c>
+      <c r="C47" s="113"/>
+      <c r="D47" s="113"/>
+      <c r="E47" s="113"/>
+      <c r="F47" s="113"/>
+      <c r="G47" s="113"/>
+      <c r="H47" s="113"/>
+      <c r="I47" s="113"/>
+      <c r="J47" s="113"/>
+      <c r="K47" s="113"/>
+      <c r="L47" s="113"/>
+      <c r="O47" s="43" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="48" spans="1:19">
       <c r="A48" s="33" t="s">
-        <v>33</v>
-      </c>
-      <c r="B48" s="112" t="s">
-        <v>45</v>
-      </c>
-      <c r="C48" s="112"/>
-      <c r="D48" s="112"/>
-      <c r="E48" s="112"/>
-      <c r="F48" s="112"/>
-      <c r="G48" s="112"/>
-      <c r="H48" s="112"/>
-      <c r="I48" s="112"/>
-      <c r="J48" s="112"/>
-      <c r="K48" s="112"/>
-      <c r="L48" s="112"/>
+        <v>32</v>
+      </c>
+      <c r="B48" s="113" t="s">
+        <v>44</v>
+      </c>
+      <c r="C48" s="113"/>
+      <c r="D48" s="113"/>
+      <c r="E48" s="113"/>
+      <c r="F48" s="113"/>
+      <c r="G48" s="113"/>
+      <c r="H48" s="113"/>
+      <c r="I48" s="113"/>
+      <c r="J48" s="113"/>
+      <c r="K48" s="113"/>
+      <c r="L48" s="113"/>
       <c r="O48" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="49" spans="1:15">
       <c r="A49" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="B49" s="112" t="s">
-        <v>34</v>
-      </c>
-      <c r="C49" s="112"/>
-      <c r="D49" s="112"/>
-      <c r="E49" s="112"/>
-      <c r="F49" s="112"/>
-      <c r="G49" s="112"/>
-      <c r="H49" s="112"/>
-      <c r="I49" s="112"/>
-      <c r="J49" s="112"/>
-      <c r="K49" s="112"/>
-      <c r="L49" s="112"/>
+        <v>52</v>
+      </c>
+      <c r="B49" s="113" t="s">
+        <v>33</v>
+      </c>
+      <c r="C49" s="113"/>
+      <c r="D49" s="113"/>
+      <c r="E49" s="113"/>
+      <c r="F49" s="113"/>
+      <c r="G49" s="113"/>
+      <c r="H49" s="113"/>
+      <c r="I49" s="113"/>
+      <c r="J49" s="113"/>
+      <c r="K49" s="113"/>
+      <c r="L49" s="113"/>
     </row>
     <row r="50" spans="1:15" ht="17.25">
       <c r="A50" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="B50" s="112" t="s">
-        <v>55</v>
-      </c>
-      <c r="C50" s="112"/>
-      <c r="D50" s="112"/>
-      <c r="E50" s="112"/>
-      <c r="F50" s="112"/>
-      <c r="G50" s="112"/>
-      <c r="H50" s="112"/>
-      <c r="I50" s="112"/>
-      <c r="J50" s="112"/>
-      <c r="K50" s="112"/>
-      <c r="L50" s="112"/>
-      <c r="N50" s="50" t="s">
-        <v>97</v>
-      </c>
-      <c r="O50" s="44" t="s">
+        <v>50</v>
+      </c>
+      <c r="B50" s="113" t="s">
+        <v>54</v>
+      </c>
+      <c r="C50" s="113"/>
+      <c r="D50" s="113"/>
+      <c r="E50" s="113"/>
+      <c r="F50" s="113"/>
+      <c r="G50" s="113"/>
+      <c r="H50" s="113"/>
+      <c r="I50" s="113"/>
+      <c r="J50" s="113"/>
+      <c r="K50" s="113"/>
+      <c r="L50" s="113"/>
+      <c r="N50" s="49" t="s">
         <v>96</v>
+      </c>
+      <c r="O50" s="43" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="51" spans="1:15">
       <c r="A51" s="33" t="s">
-        <v>52</v>
-      </c>
-      <c r="B51" s="112" t="s">
-        <v>54</v>
-      </c>
-      <c r="C51" s="112"/>
-      <c r="D51" s="112"/>
-      <c r="E51" s="112"/>
-      <c r="F51" s="112"/>
-      <c r="G51" s="112"/>
-      <c r="H51" s="112"/>
-      <c r="I51" s="112"/>
-      <c r="J51" s="112"/>
-      <c r="K51" s="112"/>
-      <c r="L51" s="112"/>
+        <v>51</v>
+      </c>
+      <c r="B51" s="113" t="s">
+        <v>53</v>
+      </c>
+      <c r="C51" s="113"/>
+      <c r="D51" s="113"/>
+      <c r="E51" s="113"/>
+      <c r="F51" s="113"/>
+      <c r="G51" s="113"/>
+      <c r="H51" s="113"/>
+      <c r="I51" s="113"/>
+      <c r="J51" s="113"/>
+      <c r="K51" s="113"/>
+      <c r="L51" s="113"/>
       <c r="O51" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="52" spans="1:15">
       <c r="C52" s="32"/>
       <c r="O52" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="53" spans="1:15">
@@ -2883,12 +2907,14 @@
   <sortState ref="A24:K25">
     <sortCondition ref="A3"/>
   </sortState>
-  <mergeCells count="55">
+  <mergeCells count="56">
+    <mergeCell ref="N20:S20"/>
     <mergeCell ref="N40:S40"/>
     <mergeCell ref="N33:S33"/>
     <mergeCell ref="N36:S36"/>
     <mergeCell ref="N30:S30"/>
     <mergeCell ref="N31:S31"/>
+    <mergeCell ref="N38:S38"/>
     <mergeCell ref="B50:L50"/>
     <mergeCell ref="B51:L51"/>
     <mergeCell ref="A39:E39"/>
@@ -2922,11 +2948,7 @@
     <mergeCell ref="C31:G31"/>
     <mergeCell ref="A31:B31"/>
     <mergeCell ref="H31:L31"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="H28:K28"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="N28:S28"/>
     <mergeCell ref="O6:U6"/>
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="A3:B3"/>
@@ -2936,9 +2958,12 @@
     <mergeCell ref="M4:N4"/>
     <mergeCell ref="O15:S16"/>
     <mergeCell ref="N24:S24"/>
-    <mergeCell ref="N38:S38"/>
     <mergeCell ref="N27:S27"/>
-    <mergeCell ref="N28:S28"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="H28:K28"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="A28:B28"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="Q4" r:id="rId1"/>
@@ -2970,116 +2995,116 @@
   <sheetData>
     <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="51" t="s">
+        <v>112</v>
+      </c>
+      <c r="B4" s="51"/>
+      <c r="C4" s="51" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="51" t="s">
+        <v>111</v>
+      </c>
+      <c r="E4" s="51" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="50" t="s">
+        <v>109</v>
+      </c>
+      <c r="B5" s="50" t="s">
+        <v>106</v>
+      </c>
+      <c r="C5" s="51"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="51"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="50"/>
+      <c r="B6" s="50" t="s">
+        <v>105</v>
+      </c>
+      <c r="C6" s="51" t="s">
         <v>114</v>
       </c>
-      <c r="B3" s="1"/>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="52" t="s">
-        <v>113</v>
-      </c>
-      <c r="B4" s="52"/>
-      <c r="C4" s="52" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="52" t="s">
-        <v>112</v>
-      </c>
-      <c r="E4" s="52" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="51" t="s">
-        <v>110</v>
-      </c>
-      <c r="B5" s="51" t="s">
+      <c r="D6" s="51" t="s">
+        <v>114</v>
+      </c>
+      <c r="E6" s="51" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="50"/>
+      <c r="B7" s="50"/>
+      <c r="C7" s="51"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="51"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="50" t="s">
+        <v>108</v>
+      </c>
+      <c r="B8" s="50" t="s">
+        <v>106</v>
+      </c>
+      <c r="C8" s="51"/>
+      <c r="D8" s="51"/>
+      <c r="E8" s="51"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="50"/>
+      <c r="B9" s="50" t="s">
+        <v>105</v>
+      </c>
+      <c r="C9" s="51" t="s">
+        <v>114</v>
+      </c>
+      <c r="D9" s="51" t="s">
+        <v>114</v>
+      </c>
+      <c r="E9" s="51" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="50"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="51"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="51"/>
+    </row>
+    <row r="11" spans="1:6" ht="15.75">
+      <c r="A11" s="50" t="s">
         <v>107</v>
       </c>
-      <c r="C5" s="52"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="51"/>
-      <c r="B6" s="51" t="s">
+      <c r="B11" s="50" t="s">
         <v>106</v>
       </c>
-      <c r="C6" s="52" t="s">
-        <v>115</v>
-      </c>
-      <c r="D6" s="52" t="s">
-        <v>115</v>
-      </c>
-      <c r="E6" s="52" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="51"/>
-      <c r="B7" s="51"/>
-      <c r="C7" s="52"/>
-      <c r="D7" s="52"/>
-      <c r="E7" s="52"/>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="51" t="s">
-        <v>109</v>
-      </c>
-      <c r="B8" s="51" t="s">
-        <v>107</v>
-      </c>
-      <c r="C8" s="52"/>
-      <c r="D8" s="52"/>
-      <c r="E8" s="52"/>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="51"/>
-      <c r="B9" s="51" t="s">
-        <v>106</v>
-      </c>
-      <c r="C9" s="52" t="s">
-        <v>115</v>
-      </c>
-      <c r="D9" s="52" t="s">
-        <v>115</v>
-      </c>
-      <c r="E9" s="52" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="51"/>
-      <c r="B10" s="51"/>
-      <c r="C10" s="52"/>
-      <c r="D10" s="52"/>
-      <c r="E10" s="52"/>
-    </row>
-    <row r="11" spans="1:6" ht="15.75">
-      <c r="A11" s="51" t="s">
-        <v>108</v>
-      </c>
-      <c r="B11" s="51" t="s">
-        <v>107</v>
-      </c>
-      <c r="C11" s="52"/>
-      <c r="D11" s="52"/>
-      <c r="E11" s="52"/>
-      <c r="F11" s="53"/>
+      <c r="C11" s="51"/>
+      <c r="D11" s="51"/>
+      <c r="E11" s="51"/>
+      <c r="F11" s="52"/>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="51"/>
-      <c r="B12" s="51" t="s">
-        <v>106</v>
-      </c>
-      <c r="C12" s="52" t="s">
-        <v>115</v>
-      </c>
-      <c r="D12" s="52" t="s">
-        <v>115</v>
-      </c>
-      <c r="E12" s="52" t="s">
-        <v>115</v>
+      <c r="A12" s="50"/>
+      <c r="B12" s="50" t="s">
+        <v>105</v>
+      </c>
+      <c r="C12" s="51" t="s">
+        <v>114</v>
+      </c>
+      <c r="D12" s="51" t="s">
+        <v>114</v>
+      </c>
+      <c r="E12" s="51" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
actualizado el archivo de cuadro de estado del proyecto
</commit_message>
<xml_diff>
--- a/Cuadro-de-estado.xlsx
+++ b/Cuadro-de-estado.xlsx
@@ -679,7 +679,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -764,12 +764,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="38">
     <border>
@@ -1247,7 +1241,7 @@
     </xf>
     <xf numFmtId="43" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="124">
+  <cellXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1363,6 +1357,144 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1404,18 +1536,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1431,133 +1551,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1860,7 +1853,7 @@
   <dimension ref="A1:U54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1877,20 +1870,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="107" t="s">
         <v>88</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="61"/>
-      <c r="K1" s="61"/>
-      <c r="L1" s="61"/>
+      <c r="B1" s="107"/>
+      <c r="C1" s="107"/>
+      <c r="D1" s="107"/>
+      <c r="E1" s="107"/>
+      <c r="F1" s="107"/>
+      <c r="G1" s="107"/>
+      <c r="H1" s="107"/>
+      <c r="I1" s="107"/>
+      <c r="J1" s="107"/>
+      <c r="K1" s="107"/>
+      <c r="L1" s="107"/>
     </row>
     <row r="2" spans="1:21" ht="19.5" thickBot="1">
       <c r="A2" s="45">
@@ -1909,30 +1902,30 @@
       </c>
     </row>
     <row r="3" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="62" t="s">
+      <c r="A3" s="108" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="63"/>
-      <c r="C3" s="64" t="s">
+      <c r="B3" s="109"/>
+      <c r="C3" s="110" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="66"/>
-      <c r="H3" s="64" t="s">
+      <c r="D3" s="111"/>
+      <c r="E3" s="111"/>
+      <c r="F3" s="111"/>
+      <c r="G3" s="112"/>
+      <c r="H3" s="110" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="65"/>
-      <c r="J3" s="67"/>
-      <c r="K3" s="66"/>
+      <c r="I3" s="111"/>
+      <c r="J3" s="113"/>
+      <c r="K3" s="112"/>
       <c r="L3" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="68" t="s">
+      <c r="M3" s="114" t="s">
         <v>79</v>
       </c>
-      <c r="N3" s="60"/>
+      <c r="N3" s="106"/>
     </row>
     <row r="4" spans="1:21" s="3" customFormat="1" ht="40.5" customHeight="1" thickBot="1">
       <c r="A4" s="17" t="s">
@@ -1971,10 +1964,10 @@
       <c r="L4" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="M4" s="69" t="s">
+      <c r="M4" s="115" t="s">
         <v>80</v>
       </c>
-      <c r="N4" s="70"/>
+      <c r="N4" s="116"/>
       <c r="O4" s="34" t="s">
         <v>61</v>
       </c>
@@ -2003,11 +1996,11 @@
       <c r="B6" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="57"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="57"/>
-      <c r="G6" s="5"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
@@ -2016,15 +2009,15 @@
       <c r="M6" s="42" t="s">
         <v>82</v>
       </c>
-      <c r="O6" s="59" t="s">
+      <c r="O6" s="105" t="s">
         <v>65</v>
       </c>
-      <c r="P6" s="60"/>
-      <c r="Q6" s="60"/>
-      <c r="R6" s="60"/>
-      <c r="S6" s="60"/>
-      <c r="T6" s="60"/>
-      <c r="U6" s="60"/>
+      <c r="P6" s="106"/>
+      <c r="Q6" s="106"/>
+      <c r="R6" s="106"/>
+      <c r="S6" s="106"/>
+      <c r="T6" s="106"/>
+      <c r="U6" s="106"/>
     </row>
     <row r="7" spans="1:21" ht="4.5" customHeight="1">
       <c r="A7" s="28"/>
@@ -2208,13 +2201,13 @@
       <c r="J15" s="4"/>
       <c r="K15" s="57"/>
       <c r="L15" s="4"/>
-      <c r="O15" s="71" t="s">
+      <c r="O15" s="117" t="s">
         <v>77</v>
       </c>
-      <c r="P15" s="71"/>
-      <c r="Q15" s="71"/>
-      <c r="R15" s="71"/>
-      <c r="S15" s="71"/>
+      <c r="P15" s="117"/>
+      <c r="Q15" s="117"/>
+      <c r="R15" s="117"/>
+      <c r="S15" s="117"/>
       <c r="T15" s="56"/>
     </row>
     <row r="16" spans="1:21">
@@ -2227,18 +2220,18 @@
       <c r="C16" s="4"/>
       <c r="D16" s="40"/>
       <c r="E16" s="4"/>
-      <c r="F16" s="123"/>
+      <c r="F16" s="57"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
       <c r="L16" s="4"/>
-      <c r="O16" s="71"/>
-      <c r="P16" s="71"/>
-      <c r="Q16" s="71"/>
-      <c r="R16" s="71"/>
-      <c r="S16" s="71"/>
+      <c r="O16" s="117"/>
+      <c r="P16" s="117"/>
+      <c r="Q16" s="117"/>
+      <c r="R16" s="117"/>
+      <c r="S16" s="117"/>
       <c r="T16" s="56"/>
     </row>
     <row r="17" spans="1:19">
@@ -2251,7 +2244,7 @@
       <c r="C17" s="4"/>
       <c r="D17" s="40"/>
       <c r="E17" s="4"/>
-      <c r="F17" s="123"/>
+      <c r="F17" s="57"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
@@ -2311,14 +2304,14 @@
       <c r="J20" s="5"/>
       <c r="K20" s="7"/>
       <c r="L20" s="53"/>
-      <c r="N20" s="72" t="s">
+      <c r="N20" s="58" t="s">
         <v>118</v>
       </c>
-      <c r="O20" s="72"/>
-      <c r="P20" s="72"/>
-      <c r="Q20" s="72"/>
-      <c r="R20" s="72"/>
-      <c r="S20" s="72"/>
+      <c r="O20" s="58"/>
+      <c r="P20" s="58"/>
+      <c r="Q20" s="58"/>
+      <c r="R20" s="58"/>
+      <c r="S20" s="58"/>
     </row>
     <row r="21" spans="1:19" ht="4.5" customHeight="1">
       <c r="A21" s="28"/>
@@ -2379,14 +2372,14 @@
       <c r="J24" s="5"/>
       <c r="K24" s="7"/>
       <c r="L24" s="4"/>
-      <c r="N24" s="72" t="s">
+      <c r="N24" s="58" t="s">
         <v>87</v>
       </c>
-      <c r="O24" s="72"/>
-      <c r="P24" s="72"/>
-      <c r="Q24" s="72"/>
-      <c r="R24" s="72"/>
-      <c r="S24" s="72"/>
+      <c r="O24" s="58"/>
+      <c r="P24" s="58"/>
+      <c r="Q24" s="58"/>
+      <c r="R24" s="58"/>
+      <c r="S24" s="58"/>
     </row>
     <row r="25" spans="1:19">
       <c r="A25" s="39" t="s">
@@ -2423,60 +2416,60 @@
     <row r="27" spans="1:19" ht="15.75" thickBot="1">
       <c r="A27" s="23"/>
       <c r="B27" s="25"/>
-      <c r="C27" s="64" t="s">
+      <c r="C27" s="110" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="65"/>
-      <c r="E27" s="65"/>
-      <c r="F27" s="65"/>
-      <c r="G27" s="66"/>
-      <c r="H27" s="64" t="s">
+      <c r="D27" s="111"/>
+      <c r="E27" s="111"/>
+      <c r="F27" s="111"/>
+      <c r="G27" s="112"/>
+      <c r="H27" s="110" t="s">
         <v>0</v>
       </c>
-      <c r="I27" s="65"/>
-      <c r="J27" s="67"/>
-      <c r="K27" s="66"/>
+      <c r="I27" s="111"/>
+      <c r="J27" s="113"/>
+      <c r="K27" s="112"/>
       <c r="L27" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="N27" s="72" t="s">
+      <c r="N27" s="58" t="s">
         <v>81</v>
       </c>
-      <c r="O27" s="72"/>
-      <c r="P27" s="72"/>
-      <c r="Q27" s="72"/>
-      <c r="R27" s="72"/>
-      <c r="S27" s="72"/>
+      <c r="O27" s="58"/>
+      <c r="P27" s="58"/>
+      <c r="Q27" s="58"/>
+      <c r="R27" s="58"/>
+      <c r="S27" s="58"/>
     </row>
     <row r="28" spans="1:19" ht="30">
-      <c r="A28" s="79" t="s">
+      <c r="A28" s="121" t="s">
         <v>29</v>
       </c>
-      <c r="B28" s="80"/>
-      <c r="C28" s="73" t="s">
+      <c r="B28" s="122"/>
+      <c r="C28" s="98" t="s">
         <v>92</v>
       </c>
-      <c r="D28" s="74"/>
-      <c r="E28" s="74"/>
-      <c r="F28" s="74"/>
-      <c r="G28" s="75"/>
-      <c r="H28" s="76" t="s">
+      <c r="D28" s="99"/>
+      <c r="E28" s="99"/>
+      <c r="F28" s="99"/>
+      <c r="G28" s="100"/>
+      <c r="H28" s="118" t="s">
         <v>90</v>
       </c>
-      <c r="I28" s="77"/>
-      <c r="J28" s="77"/>
-      <c r="K28" s="78"/>
+      <c r="I28" s="119"/>
+      <c r="J28" s="119"/>
+      <c r="K28" s="120"/>
       <c r="L28" s="48" t="s">
         <v>91</v>
       </c>
-      <c r="N28" s="58" t="s">
+      <c r="N28" s="104" t="s">
         <v>116</v>
       </c>
-      <c r="O28" s="58"/>
-      <c r="P28" s="58"/>
-      <c r="Q28" s="58"/>
-      <c r="R28" s="58"/>
-      <c r="S28" s="58"/>
+      <c r="O28" s="104"/>
+      <c r="P28" s="104"/>
+      <c r="Q28" s="104"/>
+      <c r="R28" s="104"/>
+      <c r="S28" s="104"/>
     </row>
     <row r="29" spans="1:19" ht="4.5" customHeight="1">
       <c r="A29" s="28"/>
@@ -2493,100 +2486,100 @@
       <c r="L29" s="30"/>
     </row>
     <row r="30" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A30" s="85" t="s">
+      <c r="A30" s="69" t="s">
         <v>38</v>
       </c>
-      <c r="B30" s="86"/>
-      <c r="C30" s="81"/>
-      <c r="D30" s="82"/>
-      <c r="E30" s="82"/>
-      <c r="F30" s="82"/>
-      <c r="G30" s="83"/>
-      <c r="H30" s="84"/>
-      <c r="I30" s="82"/>
-      <c r="J30" s="82"/>
-      <c r="K30" s="83"/>
+      <c r="B30" s="70"/>
+      <c r="C30" s="88"/>
+      <c r="D30" s="89"/>
+      <c r="E30" s="89"/>
+      <c r="F30" s="89"/>
+      <c r="G30" s="90"/>
+      <c r="H30" s="91"/>
+      <c r="I30" s="89"/>
+      <c r="J30" s="89"/>
+      <c r="K30" s="90"/>
       <c r="L30" s="21" t="s">
         <v>5</v>
       </c>
       <c r="M30" s="32"/>
-      <c r="N30" s="122" t="s">
+      <c r="N30" s="60" t="s">
         <v>78</v>
       </c>
-      <c r="O30" s="122"/>
-      <c r="P30" s="122"/>
-      <c r="Q30" s="122"/>
-      <c r="R30" s="122"/>
-      <c r="S30" s="122"/>
+      <c r="O30" s="60"/>
+      <c r="P30" s="60"/>
+      <c r="Q30" s="60"/>
+      <c r="R30" s="60"/>
+      <c r="S30" s="60"/>
     </row>
     <row r="31" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A31" s="85" t="s">
+      <c r="A31" s="69" t="s">
         <v>83</v>
       </c>
-      <c r="B31" s="86"/>
-      <c r="C31" s="73"/>
-      <c r="D31" s="74"/>
-      <c r="E31" s="74"/>
-      <c r="F31" s="74"/>
-      <c r="G31" s="75"/>
-      <c r="H31" s="95" t="s">
+      <c r="B31" s="70"/>
+      <c r="C31" s="98"/>
+      <c r="D31" s="99"/>
+      <c r="E31" s="99"/>
+      <c r="F31" s="99"/>
+      <c r="G31" s="100"/>
+      <c r="H31" s="101" t="s">
         <v>84</v>
       </c>
-      <c r="I31" s="96"/>
-      <c r="J31" s="96"/>
-      <c r="K31" s="96"/>
-      <c r="L31" s="97"/>
+      <c r="I31" s="102"/>
+      <c r="J31" s="102"/>
+      <c r="K31" s="102"/>
+      <c r="L31" s="103"/>
       <c r="M31" s="32"/>
-      <c r="N31" s="122" t="s">
+      <c r="N31" s="60" t="s">
         <v>74</v>
       </c>
-      <c r="O31" s="122"/>
-      <c r="P31" s="122"/>
-      <c r="Q31" s="122"/>
-      <c r="R31" s="122"/>
-      <c r="S31" s="122"/>
+      <c r="O31" s="60"/>
+      <c r="P31" s="60"/>
+      <c r="Q31" s="60"/>
+      <c r="R31" s="60"/>
+      <c r="S31" s="60"/>
     </row>
     <row r="32" spans="1:19" ht="16.5" thickBot="1">
-      <c r="A32" s="89" t="s">
+      <c r="A32" s="94" t="s">
         <v>59</v>
       </c>
-      <c r="B32" s="90"/>
-      <c r="C32" s="91"/>
-      <c r="D32" s="92"/>
-      <c r="E32" s="92"/>
-      <c r="F32" s="92"/>
-      <c r="G32" s="93"/>
-      <c r="H32" s="94"/>
-      <c r="I32" s="92"/>
-      <c r="J32" s="92"/>
-      <c r="K32" s="93"/>
+      <c r="B32" s="95"/>
+      <c r="C32" s="85"/>
+      <c r="D32" s="86"/>
+      <c r="E32" s="86"/>
+      <c r="F32" s="86"/>
+      <c r="G32" s="96"/>
+      <c r="H32" s="97"/>
+      <c r="I32" s="86"/>
+      <c r="J32" s="86"/>
+      <c r="K32" s="96"/>
       <c r="M32" s="32"/>
     </row>
     <row r="33" spans="1:19" ht="30.75" customHeight="1" thickBot="1">
-      <c r="A33" s="87" t="s">
+      <c r="A33" s="92" t="s">
         <v>34</v>
       </c>
-      <c r="B33" s="88"/>
-      <c r="C33" s="103" t="s">
+      <c r="B33" s="93"/>
+      <c r="C33" s="76" t="s">
         <v>58</v>
       </c>
-      <c r="D33" s="104"/>
-      <c r="E33" s="104"/>
-      <c r="F33" s="104"/>
-      <c r="G33" s="105"/>
-      <c r="H33" s="100"/>
-      <c r="I33" s="101"/>
-      <c r="J33" s="101"/>
-      <c r="K33" s="102"/>
+      <c r="D33" s="77"/>
+      <c r="E33" s="77"/>
+      <c r="F33" s="77"/>
+      <c r="G33" s="78"/>
+      <c r="H33" s="73"/>
+      <c r="I33" s="74"/>
+      <c r="J33" s="74"/>
+      <c r="K33" s="75"/>
       <c r="M33" s="32"/>
-      <c r="N33" s="121" t="s">
+      <c r="N33" s="59" t="s">
         <v>75</v>
       </c>
-      <c r="O33" s="121"/>
-      <c r="P33" s="121"/>
-      <c r="Q33" s="121"/>
-      <c r="R33" s="121"/>
-      <c r="S33" s="121"/>
+      <c r="O33" s="59"/>
+      <c r="P33" s="59"/>
+      <c r="Q33" s="59"/>
+      <c r="R33" s="59"/>
+      <c r="S33" s="59"/>
     </row>
     <row r="34" spans="1:19" ht="4.5" customHeight="1" thickBot="1">
       <c r="A34" s="28"/>
@@ -2602,108 +2595,108 @@
       <c r="K34" s="30"/>
     </row>
     <row r="35" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A35" s="85" t="s">
+      <c r="A35" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="86"/>
-      <c r="C35" s="91"/>
-      <c r="D35" s="92"/>
-      <c r="E35" s="92"/>
-      <c r="F35" s="92"/>
-      <c r="G35" s="112"/>
-      <c r="H35" s="106"/>
-      <c r="I35" s="107"/>
-      <c r="J35" s="107"/>
-      <c r="K35" s="108"/>
+      <c r="B35" s="70"/>
+      <c r="C35" s="85"/>
+      <c r="D35" s="86"/>
+      <c r="E35" s="86"/>
+      <c r="F35" s="86"/>
+      <c r="G35" s="87"/>
+      <c r="H35" s="79"/>
+      <c r="I35" s="80"/>
+      <c r="J35" s="80"/>
+      <c r="K35" s="81"/>
       <c r="M35" s="32"/>
     </row>
     <row r="36" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A36" s="85" t="s">
+      <c r="A36" s="69" t="s">
         <v>94</v>
       </c>
-      <c r="B36" s="86"/>
-      <c r="C36" s="91"/>
-      <c r="D36" s="92"/>
-      <c r="E36" s="92"/>
-      <c r="F36" s="92"/>
-      <c r="G36" s="112"/>
-      <c r="H36" s="106"/>
-      <c r="I36" s="107"/>
-      <c r="J36" s="107"/>
-      <c r="K36" s="108"/>
+      <c r="B36" s="70"/>
+      <c r="C36" s="85"/>
+      <c r="D36" s="86"/>
+      <c r="E36" s="86"/>
+      <c r="F36" s="86"/>
+      <c r="G36" s="87"/>
+      <c r="H36" s="79"/>
+      <c r="I36" s="80"/>
+      <c r="J36" s="80"/>
+      <c r="K36" s="81"/>
       <c r="M36" s="32"/>
-      <c r="N36" s="122" t="s">
+      <c r="N36" s="60" t="s">
         <v>76</v>
       </c>
-      <c r="O36" s="122"/>
-      <c r="P36" s="122"/>
-      <c r="Q36" s="122"/>
-      <c r="R36" s="122"/>
-      <c r="S36" s="122"/>
+      <c r="O36" s="60"/>
+      <c r="P36" s="60"/>
+      <c r="Q36" s="60"/>
+      <c r="R36" s="60"/>
+      <c r="S36" s="60"/>
     </row>
     <row r="37" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A37" s="85" t="s">
+      <c r="A37" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="B37" s="86"/>
-      <c r="C37" s="109"/>
-      <c r="D37" s="110"/>
-      <c r="E37" s="110"/>
-      <c r="F37" s="110"/>
-      <c r="G37" s="111"/>
-      <c r="H37" s="109"/>
-      <c r="I37" s="110"/>
-      <c r="J37" s="110"/>
-      <c r="K37" s="111"/>
+      <c r="B37" s="70"/>
+      <c r="C37" s="82"/>
+      <c r="D37" s="83"/>
+      <c r="E37" s="83"/>
+      <c r="F37" s="83"/>
+      <c r="G37" s="84"/>
+      <c r="H37" s="82"/>
+      <c r="I37" s="83"/>
+      <c r="J37" s="83"/>
+      <c r="K37" s="84"/>
       <c r="M37" s="32"/>
     </row>
     <row r="38" spans="1:19" ht="15.75" thickBot="1">
-      <c r="N38" s="72" t="s">
+      <c r="N38" s="58" t="s">
         <v>86</v>
       </c>
-      <c r="O38" s="72"/>
-      <c r="P38" s="72"/>
-      <c r="Q38" s="72"/>
-      <c r="R38" s="72"/>
-      <c r="S38" s="72"/>
+      <c r="O38" s="58"/>
+      <c r="P38" s="58"/>
+      <c r="Q38" s="58"/>
+      <c r="R38" s="58"/>
+      <c r="S38" s="58"/>
     </row>
     <row r="39" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A39" s="114" t="s">
+      <c r="A39" s="62" t="s">
         <v>25</v>
       </c>
-      <c r="B39" s="115"/>
-      <c r="C39" s="115"/>
-      <c r="D39" s="115"/>
-      <c r="E39" s="116"/>
+      <c r="B39" s="63"/>
+      <c r="C39" s="63"/>
+      <c r="D39" s="63"/>
+      <c r="E39" s="64"/>
     </row>
     <row r="40" spans="1:19">
       <c r="A40" s="14" t="s">
         <v>24</v>
       </c>
       <c r="B40" s="13"/>
-      <c r="C40" s="117" t="s">
+      <c r="C40" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="D40" s="118"/>
+      <c r="D40" s="66"/>
       <c r="E40" s="27"/>
-      <c r="N40" s="72" t="s">
+      <c r="N40" s="58" t="s">
         <v>115</v>
       </c>
-      <c r="O40" s="72"/>
-      <c r="P40" s="72"/>
-      <c r="Q40" s="72"/>
-      <c r="R40" s="72"/>
-      <c r="S40" s="72"/>
+      <c r="O40" s="58"/>
+      <c r="P40" s="58"/>
+      <c r="Q40" s="58"/>
+      <c r="R40" s="58"/>
+      <c r="S40" s="58"/>
     </row>
     <row r="41" spans="1:19">
       <c r="A41" s="15" t="s">
         <v>21</v>
       </c>
       <c r="B41" s="5"/>
-      <c r="C41" s="117" t="s">
+      <c r="C41" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="D41" s="118"/>
+      <c r="D41" s="66"/>
       <c r="E41" s="8"/>
     </row>
     <row r="42" spans="1:19">
@@ -2711,10 +2704,10 @@
         <v>117</v>
       </c>
       <c r="B42" s="57"/>
-      <c r="C42" s="98" t="s">
+      <c r="C42" s="71" t="s">
         <v>64</v>
       </c>
-      <c r="D42" s="99"/>
+      <c r="D42" s="72"/>
       <c r="E42" s="37"/>
     </row>
     <row r="43" spans="1:19" ht="18" thickBot="1">
@@ -2726,20 +2719,20 @@
       </c>
     </row>
     <row r="44" spans="1:19">
-      <c r="A44" s="119" t="s">
+      <c r="A44" s="67" t="s">
         <v>35</v>
       </c>
-      <c r="B44" s="120"/>
-      <c r="C44" s="120"/>
-      <c r="D44" s="120"/>
-      <c r="E44" s="120"/>
-      <c r="F44" s="120"/>
-      <c r="G44" s="120"/>
-      <c r="H44" s="120"/>
-      <c r="I44" s="120"/>
-      <c r="J44" s="120"/>
-      <c r="K44" s="120"/>
-      <c r="L44" s="120"/>
+      <c r="B44" s="68"/>
+      <c r="C44" s="68"/>
+      <c r="D44" s="68"/>
+      <c r="E44" s="68"/>
+      <c r="F44" s="68"/>
+      <c r="G44" s="68"/>
+      <c r="H44" s="68"/>
+      <c r="I44" s="68"/>
+      <c r="J44" s="68"/>
+      <c r="K44" s="68"/>
+      <c r="L44" s="68"/>
       <c r="O44" t="s">
         <v>100</v>
       </c>
@@ -2748,37 +2741,37 @@
       <c r="A45" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="B45" s="113" t="s">
+      <c r="B45" s="61" t="s">
         <v>55</v>
       </c>
-      <c r="C45" s="113"/>
-      <c r="D45" s="113"/>
-      <c r="E45" s="113"/>
-      <c r="F45" s="113"/>
-      <c r="G45" s="113"/>
-      <c r="H45" s="113"/>
-      <c r="I45" s="113"/>
-      <c r="J45" s="113"/>
-      <c r="K45" s="113"/>
-      <c r="L45" s="113"/>
+      <c r="C45" s="61"/>
+      <c r="D45" s="61"/>
+      <c r="E45" s="61"/>
+      <c r="F45" s="61"/>
+      <c r="G45" s="61"/>
+      <c r="H45" s="61"/>
+      <c r="I45" s="61"/>
+      <c r="J45" s="61"/>
+      <c r="K45" s="61"/>
+      <c r="L45" s="61"/>
     </row>
     <row r="46" spans="1:19" ht="15" customHeight="1">
       <c r="A46" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="B46" s="113" t="s">
+      <c r="B46" s="61" t="s">
         <v>56</v>
       </c>
-      <c r="C46" s="113"/>
-      <c r="D46" s="113"/>
-      <c r="E46" s="113"/>
-      <c r="F46" s="113"/>
-      <c r="G46" s="113"/>
-      <c r="H46" s="113"/>
-      <c r="I46" s="113"/>
-      <c r="J46" s="113"/>
-      <c r="K46" s="113"/>
-      <c r="L46" s="113"/>
+      <c r="C46" s="61"/>
+      <c r="D46" s="61"/>
+      <c r="E46" s="61"/>
+      <c r="F46" s="61"/>
+      <c r="G46" s="61"/>
+      <c r="H46" s="61"/>
+      <c r="I46" s="61"/>
+      <c r="J46" s="61"/>
+      <c r="K46" s="61"/>
+      <c r="L46" s="61"/>
       <c r="N46" s="49" t="s">
         <v>97</v>
       </c>
@@ -2790,19 +2783,19 @@
       <c r="A47" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="B47" s="113" t="s">
+      <c r="B47" s="61" t="s">
         <v>57</v>
       </c>
-      <c r="C47" s="113"/>
-      <c r="D47" s="113"/>
-      <c r="E47" s="113"/>
-      <c r="F47" s="113"/>
-      <c r="G47" s="113"/>
-      <c r="H47" s="113"/>
-      <c r="I47" s="113"/>
-      <c r="J47" s="113"/>
-      <c r="K47" s="113"/>
-      <c r="L47" s="113"/>
+      <c r="C47" s="61"/>
+      <c r="D47" s="61"/>
+      <c r="E47" s="61"/>
+      <c r="F47" s="61"/>
+      <c r="G47" s="61"/>
+      <c r="H47" s="61"/>
+      <c r="I47" s="61"/>
+      <c r="J47" s="61"/>
+      <c r="K47" s="61"/>
+      <c r="L47" s="61"/>
       <c r="O47" s="43" t="s">
         <v>101</v>
       </c>
@@ -2811,19 +2804,19 @@
       <c r="A48" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="B48" s="113" t="s">
+      <c r="B48" s="61" t="s">
         <v>44</v>
       </c>
-      <c r="C48" s="113"/>
-      <c r="D48" s="113"/>
-      <c r="E48" s="113"/>
-      <c r="F48" s="113"/>
-      <c r="G48" s="113"/>
-      <c r="H48" s="113"/>
-      <c r="I48" s="113"/>
-      <c r="J48" s="113"/>
-      <c r="K48" s="113"/>
-      <c r="L48" s="113"/>
+      <c r="C48" s="61"/>
+      <c r="D48" s="61"/>
+      <c r="E48" s="61"/>
+      <c r="F48" s="61"/>
+      <c r="G48" s="61"/>
+      <c r="H48" s="61"/>
+      <c r="I48" s="61"/>
+      <c r="J48" s="61"/>
+      <c r="K48" s="61"/>
+      <c r="L48" s="61"/>
       <c r="O48" t="s">
         <v>104</v>
       </c>
@@ -2832,37 +2825,37 @@
       <c r="A49" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="B49" s="113" t="s">
+      <c r="B49" s="61" t="s">
         <v>33</v>
       </c>
-      <c r="C49" s="113"/>
-      <c r="D49" s="113"/>
-      <c r="E49" s="113"/>
-      <c r="F49" s="113"/>
-      <c r="G49" s="113"/>
-      <c r="H49" s="113"/>
-      <c r="I49" s="113"/>
-      <c r="J49" s="113"/>
-      <c r="K49" s="113"/>
-      <c r="L49" s="113"/>
+      <c r="C49" s="61"/>
+      <c r="D49" s="61"/>
+      <c r="E49" s="61"/>
+      <c r="F49" s="61"/>
+      <c r="G49" s="61"/>
+      <c r="H49" s="61"/>
+      <c r="I49" s="61"/>
+      <c r="J49" s="61"/>
+      <c r="K49" s="61"/>
+      <c r="L49" s="61"/>
     </row>
     <row r="50" spans="1:15" ht="17.25">
       <c r="A50" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="B50" s="113" t="s">
+      <c r="B50" s="61" t="s">
         <v>54</v>
       </c>
-      <c r="C50" s="113"/>
-      <c r="D50" s="113"/>
-      <c r="E50" s="113"/>
-      <c r="F50" s="113"/>
-      <c r="G50" s="113"/>
-      <c r="H50" s="113"/>
-      <c r="I50" s="113"/>
-      <c r="J50" s="113"/>
-      <c r="K50" s="113"/>
-      <c r="L50" s="113"/>
+      <c r="C50" s="61"/>
+      <c r="D50" s="61"/>
+      <c r="E50" s="61"/>
+      <c r="F50" s="61"/>
+      <c r="G50" s="61"/>
+      <c r="H50" s="61"/>
+      <c r="I50" s="61"/>
+      <c r="J50" s="61"/>
+      <c r="K50" s="61"/>
+      <c r="L50" s="61"/>
       <c r="N50" s="49" t="s">
         <v>96</v>
       </c>
@@ -2874,19 +2867,19 @@
       <c r="A51" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="B51" s="113" t="s">
+      <c r="B51" s="61" t="s">
         <v>53</v>
       </c>
-      <c r="C51" s="113"/>
-      <c r="D51" s="113"/>
-      <c r="E51" s="113"/>
-      <c r="F51" s="113"/>
-      <c r="G51" s="113"/>
-      <c r="H51" s="113"/>
-      <c r="I51" s="113"/>
-      <c r="J51" s="113"/>
-      <c r="K51" s="113"/>
-      <c r="L51" s="113"/>
+      <c r="C51" s="61"/>
+      <c r="D51" s="61"/>
+      <c r="E51" s="61"/>
+      <c r="F51" s="61"/>
+      <c r="G51" s="61"/>
+      <c r="H51" s="61"/>
+      <c r="I51" s="61"/>
+      <c r="J51" s="61"/>
+      <c r="K51" s="61"/>
+      <c r="L51" s="61"/>
       <c r="O51" t="s">
         <v>102</v>
       </c>
@@ -2908,24 +2901,31 @@
     <sortCondition ref="A3"/>
   </sortState>
   <mergeCells count="56">
-    <mergeCell ref="N20:S20"/>
-    <mergeCell ref="N40:S40"/>
-    <mergeCell ref="N33:S33"/>
-    <mergeCell ref="N36:S36"/>
-    <mergeCell ref="N30:S30"/>
-    <mergeCell ref="N31:S31"/>
-    <mergeCell ref="N38:S38"/>
-    <mergeCell ref="B50:L50"/>
-    <mergeCell ref="B51:L51"/>
-    <mergeCell ref="A39:E39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="B45:L45"/>
-    <mergeCell ref="A44:L44"/>
-    <mergeCell ref="B46:L46"/>
-    <mergeCell ref="B47:L47"/>
-    <mergeCell ref="B48:L48"/>
-    <mergeCell ref="B49:L49"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="H28:K28"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="O6:U6"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="H27:K27"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="O15:S16"/>
+    <mergeCell ref="N24:S24"/>
+    <mergeCell ref="N27:S27"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="H30:K30"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="H32:K32"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="H31:L31"/>
     <mergeCell ref="A35:B35"/>
     <mergeCell ref="A36:B36"/>
     <mergeCell ref="A37:B37"/>
@@ -2938,32 +2938,25 @@
     <mergeCell ref="C35:G35"/>
     <mergeCell ref="C36:G36"/>
     <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="H30:K30"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="H32:K32"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="H31:L31"/>
+    <mergeCell ref="B50:L50"/>
+    <mergeCell ref="B51:L51"/>
+    <mergeCell ref="A39:E39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="B45:L45"/>
+    <mergeCell ref="A44:L44"/>
+    <mergeCell ref="B46:L46"/>
+    <mergeCell ref="B47:L47"/>
+    <mergeCell ref="B48:L48"/>
+    <mergeCell ref="B49:L49"/>
+    <mergeCell ref="N20:S20"/>
+    <mergeCell ref="N40:S40"/>
+    <mergeCell ref="N33:S33"/>
+    <mergeCell ref="N36:S36"/>
+    <mergeCell ref="N30:S30"/>
+    <mergeCell ref="N31:S31"/>
+    <mergeCell ref="N38:S38"/>
     <mergeCell ref="N28:S28"/>
-    <mergeCell ref="O6:U6"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="H27:K27"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="O15:S16"/>
-    <mergeCell ref="N24:S24"/>
-    <mergeCell ref="N27:S27"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="H28:K28"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="A28:B28"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="Q4" r:id="rId1"/>

</xml_diff>

<commit_message>
cuadro de estado con cambios
</commit_message>
<xml_diff>
--- a/Cuadro-de-estado.xlsx
+++ b/Cuadro-de-estado.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Test" sheetId="4" r:id="rId2"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId3"/>
+    <sheet name="Info_CV" sheetId="2" r:id="rId3"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="129">
   <si>
     <t>BACKEND</t>
   </si>
@@ -459,6 +459,36 @@
   <si>
     <t>OJO CON LOS GET HTTP, que no hayan desparramados o dobles llamadas</t>
   </si>
+  <si>
+    <t>Independencia y motivación</t>
+  </si>
+  <si>
+    <t>Un buen desarrollador es capaz de motivarse él solo y, sobre todo, es capaz de interesarse en problemas que sean difíciles de resolver sin un empuje externo</t>
+  </si>
+  <si>
+    <t>de todas maneras aprender de manera autodidacta otro lenguaje o framework, aprender es divertido</t>
+  </si>
+  <si>
+    <t>Cuando termino algo, siempre tengo más ganas de hacer lo mismo pero con mejoras o funcionalidades nuevas</t>
+  </si>
+  <si>
+    <t>No tiene que ser necesariamente libros, puede ser también artículos en Internet o posteos de algún blog, pero todos pasan al menos 30 minutos al día leyendo, algunos incluso varias horas</t>
+  </si>
+  <si>
+    <t>Intereses</t>
+  </si>
+  <si>
+    <t>Soy un desarrollador front-end ubicado en Polonia. Tengo una gran pasión por los efectos de interfaz de usuario, las animaciones y la creación de experiencias de usuario intuitivas y dinámicas.</t>
+  </si>
+  <si>
+    <t>Persona bien organizada, solucionador de problemas, empleado independiente con gran atención a los detalles. Aficionado a las MMA, las actividades al aire libre, las series de TV y la literatura inglesa. Una persona de familia y padre de dos niños rebeldes,</t>
+  </si>
+  <si>
+    <t>Interesado en todo el espectro frontend y trabajando en proyectos ambiciosos con personas positivas.</t>
+  </si>
+  <si>
+    <t>Hagamos algo especial.</t>
+  </si>
 </sst>
 </file>
 
@@ -467,7 +497,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
   </numFmts>
-  <fonts count="28">
+  <fonts count="29">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -678,6 +708,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="15">
     <fill>
@@ -1348,208 +1386,206 @@
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1853,7 +1889,7 @@
   <dimension ref="A1:U54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1870,25 +1906,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25">
-      <c r="A1" s="107" t="s">
+      <c r="A1" s="72" t="s">
         <v>88</v>
       </c>
-      <c r="B1" s="107"/>
-      <c r="C1" s="107"/>
-      <c r="D1" s="107"/>
-      <c r="E1" s="107"/>
-      <c r="F1" s="107"/>
-      <c r="G1" s="107"/>
-      <c r="H1" s="107"/>
-      <c r="I1" s="107"/>
-      <c r="J1" s="107"/>
-      <c r="K1" s="107"/>
-      <c r="L1" s="107"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="72"/>
+      <c r="I1" s="72"/>
+      <c r="J1" s="72"/>
+      <c r="K1" s="72"/>
+      <c r="L1" s="72"/>
     </row>
     <row r="2" spans="1:21" ht="19.5" thickBot="1">
       <c r="A2" s="45">
         <f ca="1">M2-TODAY()-1</f>
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B2" s="46" t="s">
         <v>89</v>
@@ -1902,30 +1938,30 @@
       </c>
     </row>
     <row r="3" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="108" t="s">
+      <c r="A3" s="73" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="109"/>
-      <c r="C3" s="110" t="s">
+      <c r="B3" s="74"/>
+      <c r="C3" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="111"/>
-      <c r="E3" s="111"/>
-      <c r="F3" s="111"/>
-      <c r="G3" s="112"/>
-      <c r="H3" s="110" t="s">
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="111"/>
-      <c r="J3" s="113"/>
-      <c r="K3" s="112"/>
+      <c r="I3" s="65"/>
+      <c r="J3" s="66"/>
+      <c r="K3" s="67"/>
       <c r="L3" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="114" t="s">
+      <c r="M3" s="75" t="s">
         <v>79</v>
       </c>
-      <c r="N3" s="106"/>
+      <c r="N3" s="71"/>
     </row>
     <row r="4" spans="1:21" s="3" customFormat="1" ht="40.5" customHeight="1" thickBot="1">
       <c r="A4" s="17" t="s">
@@ -1964,10 +2000,10 @@
       <c r="L4" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="M4" s="115" t="s">
+      <c r="M4" s="76" t="s">
         <v>80</v>
       </c>
-      <c r="N4" s="116"/>
+      <c r="N4" s="77"/>
       <c r="O4" s="34" t="s">
         <v>61</v>
       </c>
@@ -1996,11 +2032,11 @@
       <c r="B6" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
@@ -2009,15 +2045,15 @@
       <c r="M6" s="42" t="s">
         <v>82</v>
       </c>
-      <c r="O6" s="105" t="s">
+      <c r="O6" s="70" t="s">
         <v>65</v>
       </c>
-      <c r="P6" s="106"/>
-      <c r="Q6" s="106"/>
-      <c r="R6" s="106"/>
-      <c r="S6" s="106"/>
-      <c r="T6" s="106"/>
-      <c r="U6" s="106"/>
+      <c r="P6" s="71"/>
+      <c r="Q6" s="71"/>
+      <c r="R6" s="71"/>
+      <c r="S6" s="71"/>
+      <c r="T6" s="71"/>
+      <c r="U6" s="71"/>
     </row>
     <row r="7" spans="1:21" ht="4.5" customHeight="1">
       <c r="A7" s="28"/>
@@ -2127,17 +2163,17 @@
     </row>
     <row r="12" spans="1:21" ht="4.5" customHeight="1">
       <c r="A12" s="28"/>
-      <c r="B12" s="54"/>
-      <c r="C12" s="55"/>
-      <c r="D12" s="55"/>
-      <c r="E12" s="55"/>
-      <c r="F12" s="55"/>
-      <c r="G12" s="55"/>
-      <c r="H12" s="55"/>
-      <c r="I12" s="55"/>
-      <c r="J12" s="55"/>
-      <c r="K12" s="55"/>
-      <c r="L12" s="55"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="28"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="28"/>
     </row>
     <row r="13" spans="1:21">
       <c r="A13" s="38" t="s">
@@ -2154,7 +2190,7 @@
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
-      <c r="K13" s="57"/>
+      <c r="K13" s="55"/>
       <c r="L13" s="4"/>
       <c r="O13" t="s">
         <v>70</v>
@@ -2178,7 +2214,7 @@
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
-      <c r="K14" s="57"/>
+      <c r="K14" s="55"/>
       <c r="L14" s="4"/>
       <c r="O14" t="s">
         <v>93</v>
@@ -2199,16 +2235,16 @@
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
-      <c r="K15" s="57"/>
+      <c r="K15" s="55"/>
       <c r="L15" s="4"/>
-      <c r="O15" s="117" t="s">
+      <c r="O15" s="78" t="s">
         <v>77</v>
       </c>
-      <c r="P15" s="117"/>
-      <c r="Q15" s="117"/>
-      <c r="R15" s="117"/>
-      <c r="S15" s="117"/>
-      <c r="T15" s="56"/>
+      <c r="P15" s="78"/>
+      <c r="Q15" s="78"/>
+      <c r="R15" s="78"/>
+      <c r="S15" s="78"/>
+      <c r="T15" s="54"/>
     </row>
     <row r="16" spans="1:21">
       <c r="A16" s="18" t="s">
@@ -2220,19 +2256,19 @@
       <c r="C16" s="4"/>
       <c r="D16" s="40"/>
       <c r="E16" s="4"/>
-      <c r="F16" s="57"/>
+      <c r="F16" s="55"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
       <c r="L16" s="4"/>
-      <c r="O16" s="117"/>
-      <c r="P16" s="117"/>
-      <c r="Q16" s="117"/>
-      <c r="R16" s="117"/>
-      <c r="S16" s="117"/>
-      <c r="T16" s="56"/>
+      <c r="O16" s="78"/>
+      <c r="P16" s="78"/>
+      <c r="Q16" s="78"/>
+      <c r="R16" s="78"/>
+      <c r="S16" s="78"/>
+      <c r="T16" s="54"/>
     </row>
     <row r="17" spans="1:19">
       <c r="A17" s="18" t="s">
@@ -2244,7 +2280,7 @@
       <c r="C17" s="4"/>
       <c r="D17" s="40"/>
       <c r="E17" s="4"/>
-      <c r="F17" s="57"/>
+      <c r="F17" s="55"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
@@ -2278,7 +2314,7 @@
       </c>
       <c r="C19" s="22"/>
       <c r="D19" s="41"/>
-      <c r="E19" s="57"/>
+      <c r="E19" s="55"/>
       <c r="F19" s="8"/>
       <c r="G19" s="7"/>
       <c r="H19" s="5"/>
@@ -2296,7 +2332,7 @@
       </c>
       <c r="C20" s="22"/>
       <c r="D20" s="41"/>
-      <c r="E20" s="57"/>
+      <c r="E20" s="55"/>
       <c r="F20" s="8"/>
       <c r="G20" s="7"/>
       <c r="H20" s="5"/>
@@ -2304,14 +2340,14 @@
       <c r="J20" s="5"/>
       <c r="K20" s="7"/>
       <c r="L20" s="53"/>
-      <c r="N20" s="58" t="s">
+      <c r="N20" s="79" t="s">
         <v>118</v>
       </c>
-      <c r="O20" s="58"/>
-      <c r="P20" s="58"/>
-      <c r="Q20" s="58"/>
-      <c r="R20" s="58"/>
-      <c r="S20" s="58"/>
+      <c r="O20" s="79"/>
+      <c r="P20" s="79"/>
+      <c r="Q20" s="79"/>
+      <c r="R20" s="79"/>
+      <c r="S20" s="79"/>
     </row>
     <row r="21" spans="1:19" ht="4.5" customHeight="1">
       <c r="A21" s="28"/>
@@ -2334,7 +2370,7 @@
       <c r="B22" s="19"/>
       <c r="C22" s="16"/>
       <c r="D22" s="8"/>
-      <c r="E22" s="57"/>
+      <c r="E22" s="55"/>
       <c r="F22" s="8"/>
       <c r="G22" s="4"/>
       <c r="H22" s="5"/>
@@ -2364,7 +2400,7 @@
       <c r="B24" s="31"/>
       <c r="C24" s="8"/>
       <c r="D24" s="5"/>
-      <c r="E24" s="57"/>
+      <c r="E24" s="55"/>
       <c r="F24" s="8"/>
       <c r="G24" s="7"/>
       <c r="H24" s="5"/>
@@ -2372,14 +2408,14 @@
       <c r="J24" s="5"/>
       <c r="K24" s="7"/>
       <c r="L24" s="4"/>
-      <c r="N24" s="58" t="s">
+      <c r="N24" s="79" t="s">
         <v>87</v>
       </c>
-      <c r="O24" s="58"/>
-      <c r="P24" s="58"/>
-      <c r="Q24" s="58"/>
-      <c r="R24" s="58"/>
-      <c r="S24" s="58"/>
+      <c r="O24" s="79"/>
+      <c r="P24" s="79"/>
+      <c r="Q24" s="79"/>
+      <c r="R24" s="79"/>
+      <c r="S24" s="79"/>
     </row>
     <row r="25" spans="1:19">
       <c r="A25" s="39" t="s">
@@ -2390,7 +2426,7 @@
       </c>
       <c r="C25" s="22"/>
       <c r="D25" s="8"/>
-      <c r="E25" s="57"/>
+      <c r="E25" s="55"/>
       <c r="F25" s="8"/>
       <c r="G25" s="8"/>
       <c r="H25" s="5"/>
@@ -2416,60 +2452,60 @@
     <row r="27" spans="1:19" ht="15.75" thickBot="1">
       <c r="A27" s="23"/>
       <c r="B27" s="25"/>
-      <c r="C27" s="110" t="s">
+      <c r="C27" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="111"/>
-      <c r="E27" s="111"/>
-      <c r="F27" s="111"/>
-      <c r="G27" s="112"/>
-      <c r="H27" s="110" t="s">
+      <c r="D27" s="65"/>
+      <c r="E27" s="65"/>
+      <c r="F27" s="65"/>
+      <c r="G27" s="67"/>
+      <c r="H27" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="I27" s="111"/>
-      <c r="J27" s="113"/>
-      <c r="K27" s="112"/>
+      <c r="I27" s="65"/>
+      <c r="J27" s="66"/>
+      <c r="K27" s="67"/>
       <c r="L27" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="N27" s="58" t="s">
+      <c r="N27" s="79" t="s">
         <v>81</v>
       </c>
-      <c r="O27" s="58"/>
-      <c r="P27" s="58"/>
-      <c r="Q27" s="58"/>
-      <c r="R27" s="58"/>
-      <c r="S27" s="58"/>
+      <c r="O27" s="79"/>
+      <c r="P27" s="79"/>
+      <c r="Q27" s="79"/>
+      <c r="R27" s="79"/>
+      <c r="S27" s="79"/>
     </row>
     <row r="28" spans="1:19" ht="30">
-      <c r="A28" s="121" t="s">
+      <c r="A28" s="68" t="s">
         <v>29</v>
       </c>
-      <c r="B28" s="122"/>
-      <c r="C28" s="98" t="s">
+      <c r="B28" s="69"/>
+      <c r="C28" s="58" t="s">
         <v>92</v>
       </c>
-      <c r="D28" s="99"/>
-      <c r="E28" s="99"/>
-      <c r="F28" s="99"/>
-      <c r="G28" s="100"/>
-      <c r="H28" s="118" t="s">
+      <c r="D28" s="59"/>
+      <c r="E28" s="59"/>
+      <c r="F28" s="59"/>
+      <c r="G28" s="60"/>
+      <c r="H28" s="61" t="s">
         <v>90</v>
       </c>
-      <c r="I28" s="119"/>
-      <c r="J28" s="119"/>
-      <c r="K28" s="120"/>
+      <c r="I28" s="62"/>
+      <c r="J28" s="62"/>
+      <c r="K28" s="63"/>
       <c r="L28" s="48" t="s">
         <v>91</v>
       </c>
-      <c r="N28" s="104" t="s">
+      <c r="N28" s="120" t="s">
         <v>116</v>
       </c>
-      <c r="O28" s="104"/>
-      <c r="P28" s="104"/>
-      <c r="Q28" s="104"/>
-      <c r="R28" s="104"/>
-      <c r="S28" s="104"/>
+      <c r="O28" s="120"/>
+      <c r="P28" s="120"/>
+      <c r="Q28" s="120"/>
+      <c r="R28" s="120"/>
+      <c r="S28" s="120"/>
     </row>
     <row r="29" spans="1:19" ht="4.5" customHeight="1">
       <c r="A29" s="28"/>
@@ -2486,100 +2522,100 @@
       <c r="L29" s="30"/>
     </row>
     <row r="30" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A30" s="69" t="s">
+      <c r="A30" s="84" t="s">
         <v>38</v>
       </c>
-      <c r="B30" s="70"/>
-      <c r="C30" s="88"/>
-      <c r="D30" s="89"/>
-      <c r="E30" s="89"/>
-      <c r="F30" s="89"/>
-      <c r="G30" s="90"/>
-      <c r="H30" s="91"/>
-      <c r="I30" s="89"/>
-      <c r="J30" s="89"/>
-      <c r="K30" s="90"/>
+      <c r="B30" s="85"/>
+      <c r="C30" s="80"/>
+      <c r="D30" s="81"/>
+      <c r="E30" s="81"/>
+      <c r="F30" s="81"/>
+      <c r="G30" s="82"/>
+      <c r="H30" s="83"/>
+      <c r="I30" s="81"/>
+      <c r="J30" s="81"/>
+      <c r="K30" s="82"/>
       <c r="L30" s="21" t="s">
         <v>5</v>
       </c>
       <c r="M30" s="32"/>
-      <c r="N30" s="60" t="s">
+      <c r="N30" s="122" t="s">
         <v>78</v>
       </c>
-      <c r="O30" s="60"/>
-      <c r="P30" s="60"/>
-      <c r="Q30" s="60"/>
-      <c r="R30" s="60"/>
-      <c r="S30" s="60"/>
+      <c r="O30" s="122"/>
+      <c r="P30" s="122"/>
+      <c r="Q30" s="122"/>
+      <c r="R30" s="122"/>
+      <c r="S30" s="122"/>
     </row>
     <row r="31" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A31" s="69" t="s">
+      <c r="A31" s="84" t="s">
         <v>83</v>
       </c>
-      <c r="B31" s="70"/>
-      <c r="C31" s="98"/>
-      <c r="D31" s="99"/>
-      <c r="E31" s="99"/>
-      <c r="F31" s="99"/>
-      <c r="G31" s="100"/>
-      <c r="H31" s="101" t="s">
+      <c r="B31" s="85"/>
+      <c r="C31" s="58"/>
+      <c r="D31" s="59"/>
+      <c r="E31" s="59"/>
+      <c r="F31" s="59"/>
+      <c r="G31" s="60"/>
+      <c r="H31" s="94" t="s">
         <v>84</v>
       </c>
-      <c r="I31" s="102"/>
-      <c r="J31" s="102"/>
-      <c r="K31" s="102"/>
-      <c r="L31" s="103"/>
+      <c r="I31" s="95"/>
+      <c r="J31" s="95"/>
+      <c r="K31" s="95"/>
+      <c r="L31" s="96"/>
       <c r="M31" s="32"/>
-      <c r="N31" s="60" t="s">
+      <c r="N31" s="122" t="s">
         <v>74</v>
       </c>
-      <c r="O31" s="60"/>
-      <c r="P31" s="60"/>
-      <c r="Q31" s="60"/>
-      <c r="R31" s="60"/>
-      <c r="S31" s="60"/>
+      <c r="O31" s="122"/>
+      <c r="P31" s="122"/>
+      <c r="Q31" s="122"/>
+      <c r="R31" s="122"/>
+      <c r="S31" s="122"/>
     </row>
     <row r="32" spans="1:19" ht="16.5" thickBot="1">
-      <c r="A32" s="94" t="s">
+      <c r="A32" s="88" t="s">
         <v>59</v>
       </c>
-      <c r="B32" s="95"/>
-      <c r="C32" s="85"/>
-      <c r="D32" s="86"/>
-      <c r="E32" s="86"/>
-      <c r="F32" s="86"/>
-      <c r="G32" s="96"/>
-      <c r="H32" s="97"/>
-      <c r="I32" s="86"/>
-      <c r="J32" s="86"/>
-      <c r="K32" s="96"/>
+      <c r="B32" s="89"/>
+      <c r="C32" s="90"/>
+      <c r="D32" s="91"/>
+      <c r="E32" s="91"/>
+      <c r="F32" s="91"/>
+      <c r="G32" s="92"/>
+      <c r="H32" s="93"/>
+      <c r="I32" s="91"/>
+      <c r="J32" s="91"/>
+      <c r="K32" s="92"/>
       <c r="M32" s="32"/>
     </row>
     <row r="33" spans="1:19" ht="30.75" customHeight="1" thickBot="1">
-      <c r="A33" s="92" t="s">
+      <c r="A33" s="86" t="s">
         <v>34</v>
       </c>
-      <c r="B33" s="93"/>
-      <c r="C33" s="76" t="s">
+      <c r="B33" s="87"/>
+      <c r="C33" s="102" t="s">
         <v>58</v>
       </c>
-      <c r="D33" s="77"/>
-      <c r="E33" s="77"/>
-      <c r="F33" s="77"/>
-      <c r="G33" s="78"/>
-      <c r="H33" s="73"/>
-      <c r="I33" s="74"/>
-      <c r="J33" s="74"/>
-      <c r="K33" s="75"/>
+      <c r="D33" s="103"/>
+      <c r="E33" s="103"/>
+      <c r="F33" s="103"/>
+      <c r="G33" s="104"/>
+      <c r="H33" s="99"/>
+      <c r="I33" s="100"/>
+      <c r="J33" s="100"/>
+      <c r="K33" s="101"/>
       <c r="M33" s="32"/>
-      <c r="N33" s="59" t="s">
+      <c r="N33" s="121" t="s">
         <v>75</v>
       </c>
-      <c r="O33" s="59"/>
-      <c r="P33" s="59"/>
-      <c r="Q33" s="59"/>
-      <c r="R33" s="59"/>
-      <c r="S33" s="59"/>
+      <c r="O33" s="121"/>
+      <c r="P33" s="121"/>
+      <c r="Q33" s="121"/>
+      <c r="R33" s="121"/>
+      <c r="S33" s="121"/>
     </row>
     <row r="34" spans="1:19" ht="4.5" customHeight="1" thickBot="1">
       <c r="A34" s="28"/>
@@ -2595,119 +2631,119 @@
       <c r="K34" s="30"/>
     </row>
     <row r="35" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A35" s="69" t="s">
+      <c r="A35" s="84" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="70"/>
-      <c r="C35" s="85"/>
-      <c r="D35" s="86"/>
-      <c r="E35" s="86"/>
-      <c r="F35" s="86"/>
-      <c r="G35" s="87"/>
-      <c r="H35" s="79"/>
-      <c r="I35" s="80"/>
-      <c r="J35" s="80"/>
-      <c r="K35" s="81"/>
+      <c r="B35" s="85"/>
+      <c r="C35" s="90"/>
+      <c r="D35" s="91"/>
+      <c r="E35" s="91"/>
+      <c r="F35" s="91"/>
+      <c r="G35" s="111"/>
+      <c r="H35" s="105"/>
+      <c r="I35" s="106"/>
+      <c r="J35" s="106"/>
+      <c r="K35" s="107"/>
       <c r="M35" s="32"/>
     </row>
     <row r="36" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A36" s="69" t="s">
+      <c r="A36" s="84" t="s">
         <v>94</v>
       </c>
-      <c r="B36" s="70"/>
-      <c r="C36" s="85"/>
-      <c r="D36" s="86"/>
-      <c r="E36" s="86"/>
-      <c r="F36" s="86"/>
-      <c r="G36" s="87"/>
-      <c r="H36" s="79"/>
-      <c r="I36" s="80"/>
-      <c r="J36" s="80"/>
-      <c r="K36" s="81"/>
+      <c r="B36" s="85"/>
+      <c r="C36" s="90"/>
+      <c r="D36" s="91"/>
+      <c r="E36" s="91"/>
+      <c r="F36" s="91"/>
+      <c r="G36" s="111"/>
+      <c r="H36" s="105"/>
+      <c r="I36" s="106"/>
+      <c r="J36" s="106"/>
+      <c r="K36" s="107"/>
       <c r="M36" s="32"/>
-      <c r="N36" s="60" t="s">
+      <c r="N36" s="122" t="s">
         <v>76</v>
       </c>
-      <c r="O36" s="60"/>
-      <c r="P36" s="60"/>
-      <c r="Q36" s="60"/>
-      <c r="R36" s="60"/>
-      <c r="S36" s="60"/>
+      <c r="O36" s="122"/>
+      <c r="P36" s="122"/>
+      <c r="Q36" s="122"/>
+      <c r="R36" s="122"/>
+      <c r="S36" s="122"/>
     </row>
     <row r="37" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A37" s="69" t="s">
+      <c r="A37" s="84" t="s">
         <v>7</v>
       </c>
-      <c r="B37" s="70"/>
-      <c r="C37" s="82"/>
-      <c r="D37" s="83"/>
-      <c r="E37" s="83"/>
-      <c r="F37" s="83"/>
-      <c r="G37" s="84"/>
-      <c r="H37" s="82"/>
-      <c r="I37" s="83"/>
-      <c r="J37" s="83"/>
-      <c r="K37" s="84"/>
+      <c r="B37" s="85"/>
+      <c r="C37" s="108"/>
+      <c r="D37" s="109"/>
+      <c r="E37" s="109"/>
+      <c r="F37" s="109"/>
+      <c r="G37" s="110"/>
+      <c r="H37" s="108"/>
+      <c r="I37" s="109"/>
+      <c r="J37" s="109"/>
+      <c r="K37" s="110"/>
       <c r="M37" s="32"/>
     </row>
     <row r="38" spans="1:19" ht="15.75" thickBot="1">
-      <c r="N38" s="58" t="s">
+      <c r="N38" s="79" t="s">
         <v>86</v>
       </c>
-      <c r="O38" s="58"/>
-      <c r="P38" s="58"/>
-      <c r="Q38" s="58"/>
-      <c r="R38" s="58"/>
-      <c r="S38" s="58"/>
+      <c r="O38" s="79"/>
+      <c r="P38" s="79"/>
+      <c r="Q38" s="79"/>
+      <c r="R38" s="79"/>
+      <c r="S38" s="79"/>
     </row>
     <row r="39" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A39" s="62" t="s">
+      <c r="A39" s="113" t="s">
         <v>25</v>
       </c>
-      <c r="B39" s="63"/>
-      <c r="C39" s="63"/>
-      <c r="D39" s="63"/>
-      <c r="E39" s="64"/>
+      <c r="B39" s="114"/>
+      <c r="C39" s="114"/>
+      <c r="D39" s="114"/>
+      <c r="E39" s="115"/>
     </row>
     <row r="40" spans="1:19">
       <c r="A40" s="14" t="s">
         <v>24</v>
       </c>
       <c r="B40" s="13"/>
-      <c r="C40" s="65" t="s">
+      <c r="C40" s="116" t="s">
         <v>22</v>
       </c>
-      <c r="D40" s="66"/>
+      <c r="D40" s="117"/>
       <c r="E40" s="27"/>
-      <c r="N40" s="58" t="s">
+      <c r="N40" s="79" t="s">
         <v>115</v>
       </c>
-      <c r="O40" s="58"/>
-      <c r="P40" s="58"/>
-      <c r="Q40" s="58"/>
-      <c r="R40" s="58"/>
-      <c r="S40" s="58"/>
+      <c r="O40" s="79"/>
+      <c r="P40" s="79"/>
+      <c r="Q40" s="79"/>
+      <c r="R40" s="79"/>
+      <c r="S40" s="79"/>
     </row>
     <row r="41" spans="1:19">
       <c r="A41" s="15" t="s">
         <v>21</v>
       </c>
       <c r="B41" s="5"/>
-      <c r="C41" s="65" t="s">
+      <c r="C41" s="116" t="s">
         <v>23</v>
       </c>
-      <c r="D41" s="66"/>
+      <c r="D41" s="117"/>
       <c r="E41" s="8"/>
     </row>
     <row r="42" spans="1:19">
       <c r="A42" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="B42" s="57"/>
-      <c r="C42" s="71" t="s">
+      <c r="B42" s="55"/>
+      <c r="C42" s="97" t="s">
         <v>64</v>
       </c>
-      <c r="D42" s="72"/>
+      <c r="D42" s="98"/>
       <c r="E42" s="37"/>
     </row>
     <row r="43" spans="1:19" ht="18" thickBot="1">
@@ -2719,20 +2755,20 @@
       </c>
     </row>
     <row r="44" spans="1:19">
-      <c r="A44" s="67" t="s">
+      <c r="A44" s="118" t="s">
         <v>35</v>
       </c>
-      <c r="B44" s="68"/>
-      <c r="C44" s="68"/>
-      <c r="D44" s="68"/>
-      <c r="E44" s="68"/>
-      <c r="F44" s="68"/>
-      <c r="G44" s="68"/>
-      <c r="H44" s="68"/>
-      <c r="I44" s="68"/>
-      <c r="J44" s="68"/>
-      <c r="K44" s="68"/>
-      <c r="L44" s="68"/>
+      <c r="B44" s="119"/>
+      <c r="C44" s="119"/>
+      <c r="D44" s="119"/>
+      <c r="E44" s="119"/>
+      <c r="F44" s="119"/>
+      <c r="G44" s="119"/>
+      <c r="H44" s="119"/>
+      <c r="I44" s="119"/>
+      <c r="J44" s="119"/>
+      <c r="K44" s="119"/>
+      <c r="L44" s="119"/>
       <c r="O44" t="s">
         <v>100</v>
       </c>
@@ -2741,37 +2777,37 @@
       <c r="A45" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="B45" s="61" t="s">
+      <c r="B45" s="112" t="s">
         <v>55</v>
       </c>
-      <c r="C45" s="61"/>
-      <c r="D45" s="61"/>
-      <c r="E45" s="61"/>
-      <c r="F45" s="61"/>
-      <c r="G45" s="61"/>
-      <c r="H45" s="61"/>
-      <c r="I45" s="61"/>
-      <c r="J45" s="61"/>
-      <c r="K45" s="61"/>
-      <c r="L45" s="61"/>
+      <c r="C45" s="112"/>
+      <c r="D45" s="112"/>
+      <c r="E45" s="112"/>
+      <c r="F45" s="112"/>
+      <c r="G45" s="112"/>
+      <c r="H45" s="112"/>
+      <c r="I45" s="112"/>
+      <c r="J45" s="112"/>
+      <c r="K45" s="112"/>
+      <c r="L45" s="112"/>
     </row>
     <row r="46" spans="1:19" ht="15" customHeight="1">
       <c r="A46" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="B46" s="61" t="s">
+      <c r="B46" s="112" t="s">
         <v>56</v>
       </c>
-      <c r="C46" s="61"/>
-      <c r="D46" s="61"/>
-      <c r="E46" s="61"/>
-      <c r="F46" s="61"/>
-      <c r="G46" s="61"/>
-      <c r="H46" s="61"/>
-      <c r="I46" s="61"/>
-      <c r="J46" s="61"/>
-      <c r="K46" s="61"/>
-      <c r="L46" s="61"/>
+      <c r="C46" s="112"/>
+      <c r="D46" s="112"/>
+      <c r="E46" s="112"/>
+      <c r="F46" s="112"/>
+      <c r="G46" s="112"/>
+      <c r="H46" s="112"/>
+      <c r="I46" s="112"/>
+      <c r="J46" s="112"/>
+      <c r="K46" s="112"/>
+      <c r="L46" s="112"/>
       <c r="N46" s="49" t="s">
         <v>97</v>
       </c>
@@ -2783,19 +2819,19 @@
       <c r="A47" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="B47" s="61" t="s">
+      <c r="B47" s="112" t="s">
         <v>57</v>
       </c>
-      <c r="C47" s="61"/>
-      <c r="D47" s="61"/>
-      <c r="E47" s="61"/>
-      <c r="F47" s="61"/>
-      <c r="G47" s="61"/>
-      <c r="H47" s="61"/>
-      <c r="I47" s="61"/>
-      <c r="J47" s="61"/>
-      <c r="K47" s="61"/>
-      <c r="L47" s="61"/>
+      <c r="C47" s="112"/>
+      <c r="D47" s="112"/>
+      <c r="E47" s="112"/>
+      <c r="F47" s="112"/>
+      <c r="G47" s="112"/>
+      <c r="H47" s="112"/>
+      <c r="I47" s="112"/>
+      <c r="J47" s="112"/>
+      <c r="K47" s="112"/>
+      <c r="L47" s="112"/>
       <c r="O47" s="43" t="s">
         <v>101</v>
       </c>
@@ -2804,19 +2840,19 @@
       <c r="A48" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="B48" s="61" t="s">
+      <c r="B48" s="112" t="s">
         <v>44</v>
       </c>
-      <c r="C48" s="61"/>
-      <c r="D48" s="61"/>
-      <c r="E48" s="61"/>
-      <c r="F48" s="61"/>
-      <c r="G48" s="61"/>
-      <c r="H48" s="61"/>
-      <c r="I48" s="61"/>
-      <c r="J48" s="61"/>
-      <c r="K48" s="61"/>
-      <c r="L48" s="61"/>
+      <c r="C48" s="112"/>
+      <c r="D48" s="112"/>
+      <c r="E48" s="112"/>
+      <c r="F48" s="112"/>
+      <c r="G48" s="112"/>
+      <c r="H48" s="112"/>
+      <c r="I48" s="112"/>
+      <c r="J48" s="112"/>
+      <c r="K48" s="112"/>
+      <c r="L48" s="112"/>
       <c r="O48" t="s">
         <v>104</v>
       </c>
@@ -2825,37 +2861,37 @@
       <c r="A49" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="B49" s="61" t="s">
+      <c r="B49" s="112" t="s">
         <v>33</v>
       </c>
-      <c r="C49" s="61"/>
-      <c r="D49" s="61"/>
-      <c r="E49" s="61"/>
-      <c r="F49" s="61"/>
-      <c r="G49" s="61"/>
-      <c r="H49" s="61"/>
-      <c r="I49" s="61"/>
-      <c r="J49" s="61"/>
-      <c r="K49" s="61"/>
-      <c r="L49" s="61"/>
+      <c r="C49" s="112"/>
+      <c r="D49" s="112"/>
+      <c r="E49" s="112"/>
+      <c r="F49" s="112"/>
+      <c r="G49" s="112"/>
+      <c r="H49" s="112"/>
+      <c r="I49" s="112"/>
+      <c r="J49" s="112"/>
+      <c r="K49" s="112"/>
+      <c r="L49" s="112"/>
     </row>
     <row r="50" spans="1:15" ht="17.25">
       <c r="A50" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="B50" s="61" t="s">
+      <c r="B50" s="112" t="s">
         <v>54</v>
       </c>
-      <c r="C50" s="61"/>
-      <c r="D50" s="61"/>
-      <c r="E50" s="61"/>
-      <c r="F50" s="61"/>
-      <c r="G50" s="61"/>
-      <c r="H50" s="61"/>
-      <c r="I50" s="61"/>
-      <c r="J50" s="61"/>
-      <c r="K50" s="61"/>
-      <c r="L50" s="61"/>
+      <c r="C50" s="112"/>
+      <c r="D50" s="112"/>
+      <c r="E50" s="112"/>
+      <c r="F50" s="112"/>
+      <c r="G50" s="112"/>
+      <c r="H50" s="112"/>
+      <c r="I50" s="112"/>
+      <c r="J50" s="112"/>
+      <c r="K50" s="112"/>
+      <c r="L50" s="112"/>
       <c r="N50" s="49" t="s">
         <v>96</v>
       </c>
@@ -2867,19 +2903,19 @@
       <c r="A51" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="B51" s="61" t="s">
+      <c r="B51" s="112" t="s">
         <v>53</v>
       </c>
-      <c r="C51" s="61"/>
-      <c r="D51" s="61"/>
-      <c r="E51" s="61"/>
-      <c r="F51" s="61"/>
-      <c r="G51" s="61"/>
-      <c r="H51" s="61"/>
-      <c r="I51" s="61"/>
-      <c r="J51" s="61"/>
-      <c r="K51" s="61"/>
-      <c r="L51" s="61"/>
+      <c r="C51" s="112"/>
+      <c r="D51" s="112"/>
+      <c r="E51" s="112"/>
+      <c r="F51" s="112"/>
+      <c r="G51" s="112"/>
+      <c r="H51" s="112"/>
+      <c r="I51" s="112"/>
+      <c r="J51" s="112"/>
+      <c r="K51" s="112"/>
+      <c r="L51" s="112"/>
       <c r="O51" t="s">
         <v>102</v>
       </c>
@@ -2901,31 +2937,24 @@
     <sortCondition ref="A3"/>
   </sortState>
   <mergeCells count="56">
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="H28:K28"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="O6:U6"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="H27:K27"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="O15:S16"/>
-    <mergeCell ref="N24:S24"/>
-    <mergeCell ref="N27:S27"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="H30:K30"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="H32:K32"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="H31:L31"/>
+    <mergeCell ref="N28:S28"/>
+    <mergeCell ref="N40:S40"/>
+    <mergeCell ref="N33:S33"/>
+    <mergeCell ref="N36:S36"/>
+    <mergeCell ref="N30:S30"/>
+    <mergeCell ref="N31:S31"/>
+    <mergeCell ref="N38:S38"/>
+    <mergeCell ref="B50:L50"/>
+    <mergeCell ref="B51:L51"/>
+    <mergeCell ref="A39:E39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="B45:L45"/>
+    <mergeCell ref="A44:L44"/>
+    <mergeCell ref="B46:L46"/>
+    <mergeCell ref="B47:L47"/>
+    <mergeCell ref="B48:L48"/>
+    <mergeCell ref="B49:L49"/>
     <mergeCell ref="A35:B35"/>
     <mergeCell ref="A36:B36"/>
     <mergeCell ref="A37:B37"/>
@@ -2938,25 +2967,32 @@
     <mergeCell ref="C35:G35"/>
     <mergeCell ref="C36:G36"/>
     <mergeCell ref="C37:G37"/>
-    <mergeCell ref="B50:L50"/>
-    <mergeCell ref="B51:L51"/>
-    <mergeCell ref="A39:E39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="B45:L45"/>
-    <mergeCell ref="A44:L44"/>
-    <mergeCell ref="B46:L46"/>
-    <mergeCell ref="B47:L47"/>
-    <mergeCell ref="B48:L48"/>
-    <mergeCell ref="B49:L49"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="H30:K30"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="H32:K32"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="H31:L31"/>
+    <mergeCell ref="O6:U6"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="H27:K27"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="O15:S16"/>
+    <mergeCell ref="N24:S24"/>
+    <mergeCell ref="N27:S27"/>
     <mergeCell ref="N20:S20"/>
-    <mergeCell ref="N40:S40"/>
-    <mergeCell ref="N33:S33"/>
-    <mergeCell ref="N36:S36"/>
-    <mergeCell ref="N30:S30"/>
-    <mergeCell ref="N31:S31"/>
-    <mergeCell ref="N38:S38"/>
-    <mergeCell ref="N28:S28"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="H28:K28"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="A28:B28"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="Q4" r:id="rId1"/>
@@ -2976,7 +3012,7 @@
   <dimension ref="A3:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3108,14 +3144,65 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A4:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="4" spans="1:2" ht="23.25">
+      <c r="A4" s="56" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="B5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="B6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="B7" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="23.25">
+      <c r="A9" s="56" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="B10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="57" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>128</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3124,7 +3211,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>

</xml_diff>

<commit_message>
incorporando nuevo codigo que reemplaza DATOPORTFOLIO, utilizando un BehaviorSubject llamado baseData. Se está refactorizando los metodos http para no tener que usar 3 metodos para cada entidad, sólo quedaran 3 ABM.
</commit_message>
<xml_diff>
--- a/Cuadro-de-estado.xlsx
+++ b/Cuadro-de-estado.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="124">
   <si>
     <t>BACKEND</t>
   </si>
@@ -307,12 +307,6 @@
     <t>https://blog.angular-university.io/angular-file-upload/</t>
   </si>
   <si>
-    <t>DatePicker</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bootstrap / material ? </t>
-  </si>
-  <si>
     <t>Layout</t>
   </si>
   <si>
@@ -337,9 +331,6 @@
     <t>Integridad, al borrar Organization, RolePosition, Degree. Ojo con la relacion en LaboralCareer y Studie</t>
   </si>
   <si>
-    <t>En cada componente, vuelve a buscar la informacion a la DB, ¿está bien?</t>
-  </si>
-  <si>
     <t>Test en Front</t>
   </si>
   <si>
@@ -349,9 +340,6 @@
     <t>Si no tiene URL no debiera mostrar -VISITAR-</t>
   </si>
   <si>
-    <t>Input photoPath</t>
-  </si>
-  <si>
     <t>interfaz RESPONSIVA</t>
   </si>
   <si>
@@ -380,9 +368,6 @@
   </si>
   <si>
     <t>firebase</t>
-  </si>
-  <si>
-    <t>Upload file</t>
   </si>
   <si>
     <t>LOGIN</t>
@@ -497,7 +482,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
   </numFmts>
-  <fonts count="29">
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -670,13 +655,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1277,9 +1255,9 @@
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="43" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="23" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="122">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1364,15 +1342,14 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="13" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
@@ -1384,14 +1361,137 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1401,6 +1501,51 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1410,182 +1555,14 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1889,7 +1866,7 @@
   <dimension ref="A1:U54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1906,62 +1883,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25">
-      <c r="A1" s="72" t="s">
-        <v>88</v>
-      </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
-      <c r="H1" s="72"/>
-      <c r="I1" s="72"/>
-      <c r="J1" s="72"/>
-      <c r="K1" s="72"/>
-      <c r="L1" s="72"/>
+      <c r="A1" s="106" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="106"/>
+      <c r="C1" s="106"/>
+      <c r="D1" s="106"/>
+      <c r="E1" s="106"/>
+      <c r="F1" s="106"/>
+      <c r="G1" s="106"/>
+      <c r="H1" s="106"/>
+      <c r="I1" s="106"/>
+      <c r="J1" s="106"/>
+      <c r="K1" s="106"/>
+      <c r="L1" s="106"/>
     </row>
     <row r="2" spans="1:21" ht="19.5" thickBot="1">
-      <c r="A2" s="45">
+      <c r="A2" s="44">
         <f ca="1">M2-TODAY()-1</f>
-        <v>24</v>
-      </c>
-      <c r="B2" s="46" t="s">
-        <v>89</v>
-      </c>
-      <c r="C2" s="47"/>
-      <c r="M2" s="44">
+        <v>20</v>
+      </c>
+      <c r="B2" s="45" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" s="46"/>
+      <c r="M2" s="43">
         <v>45011</v>
       </c>
-      <c r="O2" s="43" t="s">
-        <v>85</v>
+      <c r="O2" s="42" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="73" t="s">
+      <c r="A3" s="107" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="74"/>
-      <c r="C3" s="64" t="s">
+      <c r="B3" s="108"/>
+      <c r="C3" s="109" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="67"/>
-      <c r="H3" s="64" t="s">
+      <c r="D3" s="110"/>
+      <c r="E3" s="110"/>
+      <c r="F3" s="110"/>
+      <c r="G3" s="111"/>
+      <c r="H3" s="109" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="65"/>
-      <c r="J3" s="66"/>
-      <c r="K3" s="67"/>
+      <c r="I3" s="110"/>
+      <c r="J3" s="112"/>
+      <c r="K3" s="111"/>
       <c r="L3" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="75" t="s">
-        <v>79</v>
-      </c>
-      <c r="N3" s="71"/>
+      <c r="M3" s="113" t="s">
+        <v>76</v>
+      </c>
+      <c r="N3" s="105"/>
     </row>
     <row r="4" spans="1:21" s="3" customFormat="1" ht="40.5" customHeight="1" thickBot="1">
       <c r="A4" s="17" t="s">
@@ -2000,10 +1977,10 @@
       <c r="L4" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="M4" s="76" t="s">
-        <v>80</v>
-      </c>
-      <c r="N4" s="77"/>
+      <c r="M4" s="114" t="s">
+        <v>77</v>
+      </c>
+      <c r="N4" s="115"/>
       <c r="O4" s="34" t="s">
         <v>61</v>
       </c>
@@ -2032,28 +2009,25 @@
       <c r="B6" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="40"/>
+      <c r="C6" s="4"/>
       <c r="D6" s="40"/>
       <c r="E6" s="4"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="40"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
-      <c r="K6" s="5"/>
+      <c r="K6" s="4"/>
       <c r="L6" s="4"/>
-      <c r="M6" s="42" t="s">
-        <v>82</v>
-      </c>
-      <c r="O6" s="70" t="s">
+      <c r="O6" s="104" t="s">
         <v>65</v>
       </c>
-      <c r="P6" s="71"/>
-      <c r="Q6" s="71"/>
-      <c r="R6" s="71"/>
-      <c r="S6" s="71"/>
-      <c r="T6" s="71"/>
-      <c r="U6" s="71"/>
+      <c r="P6" s="105"/>
+      <c r="Q6" s="105"/>
+      <c r="R6" s="105"/>
+      <c r="S6" s="105"/>
+      <c r="T6" s="105"/>
+      <c r="U6" s="105"/>
     </row>
     <row r="7" spans="1:21" ht="4.5" customHeight="1">
       <c r="A7" s="28"/>
@@ -2077,7 +2051,7 @@
         <v>12</v>
       </c>
       <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
+      <c r="D8" s="40"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
@@ -2105,7 +2079,7 @@
         <v>12</v>
       </c>
       <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
+      <c r="D9" s="40"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
@@ -2115,7 +2089,7 @@
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
       <c r="P9" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="Q9" s="6"/>
     </row>
@@ -2126,11 +2100,11 @@
       <c r="B10" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
@@ -2144,22 +2118,16 @@
       <c r="B11" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="40"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
-      <c r="O11" t="s">
-        <v>68</v>
-      </c>
-      <c r="P11" t="s">
-        <v>69</v>
-      </c>
     </row>
     <row r="12" spans="1:21" ht="4.5" customHeight="1">
       <c r="A12" s="28"/>
@@ -2182,43 +2150,47 @@
       <c r="B13" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="4"/>
+      <c r="C13" s="40"/>
       <c r="D13" s="40"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="40"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
-      <c r="K13" s="55"/>
+      <c r="K13" s="54"/>
       <c r="L13" s="4"/>
       <c r="O13" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="P13" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" ht="15" customHeight="1">
       <c r="A14" s="38" t="s">
         <v>28</v>
       </c>
       <c r="B14" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="4"/>
+      <c r="C14" s="40"/>
       <c r="D14" s="40"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="40"/>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
-      <c r="K14" s="55"/>
+      <c r="K14" s="54"/>
       <c r="L14" s="4"/>
-      <c r="O14" t="s">
-        <v>93</v>
-      </c>
+      <c r="O14" s="121" t="s">
+        <v>75</v>
+      </c>
+      <c r="P14" s="121"/>
+      <c r="Q14" s="121"/>
+      <c r="R14" s="121"/>
+      <c r="S14" s="121"/>
     </row>
     <row r="15" spans="1:21" ht="15" customHeight="1">
       <c r="A15" s="38" t="s">
@@ -2227,24 +2199,22 @@
       <c r="B15" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="4"/>
+      <c r="C15" s="40"/>
       <c r="D15" s="40"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="40"/>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
-      <c r="K15" s="55"/>
+      <c r="K15" s="54"/>
       <c r="L15" s="4"/>
-      <c r="O15" s="78" t="s">
-        <v>77</v>
-      </c>
-      <c r="P15" s="78"/>
-      <c r="Q15" s="78"/>
-      <c r="R15" s="78"/>
-      <c r="S15" s="78"/>
-      <c r="T15" s="54"/>
+      <c r="O15" s="121"/>
+      <c r="P15" s="121"/>
+      <c r="Q15" s="121"/>
+      <c r="R15" s="121"/>
+      <c r="S15" s="121"/>
+      <c r="T15" s="53"/>
     </row>
     <row r="16" spans="1:21">
       <c r="A16" s="18" t="s">
@@ -2253,22 +2223,17 @@
       <c r="B16" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="4"/>
+      <c r="C16" s="40"/>
       <c r="D16" s="40"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="55"/>
-      <c r="G16" s="4"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="54"/>
+      <c r="G16" s="40"/>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
       <c r="L16" s="4"/>
-      <c r="O16" s="78"/>
-      <c r="P16" s="78"/>
-      <c r="Q16" s="78"/>
-      <c r="R16" s="78"/>
-      <c r="S16" s="78"/>
-      <c r="T16" s="54"/>
+      <c r="T16" s="53"/>
     </row>
     <row r="17" spans="1:19">
       <c r="A17" s="18" t="s">
@@ -2277,18 +2242,18 @@
       <c r="B17" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="4"/>
+      <c r="C17" s="40"/>
       <c r="D17" s="40"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="55"/>
-      <c r="G17" s="4"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="54"/>
+      <c r="G17" s="40"/>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
       <c r="L17" s="4"/>
       <c r="O17" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:19" ht="4.5" customHeight="1">
@@ -2314,14 +2279,14 @@
       </c>
       <c r="C19" s="22"/>
       <c r="D19" s="41"/>
-      <c r="E19" s="55"/>
+      <c r="E19" s="54"/>
       <c r="F19" s="8"/>
       <c r="G19" s="7"/>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
       <c r="K19" s="7"/>
-      <c r="L19" s="53"/>
+      <c r="L19" s="52"/>
     </row>
     <row r="20" spans="1:19">
       <c r="A20" s="39" t="s">
@@ -2332,22 +2297,22 @@
       </c>
       <c r="C20" s="22"/>
       <c r="D20" s="41"/>
-      <c r="E20" s="55"/>
+      <c r="E20" s="54"/>
       <c r="F20" s="8"/>
       <c r="G20" s="7"/>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
       <c r="K20" s="7"/>
-      <c r="L20" s="53"/>
-      <c r="N20" s="79" t="s">
-        <v>118</v>
-      </c>
-      <c r="O20" s="79"/>
-      <c r="P20" s="79"/>
-      <c r="Q20" s="79"/>
-      <c r="R20" s="79"/>
-      <c r="S20" s="79"/>
+      <c r="L20" s="52"/>
+      <c r="N20" s="58" t="s">
+        <v>113</v>
+      </c>
+      <c r="O20" s="58"/>
+      <c r="P20" s="58"/>
+      <c r="Q20" s="58"/>
+      <c r="R20" s="58"/>
+      <c r="S20" s="58"/>
     </row>
     <row r="21" spans="1:19" ht="4.5" customHeight="1">
       <c r="A21" s="28"/>
@@ -2370,7 +2335,7 @@
       <c r="B22" s="19"/>
       <c r="C22" s="16"/>
       <c r="D22" s="8"/>
-      <c r="E22" s="55"/>
+      <c r="E22" s="54"/>
       <c r="F22" s="8"/>
       <c r="G22" s="4"/>
       <c r="H22" s="5"/>
@@ -2400,7 +2365,7 @@
       <c r="B24" s="31"/>
       <c r="C24" s="8"/>
       <c r="D24" s="5"/>
-      <c r="E24" s="55"/>
+      <c r="E24" s="54"/>
       <c r="F24" s="8"/>
       <c r="G24" s="7"/>
       <c r="H24" s="5"/>
@@ -2408,14 +2373,14 @@
       <c r="J24" s="5"/>
       <c r="K24" s="7"/>
       <c r="L24" s="4"/>
-      <c r="N24" s="79" t="s">
-        <v>87</v>
-      </c>
-      <c r="O24" s="79"/>
-      <c r="P24" s="79"/>
-      <c r="Q24" s="79"/>
-      <c r="R24" s="79"/>
-      <c r="S24" s="79"/>
+      <c r="N24" s="58" t="s">
+        <v>83</v>
+      </c>
+      <c r="O24" s="58"/>
+      <c r="P24" s="58"/>
+      <c r="Q24" s="58"/>
+      <c r="R24" s="58"/>
+      <c r="S24" s="58"/>
     </row>
     <row r="25" spans="1:19">
       <c r="A25" s="39" t="s">
@@ -2426,7 +2391,7 @@
       </c>
       <c r="C25" s="22"/>
       <c r="D25" s="8"/>
-      <c r="E25" s="55"/>
+      <c r="E25" s="54"/>
       <c r="F25" s="8"/>
       <c r="G25" s="8"/>
       <c r="H25" s="5"/>
@@ -2452,60 +2417,60 @@
     <row r="27" spans="1:19" ht="15.75" thickBot="1">
       <c r="A27" s="23"/>
       <c r="B27" s="25"/>
-      <c r="C27" s="64" t="s">
+      <c r="C27" s="109" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="65"/>
-      <c r="E27" s="65"/>
-      <c r="F27" s="65"/>
-      <c r="G27" s="67"/>
-      <c r="H27" s="64" t="s">
+      <c r="D27" s="110"/>
+      <c r="E27" s="110"/>
+      <c r="F27" s="110"/>
+      <c r="G27" s="111"/>
+      <c r="H27" s="109" t="s">
         <v>0</v>
       </c>
-      <c r="I27" s="65"/>
-      <c r="J27" s="66"/>
-      <c r="K27" s="67"/>
+      <c r="I27" s="110"/>
+      <c r="J27" s="112"/>
+      <c r="K27" s="111"/>
       <c r="L27" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="N27" s="79" t="s">
-        <v>81</v>
-      </c>
-      <c r="O27" s="79"/>
-      <c r="P27" s="79"/>
-      <c r="Q27" s="79"/>
-      <c r="R27" s="79"/>
-      <c r="S27" s="79"/>
+      <c r="N27" s="58" t="s">
+        <v>78</v>
+      </c>
+      <c r="O27" s="58"/>
+      <c r="P27" s="58"/>
+      <c r="Q27" s="58"/>
+      <c r="R27" s="58"/>
+      <c r="S27" s="58"/>
     </row>
     <row r="28" spans="1:19" ht="30">
-      <c r="A28" s="68" t="s">
+      <c r="A28" s="119" t="s">
         <v>29</v>
       </c>
-      <c r="B28" s="69"/>
-      <c r="C28" s="58" t="s">
-        <v>92</v>
-      </c>
-      <c r="D28" s="59"/>
-      <c r="E28" s="59"/>
-      <c r="F28" s="59"/>
-      <c r="G28" s="60"/>
-      <c r="H28" s="61" t="s">
-        <v>90</v>
-      </c>
-      <c r="I28" s="62"/>
-      <c r="J28" s="62"/>
-      <c r="K28" s="63"/>
-      <c r="L28" s="48" t="s">
-        <v>91</v>
-      </c>
-      <c r="N28" s="120" t="s">
-        <v>116</v>
-      </c>
-      <c r="O28" s="120"/>
-      <c r="P28" s="120"/>
-      <c r="Q28" s="120"/>
-      <c r="R28" s="120"/>
-      <c r="S28" s="120"/>
+      <c r="B28" s="120"/>
+      <c r="C28" s="98" t="s">
+        <v>88</v>
+      </c>
+      <c r="D28" s="99"/>
+      <c r="E28" s="99"/>
+      <c r="F28" s="99"/>
+      <c r="G28" s="100"/>
+      <c r="H28" s="116" t="s">
+        <v>86</v>
+      </c>
+      <c r="I28" s="117"/>
+      <c r="J28" s="117"/>
+      <c r="K28" s="118"/>
+      <c r="L28" s="47" t="s">
+        <v>87</v>
+      </c>
+      <c r="N28" s="57" t="s">
+        <v>111</v>
+      </c>
+      <c r="O28" s="57"/>
+      <c r="P28" s="57"/>
+      <c r="Q28" s="57"/>
+      <c r="R28" s="57"/>
+      <c r="S28" s="57"/>
     </row>
     <row r="29" spans="1:19" ht="4.5" customHeight="1">
       <c r="A29" s="28"/>
@@ -2522,100 +2487,92 @@
       <c r="L29" s="30"/>
     </row>
     <row r="30" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A30" s="84" t="s">
+      <c r="A30" s="69" t="s">
         <v>38</v>
       </c>
-      <c r="B30" s="85"/>
-      <c r="C30" s="80"/>
-      <c r="D30" s="81"/>
-      <c r="E30" s="81"/>
-      <c r="F30" s="81"/>
-      <c r="G30" s="82"/>
-      <c r="H30" s="83"/>
-      <c r="I30" s="81"/>
-      <c r="J30" s="81"/>
-      <c r="K30" s="82"/>
+      <c r="B30" s="70"/>
+      <c r="C30" s="88"/>
+      <c r="D30" s="89"/>
+      <c r="E30" s="89"/>
+      <c r="F30" s="89"/>
+      <c r="G30" s="90"/>
+      <c r="H30" s="91"/>
+      <c r="I30" s="89"/>
+      <c r="J30" s="89"/>
+      <c r="K30" s="90"/>
       <c r="L30" s="21" t="s">
         <v>5</v>
       </c>
       <c r="M30" s="32"/>
-      <c r="N30" s="122" t="s">
-        <v>78</v>
-      </c>
-      <c r="O30" s="122"/>
-      <c r="P30" s="122"/>
-      <c r="Q30" s="122"/>
-      <c r="R30" s="122"/>
-      <c r="S30" s="122"/>
+      <c r="N30" s="60" t="s">
+        <v>72</v>
+      </c>
+      <c r="O30" s="60"/>
+      <c r="P30" s="60"/>
+      <c r="Q30" s="60"/>
+      <c r="R30" s="60"/>
+      <c r="S30" s="60"/>
     </row>
     <row r="31" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A31" s="84" t="s">
-        <v>83</v>
-      </c>
-      <c r="B31" s="85"/>
-      <c r="C31" s="58"/>
-      <c r="D31" s="59"/>
-      <c r="E31" s="59"/>
-      <c r="F31" s="59"/>
-      <c r="G31" s="60"/>
-      <c r="H31" s="94" t="s">
-        <v>84</v>
-      </c>
-      <c r="I31" s="95"/>
-      <c r="J31" s="95"/>
-      <c r="K31" s="95"/>
-      <c r="L31" s="96"/>
+      <c r="A31" s="69" t="s">
+        <v>79</v>
+      </c>
+      <c r="B31" s="70"/>
+      <c r="C31" s="98"/>
+      <c r="D31" s="99"/>
+      <c r="E31" s="99"/>
+      <c r="F31" s="99"/>
+      <c r="G31" s="100"/>
+      <c r="H31" s="101" t="s">
+        <v>80</v>
+      </c>
+      <c r="I31" s="102"/>
+      <c r="J31" s="102"/>
+      <c r="K31" s="102"/>
+      <c r="L31" s="103"/>
       <c r="M31" s="32"/>
-      <c r="N31" s="122" t="s">
-        <v>74</v>
-      </c>
-      <c r="O31" s="122"/>
-      <c r="P31" s="122"/>
-      <c r="Q31" s="122"/>
-      <c r="R31" s="122"/>
-      <c r="S31" s="122"/>
     </row>
     <row r="32" spans="1:19" ht="16.5" thickBot="1">
-      <c r="A32" s="88" t="s">
+      <c r="A32" s="94" t="s">
         <v>59</v>
       </c>
-      <c r="B32" s="89"/>
-      <c r="C32" s="90"/>
-      <c r="D32" s="91"/>
-      <c r="E32" s="91"/>
-      <c r="F32" s="91"/>
-      <c r="G32" s="92"/>
-      <c r="H32" s="93"/>
-      <c r="I32" s="91"/>
-      <c r="J32" s="91"/>
-      <c r="K32" s="92"/>
+      <c r="B32" s="95"/>
+      <c r="C32" s="85"/>
+      <c r="D32" s="86"/>
+      <c r="E32" s="86"/>
+      <c r="F32" s="86"/>
+      <c r="G32" s="96"/>
+      <c r="H32" s="97"/>
+      <c r="I32" s="86"/>
+      <c r="J32" s="86"/>
+      <c r="K32" s="96"/>
       <c r="M32" s="32"/>
+      <c r="N32" s="59" t="s">
+        <v>73</v>
+      </c>
+      <c r="O32" s="59"/>
+      <c r="P32" s="59"/>
+      <c r="Q32" s="59"/>
+      <c r="R32" s="59"/>
+      <c r="S32" s="59"/>
     </row>
     <row r="33" spans="1:19" ht="30.75" customHeight="1" thickBot="1">
-      <c r="A33" s="86" t="s">
+      <c r="A33" s="92" t="s">
         <v>34</v>
       </c>
-      <c r="B33" s="87"/>
-      <c r="C33" s="102" t="s">
+      <c r="B33" s="93"/>
+      <c r="C33" s="76" t="s">
         <v>58</v>
       </c>
-      <c r="D33" s="103"/>
-      <c r="E33" s="103"/>
-      <c r="F33" s="103"/>
-      <c r="G33" s="104"/>
-      <c r="H33" s="99"/>
-      <c r="I33" s="100"/>
-      <c r="J33" s="100"/>
-      <c r="K33" s="101"/>
+      <c r="D33" s="77"/>
+      <c r="E33" s="77"/>
+      <c r="F33" s="77"/>
+      <c r="G33" s="78"/>
+      <c r="H33" s="73"/>
+      <c r="I33" s="74"/>
+      <c r="J33" s="74"/>
+      <c r="K33" s="75"/>
       <c r="M33" s="32"/>
-      <c r="N33" s="121" t="s">
-        <v>75</v>
-      </c>
-      <c r="O33" s="121"/>
-      <c r="P33" s="121"/>
-      <c r="Q33" s="121"/>
-      <c r="R33" s="121"/>
-      <c r="S33" s="121"/>
     </row>
     <row r="34" spans="1:19" ht="4.5" customHeight="1" thickBot="1">
       <c r="A34" s="28"/>
@@ -2631,300 +2588,299 @@
       <c r="K34" s="30"/>
     </row>
     <row r="35" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A35" s="84" t="s">
+      <c r="A35" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="85"/>
-      <c r="C35" s="90"/>
-      <c r="D35" s="91"/>
-      <c r="E35" s="91"/>
-      <c r="F35" s="91"/>
-      <c r="G35" s="111"/>
-      <c r="H35" s="105"/>
-      <c r="I35" s="106"/>
-      <c r="J35" s="106"/>
-      <c r="K35" s="107"/>
+      <c r="B35" s="70"/>
+      <c r="C35" s="85"/>
+      <c r="D35" s="86"/>
+      <c r="E35" s="86"/>
+      <c r="F35" s="86"/>
+      <c r="G35" s="87"/>
+      <c r="H35" s="79"/>
+      <c r="I35" s="80"/>
+      <c r="J35" s="80"/>
+      <c r="K35" s="81"/>
       <c r="M35" s="32"/>
+      <c r="N35" s="60" t="s">
+        <v>74</v>
+      </c>
+      <c r="O35" s="60"/>
+      <c r="P35" s="60"/>
+      <c r="Q35" s="60"/>
+      <c r="R35" s="60"/>
+      <c r="S35" s="60"/>
     </row>
     <row r="36" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A36" s="84" t="s">
-        <v>94</v>
-      </c>
-      <c r="B36" s="85"/>
-      <c r="C36" s="90"/>
-      <c r="D36" s="91"/>
-      <c r="E36" s="91"/>
-      <c r="F36" s="91"/>
-      <c r="G36" s="111"/>
-      <c r="H36" s="105"/>
-      <c r="I36" s="106"/>
-      <c r="J36" s="106"/>
-      <c r="K36" s="107"/>
+      <c r="A36" s="69" t="s">
+        <v>89</v>
+      </c>
+      <c r="B36" s="70"/>
+      <c r="C36" s="85"/>
+      <c r="D36" s="86"/>
+      <c r="E36" s="86"/>
+      <c r="F36" s="86"/>
+      <c r="G36" s="87"/>
+      <c r="H36" s="79"/>
+      <c r="I36" s="80"/>
+      <c r="J36" s="80"/>
+      <c r="K36" s="81"/>
       <c r="M36" s="32"/>
-      <c r="N36" s="122" t="s">
-        <v>76</v>
-      </c>
-      <c r="O36" s="122"/>
-      <c r="P36" s="122"/>
-      <c r="Q36" s="122"/>
-      <c r="R36" s="122"/>
-      <c r="S36" s="122"/>
     </row>
     <row r="37" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A37" s="84" t="s">
+      <c r="A37" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="B37" s="85"/>
-      <c r="C37" s="108"/>
-      <c r="D37" s="109"/>
-      <c r="E37" s="109"/>
-      <c r="F37" s="109"/>
-      <c r="G37" s="110"/>
-      <c r="H37" s="108"/>
-      <c r="I37" s="109"/>
-      <c r="J37" s="109"/>
-      <c r="K37" s="110"/>
+      <c r="B37" s="70"/>
+      <c r="C37" s="82"/>
+      <c r="D37" s="83"/>
+      <c r="E37" s="83"/>
+      <c r="F37" s="83"/>
+      <c r="G37" s="84"/>
+      <c r="H37" s="82"/>
+      <c r="I37" s="83"/>
+      <c r="J37" s="83"/>
+      <c r="K37" s="84"/>
       <c r="M37" s="32"/>
-    </row>
-    <row r="38" spans="1:19" ht="15.75" thickBot="1">
-      <c r="N38" s="79" t="s">
-        <v>86</v>
-      </c>
-      <c r="O38" s="79"/>
-      <c r="P38" s="79"/>
-      <c r="Q38" s="79"/>
-      <c r="R38" s="79"/>
-      <c r="S38" s="79"/>
-    </row>
+      <c r="N37" s="58" t="s">
+        <v>82</v>
+      </c>
+      <c r="O37" s="58"/>
+      <c r="P37" s="58"/>
+      <c r="Q37" s="58"/>
+      <c r="R37" s="58"/>
+      <c r="S37" s="58"/>
+    </row>
+    <row r="38" spans="1:19" ht="15.75" thickBot="1"/>
     <row r="39" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A39" s="113" t="s">
+      <c r="A39" s="62" t="s">
         <v>25</v>
       </c>
-      <c r="B39" s="114"/>
-      <c r="C39" s="114"/>
-      <c r="D39" s="114"/>
-      <c r="E39" s="115"/>
+      <c r="B39" s="63"/>
+      <c r="C39" s="63"/>
+      <c r="D39" s="63"/>
+      <c r="E39" s="64"/>
+      <c r="N39" s="58" t="s">
+        <v>110</v>
+      </c>
+      <c r="O39" s="58"/>
+      <c r="P39" s="58"/>
+      <c r="Q39" s="58"/>
+      <c r="R39" s="58"/>
+      <c r="S39" s="58"/>
     </row>
     <row r="40" spans="1:19">
       <c r="A40" s="14" t="s">
         <v>24</v>
       </c>
       <c r="B40" s="13"/>
-      <c r="C40" s="116" t="s">
+      <c r="C40" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="D40" s="117"/>
+      <c r="D40" s="66"/>
       <c r="E40" s="27"/>
-      <c r="N40" s="79" t="s">
-        <v>115</v>
-      </c>
-      <c r="O40" s="79"/>
-      <c r="P40" s="79"/>
-      <c r="Q40" s="79"/>
-      <c r="R40" s="79"/>
-      <c r="S40" s="79"/>
     </row>
     <row r="41" spans="1:19">
       <c r="A41" s="15" t="s">
         <v>21</v>
       </c>
       <c r="B41" s="5"/>
-      <c r="C41" s="116" t="s">
+      <c r="C41" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="D41" s="117"/>
+      <c r="D41" s="66"/>
       <c r="E41" s="8"/>
     </row>
-    <row r="42" spans="1:19">
+    <row r="42" spans="1:19" ht="17.25">
       <c r="A42" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="B42" s="55"/>
-      <c r="C42" s="97" t="s">
+        <v>112</v>
+      </c>
+      <c r="B42" s="54"/>
+      <c r="C42" s="71" t="s">
         <v>64</v>
       </c>
-      <c r="D42" s="98"/>
+      <c r="D42" s="72"/>
       <c r="E42" s="37"/>
-    </row>
-    <row r="43" spans="1:19" ht="18" thickBot="1">
-      <c r="N43" s="49" t="s">
+      <c r="N42" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="O43" s="43" t="s">
-        <v>99</v>
+      <c r="O42" s="42" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" ht="15.75" thickBot="1">
+      <c r="O43" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="44" spans="1:19">
-      <c r="A44" s="118" t="s">
+      <c r="A44" s="67" t="s">
         <v>35</v>
       </c>
-      <c r="B44" s="119"/>
-      <c r="C44" s="119"/>
-      <c r="D44" s="119"/>
-      <c r="E44" s="119"/>
-      <c r="F44" s="119"/>
-      <c r="G44" s="119"/>
-      <c r="H44" s="119"/>
-      <c r="I44" s="119"/>
-      <c r="J44" s="119"/>
-      <c r="K44" s="119"/>
-      <c r="L44" s="119"/>
-      <c r="O44" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="45" spans="1:19">
+      <c r="B44" s="68"/>
+      <c r="C44" s="68"/>
+      <c r="D44" s="68"/>
+      <c r="E44" s="68"/>
+      <c r="F44" s="68"/>
+      <c r="G44" s="68"/>
+      <c r="H44" s="68"/>
+      <c r="I44" s="68"/>
+      <c r="J44" s="68"/>
+      <c r="K44" s="68"/>
+      <c r="L44" s="68"/>
+    </row>
+    <row r="45" spans="1:19" ht="17.25">
       <c r="A45" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="B45" s="112" t="s">
+      <c r="B45" s="61" t="s">
         <v>55</v>
       </c>
-      <c r="C45" s="112"/>
-      <c r="D45" s="112"/>
-      <c r="E45" s="112"/>
-      <c r="F45" s="112"/>
-      <c r="G45" s="112"/>
-      <c r="H45" s="112"/>
-      <c r="I45" s="112"/>
-      <c r="J45" s="112"/>
-      <c r="K45" s="112"/>
-      <c r="L45" s="112"/>
+      <c r="C45" s="61"/>
+      <c r="D45" s="61"/>
+      <c r="E45" s="61"/>
+      <c r="F45" s="61"/>
+      <c r="G45" s="61"/>
+      <c r="H45" s="61"/>
+      <c r="I45" s="61"/>
+      <c r="J45" s="61"/>
+      <c r="K45" s="61"/>
+      <c r="L45" s="61"/>
+      <c r="N45" s="48" t="s">
+        <v>92</v>
+      </c>
+      <c r="O45" s="42" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="46" spans="1:19" ht="15" customHeight="1">
       <c r="A46" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="B46" s="112" t="s">
+      <c r="B46" s="61" t="s">
         <v>56</v>
       </c>
-      <c r="C46" s="112"/>
-      <c r="D46" s="112"/>
-      <c r="E46" s="112"/>
-      <c r="F46" s="112"/>
-      <c r="G46" s="112"/>
-      <c r="H46" s="112"/>
-      <c r="I46" s="112"/>
-      <c r="J46" s="112"/>
-      <c r="K46" s="112"/>
-      <c r="L46" s="112"/>
-      <c r="N46" s="49" t="s">
-        <v>97</v>
-      </c>
-      <c r="O46" s="43" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="47" spans="1:19" ht="17.25">
+      <c r="C46" s="61"/>
+      <c r="D46" s="61"/>
+      <c r="E46" s="61"/>
+      <c r="F46" s="61"/>
+      <c r="G46" s="61"/>
+      <c r="H46" s="61"/>
+      <c r="I46" s="61"/>
+      <c r="J46" s="61"/>
+      <c r="K46" s="61"/>
+      <c r="L46" s="61"/>
+      <c r="O46" s="42" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19">
       <c r="A47" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="B47" s="112" t="s">
+      <c r="B47" s="61" t="s">
         <v>57</v>
       </c>
-      <c r="C47" s="112"/>
-      <c r="D47" s="112"/>
-      <c r="E47" s="112"/>
-      <c r="F47" s="112"/>
-      <c r="G47" s="112"/>
-      <c r="H47" s="112"/>
-      <c r="I47" s="112"/>
-      <c r="J47" s="112"/>
-      <c r="K47" s="112"/>
-      <c r="L47" s="112"/>
-      <c r="O47" s="43" t="s">
-        <v>101</v>
+      <c r="C47" s="61"/>
+      <c r="D47" s="61"/>
+      <c r="E47" s="61"/>
+      <c r="F47" s="61"/>
+      <c r="G47" s="61"/>
+      <c r="H47" s="61"/>
+      <c r="I47" s="61"/>
+      <c r="J47" s="61"/>
+      <c r="K47" s="61"/>
+      <c r="L47" s="61"/>
+      <c r="O47" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="48" spans="1:19">
       <c r="A48" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="B48" s="112" t="s">
+      <c r="B48" s="61" t="s">
         <v>44</v>
       </c>
-      <c r="C48" s="112"/>
-      <c r="D48" s="112"/>
-      <c r="E48" s="112"/>
-      <c r="F48" s="112"/>
-      <c r="G48" s="112"/>
-      <c r="H48" s="112"/>
-      <c r="I48" s="112"/>
-      <c r="J48" s="112"/>
-      <c r="K48" s="112"/>
-      <c r="L48" s="112"/>
-      <c r="O48" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="49" spans="1:15">
+      <c r="C48" s="61"/>
+      <c r="D48" s="61"/>
+      <c r="E48" s="61"/>
+      <c r="F48" s="61"/>
+      <c r="G48" s="61"/>
+      <c r="H48" s="61"/>
+      <c r="I48" s="61"/>
+      <c r="J48" s="61"/>
+      <c r="K48" s="61"/>
+      <c r="L48" s="61"/>
+    </row>
+    <row r="49" spans="1:15" ht="17.25">
       <c r="A49" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="B49" s="112" t="s">
+      <c r="B49" s="61" t="s">
         <v>33</v>
       </c>
-      <c r="C49" s="112"/>
-      <c r="D49" s="112"/>
-      <c r="E49" s="112"/>
-      <c r="F49" s="112"/>
-      <c r="G49" s="112"/>
-      <c r="H49" s="112"/>
-      <c r="I49" s="112"/>
-      <c r="J49" s="112"/>
-      <c r="K49" s="112"/>
-      <c r="L49" s="112"/>
-    </row>
-    <row r="50" spans="1:15" ht="17.25">
+      <c r="C49" s="61"/>
+      <c r="D49" s="61"/>
+      <c r="E49" s="61"/>
+      <c r="F49" s="61"/>
+      <c r="G49" s="61"/>
+      <c r="H49" s="61"/>
+      <c r="I49" s="61"/>
+      <c r="J49" s="61"/>
+      <c r="K49" s="61"/>
+      <c r="L49" s="61"/>
+      <c r="N49" s="48" t="s">
+        <v>91</v>
+      </c>
+      <c r="O49" s="42" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15">
       <c r="A50" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="B50" s="112" t="s">
+      <c r="B50" s="61" t="s">
         <v>54</v>
       </c>
-      <c r="C50" s="112"/>
-      <c r="D50" s="112"/>
-      <c r="E50" s="112"/>
-      <c r="F50" s="112"/>
-      <c r="G50" s="112"/>
-      <c r="H50" s="112"/>
-      <c r="I50" s="112"/>
-      <c r="J50" s="112"/>
-      <c r="K50" s="112"/>
-      <c r="L50" s="112"/>
-      <c r="N50" s="49" t="s">
-        <v>96</v>
-      </c>
-      <c r="O50" s="43" t="s">
-        <v>95</v>
+      <c r="C50" s="61"/>
+      <c r="D50" s="61"/>
+      <c r="E50" s="61"/>
+      <c r="F50" s="61"/>
+      <c r="G50" s="61"/>
+      <c r="H50" s="61"/>
+      <c r="I50" s="61"/>
+      <c r="J50" s="61"/>
+      <c r="K50" s="61"/>
+      <c r="L50" s="61"/>
+      <c r="O50" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="51" spans="1:15">
       <c r="A51" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="B51" s="112" t="s">
+      <c r="B51" s="61" t="s">
         <v>53</v>
       </c>
-      <c r="C51" s="112"/>
-      <c r="D51" s="112"/>
-      <c r="E51" s="112"/>
-      <c r="F51" s="112"/>
-      <c r="G51" s="112"/>
-      <c r="H51" s="112"/>
-      <c r="I51" s="112"/>
-      <c r="J51" s="112"/>
-      <c r="K51" s="112"/>
-      <c r="L51" s="112"/>
+      <c r="C51" s="61"/>
+      <c r="D51" s="61"/>
+      <c r="E51" s="61"/>
+      <c r="F51" s="61"/>
+      <c r="G51" s="61"/>
+      <c r="H51" s="61"/>
+      <c r="I51" s="61"/>
+      <c r="J51" s="61"/>
+      <c r="K51" s="61"/>
+      <c r="L51" s="61"/>
       <c r="O51" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="52" spans="1:15">
       <c r="C52" s="32"/>
-      <c r="O52" t="s">
-        <v>103</v>
-      </c>
     </row>
     <row r="53" spans="1:15">
       <c r="C53" s="32"/>
@@ -2936,25 +2892,33 @@
   <sortState ref="A24:K25">
     <sortCondition ref="A3"/>
   </sortState>
-  <mergeCells count="56">
-    <mergeCell ref="N28:S28"/>
-    <mergeCell ref="N40:S40"/>
-    <mergeCell ref="N33:S33"/>
-    <mergeCell ref="N36:S36"/>
-    <mergeCell ref="N30:S30"/>
-    <mergeCell ref="N31:S31"/>
-    <mergeCell ref="N38:S38"/>
-    <mergeCell ref="B50:L50"/>
-    <mergeCell ref="B51:L51"/>
-    <mergeCell ref="A39:E39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="B45:L45"/>
-    <mergeCell ref="A44:L44"/>
-    <mergeCell ref="B46:L46"/>
-    <mergeCell ref="B47:L47"/>
-    <mergeCell ref="B48:L48"/>
-    <mergeCell ref="B49:L49"/>
+  <mergeCells count="55">
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="H28:K28"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="O6:U6"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="H27:K27"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="N24:S24"/>
+    <mergeCell ref="N27:S27"/>
+    <mergeCell ref="N20:S20"/>
+    <mergeCell ref="O14:S15"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="H30:K30"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="H32:K32"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="H31:L31"/>
     <mergeCell ref="A35:B35"/>
     <mergeCell ref="A36:B36"/>
     <mergeCell ref="A37:B37"/>
@@ -2967,40 +2931,31 @@
     <mergeCell ref="C35:G35"/>
     <mergeCell ref="C36:G36"/>
     <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="H30:K30"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="H32:K32"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="H31:L31"/>
-    <mergeCell ref="O6:U6"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="H27:K27"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="O15:S16"/>
-    <mergeCell ref="N24:S24"/>
-    <mergeCell ref="N27:S27"/>
-    <mergeCell ref="N20:S20"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="H28:K28"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="B50:L50"/>
+    <mergeCell ref="B51:L51"/>
+    <mergeCell ref="A39:E39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="B45:L45"/>
+    <mergeCell ref="A44:L44"/>
+    <mergeCell ref="B46:L46"/>
+    <mergeCell ref="B47:L47"/>
+    <mergeCell ref="B48:L48"/>
+    <mergeCell ref="B49:L49"/>
+    <mergeCell ref="N28:S28"/>
+    <mergeCell ref="N39:S39"/>
+    <mergeCell ref="N32:S32"/>
+    <mergeCell ref="N35:S35"/>
+    <mergeCell ref="N30:S30"/>
+    <mergeCell ref="N37:S37"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="Q4" r:id="rId1"/>
     <hyperlink ref="O2" r:id="rId2"/>
-    <hyperlink ref="O50" r:id="rId3"/>
-    <hyperlink ref="O46" r:id="rId4"/>
-    <hyperlink ref="O43" r:id="rId5"/>
-    <hyperlink ref="O47" r:id="rId6"/>
+    <hyperlink ref="O49" r:id="rId3"/>
+    <hyperlink ref="O45" r:id="rId4"/>
+    <hyperlink ref="O42" r:id="rId5"/>
+    <hyperlink ref="O46" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.51" right="0.35" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="89" orientation="portrait" r:id="rId7"/>
@@ -3024,116 +2979,116 @@
   <sheetData>
     <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B3" s="1"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="51" t="s">
-        <v>112</v>
-      </c>
-      <c r="B4" s="51"/>
-      <c r="C4" s="51" t="s">
+      <c r="A4" s="50" t="s">
+        <v>107</v>
+      </c>
+      <c r="B4" s="50"/>
+      <c r="C4" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="51" t="s">
-        <v>111</v>
-      </c>
-      <c r="E4" s="51" t="s">
-        <v>110</v>
+      <c r="D4" s="50" t="s">
+        <v>106</v>
+      </c>
+      <c r="E4" s="50" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="50" t="s">
+      <c r="A5" s="49" t="s">
+        <v>104</v>
+      </c>
+      <c r="B5" s="49" t="s">
+        <v>101</v>
+      </c>
+      <c r="C5" s="50"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="49"/>
+      <c r="B6" s="49" t="s">
+        <v>100</v>
+      </c>
+      <c r="C6" s="50" t="s">
         <v>109</v>
       </c>
-      <c r="B5" s="50" t="s">
-        <v>106</v>
-      </c>
-      <c r="C5" s="51"/>
-      <c r="D5" s="51"/>
-      <c r="E5" s="51"/>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="50"/>
-      <c r="B6" s="50" t="s">
-        <v>105</v>
-      </c>
-      <c r="C6" s="51" t="s">
-        <v>114</v>
-      </c>
-      <c r="D6" s="51" t="s">
-        <v>114</v>
-      </c>
-      <c r="E6" s="51" t="s">
-        <v>114</v>
+      <c r="D6" s="50" t="s">
+        <v>109</v>
+      </c>
+      <c r="E6" s="50" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="50"/>
-      <c r="B7" s="50"/>
-      <c r="C7" s="51"/>
-      <c r="D7" s="51"/>
-      <c r="E7" s="51"/>
+      <c r="A7" s="49"/>
+      <c r="B7" s="49"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="50"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="50" t="s">
-        <v>108</v>
-      </c>
-      <c r="B8" s="50" t="s">
-        <v>106</v>
-      </c>
-      <c r="C8" s="51"/>
-      <c r="D8" s="51"/>
-      <c r="E8" s="51"/>
+      <c r="A8" s="49" t="s">
+        <v>103</v>
+      </c>
+      <c r="B8" s="49" t="s">
+        <v>101</v>
+      </c>
+      <c r="C8" s="50"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="50"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="50"/>
-      <c r="B9" s="50" t="s">
-        <v>105</v>
-      </c>
-      <c r="C9" s="51" t="s">
-        <v>114</v>
-      </c>
-      <c r="D9" s="51" t="s">
-        <v>114</v>
-      </c>
-      <c r="E9" s="51" t="s">
-        <v>114</v>
+      <c r="A9" s="49"/>
+      <c r="B9" s="49" t="s">
+        <v>100</v>
+      </c>
+      <c r="C9" s="50" t="s">
+        <v>109</v>
+      </c>
+      <c r="D9" s="50" t="s">
+        <v>109</v>
+      </c>
+      <c r="E9" s="50" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="50"/>
-      <c r="B10" s="50"/>
-      <c r="C10" s="51"/>
-      <c r="D10" s="51"/>
-      <c r="E10" s="51"/>
+      <c r="A10" s="49"/>
+      <c r="B10" s="49"/>
+      <c r="C10" s="50"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="50"/>
     </row>
     <row r="11" spans="1:6" ht="15.75">
-      <c r="A11" s="50" t="s">
-        <v>107</v>
-      </c>
-      <c r="B11" s="50" t="s">
-        <v>106</v>
-      </c>
-      <c r="C11" s="51"/>
-      <c r="D11" s="51"/>
-      <c r="E11" s="51"/>
-      <c r="F11" s="52"/>
+      <c r="A11" s="49" t="s">
+        <v>102</v>
+      </c>
+      <c r="B11" s="49" t="s">
+        <v>101</v>
+      </c>
+      <c r="C11" s="50"/>
+      <c r="D11" s="50"/>
+      <c r="E11" s="50"/>
+      <c r="F11" s="51"/>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="50"/>
-      <c r="B12" s="50" t="s">
-        <v>105</v>
-      </c>
-      <c r="C12" s="51" t="s">
-        <v>114</v>
-      </c>
-      <c r="D12" s="51" t="s">
-        <v>114</v>
-      </c>
-      <c r="E12" s="51" t="s">
-        <v>114</v>
+      <c r="A12" s="49"/>
+      <c r="B12" s="49" t="s">
+        <v>100</v>
+      </c>
+      <c r="C12" s="50" t="s">
+        <v>109</v>
+      </c>
+      <c r="D12" s="50" t="s">
+        <v>109</v>
+      </c>
+      <c r="E12" s="50" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -3153,53 +3108,53 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="4" spans="1:2" ht="23.25">
-      <c r="A4" s="56" t="s">
-        <v>119</v>
+      <c r="A4" s="55" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="B5" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="B6" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="B7" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="23.25">
-      <c r="A9" s="56" t="s">
-        <v>124</v>
+      <c r="A9" s="55" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="B10" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="57" t="s">
-        <v>126</v>
+      <c r="A16" s="56" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implementado hasta formacion, aunque falta su testing
</commit_message>
<xml_diff>
--- a/Cuadro-de-estado.xlsx
+++ b/Cuadro-de-estado.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="125">
   <si>
     <t>BACKEND</t>
   </si>
@@ -473,6 +473,9 @@
   </si>
   <si>
     <t>Hagamos algo especial.</t>
+  </si>
+  <si>
+    <t>En SOFTSKILL form, inicializa mal el range</t>
   </si>
 </sst>
 </file>
@@ -1369,200 +1372,200 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1866,7 +1869,7 @@
   <dimension ref="A1:U54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+      <selection activeCell="A13" activeCellId="1" sqref="A17:XFD17 A13:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1883,20 +1886,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25">
-      <c r="A1" s="106" t="s">
+      <c r="A1" s="71" t="s">
         <v>84</v>
       </c>
-      <c r="B1" s="106"/>
-      <c r="C1" s="106"/>
-      <c r="D1" s="106"/>
-      <c r="E1" s="106"/>
-      <c r="F1" s="106"/>
-      <c r="G1" s="106"/>
-      <c r="H1" s="106"/>
-      <c r="I1" s="106"/>
-      <c r="J1" s="106"/>
-      <c r="K1" s="106"/>
-      <c r="L1" s="106"/>
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="71"/>
+      <c r="I1" s="71"/>
+      <c r="J1" s="71"/>
+      <c r="K1" s="71"/>
+      <c r="L1" s="71"/>
     </row>
     <row r="2" spans="1:21" ht="19.5" thickBot="1">
       <c r="A2" s="44">
@@ -1915,30 +1918,30 @@
       </c>
     </row>
     <row r="3" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="107" t="s">
+      <c r="A3" s="72" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="108"/>
-      <c r="C3" s="109" t="s">
+      <c r="B3" s="73"/>
+      <c r="C3" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="110"/>
-      <c r="E3" s="110"/>
-      <c r="F3" s="110"/>
-      <c r="G3" s="111"/>
-      <c r="H3" s="109" t="s">
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="110"/>
-      <c r="J3" s="112"/>
-      <c r="K3" s="111"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="65"/>
+      <c r="K3" s="66"/>
       <c r="L3" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="113" t="s">
+      <c r="M3" s="74" t="s">
         <v>76</v>
       </c>
-      <c r="N3" s="105"/>
+      <c r="N3" s="70"/>
     </row>
     <row r="4" spans="1:21" s="3" customFormat="1" ht="40.5" customHeight="1" thickBot="1">
       <c r="A4" s="17" t="s">
@@ -1977,10 +1980,10 @@
       <c r="L4" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="M4" s="114" t="s">
+      <c r="M4" s="75" t="s">
         <v>77</v>
       </c>
-      <c r="N4" s="115"/>
+      <c r="N4" s="76"/>
       <c r="O4" s="34" t="s">
         <v>61</v>
       </c>
@@ -2019,15 +2022,15 @@
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
-      <c r="O6" s="104" t="s">
+      <c r="O6" s="69" t="s">
         <v>65</v>
       </c>
-      <c r="P6" s="105"/>
-      <c r="Q6" s="105"/>
-      <c r="R6" s="105"/>
-      <c r="S6" s="105"/>
-      <c r="T6" s="105"/>
-      <c r="U6" s="105"/>
+      <c r="P6" s="70"/>
+      <c r="Q6" s="70"/>
+      <c r="R6" s="70"/>
+      <c r="S6" s="70"/>
+      <c r="T6" s="70"/>
+      <c r="U6" s="70"/>
     </row>
     <row r="7" spans="1:21" ht="4.5" customHeight="1">
       <c r="A7" s="28"/>
@@ -2078,7 +2081,7 @@
       <c r="B9" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="4"/>
+      <c r="C9" s="5"/>
       <c r="D9" s="40"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
@@ -2100,11 +2103,11 @@
       <c r="B10" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="40"/>
+      <c r="C10" s="5"/>
       <c r="D10" s="40"/>
-      <c r="E10" s="40"/>
-      <c r="F10" s="40"/>
-      <c r="G10" s="40"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
@@ -2118,11 +2121,11 @@
       <c r="B11" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="40"/>
+      <c r="C11" s="5"/>
       <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
@@ -2184,13 +2187,13 @@
       <c r="J14" s="4"/>
       <c r="K14" s="54"/>
       <c r="L14" s="4"/>
-      <c r="O14" s="121" t="s">
+      <c r="O14" s="78" t="s">
         <v>75</v>
       </c>
-      <c r="P14" s="121"/>
-      <c r="Q14" s="121"/>
-      <c r="R14" s="121"/>
-      <c r="S14" s="121"/>
+      <c r="P14" s="78"/>
+      <c r="Q14" s="78"/>
+      <c r="R14" s="78"/>
+      <c r="S14" s="78"/>
     </row>
     <row r="15" spans="1:21" ht="15" customHeight="1">
       <c r="A15" s="38" t="s">
@@ -2209,11 +2212,11 @@
       <c r="J15" s="4"/>
       <c r="K15" s="54"/>
       <c r="L15" s="4"/>
-      <c r="O15" s="121"/>
-      <c r="P15" s="121"/>
-      <c r="Q15" s="121"/>
-      <c r="R15" s="121"/>
-      <c r="S15" s="121"/>
+      <c r="O15" s="78"/>
+      <c r="P15" s="78"/>
+      <c r="Q15" s="78"/>
+      <c r="R15" s="78"/>
+      <c r="S15" s="78"/>
       <c r="T15" s="53"/>
     </row>
     <row r="16" spans="1:21">
@@ -2305,14 +2308,14 @@
       <c r="J20" s="5"/>
       <c r="K20" s="7"/>
       <c r="L20" s="52"/>
-      <c r="N20" s="58" t="s">
+      <c r="N20" s="77" t="s">
         <v>113</v>
       </c>
-      <c r="O20" s="58"/>
-      <c r="P20" s="58"/>
-      <c r="Q20" s="58"/>
-      <c r="R20" s="58"/>
-      <c r="S20" s="58"/>
+      <c r="O20" s="77"/>
+      <c r="P20" s="77"/>
+      <c r="Q20" s="77"/>
+      <c r="R20" s="77"/>
+      <c r="S20" s="77"/>
     </row>
     <row r="21" spans="1:19" ht="4.5" customHeight="1">
       <c r="A21" s="28"/>
@@ -2343,6 +2346,14 @@
       <c r="J22" s="5"/>
       <c r="K22" s="7"/>
       <c r="L22" s="4"/>
+      <c r="N22" s="77" t="s">
+        <v>124</v>
+      </c>
+      <c r="O22" s="77"/>
+      <c r="P22" s="77"/>
+      <c r="Q22" s="77"/>
+      <c r="R22" s="77"/>
+      <c r="S22" s="77"/>
     </row>
     <row r="23" spans="1:19" ht="4.5" customHeight="1">
       <c r="A23" s="28"/>
@@ -2373,14 +2384,14 @@
       <c r="J24" s="5"/>
       <c r="K24" s="7"/>
       <c r="L24" s="4"/>
-      <c r="N24" s="58" t="s">
+      <c r="N24" s="77" t="s">
         <v>83</v>
       </c>
-      <c r="O24" s="58"/>
-      <c r="P24" s="58"/>
-      <c r="Q24" s="58"/>
-      <c r="R24" s="58"/>
-      <c r="S24" s="58"/>
+      <c r="O24" s="77"/>
+      <c r="P24" s="77"/>
+      <c r="Q24" s="77"/>
+      <c r="R24" s="77"/>
+      <c r="S24" s="77"/>
     </row>
     <row r="25" spans="1:19">
       <c r="A25" s="39" t="s">
@@ -2417,60 +2428,60 @@
     <row r="27" spans="1:19" ht="15.75" thickBot="1">
       <c r="A27" s="23"/>
       <c r="B27" s="25"/>
-      <c r="C27" s="109" t="s">
+      <c r="C27" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="110"/>
-      <c r="E27" s="110"/>
-      <c r="F27" s="110"/>
-      <c r="G27" s="111"/>
-      <c r="H27" s="109" t="s">
+      <c r="D27" s="64"/>
+      <c r="E27" s="64"/>
+      <c r="F27" s="64"/>
+      <c r="G27" s="66"/>
+      <c r="H27" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="I27" s="110"/>
-      <c r="J27" s="112"/>
-      <c r="K27" s="111"/>
+      <c r="I27" s="64"/>
+      <c r="J27" s="65"/>
+      <c r="K27" s="66"/>
       <c r="L27" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="N27" s="58" t="s">
+      <c r="N27" s="77" t="s">
         <v>78</v>
       </c>
-      <c r="O27" s="58"/>
-      <c r="P27" s="58"/>
-      <c r="Q27" s="58"/>
-      <c r="R27" s="58"/>
-      <c r="S27" s="58"/>
+      <c r="O27" s="77"/>
+      <c r="P27" s="77"/>
+      <c r="Q27" s="77"/>
+      <c r="R27" s="77"/>
+      <c r="S27" s="77"/>
     </row>
     <row r="28" spans="1:19" ht="30">
-      <c r="A28" s="119" t="s">
+      <c r="A28" s="67" t="s">
         <v>29</v>
       </c>
-      <c r="B28" s="120"/>
-      <c r="C28" s="98" t="s">
+      <c r="B28" s="68"/>
+      <c r="C28" s="57" t="s">
         <v>88</v>
       </c>
-      <c r="D28" s="99"/>
-      <c r="E28" s="99"/>
-      <c r="F28" s="99"/>
-      <c r="G28" s="100"/>
-      <c r="H28" s="116" t="s">
+      <c r="D28" s="58"/>
+      <c r="E28" s="58"/>
+      <c r="F28" s="58"/>
+      <c r="G28" s="59"/>
+      <c r="H28" s="60" t="s">
         <v>86</v>
       </c>
-      <c r="I28" s="117"/>
-      <c r="J28" s="117"/>
-      <c r="K28" s="118"/>
+      <c r="I28" s="61"/>
+      <c r="J28" s="61"/>
+      <c r="K28" s="62"/>
       <c r="L28" s="47" t="s">
         <v>87</v>
       </c>
-      <c r="N28" s="57" t="s">
+      <c r="N28" s="119" t="s">
         <v>111</v>
       </c>
-      <c r="O28" s="57"/>
-      <c r="P28" s="57"/>
-      <c r="Q28" s="57"/>
-      <c r="R28" s="57"/>
-      <c r="S28" s="57"/>
+      <c r="O28" s="119"/>
+      <c r="P28" s="119"/>
+      <c r="Q28" s="119"/>
+      <c r="R28" s="119"/>
+      <c r="S28" s="119"/>
     </row>
     <row r="29" spans="1:19" ht="4.5" customHeight="1">
       <c r="A29" s="28"/>
@@ -2487,91 +2498,91 @@
       <c r="L29" s="30"/>
     </row>
     <row r="30" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A30" s="69" t="s">
+      <c r="A30" s="83" t="s">
         <v>38</v>
       </c>
-      <c r="B30" s="70"/>
-      <c r="C30" s="88"/>
-      <c r="D30" s="89"/>
-      <c r="E30" s="89"/>
-      <c r="F30" s="89"/>
-      <c r="G30" s="90"/>
-      <c r="H30" s="91"/>
-      <c r="I30" s="89"/>
-      <c r="J30" s="89"/>
-      <c r="K30" s="90"/>
+      <c r="B30" s="84"/>
+      <c r="C30" s="79"/>
+      <c r="D30" s="80"/>
+      <c r="E30" s="80"/>
+      <c r="F30" s="80"/>
+      <c r="G30" s="81"/>
+      <c r="H30" s="82"/>
+      <c r="I30" s="80"/>
+      <c r="J30" s="80"/>
+      <c r="K30" s="81"/>
       <c r="L30" s="21" t="s">
         <v>5</v>
       </c>
       <c r="M30" s="32"/>
-      <c r="N30" s="60" t="s">
+      <c r="N30" s="121" t="s">
         <v>72</v>
       </c>
-      <c r="O30" s="60"/>
-      <c r="P30" s="60"/>
-      <c r="Q30" s="60"/>
-      <c r="R30" s="60"/>
-      <c r="S30" s="60"/>
+      <c r="O30" s="121"/>
+      <c r="P30" s="121"/>
+      <c r="Q30" s="121"/>
+      <c r="R30" s="121"/>
+      <c r="S30" s="121"/>
     </row>
     <row r="31" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A31" s="69" t="s">
+      <c r="A31" s="83" t="s">
         <v>79</v>
       </c>
-      <c r="B31" s="70"/>
-      <c r="C31" s="98"/>
-      <c r="D31" s="99"/>
-      <c r="E31" s="99"/>
-      <c r="F31" s="99"/>
-      <c r="G31" s="100"/>
-      <c r="H31" s="101" t="s">
+      <c r="B31" s="84"/>
+      <c r="C31" s="57"/>
+      <c r="D31" s="58"/>
+      <c r="E31" s="58"/>
+      <c r="F31" s="58"/>
+      <c r="G31" s="59"/>
+      <c r="H31" s="93" t="s">
         <v>80</v>
       </c>
-      <c r="I31" s="102"/>
-      <c r="J31" s="102"/>
-      <c r="K31" s="102"/>
-      <c r="L31" s="103"/>
+      <c r="I31" s="94"/>
+      <c r="J31" s="94"/>
+      <c r="K31" s="94"/>
+      <c r="L31" s="95"/>
       <c r="M31" s="32"/>
     </row>
     <row r="32" spans="1:19" ht="16.5" thickBot="1">
-      <c r="A32" s="94" t="s">
+      <c r="A32" s="87" t="s">
         <v>59</v>
       </c>
-      <c r="B32" s="95"/>
-      <c r="C32" s="85"/>
-      <c r="D32" s="86"/>
-      <c r="E32" s="86"/>
-      <c r="F32" s="86"/>
-      <c r="G32" s="96"/>
-      <c r="H32" s="97"/>
-      <c r="I32" s="86"/>
-      <c r="J32" s="86"/>
-      <c r="K32" s="96"/>
+      <c r="B32" s="88"/>
+      <c r="C32" s="89"/>
+      <c r="D32" s="90"/>
+      <c r="E32" s="90"/>
+      <c r="F32" s="90"/>
+      <c r="G32" s="91"/>
+      <c r="H32" s="92"/>
+      <c r="I32" s="90"/>
+      <c r="J32" s="90"/>
+      <c r="K32" s="91"/>
       <c r="M32" s="32"/>
-      <c r="N32" s="59" t="s">
+      <c r="N32" s="120" t="s">
         <v>73</v>
       </c>
-      <c r="O32" s="59"/>
-      <c r="P32" s="59"/>
-      <c r="Q32" s="59"/>
-      <c r="R32" s="59"/>
-      <c r="S32" s="59"/>
+      <c r="O32" s="120"/>
+      <c r="P32" s="120"/>
+      <c r="Q32" s="120"/>
+      <c r="R32" s="120"/>
+      <c r="S32" s="120"/>
     </row>
     <row r="33" spans="1:19" ht="30.75" customHeight="1" thickBot="1">
-      <c r="A33" s="92" t="s">
+      <c r="A33" s="85" t="s">
         <v>34</v>
       </c>
-      <c r="B33" s="93"/>
-      <c r="C33" s="76" t="s">
+      <c r="B33" s="86"/>
+      <c r="C33" s="101" t="s">
         <v>58</v>
       </c>
-      <c r="D33" s="77"/>
-      <c r="E33" s="77"/>
-      <c r="F33" s="77"/>
-      <c r="G33" s="78"/>
-      <c r="H33" s="73"/>
-      <c r="I33" s="74"/>
-      <c r="J33" s="74"/>
-      <c r="K33" s="75"/>
+      <c r="D33" s="102"/>
+      <c r="E33" s="102"/>
+      <c r="F33" s="102"/>
+      <c r="G33" s="103"/>
+      <c r="H33" s="98"/>
+      <c r="I33" s="99"/>
+      <c r="J33" s="99"/>
+      <c r="K33" s="100"/>
       <c r="M33" s="32"/>
     </row>
     <row r="34" spans="1:19" ht="4.5" customHeight="1" thickBot="1">
@@ -2588,96 +2599,96 @@
       <c r="K34" s="30"/>
     </row>
     <row r="35" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A35" s="69" t="s">
+      <c r="A35" s="83" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="70"/>
-      <c r="C35" s="85"/>
-      <c r="D35" s="86"/>
-      <c r="E35" s="86"/>
-      <c r="F35" s="86"/>
-      <c r="G35" s="87"/>
-      <c r="H35" s="79"/>
-      <c r="I35" s="80"/>
-      <c r="J35" s="80"/>
-      <c r="K35" s="81"/>
+      <c r="B35" s="84"/>
+      <c r="C35" s="89"/>
+      <c r="D35" s="90"/>
+      <c r="E35" s="90"/>
+      <c r="F35" s="90"/>
+      <c r="G35" s="110"/>
+      <c r="H35" s="104"/>
+      <c r="I35" s="105"/>
+      <c r="J35" s="105"/>
+      <c r="K35" s="106"/>
       <c r="M35" s="32"/>
-      <c r="N35" s="60" t="s">
+      <c r="N35" s="121" t="s">
         <v>74</v>
       </c>
-      <c r="O35" s="60"/>
-      <c r="P35" s="60"/>
-      <c r="Q35" s="60"/>
-      <c r="R35" s="60"/>
-      <c r="S35" s="60"/>
+      <c r="O35" s="121"/>
+      <c r="P35" s="121"/>
+      <c r="Q35" s="121"/>
+      <c r="R35" s="121"/>
+      <c r="S35" s="121"/>
     </row>
     <row r="36" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A36" s="69" t="s">
+      <c r="A36" s="83" t="s">
         <v>89</v>
       </c>
-      <c r="B36" s="70"/>
-      <c r="C36" s="85"/>
-      <c r="D36" s="86"/>
-      <c r="E36" s="86"/>
-      <c r="F36" s="86"/>
-      <c r="G36" s="87"/>
-      <c r="H36" s="79"/>
-      <c r="I36" s="80"/>
-      <c r="J36" s="80"/>
-      <c r="K36" s="81"/>
+      <c r="B36" s="84"/>
+      <c r="C36" s="89"/>
+      <c r="D36" s="90"/>
+      <c r="E36" s="90"/>
+      <c r="F36" s="90"/>
+      <c r="G36" s="110"/>
+      <c r="H36" s="104"/>
+      <c r="I36" s="105"/>
+      <c r="J36" s="105"/>
+      <c r="K36" s="106"/>
       <c r="M36" s="32"/>
     </row>
     <row r="37" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A37" s="69" t="s">
+      <c r="A37" s="83" t="s">
         <v>7</v>
       </c>
-      <c r="B37" s="70"/>
-      <c r="C37" s="82"/>
-      <c r="D37" s="83"/>
-      <c r="E37" s="83"/>
-      <c r="F37" s="83"/>
-      <c r="G37" s="84"/>
-      <c r="H37" s="82"/>
-      <c r="I37" s="83"/>
-      <c r="J37" s="83"/>
-      <c r="K37" s="84"/>
+      <c r="B37" s="84"/>
+      <c r="C37" s="107"/>
+      <c r="D37" s="108"/>
+      <c r="E37" s="108"/>
+      <c r="F37" s="108"/>
+      <c r="G37" s="109"/>
+      <c r="H37" s="107"/>
+      <c r="I37" s="108"/>
+      <c r="J37" s="108"/>
+      <c r="K37" s="109"/>
       <c r="M37" s="32"/>
-      <c r="N37" s="58" t="s">
+      <c r="N37" s="77" t="s">
         <v>82</v>
       </c>
-      <c r="O37" s="58"/>
-      <c r="P37" s="58"/>
-      <c r="Q37" s="58"/>
-      <c r="R37" s="58"/>
-      <c r="S37" s="58"/>
+      <c r="O37" s="77"/>
+      <c r="P37" s="77"/>
+      <c r="Q37" s="77"/>
+      <c r="R37" s="77"/>
+      <c r="S37" s="77"/>
     </row>
     <row r="38" spans="1:19" ht="15.75" thickBot="1"/>
     <row r="39" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A39" s="62" t="s">
+      <c r="A39" s="112" t="s">
         <v>25</v>
       </c>
-      <c r="B39" s="63"/>
-      <c r="C39" s="63"/>
-      <c r="D39" s="63"/>
-      <c r="E39" s="64"/>
-      <c r="N39" s="58" t="s">
+      <c r="B39" s="113"/>
+      <c r="C39" s="113"/>
+      <c r="D39" s="113"/>
+      <c r="E39" s="114"/>
+      <c r="N39" s="77" t="s">
         <v>110</v>
       </c>
-      <c r="O39" s="58"/>
-      <c r="P39" s="58"/>
-      <c r="Q39" s="58"/>
-      <c r="R39" s="58"/>
-      <c r="S39" s="58"/>
+      <c r="O39" s="77"/>
+      <c r="P39" s="77"/>
+      <c r="Q39" s="77"/>
+      <c r="R39" s="77"/>
+      <c r="S39" s="77"/>
     </row>
     <row r="40" spans="1:19">
       <c r="A40" s="14" t="s">
         <v>24</v>
       </c>
       <c r="B40" s="13"/>
-      <c r="C40" s="65" t="s">
+      <c r="C40" s="115" t="s">
         <v>22</v>
       </c>
-      <c r="D40" s="66"/>
+      <c r="D40" s="116"/>
       <c r="E40" s="27"/>
     </row>
     <row r="41" spans="1:19">
@@ -2685,10 +2696,10 @@
         <v>21</v>
       </c>
       <c r="B41" s="5"/>
-      <c r="C41" s="65" t="s">
+      <c r="C41" s="115" t="s">
         <v>23</v>
       </c>
-      <c r="D41" s="66"/>
+      <c r="D41" s="116"/>
       <c r="E41" s="8"/>
     </row>
     <row r="42" spans="1:19" ht="17.25">
@@ -2696,10 +2707,10 @@
         <v>112</v>
       </c>
       <c r="B42" s="54"/>
-      <c r="C42" s="71" t="s">
+      <c r="C42" s="96" t="s">
         <v>64</v>
       </c>
-      <c r="D42" s="72"/>
+      <c r="D42" s="97"/>
       <c r="E42" s="37"/>
       <c r="N42" s="48" t="s">
         <v>4</v>
@@ -2714,38 +2725,38 @@
       </c>
     </row>
     <row r="44" spans="1:19">
-      <c r="A44" s="67" t="s">
+      <c r="A44" s="117" t="s">
         <v>35</v>
       </c>
-      <c r="B44" s="68"/>
-      <c r="C44" s="68"/>
-      <c r="D44" s="68"/>
-      <c r="E44" s="68"/>
-      <c r="F44" s="68"/>
-      <c r="G44" s="68"/>
-      <c r="H44" s="68"/>
-      <c r="I44" s="68"/>
-      <c r="J44" s="68"/>
-      <c r="K44" s="68"/>
-      <c r="L44" s="68"/>
+      <c r="B44" s="118"/>
+      <c r="C44" s="118"/>
+      <c r="D44" s="118"/>
+      <c r="E44" s="118"/>
+      <c r="F44" s="118"/>
+      <c r="G44" s="118"/>
+      <c r="H44" s="118"/>
+      <c r="I44" s="118"/>
+      <c r="J44" s="118"/>
+      <c r="K44" s="118"/>
+      <c r="L44" s="118"/>
     </row>
     <row r="45" spans="1:19" ht="17.25">
       <c r="A45" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="B45" s="61" t="s">
+      <c r="B45" s="111" t="s">
         <v>55</v>
       </c>
-      <c r="C45" s="61"/>
-      <c r="D45" s="61"/>
-      <c r="E45" s="61"/>
-      <c r="F45" s="61"/>
-      <c r="G45" s="61"/>
-      <c r="H45" s="61"/>
-      <c r="I45" s="61"/>
-      <c r="J45" s="61"/>
-      <c r="K45" s="61"/>
-      <c r="L45" s="61"/>
+      <c r="C45" s="111"/>
+      <c r="D45" s="111"/>
+      <c r="E45" s="111"/>
+      <c r="F45" s="111"/>
+      <c r="G45" s="111"/>
+      <c r="H45" s="111"/>
+      <c r="I45" s="111"/>
+      <c r="J45" s="111"/>
+      <c r="K45" s="111"/>
+      <c r="L45" s="111"/>
       <c r="N45" s="48" t="s">
         <v>92</v>
       </c>
@@ -2757,19 +2768,19 @@
       <c r="A46" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="B46" s="61" t="s">
+      <c r="B46" s="111" t="s">
         <v>56</v>
       </c>
-      <c r="C46" s="61"/>
-      <c r="D46" s="61"/>
-      <c r="E46" s="61"/>
-      <c r="F46" s="61"/>
-      <c r="G46" s="61"/>
-      <c r="H46" s="61"/>
-      <c r="I46" s="61"/>
-      <c r="J46" s="61"/>
-      <c r="K46" s="61"/>
-      <c r="L46" s="61"/>
+      <c r="C46" s="111"/>
+      <c r="D46" s="111"/>
+      <c r="E46" s="111"/>
+      <c r="F46" s="111"/>
+      <c r="G46" s="111"/>
+      <c r="H46" s="111"/>
+      <c r="I46" s="111"/>
+      <c r="J46" s="111"/>
+      <c r="K46" s="111"/>
+      <c r="L46" s="111"/>
       <c r="O46" s="42" t="s">
         <v>96</v>
       </c>
@@ -2778,19 +2789,19 @@
       <c r="A47" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="B47" s="61" t="s">
+      <c r="B47" s="111" t="s">
         <v>57</v>
       </c>
-      <c r="C47" s="61"/>
-      <c r="D47" s="61"/>
-      <c r="E47" s="61"/>
-      <c r="F47" s="61"/>
-      <c r="G47" s="61"/>
-      <c r="H47" s="61"/>
-      <c r="I47" s="61"/>
-      <c r="J47" s="61"/>
-      <c r="K47" s="61"/>
-      <c r="L47" s="61"/>
+      <c r="C47" s="111"/>
+      <c r="D47" s="111"/>
+      <c r="E47" s="111"/>
+      <c r="F47" s="111"/>
+      <c r="G47" s="111"/>
+      <c r="H47" s="111"/>
+      <c r="I47" s="111"/>
+      <c r="J47" s="111"/>
+      <c r="K47" s="111"/>
+      <c r="L47" s="111"/>
       <c r="O47" t="s">
         <v>99</v>
       </c>
@@ -2799,37 +2810,37 @@
       <c r="A48" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="B48" s="61" t="s">
+      <c r="B48" s="111" t="s">
         <v>44</v>
       </c>
-      <c r="C48" s="61"/>
-      <c r="D48" s="61"/>
-      <c r="E48" s="61"/>
-      <c r="F48" s="61"/>
-      <c r="G48" s="61"/>
-      <c r="H48" s="61"/>
-      <c r="I48" s="61"/>
-      <c r="J48" s="61"/>
-      <c r="K48" s="61"/>
-      <c r="L48" s="61"/>
+      <c r="C48" s="111"/>
+      <c r="D48" s="111"/>
+      <c r="E48" s="111"/>
+      <c r="F48" s="111"/>
+      <c r="G48" s="111"/>
+      <c r="H48" s="111"/>
+      <c r="I48" s="111"/>
+      <c r="J48" s="111"/>
+      <c r="K48" s="111"/>
+      <c r="L48" s="111"/>
     </row>
     <row r="49" spans="1:15" ht="17.25">
       <c r="A49" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="B49" s="61" t="s">
+      <c r="B49" s="111" t="s">
         <v>33</v>
       </c>
-      <c r="C49" s="61"/>
-      <c r="D49" s="61"/>
-      <c r="E49" s="61"/>
-      <c r="F49" s="61"/>
-      <c r="G49" s="61"/>
-      <c r="H49" s="61"/>
-      <c r="I49" s="61"/>
-      <c r="J49" s="61"/>
-      <c r="K49" s="61"/>
-      <c r="L49" s="61"/>
+      <c r="C49" s="111"/>
+      <c r="D49" s="111"/>
+      <c r="E49" s="111"/>
+      <c r="F49" s="111"/>
+      <c r="G49" s="111"/>
+      <c r="H49" s="111"/>
+      <c r="I49" s="111"/>
+      <c r="J49" s="111"/>
+      <c r="K49" s="111"/>
+      <c r="L49" s="111"/>
       <c r="N49" s="48" t="s">
         <v>91</v>
       </c>
@@ -2841,19 +2852,19 @@
       <c r="A50" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="B50" s="61" t="s">
+      <c r="B50" s="111" t="s">
         <v>54</v>
       </c>
-      <c r="C50" s="61"/>
-      <c r="D50" s="61"/>
-      <c r="E50" s="61"/>
-      <c r="F50" s="61"/>
-      <c r="G50" s="61"/>
-      <c r="H50" s="61"/>
-      <c r="I50" s="61"/>
-      <c r="J50" s="61"/>
-      <c r="K50" s="61"/>
-      <c r="L50" s="61"/>
+      <c r="C50" s="111"/>
+      <c r="D50" s="111"/>
+      <c r="E50" s="111"/>
+      <c r="F50" s="111"/>
+      <c r="G50" s="111"/>
+      <c r="H50" s="111"/>
+      <c r="I50" s="111"/>
+      <c r="J50" s="111"/>
+      <c r="K50" s="111"/>
+      <c r="L50" s="111"/>
       <c r="O50" t="s">
         <v>97</v>
       </c>
@@ -2862,19 +2873,19 @@
       <c r="A51" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="B51" s="61" t="s">
+      <c r="B51" s="111" t="s">
         <v>53</v>
       </c>
-      <c r="C51" s="61"/>
-      <c r="D51" s="61"/>
-      <c r="E51" s="61"/>
-      <c r="F51" s="61"/>
-      <c r="G51" s="61"/>
-      <c r="H51" s="61"/>
-      <c r="I51" s="61"/>
-      <c r="J51" s="61"/>
-      <c r="K51" s="61"/>
-      <c r="L51" s="61"/>
+      <c r="C51" s="111"/>
+      <c r="D51" s="111"/>
+      <c r="E51" s="111"/>
+      <c r="F51" s="111"/>
+      <c r="G51" s="111"/>
+      <c r="H51" s="111"/>
+      <c r="I51" s="111"/>
+      <c r="J51" s="111"/>
+      <c r="K51" s="111"/>
+      <c r="L51" s="111"/>
       <c r="O51" t="s">
         <v>98</v>
       </c>
@@ -2892,33 +2903,24 @@
   <sortState ref="A24:K25">
     <sortCondition ref="A3"/>
   </sortState>
-  <mergeCells count="55">
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="H28:K28"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="O6:U6"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="H27:K27"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="N24:S24"/>
-    <mergeCell ref="N27:S27"/>
-    <mergeCell ref="N20:S20"/>
-    <mergeCell ref="O14:S15"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="H30:K30"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="H32:K32"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="H31:L31"/>
+  <mergeCells count="56">
+    <mergeCell ref="N28:S28"/>
+    <mergeCell ref="N39:S39"/>
+    <mergeCell ref="N32:S32"/>
+    <mergeCell ref="N35:S35"/>
+    <mergeCell ref="N30:S30"/>
+    <mergeCell ref="N37:S37"/>
+    <mergeCell ref="B50:L50"/>
+    <mergeCell ref="B51:L51"/>
+    <mergeCell ref="A39:E39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="B45:L45"/>
+    <mergeCell ref="A44:L44"/>
+    <mergeCell ref="B46:L46"/>
+    <mergeCell ref="B47:L47"/>
+    <mergeCell ref="B48:L48"/>
+    <mergeCell ref="B49:L49"/>
     <mergeCell ref="A35:B35"/>
     <mergeCell ref="A36:B36"/>
     <mergeCell ref="A37:B37"/>
@@ -2931,23 +2933,33 @@
     <mergeCell ref="C35:G35"/>
     <mergeCell ref="C36:G36"/>
     <mergeCell ref="C37:G37"/>
-    <mergeCell ref="B50:L50"/>
-    <mergeCell ref="B51:L51"/>
-    <mergeCell ref="A39:E39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="B45:L45"/>
-    <mergeCell ref="A44:L44"/>
-    <mergeCell ref="B46:L46"/>
-    <mergeCell ref="B47:L47"/>
-    <mergeCell ref="B48:L48"/>
-    <mergeCell ref="B49:L49"/>
-    <mergeCell ref="N28:S28"/>
-    <mergeCell ref="N39:S39"/>
-    <mergeCell ref="N32:S32"/>
-    <mergeCell ref="N35:S35"/>
-    <mergeCell ref="N30:S30"/>
-    <mergeCell ref="N37:S37"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="H30:K30"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="H32:K32"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="H31:L31"/>
+    <mergeCell ref="O6:U6"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="H27:K27"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="N24:S24"/>
+    <mergeCell ref="N27:S27"/>
+    <mergeCell ref="N20:S20"/>
+    <mergeCell ref="O14:S15"/>
+    <mergeCell ref="N22:S22"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="H28:K28"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="A28:B28"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="Q4" r:id="rId1"/>

</xml_diff>

<commit_message>
sigue el proceso de la implementacion. Se realizó testig exaustivo, con y sin datos. Hubo varios bugs. Pendiente de resolver Altas en trayectoria y formacion (career y studie -> problemas para obtener el valor de los selects)
</commit_message>
<xml_diff>
--- a/Cuadro-de-estado.xlsx
+++ b/Cuadro-de-estado.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="129">
   <si>
     <t>BACKEND</t>
   </si>
@@ -476,6 +476,18 @@
   </si>
   <si>
     <t>En SOFTSKILL form, inicializa mal el range</t>
+  </si>
+  <si>
+    <t>OJO EN LOS FORM. SIN NO HAY CAMBIOS QUE NO VAYA AL HTTP</t>
+  </si>
+  <si>
+    <t>Variables temporales, que sean de los metodos, no de la clase</t>
+  </si>
+  <si>
+    <t>LOS FORM TIENEN ALGO MAL CON LAS VALIDACIONES, AL INICIAR</t>
+  </si>
+  <si>
+    <t>Estudios y trabajos, da repetido el nombre cuando modifico cualquier otro dato</t>
   </si>
 </sst>
 </file>
@@ -767,12 +779,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -783,6 +789,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="38">
     <border>
@@ -1349,13 +1361,13 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="13" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1369,9 +1381,127 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1381,6 +1511,54 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1390,181 +1568,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1869,7 +1879,7 @@
   <dimension ref="A1:U54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" activeCellId="1" sqref="A17:XFD17 A13:XFD14"/>
+      <selection activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1886,25 +1896,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="105" t="s">
         <v>84</v>
       </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="71"/>
-      <c r="I1" s="71"/>
-      <c r="J1" s="71"/>
-      <c r="K1" s="71"/>
-      <c r="L1" s="71"/>
+      <c r="B1" s="105"/>
+      <c r="C1" s="105"/>
+      <c r="D1" s="105"/>
+      <c r="E1" s="105"/>
+      <c r="F1" s="105"/>
+      <c r="G1" s="105"/>
+      <c r="H1" s="105"/>
+      <c r="I1" s="105"/>
+      <c r="J1" s="105"/>
+      <c r="K1" s="105"/>
+      <c r="L1" s="105"/>
     </row>
     <row r="2" spans="1:21" ht="19.5" thickBot="1">
       <c r="A2" s="44">
         <f ca="1">M2-TODAY()-1</f>
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B2" s="45" t="s">
         <v>85</v>
@@ -1918,30 +1928,30 @@
       </c>
     </row>
     <row r="3" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="72" t="s">
+      <c r="A3" s="106" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="73"/>
-      <c r="C3" s="63" t="s">
+      <c r="B3" s="107"/>
+      <c r="C3" s="108" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="64"/>
-      <c r="E3" s="64"/>
-      <c r="F3" s="64"/>
-      <c r="G3" s="66"/>
-      <c r="H3" s="63" t="s">
+      <c r="D3" s="109"/>
+      <c r="E3" s="109"/>
+      <c r="F3" s="109"/>
+      <c r="G3" s="110"/>
+      <c r="H3" s="108" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="64"/>
-      <c r="J3" s="65"/>
-      <c r="K3" s="66"/>
+      <c r="I3" s="109"/>
+      <c r="J3" s="111"/>
+      <c r="K3" s="110"/>
       <c r="L3" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="74" t="s">
+      <c r="M3" s="112" t="s">
         <v>76</v>
       </c>
-      <c r="N3" s="70"/>
+      <c r="N3" s="104"/>
     </row>
     <row r="4" spans="1:21" s="3" customFormat="1" ht="40.5" customHeight="1" thickBot="1">
       <c r="A4" s="17" t="s">
@@ -1980,10 +1990,10 @@
       <c r="L4" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="M4" s="75" t="s">
+      <c r="M4" s="113" t="s">
         <v>77</v>
       </c>
-      <c r="N4" s="76"/>
+      <c r="N4" s="114"/>
       <c r="O4" s="34" t="s">
         <v>61</v>
       </c>
@@ -1997,8 +2007,6 @@
       <c r="C5" s="30"/>
       <c r="D5" s="30"/>
       <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
-      <c r="G5" s="30"/>
       <c r="H5" s="30"/>
       <c r="I5" s="30"/>
       <c r="J5" s="30"/>
@@ -2015,22 +2023,22 @@
       <c r="C6" s="4"/>
       <c r="D6" s="40"/>
       <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="57"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
-      <c r="O6" s="69" t="s">
+      <c r="O6" s="103" t="s">
         <v>65</v>
       </c>
-      <c r="P6" s="70"/>
-      <c r="Q6" s="70"/>
-      <c r="R6" s="70"/>
-      <c r="S6" s="70"/>
-      <c r="T6" s="70"/>
-      <c r="U6" s="70"/>
+      <c r="P6" s="104"/>
+      <c r="Q6" s="104"/>
+      <c r="R6" s="104"/>
+      <c r="S6" s="104"/>
+      <c r="T6" s="104"/>
+      <c r="U6" s="104"/>
     </row>
     <row r="7" spans="1:21" ht="4.5" customHeight="1">
       <c r="A7" s="28"/>
@@ -2056,7 +2064,7 @@
       <c r="C8" s="4"/>
       <c r="D8" s="40"/>
       <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
+      <c r="F8" s="40"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
@@ -2081,10 +2089,10 @@
       <c r="B9" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="5"/>
+      <c r="C9" s="4"/>
       <c r="D9" s="40"/>
       <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
+      <c r="F9" s="40"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
@@ -2103,16 +2111,19 @@
       <c r="B10" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="5"/>
+      <c r="C10" s="4"/>
       <c r="D10" s="40"/>
       <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
+      <c r="F10" s="40"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
+      <c r="O10" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="11" spans="1:21">
       <c r="A11" s="18" t="s">
@@ -2121,10 +2132,10 @@
       <c r="B11" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="5"/>
+      <c r="C11" s="4"/>
       <c r="D11" s="40"/>
       <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
+      <c r="F11" s="40"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
@@ -2187,13 +2198,13 @@
       <c r="J14" s="4"/>
       <c r="K14" s="54"/>
       <c r="L14" s="4"/>
-      <c r="O14" s="78" t="s">
+      <c r="O14" s="115" t="s">
         <v>75</v>
       </c>
-      <c r="P14" s="78"/>
-      <c r="Q14" s="78"/>
-      <c r="R14" s="78"/>
-      <c r="S14" s="78"/>
+      <c r="P14" s="115"/>
+      <c r="Q14" s="115"/>
+      <c r="R14" s="115"/>
+      <c r="S14" s="115"/>
     </row>
     <row r="15" spans="1:21" ht="15" customHeight="1">
       <c r="A15" s="38" t="s">
@@ -2212,11 +2223,11 @@
       <c r="J15" s="4"/>
       <c r="K15" s="54"/>
       <c r="L15" s="4"/>
-      <c r="O15" s="78"/>
-      <c r="P15" s="78"/>
-      <c r="Q15" s="78"/>
-      <c r="R15" s="78"/>
-      <c r="S15" s="78"/>
+      <c r="O15" s="115"/>
+      <c r="P15" s="115"/>
+      <c r="Q15" s="115"/>
+      <c r="R15" s="115"/>
+      <c r="S15" s="115"/>
       <c r="T15" s="53"/>
     </row>
     <row r="16" spans="1:21">
@@ -2236,6 +2247,14 @@
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
       <c r="L16" s="4"/>
+      <c r="N16" s="59" t="s">
+        <v>110</v>
+      </c>
+      <c r="O16" s="59"/>
+      <c r="P16" s="59"/>
+      <c r="Q16" s="59"/>
+      <c r="R16" s="59"/>
+      <c r="S16" s="59"/>
       <c r="T16" s="53"/>
     </row>
     <row r="17" spans="1:19">
@@ -2255,9 +2274,14 @@
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
       <c r="L17" s="4"/>
-      <c r="O17" t="s">
-        <v>70</v>
-      </c>
+      <c r="N17" s="59" t="s">
+        <v>127</v>
+      </c>
+      <c r="O17" s="59"/>
+      <c r="P17" s="59"/>
+      <c r="Q17" s="59"/>
+      <c r="R17" s="59"/>
+      <c r="S17" s="59"/>
     </row>
     <row r="18" spans="1:19" ht="4.5" customHeight="1">
       <c r="A18" s="28"/>
@@ -2290,6 +2314,14 @@
       <c r="J19" s="5"/>
       <c r="K19" s="7"/>
       <c r="L19" s="52"/>
+      <c r="N19" s="59" t="s">
+        <v>125</v>
+      </c>
+      <c r="O19" s="59"/>
+      <c r="P19" s="59"/>
+      <c r="Q19" s="59"/>
+      <c r="R19" s="59"/>
+      <c r="S19" s="59"/>
     </row>
     <row r="20" spans="1:19">
       <c r="A20" s="39" t="s">
@@ -2308,14 +2340,14 @@
       <c r="J20" s="5"/>
       <c r="K20" s="7"/>
       <c r="L20" s="52"/>
-      <c r="N20" s="77" t="s">
+      <c r="N20" s="59" t="s">
         <v>113</v>
       </c>
-      <c r="O20" s="77"/>
-      <c r="P20" s="77"/>
-      <c r="Q20" s="77"/>
-      <c r="R20" s="77"/>
-      <c r="S20" s="77"/>
+      <c r="O20" s="59"/>
+      <c r="P20" s="59"/>
+      <c r="Q20" s="59"/>
+      <c r="R20" s="59"/>
+      <c r="S20" s="59"/>
     </row>
     <row r="21" spans="1:19" ht="4.5" customHeight="1">
       <c r="A21" s="28"/>
@@ -2346,14 +2378,14 @@
       <c r="J22" s="5"/>
       <c r="K22" s="7"/>
       <c r="L22" s="4"/>
-      <c r="N22" s="77" t="s">
+      <c r="N22" s="59" t="s">
         <v>124</v>
       </c>
-      <c r="O22" s="77"/>
-      <c r="P22" s="77"/>
-      <c r="Q22" s="77"/>
-      <c r="R22" s="77"/>
-      <c r="S22" s="77"/>
+      <c r="O22" s="59"/>
+      <c r="P22" s="59"/>
+      <c r="Q22" s="59"/>
+      <c r="R22" s="59"/>
+      <c r="S22" s="59"/>
     </row>
     <row r="23" spans="1:19" ht="4.5" customHeight="1">
       <c r="A23" s="28"/>
@@ -2384,14 +2416,14 @@
       <c r="J24" s="5"/>
       <c r="K24" s="7"/>
       <c r="L24" s="4"/>
-      <c r="N24" s="77" t="s">
+      <c r="N24" s="59" t="s">
         <v>83</v>
       </c>
-      <c r="O24" s="77"/>
-      <c r="P24" s="77"/>
-      <c r="Q24" s="77"/>
-      <c r="R24" s="77"/>
-      <c r="S24" s="77"/>
+      <c r="O24" s="59"/>
+      <c r="P24" s="59"/>
+      <c r="Q24" s="59"/>
+      <c r="R24" s="59"/>
+      <c r="S24" s="59"/>
     </row>
     <row r="25" spans="1:19">
       <c r="A25" s="39" t="s">
@@ -2410,6 +2442,14 @@
       <c r="J25" s="5"/>
       <c r="K25" s="7"/>
       <c r="L25" s="4"/>
+      <c r="N25" s="59" t="s">
+        <v>82</v>
+      </c>
+      <c r="O25" s="59"/>
+      <c r="P25" s="59"/>
+      <c r="Q25" s="59"/>
+      <c r="R25" s="59"/>
+      <c r="S25" s="59"/>
     </row>
     <row r="26" spans="1:19" ht="4.5" customHeight="1" thickBot="1">
       <c r="A26" s="28"/>
@@ -2428,60 +2468,60 @@
     <row r="27" spans="1:19" ht="15.75" thickBot="1">
       <c r="A27" s="23"/>
       <c r="B27" s="25"/>
-      <c r="C27" s="63" t="s">
+      <c r="C27" s="108" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="64"/>
-      <c r="E27" s="64"/>
-      <c r="F27" s="64"/>
-      <c r="G27" s="66"/>
-      <c r="H27" s="63" t="s">
+      <c r="D27" s="109"/>
+      <c r="E27" s="109"/>
+      <c r="F27" s="109"/>
+      <c r="G27" s="110"/>
+      <c r="H27" s="108" t="s">
         <v>0</v>
       </c>
-      <c r="I27" s="64"/>
-      <c r="J27" s="65"/>
-      <c r="K27" s="66"/>
+      <c r="I27" s="109"/>
+      <c r="J27" s="111"/>
+      <c r="K27" s="110"/>
       <c r="L27" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="N27" s="77" t="s">
+      <c r="N27" s="59" t="s">
         <v>78</v>
       </c>
-      <c r="O27" s="77"/>
-      <c r="P27" s="77"/>
-      <c r="Q27" s="77"/>
-      <c r="R27" s="77"/>
-      <c r="S27" s="77"/>
+      <c r="O27" s="59"/>
+      <c r="P27" s="59"/>
+      <c r="Q27" s="59"/>
+      <c r="R27" s="59"/>
+      <c r="S27" s="59"/>
     </row>
     <row r="28" spans="1:19" ht="30">
-      <c r="A28" s="67" t="s">
+      <c r="A28" s="119" t="s">
         <v>29</v>
       </c>
-      <c r="B28" s="68"/>
-      <c r="C28" s="57" t="s">
+      <c r="B28" s="120"/>
+      <c r="C28" s="97" t="s">
         <v>88</v>
       </c>
-      <c r="D28" s="58"/>
-      <c r="E28" s="58"/>
-      <c r="F28" s="58"/>
-      <c r="G28" s="59"/>
-      <c r="H28" s="60" t="s">
+      <c r="D28" s="98"/>
+      <c r="E28" s="98"/>
+      <c r="F28" s="98"/>
+      <c r="G28" s="99"/>
+      <c r="H28" s="116" t="s">
         <v>86</v>
       </c>
-      <c r="I28" s="61"/>
-      <c r="J28" s="61"/>
-      <c r="K28" s="62"/>
+      <c r="I28" s="117"/>
+      <c r="J28" s="117"/>
+      <c r="K28" s="118"/>
       <c r="L28" s="47" t="s">
         <v>87</v>
       </c>
-      <c r="N28" s="119" t="s">
+      <c r="N28" s="58" t="s">
         <v>111</v>
       </c>
-      <c r="O28" s="119"/>
-      <c r="P28" s="119"/>
-      <c r="Q28" s="119"/>
-      <c r="R28" s="119"/>
-      <c r="S28" s="119"/>
+      <c r="O28" s="58"/>
+      <c r="P28" s="58"/>
+      <c r="Q28" s="58"/>
+      <c r="R28" s="58"/>
+      <c r="S28" s="58"/>
     </row>
     <row r="29" spans="1:19" ht="4.5" customHeight="1">
       <c r="A29" s="28"/>
@@ -2498,92 +2538,100 @@
       <c r="L29" s="30"/>
     </row>
     <row r="30" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A30" s="83" t="s">
+      <c r="A30" s="68" t="s">
         <v>38</v>
       </c>
-      <c r="B30" s="84"/>
-      <c r="C30" s="79"/>
-      <c r="D30" s="80"/>
-      <c r="E30" s="80"/>
-      <c r="F30" s="80"/>
-      <c r="G30" s="81"/>
-      <c r="H30" s="82"/>
-      <c r="I30" s="80"/>
-      <c r="J30" s="80"/>
-      <c r="K30" s="81"/>
+      <c r="B30" s="69"/>
+      <c r="C30" s="87"/>
+      <c r="D30" s="88"/>
+      <c r="E30" s="88"/>
+      <c r="F30" s="88"/>
+      <c r="G30" s="89"/>
+      <c r="H30" s="90"/>
+      <c r="I30" s="88"/>
+      <c r="J30" s="88"/>
+      <c r="K30" s="89"/>
       <c r="L30" s="21" t="s">
         <v>5</v>
       </c>
       <c r="M30" s="32"/>
-      <c r="N30" s="121" t="s">
+      <c r="N30" s="59" t="s">
         <v>72</v>
       </c>
-      <c r="O30" s="121"/>
-      <c r="P30" s="121"/>
-      <c r="Q30" s="121"/>
-      <c r="R30" s="121"/>
-      <c r="S30" s="121"/>
+      <c r="O30" s="59"/>
+      <c r="P30" s="59"/>
+      <c r="Q30" s="59"/>
+      <c r="R30" s="59"/>
+      <c r="S30" s="59"/>
     </row>
     <row r="31" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A31" s="83" t="s">
+      <c r="A31" s="68" t="s">
         <v>79</v>
       </c>
-      <c r="B31" s="84"/>
-      <c r="C31" s="57"/>
-      <c r="D31" s="58"/>
-      <c r="E31" s="58"/>
-      <c r="F31" s="58"/>
-      <c r="G31" s="59"/>
-      <c r="H31" s="93" t="s">
+      <c r="B31" s="69"/>
+      <c r="C31" s="97"/>
+      <c r="D31" s="98"/>
+      <c r="E31" s="98"/>
+      <c r="F31" s="98"/>
+      <c r="G31" s="99"/>
+      <c r="H31" s="100" t="s">
         <v>80</v>
       </c>
-      <c r="I31" s="94"/>
-      <c r="J31" s="94"/>
-      <c r="K31" s="94"/>
-      <c r="L31" s="95"/>
+      <c r="I31" s="101"/>
+      <c r="J31" s="101"/>
+      <c r="K31" s="101"/>
+      <c r="L31" s="102"/>
       <c r="M31" s="32"/>
+      <c r="N31" s="58" t="s">
+        <v>73</v>
+      </c>
+      <c r="O31" s="58"/>
+      <c r="P31" s="58"/>
+      <c r="Q31" s="58"/>
+      <c r="R31" s="58"/>
+      <c r="S31" s="58"/>
     </row>
     <row r="32" spans="1:19" ht="16.5" thickBot="1">
-      <c r="A32" s="87" t="s">
+      <c r="A32" s="93" t="s">
         <v>59</v>
       </c>
-      <c r="B32" s="88"/>
-      <c r="C32" s="89"/>
-      <c r="D32" s="90"/>
-      <c r="E32" s="90"/>
-      <c r="F32" s="90"/>
-      <c r="G32" s="91"/>
-      <c r="H32" s="92"/>
-      <c r="I32" s="90"/>
-      <c r="J32" s="90"/>
-      <c r="K32" s="91"/>
+      <c r="B32" s="94"/>
+      <c r="C32" s="84"/>
+      <c r="D32" s="85"/>
+      <c r="E32" s="85"/>
+      <c r="F32" s="85"/>
+      <c r="G32" s="95"/>
+      <c r="H32" s="96"/>
+      <c r="I32" s="85"/>
+      <c r="J32" s="85"/>
+      <c r="K32" s="95"/>
       <c r="M32" s="32"/>
-      <c r="N32" s="120" t="s">
-        <v>73</v>
-      </c>
-      <c r="O32" s="120"/>
-      <c r="P32" s="120"/>
-      <c r="Q32" s="120"/>
-      <c r="R32" s="120"/>
-      <c r="S32" s="120"/>
     </row>
     <row r="33" spans="1:19" ht="30.75" customHeight="1" thickBot="1">
-      <c r="A33" s="85" t="s">
+      <c r="A33" s="91" t="s">
         <v>34</v>
       </c>
-      <c r="B33" s="86"/>
-      <c r="C33" s="101" t="s">
+      <c r="B33" s="92"/>
+      <c r="C33" s="75" t="s">
         <v>58</v>
       </c>
-      <c r="D33" s="102"/>
-      <c r="E33" s="102"/>
-      <c r="F33" s="102"/>
-      <c r="G33" s="103"/>
-      <c r="H33" s="98"/>
-      <c r="I33" s="99"/>
-      <c r="J33" s="99"/>
-      <c r="K33" s="100"/>
+      <c r="D33" s="76"/>
+      <c r="E33" s="76"/>
+      <c r="F33" s="76"/>
+      <c r="G33" s="77"/>
+      <c r="H33" s="72"/>
+      <c r="I33" s="73"/>
+      <c r="J33" s="73"/>
+      <c r="K33" s="74"/>
       <c r="M33" s="32"/>
+      <c r="N33" s="58" t="s">
+        <v>126</v>
+      </c>
+      <c r="O33" s="58"/>
+      <c r="P33" s="58"/>
+      <c r="Q33" s="58"/>
+      <c r="R33" s="58"/>
+      <c r="S33" s="58"/>
     </row>
     <row r="34" spans="1:19" ht="4.5" customHeight="1" thickBot="1">
       <c r="A34" s="28"/>
@@ -2599,96 +2647,89 @@
       <c r="K34" s="30"/>
     </row>
     <row r="35" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A35" s="83" t="s">
+      <c r="A35" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="84"/>
-      <c r="C35" s="89"/>
-      <c r="D35" s="90"/>
-      <c r="E35" s="90"/>
-      <c r="F35" s="90"/>
-      <c r="G35" s="110"/>
-      <c r="H35" s="104"/>
-      <c r="I35" s="105"/>
-      <c r="J35" s="105"/>
-      <c r="K35" s="106"/>
+      <c r="B35" s="69"/>
+      <c r="C35" s="84"/>
+      <c r="D35" s="85"/>
+      <c r="E35" s="85"/>
+      <c r="F35" s="85"/>
+      <c r="G35" s="86"/>
+      <c r="H35" s="78"/>
+      <c r="I35" s="79"/>
+      <c r="J35" s="79"/>
+      <c r="K35" s="80"/>
       <c r="M35" s="32"/>
-      <c r="N35" s="121" t="s">
+    </row>
+    <row r="36" spans="1:19" ht="15.75" thickBot="1">
+      <c r="A36" s="68" t="s">
+        <v>89</v>
+      </c>
+      <c r="B36" s="69"/>
+      <c r="C36" s="84"/>
+      <c r="D36" s="85"/>
+      <c r="E36" s="85"/>
+      <c r="F36" s="85"/>
+      <c r="G36" s="86"/>
+      <c r="H36" s="78"/>
+      <c r="I36" s="79"/>
+      <c r="J36" s="79"/>
+      <c r="K36" s="80"/>
+      <c r="M36" s="32"/>
+    </row>
+    <row r="37" spans="1:19" ht="15.75" thickBot="1">
+      <c r="A37" s="68" t="s">
+        <v>7</v>
+      </c>
+      <c r="B37" s="69"/>
+      <c r="C37" s="81"/>
+      <c r="D37" s="82"/>
+      <c r="E37" s="82"/>
+      <c r="F37" s="82"/>
+      <c r="G37" s="83"/>
+      <c r="H37" s="81"/>
+      <c r="I37" s="82"/>
+      <c r="J37" s="82"/>
+      <c r="K37" s="83"/>
+      <c r="M37" s="32"/>
+      <c r="N37" s="121" t="s">
         <v>74</v>
       </c>
-      <c r="O35" s="121"/>
-      <c r="P35" s="121"/>
-      <c r="Q35" s="121"/>
-      <c r="R35" s="121"/>
-      <c r="S35" s="121"/>
-    </row>
-    <row r="36" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A36" s="83" t="s">
-        <v>89</v>
-      </c>
-      <c r="B36" s="84"/>
-      <c r="C36" s="89"/>
-      <c r="D36" s="90"/>
-      <c r="E36" s="90"/>
-      <c r="F36" s="90"/>
-      <c r="G36" s="110"/>
-      <c r="H36" s="104"/>
-      <c r="I36" s="105"/>
-      <c r="J36" s="105"/>
-      <c r="K36" s="106"/>
-      <c r="M36" s="32"/>
-    </row>
-    <row r="37" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A37" s="83" t="s">
-        <v>7</v>
-      </c>
-      <c r="B37" s="84"/>
-      <c r="C37" s="107"/>
-      <c r="D37" s="108"/>
-      <c r="E37" s="108"/>
-      <c r="F37" s="108"/>
-      <c r="G37" s="109"/>
-      <c r="H37" s="107"/>
-      <c r="I37" s="108"/>
-      <c r="J37" s="108"/>
-      <c r="K37" s="109"/>
-      <c r="M37" s="32"/>
-      <c r="N37" s="77" t="s">
-        <v>82</v>
-      </c>
-      <c r="O37" s="77"/>
-      <c r="P37" s="77"/>
-      <c r="Q37" s="77"/>
-      <c r="R37" s="77"/>
-      <c r="S37" s="77"/>
-    </row>
-    <row r="38" spans="1:19" ht="15.75" thickBot="1"/>
+      <c r="O37" s="121"/>
+      <c r="P37" s="121"/>
+      <c r="Q37" s="121"/>
+      <c r="R37" s="121"/>
+      <c r="S37" s="121"/>
+    </row>
+    <row r="38" spans="1:19" ht="15.75" thickBot="1">
+      <c r="N38" s="121" t="s">
+        <v>128</v>
+      </c>
+      <c r="O38" s="121"/>
+      <c r="P38" s="121"/>
+      <c r="Q38" s="121"/>
+      <c r="R38" s="121"/>
+      <c r="S38" s="121"/>
+    </row>
     <row r="39" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A39" s="112" t="s">
+      <c r="A39" s="61" t="s">
         <v>25</v>
       </c>
-      <c r="B39" s="113"/>
-      <c r="C39" s="113"/>
-      <c r="D39" s="113"/>
-      <c r="E39" s="114"/>
-      <c r="N39" s="77" t="s">
-        <v>110</v>
-      </c>
-      <c r="O39" s="77"/>
-      <c r="P39" s="77"/>
-      <c r="Q39" s="77"/>
-      <c r="R39" s="77"/>
-      <c r="S39" s="77"/>
+      <c r="B39" s="62"/>
+      <c r="C39" s="62"/>
+      <c r="D39" s="62"/>
+      <c r="E39" s="63"/>
     </row>
     <row r="40" spans="1:19">
       <c r="A40" s="14" t="s">
         <v>24</v>
       </c>
       <c r="B40" s="13"/>
-      <c r="C40" s="115" t="s">
+      <c r="C40" s="64" t="s">
         <v>22</v>
       </c>
-      <c r="D40" s="116"/>
+      <c r="D40" s="65"/>
       <c r="E40" s="27"/>
     </row>
     <row r="41" spans="1:19">
@@ -2696,10 +2737,10 @@
         <v>21</v>
       </c>
       <c r="B41" s="5"/>
-      <c r="C41" s="115" t="s">
+      <c r="C41" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="D41" s="116"/>
+      <c r="D41" s="65"/>
       <c r="E41" s="8"/>
     </row>
     <row r="42" spans="1:19" ht="17.25">
@@ -2707,10 +2748,10 @@
         <v>112</v>
       </c>
       <c r="B42" s="54"/>
-      <c r="C42" s="96" t="s">
+      <c r="C42" s="70" t="s">
         <v>64</v>
       </c>
-      <c r="D42" s="97"/>
+      <c r="D42" s="71"/>
       <c r="E42" s="37"/>
       <c r="N42" s="48" t="s">
         <v>4</v>
@@ -2725,38 +2766,38 @@
       </c>
     </row>
     <row r="44" spans="1:19">
-      <c r="A44" s="117" t="s">
+      <c r="A44" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="B44" s="118"/>
-      <c r="C44" s="118"/>
-      <c r="D44" s="118"/>
-      <c r="E44" s="118"/>
-      <c r="F44" s="118"/>
-      <c r="G44" s="118"/>
-      <c r="H44" s="118"/>
-      <c r="I44" s="118"/>
-      <c r="J44" s="118"/>
-      <c r="K44" s="118"/>
-      <c r="L44" s="118"/>
+      <c r="B44" s="67"/>
+      <c r="C44" s="67"/>
+      <c r="D44" s="67"/>
+      <c r="E44" s="67"/>
+      <c r="F44" s="67"/>
+      <c r="G44" s="67"/>
+      <c r="H44" s="67"/>
+      <c r="I44" s="67"/>
+      <c r="J44" s="67"/>
+      <c r="K44" s="67"/>
+      <c r="L44" s="67"/>
     </row>
     <row r="45" spans="1:19" ht="17.25">
       <c r="A45" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="B45" s="111" t="s">
+      <c r="B45" s="60" t="s">
         <v>55</v>
       </c>
-      <c r="C45" s="111"/>
-      <c r="D45" s="111"/>
-      <c r="E45" s="111"/>
-      <c r="F45" s="111"/>
-      <c r="G45" s="111"/>
-      <c r="H45" s="111"/>
-      <c r="I45" s="111"/>
-      <c r="J45" s="111"/>
-      <c r="K45" s="111"/>
-      <c r="L45" s="111"/>
+      <c r="C45" s="60"/>
+      <c r="D45" s="60"/>
+      <c r="E45" s="60"/>
+      <c r="F45" s="60"/>
+      <c r="G45" s="60"/>
+      <c r="H45" s="60"/>
+      <c r="I45" s="60"/>
+      <c r="J45" s="60"/>
+      <c r="K45" s="60"/>
+      <c r="L45" s="60"/>
       <c r="N45" s="48" t="s">
         <v>92</v>
       </c>
@@ -2768,19 +2809,19 @@
       <c r="A46" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="B46" s="111" t="s">
+      <c r="B46" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="C46" s="111"/>
-      <c r="D46" s="111"/>
-      <c r="E46" s="111"/>
-      <c r="F46" s="111"/>
-      <c r="G46" s="111"/>
-      <c r="H46" s="111"/>
-      <c r="I46" s="111"/>
-      <c r="J46" s="111"/>
-      <c r="K46" s="111"/>
-      <c r="L46" s="111"/>
+      <c r="C46" s="60"/>
+      <c r="D46" s="60"/>
+      <c r="E46" s="60"/>
+      <c r="F46" s="60"/>
+      <c r="G46" s="60"/>
+      <c r="H46" s="60"/>
+      <c r="I46" s="60"/>
+      <c r="J46" s="60"/>
+      <c r="K46" s="60"/>
+      <c r="L46" s="60"/>
       <c r="O46" s="42" t="s">
         <v>96</v>
       </c>
@@ -2789,19 +2830,19 @@
       <c r="A47" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="B47" s="111" t="s">
+      <c r="B47" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="C47" s="111"/>
-      <c r="D47" s="111"/>
-      <c r="E47" s="111"/>
-      <c r="F47" s="111"/>
-      <c r="G47" s="111"/>
-      <c r="H47" s="111"/>
-      <c r="I47" s="111"/>
-      <c r="J47" s="111"/>
-      <c r="K47" s="111"/>
-      <c r="L47" s="111"/>
+      <c r="C47" s="60"/>
+      <c r="D47" s="60"/>
+      <c r="E47" s="60"/>
+      <c r="F47" s="60"/>
+      <c r="G47" s="60"/>
+      <c r="H47" s="60"/>
+      <c r="I47" s="60"/>
+      <c r="J47" s="60"/>
+      <c r="K47" s="60"/>
+      <c r="L47" s="60"/>
       <c r="O47" t="s">
         <v>99</v>
       </c>
@@ -2810,37 +2851,37 @@
       <c r="A48" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="B48" s="111" t="s">
+      <c r="B48" s="60" t="s">
         <v>44</v>
       </c>
-      <c r="C48" s="111"/>
-      <c r="D48" s="111"/>
-      <c r="E48" s="111"/>
-      <c r="F48" s="111"/>
-      <c r="G48" s="111"/>
-      <c r="H48" s="111"/>
-      <c r="I48" s="111"/>
-      <c r="J48" s="111"/>
-      <c r="K48" s="111"/>
-      <c r="L48" s="111"/>
+      <c r="C48" s="60"/>
+      <c r="D48" s="60"/>
+      <c r="E48" s="60"/>
+      <c r="F48" s="60"/>
+      <c r="G48" s="60"/>
+      <c r="H48" s="60"/>
+      <c r="I48" s="60"/>
+      <c r="J48" s="60"/>
+      <c r="K48" s="60"/>
+      <c r="L48" s="60"/>
     </row>
     <row r="49" spans="1:15" ht="17.25">
       <c r="A49" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="B49" s="111" t="s">
+      <c r="B49" s="60" t="s">
         <v>33</v>
       </c>
-      <c r="C49" s="111"/>
-      <c r="D49" s="111"/>
-      <c r="E49" s="111"/>
-      <c r="F49" s="111"/>
-      <c r="G49" s="111"/>
-      <c r="H49" s="111"/>
-      <c r="I49" s="111"/>
-      <c r="J49" s="111"/>
-      <c r="K49" s="111"/>
-      <c r="L49" s="111"/>
+      <c r="C49" s="60"/>
+      <c r="D49" s="60"/>
+      <c r="E49" s="60"/>
+      <c r="F49" s="60"/>
+      <c r="G49" s="60"/>
+      <c r="H49" s="60"/>
+      <c r="I49" s="60"/>
+      <c r="J49" s="60"/>
+      <c r="K49" s="60"/>
+      <c r="L49" s="60"/>
       <c r="N49" s="48" t="s">
         <v>91</v>
       </c>
@@ -2852,19 +2893,19 @@
       <c r="A50" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="B50" s="111" t="s">
+      <c r="B50" s="60" t="s">
         <v>54</v>
       </c>
-      <c r="C50" s="111"/>
-      <c r="D50" s="111"/>
-      <c r="E50" s="111"/>
-      <c r="F50" s="111"/>
-      <c r="G50" s="111"/>
-      <c r="H50" s="111"/>
-      <c r="I50" s="111"/>
-      <c r="J50" s="111"/>
-      <c r="K50" s="111"/>
-      <c r="L50" s="111"/>
+      <c r="C50" s="60"/>
+      <c r="D50" s="60"/>
+      <c r="E50" s="60"/>
+      <c r="F50" s="60"/>
+      <c r="G50" s="60"/>
+      <c r="H50" s="60"/>
+      <c r="I50" s="60"/>
+      <c r="J50" s="60"/>
+      <c r="K50" s="60"/>
+      <c r="L50" s="60"/>
       <c r="O50" t="s">
         <v>97</v>
       </c>
@@ -2873,19 +2914,19 @@
       <c r="A51" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="B51" s="111" t="s">
+      <c r="B51" s="60" t="s">
         <v>53</v>
       </c>
-      <c r="C51" s="111"/>
-      <c r="D51" s="111"/>
-      <c r="E51" s="111"/>
-      <c r="F51" s="111"/>
-      <c r="G51" s="111"/>
-      <c r="H51" s="111"/>
-      <c r="I51" s="111"/>
-      <c r="J51" s="111"/>
-      <c r="K51" s="111"/>
-      <c r="L51" s="111"/>
+      <c r="C51" s="60"/>
+      <c r="D51" s="60"/>
+      <c r="E51" s="60"/>
+      <c r="F51" s="60"/>
+      <c r="G51" s="60"/>
+      <c r="H51" s="60"/>
+      <c r="I51" s="60"/>
+      <c r="J51" s="60"/>
+      <c r="K51" s="60"/>
+      <c r="L51" s="60"/>
       <c r="O51" t="s">
         <v>98</v>
       </c>
@@ -2903,24 +2944,37 @@
   <sortState ref="A24:K25">
     <sortCondition ref="A3"/>
   </sortState>
-  <mergeCells count="56">
-    <mergeCell ref="N28:S28"/>
-    <mergeCell ref="N39:S39"/>
-    <mergeCell ref="N32:S32"/>
-    <mergeCell ref="N35:S35"/>
-    <mergeCell ref="N30:S30"/>
-    <mergeCell ref="N37:S37"/>
-    <mergeCell ref="B50:L50"/>
-    <mergeCell ref="B51:L51"/>
-    <mergeCell ref="A39:E39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="B45:L45"/>
-    <mergeCell ref="A44:L44"/>
-    <mergeCell ref="B46:L46"/>
-    <mergeCell ref="B47:L47"/>
-    <mergeCell ref="B48:L48"/>
-    <mergeCell ref="B49:L49"/>
+  <mergeCells count="60">
+    <mergeCell ref="N38:S38"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="H28:K28"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="O6:U6"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="H27:K27"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="N24:S24"/>
+    <mergeCell ref="N27:S27"/>
+    <mergeCell ref="N20:S20"/>
+    <mergeCell ref="O14:S15"/>
+    <mergeCell ref="N22:S22"/>
+    <mergeCell ref="N19:S19"/>
+    <mergeCell ref="N17:S17"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="H30:K30"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="H32:K32"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="H31:L31"/>
     <mergeCell ref="A35:B35"/>
     <mergeCell ref="A36:B36"/>
     <mergeCell ref="A37:B37"/>
@@ -2933,33 +2987,24 @@
     <mergeCell ref="C35:G35"/>
     <mergeCell ref="C36:G36"/>
     <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="H30:K30"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="H32:K32"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="H31:L31"/>
-    <mergeCell ref="O6:U6"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="H27:K27"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="N24:S24"/>
-    <mergeCell ref="N27:S27"/>
-    <mergeCell ref="N20:S20"/>
-    <mergeCell ref="O14:S15"/>
-    <mergeCell ref="N22:S22"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="H28:K28"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="B50:L50"/>
+    <mergeCell ref="B51:L51"/>
+    <mergeCell ref="A39:E39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="B45:L45"/>
+    <mergeCell ref="A44:L44"/>
+    <mergeCell ref="B46:L46"/>
+    <mergeCell ref="B47:L47"/>
+    <mergeCell ref="B48:L48"/>
+    <mergeCell ref="B49:L49"/>
+    <mergeCell ref="N28:S28"/>
+    <mergeCell ref="N16:S16"/>
+    <mergeCell ref="N31:S31"/>
+    <mergeCell ref="N37:S37"/>
+    <mergeCell ref="N30:S30"/>
+    <mergeCell ref="N25:S25"/>
+    <mergeCell ref="N33:S33"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="Q4" r:id="rId1"/>

</xml_diff>

<commit_message>
problemas con git por el cuadro de datos
</commit_message>
<xml_diff>
--- a/Cuadro-de-estado.xlsx
+++ b/Cuadro-de-estado.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="129">
   <si>
     <t>BACKEND</t>
   </si>
@@ -301,6 +301,12 @@
     <t>Postergados/Pendientes importantes</t>
   </si>
   <si>
+    <t>Upload files</t>
+  </si>
+  <si>
+    <t>https://blog.angular-university.io/angular-file-upload/</t>
+  </si>
+  <si>
     <t>Layout</t>
   </si>
   <si>
@@ -436,6 +442,9 @@
     <t>Completando</t>
   </si>
   <si>
+    <t>OJO CON LOS GET HTTP, que no hayan desparramados o dobles llamadas</t>
+  </si>
+  <si>
     <t>Independencia y motivación</t>
   </si>
   <si>
@@ -466,13 +475,19 @@
     <t>Hagamos algo especial.</t>
   </si>
   <si>
-    <t>1:0</t>
-  </si>
-  <si>
-    <t>googlemaps?</t>
-  </si>
-  <si>
-    <t>reemplazar los Alert( y algunos console.log()) por snack-bar notifications</t>
+    <t>En SOFTSKILL form, inicializa mal el range</t>
+  </si>
+  <si>
+    <t>OJO EN LOS FORM. SIN NO HAY CAMBIOS QUE NO VAYA AL HTTP</t>
+  </si>
+  <si>
+    <t>Variables temporales, que sean de los metodos, no de la clase</t>
+  </si>
+  <si>
+    <t>LOS FORM TIENEN ALGO MAL CON LAS VALIDACIONES, AL INICIAR</t>
+  </si>
+  <si>
+    <t>Estudios y trabajos, da repetido el nombre cuando modifico cualquier otro dato</t>
   </si>
 </sst>
 </file>
@@ -695,7 +710,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -746,6 +761,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -753,12 +774,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -774,6 +789,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="38">
     <border>
@@ -1251,7 +1272,7 @@
     </xf>
     <xf numFmtId="43" fontId="23" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="122">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1289,7 +1310,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1310,6 +1334,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -1320,10 +1347,10 @@
     <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1357,182 +1384,177 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1543,22 +1565,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="2" borderId="19" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1862,8 +1878,8 @@
   </sheetPr>
   <dimension ref="A1:U54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="N26" sqref="N26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1880,62 +1896,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25">
-      <c r="A1" s="103" t="s">
-        <v>82</v>
-      </c>
-      <c r="B1" s="103"/>
-      <c r="C1" s="103"/>
-      <c r="D1" s="103"/>
-      <c r="E1" s="103"/>
-      <c r="F1" s="103"/>
-      <c r="G1" s="103"/>
-      <c r="H1" s="103"/>
-      <c r="I1" s="103"/>
-      <c r="J1" s="103"/>
-      <c r="K1" s="103"/>
-      <c r="L1" s="103"/>
+      <c r="A1" s="101" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="101"/>
+      <c r="C1" s="101"/>
+      <c r="D1" s="101"/>
+      <c r="E1" s="101"/>
+      <c r="F1" s="101"/>
+      <c r="G1" s="101"/>
+      <c r="H1" s="101"/>
+      <c r="I1" s="101"/>
+      <c r="J1" s="101"/>
+      <c r="K1" s="101"/>
+      <c r="L1" s="101"/>
     </row>
     <row r="2" spans="1:21" ht="19.5" thickBot="1">
-      <c r="A2" s="42">
+      <c r="A2" s="44">
         <f ca="1">M2-TODAY()-1</f>
-        <v>19</v>
-      </c>
-      <c r="B2" s="43" t="s">
-        <v>83</v>
-      </c>
-      <c r="C2" s="44"/>
-      <c r="M2" s="41">
+        <v>17</v>
+      </c>
+      <c r="B2" s="45" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" s="46"/>
+      <c r="M2" s="43">
         <v>45011</v>
       </c>
-      <c r="O2" s="40" t="s">
-        <v>79</v>
+      <c r="O2" s="42" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="104" t="s">
+      <c r="A3" s="102" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="105"/>
-      <c r="C3" s="106" t="s">
+      <c r="B3" s="103"/>
+      <c r="C3" s="104" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="107"/>
-      <c r="E3" s="107"/>
-      <c r="F3" s="107"/>
-      <c r="G3" s="108"/>
-      <c r="H3" s="106" t="s">
+      <c r="D3" s="105"/>
+      <c r="E3" s="105"/>
+      <c r="F3" s="105"/>
+      <c r="G3" s="106"/>
+      <c r="H3" s="104" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="107"/>
-      <c r="J3" s="109"/>
-      <c r="K3" s="108"/>
-      <c r="L3" s="19" t="s">
+      <c r="I3" s="105"/>
+      <c r="J3" s="107"/>
+      <c r="K3" s="106"/>
+      <c r="L3" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="110" t="s">
-        <v>74</v>
-      </c>
-      <c r="N3" s="102"/>
+      <c r="M3" s="108" t="s">
+        <v>76</v>
+      </c>
+      <c r="N3" s="100"/>
     </row>
     <row r="4" spans="1:21" s="3" customFormat="1" ht="40.5" customHeight="1" thickBot="1">
       <c r="A4" s="17" t="s">
@@ -1974,83 +1990,81 @@
       <c r="L4" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="M4" s="111" t="s">
-        <v>75</v>
-      </c>
-      <c r="N4" s="112"/>
-      <c r="O4" s="32" t="s">
+      <c r="M4" s="109" t="s">
+        <v>77</v>
+      </c>
+      <c r="N4" s="110"/>
+      <c r="O4" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="Q4" s="33" t="s">
+      <c r="Q4" s="35" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="4.5" customHeight="1">
-      <c r="A5" s="27"/>
-      <c r="B5" s="28"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="29"/>
-      <c r="J5" s="29"/>
-      <c r="K5" s="29"/>
-      <c r="L5" s="29"/>
+      <c r="A5" s="28"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="30"/>
+      <c r="K5" s="30"/>
+      <c r="L5" s="30"/>
     </row>
     <row r="6" spans="1:21">
       <c r="A6" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="38"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="40"/>
       <c r="E6" s="4"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="4"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="57"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
-      <c r="O6" s="101" t="s">
+      <c r="O6" s="99" t="s">
         <v>65</v>
       </c>
-      <c r="P6" s="102"/>
-      <c r="Q6" s="102"/>
-      <c r="R6" s="102"/>
-      <c r="S6" s="102"/>
-      <c r="T6" s="102"/>
-      <c r="U6" s="102"/>
+      <c r="P6" s="100"/>
+      <c r="Q6" s="100"/>
+      <c r="R6" s="100"/>
+      <c r="S6" s="100"/>
+      <c r="T6" s="100"/>
+      <c r="U6" s="100"/>
     </row>
     <row r="7" spans="1:21" ht="4.5" customHeight="1">
-      <c r="A7" s="27"/>
-      <c r="B7" s="28"/>
-      <c r="C7" s="29"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="29"/>
-      <c r="H7" s="29"/>
-      <c r="I7" s="29"/>
-      <c r="J7" s="29"/>
-      <c r="K7" s="29"/>
-      <c r="L7" s="29"/>
+      <c r="A7" s="28"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="30"/>
+      <c r="I7" s="30"/>
+      <c r="J7" s="30"/>
+      <c r="K7" s="30"/>
+      <c r="L7" s="30"/>
     </row>
     <row r="8" spans="1:21">
       <c r="A8" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="24" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="4"/>
-      <c r="D8" s="38"/>
+      <c r="D8" s="40"/>
       <c r="E8" s="4"/>
-      <c r="F8" s="38"/>
+      <c r="F8" s="40"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
@@ -2058,39 +2072,49 @@
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
       <c r="O8" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="P8" s="6"/>
+        <v>66</v>
+      </c>
+      <c r="P8" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="6"/>
+      <c r="T8" s="6"/>
     </row>
     <row r="9" spans="1:21">
-      <c r="A9" s="25" t="s">
+      <c r="A9" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="24" t="s">
         <v>12</v>
       </c>
       <c r="C9" s="4"/>
-      <c r="D9" s="38"/>
+      <c r="D9" s="40"/>
       <c r="E9" s="4"/>
-      <c r="F9" s="38"/>
+      <c r="F9" s="40"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
+      <c r="P9" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q9" s="6"/>
     </row>
     <row r="10" spans="1:21">
       <c r="A10" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="24" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="4"/>
-      <c r="D10" s="38"/>
+      <c r="D10" s="40"/>
       <c r="E10" s="4"/>
-      <c r="F10" s="38"/>
+      <c r="F10" s="40"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
@@ -2098,20 +2122,20 @@
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
       <c r="O10" t="s">
-        <v>122</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:21">
       <c r="A11" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="24" t="s">
         <v>12</v>
       </c>
       <c r="C11" s="4"/>
-      <c r="D11" s="38"/>
+      <c r="D11" s="40"/>
       <c r="E11" s="4"/>
-      <c r="F11" s="38"/>
+      <c r="F11" s="40"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
@@ -2120,214 +2144,233 @@
       <c r="L11" s="4"/>
     </row>
     <row r="12" spans="1:21" ht="4.5" customHeight="1">
-      <c r="A12" s="27"/>
-      <c r="B12" s="27"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="27"/>
-      <c r="I12" s="27"/>
-      <c r="J12" s="27"/>
-      <c r="K12" s="27"/>
-      <c r="L12" s="27"/>
+      <c r="A12" s="28"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="28"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="28"/>
     </row>
     <row r="13" spans="1:21">
-      <c r="A13" s="36" t="s">
+      <c r="A13" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="23" t="s">
+      <c r="B13" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="20"/>
-      <c r="D13" s="38"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="38"/>
-      <c r="G13" s="4"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="40"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
-      <c r="K13" s="52"/>
+      <c r="K13" s="54"/>
       <c r="L13" s="4"/>
       <c r="O13" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="P13" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="15" customHeight="1">
-      <c r="A14" s="36" t="s">
+      <c r="A14" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="20"/>
-      <c r="D14" s="38"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="4"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="40"/>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
-      <c r="K14" s="52"/>
+      <c r="K14" s="54"/>
       <c r="L14" s="4"/>
-      <c r="O14" s="113" t="s">
-        <v>73</v>
-      </c>
-      <c r="P14" s="113"/>
-      <c r="Q14" s="113"/>
-      <c r="R14" s="113"/>
-      <c r="S14" s="113"/>
+      <c r="O14" s="112" t="s">
+        <v>75</v>
+      </c>
+      <c r="P14" s="112"/>
+      <c r="Q14" s="112"/>
+      <c r="R14" s="112"/>
+      <c r="S14" s="112"/>
     </row>
     <row r="15" spans="1:21" ht="15" customHeight="1">
-      <c r="A15" s="36" t="s">
+      <c r="A15" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="20"/>
-      <c r="D15" s="38"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="38"/>
-      <c r="G15" s="4"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="40"/>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
-      <c r="K15" s="52"/>
+      <c r="K15" s="54"/>
       <c r="L15" s="4"/>
-      <c r="O15" s="113"/>
-      <c r="P15" s="113"/>
-      <c r="Q15" s="113"/>
-      <c r="R15" s="113"/>
-      <c r="S15" s="113"/>
-      <c r="T15" s="51"/>
+      <c r="O15" s="112"/>
+      <c r="P15" s="112"/>
+      <c r="Q15" s="112"/>
+      <c r="R15" s="112"/>
+      <c r="S15" s="112"/>
+      <c r="T15" s="53"/>
     </row>
     <row r="16" spans="1:21">
       <c r="A16" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="23" t="s">
+      <c r="B16" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="20"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="52"/>
-      <c r="G16" s="4"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="54"/>
+      <c r="G16" s="40"/>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
       <c r="L16" s="4"/>
-      <c r="T16" s="51"/>
+      <c r="N16" s="111" t="s">
+        <v>110</v>
+      </c>
+      <c r="O16" s="111"/>
+      <c r="P16" s="111"/>
+      <c r="Q16" s="111"/>
+      <c r="R16" s="111"/>
+      <c r="S16" s="111"/>
+      <c r="T16" s="53"/>
     </row>
     <row r="17" spans="1:19">
       <c r="A17" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="B17" s="23" t="s">
+      <c r="B17" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="20"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="52"/>
-      <c r="G17" s="4"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="54"/>
+      <c r="G17" s="40"/>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
       <c r="L17" s="4"/>
-      <c r="O17" t="s">
-        <v>68</v>
-      </c>
+      <c r="N17" s="111" t="s">
+        <v>127</v>
+      </c>
+      <c r="O17" s="111"/>
+      <c r="P17" s="111"/>
+      <c r="Q17" s="111"/>
+      <c r="R17" s="111"/>
+      <c r="S17" s="111"/>
     </row>
     <row r="18" spans="1:19" ht="4.5" customHeight="1">
-      <c r="A18" s="27"/>
-      <c r="B18" s="28"/>
-      <c r="C18" s="29"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="29"/>
-      <c r="F18" s="29"/>
-      <c r="G18" s="29"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
-      <c r="K18" s="29"/>
-      <c r="L18" s="29"/>
+      <c r="A18" s="28"/>
+      <c r="B18" s="29"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="30"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="30"/>
+      <c r="J18" s="30"/>
+      <c r="K18" s="30"/>
+      <c r="L18" s="30"/>
     </row>
     <row r="19" spans="1:19">
-      <c r="A19" s="37" t="s">
+      <c r="A19" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="23" t="s">
+      <c r="B19" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="21"/>
-      <c r="D19" s="39"/>
-      <c r="E19" s="52"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="54"/>
       <c r="F19" s="8"/>
       <c r="G19" s="7"/>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
       <c r="K19" s="7"/>
-      <c r="L19" s="50"/>
+      <c r="L19" s="52"/>
+      <c r="N19" s="111" t="s">
+        <v>125</v>
+      </c>
+      <c r="O19" s="111"/>
+      <c r="P19" s="111"/>
+      <c r="Q19" s="111"/>
+      <c r="R19" s="111"/>
+      <c r="S19" s="111"/>
     </row>
     <row r="20" spans="1:19">
-      <c r="A20" s="37" t="s">
+      <c r="A20" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="23" t="s">
+      <c r="B20" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="21"/>
-      <c r="D20" s="39"/>
-      <c r="E20" s="52"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="54"/>
       <c r="F20" s="8"/>
       <c r="G20" s="7"/>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
       <c r="K20" s="7"/>
-      <c r="L20" s="50"/>
-      <c r="N20" s="56" t="s">
-        <v>76</v>
-      </c>
-      <c r="O20" s="56"/>
-      <c r="P20" s="56"/>
-      <c r="Q20" s="56"/>
-      <c r="R20" s="56"/>
-      <c r="S20" s="56"/>
+      <c r="L20" s="52"/>
+      <c r="N20" s="111" t="s">
+        <v>113</v>
+      </c>
+      <c r="O20" s="111"/>
+      <c r="P20" s="111"/>
+      <c r="Q20" s="111"/>
+      <c r="R20" s="111"/>
+      <c r="S20" s="111"/>
     </row>
     <row r="21" spans="1:19" ht="4.5" customHeight="1">
-      <c r="A21" s="27"/>
-      <c r="B21" s="28"/>
-      <c r="C21" s="29"/>
-      <c r="D21" s="29"/>
-      <c r="E21" s="29"/>
-      <c r="F21" s="29"/>
-      <c r="G21" s="29"/>
-      <c r="H21" s="29"/>
-      <c r="I21" s="29"/>
-      <c r="J21" s="29"/>
-      <c r="K21" s="29"/>
-      <c r="L21" s="29"/>
+      <c r="A21" s="28"/>
+      <c r="B21" s="29"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="30"/>
+      <c r="I21" s="30"/>
+      <c r="J21" s="30"/>
+      <c r="K21" s="30"/>
+      <c r="L21" s="30"/>
     </row>
     <row r="22" spans="1:19">
-      <c r="A22" s="37" t="s">
+      <c r="A22" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="B22" s="119" t="s">
-        <v>121</v>
-      </c>
+      <c r="B22" s="19"/>
       <c r="C22" s="16"/>
       <c r="D22" s="8"/>
-      <c r="E22" s="52"/>
+      <c r="E22" s="54"/>
       <c r="F22" s="8"/>
       <c r="G22" s="4"/>
       <c r="H22" s="5"/>
@@ -2335,39 +2378,37 @@
       <c r="J22" s="5"/>
       <c r="K22" s="7"/>
       <c r="L22" s="4"/>
-      <c r="N22" s="56" t="s">
-        <v>81</v>
-      </c>
-      <c r="O22" s="56"/>
-      <c r="P22" s="56"/>
-      <c r="Q22" s="56"/>
-      <c r="R22" s="56"/>
-      <c r="S22" s="56"/>
+      <c r="N22" s="111" t="s">
+        <v>124</v>
+      </c>
+      <c r="O22" s="111"/>
+      <c r="P22" s="111"/>
+      <c r="Q22" s="111"/>
+      <c r="R22" s="111"/>
+      <c r="S22" s="111"/>
     </row>
     <row r="23" spans="1:19" ht="4.5" customHeight="1">
-      <c r="A23" s="27"/>
-      <c r="B23" s="28"/>
-      <c r="C23" s="29"/>
-      <c r="D23" s="29"/>
-      <c r="E23" s="29"/>
-      <c r="F23" s="29"/>
-      <c r="G23" s="29"/>
-      <c r="H23" s="29"/>
-      <c r="I23" s="29"/>
-      <c r="J23" s="29"/>
-      <c r="K23" s="29"/>
-      <c r="L23" s="29"/>
+      <c r="A23" s="28"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="30"/>
+      <c r="G23" s="30"/>
+      <c r="H23" s="30"/>
+      <c r="I23" s="30"/>
+      <c r="J23" s="30"/>
+      <c r="K23" s="30"/>
+      <c r="L23" s="30"/>
     </row>
     <row r="24" spans="1:19">
-      <c r="A24" s="37" t="s">
+      <c r="A24" s="39" t="s">
         <v>48</v>
       </c>
-      <c r="B24" s="119" t="s">
-        <v>121</v>
-      </c>
+      <c r="B24" s="31"/>
       <c r="C24" s="8"/>
       <c r="D24" s="5"/>
-      <c r="E24" s="52"/>
+      <c r="E24" s="54"/>
       <c r="F24" s="8"/>
       <c r="G24" s="7"/>
       <c r="H24" s="5"/>
@@ -2375,17 +2416,25 @@
       <c r="J24" s="5"/>
       <c r="K24" s="7"/>
       <c r="L24" s="4"/>
+      <c r="N24" s="111" t="s">
+        <v>83</v>
+      </c>
+      <c r="O24" s="111"/>
+      <c r="P24" s="111"/>
+      <c r="Q24" s="111"/>
+      <c r="R24" s="111"/>
+      <c r="S24" s="111"/>
     </row>
     <row r="25" spans="1:19">
-      <c r="A25" s="37" t="s">
+      <c r="A25" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="B25" s="23" t="s">
+      <c r="B25" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C25" s="21"/>
+      <c r="C25" s="22"/>
       <c r="D25" s="8"/>
-      <c r="E25" s="52"/>
+      <c r="E25" s="54"/>
       <c r="F25" s="8"/>
       <c r="G25" s="8"/>
       <c r="H25" s="5"/>
@@ -2393,504 +2442,522 @@
       <c r="J25" s="5"/>
       <c r="K25" s="7"/>
       <c r="L25" s="4"/>
-      <c r="N25" s="56" t="s">
-        <v>123</v>
-      </c>
-      <c r="O25" s="56"/>
-      <c r="P25" s="56"/>
-      <c r="Q25" s="56"/>
-      <c r="R25" s="56"/>
-      <c r="S25" s="56"/>
+      <c r="N25" s="111" t="s">
+        <v>82</v>
+      </c>
+      <c r="O25" s="111"/>
+      <c r="P25" s="111"/>
+      <c r="Q25" s="111"/>
+      <c r="R25" s="111"/>
+      <c r="S25" s="111"/>
     </row>
     <row r="26" spans="1:19" ht="4.5" customHeight="1" thickBot="1">
-      <c r="A26" s="27"/>
-      <c r="B26" s="28"/>
-      <c r="C26" s="29"/>
-      <c r="D26" s="29"/>
-      <c r="E26" s="29"/>
-      <c r="F26" s="29"/>
-      <c r="G26" s="29"/>
-      <c r="H26" s="29"/>
-      <c r="I26" s="29"/>
-      <c r="J26" s="29"/>
-      <c r="K26" s="29"/>
-      <c r="L26" s="29"/>
+      <c r="A26" s="28"/>
+      <c r="B26" s="29"/>
+      <c r="C26" s="30"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="30"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="30"/>
+      <c r="I26" s="30"/>
+      <c r="J26" s="30"/>
+      <c r="K26" s="30"/>
+      <c r="L26" s="30"/>
     </row>
     <row r="27" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A27" s="22"/>
-      <c r="B27" s="24"/>
-      <c r="C27" s="106" t="s">
+      <c r="A27" s="23"/>
+      <c r="B27" s="25"/>
+      <c r="C27" s="104" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="107"/>
-      <c r="E27" s="107"/>
-      <c r="F27" s="107"/>
-      <c r="G27" s="108"/>
-      <c r="H27" s="106" t="s">
+      <c r="D27" s="105"/>
+      <c r="E27" s="105"/>
+      <c r="F27" s="105"/>
+      <c r="G27" s="106"/>
+      <c r="H27" s="104" t="s">
         <v>0</v>
       </c>
-      <c r="I27" s="107"/>
-      <c r="J27" s="109"/>
-      <c r="K27" s="108"/>
-      <c r="L27" s="19" t="s">
+      <c r="I27" s="105"/>
+      <c r="J27" s="107"/>
+      <c r="K27" s="106"/>
+      <c r="L27" s="20" t="s">
         <v>4</v>
       </c>
+      <c r="N27" s="111" t="s">
+        <v>78</v>
+      </c>
+      <c r="O27" s="111"/>
+      <c r="P27" s="111"/>
+      <c r="Q27" s="111"/>
+      <c r="R27" s="111"/>
+      <c r="S27" s="111"/>
     </row>
     <row r="28" spans="1:19" ht="30">
-      <c r="A28" s="117" t="s">
+      <c r="A28" s="97" t="s">
         <v>29</v>
       </c>
-      <c r="B28" s="118"/>
-      <c r="C28" s="95" t="s">
+      <c r="B28" s="98"/>
+      <c r="C28" s="91" t="s">
+        <v>88</v>
+      </c>
+      <c r="D28" s="92"/>
+      <c r="E28" s="92"/>
+      <c r="F28" s="92"/>
+      <c r="G28" s="93"/>
+      <c r="H28" s="115" t="s">
         <v>86</v>
       </c>
-      <c r="D28" s="96"/>
-      <c r="E28" s="96"/>
-      <c r="F28" s="96"/>
-      <c r="G28" s="97"/>
-      <c r="H28" s="114" t="s">
-        <v>84</v>
-      </c>
-      <c r="I28" s="115"/>
-      <c r="J28" s="115"/>
-      <c r="K28" s="116"/>
-      <c r="L28" s="45" t="s">
-        <v>85</v>
-      </c>
-      <c r="N28" s="55" t="s">
-        <v>109</v>
-      </c>
-      <c r="O28" s="55"/>
-      <c r="P28" s="55"/>
-      <c r="Q28" s="55"/>
-      <c r="R28" s="55"/>
-      <c r="S28" s="55"/>
+      <c r="I28" s="116"/>
+      <c r="J28" s="116"/>
+      <c r="K28" s="117"/>
+      <c r="L28" s="47" t="s">
+        <v>87</v>
+      </c>
+      <c r="N28" s="113" t="s">
+        <v>111</v>
+      </c>
+      <c r="O28" s="113"/>
+      <c r="P28" s="113"/>
+      <c r="Q28" s="113"/>
+      <c r="R28" s="113"/>
+      <c r="S28" s="113"/>
     </row>
     <row r="29" spans="1:19" ht="4.5" customHeight="1">
-      <c r="A29" s="27"/>
-      <c r="B29" s="28"/>
-      <c r="C29" s="29"/>
-      <c r="D29" s="29"/>
-      <c r="E29" s="29"/>
-      <c r="F29" s="29"/>
-      <c r="G29" s="29"/>
-      <c r="H29" s="29"/>
-      <c r="I29" s="29"/>
-      <c r="J29" s="29"/>
-      <c r="K29" s="29"/>
-      <c r="L29" s="29"/>
+      <c r="A29" s="28"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="30"/>
+      <c r="G29" s="30"/>
+      <c r="H29" s="30"/>
+      <c r="I29" s="30"/>
+      <c r="J29" s="30"/>
+      <c r="K29" s="30"/>
+      <c r="L29" s="30"/>
     </row>
     <row r="30" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A30" s="67" t="s">
+      <c r="A30" s="66" t="s">
         <v>38</v>
       </c>
-      <c r="B30" s="68"/>
-      <c r="C30" s="85"/>
-      <c r="D30" s="86"/>
-      <c r="E30" s="86"/>
-      <c r="F30" s="86"/>
-      <c r="G30" s="87"/>
-      <c r="H30" s="88"/>
-      <c r="I30" s="86"/>
-      <c r="J30" s="86"/>
-      <c r="K30" s="87"/>
-      <c r="L30" s="20" t="s">
+      <c r="B30" s="67"/>
+      <c r="C30" s="118"/>
+      <c r="D30" s="119"/>
+      <c r="E30" s="119"/>
+      <c r="F30" s="119"/>
+      <c r="G30" s="120"/>
+      <c r="H30" s="121"/>
+      <c r="I30" s="119"/>
+      <c r="J30" s="119"/>
+      <c r="K30" s="120"/>
+      <c r="L30" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="M30" s="30"/>
-      <c r="N30" s="58" t="s">
-        <v>70</v>
-      </c>
-      <c r="O30" s="58"/>
-      <c r="P30" s="58"/>
-      <c r="Q30" s="58"/>
-      <c r="R30" s="58"/>
-      <c r="S30" s="58"/>
+      <c r="M30" s="32"/>
+      <c r="N30" s="111" t="s">
+        <v>72</v>
+      </c>
+      <c r="O30" s="111"/>
+      <c r="P30" s="111"/>
+      <c r="Q30" s="111"/>
+      <c r="R30" s="111"/>
+      <c r="S30" s="111"/>
     </row>
     <row r="31" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A31" s="67" t="s">
-        <v>77</v>
-      </c>
-      <c r="B31" s="68"/>
-      <c r="C31" s="95"/>
-      <c r="D31" s="96"/>
-      <c r="E31" s="96"/>
-      <c r="F31" s="96"/>
-      <c r="G31" s="97"/>
-      <c r="H31" s="98" t="s">
-        <v>78</v>
-      </c>
-      <c r="I31" s="99"/>
-      <c r="J31" s="99"/>
-      <c r="K31" s="99"/>
-      <c r="L31" s="100"/>
-      <c r="M31" s="30"/>
+      <c r="A31" s="66" t="s">
+        <v>79</v>
+      </c>
+      <c r="B31" s="67"/>
+      <c r="C31" s="91"/>
+      <c r="D31" s="92"/>
+      <c r="E31" s="92"/>
+      <c r="F31" s="92"/>
+      <c r="G31" s="93"/>
+      <c r="H31" s="94" t="s">
+        <v>80</v>
+      </c>
+      <c r="I31" s="95"/>
+      <c r="J31" s="95"/>
+      <c r="K31" s="95"/>
+      <c r="L31" s="96"/>
+      <c r="M31" s="32"/>
+      <c r="N31" s="113" t="s">
+        <v>73</v>
+      </c>
+      <c r="O31" s="113"/>
+      <c r="P31" s="113"/>
+      <c r="Q31" s="113"/>
+      <c r="R31" s="113"/>
+      <c r="S31" s="113"/>
     </row>
     <row r="32" spans="1:19" ht="16.5" thickBot="1">
-      <c r="A32" s="91" t="s">
+      <c r="A32" s="87" t="s">
         <v>59</v>
       </c>
-      <c r="B32" s="92"/>
-      <c r="C32" s="83"/>
-      <c r="D32" s="84"/>
-      <c r="E32" s="84"/>
-      <c r="F32" s="84"/>
-      <c r="G32" s="93"/>
-      <c r="H32" s="94"/>
-      <c r="I32" s="84"/>
-      <c r="J32" s="84"/>
-      <c r="K32" s="93"/>
-      <c r="M32" s="30"/>
-      <c r="N32" s="57" t="s">
-        <v>71</v>
-      </c>
-      <c r="O32" s="57"/>
-      <c r="P32" s="57"/>
-      <c r="Q32" s="57"/>
-      <c r="R32" s="57"/>
-      <c r="S32" s="57"/>
+      <c r="B32" s="88"/>
+      <c r="C32" s="82"/>
+      <c r="D32" s="83"/>
+      <c r="E32" s="83"/>
+      <c r="F32" s="83"/>
+      <c r="G32" s="89"/>
+      <c r="H32" s="90"/>
+      <c r="I32" s="83"/>
+      <c r="J32" s="83"/>
+      <c r="K32" s="89"/>
+      <c r="M32" s="32"/>
     </row>
     <row r="33" spans="1:19" ht="30.75" customHeight="1" thickBot="1">
-      <c r="A33" s="89" t="s">
+      <c r="A33" s="85" t="s">
         <v>34</v>
       </c>
-      <c r="B33" s="90"/>
-      <c r="C33" s="74" t="s">
+      <c r="B33" s="86"/>
+      <c r="C33" s="73" t="s">
         <v>58</v>
       </c>
-      <c r="D33" s="75"/>
-      <c r="E33" s="75"/>
-      <c r="F33" s="75"/>
-      <c r="G33" s="76"/>
-      <c r="H33" s="71"/>
-      <c r="I33" s="72"/>
-      <c r="J33" s="72"/>
-      <c r="K33" s="73"/>
-      <c r="M33" s="30"/>
+      <c r="D33" s="74"/>
+      <c r="E33" s="74"/>
+      <c r="F33" s="74"/>
+      <c r="G33" s="75"/>
+      <c r="H33" s="70"/>
+      <c r="I33" s="71"/>
+      <c r="J33" s="71"/>
+      <c r="K33" s="72"/>
+      <c r="M33" s="32"/>
+      <c r="N33" s="113" t="s">
+        <v>126</v>
+      </c>
+      <c r="O33" s="113"/>
+      <c r="P33" s="113"/>
+      <c r="Q33" s="113"/>
+      <c r="R33" s="113"/>
+      <c r="S33" s="113"/>
     </row>
     <row r="34" spans="1:19" ht="4.5" customHeight="1" thickBot="1">
-      <c r="A34" s="27"/>
-      <c r="B34" s="28"/>
-      <c r="C34" s="34"/>
-      <c r="D34" s="34"/>
-      <c r="E34" s="34"/>
-      <c r="F34" s="34"/>
-      <c r="G34" s="34"/>
-      <c r="H34" s="29"/>
-      <c r="I34" s="29"/>
-      <c r="J34" s="29"/>
-      <c r="K34" s="29"/>
+      <c r="A34" s="28"/>
+      <c r="B34" s="29"/>
+      <c r="C34" s="36"/>
+      <c r="D34" s="36"/>
+      <c r="E34" s="36"/>
+      <c r="F34" s="36"/>
+      <c r="G34" s="36"/>
+      <c r="H34" s="30"/>
+      <c r="I34" s="30"/>
+      <c r="J34" s="30"/>
+      <c r="K34" s="30"/>
     </row>
     <row r="35" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A35" s="67" t="s">
+      <c r="A35" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="68"/>
-      <c r="C35" s="120"/>
-      <c r="D35" s="121"/>
-      <c r="E35" s="121"/>
-      <c r="F35" s="121"/>
-      <c r="G35" s="122"/>
-      <c r="H35" s="77"/>
-      <c r="I35" s="78"/>
-      <c r="J35" s="78"/>
-      <c r="K35" s="79"/>
-      <c r="M35" s="30"/>
-      <c r="N35" s="58" t="s">
-        <v>72</v>
-      </c>
-      <c r="O35" s="58"/>
-      <c r="P35" s="58"/>
-      <c r="Q35" s="58"/>
-      <c r="R35" s="58"/>
-      <c r="S35" s="58"/>
+      <c r="B35" s="67"/>
+      <c r="C35" s="82"/>
+      <c r="D35" s="83"/>
+      <c r="E35" s="83"/>
+      <c r="F35" s="83"/>
+      <c r="G35" s="84"/>
+      <c r="H35" s="76"/>
+      <c r="I35" s="77"/>
+      <c r="J35" s="77"/>
+      <c r="K35" s="78"/>
+      <c r="M35" s="32"/>
     </row>
     <row r="36" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A36" s="67" t="s">
-        <v>87</v>
-      </c>
-      <c r="B36" s="68"/>
-      <c r="C36" s="120"/>
-      <c r="D36" s="121"/>
-      <c r="E36" s="121"/>
-      <c r="F36" s="121"/>
-      <c r="G36" s="122"/>
-      <c r="H36" s="77"/>
-      <c r="I36" s="78"/>
-      <c r="J36" s="78"/>
-      <c r="K36" s="79"/>
-      <c r="M36" s="30"/>
+      <c r="A36" s="66" t="s">
+        <v>89</v>
+      </c>
+      <c r="B36" s="67"/>
+      <c r="C36" s="82"/>
+      <c r="D36" s="83"/>
+      <c r="E36" s="83"/>
+      <c r="F36" s="83"/>
+      <c r="G36" s="84"/>
+      <c r="H36" s="76"/>
+      <c r="I36" s="77"/>
+      <c r="J36" s="77"/>
+      <c r="K36" s="78"/>
+      <c r="M36" s="32"/>
     </row>
     <row r="37" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A37" s="67" t="s">
+      <c r="A37" s="66" t="s">
         <v>7</v>
       </c>
-      <c r="B37" s="68"/>
-      <c r="C37" s="80"/>
-      <c r="D37" s="81"/>
-      <c r="E37" s="81"/>
-      <c r="F37" s="81"/>
-      <c r="G37" s="82"/>
-      <c r="H37" s="80"/>
-      <c r="I37" s="81"/>
-      <c r="J37" s="81"/>
-      <c r="K37" s="82"/>
-      <c r="M37" s="30"/>
-      <c r="N37" s="56" t="s">
-        <v>80</v>
-      </c>
-      <c r="O37" s="56"/>
-      <c r="P37" s="56"/>
-      <c r="Q37" s="56"/>
-      <c r="R37" s="56"/>
-      <c r="S37" s="56"/>
-    </row>
-    <row r="38" spans="1:19" ht="15.75" thickBot="1"/>
+      <c r="B37" s="67"/>
+      <c r="C37" s="79"/>
+      <c r="D37" s="80"/>
+      <c r="E37" s="80"/>
+      <c r="F37" s="80"/>
+      <c r="G37" s="81"/>
+      <c r="H37" s="79"/>
+      <c r="I37" s="80"/>
+      <c r="J37" s="80"/>
+      <c r="K37" s="81"/>
+      <c r="M37" s="32"/>
+      <c r="N37" s="114" t="s">
+        <v>74</v>
+      </c>
+      <c r="O37" s="114"/>
+      <c r="P37" s="114"/>
+      <c r="Q37" s="114"/>
+      <c r="R37" s="114"/>
+      <c r="S37" s="114"/>
+    </row>
+    <row r="38" spans="1:19" ht="15.75" thickBot="1">
+      <c r="N38" s="114" t="s">
+        <v>128</v>
+      </c>
+      <c r="O38" s="114"/>
+      <c r="P38" s="114"/>
+      <c r="Q38" s="114"/>
+      <c r="R38" s="114"/>
+      <c r="S38" s="114"/>
+    </row>
     <row r="39" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A39" s="60" t="s">
+      <c r="A39" s="59" t="s">
         <v>25</v>
       </c>
-      <c r="B39" s="61"/>
-      <c r="C39" s="61"/>
-      <c r="D39" s="61"/>
-      <c r="E39" s="62"/>
-      <c r="N39" s="56" t="s">
-        <v>108</v>
-      </c>
-      <c r="O39" s="56"/>
-      <c r="P39" s="56"/>
-      <c r="Q39" s="56"/>
-      <c r="R39" s="56"/>
-      <c r="S39" s="56"/>
+      <c r="B39" s="60"/>
+      <c r="C39" s="60"/>
+      <c r="D39" s="60"/>
+      <c r="E39" s="61"/>
     </row>
     <row r="40" spans="1:19">
       <c r="A40" s="14" t="s">
         <v>24</v>
       </c>
       <c r="B40" s="13"/>
-      <c r="C40" s="63" t="s">
+      <c r="C40" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="D40" s="64"/>
-      <c r="E40" s="26"/>
+      <c r="D40" s="63"/>
+      <c r="E40" s="27"/>
     </row>
     <row r="41" spans="1:19">
       <c r="A41" s="15" t="s">
         <v>21</v>
       </c>
       <c r="B41" s="5"/>
-      <c r="C41" s="63" t="s">
+      <c r="C41" s="62" t="s">
         <v>23</v>
       </c>
-      <c r="D41" s="64"/>
+      <c r="D41" s="63"/>
       <c r="E41" s="8"/>
     </row>
     <row r="42" spans="1:19" ht="17.25">
       <c r="A42" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="B42" s="52"/>
-      <c r="C42" s="69" t="s">
+        <v>112</v>
+      </c>
+      <c r="B42" s="54"/>
+      <c r="C42" s="68" t="s">
         <v>64</v>
       </c>
-      <c r="D42" s="70"/>
-      <c r="E42" s="35"/>
-      <c r="N42" s="46" t="s">
+      <c r="D42" s="69"/>
+      <c r="E42" s="37"/>
+      <c r="N42" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="O42" s="40" t="s">
-        <v>92</v>
+      <c r="O42" s="42" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="43" spans="1:19" ht="15.75" thickBot="1">
       <c r="O43" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19">
+      <c r="A44" s="64" t="s">
+        <v>35</v>
+      </c>
+      <c r="B44" s="65"/>
+      <c r="C44" s="65"/>
+      <c r="D44" s="65"/>
+      <c r="E44" s="65"/>
+      <c r="F44" s="65"/>
+      <c r="G44" s="65"/>
+      <c r="H44" s="65"/>
+      <c r="I44" s="65"/>
+      <c r="J44" s="65"/>
+      <c r="K44" s="65"/>
+      <c r="L44" s="65"/>
+    </row>
+    <row r="45" spans="1:19" ht="17.25">
+      <c r="A45" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="B45" s="58" t="s">
+        <v>55</v>
+      </c>
+      <c r="C45" s="58"/>
+      <c r="D45" s="58"/>
+      <c r="E45" s="58"/>
+      <c r="F45" s="58"/>
+      <c r="G45" s="58"/>
+      <c r="H45" s="58"/>
+      <c r="I45" s="58"/>
+      <c r="J45" s="58"/>
+      <c r="K45" s="58"/>
+      <c r="L45" s="58"/>
+      <c r="N45" s="48" t="s">
+        <v>92</v>
+      </c>
+      <c r="O45" s="42" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="44" spans="1:19">
-      <c r="A44" s="65" t="s">
-        <v>35</v>
-      </c>
-      <c r="B44" s="66"/>
-      <c r="C44" s="66"/>
-      <c r="D44" s="66"/>
-      <c r="E44" s="66"/>
-      <c r="F44" s="66"/>
-      <c r="G44" s="66"/>
-      <c r="H44" s="66"/>
-      <c r="I44" s="66"/>
-      <c r="J44" s="66"/>
-      <c r="K44" s="66"/>
-      <c r="L44" s="66"/>
-    </row>
-    <row r="45" spans="1:19" ht="17.25">
-      <c r="A45" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="B45" s="59" t="s">
-        <v>55</v>
-      </c>
-      <c r="C45" s="59"/>
-      <c r="D45" s="59"/>
-      <c r="E45" s="59"/>
-      <c r="F45" s="59"/>
-      <c r="G45" s="59"/>
-      <c r="H45" s="59"/>
-      <c r="I45" s="59"/>
-      <c r="J45" s="59"/>
-      <c r="K45" s="59"/>
-      <c r="L45" s="59"/>
-      <c r="N45" s="46" t="s">
+    <row r="46" spans="1:19" ht="15" customHeight="1">
+      <c r="A46" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="B46" s="58" t="s">
+        <v>56</v>
+      </c>
+      <c r="C46" s="58"/>
+      <c r="D46" s="58"/>
+      <c r="E46" s="58"/>
+      <c r="F46" s="58"/>
+      <c r="G46" s="58"/>
+      <c r="H46" s="58"/>
+      <c r="I46" s="58"/>
+      <c r="J46" s="58"/>
+      <c r="K46" s="58"/>
+      <c r="L46" s="58"/>
+      <c r="O46" s="42" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19">
+      <c r="A47" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="B47" s="58" t="s">
+        <v>57</v>
+      </c>
+      <c r="C47" s="58"/>
+      <c r="D47" s="58"/>
+      <c r="E47" s="58"/>
+      <c r="F47" s="58"/>
+      <c r="G47" s="58"/>
+      <c r="H47" s="58"/>
+      <c r="I47" s="58"/>
+      <c r="J47" s="58"/>
+      <c r="K47" s="58"/>
+      <c r="L47" s="58"/>
+      <c r="O47" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19">
+      <c r="A48" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B48" s="58" t="s">
+        <v>44</v>
+      </c>
+      <c r="C48" s="58"/>
+      <c r="D48" s="58"/>
+      <c r="E48" s="58"/>
+      <c r="F48" s="58"/>
+      <c r="G48" s="58"/>
+      <c r="H48" s="58"/>
+      <c r="I48" s="58"/>
+      <c r="J48" s="58"/>
+      <c r="K48" s="58"/>
+      <c r="L48" s="58"/>
+    </row>
+    <row r="49" spans="1:15" ht="17.25">
+      <c r="A49" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="B49" s="58" t="s">
+        <v>33</v>
+      </c>
+      <c r="C49" s="58"/>
+      <c r="D49" s="58"/>
+      <c r="E49" s="58"/>
+      <c r="F49" s="58"/>
+      <c r="G49" s="58"/>
+      <c r="H49" s="58"/>
+      <c r="I49" s="58"/>
+      <c r="J49" s="58"/>
+      <c r="K49" s="58"/>
+      <c r="L49" s="58"/>
+      <c r="N49" s="48" t="s">
+        <v>91</v>
+      </c>
+      <c r="O49" s="42" t="s">
         <v>90</v>
       </c>
-      <c r="O45" s="40" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="46" spans="1:19" ht="15" customHeight="1">
-      <c r="A46" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="B46" s="59" t="s">
-        <v>56</v>
-      </c>
-      <c r="C46" s="59"/>
-      <c r="D46" s="59"/>
-      <c r="E46" s="59"/>
-      <c r="F46" s="59"/>
-      <c r="G46" s="59"/>
-      <c r="H46" s="59"/>
-      <c r="I46" s="59"/>
-      <c r="J46" s="59"/>
-      <c r="K46" s="59"/>
-      <c r="L46" s="59"/>
-      <c r="O46" s="40" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="47" spans="1:19">
-      <c r="A47" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="B47" s="59" t="s">
-        <v>57</v>
-      </c>
-      <c r="C47" s="59"/>
-      <c r="D47" s="59"/>
-      <c r="E47" s="59"/>
-      <c r="F47" s="59"/>
-      <c r="G47" s="59"/>
-      <c r="H47" s="59"/>
-      <c r="I47" s="59"/>
-      <c r="J47" s="59"/>
-      <c r="K47" s="59"/>
-      <c r="L47" s="59"/>
-      <c r="O47" t="s">
+    </row>
+    <row r="50" spans="1:15">
+      <c r="A50" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="B50" s="58" t="s">
+        <v>54</v>
+      </c>
+      <c r="C50" s="58"/>
+      <c r="D50" s="58"/>
+      <c r="E50" s="58"/>
+      <c r="F50" s="58"/>
+      <c r="G50" s="58"/>
+      <c r="H50" s="58"/>
+      <c r="I50" s="58"/>
+      <c r="J50" s="58"/>
+      <c r="K50" s="58"/>
+      <c r="L50" s="58"/>
+      <c r="O50" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="48" spans="1:19">
-      <c r="A48" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="B48" s="59" t="s">
-        <v>44</v>
-      </c>
-      <c r="C48" s="59"/>
-      <c r="D48" s="59"/>
-      <c r="E48" s="59"/>
-      <c r="F48" s="59"/>
-      <c r="G48" s="59"/>
-      <c r="H48" s="59"/>
-      <c r="I48" s="59"/>
-      <c r="J48" s="59"/>
-      <c r="K48" s="59"/>
-      <c r="L48" s="59"/>
-    </row>
-    <row r="49" spans="1:15" ht="17.25">
-      <c r="A49" s="31" t="s">
-        <v>52</v>
-      </c>
-      <c r="B49" s="59" t="s">
-        <v>33</v>
-      </c>
-      <c r="C49" s="59"/>
-      <c r="D49" s="59"/>
-      <c r="E49" s="59"/>
-      <c r="F49" s="59"/>
-      <c r="G49" s="59"/>
-      <c r="H49" s="59"/>
-      <c r="I49" s="59"/>
-      <c r="J49" s="59"/>
-      <c r="K49" s="59"/>
-      <c r="L49" s="59"/>
-      <c r="N49" s="46" t="s">
-        <v>89</v>
-      </c>
-      <c r="O49" s="40" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="50" spans="1:15">
-      <c r="A50" s="31" t="s">
-        <v>50</v>
-      </c>
-      <c r="B50" s="59" t="s">
-        <v>54</v>
-      </c>
-      <c r="C50" s="59"/>
-      <c r="D50" s="59"/>
-      <c r="E50" s="59"/>
-      <c r="F50" s="59"/>
-      <c r="G50" s="59"/>
-      <c r="H50" s="59"/>
-      <c r="I50" s="59"/>
-      <c r="J50" s="59"/>
-      <c r="K50" s="59"/>
-      <c r="L50" s="59"/>
-      <c r="O50" t="s">
-        <v>95</v>
-      </c>
-    </row>
     <row r="51" spans="1:15">
-      <c r="A51" s="31" t="s">
+      <c r="A51" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="B51" s="59" t="s">
+      <c r="B51" s="58" t="s">
         <v>53</v>
       </c>
-      <c r="C51" s="59"/>
-      <c r="D51" s="59"/>
-      <c r="E51" s="59"/>
-      <c r="F51" s="59"/>
-      <c r="G51" s="59"/>
-      <c r="H51" s="59"/>
-      <c r="I51" s="59"/>
-      <c r="J51" s="59"/>
-      <c r="K51" s="59"/>
-      <c r="L51" s="59"/>
+      <c r="C51" s="58"/>
+      <c r="D51" s="58"/>
+      <c r="E51" s="58"/>
+      <c r="F51" s="58"/>
+      <c r="G51" s="58"/>
+      <c r="H51" s="58"/>
+      <c r="I51" s="58"/>
+      <c r="J51" s="58"/>
+      <c r="K51" s="58"/>
+      <c r="L51" s="58"/>
       <c r="O51" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="52" spans="1:15">
-      <c r="C52" s="30"/>
+      <c r="C52" s="32"/>
     </row>
     <row r="53" spans="1:15">
-      <c r="C53" s="30"/>
+      <c r="C53" s="32"/>
     </row>
     <row r="54" spans="1:15">
-      <c r="B54" s="30"/>
+      <c r="B54" s="32"/>
     </row>
   </sheetData>
   <sortState ref="A24:K25">
     <sortCondition ref="A3"/>
   </sortState>
-  <mergeCells count="55">
+  <mergeCells count="60">
+    <mergeCell ref="N38:S38"/>
     <mergeCell ref="C28:G28"/>
     <mergeCell ref="H28:K28"/>
     <mergeCell ref="H3:K3"/>
     <mergeCell ref="C3:G3"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="H30:K30"/>
+    <mergeCell ref="N16:S16"/>
+    <mergeCell ref="N31:S31"/>
+    <mergeCell ref="N37:S37"/>
+    <mergeCell ref="N30:S30"/>
+    <mergeCell ref="N25:S25"/>
+    <mergeCell ref="N33:S33"/>
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="O6:U6"/>
     <mergeCell ref="A1:L1"/>
@@ -2899,12 +2966,14 @@
     <mergeCell ref="H27:K27"/>
     <mergeCell ref="M3:N3"/>
     <mergeCell ref="M4:N4"/>
-    <mergeCell ref="N22:S22"/>
+    <mergeCell ref="N24:S24"/>
+    <mergeCell ref="N27:S27"/>
     <mergeCell ref="N20:S20"/>
     <mergeCell ref="O14:S15"/>
-    <mergeCell ref="N25:S25"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="H30:K30"/>
+    <mergeCell ref="N22:S22"/>
+    <mergeCell ref="N19:S19"/>
+    <mergeCell ref="N17:S17"/>
+    <mergeCell ref="N28:S28"/>
     <mergeCell ref="A30:B30"/>
     <mergeCell ref="A33:B33"/>
     <mergeCell ref="A32:B32"/>
@@ -2936,12 +3005,6 @@
     <mergeCell ref="B47:L47"/>
     <mergeCell ref="B48:L48"/>
     <mergeCell ref="B49:L49"/>
-    <mergeCell ref="N28:S28"/>
-    <mergeCell ref="N39:S39"/>
-    <mergeCell ref="N32:S32"/>
-    <mergeCell ref="N35:S35"/>
-    <mergeCell ref="N30:S30"/>
-    <mergeCell ref="N37:S37"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="Q4" r:id="rId1"/>
@@ -2973,116 +3036,116 @@
   <sheetData>
     <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="50" t="s">
+        <v>107</v>
+      </c>
+      <c r="B4" s="50"/>
+      <c r="C4" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="50" t="s">
         <v>106</v>
       </c>
-      <c r="B3" s="1"/>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="48" t="s">
+      <c r="E4" s="50" t="s">
         <v>105</v>
       </c>
-      <c r="B4" s="48"/>
-      <c r="C4" s="48" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="48" t="s">
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="49" t="s">
         <v>104</v>
       </c>
-      <c r="E4" s="48" t="s">
+      <c r="B5" s="49" t="s">
+        <v>101</v>
+      </c>
+      <c r="C5" s="50"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="49"/>
+      <c r="B6" s="49" t="s">
+        <v>100</v>
+      </c>
+      <c r="C6" s="50" t="s">
+        <v>109</v>
+      </c>
+      <c r="D6" s="50" t="s">
+        <v>109</v>
+      </c>
+      <c r="E6" s="50" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="49"/>
+      <c r="B7" s="49"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="50"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="49" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="47" t="s">
+      <c r="B8" s="49" t="s">
+        <v>101</v>
+      </c>
+      <c r="C8" s="50"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="50"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="49"/>
+      <c r="B9" s="49" t="s">
+        <v>100</v>
+      </c>
+      <c r="C9" s="50" t="s">
+        <v>109</v>
+      </c>
+      <c r="D9" s="50" t="s">
+        <v>109</v>
+      </c>
+      <c r="E9" s="50" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="49"/>
+      <c r="B10" s="49"/>
+      <c r="C10" s="50"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="50"/>
+    </row>
+    <row r="11" spans="1:6" ht="15.75">
+      <c r="A11" s="49" t="s">
         <v>102</v>
       </c>
-      <c r="B5" s="47" t="s">
-        <v>99</v>
-      </c>
-      <c r="C5" s="48"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="47"/>
-      <c r="B6" s="47" t="s">
-        <v>98</v>
-      </c>
-      <c r="C6" s="48" t="s">
-        <v>107</v>
-      </c>
-      <c r="D6" s="48" t="s">
-        <v>107</v>
-      </c>
-      <c r="E6" s="48" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="47"/>
-      <c r="B7" s="47"/>
-      <c r="C7" s="48"/>
-      <c r="D7" s="48"/>
-      <c r="E7" s="48"/>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="47" t="s">
+      <c r="B11" s="49" t="s">
         <v>101</v>
       </c>
-      <c r="B8" s="47" t="s">
-        <v>99</v>
-      </c>
-      <c r="C8" s="48"/>
-      <c r="D8" s="48"/>
-      <c r="E8" s="48"/>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="47"/>
-      <c r="B9" s="47" t="s">
-        <v>98</v>
-      </c>
-      <c r="C9" s="48" t="s">
-        <v>107</v>
-      </c>
-      <c r="D9" s="48" t="s">
-        <v>107</v>
-      </c>
-      <c r="E9" s="48" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="47"/>
-      <c r="B10" s="47"/>
-      <c r="C10" s="48"/>
-      <c r="D10" s="48"/>
-      <c r="E10" s="48"/>
-    </row>
-    <row r="11" spans="1:6" ht="15.75">
-      <c r="A11" s="47" t="s">
+      <c r="C11" s="50"/>
+      <c r="D11" s="50"/>
+      <c r="E11" s="50"/>
+      <c r="F11" s="51"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="49"/>
+      <c r="B12" s="49" t="s">
         <v>100</v>
       </c>
-      <c r="B11" s="47" t="s">
-        <v>99</v>
-      </c>
-      <c r="C11" s="48"/>
-      <c r="D11" s="48"/>
-      <c r="E11" s="48"/>
-      <c r="F11" s="49"/>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="47"/>
-      <c r="B12" s="47" t="s">
-        <v>98</v>
-      </c>
-      <c r="C12" s="48" t="s">
-        <v>107</v>
-      </c>
-      <c r="D12" s="48" t="s">
-        <v>107</v>
-      </c>
-      <c r="E12" s="48" t="s">
-        <v>107</v>
+      <c r="C12" s="50" t="s">
+        <v>109</v>
+      </c>
+      <c r="D12" s="50" t="s">
+        <v>109</v>
+      </c>
+      <c r="E12" s="50" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -3102,53 +3165,53 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="4" spans="1:2" ht="23.25">
-      <c r="A4" s="53" t="s">
-        <v>111</v>
+      <c r="A4" s="55" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="B5" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="B6" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="B7" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="23.25">
-      <c r="A9" s="53" t="s">
-        <v>116</v>
+      <c r="A9" s="55" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="B10" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="54" t="s">
-        <v>118</v>
+      <c r="A16" s="56" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Avanzando con el testing, validaciones del form, y mejora en stylo ante error de: Career-component, particularmente el form
</commit_message>
<xml_diff>
--- a/Cuadro-de-estado.xlsx
+++ b/Cuadro-de-estado.xlsx
@@ -13,11 +13,12 @@
     <sheet name="Hoja3" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="128">
   <si>
     <t>BACKEND</t>
   </si>
@@ -475,9 +476,6 @@
     <t>Hagamos algo especial.</t>
   </si>
   <si>
-    <t>En SOFTSKILL form, inicializa mal el range</t>
-  </si>
-  <si>
     <t>OJO EN LOS FORM. SIN NO HAY CAMBIOS QUE NO VAYA AL HTTP</t>
   </si>
   <si>
@@ -487,7 +485,7 @@
     <t>LOS FORM TIENEN ALGO MAL CON LAS VALIDACIONES, AL INICIAR</t>
   </si>
   <si>
-    <t>Estudios y trabajos, da repetido el nombre cuando modifico cualquier otro dato</t>
+    <t>Estudios y trabajos, da repetido el nombre cuando modifico cualquier otro dato, ver si puedo aceptar con organizaciones diferentes</t>
   </si>
 </sst>
 </file>
@@ -1272,7 +1270,7 @@
     </xf>
     <xf numFmtId="43" fontId="23" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="122">
+  <cellXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1385,6 +1383,7 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1553,29 +1552,32 @@
     <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1879,7 +1881,7 @@
   <dimension ref="A1:U54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I40" sqref="I40"/>
+      <selection activeCell="M39" sqref="M39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1896,20 +1898,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25">
-      <c r="A1" s="101" t="s">
+      <c r="A1" s="102" t="s">
         <v>84</v>
       </c>
-      <c r="B1" s="101"/>
-      <c r="C1" s="101"/>
-      <c r="D1" s="101"/>
-      <c r="E1" s="101"/>
-      <c r="F1" s="101"/>
-      <c r="G1" s="101"/>
-      <c r="H1" s="101"/>
-      <c r="I1" s="101"/>
-      <c r="J1" s="101"/>
-      <c r="K1" s="101"/>
-      <c r="L1" s="101"/>
+      <c r="B1" s="102"/>
+      <c r="C1" s="102"/>
+      <c r="D1" s="102"/>
+      <c r="E1" s="102"/>
+      <c r="F1" s="102"/>
+      <c r="G1" s="102"/>
+      <c r="H1" s="102"/>
+      <c r="I1" s="102"/>
+      <c r="J1" s="102"/>
+      <c r="K1" s="102"/>
+      <c r="L1" s="102"/>
     </row>
     <row r="2" spans="1:21" ht="19.5" thickBot="1">
       <c r="A2" s="44">
@@ -1928,30 +1930,30 @@
       </c>
     </row>
     <row r="3" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="102" t="s">
+      <c r="A3" s="103" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="103"/>
-      <c r="C3" s="104" t="s">
+      <c r="B3" s="104"/>
+      <c r="C3" s="105" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="105"/>
-      <c r="E3" s="105"/>
-      <c r="F3" s="105"/>
-      <c r="G3" s="106"/>
-      <c r="H3" s="104" t="s">
+      <c r="D3" s="106"/>
+      <c r="E3" s="106"/>
+      <c r="F3" s="106"/>
+      <c r="G3" s="107"/>
+      <c r="H3" s="105" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="105"/>
-      <c r="J3" s="107"/>
-      <c r="K3" s="106"/>
+      <c r="I3" s="106"/>
+      <c r="J3" s="108"/>
+      <c r="K3" s="107"/>
       <c r="L3" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="108" t="s">
+      <c r="M3" s="109" t="s">
         <v>76</v>
       </c>
-      <c r="N3" s="100"/>
+      <c r="N3" s="101"/>
     </row>
     <row r="4" spans="1:21" s="3" customFormat="1" ht="40.5" customHeight="1" thickBot="1">
       <c r="A4" s="17" t="s">
@@ -1990,10 +1992,10 @@
       <c r="L4" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="M4" s="109" t="s">
+      <c r="M4" s="110" t="s">
         <v>77</v>
       </c>
-      <c r="N4" s="110"/>
+      <c r="N4" s="111"/>
       <c r="O4" s="34" t="s">
         <v>61</v>
       </c>
@@ -2030,15 +2032,15 @@
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
-      <c r="O6" s="99" t="s">
+      <c r="O6" s="100" t="s">
         <v>65</v>
       </c>
-      <c r="P6" s="100"/>
-      <c r="Q6" s="100"/>
-      <c r="R6" s="100"/>
-      <c r="S6" s="100"/>
-      <c r="T6" s="100"/>
-      <c r="U6" s="100"/>
+      <c r="P6" s="101"/>
+      <c r="Q6" s="101"/>
+      <c r="R6" s="101"/>
+      <c r="S6" s="101"/>
+      <c r="T6" s="101"/>
+      <c r="U6" s="101"/>
     </row>
     <row r="7" spans="1:21" ht="4.5" customHeight="1">
       <c r="A7" s="28"/>
@@ -2164,11 +2166,11 @@
       <c r="B13" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="40"/>
+      <c r="C13" s="4"/>
       <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
+      <c r="E13" s="4"/>
       <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
+      <c r="G13" s="4"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
@@ -2188,23 +2190,23 @@
       <c r="B14" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="40"/>
+      <c r="C14" s="4"/>
       <c r="D14" s="40"/>
-      <c r="E14" s="40"/>
+      <c r="E14" s="4"/>
       <c r="F14" s="40"/>
-      <c r="G14" s="40"/>
+      <c r="G14" s="4"/>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
       <c r="K14" s="54"/>
       <c r="L14" s="4"/>
-      <c r="O14" s="112" t="s">
+      <c r="O14" s="113" t="s">
         <v>75</v>
       </c>
-      <c r="P14" s="112"/>
-      <c r="Q14" s="112"/>
-      <c r="R14" s="112"/>
-      <c r="S14" s="112"/>
+      <c r="P14" s="113"/>
+      <c r="Q14" s="113"/>
+      <c r="R14" s="113"/>
+      <c r="S14" s="113"/>
     </row>
     <row r="15" spans="1:21" ht="15" customHeight="1">
       <c r="A15" s="38" t="s">
@@ -2223,11 +2225,11 @@
       <c r="J15" s="4"/>
       <c r="K15" s="54"/>
       <c r="L15" s="4"/>
-      <c r="O15" s="112"/>
-      <c r="P15" s="112"/>
-      <c r="Q15" s="112"/>
-      <c r="R15" s="112"/>
-      <c r="S15" s="112"/>
+      <c r="O15" s="113"/>
+      <c r="P15" s="113"/>
+      <c r="Q15" s="113"/>
+      <c r="R15" s="113"/>
+      <c r="S15" s="113"/>
       <c r="T15" s="53"/>
     </row>
     <row r="16" spans="1:21">
@@ -2247,14 +2249,14 @@
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
       <c r="L16" s="4"/>
-      <c r="N16" s="111" t="s">
+      <c r="N16" s="112" t="s">
         <v>110</v>
       </c>
-      <c r="O16" s="111"/>
-      <c r="P16" s="111"/>
-      <c r="Q16" s="111"/>
-      <c r="R16" s="111"/>
-      <c r="S16" s="111"/>
+      <c r="O16" s="112"/>
+      <c r="P16" s="112"/>
+      <c r="Q16" s="112"/>
+      <c r="R16" s="112"/>
+      <c r="S16" s="112"/>
       <c r="T16" s="53"/>
     </row>
     <row r="17" spans="1:19">
@@ -2264,24 +2266,24 @@
       <c r="B17" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="40"/>
+      <c r="C17" s="4"/>
       <c r="D17" s="40"/>
-      <c r="E17" s="40"/>
-      <c r="F17" s="54"/>
-      <c r="G17" s="40"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="4"/>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
       <c r="L17" s="4"/>
-      <c r="N17" s="111" t="s">
-        <v>127</v>
-      </c>
-      <c r="O17" s="111"/>
-      <c r="P17" s="111"/>
-      <c r="Q17" s="111"/>
-      <c r="R17" s="111"/>
-      <c r="S17" s="111"/>
+      <c r="N17" s="112" t="s">
+        <v>126</v>
+      </c>
+      <c r="O17" s="112"/>
+      <c r="P17" s="112"/>
+      <c r="Q17" s="112"/>
+      <c r="R17" s="112"/>
+      <c r="S17" s="112"/>
     </row>
     <row r="18" spans="1:19" ht="4.5" customHeight="1">
       <c r="A18" s="28"/>
@@ -2314,14 +2316,14 @@
       <c r="J19" s="5"/>
       <c r="K19" s="7"/>
       <c r="L19" s="52"/>
-      <c r="N19" s="111" t="s">
-        <v>125</v>
-      </c>
-      <c r="O19" s="111"/>
-      <c r="P19" s="111"/>
-      <c r="Q19" s="111"/>
-      <c r="R19" s="111"/>
-      <c r="S19" s="111"/>
+      <c r="N19" s="112" t="s">
+        <v>124</v>
+      </c>
+      <c r="O19" s="112"/>
+      <c r="P19" s="112"/>
+      <c r="Q19" s="112"/>
+      <c r="R19" s="112"/>
+      <c r="S19" s="112"/>
     </row>
     <row r="20" spans="1:19">
       <c r="A20" s="39" t="s">
@@ -2340,14 +2342,14 @@
       <c r="J20" s="5"/>
       <c r="K20" s="7"/>
       <c r="L20" s="52"/>
-      <c r="N20" s="111" t="s">
+      <c r="N20" s="112" t="s">
         <v>113</v>
       </c>
-      <c r="O20" s="111"/>
-      <c r="P20" s="111"/>
-      <c r="Q20" s="111"/>
-      <c r="R20" s="111"/>
-      <c r="S20" s="111"/>
+      <c r="O20" s="112"/>
+      <c r="P20" s="112"/>
+      <c r="Q20" s="112"/>
+      <c r="R20" s="112"/>
+      <c r="S20" s="112"/>
     </row>
     <row r="21" spans="1:19" ht="4.5" customHeight="1">
       <c r="A21" s="28"/>
@@ -2378,14 +2380,12 @@
       <c r="J22" s="5"/>
       <c r="K22" s="7"/>
       <c r="L22" s="4"/>
-      <c r="N22" s="111" t="s">
-        <v>124</v>
-      </c>
-      <c r="O22" s="111"/>
-      <c r="P22" s="111"/>
-      <c r="Q22" s="111"/>
-      <c r="R22" s="111"/>
-      <c r="S22" s="111"/>
+      <c r="N22" s="58"/>
+      <c r="O22" s="58"/>
+      <c r="P22" s="58"/>
+      <c r="Q22" s="58"/>
+      <c r="R22" s="58"/>
+      <c r="S22" s="58"/>
     </row>
     <row r="23" spans="1:19" ht="4.5" customHeight="1">
       <c r="A23" s="28"/>
@@ -2416,14 +2416,14 @@
       <c r="J24" s="5"/>
       <c r="K24" s="7"/>
       <c r="L24" s="4"/>
-      <c r="N24" s="111" t="s">
+      <c r="N24" s="112" t="s">
         <v>83</v>
       </c>
-      <c r="O24" s="111"/>
-      <c r="P24" s="111"/>
-      <c r="Q24" s="111"/>
-      <c r="R24" s="111"/>
-      <c r="S24" s="111"/>
+      <c r="O24" s="112"/>
+      <c r="P24" s="112"/>
+      <c r="Q24" s="112"/>
+      <c r="R24" s="112"/>
+      <c r="S24" s="112"/>
     </row>
     <row r="25" spans="1:19">
       <c r="A25" s="39" t="s">
@@ -2442,14 +2442,14 @@
       <c r="J25" s="5"/>
       <c r="K25" s="7"/>
       <c r="L25" s="4"/>
-      <c r="N25" s="111" t="s">
+      <c r="N25" s="112" t="s">
         <v>82</v>
       </c>
-      <c r="O25" s="111"/>
-      <c r="P25" s="111"/>
-      <c r="Q25" s="111"/>
-      <c r="R25" s="111"/>
-      <c r="S25" s="111"/>
+      <c r="O25" s="112"/>
+      <c r="P25" s="112"/>
+      <c r="Q25" s="112"/>
+      <c r="R25" s="112"/>
+      <c r="S25" s="112"/>
     </row>
     <row r="26" spans="1:19" ht="4.5" customHeight="1" thickBot="1">
       <c r="A26" s="28"/>
@@ -2468,43 +2468,43 @@
     <row r="27" spans="1:19" ht="15.75" thickBot="1">
       <c r="A27" s="23"/>
       <c r="B27" s="25"/>
-      <c r="C27" s="104" t="s">
+      <c r="C27" s="105" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="105"/>
-      <c r="E27" s="105"/>
-      <c r="F27" s="105"/>
-      <c r="G27" s="106"/>
-      <c r="H27" s="104" t="s">
+      <c r="D27" s="106"/>
+      <c r="E27" s="106"/>
+      <c r="F27" s="106"/>
+      <c r="G27" s="107"/>
+      <c r="H27" s="105" t="s">
         <v>0</v>
       </c>
-      <c r="I27" s="105"/>
-      <c r="J27" s="107"/>
-      <c r="K27" s="106"/>
+      <c r="I27" s="106"/>
+      <c r="J27" s="108"/>
+      <c r="K27" s="107"/>
       <c r="L27" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="N27" s="111" t="s">
+      <c r="N27" s="112" t="s">
         <v>78</v>
       </c>
-      <c r="O27" s="111"/>
-      <c r="P27" s="111"/>
-      <c r="Q27" s="111"/>
-      <c r="R27" s="111"/>
-      <c r="S27" s="111"/>
+      <c r="O27" s="112"/>
+      <c r="P27" s="112"/>
+      <c r="Q27" s="112"/>
+      <c r="R27" s="112"/>
+      <c r="S27" s="112"/>
     </row>
     <row r="28" spans="1:19" ht="30">
-      <c r="A28" s="97" t="s">
+      <c r="A28" s="98" t="s">
         <v>29</v>
       </c>
-      <c r="B28" s="98"/>
-      <c r="C28" s="91" t="s">
+      <c r="B28" s="99"/>
+      <c r="C28" s="92" t="s">
         <v>88</v>
       </c>
-      <c r="D28" s="92"/>
-      <c r="E28" s="92"/>
-      <c r="F28" s="92"/>
-      <c r="G28" s="93"/>
+      <c r="D28" s="93"/>
+      <c r="E28" s="93"/>
+      <c r="F28" s="93"/>
+      <c r="G28" s="94"/>
       <c r="H28" s="115" t="s">
         <v>86</v>
       </c>
@@ -2514,14 +2514,14 @@
       <c r="L28" s="47" t="s">
         <v>87</v>
       </c>
-      <c r="N28" s="113" t="s">
+      <c r="N28" s="114" t="s">
         <v>111</v>
       </c>
-      <c r="O28" s="113"/>
-      <c r="P28" s="113"/>
-      <c r="Q28" s="113"/>
-      <c r="R28" s="113"/>
-      <c r="S28" s="113"/>
+      <c r="O28" s="114"/>
+      <c r="P28" s="114"/>
+      <c r="Q28" s="114"/>
+      <c r="R28" s="114"/>
+      <c r="S28" s="114"/>
     </row>
     <row r="29" spans="1:19" ht="4.5" customHeight="1">
       <c r="A29" s="28"/>
@@ -2538,10 +2538,10 @@
       <c r="L29" s="30"/>
     </row>
     <row r="30" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A30" s="66" t="s">
+      <c r="A30" s="67" t="s">
         <v>38</v>
       </c>
-      <c r="B30" s="67"/>
+      <c r="B30" s="68"/>
       <c r="C30" s="118"/>
       <c r="D30" s="119"/>
       <c r="E30" s="119"/>
@@ -2555,83 +2555,83 @@
         <v>5</v>
       </c>
       <c r="M30" s="32"/>
-      <c r="N30" s="111" t="s">
+      <c r="N30" s="112" t="s">
         <v>72</v>
       </c>
-      <c r="O30" s="111"/>
-      <c r="P30" s="111"/>
-      <c r="Q30" s="111"/>
-      <c r="R30" s="111"/>
-      <c r="S30" s="111"/>
+      <c r="O30" s="112"/>
+      <c r="P30" s="112"/>
+      <c r="Q30" s="112"/>
+      <c r="R30" s="112"/>
+      <c r="S30" s="112"/>
     </row>
     <row r="31" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A31" s="66" t="s">
+      <c r="A31" s="67" t="s">
         <v>79</v>
       </c>
-      <c r="B31" s="67"/>
-      <c r="C31" s="91"/>
-      <c r="D31" s="92"/>
-      <c r="E31" s="92"/>
-      <c r="F31" s="92"/>
-      <c r="G31" s="93"/>
-      <c r="H31" s="94" t="s">
+      <c r="B31" s="68"/>
+      <c r="C31" s="92"/>
+      <c r="D31" s="93"/>
+      <c r="E31" s="93"/>
+      <c r="F31" s="93"/>
+      <c r="G31" s="94"/>
+      <c r="H31" s="95" t="s">
         <v>80</v>
       </c>
-      <c r="I31" s="95"/>
-      <c r="J31" s="95"/>
-      <c r="K31" s="95"/>
-      <c r="L31" s="96"/>
+      <c r="I31" s="96"/>
+      <c r="J31" s="96"/>
+      <c r="K31" s="96"/>
+      <c r="L31" s="97"/>
       <c r="M31" s="32"/>
-      <c r="N31" s="113" t="s">
+      <c r="N31" s="114" t="s">
         <v>73</v>
       </c>
-      <c r="O31" s="113"/>
-      <c r="P31" s="113"/>
-      <c r="Q31" s="113"/>
-      <c r="R31" s="113"/>
-      <c r="S31" s="113"/>
+      <c r="O31" s="114"/>
+      <c r="P31" s="114"/>
+      <c r="Q31" s="114"/>
+      <c r="R31" s="114"/>
+      <c r="S31" s="114"/>
     </row>
     <row r="32" spans="1:19" ht="16.5" thickBot="1">
-      <c r="A32" s="87" t="s">
+      <c r="A32" s="88" t="s">
         <v>59</v>
       </c>
-      <c r="B32" s="88"/>
-      <c r="C32" s="82"/>
-      <c r="D32" s="83"/>
-      <c r="E32" s="83"/>
-      <c r="F32" s="83"/>
-      <c r="G32" s="89"/>
-      <c r="H32" s="90"/>
-      <c r="I32" s="83"/>
-      <c r="J32" s="83"/>
-      <c r="K32" s="89"/>
+      <c r="B32" s="89"/>
+      <c r="C32" s="83"/>
+      <c r="D32" s="84"/>
+      <c r="E32" s="84"/>
+      <c r="F32" s="84"/>
+      <c r="G32" s="90"/>
+      <c r="H32" s="91"/>
+      <c r="I32" s="84"/>
+      <c r="J32" s="84"/>
+      <c r="K32" s="90"/>
       <c r="M32" s="32"/>
     </row>
     <row r="33" spans="1:19" ht="30.75" customHeight="1" thickBot="1">
-      <c r="A33" s="85" t="s">
+      <c r="A33" s="86" t="s">
         <v>34</v>
       </c>
-      <c r="B33" s="86"/>
-      <c r="C33" s="73" t="s">
+      <c r="B33" s="87"/>
+      <c r="C33" s="74" t="s">
         <v>58</v>
       </c>
-      <c r="D33" s="74"/>
-      <c r="E33" s="74"/>
-      <c r="F33" s="74"/>
-      <c r="G33" s="75"/>
-      <c r="H33" s="70"/>
-      <c r="I33" s="71"/>
-      <c r="J33" s="71"/>
-      <c r="K33" s="72"/>
+      <c r="D33" s="75"/>
+      <c r="E33" s="75"/>
+      <c r="F33" s="75"/>
+      <c r="G33" s="76"/>
+      <c r="H33" s="71"/>
+      <c r="I33" s="72"/>
+      <c r="J33" s="72"/>
+      <c r="K33" s="73"/>
       <c r="M33" s="32"/>
-      <c r="N33" s="113" t="s">
-        <v>126</v>
-      </c>
-      <c r="O33" s="113"/>
-      <c r="P33" s="113"/>
-      <c r="Q33" s="113"/>
-      <c r="R33" s="113"/>
-      <c r="S33" s="113"/>
+      <c r="N33" s="114" t="s">
+        <v>125</v>
+      </c>
+      <c r="O33" s="114"/>
+      <c r="P33" s="114"/>
+      <c r="Q33" s="114"/>
+      <c r="R33" s="114"/>
+      <c r="S33" s="114"/>
     </row>
     <row r="34" spans="1:19" ht="4.5" customHeight="1" thickBot="1">
       <c r="A34" s="28"/>
@@ -2647,89 +2647,95 @@
       <c r="K34" s="30"/>
     </row>
     <row r="35" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A35" s="66" t="s">
+      <c r="A35" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="67"/>
-      <c r="C35" s="82"/>
-      <c r="D35" s="83"/>
-      <c r="E35" s="83"/>
-      <c r="F35" s="83"/>
-      <c r="G35" s="84"/>
-      <c r="H35" s="76"/>
-      <c r="I35" s="77"/>
-      <c r="J35" s="77"/>
-      <c r="K35" s="78"/>
+      <c r="B35" s="68"/>
+      <c r="C35" s="83"/>
+      <c r="D35" s="84"/>
+      <c r="E35" s="84"/>
+      <c r="F35" s="84"/>
+      <c r="G35" s="85"/>
+      <c r="H35" s="77"/>
+      <c r="I35" s="78"/>
+      <c r="J35" s="78"/>
+      <c r="K35" s="79"/>
       <c r="M35" s="32"/>
+      <c r="N35" s="123" t="s">
+        <v>127</v>
+      </c>
+      <c r="O35" s="123"/>
+      <c r="P35" s="123"/>
+      <c r="Q35" s="123"/>
+      <c r="R35" s="123"/>
+      <c r="S35" s="123"/>
     </row>
     <row r="36" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A36" s="66" t="s">
+      <c r="A36" s="67" t="s">
         <v>89</v>
       </c>
-      <c r="B36" s="67"/>
-      <c r="C36" s="82"/>
-      <c r="D36" s="83"/>
-      <c r="E36" s="83"/>
-      <c r="F36" s="83"/>
-      <c r="G36" s="84"/>
-      <c r="H36" s="76"/>
-      <c r="I36" s="77"/>
-      <c r="J36" s="77"/>
-      <c r="K36" s="78"/>
+      <c r="B36" s="68"/>
+      <c r="C36" s="83"/>
+      <c r="D36" s="84"/>
+      <c r="E36" s="84"/>
+      <c r="F36" s="84"/>
+      <c r="G36" s="85"/>
+      <c r="H36" s="77"/>
+      <c r="I36" s="78"/>
+      <c r="J36" s="78"/>
+      <c r="K36" s="79"/>
       <c r="M36" s="32"/>
+      <c r="N36" s="123"/>
+      <c r="O36" s="123"/>
+      <c r="P36" s="123"/>
+      <c r="Q36" s="123"/>
+      <c r="R36" s="123"/>
+      <c r="S36" s="123"/>
     </row>
     <row r="37" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A37" s="66" t="s">
+      <c r="A37" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="B37" s="67"/>
-      <c r="C37" s="79"/>
-      <c r="D37" s="80"/>
-      <c r="E37" s="80"/>
-      <c r="F37" s="80"/>
-      <c r="G37" s="81"/>
-      <c r="H37" s="79"/>
-      <c r="I37" s="80"/>
-      <c r="J37" s="80"/>
-      <c r="K37" s="81"/>
+      <c r="B37" s="68"/>
+      <c r="C37" s="80"/>
+      <c r="D37" s="81"/>
+      <c r="E37" s="81"/>
+      <c r="F37" s="81"/>
+      <c r="G37" s="82"/>
+      <c r="H37" s="80"/>
+      <c r="I37" s="81"/>
+      <c r="J37" s="81"/>
+      <c r="K37" s="82"/>
       <c r="M37" s="32"/>
-      <c r="N37" s="114" t="s">
+    </row>
+    <row r="38" spans="1:19" ht="15.75" thickBot="1">
+      <c r="N38" s="122" t="s">
         <v>74</v>
       </c>
-      <c r="O37" s="114"/>
-      <c r="P37" s="114"/>
-      <c r="Q37" s="114"/>
-      <c r="R37" s="114"/>
-      <c r="S37" s="114"/>
-    </row>
-    <row r="38" spans="1:19" ht="15.75" thickBot="1">
-      <c r="N38" s="114" t="s">
-        <v>128</v>
-      </c>
-      <c r="O38" s="114"/>
-      <c r="P38" s="114"/>
-      <c r="Q38" s="114"/>
-      <c r="R38" s="114"/>
-      <c r="S38" s="114"/>
+      <c r="O38" s="122"/>
+      <c r="P38" s="122"/>
+      <c r="Q38" s="122"/>
+      <c r="R38" s="122"/>
+      <c r="S38" s="122"/>
     </row>
     <row r="39" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A39" s="59" t="s">
+      <c r="A39" s="60" t="s">
         <v>25</v>
       </c>
-      <c r="B39" s="60"/>
-      <c r="C39" s="60"/>
-      <c r="D39" s="60"/>
-      <c r="E39" s="61"/>
+      <c r="B39" s="61"/>
+      <c r="C39" s="61"/>
+      <c r="D39" s="61"/>
+      <c r="E39" s="62"/>
     </row>
     <row r="40" spans="1:19">
       <c r="A40" s="14" t="s">
         <v>24</v>
       </c>
       <c r="B40" s="13"/>
-      <c r="C40" s="62" t="s">
+      <c r="C40" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="D40" s="63"/>
+      <c r="D40" s="64"/>
       <c r="E40" s="27"/>
     </row>
     <row r="41" spans="1:19">
@@ -2737,10 +2743,10 @@
         <v>21</v>
       </c>
       <c r="B41" s="5"/>
-      <c r="C41" s="62" t="s">
+      <c r="C41" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="D41" s="63"/>
+      <c r="D41" s="64"/>
       <c r="E41" s="8"/>
     </row>
     <row r="42" spans="1:19" ht="17.25">
@@ -2748,10 +2754,10 @@
         <v>112</v>
       </c>
       <c r="B42" s="54"/>
-      <c r="C42" s="68" t="s">
+      <c r="C42" s="69" t="s">
         <v>64</v>
       </c>
-      <c r="D42" s="69"/>
+      <c r="D42" s="70"/>
       <c r="E42" s="37"/>
       <c r="N42" s="48" t="s">
         <v>4</v>
@@ -2766,38 +2772,38 @@
       </c>
     </row>
     <row r="44" spans="1:19">
-      <c r="A44" s="64" t="s">
+      <c r="A44" s="65" t="s">
         <v>35</v>
       </c>
-      <c r="B44" s="65"/>
-      <c r="C44" s="65"/>
-      <c r="D44" s="65"/>
-      <c r="E44" s="65"/>
-      <c r="F44" s="65"/>
-      <c r="G44" s="65"/>
-      <c r="H44" s="65"/>
-      <c r="I44" s="65"/>
-      <c r="J44" s="65"/>
-      <c r="K44" s="65"/>
-      <c r="L44" s="65"/>
+      <c r="B44" s="66"/>
+      <c r="C44" s="66"/>
+      <c r="D44" s="66"/>
+      <c r="E44" s="66"/>
+      <c r="F44" s="66"/>
+      <c r="G44" s="66"/>
+      <c r="H44" s="66"/>
+      <c r="I44" s="66"/>
+      <c r="J44" s="66"/>
+      <c r="K44" s="66"/>
+      <c r="L44" s="66"/>
     </row>
     <row r="45" spans="1:19" ht="17.25">
       <c r="A45" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="B45" s="58" t="s">
+      <c r="B45" s="59" t="s">
         <v>55</v>
       </c>
-      <c r="C45" s="58"/>
-      <c r="D45" s="58"/>
-      <c r="E45" s="58"/>
-      <c r="F45" s="58"/>
-      <c r="G45" s="58"/>
-      <c r="H45" s="58"/>
-      <c r="I45" s="58"/>
-      <c r="J45" s="58"/>
-      <c r="K45" s="58"/>
-      <c r="L45" s="58"/>
+      <c r="C45" s="59"/>
+      <c r="D45" s="59"/>
+      <c r="E45" s="59"/>
+      <c r="F45" s="59"/>
+      <c r="G45" s="59"/>
+      <c r="H45" s="59"/>
+      <c r="I45" s="59"/>
+      <c r="J45" s="59"/>
+      <c r="K45" s="59"/>
+      <c r="L45" s="59"/>
       <c r="N45" s="48" t="s">
         <v>92</v>
       </c>
@@ -2809,19 +2815,19 @@
       <c r="A46" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="B46" s="58" t="s">
+      <c r="B46" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="C46" s="58"/>
-      <c r="D46" s="58"/>
-      <c r="E46" s="58"/>
-      <c r="F46" s="58"/>
-      <c r="G46" s="58"/>
-      <c r="H46" s="58"/>
-      <c r="I46" s="58"/>
-      <c r="J46" s="58"/>
-      <c r="K46" s="58"/>
-      <c r="L46" s="58"/>
+      <c r="C46" s="59"/>
+      <c r="D46" s="59"/>
+      <c r="E46" s="59"/>
+      <c r="F46" s="59"/>
+      <c r="G46" s="59"/>
+      <c r="H46" s="59"/>
+      <c r="I46" s="59"/>
+      <c r="J46" s="59"/>
+      <c r="K46" s="59"/>
+      <c r="L46" s="59"/>
       <c r="O46" s="42" t="s">
         <v>96</v>
       </c>
@@ -2830,19 +2836,19 @@
       <c r="A47" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="B47" s="58" t="s">
+      <c r="B47" s="59" t="s">
         <v>57</v>
       </c>
-      <c r="C47" s="58"/>
-      <c r="D47" s="58"/>
-      <c r="E47" s="58"/>
-      <c r="F47" s="58"/>
-      <c r="G47" s="58"/>
-      <c r="H47" s="58"/>
-      <c r="I47" s="58"/>
-      <c r="J47" s="58"/>
-      <c r="K47" s="58"/>
-      <c r="L47" s="58"/>
+      <c r="C47" s="59"/>
+      <c r="D47" s="59"/>
+      <c r="E47" s="59"/>
+      <c r="F47" s="59"/>
+      <c r="G47" s="59"/>
+      <c r="H47" s="59"/>
+      <c r="I47" s="59"/>
+      <c r="J47" s="59"/>
+      <c r="K47" s="59"/>
+      <c r="L47" s="59"/>
       <c r="O47" t="s">
         <v>99</v>
       </c>
@@ -2851,37 +2857,37 @@
       <c r="A48" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="B48" s="58" t="s">
+      <c r="B48" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="C48" s="58"/>
-      <c r="D48" s="58"/>
-      <c r="E48" s="58"/>
-      <c r="F48" s="58"/>
-      <c r="G48" s="58"/>
-      <c r="H48" s="58"/>
-      <c r="I48" s="58"/>
-      <c r="J48" s="58"/>
-      <c r="K48" s="58"/>
-      <c r="L48" s="58"/>
+      <c r="C48" s="59"/>
+      <c r="D48" s="59"/>
+      <c r="E48" s="59"/>
+      <c r="F48" s="59"/>
+      <c r="G48" s="59"/>
+      <c r="H48" s="59"/>
+      <c r="I48" s="59"/>
+      <c r="J48" s="59"/>
+      <c r="K48" s="59"/>
+      <c r="L48" s="59"/>
     </row>
     <row r="49" spans="1:15" ht="17.25">
       <c r="A49" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="B49" s="58" t="s">
+      <c r="B49" s="59" t="s">
         <v>33</v>
       </c>
-      <c r="C49" s="58"/>
-      <c r="D49" s="58"/>
-      <c r="E49" s="58"/>
-      <c r="F49" s="58"/>
-      <c r="G49" s="58"/>
-      <c r="H49" s="58"/>
-      <c r="I49" s="58"/>
-      <c r="J49" s="58"/>
-      <c r="K49" s="58"/>
-      <c r="L49" s="58"/>
+      <c r="C49" s="59"/>
+      <c r="D49" s="59"/>
+      <c r="E49" s="59"/>
+      <c r="F49" s="59"/>
+      <c r="G49" s="59"/>
+      <c r="H49" s="59"/>
+      <c r="I49" s="59"/>
+      <c r="J49" s="59"/>
+      <c r="K49" s="59"/>
+      <c r="L49" s="59"/>
       <c r="N49" s="48" t="s">
         <v>91</v>
       </c>
@@ -2893,19 +2899,19 @@
       <c r="A50" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="B50" s="58" t="s">
+      <c r="B50" s="59" t="s">
         <v>54</v>
       </c>
-      <c r="C50" s="58"/>
-      <c r="D50" s="58"/>
-      <c r="E50" s="58"/>
-      <c r="F50" s="58"/>
-      <c r="G50" s="58"/>
-      <c r="H50" s="58"/>
-      <c r="I50" s="58"/>
-      <c r="J50" s="58"/>
-      <c r="K50" s="58"/>
-      <c r="L50" s="58"/>
+      <c r="C50" s="59"/>
+      <c r="D50" s="59"/>
+      <c r="E50" s="59"/>
+      <c r="F50" s="59"/>
+      <c r="G50" s="59"/>
+      <c r="H50" s="59"/>
+      <c r="I50" s="59"/>
+      <c r="J50" s="59"/>
+      <c r="K50" s="59"/>
+      <c r="L50" s="59"/>
       <c r="O50" t="s">
         <v>97</v>
       </c>
@@ -2914,19 +2920,19 @@
       <c r="A51" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="B51" s="58" t="s">
+      <c r="B51" s="59" t="s">
         <v>53</v>
       </c>
-      <c r="C51" s="58"/>
-      <c r="D51" s="58"/>
-      <c r="E51" s="58"/>
-      <c r="F51" s="58"/>
-      <c r="G51" s="58"/>
-      <c r="H51" s="58"/>
-      <c r="I51" s="58"/>
-      <c r="J51" s="58"/>
-      <c r="K51" s="58"/>
-      <c r="L51" s="58"/>
+      <c r="C51" s="59"/>
+      <c r="D51" s="59"/>
+      <c r="E51" s="59"/>
+      <c r="F51" s="59"/>
+      <c r="G51" s="59"/>
+      <c r="H51" s="59"/>
+      <c r="I51" s="59"/>
+      <c r="J51" s="59"/>
+      <c r="K51" s="59"/>
+      <c r="L51" s="59"/>
       <c r="O51" t="s">
         <v>98</v>
       </c>
@@ -2944,20 +2950,19 @@
   <sortState ref="A24:K25">
     <sortCondition ref="A3"/>
   </sortState>
-  <mergeCells count="60">
+  <mergeCells count="59">
+    <mergeCell ref="N16:S16"/>
+    <mergeCell ref="N31:S31"/>
     <mergeCell ref="N38:S38"/>
-    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="N30:S30"/>
+    <mergeCell ref="N25:S25"/>
+    <mergeCell ref="N33:S33"/>
+    <mergeCell ref="N35:S36"/>
     <mergeCell ref="H28:K28"/>
     <mergeCell ref="H3:K3"/>
     <mergeCell ref="C3:G3"/>
     <mergeCell ref="C30:G30"/>
     <mergeCell ref="H30:K30"/>
-    <mergeCell ref="N16:S16"/>
-    <mergeCell ref="N31:S31"/>
-    <mergeCell ref="N37:S37"/>
-    <mergeCell ref="N30:S30"/>
-    <mergeCell ref="N25:S25"/>
-    <mergeCell ref="N33:S33"/>
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="O6:U6"/>
     <mergeCell ref="A1:L1"/>
@@ -2970,10 +2975,10 @@
     <mergeCell ref="N27:S27"/>
     <mergeCell ref="N20:S20"/>
     <mergeCell ref="O14:S15"/>
-    <mergeCell ref="N22:S22"/>
     <mergeCell ref="N19:S19"/>
     <mergeCell ref="N17:S17"/>
     <mergeCell ref="N28:S28"/>
+    <mergeCell ref="C28:G28"/>
     <mergeCell ref="A30:B30"/>
     <mergeCell ref="A33:B33"/>
     <mergeCell ref="A32:B32"/>

</xml_diff>

<commit_message>
se trabajo con la logica de negocio esperada en Trayectoria. Seguir testeando y dondole estilo antes de pasar a formacion
</commit_message>
<xml_diff>
--- a/Cuadro-de-estado.xlsx
+++ b/Cuadro-de-estado.xlsx
@@ -1384,6 +1384,177 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1407,177 +1578,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1881,7 +1881,7 @@
   <dimension ref="A1:U54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M39" sqref="M39"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1898,25 +1898,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="23.25">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="78" t="s">
         <v>84</v>
       </c>
-      <c r="B1" s="102"/>
-      <c r="C1" s="102"/>
-      <c r="D1" s="102"/>
-      <c r="E1" s="102"/>
-      <c r="F1" s="102"/>
-      <c r="G1" s="102"/>
-      <c r="H1" s="102"/>
-      <c r="I1" s="102"/>
-      <c r="J1" s="102"/>
-      <c r="K1" s="102"/>
-      <c r="L1" s="102"/>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="78"/>
+      <c r="K1" s="78"/>
+      <c r="L1" s="78"/>
     </row>
     <row r="2" spans="1:21" ht="19.5" thickBot="1">
       <c r="A2" s="44">
         <f ca="1">M2-TODAY()-1</f>
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B2" s="45" t="s">
         <v>85</v>
@@ -1930,30 +1930,30 @@
       </c>
     </row>
     <row r="3" spans="1:21" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="103" t="s">
+      <c r="A3" s="79" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="104"/>
-      <c r="C3" s="105" t="s">
+      <c r="B3" s="80"/>
+      <c r="C3" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="106"/>
-      <c r="E3" s="106"/>
-      <c r="F3" s="106"/>
-      <c r="G3" s="107"/>
-      <c r="H3" s="105" t="s">
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="69"/>
+      <c r="H3" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="106"/>
-      <c r="J3" s="108"/>
-      <c r="K3" s="107"/>
+      <c r="I3" s="67"/>
+      <c r="J3" s="68"/>
+      <c r="K3" s="69"/>
       <c r="L3" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="109" t="s">
+      <c r="M3" s="81" t="s">
         <v>76</v>
       </c>
-      <c r="N3" s="101"/>
+      <c r="N3" s="77"/>
     </row>
     <row r="4" spans="1:21" s="3" customFormat="1" ht="40.5" customHeight="1" thickBot="1">
       <c r="A4" s="17" t="s">
@@ -1992,10 +1992,10 @@
       <c r="L4" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="M4" s="110" t="s">
+      <c r="M4" s="82" t="s">
         <v>77</v>
       </c>
-      <c r="N4" s="111"/>
+      <c r="N4" s="83"/>
       <c r="O4" s="34" t="s">
         <v>61</v>
       </c>
@@ -2032,15 +2032,15 @@
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
-      <c r="O6" s="100" t="s">
+      <c r="O6" s="76" t="s">
         <v>65</v>
       </c>
-      <c r="P6" s="101"/>
-      <c r="Q6" s="101"/>
-      <c r="R6" s="101"/>
-      <c r="S6" s="101"/>
-      <c r="T6" s="101"/>
-      <c r="U6" s="101"/>
+      <c r="P6" s="77"/>
+      <c r="Q6" s="77"/>
+      <c r="R6" s="77"/>
+      <c r="S6" s="77"/>
+      <c r="T6" s="77"/>
+      <c r="U6" s="77"/>
     </row>
     <row r="7" spans="1:21" ht="4.5" customHeight="1">
       <c r="A7" s="28"/>
@@ -2200,13 +2200,13 @@
       <c r="J14" s="4"/>
       <c r="K14" s="54"/>
       <c r="L14" s="4"/>
-      <c r="O14" s="113" t="s">
+      <c r="O14" s="84" t="s">
         <v>75</v>
       </c>
-      <c r="P14" s="113"/>
-      <c r="Q14" s="113"/>
-      <c r="R14" s="113"/>
-      <c r="S14" s="113"/>
+      <c r="P14" s="84"/>
+      <c r="Q14" s="84"/>
+      <c r="R14" s="84"/>
+      <c r="S14" s="84"/>
     </row>
     <row r="15" spans="1:21" ht="15" customHeight="1">
       <c r="A15" s="38" t="s">
@@ -2215,21 +2215,21 @@
       <c r="B15" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="40"/>
+      <c r="C15" s="4"/>
       <c r="D15" s="40"/>
-      <c r="E15" s="40"/>
+      <c r="E15" s="4"/>
       <c r="F15" s="40"/>
-      <c r="G15" s="40"/>
+      <c r="G15" s="4"/>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
       <c r="K15" s="54"/>
       <c r="L15" s="4"/>
-      <c r="O15" s="113"/>
-      <c r="P15" s="113"/>
-      <c r="Q15" s="113"/>
-      <c r="R15" s="113"/>
-      <c r="S15" s="113"/>
+      <c r="O15" s="84"/>
+      <c r="P15" s="84"/>
+      <c r="Q15" s="84"/>
+      <c r="R15" s="84"/>
+      <c r="S15" s="84"/>
       <c r="T15" s="53"/>
     </row>
     <row r="16" spans="1:21">
@@ -2249,14 +2249,14 @@
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
       <c r="L16" s="4"/>
-      <c r="N16" s="112" t="s">
+      <c r="N16" s="59" t="s">
         <v>110</v>
       </c>
-      <c r="O16" s="112"/>
-      <c r="P16" s="112"/>
-      <c r="Q16" s="112"/>
-      <c r="R16" s="112"/>
-      <c r="S16" s="112"/>
+      <c r="O16" s="59"/>
+      <c r="P16" s="59"/>
+      <c r="Q16" s="59"/>
+      <c r="R16" s="59"/>
+      <c r="S16" s="59"/>
       <c r="T16" s="53"/>
     </row>
     <row r="17" spans="1:19">
@@ -2266,24 +2266,24 @@
       <c r="B17" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="4"/>
+      <c r="C17" s="40"/>
       <c r="D17" s="40"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="4"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="54"/>
+      <c r="G17" s="40"/>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
       <c r="L17" s="4"/>
-      <c r="N17" s="112" t="s">
+      <c r="N17" s="59" t="s">
         <v>126</v>
       </c>
-      <c r="O17" s="112"/>
-      <c r="P17" s="112"/>
-      <c r="Q17" s="112"/>
-      <c r="R17" s="112"/>
-      <c r="S17" s="112"/>
+      <c r="O17" s="59"/>
+      <c r="P17" s="59"/>
+      <c r="Q17" s="59"/>
+      <c r="R17" s="59"/>
+      <c r="S17" s="59"/>
     </row>
     <row r="18" spans="1:19" ht="4.5" customHeight="1">
       <c r="A18" s="28"/>
@@ -2316,14 +2316,14 @@
       <c r="J19" s="5"/>
       <c r="K19" s="7"/>
       <c r="L19" s="52"/>
-      <c r="N19" s="112" t="s">
+      <c r="N19" s="59" t="s">
         <v>124</v>
       </c>
-      <c r="O19" s="112"/>
-      <c r="P19" s="112"/>
-      <c r="Q19" s="112"/>
-      <c r="R19" s="112"/>
-      <c r="S19" s="112"/>
+      <c r="O19" s="59"/>
+      <c r="P19" s="59"/>
+      <c r="Q19" s="59"/>
+      <c r="R19" s="59"/>
+      <c r="S19" s="59"/>
     </row>
     <row r="20" spans="1:19">
       <c r="A20" s="39" t="s">
@@ -2342,14 +2342,14 @@
       <c r="J20" s="5"/>
       <c r="K20" s="7"/>
       <c r="L20" s="52"/>
-      <c r="N20" s="112" t="s">
+      <c r="N20" s="59" t="s">
         <v>113</v>
       </c>
-      <c r="O20" s="112"/>
-      <c r="P20" s="112"/>
-      <c r="Q20" s="112"/>
-      <c r="R20" s="112"/>
-      <c r="S20" s="112"/>
+      <c r="O20" s="59"/>
+      <c r="P20" s="59"/>
+      <c r="Q20" s="59"/>
+      <c r="R20" s="59"/>
+      <c r="S20" s="59"/>
     </row>
     <row r="21" spans="1:19" ht="4.5" customHeight="1">
       <c r="A21" s="28"/>
@@ -2416,14 +2416,14 @@
       <c r="J24" s="5"/>
       <c r="K24" s="7"/>
       <c r="L24" s="4"/>
-      <c r="N24" s="112" t="s">
+      <c r="N24" s="59" t="s">
         <v>83</v>
       </c>
-      <c r="O24" s="112"/>
-      <c r="P24" s="112"/>
-      <c r="Q24" s="112"/>
-      <c r="R24" s="112"/>
-      <c r="S24" s="112"/>
+      <c r="O24" s="59"/>
+      <c r="P24" s="59"/>
+      <c r="Q24" s="59"/>
+      <c r="R24" s="59"/>
+      <c r="S24" s="59"/>
     </row>
     <row r="25" spans="1:19">
       <c r="A25" s="39" t="s">
@@ -2442,14 +2442,14 @@
       <c r="J25" s="5"/>
       <c r="K25" s="7"/>
       <c r="L25" s="4"/>
-      <c r="N25" s="112" t="s">
+      <c r="N25" s="59" t="s">
         <v>82</v>
       </c>
-      <c r="O25" s="112"/>
-      <c r="P25" s="112"/>
-      <c r="Q25" s="112"/>
-      <c r="R25" s="112"/>
-      <c r="S25" s="112"/>
+      <c r="O25" s="59"/>
+      <c r="P25" s="59"/>
+      <c r="Q25" s="59"/>
+      <c r="R25" s="59"/>
+      <c r="S25" s="59"/>
     </row>
     <row r="26" spans="1:19" ht="4.5" customHeight="1" thickBot="1">
       <c r="A26" s="28"/>
@@ -2468,60 +2468,60 @@
     <row r="27" spans="1:19" ht="15.75" thickBot="1">
       <c r="A27" s="23"/>
       <c r="B27" s="25"/>
-      <c r="C27" s="105" t="s">
+      <c r="C27" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="106"/>
-      <c r="E27" s="106"/>
-      <c r="F27" s="106"/>
-      <c r="G27" s="107"/>
-      <c r="H27" s="105" t="s">
+      <c r="D27" s="67"/>
+      <c r="E27" s="67"/>
+      <c r="F27" s="67"/>
+      <c r="G27" s="69"/>
+      <c r="H27" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="I27" s="106"/>
-      <c r="J27" s="108"/>
-      <c r="K27" s="107"/>
+      <c r="I27" s="67"/>
+      <c r="J27" s="68"/>
+      <c r="K27" s="69"/>
       <c r="L27" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="N27" s="112" t="s">
+      <c r="N27" s="59" t="s">
         <v>78</v>
       </c>
-      <c r="O27" s="112"/>
-      <c r="P27" s="112"/>
-      <c r="Q27" s="112"/>
-      <c r="R27" s="112"/>
-      <c r="S27" s="112"/>
+      <c r="O27" s="59"/>
+      <c r="P27" s="59"/>
+      <c r="Q27" s="59"/>
+      <c r="R27" s="59"/>
+      <c r="S27" s="59"/>
     </row>
     <row r="28" spans="1:19" ht="30">
-      <c r="A28" s="98" t="s">
+      <c r="A28" s="74" t="s">
         <v>29</v>
       </c>
-      <c r="B28" s="99"/>
-      <c r="C28" s="92" t="s">
+      <c r="B28" s="75"/>
+      <c r="C28" s="85" t="s">
         <v>88</v>
       </c>
-      <c r="D28" s="93"/>
-      <c r="E28" s="93"/>
-      <c r="F28" s="93"/>
-      <c r="G28" s="94"/>
-      <c r="H28" s="115" t="s">
+      <c r="D28" s="86"/>
+      <c r="E28" s="86"/>
+      <c r="F28" s="86"/>
+      <c r="G28" s="87"/>
+      <c r="H28" s="63" t="s">
         <v>86</v>
       </c>
-      <c r="I28" s="116"/>
-      <c r="J28" s="116"/>
-      <c r="K28" s="117"/>
+      <c r="I28" s="64"/>
+      <c r="J28" s="64"/>
+      <c r="K28" s="65"/>
       <c r="L28" s="47" t="s">
         <v>87</v>
       </c>
-      <c r="N28" s="114" t="s">
+      <c r="N28" s="60" t="s">
         <v>111</v>
       </c>
-      <c r="O28" s="114"/>
-      <c r="P28" s="114"/>
-      <c r="Q28" s="114"/>
-      <c r="R28" s="114"/>
-      <c r="S28" s="114"/>
+      <c r="O28" s="60"/>
+      <c r="P28" s="60"/>
+      <c r="Q28" s="60"/>
+      <c r="R28" s="60"/>
+      <c r="S28" s="60"/>
     </row>
     <row r="29" spans="1:19" ht="4.5" customHeight="1">
       <c r="A29" s="28"/>
@@ -2538,100 +2538,100 @@
       <c r="L29" s="30"/>
     </row>
     <row r="30" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A30" s="67" t="s">
+      <c r="A30" s="88" t="s">
         <v>38</v>
       </c>
-      <c r="B30" s="68"/>
-      <c r="C30" s="118"/>
-      <c r="D30" s="119"/>
-      <c r="E30" s="119"/>
-      <c r="F30" s="119"/>
-      <c r="G30" s="120"/>
-      <c r="H30" s="121"/>
-      <c r="I30" s="119"/>
-      <c r="J30" s="119"/>
-      <c r="K30" s="120"/>
+      <c r="B30" s="89"/>
+      <c r="C30" s="70"/>
+      <c r="D30" s="71"/>
+      <c r="E30" s="71"/>
+      <c r="F30" s="71"/>
+      <c r="G30" s="72"/>
+      <c r="H30" s="73"/>
+      <c r="I30" s="71"/>
+      <c r="J30" s="71"/>
+      <c r="K30" s="72"/>
       <c r="L30" s="21" t="s">
         <v>5</v>
       </c>
       <c r="M30" s="32"/>
-      <c r="N30" s="112" t="s">
+      <c r="N30" s="59" t="s">
         <v>72</v>
       </c>
-      <c r="O30" s="112"/>
-      <c r="P30" s="112"/>
-      <c r="Q30" s="112"/>
-      <c r="R30" s="112"/>
-      <c r="S30" s="112"/>
+      <c r="O30" s="59"/>
+      <c r="P30" s="59"/>
+      <c r="Q30" s="59"/>
+      <c r="R30" s="59"/>
+      <c r="S30" s="59"/>
     </row>
     <row r="31" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A31" s="67" t="s">
+      <c r="A31" s="88" t="s">
         <v>79</v>
       </c>
-      <c r="B31" s="68"/>
-      <c r="C31" s="92"/>
-      <c r="D31" s="93"/>
-      <c r="E31" s="93"/>
-      <c r="F31" s="93"/>
-      <c r="G31" s="94"/>
-      <c r="H31" s="95" t="s">
+      <c r="B31" s="89"/>
+      <c r="C31" s="85"/>
+      <c r="D31" s="86"/>
+      <c r="E31" s="86"/>
+      <c r="F31" s="86"/>
+      <c r="G31" s="87"/>
+      <c r="H31" s="98" t="s">
         <v>80</v>
       </c>
-      <c r="I31" s="96"/>
-      <c r="J31" s="96"/>
-      <c r="K31" s="96"/>
-      <c r="L31" s="97"/>
+      <c r="I31" s="99"/>
+      <c r="J31" s="99"/>
+      <c r="K31" s="99"/>
+      <c r="L31" s="100"/>
       <c r="M31" s="32"/>
-      <c r="N31" s="114" t="s">
+      <c r="N31" s="60" t="s">
         <v>73</v>
       </c>
-      <c r="O31" s="114"/>
-      <c r="P31" s="114"/>
-      <c r="Q31" s="114"/>
-      <c r="R31" s="114"/>
-      <c r="S31" s="114"/>
+      <c r="O31" s="60"/>
+      <c r="P31" s="60"/>
+      <c r="Q31" s="60"/>
+      <c r="R31" s="60"/>
+      <c r="S31" s="60"/>
     </row>
     <row r="32" spans="1:19" ht="16.5" thickBot="1">
-      <c r="A32" s="88" t="s">
+      <c r="A32" s="92" t="s">
         <v>59</v>
       </c>
-      <c r="B32" s="89"/>
-      <c r="C32" s="83"/>
-      <c r="D32" s="84"/>
-      <c r="E32" s="84"/>
-      <c r="F32" s="84"/>
-      <c r="G32" s="90"/>
-      <c r="H32" s="91"/>
-      <c r="I32" s="84"/>
-      <c r="J32" s="84"/>
-      <c r="K32" s="90"/>
+      <c r="B32" s="93"/>
+      <c r="C32" s="94"/>
+      <c r="D32" s="95"/>
+      <c r="E32" s="95"/>
+      <c r="F32" s="95"/>
+      <c r="G32" s="96"/>
+      <c r="H32" s="97"/>
+      <c r="I32" s="95"/>
+      <c r="J32" s="95"/>
+      <c r="K32" s="96"/>
       <c r="M32" s="32"/>
     </row>
     <row r="33" spans="1:19" ht="30.75" customHeight="1" thickBot="1">
-      <c r="A33" s="86" t="s">
+      <c r="A33" s="90" t="s">
         <v>34</v>
       </c>
-      <c r="B33" s="87"/>
-      <c r="C33" s="74" t="s">
+      <c r="B33" s="91"/>
+      <c r="C33" s="106" t="s">
         <v>58</v>
       </c>
-      <c r="D33" s="75"/>
-      <c r="E33" s="75"/>
-      <c r="F33" s="75"/>
-      <c r="G33" s="76"/>
-      <c r="H33" s="71"/>
-      <c r="I33" s="72"/>
-      <c r="J33" s="72"/>
-      <c r="K33" s="73"/>
+      <c r="D33" s="107"/>
+      <c r="E33" s="107"/>
+      <c r="F33" s="107"/>
+      <c r="G33" s="108"/>
+      <c r="H33" s="103"/>
+      <c r="I33" s="104"/>
+      <c r="J33" s="104"/>
+      <c r="K33" s="105"/>
       <c r="M33" s="32"/>
-      <c r="N33" s="114" t="s">
+      <c r="N33" s="60" t="s">
         <v>125</v>
       </c>
-      <c r="O33" s="114"/>
-      <c r="P33" s="114"/>
-      <c r="Q33" s="114"/>
-      <c r="R33" s="114"/>
-      <c r="S33" s="114"/>
+      <c r="O33" s="60"/>
+      <c r="P33" s="60"/>
+      <c r="Q33" s="60"/>
+      <c r="R33" s="60"/>
+      <c r="S33" s="60"/>
     </row>
     <row r="34" spans="1:19" ht="4.5" customHeight="1" thickBot="1">
       <c r="A34" s="28"/>
@@ -2647,95 +2647,95 @@
       <c r="K34" s="30"/>
     </row>
     <row r="35" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A35" s="67" t="s">
+      <c r="A35" s="88" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="68"/>
-      <c r="C35" s="83"/>
-      <c r="D35" s="84"/>
-      <c r="E35" s="84"/>
-      <c r="F35" s="84"/>
-      <c r="G35" s="85"/>
-      <c r="H35" s="77"/>
-      <c r="I35" s="78"/>
-      <c r="J35" s="78"/>
-      <c r="K35" s="79"/>
+      <c r="B35" s="89"/>
+      <c r="C35" s="94"/>
+      <c r="D35" s="95"/>
+      <c r="E35" s="95"/>
+      <c r="F35" s="95"/>
+      <c r="G35" s="115"/>
+      <c r="H35" s="109"/>
+      <c r="I35" s="110"/>
+      <c r="J35" s="110"/>
+      <c r="K35" s="111"/>
       <c r="M35" s="32"/>
-      <c r="N35" s="123" t="s">
+      <c r="N35" s="62" t="s">
         <v>127</v>
       </c>
-      <c r="O35" s="123"/>
-      <c r="P35" s="123"/>
-      <c r="Q35" s="123"/>
-      <c r="R35" s="123"/>
-      <c r="S35" s="123"/>
+      <c r="O35" s="62"/>
+      <c r="P35" s="62"/>
+      <c r="Q35" s="62"/>
+      <c r="R35" s="62"/>
+      <c r="S35" s="62"/>
     </row>
     <row r="36" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A36" s="67" t="s">
+      <c r="A36" s="88" t="s">
         <v>89</v>
       </c>
-      <c r="B36" s="68"/>
-      <c r="C36" s="83"/>
-      <c r="D36" s="84"/>
-      <c r="E36" s="84"/>
-      <c r="F36" s="84"/>
-      <c r="G36" s="85"/>
-      <c r="H36" s="77"/>
-      <c r="I36" s="78"/>
-      <c r="J36" s="78"/>
-      <c r="K36" s="79"/>
+      <c r="B36" s="89"/>
+      <c r="C36" s="94"/>
+      <c r="D36" s="95"/>
+      <c r="E36" s="95"/>
+      <c r="F36" s="95"/>
+      <c r="G36" s="115"/>
+      <c r="H36" s="109"/>
+      <c r="I36" s="110"/>
+      <c r="J36" s="110"/>
+      <c r="K36" s="111"/>
       <c r="M36" s="32"/>
-      <c r="N36" s="123"/>
-      <c r="O36" s="123"/>
-      <c r="P36" s="123"/>
-      <c r="Q36" s="123"/>
-      <c r="R36" s="123"/>
-      <c r="S36" s="123"/>
+      <c r="N36" s="62"/>
+      <c r="O36" s="62"/>
+      <c r="P36" s="62"/>
+      <c r="Q36" s="62"/>
+      <c r="R36" s="62"/>
+      <c r="S36" s="62"/>
     </row>
     <row r="37" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A37" s="67" t="s">
+      <c r="A37" s="88" t="s">
         <v>7</v>
       </c>
-      <c r="B37" s="68"/>
-      <c r="C37" s="80"/>
-      <c r="D37" s="81"/>
-      <c r="E37" s="81"/>
-      <c r="F37" s="81"/>
-      <c r="G37" s="82"/>
-      <c r="H37" s="80"/>
-      <c r="I37" s="81"/>
-      <c r="J37" s="81"/>
-      <c r="K37" s="82"/>
+      <c r="B37" s="89"/>
+      <c r="C37" s="112"/>
+      <c r="D37" s="113"/>
+      <c r="E37" s="113"/>
+      <c r="F37" s="113"/>
+      <c r="G37" s="114"/>
+      <c r="H37" s="112"/>
+      <c r="I37" s="113"/>
+      <c r="J37" s="113"/>
+      <c r="K37" s="114"/>
       <c r="M37" s="32"/>
     </row>
     <row r="38" spans="1:19" ht="15.75" thickBot="1">
-      <c r="N38" s="122" t="s">
+      <c r="N38" s="61" t="s">
         <v>74</v>
       </c>
-      <c r="O38" s="122"/>
-      <c r="P38" s="122"/>
-      <c r="Q38" s="122"/>
-      <c r="R38" s="122"/>
-      <c r="S38" s="122"/>
+      <c r="O38" s="61"/>
+      <c r="P38" s="61"/>
+      <c r="Q38" s="61"/>
+      <c r="R38" s="61"/>
+      <c r="S38" s="61"/>
     </row>
     <row r="39" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A39" s="60" t="s">
+      <c r="A39" s="117" t="s">
         <v>25</v>
       </c>
-      <c r="B39" s="61"/>
-      <c r="C39" s="61"/>
-      <c r="D39" s="61"/>
-      <c r="E39" s="62"/>
+      <c r="B39" s="118"/>
+      <c r="C39" s="118"/>
+      <c r="D39" s="118"/>
+      <c r="E39" s="119"/>
     </row>
     <row r="40" spans="1:19">
       <c r="A40" s="14" t="s">
         <v>24</v>
       </c>
       <c r="B40" s="13"/>
-      <c r="C40" s="63" t="s">
+      <c r="C40" s="120" t="s">
         <v>22</v>
       </c>
-      <c r="D40" s="64"/>
+      <c r="D40" s="121"/>
       <c r="E40" s="27"/>
     </row>
     <row r="41" spans="1:19">
@@ -2743,10 +2743,10 @@
         <v>21</v>
       </c>
       <c r="B41" s="5"/>
-      <c r="C41" s="63" t="s">
+      <c r="C41" s="120" t="s">
         <v>23</v>
       </c>
-      <c r="D41" s="64"/>
+      <c r="D41" s="121"/>
       <c r="E41" s="8"/>
     </row>
     <row r="42" spans="1:19" ht="17.25">
@@ -2754,10 +2754,10 @@
         <v>112</v>
       </c>
       <c r="B42" s="54"/>
-      <c r="C42" s="69" t="s">
+      <c r="C42" s="101" t="s">
         <v>64</v>
       </c>
-      <c r="D42" s="70"/>
+      <c r="D42" s="102"/>
       <c r="E42" s="37"/>
       <c r="N42" s="48" t="s">
         <v>4</v>
@@ -2772,38 +2772,38 @@
       </c>
     </row>
     <row r="44" spans="1:19">
-      <c r="A44" s="65" t="s">
+      <c r="A44" s="122" t="s">
         <v>35</v>
       </c>
-      <c r="B44" s="66"/>
-      <c r="C44" s="66"/>
-      <c r="D44" s="66"/>
-      <c r="E44" s="66"/>
-      <c r="F44" s="66"/>
-      <c r="G44" s="66"/>
-      <c r="H44" s="66"/>
-      <c r="I44" s="66"/>
-      <c r="J44" s="66"/>
-      <c r="K44" s="66"/>
-      <c r="L44" s="66"/>
+      <c r="B44" s="123"/>
+      <c r="C44" s="123"/>
+      <c r="D44" s="123"/>
+      <c r="E44" s="123"/>
+      <c r="F44" s="123"/>
+      <c r="G44" s="123"/>
+      <c r="H44" s="123"/>
+      <c r="I44" s="123"/>
+      <c r="J44" s="123"/>
+      <c r="K44" s="123"/>
+      <c r="L44" s="123"/>
     </row>
     <row r="45" spans="1:19" ht="17.25">
       <c r="A45" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="B45" s="59" t="s">
+      <c r="B45" s="116" t="s">
         <v>55</v>
       </c>
-      <c r="C45" s="59"/>
-      <c r="D45" s="59"/>
-      <c r="E45" s="59"/>
-      <c r="F45" s="59"/>
-      <c r="G45" s="59"/>
-      <c r="H45" s="59"/>
-      <c r="I45" s="59"/>
-      <c r="J45" s="59"/>
-      <c r="K45" s="59"/>
-      <c r="L45" s="59"/>
+      <c r="C45" s="116"/>
+      <c r="D45" s="116"/>
+      <c r="E45" s="116"/>
+      <c r="F45" s="116"/>
+      <c r="G45" s="116"/>
+      <c r="H45" s="116"/>
+      <c r="I45" s="116"/>
+      <c r="J45" s="116"/>
+      <c r="K45" s="116"/>
+      <c r="L45" s="116"/>
       <c r="N45" s="48" t="s">
         <v>92</v>
       </c>
@@ -2815,19 +2815,19 @@
       <c r="A46" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="B46" s="59" t="s">
+      <c r="B46" s="116" t="s">
         <v>56</v>
       </c>
-      <c r="C46" s="59"/>
-      <c r="D46" s="59"/>
-      <c r="E46" s="59"/>
-      <c r="F46" s="59"/>
-      <c r="G46" s="59"/>
-      <c r="H46" s="59"/>
-      <c r="I46" s="59"/>
-      <c r="J46" s="59"/>
-      <c r="K46" s="59"/>
-      <c r="L46" s="59"/>
+      <c r="C46" s="116"/>
+      <c r="D46" s="116"/>
+      <c r="E46" s="116"/>
+      <c r="F46" s="116"/>
+      <c r="G46" s="116"/>
+      <c r="H46" s="116"/>
+      <c r="I46" s="116"/>
+      <c r="J46" s="116"/>
+      <c r="K46" s="116"/>
+      <c r="L46" s="116"/>
       <c r="O46" s="42" t="s">
         <v>96</v>
       </c>
@@ -2836,19 +2836,19 @@
       <c r="A47" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="B47" s="59" t="s">
+      <c r="B47" s="116" t="s">
         <v>57</v>
       </c>
-      <c r="C47" s="59"/>
-      <c r="D47" s="59"/>
-      <c r="E47" s="59"/>
-      <c r="F47" s="59"/>
-      <c r="G47" s="59"/>
-      <c r="H47" s="59"/>
-      <c r="I47" s="59"/>
-      <c r="J47" s="59"/>
-      <c r="K47" s="59"/>
-      <c r="L47" s="59"/>
+      <c r="C47" s="116"/>
+      <c r="D47" s="116"/>
+      <c r="E47" s="116"/>
+      <c r="F47" s="116"/>
+      <c r="G47" s="116"/>
+      <c r="H47" s="116"/>
+      <c r="I47" s="116"/>
+      <c r="J47" s="116"/>
+      <c r="K47" s="116"/>
+      <c r="L47" s="116"/>
       <c r="O47" t="s">
         <v>99</v>
       </c>
@@ -2857,37 +2857,37 @@
       <c r="A48" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="B48" s="59" t="s">
+      <c r="B48" s="116" t="s">
         <v>44</v>
       </c>
-      <c r="C48" s="59"/>
-      <c r="D48" s="59"/>
-      <c r="E48" s="59"/>
-      <c r="F48" s="59"/>
-      <c r="G48" s="59"/>
-      <c r="H48" s="59"/>
-      <c r="I48" s="59"/>
-      <c r="J48" s="59"/>
-      <c r="K48" s="59"/>
-      <c r="L48" s="59"/>
+      <c r="C48" s="116"/>
+      <c r="D48" s="116"/>
+      <c r="E48" s="116"/>
+      <c r="F48" s="116"/>
+      <c r="G48" s="116"/>
+      <c r="H48" s="116"/>
+      <c r="I48" s="116"/>
+      <c r="J48" s="116"/>
+      <c r="K48" s="116"/>
+      <c r="L48" s="116"/>
     </row>
     <row r="49" spans="1:15" ht="17.25">
       <c r="A49" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="B49" s="59" t="s">
+      <c r="B49" s="116" t="s">
         <v>33</v>
       </c>
-      <c r="C49" s="59"/>
-      <c r="D49" s="59"/>
-      <c r="E49" s="59"/>
-      <c r="F49" s="59"/>
-      <c r="G49" s="59"/>
-      <c r="H49" s="59"/>
-      <c r="I49" s="59"/>
-      <c r="J49" s="59"/>
-      <c r="K49" s="59"/>
-      <c r="L49" s="59"/>
+      <c r="C49" s="116"/>
+      <c r="D49" s="116"/>
+      <c r="E49" s="116"/>
+      <c r="F49" s="116"/>
+      <c r="G49" s="116"/>
+      <c r="H49" s="116"/>
+      <c r="I49" s="116"/>
+      <c r="J49" s="116"/>
+      <c r="K49" s="116"/>
+      <c r="L49" s="116"/>
       <c r="N49" s="48" t="s">
         <v>91</v>
       </c>
@@ -2899,19 +2899,19 @@
       <c r="A50" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="B50" s="59" t="s">
+      <c r="B50" s="116" t="s">
         <v>54</v>
       </c>
-      <c r="C50" s="59"/>
-      <c r="D50" s="59"/>
-      <c r="E50" s="59"/>
-      <c r="F50" s="59"/>
-      <c r="G50" s="59"/>
-      <c r="H50" s="59"/>
-      <c r="I50" s="59"/>
-      <c r="J50" s="59"/>
-      <c r="K50" s="59"/>
-      <c r="L50" s="59"/>
+      <c r="C50" s="116"/>
+      <c r="D50" s="116"/>
+      <c r="E50" s="116"/>
+      <c r="F50" s="116"/>
+      <c r="G50" s="116"/>
+      <c r="H50" s="116"/>
+      <c r="I50" s="116"/>
+      <c r="J50" s="116"/>
+      <c r="K50" s="116"/>
+      <c r="L50" s="116"/>
       <c r="O50" t="s">
         <v>97</v>
       </c>
@@ -2920,19 +2920,19 @@
       <c r="A51" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="B51" s="59" t="s">
+      <c r="B51" s="116" t="s">
         <v>53</v>
       </c>
-      <c r="C51" s="59"/>
-      <c r="D51" s="59"/>
-      <c r="E51" s="59"/>
-      <c r="F51" s="59"/>
-      <c r="G51" s="59"/>
-      <c r="H51" s="59"/>
-      <c r="I51" s="59"/>
-      <c r="J51" s="59"/>
-      <c r="K51" s="59"/>
-      <c r="L51" s="59"/>
+      <c r="C51" s="116"/>
+      <c r="D51" s="116"/>
+      <c r="E51" s="116"/>
+      <c r="F51" s="116"/>
+      <c r="G51" s="116"/>
+      <c r="H51" s="116"/>
+      <c r="I51" s="116"/>
+      <c r="J51" s="116"/>
+      <c r="K51" s="116"/>
+      <c r="L51" s="116"/>
       <c r="O51" t="s">
         <v>98</v>
       </c>
@@ -2951,18 +2951,37 @@
     <sortCondition ref="A3"/>
   </sortState>
   <mergeCells count="59">
-    <mergeCell ref="N16:S16"/>
-    <mergeCell ref="N31:S31"/>
-    <mergeCell ref="N38:S38"/>
-    <mergeCell ref="N30:S30"/>
-    <mergeCell ref="N25:S25"/>
-    <mergeCell ref="N33:S33"/>
-    <mergeCell ref="N35:S36"/>
-    <mergeCell ref="H28:K28"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="H30:K30"/>
+    <mergeCell ref="B50:L50"/>
+    <mergeCell ref="B51:L51"/>
+    <mergeCell ref="A39:E39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="B45:L45"/>
+    <mergeCell ref="A44:L44"/>
+    <mergeCell ref="B46:L46"/>
+    <mergeCell ref="B47:L47"/>
+    <mergeCell ref="B48:L48"/>
+    <mergeCell ref="B49:L49"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="H33:K33"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="H35:K35"/>
+    <mergeCell ref="H36:K36"/>
+    <mergeCell ref="H37:K37"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="H32:K32"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="H31:L31"/>
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="O6:U6"/>
     <mergeCell ref="A1:L1"/>
@@ -2979,37 +2998,18 @@
     <mergeCell ref="N17:S17"/>
     <mergeCell ref="N28:S28"/>
     <mergeCell ref="C28:G28"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="H32:K32"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="H31:L31"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="H33:K33"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="H35:K35"/>
-    <mergeCell ref="H36:K36"/>
-    <mergeCell ref="H37:K37"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="B50:L50"/>
-    <mergeCell ref="B51:L51"/>
-    <mergeCell ref="A39:E39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="B45:L45"/>
-    <mergeCell ref="A44:L44"/>
-    <mergeCell ref="B46:L46"/>
-    <mergeCell ref="B47:L47"/>
-    <mergeCell ref="B48:L48"/>
-    <mergeCell ref="B49:L49"/>
+    <mergeCell ref="H28:K28"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="H30:K30"/>
+    <mergeCell ref="N16:S16"/>
+    <mergeCell ref="N31:S31"/>
+    <mergeCell ref="N38:S38"/>
+    <mergeCell ref="N30:S30"/>
+    <mergeCell ref="N25:S25"/>
+    <mergeCell ref="N33:S33"/>
+    <mergeCell ref="N35:S36"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="Q4" r:id="rId1"/>

</xml_diff>